<commit_message>
add faq build week 2
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$D$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$D$90</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="133">
   <si>
     <t>Finals Week</t>
   </si>
@@ -76,17 +76,6 @@
   </si>
   <si>
     <t>Moderation</t>
-  </si>
-  <si>
-    <t>Model building/ fit</t>
-  </si>
-  <si>
-    <t>Poster Design
-Special Analysis Topics</t>
-  </si>
-  <si>
-    <t>Poster Presentations
-Final Review</t>
   </si>
   <si>
     <t>Assignment</t>
@@ -157,10 +146,6 @@
 Multiple Regression</t>
   </si>
   <si>
-    <t xml:space="preserve">Categorical Predictors
-Log and logit transformations </t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -200,12 +185,6 @@
     <t>Data Camp: OI Intro to R</t>
   </si>
   <si>
-    <t>Personal Codebook/RQ</t>
-  </si>
-  <si>
-    <t>Citation Assignment</t>
-  </si>
-  <si>
     <t>Not Started</t>
   </si>
   <si>
@@ -233,37 +212,22 @@
     <t>needs template &amp; solutions</t>
   </si>
   <si>
-    <t>DM steps preparation</t>
-  </si>
-  <si>
     <t>RAT: DM</t>
   </si>
   <si>
-    <t>DM assignment</t>
-  </si>
-  <si>
     <t>Univariate graphing</t>
   </si>
   <si>
-    <t>Peer Review univ graphics</t>
-  </si>
-  <si>
     <t>RAT: Bivariate</t>
   </si>
   <si>
     <t>PS 2.8, 2.10</t>
   </si>
   <si>
-    <t>Peer Review bivariate graphing</t>
-  </si>
-  <si>
     <t>Exam 1</t>
   </si>
   <si>
     <t>PS 3.1, 3.2</t>
-  </si>
-  <si>
-    <t>Research Plan Outline</t>
   </si>
   <si>
     <t>Poster Prep I</t>
@@ -412,9 +376,6 @@
 </t>
   </si>
   <si>
-    <t>HW 1: Team Formation, Reading, project data</t>
-  </si>
-  <si>
     <t>rubric</t>
   </si>
   <si>
@@ -422,6 +383,106 @@
   </si>
   <si>
     <t>assign</t>
+  </si>
+  <si>
+    <t>**Prepare** - Watch PDS Video 4
+**Prepare** - Read: How to read a journal article
+**Prepare** - Read: Lecture notes on literature reviews</t>
+  </si>
+  <si>
+    <t>**Prepare** - Watch [[PDS video 1]](http://passiondrivenstatistics.com/2015/05/20/chapter-01-course-introduction/) (6 min)
+**Prepare** - Look through the [[research data available]](https://drive.google.com/drive/u/3/folders/1jULudBjRbHdW-uLIvmMbxRBEJJkq9crY)
+Readiness Assurance Test (RAT) on class logistics
+Introduction to the semester long project
+Form analysis pairs - start to discuss what research topics you want to analyze</t>
+  </si>
+  <si>
+    <t>**Prepare** - Download your research data into your `project/data` folder
+**Prepare** - Start a code file called `dm.Rmd`, save into your `project/code` folder
+Import your research data into R. 
+Work with your partner to decide on what variables you will be working with. 
+Start the research question assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communicate with your partner to decide which research data you want to analyze. 
+Schedule a time outside of class to work with your analysis partner on a weekly basis. </t>
+  </si>
+  <si>
+    <t>Identify and differentiate between continuous and categorical data types
+Import data into R using code</t>
+  </si>
+  <si>
+    <t>**Prepare** - Watch [PDS Video 2](http://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)
+**Prepare** - read Course Notes (CN) section 2.1 and Open Intro (OI) textbook section 1.2
+RAT on Data Types
+Review of how data is stored in spreadsheets
+Discuss continuous vs categorical data types</t>
+  </si>
+  <si>
+    <t>PR Personal Codebook</t>
+  </si>
+  <si>
+    <t>Campus Closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No School
+Categorical Predictors
+Log and logit transformations </t>
+  </si>
+  <si>
+    <t>Poster Presentations
+Poster Presentations
+Final Review</t>
+  </si>
+  <si>
+    <t>Model building
+Poster Design
+Open work day</t>
+  </si>
+  <si>
+    <t>Model building</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problem set (PS) 2.2 (Due Sun 9/9 )
+Data Camp Open Intro - Intro to R **AND**  Intro to Data [BBL] (Due Sun 9/9 )
+Research question assignment [[HTML]](hw/hw02_research_codebook.html)[[PDF]](hw/hw02_research_codebook.html) (Due Sun 9/9 )
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Peer review of research question (Due Tue 9/11 )</t>
+    </r>
+  </si>
+  <si>
+    <t>No School
+Data architecture and entry
+Creating research questions</t>
+  </si>
+  <si>
+    <t>[PDS video 2](http://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)
+Course Notes (CN) section 2.1
+Open Intro (OI) Section 1.2
+[Research data](https://drive.google.com/drive/u/3/folders/1jULudBjRbHdW-uLIvmMbxRBEJJkq9crY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Syllabus](https://norcalbiostat.github.io/MATH615/syllabus_315_f18.html)
+[Passion Driven Statistics](reading/PDS_Intro_Stat.pdf)
+[List of Articles](http://www.norcalbiostat.com/articles/articles.html)
+[PDS video 1](http://passiondrivenstatistics.com/2015/05/20/chapter-01-course-introduction/) </t>
   </si>
   <si>
     <r>
@@ -437,7 +498,7 @@
 [Data Camp](https://www.datacamp.com/users/sign_in) Intro to R - Intro to Basics Chapter [BBL] (Due Sun 9/2 )
 [Metacognition Awareness Inventory](https://www.datacamp.com/users/sign_in)  [BBL] (Due Sun 9/2 )
 R Markdown test file (Due Wed 8/29 )
-HW 1 [[Template]](hw/hw01_template.Rmd)(Due Sun 9/2 )</t>
+HW 1 [[RMD]](hw/hw01_template.Rmd)(Due Sun 9/2 )</t>
     </r>
     <r>
       <rPr>
@@ -451,65 +512,34 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">No School
-Data architecture and entry
-Creating research questions
-</t>
-  </si>
-  <si>
-    <t>**Prepare** - Watch PDS Video 4
-**Prepare** - Read: How to read a journal article
-**Prepare** - Read: Lecture notes on literature reviews</t>
-  </si>
-  <si>
-    <t>**Prepare** - Watch [[PDS video 1]](http://passiondrivenstatistics.com/2015/05/20/chapter-01-course-introduction/) (6 min)
-**Prepare** - Look through the [[research data available]](https://drive.google.com/drive/u/3/folders/1jULudBjRbHdW-uLIvmMbxRBEJJkq9crY)
-Readiness Assurance Test (RAT) on class logistics
-Introduction to the semester long project
-Form analysis pairs - start to discuss what research topics you want to analyze</t>
-  </si>
-  <si>
-    <t>**Prepare** - Download your research data into your `project/data` folder
-**Prepare** - Start a code file called `dm.Rmd`, save into your `project/code` folder
-Import your research data into R. 
-Work with your partner to decide on what variables you will be working with. 
-Start the research question assignment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Syllabus](https://norcalbiostat.github.io/MATH615/syllabus_315_f18.html)
-[Passion Driven Statistics](reading/PDS_Intro_Stat.pdf)
-[List of Articles](http://www.norcalbiostat.com/articles/articles.html)
-[[PDS video 1]](http://passiondrivenstatistics.com/2015/05/20/chapter-01-course-introduction/) </t>
-  </si>
-  <si>
-    <t>[[PDS video 2]](http://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)
-Course Notes (CN) section 2.1
-Open Intro (OI) Section 1.2
-[[Research data]](https://drive.google.com/drive/u/3/folders/1jULudBjRbHdW-uLIvmMbxRBEJJkq9crY)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Communicate with your partner to decide which research data you want to analyze. 
-Schedule a time outside of class to work with your analysis partner on a weekly basis. </t>
-  </si>
-  <si>
-    <t>Identify and differentiate between continuous and categorical data types
-Import data into R using code</t>
-  </si>
-  <si>
-    <t>**Prepare** - Watch [PDS Video 2](http://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)
-**Prepare** - read Course Notes (CN) section 2.1 and Open Intro (OI) textbook section 1.2
-RAT on Data Types
-Review of how data is stored in spreadsheets
-Discuss continuous vs categorical data types</t>
-  </si>
-  <si>
-    <t>PR Personal Codebook</t>
-  </si>
-  <si>
-    <t>Problem set (PS) 2.2 (Due Sun 9/9 )
-Data Camp Open Intro - Intro to R **AND**  Intro to Data [BBL] (Due Sun 9/9 )
-Research question assignment [[HTML]](hw/hw02_research_codebook.html)[[PDF]](hw/hw02_research_codebook.html) (Due Sun 9/9 )
-Peer review of research question (Due Tue 9/11 )</t>
+    <t>hw01 1: Team Formation, Reading, project data</t>
+  </si>
+  <si>
+    <t>hw02 Personal Codebook/RQ</t>
+  </si>
+  <si>
+    <t>hw03 Citation Assignment</t>
+  </si>
+  <si>
+    <t>PR citation assignment</t>
+  </si>
+  <si>
+    <t>PR DM steps</t>
+  </si>
+  <si>
+    <t>Research Proposal</t>
+  </si>
+  <si>
+    <t>hw04 DM steps preparation</t>
+  </si>
+  <si>
+    <t>hw05  DM assignment</t>
+  </si>
+  <si>
+    <t>Peer review Research Proposal</t>
+  </si>
+  <si>
+    <t>Ready to be used, % based</t>
   </si>
 </sst>
 </file>
@@ -519,9 +549,23 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -615,7 +659,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -688,6 +732,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -738,123 +806,123 @@
   </borders>
   <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="77" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="77" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="77" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="78" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="78" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="81" applyFont="1" applyAlignment="1">
@@ -866,34 +934,34 @@
     <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="81" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="4" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="7" borderId="4" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="8" borderId="4" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -902,79 +970,102 @@
     <xf numFmtId="1" fontId="0" fillId="8" borderId="4" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="9" borderId="4" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="77" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="77" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="82">
@@ -1399,12 +1490,12 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="38" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="38" customWidth="1"/>
     <col min="2" max="2" width="10.125" style="38" customWidth="1"/>
     <col min="3" max="3" width="24.625" style="38" customWidth="1"/>
     <col min="4" max="4" width="27.375" style="45" customWidth="1"/>
@@ -1436,13 +1527,13 @@
         <v>6</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J1" s="36" t="s">
         <v>7</v>
@@ -1456,28 +1547,28 @@
         <v>41877</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -1492,25 +1583,25 @@
         <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>129</v>
+        <v>108</v>
+      </c>
+      <c r="J3" s="55" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1528,7 +1619,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1543,7 +1634,7 @@
         <v>41898</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1581,7 +1672,7 @@
         <v>41912</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1619,7 +1710,7 @@
         <v>41926</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1638,7 +1729,7 @@
         <v>41933</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1676,7 +1767,7 @@
         <v>41947</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1686,7 +1777,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>12</v>
       </c>
@@ -1695,12 +1786,14 @@
         <v>41954</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
@@ -1729,7 +1822,7 @@
         <v>41968</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1739,7 +1832,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>14</v>
       </c>
@@ -1748,7 +1841,7 @@
         <v>41975</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1758,7 +1851,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>15</v>
       </c>
@@ -1767,7 +1860,7 @@
         <v>41982</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1777,7 +1870,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>0</v>
       </c>
@@ -1796,15 +1889,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V88"/>
+  <dimension ref="A1:V91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,61 +1919,61 @@
   <sheetData>
     <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="L1" s="27" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M1" s="27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="N1" s="27" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="P1" s="27" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="Q1" s="27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="R1" s="27" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="T1" s="31" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="U1" s="31" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="V1" s="31" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1887,27 +1981,27 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D2" s="13">
         <v>10</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="I2" s="8">
-        <f t="shared" ref="I2:I8" si="0">SUMIF($C$2:$C$79,H2,$D$2:$D$79)</f>
+        <f>SUMIF($C$2:$C$82,H2,$D$2:$D$82)</f>
         <v>42</v>
       </c>
       <c r="J2" s="14">
-        <f t="shared" ref="J2:J8" si="1">I2/$I$9</f>
-        <v>8.9171974522292988E-2</v>
+        <f t="shared" ref="J2:J8" si="0">I2/$I$9</f>
+        <v>8.6065573770491802E-2</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M2" s="9">
         <v>16</v>
@@ -1916,7 +2010,7 @@
         <v>3.9506172839506172E-2</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="Q2" s="26">
         <v>20</v>
@@ -1925,7 +2019,7 @@
         <v>4.3956043956043959E-2</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="U2" s="10">
         <v>14</v>
@@ -1939,10 +2033,10 @@
         <v>1.3</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D3" s="13">
         <v>3</v>
@@ -1950,19 +2044,22 @@
       <c r="E3" s="47">
         <v>41883</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>15</v>
+      <c r="G3" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="I3" s="8">
+        <f>SUMIF($C$2:$C$82,H3,$D$2:$D$82)</f>
+        <v>52</v>
+      </c>
+      <c r="J3" s="14">
         <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="J3" s="14">
-        <f t="shared" si="1"/>
-        <v>0.12738853503184713</v>
+        <v>0.10655737704918032</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M3" s="9">
         <v>36</v>
@@ -1971,7 +2068,7 @@
         <v>8.8888888888888892E-2</v>
       </c>
       <c r="P3" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="26">
         <v>100</v>
@@ -1980,7 +2077,7 @@
         <v>0.21978021978021978</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="U3" s="10">
         <v>99</v>
@@ -1994,10 +2091,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>12</v>
       </c>
       <c r="D4" s="13">
         <v>2</v>
@@ -2005,22 +2102,22 @@
       <c r="E4" s="47">
         <v>41879</v>
       </c>
-      <c r="G4" s="58" t="s">
-        <v>116</v>
+      <c r="G4" s="52" t="s">
+        <v>104</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I4" s="8">
+        <f>SUMIF($C$2:$C$82,H4,$D$2:$D$82)</f>
+        <v>64</v>
+      </c>
+      <c r="J4" s="14">
         <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="J4" s="14">
-        <f t="shared" si="1"/>
-        <v>0.12526539278131635</v>
+        <v>0.13114754098360656</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M4" s="9">
         <v>40</v>
@@ -2029,7 +2126,7 @@
         <v>9.8765432098765427E-2</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q4" s="26">
         <v>25</v>
@@ -2038,7 +2135,7 @@
         <v>5.4945054945054944E-2</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="U4" s="10">
         <v>20</v>
@@ -2052,10 +2149,10 @@
         <v>1.2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="13">
         <v>1</v>
@@ -2063,9 +2160,12 @@
       <c r="E5" s="47">
         <v>41881</v>
       </c>
+      <c r="G5" s="53" t="s">
+        <v>104</v>
+      </c>
       <c r="J5" s="14"/>
       <c r="L5" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="M5" s="9">
         <v>26</v>
@@ -2074,7 +2174,7 @@
         <v>6.4197530864197536E-2</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="Q5" s="26">
         <v>10</v>
@@ -2083,7 +2183,7 @@
         <v>2.197802197802198E-2</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="U5" s="10">
         <v>32</v>
@@ -2097,10 +2197,10 @@
         <v>1.4</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="19">
         <v>1</v>
@@ -2108,19 +2208,22 @@
       <c r="E6" s="47">
         <v>41883</v>
       </c>
+      <c r="G6" s="53" t="s">
+        <v>104</v>
+      </c>
       <c r="H6" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I6" s="8">
+        <f>SUMIF($C$2:$C$82,H6,$D$2:$D$82)</f>
+        <v>30</v>
+      </c>
+      <c r="J6" s="14">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="J6" s="14">
-        <f t="shared" si="1"/>
-        <v>6.3694267515923567E-2</v>
+        <v>6.1475409836065573E-2</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M6" s="9">
         <v>27</v>
@@ -2129,7 +2232,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="Q6" s="26">
         <v>150</v>
@@ -2138,7 +2241,7 @@
         <v>0.32967032967032966</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="U6" s="10">
         <v>10</v>
@@ -2151,11 +2254,11 @@
       <c r="A7" s="11">
         <v>1.5</v>
       </c>
-      <c r="B7" s="57" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>15</v>
+      <c r="B7" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>12</v>
       </c>
       <c r="D7" s="13">
         <v>5</v>
@@ -2163,22 +2266,22 @@
       <c r="E7" s="47">
         <v>41883</v>
       </c>
-      <c r="G7" s="58" t="s">
-        <v>116</v>
+      <c r="G7" s="52" t="s">
+        <v>104</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I7" s="8">
+        <f>SUMIF($C$2:$C$82,H7,$D$2:$D$82)</f>
+        <v>150</v>
+      </c>
+      <c r="J7" s="14">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="J7" s="14">
-        <f t="shared" si="1"/>
-        <v>0.31847133757961782</v>
+        <v>0.30737704918032788</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M7" s="9">
         <v>150</v>
@@ -2187,7 +2290,7 @@
         <v>0.37037037037037035</v>
       </c>
       <c r="P7" s="29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q7" s="30">
         <v>150</v>
@@ -2196,7 +2299,7 @@
         <v>0.32967032967032966</v>
       </c>
       <c r="T7" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="U7" s="10">
         <v>175</v>
@@ -2210,10 +2313,10 @@
         <v>1.6</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D8" s="21">
         <v>2.5</v>
@@ -2221,22 +2324,22 @@
       <c r="E8" s="47">
         <v>41883</v>
       </c>
-      <c r="G8" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>22</v>
+      <c r="G8" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="70" t="s">
+        <v>19</v>
       </c>
       <c r="I8" s="8">
+        <f>SUMIF($C$2:$C$82,H8,$D$2:$D$82)</f>
+        <v>150</v>
+      </c>
+      <c r="J8" s="14">
         <f t="shared" si="0"/>
-        <v>130</v>
-      </c>
-      <c r="J8" s="14">
-        <f t="shared" si="1"/>
-        <v>0.27600849256900212</v>
+        <v>0.30737704918032788</v>
       </c>
       <c r="L8" s="27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M8" s="27">
         <v>110</v>
@@ -2250,7 +2353,7 @@
       </c>
       <c r="R8" s="17"/>
       <c r="T8" s="31" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="U8" s="31">
         <v>105</v>
@@ -2264,10 +2367,10 @@
         <v>2.1</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D9" s="13">
         <v>2</v>
@@ -2275,9 +2378,12 @@
       <c r="E9" s="47">
         <v>41886</v>
       </c>
+      <c r="G9" s="53" t="s">
+        <v>104</v>
+      </c>
       <c r="I9" s="6">
         <f>SUM(I2:I8)</f>
-        <v>471</v>
+        <v>488</v>
       </c>
       <c r="M9" s="8">
         <v>405</v>
@@ -2293,16 +2399,19 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D10" s="13">
         <v>1</v>
       </c>
       <c r="E10" s="47">
         <v>41890</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -2310,16 +2419,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D11" s="13">
         <v>5</v>
       </c>
       <c r="E11" s="47">
         <v>41890</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -2327,10 +2439,10 @@
         <v>2.4</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D12" s="13">
         <v>3</v>
@@ -2338,17 +2450,19 @@
       <c r="E12" s="47">
         <v>41890</v>
       </c>
-      <c r="G12" s="58"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="G12" s="53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>2.5</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>22</v>
+      <c r="B13" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="69" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="13">
         <v>10</v>
@@ -2356,224 +2470,228 @@
       <c r="E13" s="47">
         <v>41890</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="F13" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="G13" s="53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20">
         <v>2.6</v>
       </c>
-      <c r="B14" s="57" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="13">
+      <c r="B14" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="21">
         <v>4</v>
       </c>
       <c r="E14" s="47">
         <v>41892</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>3</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>22</v>
+      <c r="B15" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>19</v>
       </c>
       <c r="D15" s="13">
         <v>10</v>
       </c>
-      <c r="H15" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" s="52"/>
+      <c r="H15" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>3</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>20</v>
+      <c r="B16" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="63" t="s">
+        <v>38</v>
       </c>
       <c r="D16" s="13">
-        <v>2</v>
-      </c>
-      <c r="H16" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="53"/>
+        <v>4</v>
+      </c>
+      <c r="H16" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="57"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>3</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>105</v>
+        <v>47</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="D17" s="13">
         <v>2</v>
       </c>
-      <c r="H17" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" s="54"/>
+      <c r="H17" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="58"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>3</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>105</v>
+        <v>49</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>94</v>
       </c>
       <c r="D18" s="13">
         <v>2</v>
       </c>
-      <c r="H18" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="I18" s="55"/>
+      <c r="H18" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="59"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>3</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D19" s="13">
-        <v>1</v>
-      </c>
-      <c r="H19" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="56"/>
+        <v>2</v>
+      </c>
+      <c r="H19" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="60"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>3</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="D20" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>4</v>
       </c>
-      <c r="B21" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>20</v>
+      <c r="B21" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="62" t="s">
+        <v>19</v>
       </c>
       <c r="D21" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>4</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>15</v>
+      <c r="B22" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="63" t="s">
+        <v>38</v>
       </c>
       <c r="D22" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>4</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>64</v>
+      <c r="B23" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>4</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>42</v>
+      <c r="B24" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="62" t="s">
+        <v>19</v>
       </c>
       <c r="D24" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="B25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="13">
         <v>5</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="13">
-        <v>2</v>
+      <c r="F25" s="75" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
-        <v>5</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" s="13">
-        <v>2</v>
-      </c>
+      <c r="A26" s="11"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>5</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D27" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2581,55 +2699,47 @@
         <v>5</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="D28" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="C29" s="65" t="s">
+        <v>12</v>
       </c>
       <c r="D29" s="13">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
-        <v>6</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="13">
-        <v>2</v>
-      </c>
+      <c r="A30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="13"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>6</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>22</v>
+        <v>59</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>18</v>
       </c>
       <c r="D31" s="13">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2637,84 +2747,86 @@
         <v>6</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="D32" s="13">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>6</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>42</v>
+      <c r="B33" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="68" t="s">
+        <v>19</v>
       </c>
       <c r="D33" s="13">
-        <v>4</v>
-      </c>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
-        <v>7</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="B34" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="73" t="s">
+        <v>38</v>
       </c>
       <c r="D34" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>105</v>
+        <v>61</v>
+      </c>
+      <c r="C35" s="68" t="s">
+        <v>19</v>
       </c>
       <c r="D35" s="13">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
+        <v>6</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="13">
+        <v>4</v>
+      </c>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
         <v>7</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36" s="13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" s="35" t="s">
-        <v>15</v>
+      <c r="B37" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="D37" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2722,13 +2834,13 @@
         <v>7</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D38" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2736,92 +2848,81 @@
         <v>7</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D39" s="13">
-        <v>2.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
-        <v>7</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>105</v>
+      <c r="A40" s="11"/>
+      <c r="B40" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="66" t="s">
+        <v>12</v>
       </c>
       <c r="D40" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D41" s="13">
-        <v>2</v>
-      </c>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="33" t="s">
-        <v>21</v>
+        <v>67</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="D42" s="13">
-        <v>50</v>
-      </c>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D43" s="13">
         <v>2</v>
       </c>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>105</v>
+        <v>17</v>
       </c>
       <c r="D44" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="48"/>
       <c r="F44" s="48"/>
@@ -2829,16 +2930,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>15</v>
+        <v>70</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>18</v>
       </c>
       <c r="D45" s="13">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E45" s="48"/>
       <c r="F45" s="48"/>
@@ -2846,13 +2947,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D46" s="13">
         <v>2</v>
@@ -2863,50 +2964,52 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="51" t="s">
-        <v>105</v>
+        <v>72</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="D47" s="13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E47" s="48"/>
       <c r="F47" s="48"/>
       <c r="G47" s="48"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
+        <v>9</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="13">
         <v>10</v>
       </c>
-      <c r="B48" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" s="13">
-        <v>2</v>
-      </c>
       <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
+      <c r="F48" s="75" t="s">
+        <v>132</v>
+      </c>
       <c r="G48" s="48"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D49" s="13">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E49" s="48"/>
       <c r="F49" s="48"/>
@@ -2914,16 +3017,16 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>20</v>
+        <v>74</v>
+      </c>
+      <c r="C50" s="51" t="s">
+        <v>94</v>
       </c>
       <c r="D50" s="13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E50" s="48"/>
       <c r="F50" s="48"/>
@@ -2931,333 +3034,323 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="D51" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E51" s="48"/>
       <c r="F51" s="48"/>
       <c r="G51" s="48"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>11</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="C52" s="68" t="s">
+        <v>19</v>
       </c>
       <c r="D52" s="13">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E52" s="48"/>
-      <c r="F52" s="48"/>
+      <c r="F52" s="75" t="s">
+        <v>132</v>
+      </c>
       <c r="G52" s="48"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="22">
-        <v>12</v>
-      </c>
-      <c r="B53" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" s="13"/>
+      <c r="A53" s="11">
+        <v>11</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="13">
+        <v>2</v>
+      </c>
       <c r="E53" s="48"/>
       <c r="F53" s="48"/>
       <c r="G53" s="48"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
-        <v>12</v>
-      </c>
-      <c r="B54" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="73" t="s">
+        <v>38</v>
       </c>
       <c r="D54" s="13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E54" s="48"/>
       <c r="F54" s="48"/>
       <c r="G54" s="48"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="22">
-        <v>13</v>
-      </c>
-      <c r="B55" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="23" t="s">
-        <v>20</v>
+    <row r="55" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="11">
+        <v>11</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="65" t="s">
+        <v>12</v>
       </c>
       <c r="D55" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E55" s="48"/>
-      <c r="F55" s="48"/>
+      <c r="F55" s="75" t="s">
+        <v>132</v>
+      </c>
       <c r="G55" s="48"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="22">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="13">
-        <v>20</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="13"/>
       <c r="E56" s="48"/>
       <c r="F56" s="48"/>
       <c r="G56" s="48"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="22">
-        <v>13</v>
+      <c r="A57" s="11">
+        <v>12</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>42</v>
+        <v>80</v>
+      </c>
+      <c r="C57" s="65" t="s">
+        <v>12</v>
       </c>
       <c r="D57" s="13">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E57" s="48"/>
       <c r="F57" s="48"/>
       <c r="G57" s="48"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="11">
-        <v>14</v>
+      <c r="A58" s="22">
+        <v>13</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D58" s="13">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E58" s="48"/>
       <c r="F58" s="48"/>
       <c r="G58" s="48"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="11">
+    <row r="59" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="22">
+        <v>13</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="13">
+        <v>20</v>
+      </c>
+      <c r="E59" s="48"/>
+      <c r="F59" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="G59" s="48"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="22">
+        <v>13</v>
+      </c>
+      <c r="B60" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C60" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" s="13">
+        <v>4</v>
+      </c>
+      <c r="E60" s="48"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="48"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="11">
         <v>14</v>
       </c>
-      <c r="B59" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D59" s="13">
+      <c r="B61" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61" s="13">
+        <v>10</v>
+      </c>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+    </row>
+    <row r="62" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="11">
+        <v>14</v>
+      </c>
+      <c r="B62" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" s="13">
         <v>2</v>
-      </c>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-    </row>
-    <row r="60" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="11">
-        <v>15</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D60" s="13">
-        <v>20</v>
-      </c>
-      <c r="E60" s="49"/>
-      <c r="F60" s="49"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="17"/>
-    </row>
-    <row r="61" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="11">
-        <v>15</v>
-      </c>
-      <c r="B61" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D61" s="13">
-        <v>5</v>
-      </c>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="11">
-        <v>15</v>
-      </c>
-      <c r="B62" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D62" s="13">
-        <v>5</v>
       </c>
       <c r="E62" s="48"/>
       <c r="F62" s="48"/>
       <c r="G62" s="48"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="17"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H62" s="7"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="17"/>
+    </row>
+    <row r="63" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>15</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C63" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" s="13">
         <v>20</v>
       </c>
-      <c r="D63" s="13">
-        <v>5</v>
-      </c>
-      <c r="E63" s="48"/>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
-        <v>17</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" s="33" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="74" t="s">
+        <v>38</v>
       </c>
       <c r="D64" s="13">
-        <v>50</v>
-      </c>
-      <c r="E64" s="48"/>
-      <c r="F64" s="48"/>
-      <c r="G64" s="48"/>
+        <v>5</v>
+      </c>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>17</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="D65" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E65" s="48"/>
       <c r="F65" s="48"/>
       <c r="G65" s="48"/>
     </row>
-    <row r="66" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
+        <v>15</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B66" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>20</v>
-      </c>
       <c r="D66" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E66" s="48"/>
       <c r="F66" s="48"/>
       <c r="G66" s="48"/>
-      <c r="H66" s="7"/>
-      <c r="L66" s="7"/>
-      <c r="M66" s="7"/>
-      <c r="N66" s="7"/>
-      <c r="O66" s="7"/>
-      <c r="P66" s="7"/>
-      <c r="Q66" s="7"/>
-      <c r="R66" s="7"/>
-      <c r="S66" s="7"/>
-      <c r="T66" s="7"/>
-      <c r="U66" s="7"/>
-      <c r="V66" s="7"/>
-    </row>
-    <row r="67" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
+        <v>17</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B67" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="D67" s="13">
-        <v>10</v>
-      </c>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="47"/>
-      <c r="H67" s="7"/>
-      <c r="L67" s="7"/>
-      <c r="M67" s="7"/>
-      <c r="N67" s="7"/>
-      <c r="O67" s="7"/>
-      <c r="P67" s="7"/>
-      <c r="Q67" s="7"/>
-      <c r="R67" s="7"/>
-      <c r="S67" s="7"/>
-      <c r="T67" s="7"/>
-      <c r="U67" s="7"/>
-      <c r="V67" s="7"/>
+        <v>50</v>
+      </c>
+      <c r="E67" s="48"/>
+      <c r="F67" s="48"/>
+      <c r="G67" s="48"/>
     </row>
     <row r="68" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
+      <c r="A68" s="11">
+        <v>17</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" s="13">
+        <v>2</v>
+      </c>
+      <c r="E68" s="48"/>
+      <c r="F68" s="48"/>
+      <c r="G68" s="48"/>
       <c r="H68" s="7"/>
       <c r="L68" s="7"/>
       <c r="M68" s="7"/>
@@ -3272,13 +3365,21 @@
       <c r="V68" s="7"/>
     </row>
     <row r="69" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="11"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
+      <c r="A69" s="11">
+        <v>17</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="13">
+        <v>1</v>
+      </c>
+      <c r="E69" s="48"/>
+      <c r="F69" s="48"/>
+      <c r="G69" s="48"/>
       <c r="H69" s="7"/>
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
@@ -3293,10 +3394,18 @@
       <c r="V69" s="7"/>
     </row>
     <row r="70" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="13"/>
+      <c r="A70" s="11">
+        <v>18</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D70" s="13">
+        <v>10</v>
+      </c>
       <c r="E70" s="47"/>
       <c r="F70" s="47"/>
       <c r="G70" s="47"/>
@@ -3360,9 +3469,9 @@
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="50"/>
-      <c r="G73" s="50"/>
+      <c r="E73" s="47"/>
+      <c r="F73" s="47"/>
+      <c r="G73" s="47"/>
       <c r="H73" s="7"/>
       <c r="L73" s="7"/>
       <c r="M73" s="7"/>
@@ -3381,9 +3490,9 @@
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
-      <c r="E74" s="50"/>
-      <c r="F74" s="50"/>
-      <c r="G74" s="50"/>
+      <c r="E74" s="47"/>
+      <c r="F74" s="47"/>
+      <c r="G74" s="47"/>
       <c r="H74" s="7"/>
       <c r="L74" s="7"/>
       <c r="M74" s="7"/>
@@ -3402,9 +3511,9 @@
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
-      <c r="E75" s="50"/>
-      <c r="F75" s="50"/>
-      <c r="G75" s="50"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
       <c r="H75" s="7"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
@@ -3423,9 +3532,9 @@
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
+      <c r="E76" s="50"/>
+      <c r="F76" s="50"/>
+      <c r="G76" s="50"/>
       <c r="H76" s="7"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
@@ -3444,12 +3553,10 @@
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
-      <c r="E77" s="47"/>
-      <c r="F77" s="47"/>
-      <c r="G77" s="47"/>
+      <c r="E77" s="50"/>
+      <c r="F77" s="50"/>
+      <c r="G77" s="50"/>
       <c r="H77" s="7"/>
-      <c r="I77" s="7"/>
-      <c r="J77" s="7"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
@@ -3467,9 +3574,9 @@
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
-      <c r="E78" s="47"/>
-      <c r="F78" s="47"/>
-      <c r="G78" s="47"/>
+      <c r="E78" s="50"/>
+      <c r="F78" s="50"/>
+      <c r="G78" s="50"/>
       <c r="H78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="7"/>
@@ -3515,8 +3622,6 @@
       <c r="F80" s="47"/>
       <c r="G80" s="47"/>
       <c r="H80" s="7"/>
-      <c r="I80" s="7"/>
-      <c r="J80" s="7"/>
       <c r="L80" s="7"/>
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
@@ -3676,6 +3781,8 @@
       <c r="F87" s="47"/>
       <c r="G87" s="47"/>
       <c r="H87" s="7"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
       <c r="L87" s="7"/>
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
@@ -3688,9 +3795,59 @@
       <c r="U87" s="7"/>
       <c r="V87" s="7"/>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A88" s="24"/>
-      <c r="B88" s="25"/>
+    <row r="88" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="11"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="47"/>
+      <c r="F88" s="47"/>
+      <c r="G88" s="47"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7"/>
+      <c r="J88" s="7"/>
+      <c r="L88" s="7"/>
+      <c r="M88" s="7"/>
+      <c r="N88" s="7"/>
+      <c r="O88" s="7"/>
+      <c r="P88" s="7"/>
+      <c r="Q88" s="7"/>
+      <c r="R88" s="7"/>
+      <c r="S88" s="7"/>
+      <c r="T88" s="7"/>
+      <c r="U88" s="7"/>
+      <c r="V88" s="7"/>
+    </row>
+    <row r="89" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="11"/>
+      <c r="B89" s="12"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="47"/>
+      <c r="F89" s="47"/>
+      <c r="G89" s="47"/>
+      <c r="H89" s="7"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="7"/>
+      <c r="N89" s="7"/>
+      <c r="O89" s="7"/>
+      <c r="P89" s="7"/>
+      <c r="Q89" s="7"/>
+      <c r="R89" s="7"/>
+      <c r="S89" s="7"/>
+      <c r="T89" s="7"/>
+      <c r="U89" s="7"/>
+      <c r="V89" s="7"/>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A90" s="11"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="13"/>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A91" s="24"/>
+      <c r="B91" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
work on wk3 and 4
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158CA5E7-EDD7-449D-94A2-FFD5012A9991}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="5" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$D$90</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="142">
   <si>
     <t>Finals Week</t>
   </si>
@@ -61,10 +62,6 @@
   </si>
   <si>
     <t>Assignments</t>
-  </si>
-  <si>
-    <t>Preparing your data for analysis
-Recoding, data editing and transformations</t>
   </si>
   <si>
     <t>Writing about empirical research
@@ -124,9 +121,6 @@
   </si>
   <si>
     <t>Labor day - Campus closed</t>
-  </si>
-  <si>
-    <t>Exploring bivariate relationships</t>
   </si>
   <si>
     <t>Probability &amp; Confidence Intervals
@@ -367,15 +361,6 @@
 New communication tools (hack, slack)</t>
   </si>
   <si>
-    <t xml:space="preserve">**Prepare** - Install R, R Studio and LaTeX software before Wednesday [[Walkthrough]](https://norcalbiostat.netlify.com/post/software-overview/) (LaTeX can be postponed until next week)
-**Prepare** - Watch the R Markdown [Tutorial](http://rmarkdown.rstudio.com/lesson-1.html)
-**Prepare** - Create a `MATH315` folder on your computer in an easy to find spot. Create subfolders for `hw`, `project`
-Form support groups
-Learn how to use Rstudio to do and turn in homework (test markdownfile, hw1 template)
-Write down questions about class logistics and structure [[Google Form]](https://goo.gl/forms/T1aDys2sFeLlsk2A3)
-</t>
-  </si>
-  <si>
     <t>rubric</t>
   </si>
   <si>
@@ -383,11 +368,6 @@
   </si>
   <si>
     <t>assign</t>
-  </si>
-  <si>
-    <t>**Prepare** - Watch PDS Video 4
-**Prepare** - Read: How to read a journal article
-**Prepare** - Read: Lecture notes on literature reviews</t>
   </si>
   <si>
     <t>**Prepare** - Watch [[PDS video 1]](http://passiondrivenstatistics.com/2015/05/20/chapter-01-course-introduction/) (6 min)
@@ -422,9 +402,6 @@
     <t>PR Personal Codebook</t>
   </si>
   <si>
-    <t>Campus Closed</t>
-  </si>
-  <si>
     <t xml:space="preserve">No School
 Categorical Predictors
 Log and logit transformations </t>
@@ -441,31 +418,6 @@
   </si>
   <si>
     <t>Model building</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Problem set (PS) 2.2 (Due Sun 9/9 )
-Data Camp Open Intro - Intro to R **AND**  Intro to Data [BBL] (Due Sun 9/9 )
-Research question assignment [[HTML]](hw/hw02_research_codebook.html)[[PDF]](hw/hw02_research_codebook.html) (Due Sun 9/9 )
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Peer review of research question (Due Tue 9/11 )</t>
-    </r>
   </si>
   <si>
     <t>No School
@@ -479,10 +431,46 @@
 [Research data](https://drive.google.com/drive/u/3/folders/1jULudBjRbHdW-uLIvmMbxRBEJJkq9crY)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Syllabus](https://norcalbiostat.github.io/MATH615/syllabus_315_f18.html)
-[Passion Driven Statistics](reading/PDS_Intro_Stat.pdf)
-[List of Articles](http://www.norcalbiostat.com/articles/articles.html)
-[PDS video 1](http://passiondrivenstatistics.com/2015/05/20/chapter-01-course-introduction/) </t>
+    <t>hw01 1: Team Formation, Reading, project data</t>
+  </si>
+  <si>
+    <t>hw02 Personal Codebook/RQ</t>
+  </si>
+  <si>
+    <t>hw03 Citation Assignment</t>
+  </si>
+  <si>
+    <t>PR citation assignment</t>
+  </si>
+  <si>
+    <t>PR DM steps</t>
+  </si>
+  <si>
+    <t>Research Proposal</t>
+  </si>
+  <si>
+    <t>hw04 DM steps preparation</t>
+  </si>
+  <si>
+    <t>hw05  DM assignment</t>
+  </si>
+  <si>
+    <t>Peer review Research Proposal</t>
+  </si>
+  <si>
+    <t>Ready to be used, % based</t>
+  </si>
+  <si>
+    <t>in used, % based</t>
+  </si>
+  <si>
+    <t>Campus closed</t>
+  </si>
+  <si>
+    <t>Problem set (PS) 2.2 (Due Sun 9/9 )
+Data Camp Open Intro - Intro to R **AND**  Intro to Data [BBL] (Due Sun 9/9 )
+hw02 Research question and codebook assignment [[HTML]](hw/hw02_research_codebook.html)[[PDF]](hw/hw02_research_codebook.html) (Due Sun 9/9 )
+Peer review of research question (Due Tue 9/11 )</t>
   </si>
   <si>
     <r>
@@ -498,7 +486,7 @@
 [Data Camp](https://www.datacamp.com/users/sign_in) Intro to R - Intro to Basics Chapter [BBL] (Due Sun 9/2 )
 [Metacognition Awareness Inventory](https://www.datacamp.com/users/sign_in)  [BBL] (Due Sun 9/2 )
 R Markdown test file (Due Wed 8/29 )
-HW 1 [[RMD]](hw/hw01_template.Rmd)(Due Sun 9/2 )</t>
+hw01 Introductions [[HTML]](hw/hw01_introductions.html)[[PDF]](hw/hw01_introductions.pdf)(Due Sun 9/2 )</t>
     </r>
     <r>
       <rPr>
@@ -512,46 +500,102 @@
     </r>
   </si>
   <si>
-    <t>hw01 1: Team Formation, Reading, project data</t>
-  </si>
-  <si>
-    <t>hw02 Personal Codebook/RQ</t>
-  </si>
-  <si>
-    <t>hw03 Citation Assignment</t>
-  </si>
-  <si>
-    <t>PR citation assignment</t>
-  </si>
-  <si>
-    <t>PR DM steps</t>
-  </si>
-  <si>
-    <t>Research Proposal</t>
-  </si>
-  <si>
-    <t>hw04 DM steps preparation</t>
-  </si>
-  <si>
-    <t>hw05  DM assignment</t>
-  </si>
-  <si>
-    <t>Peer review Research Proposal</t>
-  </si>
-  <si>
-    <t>Ready to be used, % based</t>
+    <t>Watch PDS Video 4 &amp; 6
+Reading:
+* How to read a journal article
+* Lecture notes on literature reviews
+* Citation assignment
+* Course notes section 2.2, 2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refining your research question
+Describing univariate numerical data
+Describing univariate categorical data
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Prepare** Watch PDS Video 6
+The PDS video uses an R script instead of a RMD file. That's OK. I want you to use a Rmarkdown file. 
+We will discuss how to summarize categorical data using tables, charts and words. 
+We will be working through the course packet section 2.3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAT on Univariate numerical data (CN 2.2)
+Discuss how to summarize numerical data using summary statistics, plots and words. 
+We will be working through the course packet section 2.2 </t>
+  </si>
+  <si>
+    <t>**Prepare** - Watch PDS Video 4
+**Prepare** - Read: How to read a journal article, lecture notes on literature reviews, citation assignment. 
+Learn more about your topic area by conducting a literature review. 
+What is already known, what questions have not yet been explored? 
+The idea is to find an area where you can contribute to new research. 
+You will learn how to conduct a literature review without burning yourself out or getting lost</t>
+  </si>
+  <si>
+    <t>[PDS Video 4](http://passiondrivenstatistics.com/2015/09/16/chapter-04/)
+[PDS Video 6](http://passiondrivenstatistics.com/2015/12/18/r-chapter-6/)
+Course notes Section 2.2, 2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hw03 Citation Assignment [[HTML]](hw/hw03_citation.html) [[PDF]](hw/hw03_citation.pdf) (Due Sun 9/16 )
+PS 2.4, 2.5, 2.7 [BBL] (Due Sun 9/16 )
+Data Camp: Intro to ggplot (Due Sun 9/16)
+</t>
+  </si>
+  <si>
+    <t>Data Management
+Creating visualizations in R
+Open work time</t>
+  </si>
+  <si>
+    <t>[PDS Video 7](http://passiondrivenstatistics.com/2016/01/08/r-chapter-7/)
+Data Visualization Lab from [[Math 130]](https://norcalbiostat.github.io/MATH130/07_graphs.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Prepare** - Install R, R Studio and LaTeX software before Wednesday [[Walkthrough]](https://norcalbiostat.netlify.com/post/software-overview/) 
+**Prepare** - Watch the R Markdown [Tutorial](http://rmarkdown.rstudio.com/lesson-1.html)
+**Prepare** - Read the Applied Stats Course Notes [Chapter 1.0.1](https://norcalbiostat.github.io/AppliedStatistics_notes/data-prep.html) 
+**Prepare** - Create a `MATH315` folder on your computer in an easy to find spot. Create subfolders for `hw`, `project`
+Form support groups
+Learn how to use Rstudio to do and turn in homework (test markdownfile, hw1 template)
+Write down questions about class logistics and structure [[Google Form]](https://goo.gl/forms/T1aDys2sFeLlsk2A3)
+</t>
+  </si>
+  <si>
+    <t>[Syllabus](https://norcalbiostat.github.io/MATH615/syllabus_315_f18.html)
+[Passion Driven Statistics](reading/PDS_Intro_Stat.pdf)
+[List of Articles](http://www.norcalbiostat.com/articles/articles.html)
+[PDS video 1](http://passiondrivenstatistics.com/2015/05/20/chapter-01-course-introduction/) 
+Applied Stats Course Notes [Chapter 1.0.1](https://norcalbiostat.github.io/AppliedStatistics_notes/data-prep.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Install the `ggplot2` package
+Read the Applied Stats Course Notes [Chapter 1](https://norcalbiostat.github.io/AppliedStatistics_notes/data-prep.html) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">More often than not you will have to do some level of data transformation or cleaning before you can conduct an analysis.
+We will walk through the material in the AS course notes 1.2-1.6 during class. 
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -658,8 +702,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -756,6 +807,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -806,123 +863,123 @@
   </borders>
   <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="77" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="77" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="77" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="78" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="78" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="81" applyFont="1" applyAlignment="1">
@@ -934,34 +991,34 @@
     <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="81" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="7" borderId="4" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="7" borderId="4" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="8" borderId="4" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -970,102 +1027,108 @@
     <xf numFmtId="1" fontId="0" fillId="8" borderId="4" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="9" borderId="4" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="77" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="77" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="80" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="80" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="82">
@@ -1146,10 +1209,10 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Normal 3" xfId="80"/>
-    <cellStyle name="Percent 2" xfId="52"/>
-    <cellStyle name="Percent 3" xfId="81"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Percent 3" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
     <cellStyle name="Total" xfId="78" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1486,11 +1549,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,19 +1590,19 @@
         <v>6</v>
       </c>
       <c r="G1" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>25</v>
-      </c>
-      <c r="I1" s="37" t="s">
-        <v>26</v>
       </c>
       <c r="J1" s="36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="405" x14ac:dyDescent="0.25">
       <c r="A2" s="39">
         <v>1</v>
       </c>
@@ -1547,28 +1610,28 @@
         <v>41877</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -1580,31 +1643,31 @@
         <v>41884</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>114</v>
+      </c>
+      <c r="G3" s="77" t="s">
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J3" s="55" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="39">
         <v>3</v>
       </c>
@@ -1613,19 +1676,29 @@
         <v>41891</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
         <v>4</v>
       </c>
@@ -1634,12 +1707,18 @@
         <v>41898</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1"/>
+      <c r="E5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
@@ -1653,7 +1732,7 @@
         <v>41905</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1672,7 +1751,7 @@
         <v>41912</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1691,7 +1770,7 @@
         <v>41919</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1710,7 +1789,7 @@
         <v>41926</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1729,7 +1808,7 @@
         <v>41933</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1748,7 +1827,7 @@
         <v>41940</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1767,7 +1846,7 @@
         <v>41947</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1786,13 +1865,13 @@
         <v>41954</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="1" t="s">
-        <v>113</v>
+      <c r="G13" s="77" t="s">
+        <v>126</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1822,7 +1901,7 @@
         <v>41968</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1841,7 +1920,7 @@
         <v>41975</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1860,7 +1939,7 @@
         <v>41982</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1894,11 +1973,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1919,61 +1998,61 @@
   <sheetData>
     <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="N1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="27" t="s">
+      <c r="P1" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="R1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="27" t="s">
+      <c r="T1" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="V1" s="31" t="s">
         <v>14</v>
-      </c>
-      <c r="R1" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" s="31" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1981,16 +2060,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" s="13">
         <v>10</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I2" s="8">
         <f>SUMIF($C$2:$C$82,H2,$D$2:$D$82)</f>
@@ -2001,7 +2080,7 @@
         <v>8.6065573770491802E-2</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M2" s="9">
         <v>16</v>
@@ -2010,7 +2089,7 @@
         <v>3.9506172839506172E-2</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q2" s="26">
         <v>20</v>
@@ -2019,7 +2098,7 @@
         <v>4.3956043956043959E-2</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U2" s="10">
         <v>14</v>
@@ -2033,10 +2112,10 @@
         <v>1.3</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="13">
         <v>3</v>
@@ -2045,10 +2124,10 @@
         <v>41883</v>
       </c>
       <c r="G3" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="H3" s="71" t="s">
-        <v>12</v>
+        <v>101</v>
+      </c>
+      <c r="H3" s="66" t="s">
+        <v>11</v>
       </c>
       <c r="I3" s="8">
         <f>SUMIF($C$2:$C$82,H3,$D$2:$D$82)</f>
@@ -2059,7 +2138,7 @@
         <v>0.10655737704918032</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M3" s="9">
         <v>36</v>
@@ -2068,7 +2147,7 @@
         <v>8.8888888888888892E-2</v>
       </c>
       <c r="P3" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="26">
         <v>100</v>
@@ -2077,7 +2156,7 @@
         <v>0.21978021978021978</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="U3" s="10">
         <v>99</v>
@@ -2091,10 +2170,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="65" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>11</v>
       </c>
       <c r="D4" s="13">
         <v>2</v>
@@ -2103,10 +2182,10 @@
         <v>41879</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I4" s="8">
         <f>SUMIF($C$2:$C$82,H4,$D$2:$D$82)</f>
@@ -2117,7 +2196,7 @@
         <v>0.13114754098360656</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M4" s="9">
         <v>40</v>
@@ -2126,7 +2205,7 @@
         <v>9.8765432098765427E-2</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="26">
         <v>25</v>
@@ -2135,7 +2214,7 @@
         <v>5.4945054945054944E-2</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U4" s="10">
         <v>20</v>
@@ -2149,10 +2228,10 @@
         <v>1.2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="13">
         <v>1</v>
@@ -2161,11 +2240,11 @@
         <v>41881</v>
       </c>
       <c r="G5" s="53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J5" s="14"/>
       <c r="L5" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M5" s="9">
         <v>26</v>
@@ -2174,7 +2253,7 @@
         <v>6.4197530864197536E-2</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q5" s="26">
         <v>10</v>
@@ -2183,7 +2262,7 @@
         <v>2.197802197802198E-2</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="U5" s="10">
         <v>32</v>
@@ -2197,10 +2276,10 @@
         <v>1.4</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="19">
         <v>1</v>
@@ -2209,10 +2288,10 @@
         <v>41883</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="8">
         <f>SUMIF($C$2:$C$82,H6,$D$2:$D$82)</f>
@@ -2223,7 +2302,7 @@
         <v>6.1475409836065573E-2</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M6" s="9">
         <v>27</v>
@@ -2232,7 +2311,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q6" s="26">
         <v>150</v>
@@ -2241,7 +2320,7 @@
         <v>0.32967032967032966</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U6" s="10">
         <v>10</v>
@@ -2254,11 +2333,11 @@
       <c r="A7" s="11">
         <v>1.5</v>
       </c>
-      <c r="B7" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="65" t="s">
-        <v>12</v>
+      <c r="B7" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>11</v>
       </c>
       <c r="D7" s="13">
         <v>5</v>
@@ -2267,10 +2346,10 @@
         <v>41883</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="8">
         <f>SUMIF($C$2:$C$82,H7,$D$2:$D$82)</f>
@@ -2281,7 +2360,7 @@
         <v>0.30737704918032788</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M7" s="9">
         <v>150</v>
@@ -2290,7 +2369,7 @@
         <v>0.37037037037037035</v>
       </c>
       <c r="P7" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q7" s="30">
         <v>150</v>
@@ -2299,7 +2378,7 @@
         <v>0.32967032967032966</v>
       </c>
       <c r="T7" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U7" s="10">
         <v>175</v>
@@ -2313,10 +2392,10 @@
         <v>1.6</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" s="21">
         <v>2.5</v>
@@ -2325,10 +2404,10 @@
         <v>41883</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="70" t="s">
-        <v>19</v>
+        <v>101</v>
+      </c>
+      <c r="H8" s="65" t="s">
+        <v>18</v>
       </c>
       <c r="I8" s="8">
         <f>SUMIF($C$2:$C$82,H8,$D$2:$D$82)</f>
@@ -2339,7 +2418,7 @@
         <v>0.30737704918032788</v>
       </c>
       <c r="L8" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M8" s="27">
         <v>110</v>
@@ -2353,7 +2432,7 @@
       </c>
       <c r="R8" s="17"/>
       <c r="T8" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U8" s="31">
         <v>105</v>
@@ -2367,10 +2446,10 @@
         <v>2.1</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="13">
         <v>2</v>
@@ -2379,7 +2458,7 @@
         <v>41886</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I9" s="6">
         <f>SUM(I2:I8)</f>
@@ -2399,10 +2478,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D10" s="13">
         <v>1</v>
@@ -2411,7 +2490,7 @@
         <v>41890</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -2419,10 +2498,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D11" s="13">
         <v>5</v>
@@ -2431,7 +2510,7 @@
         <v>41890</v>
       </c>
       <c r="G11" s="53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -2439,10 +2518,10 @@
         <v>2.4</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D12" s="13">
         <v>3</v>
@@ -2451,18 +2530,18 @@
         <v>41890</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>2.5</v>
       </c>
-      <c r="B13" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="C13" s="69" t="s">
-        <v>19</v>
+      <c r="B13" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="64" t="s">
+        <v>18</v>
       </c>
       <c r="D13" s="13">
         <v>10</v>
@@ -2470,11 +2549,11 @@
       <c r="E13" s="47">
         <v>41890</v>
       </c>
-      <c r="F13" s="75" t="s">
-        <v>132</v>
+      <c r="F13" s="70" t="s">
+        <v>125</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2482,10 +2561,10 @@
         <v>2.6</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="72" t="s">
-        <v>38</v>
+        <v>108</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>36</v>
       </c>
       <c r="D14" s="21">
         <v>4</v>
@@ -2494,108 +2573,111 @@
         <v>41892</v>
       </c>
       <c r="G14" s="53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>3</v>
       </c>
-      <c r="B15" s="64" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="69" t="s">
-        <v>19</v>
+      <c r="B15" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="64" t="s">
+        <v>18</v>
       </c>
       <c r="D15" s="13">
         <v>10</v>
       </c>
-      <c r="H15" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="56"/>
+      <c r="G15" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="71"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>3</v>
       </c>
-      <c r="B16" s="61" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="63" t="s">
-        <v>38</v>
+      <c r="B16" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>36</v>
       </c>
       <c r="D16" s="13">
         <v>4</v>
       </c>
-      <c r="H16" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="57"/>
+      <c r="H16" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="72"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>3</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="13">
         <v>2</v>
       </c>
-      <c r="H17" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="58"/>
+      <c r="H17" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="73"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>3</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D18" s="13">
         <v>2</v>
       </c>
-      <c r="H18" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="59"/>
+      <c r="H18" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="74"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>3</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D19" s="13">
         <v>2</v>
       </c>
-      <c r="H19" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="60"/>
+      <c r="H19" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="75"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>3</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D20" s="13">
         <v>1</v>
@@ -2605,11 +2687,11 @@
       <c r="A21" s="11">
         <v>4</v>
       </c>
-      <c r="B21" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="C21" s="62" t="s">
-        <v>19</v>
+      <c r="B21" s="59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>18</v>
       </c>
       <c r="D21" s="13">
         <v>10</v>
@@ -2619,11 +2701,11 @@
       <c r="A22" s="11">
         <v>4</v>
       </c>
-      <c r="B22" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" s="63" t="s">
-        <v>38</v>
+      <c r="B22" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="58" t="s">
+        <v>36</v>
       </c>
       <c r="D22" s="13">
         <v>4</v>
@@ -2634,10 +2716,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="13">
         <v>2</v>
@@ -2647,11 +2729,11 @@
       <c r="A24" s="11">
         <v>4</v>
       </c>
-      <c r="B24" s="64" t="s">
-        <v>130</v>
-      </c>
-      <c r="C24" s="62" t="s">
-        <v>19</v>
+      <c r="B24" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>18</v>
       </c>
       <c r="D24" s="13">
         <v>10</v>
@@ -2662,21 +2744,21 @@
         <v>4</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="65" t="s">
-        <v>12</v>
+        <v>54</v>
+      </c>
+      <c r="C25" s="60" t="s">
+        <v>11</v>
       </c>
       <c r="D25" s="13">
         <v>5</v>
       </c>
-      <c r="F25" s="75" t="s">
-        <v>132</v>
+      <c r="F25" s="70" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
-      <c r="B26" s="61"/>
+      <c r="B26" s="56"/>
       <c r="C26" s="23"/>
       <c r="D26" s="13"/>
     </row>
@@ -2685,10 +2767,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D27" s="13">
         <v>2</v>
@@ -2699,10 +2781,10 @@
         <v>5</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D28" s="13">
         <v>2</v>
@@ -2713,10 +2795,10 @@
         <v>5</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="65" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="C29" s="60" t="s">
+        <v>11</v>
       </c>
       <c r="D29" s="13">
         <v>5</v>
@@ -2733,10 +2815,10 @@
         <v>6</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" s="13">
         <v>50</v>
@@ -2747,10 +2829,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" s="13">
         <v>2</v>
@@ -2760,11 +2842,11 @@
       <c r="A33" s="11">
         <v>6</v>
       </c>
-      <c r="B33" s="61" t="s">
-        <v>128</v>
-      </c>
-      <c r="C33" s="68" t="s">
-        <v>19</v>
+      <c r="B33" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="63" t="s">
+        <v>18</v>
       </c>
       <c r="D33" s="13">
         <v>20</v>
@@ -2774,11 +2856,11 @@
       <c r="A34" s="11">
         <v>6</v>
       </c>
-      <c r="B34" s="61" t="s">
-        <v>131</v>
-      </c>
-      <c r="C34" s="73" t="s">
-        <v>38</v>
+      <c r="B34" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="68" t="s">
+        <v>36</v>
       </c>
       <c r="D34" s="13">
         <v>5</v>
@@ -2789,10 +2871,10 @@
         <v>6</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="68" t="s">
-        <v>19</v>
+        <v>59</v>
+      </c>
+      <c r="C35" s="63" t="s">
+        <v>18</v>
       </c>
       <c r="D35" s="13">
         <v>20</v>
@@ -2803,10 +2885,10 @@
         <v>6</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="73" t="s">
-        <v>38</v>
+        <v>60</v>
+      </c>
+      <c r="C36" s="68" t="s">
+        <v>36</v>
       </c>
       <c r="D36" s="13">
         <v>4</v>
@@ -2820,10 +2902,10 @@
         <v>7</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" s="13">
         <v>2</v>
@@ -2834,10 +2916,10 @@
         <v>7</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D38" s="13">
         <v>2</v>
@@ -2848,10 +2930,10 @@
         <v>7</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D39" s="13">
         <v>5</v>
@@ -2860,10 +2942,10 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="66" t="s">
-        <v>12</v>
+        <v>94</v>
+      </c>
+      <c r="C40" s="61" t="s">
+        <v>11</v>
       </c>
       <c r="D40" s="13">
         <v>5</v>
@@ -2874,10 +2956,10 @@
         <v>7</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D41" s="13">
         <v>1</v>
@@ -2888,10 +2970,10 @@
         <v>7</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D42" s="13">
         <v>2.5</v>
@@ -2902,10 +2984,10 @@
         <v>7</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D43" s="13">
         <v>2</v>
@@ -2916,10 +2998,10 @@
         <v>8</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D44" s="13">
         <v>2</v>
@@ -2933,10 +3015,10 @@
         <v>8</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" s="13">
         <v>50</v>
@@ -2950,10 +3032,10 @@
         <v>9</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D46" s="13">
         <v>2</v>
@@ -2967,10 +3049,10 @@
         <v>9</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D47" s="13">
         <v>1</v>
@@ -2984,17 +3066,17 @@
         <v>9</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="65" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="C48" s="60" t="s">
+        <v>11</v>
       </c>
       <c r="D48" s="13">
         <v>10</v>
       </c>
       <c r="E48" s="48"/>
-      <c r="F48" s="75" t="s">
-        <v>132</v>
+      <c r="F48" s="70" t="s">
+        <v>124</v>
       </c>
       <c r="G48" s="48"/>
     </row>
@@ -3003,10 +3085,10 @@
         <v>10</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D49" s="13">
         <v>2</v>
@@ -3020,10 +3102,10 @@
         <v>10</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C50" s="51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D50" s="13">
         <v>6</v>
@@ -3037,10 +3119,10 @@
         <v>10</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D51" s="13">
         <v>2</v>
@@ -3054,17 +3136,17 @@
         <v>11</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C52" s="68" t="s">
-        <v>19</v>
+        <v>74</v>
+      </c>
+      <c r="C52" s="63" t="s">
+        <v>18</v>
       </c>
       <c r="D52" s="13">
         <v>20</v>
       </c>
       <c r="E52" s="48"/>
-      <c r="F52" s="75" t="s">
-        <v>132</v>
+      <c r="F52" s="70" t="s">
+        <v>124</v>
       </c>
       <c r="G52" s="48"/>
     </row>
@@ -3073,10 +3155,10 @@
         <v>11</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D53" s="13">
         <v>2</v>
@@ -3090,10 +3172,10 @@
         <v>11</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="73" t="s">
-        <v>38</v>
+        <v>93</v>
+      </c>
+      <c r="C54" s="68" t="s">
+        <v>36</v>
       </c>
       <c r="D54" s="13">
         <v>4</v>
@@ -3107,17 +3189,17 @@
         <v>11</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C55" s="65" t="s">
-        <v>12</v>
+        <v>76</v>
+      </c>
+      <c r="C55" s="60" t="s">
+        <v>11</v>
       </c>
       <c r="D55" s="13">
         <v>10</v>
       </c>
       <c r="E55" s="48"/>
-      <c r="F55" s="75" t="s">
-        <v>132</v>
+      <c r="F55" s="70" t="s">
+        <v>124</v>
       </c>
       <c r="G55" s="48"/>
     </row>
@@ -3126,10 +3208,10 @@
         <v>12</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D56" s="13"/>
       <c r="E56" s="48"/>
@@ -3141,10 +3223,10 @@
         <v>12</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C57" s="65" t="s">
-        <v>12</v>
+        <v>78</v>
+      </c>
+      <c r="C57" s="60" t="s">
+        <v>11</v>
       </c>
       <c r="D57" s="13">
         <v>10</v>
@@ -3158,10 +3240,10 @@
         <v>13</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D58" s="13">
         <v>2</v>
@@ -3175,17 +3257,17 @@
         <v>13</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C59" s="68" t="s">
-        <v>19</v>
+        <v>80</v>
+      </c>
+      <c r="C59" s="63" t="s">
+        <v>18</v>
       </c>
       <c r="D59" s="13">
         <v>20</v>
       </c>
       <c r="E59" s="48"/>
-      <c r="F59" s="75" t="s">
-        <v>132</v>
+      <c r="F59" s="70" t="s">
+        <v>124</v>
       </c>
       <c r="G59" s="48"/>
     </row>
@@ -3194,10 +3276,10 @@
         <v>13</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C60" s="73" t="s">
-        <v>38</v>
+        <v>81</v>
+      </c>
+      <c r="C60" s="68" t="s">
+        <v>36</v>
       </c>
       <c r="D60" s="13">
         <v>4</v>
@@ -3211,10 +3293,10 @@
         <v>14</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C61" s="67" t="s">
-        <v>19</v>
+        <v>82</v>
+      </c>
+      <c r="C61" s="62" t="s">
+        <v>18</v>
       </c>
       <c r="D61" s="13">
         <v>10</v>
@@ -3228,10 +3310,10 @@
         <v>14</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" s="73" t="s">
-        <v>38</v>
+        <v>83</v>
+      </c>
+      <c r="C62" s="68" t="s">
+        <v>36</v>
       </c>
       <c r="D62" s="13">
         <v>2</v>
@@ -3249,10 +3331,10 @@
         <v>15</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" s="67" t="s">
-        <v>19</v>
+        <v>84</v>
+      </c>
+      <c r="C63" s="62" t="s">
+        <v>18</v>
       </c>
       <c r="D63" s="13">
         <v>20</v>
@@ -3269,10 +3351,10 @@
         <v>15</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C64" s="74" t="s">
-        <v>38</v>
+        <v>85</v>
+      </c>
+      <c r="C64" s="69" t="s">
+        <v>36</v>
       </c>
       <c r="D64" s="13">
         <v>5</v>
@@ -3289,10 +3371,10 @@
         <v>15</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D65" s="13">
         <v>5</v>
@@ -3306,10 +3388,10 @@
         <v>15</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D66" s="13">
         <v>5</v>
@@ -3323,10 +3405,10 @@
         <v>17</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D67" s="13">
         <v>50</v>
@@ -3340,10 +3422,10 @@
         <v>17</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D68" s="13">
         <v>2</v>
@@ -3369,10 +3451,10 @@
         <v>17</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D69" s="13">
         <v>1</v>
@@ -3398,10 +3480,10 @@
         <v>18</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D70" s="13">
         <v>10</v>

</xml_diff>

<commit_message>
rebuild up to wk4
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E35164-F3E7-4C77-BE1E-7486EF82B90A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CF1202-A8A3-4A6D-A17D-B09530E438A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="162">
   <si>
     <t>Finals Week</t>
   </si>
@@ -302,11 +302,6 @@
   </si>
   <si>
     <t>Foundations Worksheet</t>
-  </si>
-  <si>
-    <t>Introduction to the class, logistics
-Reproducible research
-Data analysis life cycle</t>
   </si>
   <si>
     <t>Data Camp: Intro to basics</t>
@@ -500,33 +495,6 @@
 * Course packet  section 2.2, 2.3</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Take [this survey](https://goo.gl/forms/qLBv2jMF6fBv3BTR2) to help me set my OH (Due Thu 8/30 )
-Join our [Slack team](http://math-315.slack.com) and post an `#introduction` (instructions in channel) (Due Sun 9/2 )
-[Data Camp](https://www.datacamp.com/users/sign_in) Intro to R - Intro to Basics Chapter [BBL] (Due Sun 9/2 )
-Metacognition Awareness Inventory [BBL] (Due Sun 9/2 )
-R Markdown test file (Due Wed 8/29 )
-hw01 Introductions [[HTML]](hw/hw01_introductions.html)[[PDF]](hw/hw01_introductions.pdf)(Due Sun 9/2 )</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>Problem set 2.2 (Due Sun 9/9 )
 Data Camp Open Intro - Intro to R [BBL] (Due Sun 9/9 )
 Data Camp Open Intro - Intro to Data [BBL] (Due Sun 9/9 )
@@ -611,12 +579,6 @@
     <t xml:space="preserve">We already talked about what visualizations are appropriate to create for different quantitative and categorical variable types last week. 
 Now it's time to build them in R. 
 After a quick recap on how to use ggplot syntax, and where you can find resources you're on your own to work with your team on the Univariate graphing assignment. </t>
-  </si>
-  <si>
-    <t>Readiness Assurance Test (RAT) on class logistics
-Introduction to the semester long project
-Form support groups and analysis pairs - start to discuss what research topics you want to analyze
-* I want all 4 members of a team to be analyzing different research questions from the same data set</t>
   </si>
   <si>
     <t>Introduction to the instructor, class structure, materials, requirements, expectations and resources. 
@@ -718,6 +680,68 @@
     <t xml:space="preserve">Learn how to use RStudio to do and turn in homework (test markdown file, hw1 template)
 Write down questions about class logistics and structure [[Google Form]](https://goo.gl/forms/T1aDys2sFeLlsk2A3)
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to the class, logistics
+Data analysis life cycle
+Reproducible research
+</t>
+  </si>
+  <si>
+    <t>Readiness Assurance Test (RAT) on class logistics
+Introduction to the semester long project
+Form support groups and analysis pairs - start to discuss what research topics you want to analyze
+* I want all 4 members of a group to be analyzing different research questions from the same data set</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Take [this survey](https://goo.gl/forms/qLBv2jMF6fBv3BTR2) to help me set my OH (Due Thu 8/30 )
+Join our [Slack team](http://math-315.slack.com) and post an `#introduction` (instructions in channel) (Due Sun 9/2 )
+[Data Camp](https://www.datacamp.com/users/sign_in) Intro to R - Intro to Basics Chapter [BBL] (Due Thu 9/6 )
+Metacognition Awareness Inventory [BBL] (Due Sun 9/2 )
+R Markdown test file (Due Wed 8/29 )
+hw01 Introductions [[HTML]](hw/hw01_introductions.html)[[PDF]](hw/hw01_introductions.pdf)(Due Sun 9/2 )</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data Management Assignment [[HTML]](hw/hw04_data_management.html] [[PDF]](hw/hw04_data_management.pdf](Due Sun 9/23 )</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Univariate Graphing Assignment (Due Sun 9/23 )</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1291,24 +1315,24 @@
     <xf numFmtId="164" fontId="9" fillId="18" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="82">
     <cellStyle name="20% - Accent6" xfId="79" builtinId="50"/>
@@ -1732,8 +1756,8 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,32 +1814,32 @@
         <v>41877</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="I2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="255" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>2</v>
       </c>
@@ -1824,31 +1848,31 @@
         <v>41884</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G3" s="72" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="J3" s="55" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="270" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="39">
         <v>3</v>
       </c>
@@ -1857,28 +1881,28 @@
         <v>41891</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" s="55" t="s">
         <v>140</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="390" x14ac:dyDescent="0.25">
@@ -1890,28 +1914,28 @@
         <v>41898</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="J5" s="73" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1923,20 +1947,20 @@
         <v>41905</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="73" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1948,22 +1972,22 @@
         <v>41912</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="73" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1975,7 +1999,7 @@
         <v>41919</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1984,7 +2008,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1996,7 +2020,7 @@
         <v>41926</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2005,7 +2029,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="73" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2017,7 +2041,7 @@
         <v>41933</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2036,7 +2060,7 @@
         <v>41940</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2045,7 +2069,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2057,7 +2081,7 @@
         <v>41947</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2066,7 +2090,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="73" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2078,18 +2102,18 @@
         <v>41954</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2116,7 +2140,7 @@
         <v>41968</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -2125,7 +2149,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2137,7 +2161,7 @@
         <v>41975</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -2146,7 +2170,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2158,7 +2182,7 @@
         <v>41982</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2167,7 +2191,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2234,10 +2258,10 @@
         <v>85</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>9</v>
@@ -2345,7 +2369,7 @@
         <v>41879</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3" s="66" t="s">
         <v>8</v>
@@ -2403,7 +2427,7 @@
         <v>41881</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>29</v>
@@ -2461,7 +2485,7 @@
         <v>41883</v>
       </c>
       <c r="G5" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J5" s="14"/>
       <c r="L5" s="9" t="s">
@@ -2509,7 +2533,7 @@
         <v>41883</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>13</v>
@@ -2555,7 +2579,7 @@
         <v>1.5</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="60" t="s">
         <v>8</v>
@@ -2567,7 +2591,7 @@
         <v>41883</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>14</v>
@@ -2613,7 +2637,7 @@
         <v>1.6</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="46" t="s">
         <v>85</v>
@@ -2625,7 +2649,7 @@
         <v>41883</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H8" s="65" t="s">
         <v>15</v>
@@ -2679,7 +2703,7 @@
         <v>41886</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I9" s="6">
         <f>SUM(I2:I8)</f>
@@ -2711,7 +2735,7 @@
         <v>41890</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -2731,7 +2755,7 @@
         <v>41890</v>
       </c>
       <c r="G11" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -2751,7 +2775,7 @@
         <v>41890</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -2759,7 +2783,7 @@
         <v>2.5</v>
       </c>
       <c r="B13" s="59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C13" s="64" t="s">
         <v>15</v>
@@ -2771,10 +2795,10 @@
         <v>41890</v>
       </c>
       <c r="F13" s="70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2782,7 +2806,7 @@
         <v>2.6</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" s="67" t="s">
         <v>29</v>
@@ -2794,7 +2818,7 @@
         <v>41892</v>
       </c>
       <c r="G14" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -2814,12 +2838,12 @@
         <v>41893</v>
       </c>
       <c r="G15" s="75" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="78"/>
+      <c r="I15" s="81"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
@@ -2838,12 +2862,12 @@
         <v>41897</v>
       </c>
       <c r="G16" s="75" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" s="79" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="79"/>
+      <c r="I16" s="82"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
@@ -2862,12 +2886,12 @@
         <v>41897</v>
       </c>
       <c r="G17" s="75" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="80"/>
+      <c r="I17" s="83"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
@@ -2886,19 +2910,19 @@
         <v>41897</v>
       </c>
       <c r="G18" s="75" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" s="81" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="81"/>
+      <c r="I18" s="84"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>3.5</v>
       </c>
       <c r="B19" s="59" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="64" t="s">
         <v>15</v>
@@ -2911,21 +2935,21 @@
       </c>
       <c r="F19" s="77"/>
       <c r="G19" s="71" t="s">
-        <v>92</v>
-      </c>
-      <c r="H19" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="82"/>
+      <c r="I19" s="85"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20">
         <v>3.6</v>
       </c>
-      <c r="B20" s="84" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="85" t="s">
+      <c r="B20" s="79" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="80" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="21">
@@ -2935,7 +2959,7 @@
         <v>41899</v>
       </c>
       <c r="G20" s="75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2969,15 +2993,15 @@
         <v>5</v>
       </c>
       <c r="F22" s="70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>4.3</v>
       </c>
-      <c r="B23" s="83" t="s">
-        <v>154</v>
+      <c r="B23" s="78" t="s">
+        <v>151</v>
       </c>
       <c r="C23" s="57" t="s">
         <v>15</v>
@@ -2994,7 +3018,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B24" s="56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="58" t="s">
         <v>29</v>
@@ -3081,7 +3105,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="63" t="s">
         <v>15</v>
@@ -3095,7 +3119,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="68" t="s">
         <v>29</v>
@@ -3302,7 +3326,7 @@
       </c>
       <c r="E44" s="48"/>
       <c r="F44" s="70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G44" s="48"/>
     </row>
@@ -3372,7 +3396,7 @@
       </c>
       <c r="E48" s="48"/>
       <c r="F48" s="70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G48" s="48"/>
     </row>
@@ -3425,7 +3449,7 @@
       </c>
       <c r="E51" s="48"/>
       <c r="F51" s="70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G51" s="48"/>
     </row>
@@ -3493,7 +3517,7 @@
       </c>
       <c r="E55" s="48"/>
       <c r="F55" s="70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G55" s="48"/>
     </row>

</xml_diff>

<commit_message>
fix due date and build faq
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH315/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA60D3C-01A0-4041-8664-89506C82381B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="5" r:id="rId1"/>
@@ -631,33 +630,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Take [this survey](https://goo.gl/forms/qLBv2jMF6fBv3BTR2) to help me set my OH (Due Thu 8/30 )
-Join our [Slack team](http://math-315.slack.com) and post an `#introduction` (instructions in channel) (Due Sun 9/2 )
-[Data Camp](https://www.datacamp.com/users/sign_in) Intro to R - Intro to Basics Chapter [BBL] (Due Thu 9/6 )
-Metacognition Awareness Inventory [BBL] (Due Sun 9/2 )
-R Markdown test file (Due Wed 8/29 )
-hw01 Introductions [[HTML]](hw/hw01_introductions.html)[[PDF]](hw/hw01_introductions.pdf)(Due Sun 9/2 )</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Data Management Assignment [[HTML]](hw/hw04_data_management.html] [[PDF]](hw/hw04_data_management.pdf](Due Sun 9/23 )</t>
     </r>
     <r>
@@ -716,15 +688,42 @@
 * MAI and academic achievement
 * Create a `MATH315` folder on your computer in an easy to find spot. Create subfolders for `hw`, `project`</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Take [this survey](https://goo.gl/forms/qLBv2jMF6fBv3BTR2) to help me set my OH (Due Thu 8/30 )
+Join our [Slack team](http://math-315.slack.com) and post an `#introduction` (instructions in channel) (Due Sun 9/2 )
+[Data Camp](https://www.datacamp.com/users/sign_in) Intro to R - Intro to Basics Chapter [BBL] (Due Thu 9/6 )
+Metacognition Awareness Inventory [BBL] (Due Sun 9/2 )
+R Markdown test file (Due Fri 8/31 )
+hw01 Introductions [[HTML]](hw/hw01_introductions.html)[[PDF]](hw/hw01_introductions.pdf)(Due Sun 9/2 )</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1385,10 +1384,10 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Percent 3" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Normal 3" xfId="80"/>
+    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Percent 3" xfId="81"/>
     <cellStyle name="Total" xfId="78" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1725,29 +1724,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="38" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="38" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="45" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" style="45" customWidth="1"/>
-    <col min="6" max="6" width="45.83203125" style="45" customWidth="1"/>
-    <col min="7" max="7" width="30.1640625" style="45" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="33.625" style="38" customWidth="1"/>
+    <col min="4" max="4" width="27.375" style="45" customWidth="1"/>
+    <col min="5" max="5" width="47.625" style="45" customWidth="1"/>
+    <col min="6" max="6" width="45.875" style="45" customWidth="1"/>
+    <col min="7" max="7" width="30.125" style="45" customWidth="1"/>
     <col min="8" max="9" width="38" style="45" customWidth="1"/>
     <col min="10" max="10" width="46.5" style="45" customWidth="1"/>
-    <col min="11" max="16384" width="14.83203125" style="38"/>
+    <col min="11" max="16384" width="14.875" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="409.6">
+    <row r="2" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="39">
         <v>1</v>
       </c>
@@ -1793,10 +1792,10 @@
         <v>89</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>144</v>
@@ -1808,11 +1807,11 @@
         <v>152</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="240">
+    <row r="3" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>2</v>
       </c>
@@ -1845,7 +1844,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="256">
+    <row r="4" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="39">
         <v>3</v>
       </c>
@@ -1863,7 +1862,7 @@
         <v>133</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>126</v>
@@ -1878,7 +1877,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="380">
+    <row r="5" spans="1:11" ht="390" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
         <v>4</v>
       </c>
@@ -1896,7 +1895,7 @@
         <v>149</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>142</v>
@@ -1908,10 +1907,10 @@
         <v>145</v>
       </c>
       <c r="J5" s="73" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="64">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="39">
         <v>5</v>
       </c>
@@ -1936,7 +1935,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="112">
+    <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="39">
         <v>6</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="48">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
         <v>7</v>
       </c>
@@ -1984,7 +1983,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="48">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <v>8</v>
       </c>
@@ -2005,7 +2004,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="48">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>9</v>
       </c>
@@ -2024,7 +2023,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="73"/>
     </row>
-    <row r="11" spans="1:11" ht="48">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>10</v>
       </c>
@@ -2045,7 +2044,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="48">
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>11</v>
       </c>
@@ -2066,7 +2065,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="48">
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>12</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="44">
         <f t="shared" si="0"/>
@@ -2104,7 +2103,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="74"/>
     </row>
-    <row r="15" spans="1:11" ht="48">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>13</v>
       </c>
@@ -2125,7 +2124,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="48">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>14</v>
       </c>
@@ -2146,7 +2145,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="48">
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>15</v>
       </c>
@@ -2167,7 +2166,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="32">
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>0</v>
       </c>
@@ -2191,30 +2190,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="17"/>
-    <col min="2" max="2" width="32.1640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="19"/>
-    <col min="5" max="5" width="7.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.6640625" style="47" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="17"/>
+    <col min="2" max="2" width="32.125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="10.625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" style="19"/>
+    <col min="5" max="5" width="7.625" style="47" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.625" style="47" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="7" customWidth="1"/>
     <col min="9" max="9" width="10" style="8" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" style="8"/>
-    <col min="11" max="11" width="4.6640625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="7.6640625" style="7"/>
+    <col min="10" max="10" width="7.625" style="8"/>
+    <col min="11" max="11" width="4.625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="10.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="7.625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" thickBot="1">
+    <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -2273,7 +2272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="17" thickTop="1">
+    <row r="2" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>0</v>
       </c>
@@ -2295,7 +2294,7 @@
       </c>
       <c r="J2" s="14">
         <f t="shared" ref="J2:J8" si="0">I2/$I$9</f>
-        <v>8.6956521739130432E-2</v>
+        <v>8.7136929460580909E-2</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>25</v>
@@ -2325,7 +2324,7 @@
         <v>3.0837004405286344E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="16">
+    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1.1000000000000001</v>
       </c>
@@ -2339,7 +2338,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="47">
-        <v>41879</v>
+        <v>41881</v>
       </c>
       <c r="G3" s="52" t="s">
         <v>91</v>
@@ -2353,7 +2352,7 @@
       </c>
       <c r="J3" s="14">
         <f t="shared" si="0"/>
-        <v>0.10766045548654245</v>
+        <v>0.1078838174273859</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>8</v>
@@ -2383,7 +2382,7 @@
         <v>0.21806167400881057</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="16">
+    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1.2</v>
       </c>
@@ -2394,10 +2393,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="47">
-        <v>41881</v>
+        <v>41879</v>
       </c>
       <c r="G4" s="53" t="s">
         <v>91</v>
@@ -2411,7 +2410,7 @@
       </c>
       <c r="J4" s="14">
         <f t="shared" si="0"/>
-        <v>0.13250517598343686</v>
+        <v>0.13278008298755187</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>29</v>
@@ -2441,7 +2440,7 @@
         <v>4.405286343612335E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="16">
+    <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>1.3</v>
       </c>
@@ -2489,7 +2488,7 @@
         <v>6.8281938325991193E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16">
+    <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>1.4</v>
       </c>
@@ -2513,11 +2512,11 @@
       </c>
       <c r="I6" s="8">
         <f>SUMIF($C$2:$C$80,H6,$D$2:$D$80)</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J6" s="14">
         <f t="shared" si="0"/>
-        <v>6.2111801242236024E-2</v>
+        <v>6.0165975103734441E-2</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>13</v>
@@ -2547,7 +2546,7 @@
         <v>2.2026431718061675E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="16">
+    <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>1.5</v>
       </c>
@@ -2575,7 +2574,7 @@
       </c>
       <c r="J7" s="14">
         <f t="shared" si="0"/>
-        <v>0.3105590062111801</v>
+        <v>0.31120331950207469</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>14</v>
@@ -2605,7 +2604,7 @@
         <v>0.38546255506607929</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="17" thickBot="1">
+    <row r="8" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>1.6</v>
       </c>
@@ -2633,7 +2632,7 @@
       </c>
       <c r="J8" s="14">
         <f t="shared" si="0"/>
-        <v>0.30020703933747411</v>
+        <v>0.30082987551867219</v>
       </c>
       <c r="L8" s="27" t="s">
         <v>15</v>
@@ -2659,7 +2658,7 @@
         <v>0.23127753303964757</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="16" thickBot="1">
+    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>2.1</v>
       </c>
@@ -2680,7 +2679,7 @@
       </c>
       <c r="I9" s="6">
         <f>SUM(I2:I8)</f>
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="M9" s="8">
         <v>405</v>
@@ -2691,7 +2690,7 @@
       </c>
       <c r="V9" s="17"/>
     </row>
-    <row r="10" spans="1:22" ht="16" thickTop="1">
+    <row r="10" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>2.2000000000000002</v>
       </c>
@@ -2711,7 +2710,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>2.2999999999999998</v>
       </c>
@@ -2731,7 +2730,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>2.4</v>
       </c>
@@ -2751,7 +2750,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="16">
+    <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>2.5</v>
       </c>
@@ -2774,7 +2773,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="16" thickBot="1">
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20">
         <v>2.6</v>
       </c>
@@ -2794,7 +2793,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>3.1</v>
       </c>
@@ -2818,7 +2817,7 @@
       </c>
       <c r="I15" s="81"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>3.2</v>
       </c>
@@ -2842,7 +2841,7 @@
       </c>
       <c r="I16" s="82"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>3.3</v>
       </c>
@@ -2866,7 +2865,7 @@
       </c>
       <c r="I17" s="83"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>3.4</v>
       </c>
@@ -2890,7 +2889,7 @@
       </c>
       <c r="I18" s="84"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>3.5</v>
       </c>
@@ -2915,7 +2914,7 @@
       </c>
       <c r="I19" s="85"/>
     </row>
-    <row r="20" spans="1:9" ht="16" thickBot="1">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20">
         <v>3.6</v>
       </c>
@@ -2935,7 +2934,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>4.0999999999999996</v>
       </c>
@@ -2952,7 +2951,7 @@
         <v>41898</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="16">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>4.2</v>
       </c>
@@ -2969,7 +2968,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>4.3</v>
       </c>
@@ -2986,7 +2985,7 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>4.4000000000000004</v>
       </c>
@@ -3003,7 +3002,7 @@
         <v>41906</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>5</v>
       </c>
@@ -3017,7 +3016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>5</v>
       </c>
@@ -3031,7 +3030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>5</v>
       </c>
@@ -3045,7 +3044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>6</v>
       </c>
@@ -3059,7 +3058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>6</v>
       </c>
@@ -3073,7 +3072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>6</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>6</v>
       </c>
@@ -3101,7 +3100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>6</v>
       </c>
@@ -3115,7 +3114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>6</v>
       </c>
@@ -3132,7 +3131,7 @@
       <c r="F33" s="48"/>
       <c r="G33" s="48"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>7</v>
       </c>
@@ -3146,7 +3145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>7</v>
       </c>
@@ -3160,7 +3159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>7</v>
       </c>
@@ -3174,7 +3173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>7</v>
       </c>
@@ -3188,7 +3187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>7</v>
       </c>
@@ -3202,7 +3201,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>7</v>
       </c>
@@ -3216,7 +3215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>8</v>
       </c>
@@ -3233,7 +3232,7 @@
       <c r="F40" s="48"/>
       <c r="G40" s="48"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>8</v>
       </c>
@@ -3250,7 +3249,7 @@
       <c r="F41" s="48"/>
       <c r="G41" s="48"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>9</v>
       </c>
@@ -3267,7 +3266,7 @@
       <c r="F42" s="48"/>
       <c r="G42" s="48"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>9</v>
       </c>
@@ -3284,7 +3283,7 @@
       <c r="F43" s="48"/>
       <c r="G43" s="48"/>
     </row>
-    <row r="44" spans="1:7" ht="16">
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>9</v>
       </c>
@@ -3303,7 +3302,7 @@
       </c>
       <c r="G44" s="48"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>10</v>
       </c>
@@ -3320,7 +3319,7 @@
       <c r="F45" s="48"/>
       <c r="G45" s="48"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>10</v>
       </c>
@@ -3337,7 +3336,7 @@
       <c r="F46" s="48"/>
       <c r="G46" s="48"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>10</v>
       </c>
@@ -3354,7 +3353,7 @@
       <c r="F47" s="48"/>
       <c r="G47" s="48"/>
     </row>
-    <row r="48" spans="1:7" ht="16">
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>11</v>
       </c>
@@ -3373,7 +3372,7 @@
       </c>
       <c r="G48" s="48"/>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>11</v>
       </c>
@@ -3390,7 +3389,7 @@
       <c r="F49" s="48"/>
       <c r="G49" s="48"/>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>11</v>
       </c>
@@ -3407,7 +3406,7 @@
       <c r="F50" s="48"/>
       <c r="G50" s="48"/>
     </row>
-    <row r="51" spans="1:11" ht="16">
+    <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>11</v>
       </c>
@@ -3426,7 +3425,7 @@
       </c>
       <c r="G51" s="48"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="22">
         <v>12</v>
       </c>
@@ -3441,7 +3440,7 @@
       <c r="F52" s="48"/>
       <c r="G52" s="48"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <v>12</v>
       </c>
@@ -3458,7 +3457,7 @@
       <c r="F53" s="48"/>
       <c r="G53" s="48"/>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="22">
         <v>13</v>
       </c>
@@ -3475,7 +3474,7 @@
       <c r="F54" s="48"/>
       <c r="G54" s="48"/>
     </row>
-    <row r="55" spans="1:11" ht="16">
+    <row r="55" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="22">
         <v>13</v>
       </c>
@@ -3494,7 +3493,7 @@
       </c>
       <c r="G55" s="48"/>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="22">
         <v>13</v>
       </c>
@@ -3511,7 +3510,7 @@
       <c r="F56" s="48"/>
       <c r="G56" s="48"/>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>14</v>
       </c>
@@ -3528,7 +3527,7 @@
       <c r="F57" s="48"/>
       <c r="G57" s="48"/>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>14</v>
       </c>
@@ -3545,7 +3544,7 @@
       <c r="F58" s="48"/>
       <c r="G58" s="48"/>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <v>15</v>
       </c>
@@ -3562,7 +3561,7 @@
       <c r="F59" s="49"/>
       <c r="G59" s="49"/>
     </row>
-    <row r="60" spans="1:11" s="18" customFormat="1">
+    <row r="60" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <v>15</v>
       </c>
@@ -3583,7 +3582,7 @@
       <c r="J60" s="8"/>
       <c r="K60" s="17"/>
     </row>
-    <row r="61" spans="1:11" s="18" customFormat="1">
+    <row r="61" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>15</v>
       </c>
@@ -3603,7 +3602,7 @@
       <c r="J61" s="17"/>
       <c r="K61" s="17"/>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>15</v>
       </c>
@@ -3623,7 +3622,7 @@
       <c r="I62" s="17"/>
       <c r="J62" s="17"/>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>17</v>
       </c>
@@ -3640,7 +3639,7 @@
       <c r="F63" s="48"/>
       <c r="G63" s="48"/>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>17</v>
       </c>
@@ -3657,7 +3656,7 @@
       <c r="F64" s="48"/>
       <c r="G64" s="48"/>
     </row>
-    <row r="65" spans="1:22">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>17</v>
       </c>
@@ -3674,7 +3673,7 @@
       <c r="F65" s="48"/>
       <c r="G65" s="48"/>
     </row>
-    <row r="66" spans="1:22" s="8" customFormat="1">
+    <row r="66" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>18</v>
       </c>
@@ -3703,7 +3702,7 @@
       <c r="U66" s="7"/>
       <c r="V66" s="7"/>
     </row>
-    <row r="67" spans="1:22" s="8" customFormat="1">
+    <row r="67" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
@@ -3724,7 +3723,7 @@
       <c r="U67" s="7"/>
       <c r="V67" s="7"/>
     </row>
-    <row r="68" spans="1:22" s="8" customFormat="1">
+    <row r="68" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="35" t="s">
         <v>87</v>
@@ -3751,7 +3750,7 @@
       <c r="U68" s="7"/>
       <c r="V68" s="7"/>
     </row>
-    <row r="69" spans="1:22" s="8" customFormat="1">
+    <row r="69" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
@@ -3772,7 +3771,7 @@
       <c r="U69" s="7"/>
       <c r="V69" s="7"/>
     </row>
-    <row r="70" spans="1:22" s="8" customFormat="1">
+    <row r="70" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
@@ -3793,7 +3792,7 @@
       <c r="U70" s="7"/>
       <c r="V70" s="7"/>
     </row>
-    <row r="71" spans="1:22" s="8" customFormat="1">
+    <row r="71" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
@@ -3814,7 +3813,7 @@
       <c r="U71" s="7"/>
       <c r="V71" s="7"/>
     </row>
-    <row r="72" spans="1:22" s="8" customFormat="1">
+    <row r="72" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
@@ -3835,7 +3834,7 @@
       <c r="U72" s="7"/>
       <c r="V72" s="7"/>
     </row>
-    <row r="73" spans="1:22" s="8" customFormat="1">
+    <row r="73" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
@@ -3856,7 +3855,7 @@
       <c r="U73" s="7"/>
       <c r="V73" s="7"/>
     </row>
-    <row r="74" spans="1:22" s="8" customFormat="1">
+    <row r="74" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
@@ -3877,7 +3876,7 @@
       <c r="U74" s="7"/>
       <c r="V74" s="7"/>
     </row>
-    <row r="75" spans="1:22" s="8" customFormat="1">
+    <row r="75" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11"/>
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
@@ -3898,7 +3897,7 @@
       <c r="U75" s="7"/>
       <c r="V75" s="7"/>
     </row>
-    <row r="76" spans="1:22" s="8" customFormat="1">
+    <row r="76" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
@@ -3919,7 +3918,7 @@
       <c r="U76" s="7"/>
       <c r="V76" s="7"/>
     </row>
-    <row r="77" spans="1:22" s="8" customFormat="1">
+    <row r="77" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
@@ -3942,7 +3941,7 @@
       <c r="U77" s="7"/>
       <c r="V77" s="7"/>
     </row>
-    <row r="78" spans="1:22" s="8" customFormat="1">
+    <row r="78" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
@@ -3963,7 +3962,7 @@
       <c r="U78" s="7"/>
       <c r="V78" s="7"/>
     </row>
-    <row r="79" spans="1:22" s="8" customFormat="1">
+    <row r="79" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
@@ -3986,7 +3985,7 @@
       <c r="U79" s="7"/>
       <c r="V79" s="7"/>
     </row>
-    <row r="80" spans="1:22" s="8" customFormat="1">
+    <row r="80" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
@@ -4009,7 +4008,7 @@
       <c r="U80" s="7"/>
       <c r="V80" s="7"/>
     </row>
-    <row r="81" spans="1:22" s="8" customFormat="1">
+    <row r="81" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
@@ -4032,7 +4031,7 @@
       <c r="U81" s="7"/>
       <c r="V81" s="7"/>
     </row>
-    <row r="82" spans="1:22" s="8" customFormat="1">
+    <row r="82" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11"/>
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
@@ -4055,7 +4054,7 @@
       <c r="U82" s="7"/>
       <c r="V82" s="7"/>
     </row>
-    <row r="83" spans="1:22" s="8" customFormat="1">
+    <row r="83" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
@@ -4078,7 +4077,7 @@
       <c r="U83" s="7"/>
       <c r="V83" s="7"/>
     </row>
-    <row r="84" spans="1:22" s="8" customFormat="1">
+    <row r="84" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
@@ -4101,7 +4100,7 @@
       <c r="U84" s="7"/>
       <c r="V84" s="7"/>
     </row>
-    <row r="85" spans="1:22" s="8" customFormat="1">
+    <row r="85" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11"/>
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
@@ -4124,7 +4123,7 @@
       <c r="U85" s="7"/>
       <c r="V85" s="7"/>
     </row>
-    <row r="86" spans="1:22" s="8" customFormat="1">
+    <row r="86" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11"/>
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
@@ -4147,7 +4146,7 @@
       <c r="U86" s="7"/>
       <c r="V86" s="7"/>
     </row>
-    <row r="87" spans="1:22" s="8" customFormat="1">
+    <row r="87" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11"/>
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
@@ -4168,13 +4167,13 @@
       <c r="U87" s="7"/>
       <c r="V87" s="7"/>
     </row>
-    <row r="88" spans="1:22">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
     </row>
-    <row r="89" spans="1:22">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A89" s="24"/>
       <c r="B89" s="25"/>
     </row>

</xml_diff>

<commit_message>
build wk 8 and 9
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B4D9A6-4195-4303-B02E-882900A6D9BD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="5" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$D$91</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="195">
   <si>
     <t>Finals Week</t>
   </si>
@@ -724,9 +725,6 @@
 Define the margin of error</t>
   </si>
   <si>
-    <t>**RAT** on Linear Regression</t>
-  </si>
-  <si>
     <t>**RAT** on Study Design</t>
   </si>
   <si>
@@ -824,11 +822,46 @@
 Explain what can make the width of a confidence interval larger or smaller
 Conduct a full 5 step hypothesis test</t>
   </si>
+  <si>
+    <t>Conduct and interpret a chi-squared test of association
+Calculate a linear regression equation and interpret the coefficients
+Conduct and interpret a test of correlation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch the assigned PDS Videos on correlation and tests for equal proportions
+Complete the T-Test and ANOVA questions in the Homework
+Review the AS Notebook on Simple Linear Regression
+</t>
+  </si>
+  <si>
+    <t>How to use the chi-squared distribution to test if the proportion of an event is equally likely across multiple groups</t>
+  </si>
+  <si>
+    <t>Assessing simple correlation between two quantitative variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**RAT** on Linear Regression
+What is "best" about the best fit line? 
+Why is it called the least squares line? 
+How do you interpret the slope and intercept of this line? </t>
+  </si>
+  <si>
+    <t>Open work day to finish the Bivarate inference homework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multivariable analysis - How does a third variable modify an existing relationship between a response and explanatory variable? </t>
+  </si>
+  <si>
+    <t>Exam 2 - Choosing appropriate inference
+interpreting results in context of the problem
+conducting hypothesis testing
+Calculating and interpreting confidence intervals</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
@@ -1252,7 +1285,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1353,9 +1386,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1575,10 +1605,10 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Normal 3" xfId="80"/>
-    <cellStyle name="Percent 2" xfId="52"/>
-    <cellStyle name="Percent 3" xfId="81"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Percent 3" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
     <cellStyle name="Total" xfId="78" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1915,12 +1945,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,12 +1958,12 @@
     <col min="1" max="1" width="8.125" style="38" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="38" customWidth="1"/>
     <col min="3" max="3" width="33.625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="27.375" style="44" customWidth="1"/>
-    <col min="5" max="5" width="47.625" style="44" customWidth="1"/>
-    <col min="6" max="6" width="45.875" style="44" customWidth="1"/>
-    <col min="7" max="7" width="30.125" style="44" customWidth="1"/>
-    <col min="8" max="9" width="38" style="44" customWidth="1"/>
-    <col min="10" max="10" width="46.5" style="44" customWidth="1"/>
+    <col min="4" max="4" width="27.375" style="43" customWidth="1"/>
+    <col min="5" max="5" width="47.625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="45.875" style="43" customWidth="1"/>
+    <col min="7" max="7" width="30.125" style="43" customWidth="1"/>
+    <col min="8" max="9" width="38" style="43" customWidth="1"/>
+    <col min="10" max="10" width="46.5" style="43" customWidth="1"/>
     <col min="11" max="16384" width="14.875" style="38"/>
   </cols>
   <sheetData>
@@ -1969,296 +1999,304 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="85" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="81">
+    <row r="2" spans="1:11" s="84" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="80">
         <v>1</v>
       </c>
-      <c r="B2" s="82">
+      <c r="B2" s="81">
         <v>41877</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="83" t="s">
+      <c r="D2" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="F2" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="G2" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="H2" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="I2" s="82" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="J2" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="K2" s="83"/>
-    </row>
-    <row r="3" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A3" s="81">
+      <c r="K2" s="82"/>
+    </row>
+    <row r="3" spans="1:11" ht="225" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="80">
         <v>2</v>
       </c>
-      <c r="B3" s="82">
+      <c r="B3" s="81">
         <f t="shared" ref="B3:B18" si="0">B2+7</f>
         <v>41884</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="82" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="E3" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="G3" s="86" t="s">
+      <c r="G3" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="83" t="s">
+      <c r="H3" s="82" t="s">
         <v>123</v>
       </c>
-      <c r="I3" s="83" t="s">
+      <c r="I3" s="82" t="s">
         <v>130</v>
       </c>
-      <c r="J3" s="87" t="s">
+      <c r="J3" s="86" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="240" x14ac:dyDescent="0.25">
-      <c r="A4" s="81">
+    <row r="4" spans="1:11" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80">
         <v>3</v>
       </c>
-      <c r="B4" s="82">
+      <c r="B4" s="81">
         <f t="shared" si="0"/>
         <v>41891</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="82" t="s">
         <v>108</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="82" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="H4" s="83" t="s">
+      <c r="H4" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="I4" s="83" t="s">
+      <c r="I4" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="87" t="s">
+      <c r="J4" s="86" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="300" x14ac:dyDescent="0.25">
-      <c r="A5" s="81">
+    <row r="5" spans="1:11" ht="300" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="80">
         <v>4</v>
       </c>
-      <c r="B5" s="82">
+      <c r="B5" s="81">
         <f>B4+7</f>
         <v>41898</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="83" t="s">
+      <c r="E5" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="83" t="s">
+      <c r="F5" s="82" t="s">
         <v>139</v>
       </c>
-      <c r="G5" s="83" t="s">
+      <c r="G5" s="82" t="s">
         <v>135</v>
       </c>
-      <c r="H5" s="83" t="s">
+      <c r="H5" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="I5" s="83" t="s">
+      <c r="I5" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="J5" s="87" t="s">
+      <c r="J5" s="86" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A6" s="81">
+    <row r="6" spans="1:11" ht="180" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="80">
         <v>5</v>
       </c>
-      <c r="B6" s="82">
+      <c r="B6" s="81">
         <f t="shared" si="0"/>
         <v>41905</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="82" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="83" t="s">
+      <c r="E6" s="82" t="s">
         <v>146</v>
       </c>
-      <c r="F6" s="83" t="s">
+      <c r="F6" s="82" t="s">
         <v>151</v>
       </c>
-      <c r="G6" s="83" t="s">
+      <c r="G6" s="82" t="s">
         <v>148</v>
       </c>
-      <c r="H6" s="83" t="s">
+      <c r="H6" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="I6" s="83" t="s">
+      <c r="I6" s="82" t="s">
         <v>145</v>
       </c>
-      <c r="J6" s="87" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="81">
+      <c r="J6" s="86" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="80">
         <v>6</v>
       </c>
-      <c r="B7" s="82">
+      <c r="B7" s="81">
         <f t="shared" si="0"/>
         <v>41912</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="83" t="s">
-        <v>182</v>
-      </c>
-      <c r="F7" s="83" t="s">
+      <c r="E7" s="82" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" s="82" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="83" t="s">
+      <c r="G7" s="82" t="s">
         <v>150</v>
       </c>
-      <c r="H7" s="83" t="s">
+      <c r="H7" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="83" t="s">
+      <c r="I7" s="82" t="s">
         <v>149</v>
       </c>
-      <c r="J7" s="87" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="270" x14ac:dyDescent="0.25">
-      <c r="A8" s="39">
+      <c r="J7" s="86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="270" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="80">
         <v>7</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="81">
         <f t="shared" si="0"/>
         <v>41919</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="82" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="82" t="s">
+        <v>179</v>
+      </c>
+      <c r="G8" s="82" t="s">
         <v>154</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="82" t="s">
         <v>165</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="J8" s="79" t="s">
+      <c r="I8" s="82" t="s">
+        <v>182</v>
+      </c>
+      <c r="J8" s="86" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="195" x14ac:dyDescent="0.25">
-      <c r="A9" s="39">
+      <c r="A9" s="80">
         <v>8</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="81">
         <f t="shared" si="0"/>
         <v>41926</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="82" t="s">
+        <v>183</v>
+      </c>
+      <c r="E9" s="82" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="79" t="s">
+      <c r="G9" s="82"/>
+      <c r="H9" s="82" t="s">
+        <v>170</v>
+      </c>
+      <c r="I9" s="82"/>
+      <c r="J9" s="86" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="41">
+      <c r="A10" s="40">
         <v>9</v>
       </c>
-      <c r="B10" s="40">
+      <c r="B10" s="39">
         <f t="shared" si="0"/>
         <v>41933</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="F10" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+        <v>178</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="I10" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="J10" s="79" t="s">
+        <v>191</v>
+      </c>
+      <c r="J10" s="78" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="41">
+    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
         <v>10</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B11" s="39">
         <f t="shared" si="0"/>
         <v>41940</v>
       </c>
@@ -2268,70 +2306,76 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J11" s="78" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="41">
+      <c r="A12" s="40">
         <v>11</v>
       </c>
-      <c r="B12" s="40">
+      <c r="B12" s="39">
         <f t="shared" si="0"/>
         <v>41947</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="79" t="s">
+      <c r="J12" s="78" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="41">
+      <c r="A13" s="40">
         <v>12</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="39">
         <f t="shared" si="0"/>
         <v>41954</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="G13" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="69" t="s">
         <v>101</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J13" s="79" t="s">
-        <v>174</v>
+        <v>168</v>
+      </c>
+      <c r="J13" s="78" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="43">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42">
         <f t="shared" si="0"/>
         <v>41961</v>
       </c>
@@ -2342,18 +2386,18 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="71"/>
+      <c r="J14" s="70"/>
     </row>
     <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="41">
+      <c r="A15" s="40">
         <v>13</v>
       </c>
-      <c r="B15" s="40">
+      <c r="B15" s="39">
         <f t="shared" si="0"/>
         <v>41968</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -2361,15 +2405,15 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="78" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="41">
+      <c r="A16" s="40">
         <v>14</v>
       </c>
-      <c r="B16" s="40">
+      <c r="B16" s="39">
         <f t="shared" si="0"/>
         <v>41975</v>
       </c>
@@ -2379,20 +2423,20 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="79" t="s">
+      <c r="J16" s="78" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="41">
+      <c r="A17" s="40">
         <v>15</v>
       </c>
-      <c r="B17" s="40">
+      <c r="B17" s="39">
         <f t="shared" si="0"/>
         <v>41982</v>
       </c>
@@ -2405,15 +2449,15 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="79" t="s">
+      <c r="J17" s="78" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="39">
         <f t="shared" si="0"/>
         <v>41989</v>
       </c>
@@ -2433,7 +2477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V92"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -2446,8 +2490,8 @@
     <col min="2" max="2" width="32.125" style="18" customWidth="1"/>
     <col min="3" max="3" width="10.625" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.625" style="19"/>
-    <col min="5" max="5" width="10.5" style="46" customWidth="1"/>
-    <col min="6" max="7" width="7.625" style="46" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="45" customWidth="1"/>
+    <col min="6" max="7" width="7.625" style="45" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="7" customWidth="1"/>
     <col min="9" max="9" width="10" style="8" customWidth="1"/>
     <col min="10" max="10" width="7.625" style="8"/>
@@ -2574,19 +2618,19 @@
       <c r="B3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="13">
         <v>2</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>41881</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="63" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="8">
@@ -2638,10 +2682,10 @@
       <c r="D4" s="13">
         <v>0</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>41879</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="51" t="s">
         <v>88</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -2696,10 +2740,10 @@
       <c r="D5" s="13">
         <v>3</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>41883</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="51" t="s">
         <v>88</v>
       </c>
       <c r="J5" s="14"/>
@@ -2744,10 +2788,10 @@
       <c r="D6" s="19">
         <v>1</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>41883</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="51" t="s">
         <v>88</v>
       </c>
       <c r="H6" s="7" t="s">
@@ -2793,19 +2837,19 @@
       <c r="A7" s="11">
         <v>1.5</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="13">
         <v>5</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>41883</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="G7" s="50" t="s">
         <v>88</v>
       </c>
       <c r="H7" s="7" t="s">
@@ -2851,22 +2895,22 @@
       <c r="A8" s="20">
         <v>1.6</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="44" t="s">
         <v>82</v>
       </c>
       <c r="D8" s="21">
         <v>2.5</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <v>41883</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="63" t="s">
+      <c r="H8" s="62" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="8">
@@ -2914,10 +2958,10 @@
       <c r="D9" s="13">
         <v>2</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <v>41886</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="51" t="s">
         <v>88</v>
       </c>
       <c r="I9" s="6">
@@ -2946,10 +2990,10 @@
       <c r="D10" s="13">
         <v>1</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>41890</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="51" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2960,16 +3004,16 @@
       <c r="B11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="49" t="s">
         <v>82</v>
       </c>
       <c r="D11" s="13">
         <v>5</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="45">
         <v>41890</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="51" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2980,16 +3024,16 @@
       <c r="B12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="49" t="s">
         <v>82</v>
       </c>
       <c r="D12" s="13">
         <v>3</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="45">
         <v>41890</v>
       </c>
-      <c r="G12" s="52" t="s">
+      <c r="G12" s="51" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2997,22 +3041,22 @@
       <c r="A13" s="11">
         <v>2.5</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="13">
         <v>10</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="45">
         <v>41890</v>
       </c>
-      <c r="F13" s="68" t="s">
+      <c r="F13" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="52" t="s">
+      <c r="G13" s="51" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3020,19 +3064,19 @@
       <c r="A14" s="20">
         <v>2.6</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="65" t="s">
+      <c r="C14" s="64" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="21">
         <v>4</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>41892</v>
       </c>
-      <c r="G14" s="52" t="s">
+      <c r="G14" s="51" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3049,16 +3093,16 @@
       <c r="D15" s="13">
         <v>2</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="45">
         <v>41893</v>
       </c>
-      <c r="G15" s="72" t="s">
+      <c r="G15" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="H15" s="98" t="s">
+      <c r="H15" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="98"/>
+      <c r="I15" s="97"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
@@ -3073,16 +3117,16 @@
       <c r="D16" s="13">
         <v>2</v>
       </c>
-      <c r="E16" s="46">
+      <c r="E16" s="45">
         <v>41897</v>
       </c>
-      <c r="G16" s="72" t="s">
+      <c r="G16" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="99" t="s">
+      <c r="H16" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="99"/>
+      <c r="I16" s="98"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
@@ -3097,16 +3141,16 @@
       <c r="D17" s="13">
         <v>1</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="46">
         <v>41897</v>
       </c>
-      <c r="G17" s="72" t="s">
+      <c r="G17" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="100" t="s">
+      <c r="H17" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="100"/>
+      <c r="I17" s="99"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
@@ -3115,65 +3159,65 @@
       <c r="B18" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="49" t="s">
         <v>82</v>
       </c>
       <c r="D18" s="13">
         <v>2</v>
       </c>
-      <c r="E18" s="46">
+      <c r="E18" s="45">
         <v>41897</v>
       </c>
-      <c r="G18" s="72" t="s">
+      <c r="G18" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="H18" s="101" t="s">
+      <c r="H18" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="101"/>
+      <c r="I18" s="100"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>3.5</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="13">
         <v>10</v>
       </c>
-      <c r="E19" s="46">
+      <c r="E19" s="45">
         <v>41897</v>
       </c>
-      <c r="F19" s="74"/>
-      <c r="G19" s="69" t="s">
+      <c r="F19" s="73"/>
+      <c r="G19" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="H19" s="102" t="s">
+      <c r="H19" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="102"/>
+      <c r="I19" s="101"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20">
         <v>3.6</v>
       </c>
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="77" t="s">
+      <c r="C20" s="76" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="21">
         <v>4</v>
       </c>
-      <c r="E20" s="73">
+      <c r="E20" s="72">
         <v>41899</v>
       </c>
-      <c r="G20" s="72" t="s">
+      <c r="G20" s="71" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3190,10 +3234,10 @@
       <c r="D21" s="13">
         <v>2</v>
       </c>
-      <c r="E21" s="46">
+      <c r="E21" s="45">
         <v>41898</v>
       </c>
-      <c r="G21" s="80" t="s">
+      <c r="G21" s="79" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3201,22 +3245,22 @@
       <c r="A22" s="11">
         <v>4.2</v>
       </c>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="13">
         <v>5</v>
       </c>
-      <c r="E22" s="46">
+      <c r="E22" s="45">
         <v>41904</v>
       </c>
-      <c r="F22" s="68" t="s">
+      <c r="F22" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="G22" s="80" t="s">
+      <c r="G22" s="79" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3224,20 +3268,20 @@
       <c r="A23" s="11">
         <v>4.3</v>
       </c>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="87" t="s">
         <v>140</v>
       </c>
-      <c r="C23" s="56" t="s">
+      <c r="C23" s="55" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="13">
         <v>4</v>
       </c>
-      <c r="E23" s="46">
+      <c r="E23" s="45">
         <v>41906</v>
       </c>
-      <c r="F23" s="68"/>
-      <c r="G23" s="91" t="s">
+      <c r="F23" s="67"/>
+      <c r="G23" s="90" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3245,19 +3289,19 @@
       <c r="A24" s="11">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="54" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="13">
         <v>15</v>
       </c>
-      <c r="E24" s="46">
+      <c r="E24" s="45">
         <v>41904</v>
       </c>
-      <c r="G24" s="80" t="s">
+      <c r="G24" s="79" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3265,20 +3309,20 @@
       <c r="A25" s="20">
         <v>4.5</v>
       </c>
-      <c r="B25" s="89" t="s">
+      <c r="B25" s="88" t="s">
         <v>128</v>
       </c>
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="76" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="21">
         <v>4</v>
       </c>
-      <c r="E25" s="73">
+      <c r="E25" s="72">
         <v>41906</v>
       </c>
-      <c r="F25" s="73"/>
-      <c r="G25" s="90" t="s">
+      <c r="F25" s="72"/>
+      <c r="G25" s="89" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3295,10 +3339,10 @@
       <c r="D26" s="13">
         <v>2</v>
       </c>
-      <c r="E26" s="46">
+      <c r="E26" s="45">
         <v>41905</v>
       </c>
-      <c r="G26" s="94" t="s">
+      <c r="G26" s="93" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3315,10 +3359,10 @@
       <c r="D27" s="13">
         <v>2</v>
       </c>
-      <c r="E27" s="46">
+      <c r="E27" s="45">
         <v>41911</v>
       </c>
-      <c r="G27" s="91" t="s">
+      <c r="G27" s="90" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3326,19 +3370,19 @@
       <c r="A28" s="11">
         <v>5.3</v>
       </c>
-      <c r="B28" s="88" t="s">
+      <c r="B28" s="87" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="13">
         <v>5</v>
       </c>
-      <c r="E28" s="46">
+      <c r="E28" s="45">
         <v>41911</v>
       </c>
-      <c r="G28" s="94" t="s">
+      <c r="G28" s="93" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3346,20 +3390,20 @@
       <c r="A29" s="20">
         <v>5.4</v>
       </c>
-      <c r="B29" s="92" t="s">
+      <c r="B29" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="76" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="21">
         <v>4</v>
       </c>
-      <c r="E29" s="73">
+      <c r="E29" s="72">
         <v>41913</v>
       </c>
-      <c r="F29" s="73"/>
-      <c r="G29" s="93" t="s">
+      <c r="F29" s="72"/>
+      <c r="G29" s="92" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3376,7 +3420,7 @@
       <c r="D30" s="13">
         <v>50</v>
       </c>
-      <c r="E30" s="46">
+      <c r="E30" s="45">
         <v>41914</v>
       </c>
     </row>
@@ -3398,10 +3442,10 @@
       <c r="A32" s="11">
         <v>6</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="61" t="s">
+      <c r="C32" s="60" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="13"/>
@@ -3410,10 +3454,10 @@
       <c r="A33" s="11">
         <v>6</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="66" t="s">
+      <c r="C33" s="65" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="13"/>
@@ -3425,13 +3469,13 @@
       <c r="B34" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="61" t="s">
+      <c r="C34" s="60" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="13">
         <v>20</v>
       </c>
-      <c r="E34" s="46">
+      <c r="E34" s="45">
         <v>41918</v>
       </c>
     </row>
@@ -3442,17 +3486,17 @@
       <c r="B35" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="66" t="s">
+      <c r="C35" s="65" t="s">
         <v>28</v>
       </c>
       <c r="D35" s="13">
         <v>4</v>
       </c>
-      <c r="E35" s="47">
+      <c r="E35" s="46">
         <v>41920</v>
       </c>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
@@ -3467,7 +3511,7 @@
       <c r="D36" s="13">
         <v>2</v>
       </c>
-      <c r="E36" s="46">
+      <c r="E36" s="45">
         <v>41921</v>
       </c>
     </row>
@@ -3529,7 +3573,7 @@
       <c r="A41" s="11">
         <v>7</v>
       </c>
-      <c r="B41" s="97" t="s">
+      <c r="B41" s="96" t="s">
         <v>160</v>
       </c>
       <c r="C41" s="12" t="s">
@@ -3546,7 +3590,7 @@
       <c r="B42" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="59" t="s">
+      <c r="C42" s="58" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="13">
@@ -3566,9 +3610,9 @@
       <c r="D43" s="13">
         <v>2</v>
       </c>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
@@ -3583,9 +3627,9 @@
       <c r="D44" s="13">
         <v>50</v>
       </c>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
@@ -3600,9 +3644,9 @@
       <c r="D45" s="13">
         <v>2</v>
       </c>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
@@ -3617,9 +3661,9 @@
       <c r="D46" s="13">
         <v>1</v>
       </c>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
@@ -3628,17 +3672,17 @@
       <c r="B47" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="58" t="s">
+      <c r="C47" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D47" s="13">
         <v>15</v>
       </c>
-      <c r="E47" s="47"/>
-      <c r="F47" s="95" t="s">
+      <c r="E47" s="46"/>
+      <c r="F47" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="G47" s="47"/>
+      <c r="G47" s="46"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
@@ -3653,9 +3697,9 @@
       <c r="D48" s="13">
         <v>2</v>
       </c>
-      <c r="E48" s="47"/>
-      <c r="F48" s="96"/>
-      <c r="G48" s="47"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="95"/>
+      <c r="G48" s="46"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
@@ -3664,15 +3708,15 @@
       <c r="B49" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="50" t="s">
+      <c r="C49" s="49" t="s">
         <v>82</v>
       </c>
       <c r="D49" s="13">
         <v>6</v>
       </c>
-      <c r="E49" s="47"/>
-      <c r="F49" s="96"/>
-      <c r="G49" s="47"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="95"/>
+      <c r="G49" s="46"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
@@ -3687,9 +3731,9 @@
       <c r="D50" s="13">
         <v>2</v>
       </c>
-      <c r="E50" s="47"/>
-      <c r="F50" s="96"/>
-      <c r="G50" s="47"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="95"/>
+      <c r="G50" s="46"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
@@ -3698,17 +3742,17 @@
       <c r="B51" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="61" t="s">
+      <c r="C51" s="60" t="s">
         <v>15</v>
       </c>
       <c r="D51" s="13">
         <v>20</v>
       </c>
-      <c r="E51" s="47"/>
-      <c r="F51" s="95" t="s">
+      <c r="E51" s="46"/>
+      <c r="F51" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="G51" s="47"/>
+      <c r="G51" s="46"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
@@ -3723,9 +3767,9 @@
       <c r="D52" s="13">
         <v>2</v>
       </c>
-      <c r="E52" s="47"/>
-      <c r="F52" s="96"/>
-      <c r="G52" s="47"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="95"/>
+      <c r="G52" s="46"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
@@ -3734,15 +3778,15 @@
       <c r="B53" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C53" s="66" t="s">
+      <c r="C53" s="65" t="s">
         <v>28</v>
       </c>
       <c r="D53" s="13">
         <v>4</v>
       </c>
-      <c r="E53" s="47"/>
-      <c r="F53" s="96"/>
-      <c r="G53" s="47"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="95"/>
+      <c r="G53" s="46"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
@@ -3751,17 +3795,17 @@
       <c r="B54" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="58" t="s">
+      <c r="C54" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D54" s="13">
         <v>15</v>
       </c>
-      <c r="E54" s="47"/>
-      <c r="F54" s="95" t="s">
+      <c r="E54" s="46"/>
+      <c r="F54" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="G54" s="47"/>
+      <c r="G54" s="46"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="22">
@@ -3774,9 +3818,9 @@
         <v>13</v>
       </c>
       <c r="D55" s="13"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="96"/>
-      <c r="G55" s="47"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="95"/>
+      <c r="G55" s="46"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
@@ -3785,15 +3829,15 @@
       <c r="B56" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="58" t="s">
+      <c r="C56" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D56" s="13">
         <v>15</v>
       </c>
-      <c r="E56" s="47"/>
-      <c r="F56" s="96"/>
-      <c r="G56" s="47"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="95"/>
+      <c r="G56" s="46"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="22">
@@ -3808,9 +3852,9 @@
       <c r="D57" s="13">
         <v>2</v>
       </c>
-      <c r="E57" s="47"/>
-      <c r="F57" s="96"/>
-      <c r="G57" s="47"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="95"/>
+      <c r="G57" s="46"/>
     </row>
     <row r="58" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="22">
@@ -3819,17 +3863,17 @@
       <c r="B58" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="61" t="s">
+      <c r="C58" s="60" t="s">
         <v>15</v>
       </c>
       <c r="D58" s="13">
         <v>20</v>
       </c>
-      <c r="E58" s="47"/>
-      <c r="F58" s="95" t="s">
+      <c r="E58" s="46"/>
+      <c r="F58" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="G58" s="47"/>
+      <c r="G58" s="46"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="22">
@@ -3838,15 +3882,15 @@
       <c r="B59" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C59" s="66" t="s">
+      <c r="C59" s="65" t="s">
         <v>28</v>
       </c>
       <c r="D59" s="13">
         <v>4</v>
       </c>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="47"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
@@ -3855,15 +3899,15 @@
       <c r="B60" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="60" t="s">
+      <c r="C60" s="59" t="s">
         <v>15</v>
       </c>
       <c r="D60" s="13">
         <v>10</v>
       </c>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
@@ -3872,15 +3916,15 @@
       <c r="B61" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="66" t="s">
+      <c r="C61" s="65" t="s">
         <v>28</v>
       </c>
       <c r="D61" s="13">
         <v>2</v>
       </c>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
@@ -3889,17 +3933,17 @@
       <c r="B62" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C62" s="60" t="s">
+      <c r="C62" s="59" t="s">
         <v>15</v>
       </c>
       <c r="D62" s="13">
         <v>20</v>
       </c>
-      <c r="E62" s="48">
+      <c r="E62" s="47">
         <v>41986</v>
       </c>
-      <c r="F62" s="48"/>
-      <c r="G62" s="48"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
     </row>
     <row r="63" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
@@ -3908,17 +3952,17 @@
       <c r="B63" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C63" s="67" t="s">
+      <c r="C63" s="66" t="s">
         <v>28</v>
       </c>
       <c r="D63" s="13">
         <v>5</v>
       </c>
-      <c r="E63" s="48">
+      <c r="E63" s="47">
         <v>41988</v>
       </c>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="47"/>
       <c r="H63" s="7"/>
       <c r="I63" s="8"/>
       <c r="J63" s="8"/>
@@ -3937,9 +3981,9 @@
       <c r="D64" s="13">
         <v>5</v>
       </c>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="47"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="46"/>
       <c r="I64" s="17"/>
       <c r="J64" s="17"/>
       <c r="K64" s="17"/>
@@ -3957,9 +4001,9 @@
       <c r="D65" s="13">
         <v>5</v>
       </c>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
-      <c r="G65" s="47"/>
+      <c r="E65" s="46"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="46"/>
       <c r="H65" s="18"/>
       <c r="I65" s="17"/>
       <c r="J65" s="17"/>
@@ -3977,9 +4021,9 @@
       <c r="D66" s="13">
         <v>50</v>
       </c>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="47"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
@@ -3994,9 +4038,9 @@
       <c r="D67" s="13">
         <v>2</v>
       </c>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="47"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
@@ -4011,9 +4055,9 @@
       <c r="D68" s="13">
         <v>1</v>
       </c>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
     </row>
     <row r="69" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
@@ -4028,9 +4072,9 @@
       <c r="D69" s="13">
         <v>10</v>
       </c>
-      <c r="E69" s="46"/>
-      <c r="F69" s="46"/>
-      <c r="G69" s="46"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="45"/>
       <c r="H69" s="7"/>
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
@@ -4049,9 +4093,9 @@
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
-      <c r="E70" s="46"/>
-      <c r="F70" s="46"/>
-      <c r="G70" s="46"/>
+      <c r="E70" s="45"/>
+      <c r="F70" s="45"/>
+      <c r="G70" s="45"/>
       <c r="H70" s="7"/>
       <c r="L70" s="7"/>
       <c r="M70" s="7"/>
@@ -4067,9 +4111,9 @@
     </row>
     <row r="71" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
-      <c r="E71" s="46"/>
-      <c r="F71" s="46"/>
-      <c r="G71" s="46"/>
+      <c r="E71" s="45"/>
+      <c r="F71" s="45"/>
+      <c r="G71" s="45"/>
       <c r="H71" s="7"/>
       <c r="L71" s="7"/>
       <c r="M71" s="7"/>
@@ -4088,9 +4132,9 @@
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="46"/>
+      <c r="E72" s="45"/>
+      <c r="F72" s="45"/>
+      <c r="G72" s="45"/>
       <c r="H72" s="7"/>
       <c r="L72" s="7"/>
       <c r="M72" s="7"/>
@@ -4109,9 +4153,9 @@
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
-      <c r="E73" s="46"/>
-      <c r="F73" s="46"/>
-      <c r="G73" s="46"/>
+      <c r="E73" s="45"/>
+      <c r="F73" s="45"/>
+      <c r="G73" s="45"/>
       <c r="H73" s="7"/>
       <c r="L73" s="7"/>
       <c r="M73" s="7"/>
@@ -4130,9 +4174,9 @@
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
-      <c r="E74" s="46"/>
-      <c r="F74" s="46"/>
-      <c r="G74" s="46"/>
+      <c r="E74" s="45"/>
+      <c r="F74" s="45"/>
+      <c r="G74" s="45"/>
       <c r="H74" s="7"/>
       <c r="L74" s="7"/>
       <c r="M74" s="7"/>
@@ -4151,9 +4195,9 @@
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
-      <c r="E75" s="46"/>
-      <c r="F75" s="46"/>
-      <c r="G75" s="46"/>
+      <c r="E75" s="45"/>
+      <c r="F75" s="45"/>
+      <c r="G75" s="45"/>
       <c r="H75" s="7"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
@@ -4172,9 +4216,9 @@
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
-      <c r="E76" s="46"/>
-      <c r="F76" s="46"/>
-      <c r="G76" s="46"/>
+      <c r="E76" s="45"/>
+      <c r="F76" s="45"/>
+      <c r="G76" s="45"/>
       <c r="H76" s="7"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
@@ -4193,9 +4237,9 @@
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
-      <c r="E77" s="49"/>
-      <c r="F77" s="49"/>
-      <c r="G77" s="49"/>
+      <c r="E77" s="48"/>
+      <c r="F77" s="48"/>
+      <c r="G77" s="48"/>
       <c r="H77" s="7"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
@@ -4214,9 +4258,9 @@
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
-      <c r="E78" s="49"/>
-      <c r="F78" s="49"/>
-      <c r="G78" s="49"/>
+      <c r="E78" s="48"/>
+      <c r="F78" s="48"/>
+      <c r="G78" s="48"/>
       <c r="H78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="7"/>
@@ -4235,9 +4279,9 @@
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
-      <c r="E79" s="49"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="49"/>
+      <c r="E79" s="48"/>
+      <c r="F79" s="48"/>
+      <c r="G79" s="48"/>
       <c r="H79" s="7"/>
       <c r="L79" s="7"/>
       <c r="M79" s="7"/>
@@ -4256,9 +4300,9 @@
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
-      <c r="E80" s="46"/>
-      <c r="F80" s="46"/>
-      <c r="G80" s="46"/>
+      <c r="E80" s="45"/>
+      <c r="F80" s="45"/>
+      <c r="G80" s="45"/>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
@@ -4279,9 +4323,9 @@
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
-      <c r="E81" s="46"/>
-      <c r="F81" s="46"/>
-      <c r="G81" s="46"/>
+      <c r="E81" s="45"/>
+      <c r="F81" s="45"/>
+      <c r="G81" s="45"/>
       <c r="H81" s="7"/>
       <c r="L81" s="7"/>
       <c r="M81" s="7"/>
@@ -4300,9 +4344,9 @@
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
-      <c r="E82" s="46"/>
-      <c r="F82" s="46"/>
-      <c r="G82" s="46"/>
+      <c r="E82" s="45"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="45"/>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
@@ -4323,9 +4367,9 @@
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
-      <c r="E83" s="46"/>
-      <c r="F83" s="46"/>
-      <c r="G83" s="46"/>
+      <c r="E83" s="45"/>
+      <c r="F83" s="45"/>
+      <c r="G83" s="45"/>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
@@ -4346,9 +4390,9 @@
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
-      <c r="E84" s="46"/>
-      <c r="F84" s="46"/>
-      <c r="G84" s="46"/>
+      <c r="E84" s="45"/>
+      <c r="F84" s="45"/>
+      <c r="G84" s="45"/>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
@@ -4369,9 +4413,9 @@
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
-      <c r="E85" s="46"/>
-      <c r="F85" s="46"/>
-      <c r="G85" s="46"/>
+      <c r="E85" s="45"/>
+      <c r="F85" s="45"/>
+      <c r="G85" s="45"/>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
@@ -4392,9 +4436,9 @@
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
-      <c r="E86" s="46"/>
-      <c r="F86" s="46"/>
-      <c r="G86" s="46"/>
+      <c r="E86" s="45"/>
+      <c r="F86" s="45"/>
+      <c r="G86" s="45"/>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
@@ -4415,9 +4459,9 @@
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
-      <c r="E87" s="46"/>
-      <c r="F87" s="46"/>
-      <c r="G87" s="46"/>
+      <c r="E87" s="45"/>
+      <c r="F87" s="45"/>
+      <c r="G87" s="45"/>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
@@ -4438,9 +4482,9 @@
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
-      <c r="E88" s="46"/>
-      <c r="F88" s="46"/>
-      <c r="G88" s="46"/>
+      <c r="E88" s="45"/>
+      <c r="F88" s="45"/>
+      <c r="G88" s="45"/>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
@@ -4461,9 +4505,9 @@
       <c r="B89" s="12"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
-      <c r="E89" s="46"/>
-      <c r="F89" s="46"/>
-      <c r="G89" s="46"/>
+      <c r="E89" s="45"/>
+      <c r="F89" s="45"/>
+      <c r="G89" s="45"/>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
@@ -4484,9 +4528,9 @@
       <c r="B90" s="12"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
-      <c r="E90" s="46"/>
-      <c r="F90" s="46"/>
-      <c r="G90" s="46"/>
+      <c r="E90" s="45"/>
+      <c r="F90" s="45"/>
+      <c r="G90" s="45"/>
       <c r="H90" s="7"/>
       <c r="L90" s="7"/>
       <c r="M90" s="7"/>

</xml_diff>

<commit_message>
add moderation notes and hw
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11015"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH315/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32209C80-841F-4116-9BD0-FACCD9BDE982}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44EB896-B1EA-D140-BCD9-EE23423EE51D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="5" r:id="rId1"/>
@@ -19,16 +19,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$D$91</definedName>
   </definedNames>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -38,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="198">
   <si>
     <t>Finals Week</t>
   </si>
@@ -702,9 +697,6 @@
     <t>Bivariate Inference Assignment  [[HTML]](hw/hw08_bivariate_inference.html) [[PDF]](hw/hw08_bivariate_inference.pdf) (Due Mon 10/29 )</t>
   </si>
   <si>
-    <t>Moderation assignment [[HTML]](hw/hw09_moderation.html) [[PDF]](hw/hw09_moderation.pdf) (Due Tue 11/6 )</t>
-  </si>
-  <si>
     <t>**RAT on Foundations for Inference**
 How is an interval estimate different from a point estimate? 
 How is an interval estimate created?
@@ -750,10 +742,6 @@
   <si>
     <t>PDS Video 17 - start at 43 minutes for Logistic Regression
 [AS notes binary outcomes (8.2) and categorical predictors (7.1)](https://norcalbiostat.github.io/AppliedStatistics_notes/binary-data.html)</t>
-  </si>
-  <si>
-    <t>[AS notes on Stratification (7.2) and Moderation (7.3)](https://norcalbiostat.github.io/AppliedStatistics_notes/stratification.html)
-PDS Video 14</t>
   </si>
   <si>
     <t>Shiny Ed apps for learning distributions https://www2.stat.duke.edu/~mc301/shinyed/
@@ -871,13 +859,19 @@
 </t>
   </si>
   <si>
+    <t>Poster Draft (Due Fri 12/7 )(PR Due Sun 12/9 )
+Build your own exam questions [[HTML]]() [[PDF]]()(Due Sat 12/8 )</t>
+  </si>
+  <si>
+    <t>[AS notes on Stratification (7.2) and Moderation (7.3)](https://norcalbiostat.github.io/AppliedStatistics_notes/stratification.html)
+PDS Video 14
+Additional [Lecture notes on Moderation](lecture/lec05_moderation.html)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Poster prep stage II (Due Wed 10/31 ) (PR Due Fri 11/2 )(Final Due Sun 11/4 )
+Moderation assignment [[HTML]](hw/hw09_moderation.html) [[PDF]](hw/hw09_moderation.pdf) (Due Tue 11/6 )
 Optional Analyzing Exam Errors  (Due Fri 11/30 )
 </t>
-  </si>
-  <si>
-    <t>Poster Draft (Due Fri 12/7 )(PR Due Sun 12/9 )
-Build your own exam questions [[HTML]]() [[PDF]]()(Due Sat 12/8 )</t>
   </si>
 </sst>
 </file>
@@ -1533,6 +1527,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1547,12 +1547,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="82">
@@ -1976,26 +1970,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="38" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="38" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="38" customWidth="1"/>
-    <col min="3" max="3" width="33.625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="27.375" style="43" customWidth="1"/>
-    <col min="5" max="5" width="47.625" style="43" customWidth="1"/>
-    <col min="6" max="6" width="45.875" style="43" customWidth="1"/>
-    <col min="7" max="7" width="30.125" style="43" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" style="38" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="43" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" style="43" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" style="43" customWidth="1"/>
     <col min="8" max="9" width="38" style="43" customWidth="1"/>
     <col min="10" max="10" width="46.5" style="43" customWidth="1"/>
-    <col min="11" max="16384" width="14.875" style="38"/>
+    <col min="11" max="16384" width="14.83203125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
@@ -2027,7 +2021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="84" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="84" customFormat="1" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="80">
         <v>1</v>
       </c>
@@ -2060,7 +2054,7 @@
       </c>
       <c r="K2" s="82"/>
     </row>
-    <row r="3" spans="1:11" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="80">
         <v>2</v>
       </c>
@@ -2093,7 +2087,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="80">
         <v>3</v>
       </c>
@@ -2126,7 +2120,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="320" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="80">
         <v>4</v>
       </c>
@@ -2159,7 +2153,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="80">
         <v>5</v>
       </c>
@@ -2189,10 +2183,10 @@
         <v>144</v>
       </c>
       <c r="J6" s="86" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="80">
         <v>6</v>
       </c>
@@ -2207,7 +2201,7 @@
         <v>109</v>
       </c>
       <c r="E7" s="82" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F7" s="82" t="s">
         <v>151</v>
@@ -2222,10 +2216,10 @@
         <v>148</v>
       </c>
       <c r="J7" s="86" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="270" hidden="1" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="272" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="80">
         <v>7</v>
       </c>
@@ -2237,28 +2231,28 @@
         <v>101</v>
       </c>
       <c r="D8" s="82" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E8" s="82" t="s">
         <v>152</v>
       </c>
       <c r="F8" s="82" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G8" s="82" t="s">
         <v>153</v>
       </c>
       <c r="H8" s="82" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I8" s="82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J8" s="86" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="208" x14ac:dyDescent="0.2">
       <c r="A9" s="80">
         <v>8</v>
       </c>
@@ -2270,24 +2264,24 @@
         <v>102</v>
       </c>
       <c r="D9" s="82" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="82" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="82" t="s">
-        <v>179</v>
-      </c>
       <c r="F9" s="82" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G9" s="82"/>
       <c r="H9" s="82" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I9" s="82"/>
       <c r="J9" s="86" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="160" x14ac:dyDescent="0.2">
       <c r="A10" s="80">
         <v>9</v>
       </c>
@@ -2299,28 +2293,28 @@
         <v>116</v>
       </c>
       <c r="D10" s="82" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="82" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" s="82" t="s">
+        <v>187</v>
+      </c>
+      <c r="G10" s="82" t="s">
         <v>181</v>
       </c>
-      <c r="E10" s="82" t="s">
+      <c r="H10" s="82" t="s">
         <v>182</v>
       </c>
-      <c r="F10" s="82" t="s">
-        <v>189</v>
-      </c>
-      <c r="G10" s="82" t="s">
+      <c r="I10" s="82" t="s">
         <v>183</v>
-      </c>
-      <c r="H10" s="82" t="s">
-        <v>184</v>
-      </c>
-      <c r="I10" s="82" t="s">
-        <v>185</v>
       </c>
       <c r="J10" s="86" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="160" x14ac:dyDescent="0.2">
       <c r="A11" s="40">
         <v>10</v>
       </c>
@@ -2332,28 +2326,28 @@
         <v>155</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="J11" s="78" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="40">
         <v>11</v>
       </c>
@@ -2362,23 +2356,23 @@
         <v>41947</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="78" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="40">
         <v>12</v>
       </c>
@@ -2387,25 +2381,23 @@
         <v>41954</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G13" s="69" t="s">
         <v>100</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="J13" s="78" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="J13" s="78"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="41"/>
       <c r="B14" s="42">
         <f t="shared" si="0"/>
@@ -2420,7 +2412,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="70"/>
     </row>
-    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="40">
         <v>13</v>
       </c>
@@ -2429,7 +2421,7 @@
         <v>41968</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -2438,10 +2430,10 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="78" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="40">
         <v>14</v>
       </c>
@@ -2455,16 +2447,16 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="103" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="J16" s="98" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="40">
         <v>15</v>
       </c>
@@ -2481,11 +2473,11 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="103" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="J17" s="98" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="40" t="s">
         <v>0</v>
       </c>
@@ -2493,8 +2485,8 @@
         <f t="shared" si="0"/>
         <v>41989</v>
       </c>
-      <c r="C18" s="102" t="s">
-        <v>194</v>
+      <c r="C18" s="97" t="s">
+        <v>192</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -2502,8 +2494,8 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="103" t="s">
-        <v>195</v>
+      <c r="J18" s="98" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2520,23 +2512,23 @@
       <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="17"/>
-    <col min="2" max="2" width="32.125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="10.625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="19"/>
+    <col min="1" max="1" width="7.6640625" style="17"/>
+    <col min="2" max="2" width="32.1640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="19"/>
     <col min="5" max="5" width="10.5" style="45" customWidth="1"/>
-    <col min="6" max="7" width="7.625" style="45" customWidth="1"/>
+    <col min="6" max="7" width="7.6640625" style="45" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="7" customWidth="1"/>
     <col min="9" max="9" width="10" style="8" customWidth="1"/>
-    <col min="10" max="10" width="7.625" style="8"/>
-    <col min="11" max="11" width="4.625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="10.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="7.625" style="7"/>
+    <col min="10" max="10" width="7.6640625" style="8"/>
+    <col min="11" max="11" width="4.6640625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="7.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
@@ -2595,7 +2587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>0</v>
       </c>
@@ -2647,7 +2639,7 @@
         <v>3.0837004405286344E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>1.1000000000000001</v>
       </c>
@@ -2705,7 +2697,7 @@
         <v>0.21806167400881057</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1.2</v>
       </c>
@@ -2763,7 +2755,7 @@
         <v>4.405286343612335E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>1.3</v>
       </c>
@@ -2811,7 +2803,7 @@
         <v>6.8281938325991193E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>1.4</v>
       </c>
@@ -2869,7 +2861,7 @@
         <v>2.2026431718061675E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>1.5</v>
       </c>
@@ -2927,7 +2919,7 @@
         <v>0.38546255506607929</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>1.6</v>
       </c>
@@ -2981,7 +2973,7 @@
         <v>0.23127753303964757</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>2.1</v>
       </c>
@@ -3013,7 +3005,7 @@
       </c>
       <c r="V9" s="17"/>
     </row>
-    <row r="10" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2.2000000000000002</v>
       </c>
@@ -3033,7 +3025,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>2.2999999999999998</v>
       </c>
@@ -3053,7 +3045,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2.4</v>
       </c>
@@ -3073,7 +3065,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>2.5</v>
       </c>
@@ -3096,7 +3088,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>2.6</v>
       </c>
@@ -3116,7 +3108,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>3.1</v>
       </c>
@@ -3135,12 +3127,12 @@
       <c r="G15" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="H15" s="97" t="s">
+      <c r="H15" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="97"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I15" s="99"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>3.2</v>
       </c>
@@ -3159,12 +3151,12 @@
       <c r="G16" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="98" t="s">
+      <c r="H16" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="98"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="100"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>3.3</v>
       </c>
@@ -3183,12 +3175,12 @@
       <c r="G17" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="99" t="s">
+      <c r="H17" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="99"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="101"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>3.4</v>
       </c>
@@ -3207,12 +3199,12 @@
       <c r="G18" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="H18" s="100" t="s">
+      <c r="H18" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="100"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="102"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>3.5</v>
       </c>
@@ -3232,12 +3224,12 @@
       <c r="G19" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="H19" s="101" t="s">
+      <c r="H19" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="101"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="103"/>
+    </row>
+    <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>3.6</v>
       </c>
@@ -3257,7 +3249,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>4.0999999999999996</v>
       </c>
@@ -3277,7 +3269,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>4.2</v>
       </c>
@@ -3300,7 +3292,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>4.3</v>
       </c>
@@ -3321,7 +3313,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>4.4000000000000004</v>
       </c>
@@ -3341,7 +3333,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>4.5</v>
       </c>
@@ -3362,7 +3354,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>5.0999999999999996</v>
       </c>
@@ -3382,7 +3374,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>5.2</v>
       </c>
@@ -3402,7 +3394,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>5.3</v>
       </c>
@@ -3422,7 +3414,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
         <v>5.4</v>
       </c>
@@ -3443,7 +3435,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>6</v>
       </c>
@@ -3460,7 +3452,7 @@
         <v>41914</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>6</v>
       </c>
@@ -3474,7 +3466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
         <v>6</v>
       </c>
@@ -3486,7 +3478,7 @@
       </c>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>6</v>
       </c>
@@ -3498,7 +3490,7 @@
       </c>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>6</v>
       </c>
@@ -3515,7 +3507,7 @@
         <v>41918</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
         <v>6</v>
       </c>
@@ -3534,7 +3526,7 @@
       <c r="F35" s="46"/>
       <c r="G35" s="46"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
         <v>7</v>
       </c>
@@ -3551,7 +3543,7 @@
         <v>41921</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>7</v>
       </c>
@@ -3565,7 +3557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>7</v>
       </c>
@@ -3577,7 +3569,7 @@
       </c>
       <c r="D38" s="13"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
         <v>7</v>
       </c>
@@ -3591,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
         <v>7</v>
       </c>
@@ -3605,7 +3597,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
         <v>7</v>
       </c>
@@ -3619,7 +3611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
         <v>7</v>
       </c>
@@ -3633,7 +3625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
         <v>8</v>
       </c>
@@ -3650,7 +3642,7 @@
       <c r="F43" s="46"/>
       <c r="G43" s="46"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
         <v>8</v>
       </c>
@@ -3667,7 +3659,7 @@
       <c r="F44" s="46"/>
       <c r="G44" s="46"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>9</v>
       </c>
@@ -3684,7 +3676,7 @@
       <c r="F45" s="46"/>
       <c r="G45" s="46"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
         <v>9</v>
       </c>
@@ -3701,7 +3693,7 @@
       <c r="F46" s="46"/>
       <c r="G46" s="46"/>
     </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
         <v>9</v>
       </c>
@@ -3720,7 +3712,7 @@
       </c>
       <c r="G47" s="46"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
         <v>10</v>
       </c>
@@ -3737,7 +3729,7 @@
       <c r="F48" s="95"/>
       <c r="G48" s="46"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="11">
         <v>10</v>
       </c>
@@ -3754,7 +3746,7 @@
       <c r="F49" s="95"/>
       <c r="G49" s="46"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
         <v>10</v>
       </c>
@@ -3771,7 +3763,7 @@
       <c r="F50" s="95"/>
       <c r="G50" s="46"/>
     </row>
-    <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="11">
         <v>11</v>
       </c>
@@ -3790,7 +3782,7 @@
       </c>
       <c r="G51" s="46"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="11">
         <v>11</v>
       </c>
@@ -3807,7 +3799,7 @@
       <c r="F52" s="95"/>
       <c r="G52" s="46"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="11">
         <v>11</v>
       </c>
@@ -3824,7 +3816,7 @@
       <c r="F53" s="95"/>
       <c r="G53" s="46"/>
     </row>
-    <row r="54" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="11">
         <v>11</v>
       </c>
@@ -3843,7 +3835,7 @@
       </c>
       <c r="G54" s="46"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="22">
         <v>12</v>
       </c>
@@ -3858,7 +3850,7 @@
       <c r="F55" s="95"/>
       <c r="G55" s="46"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="11">
         <v>12</v>
       </c>
@@ -3875,7 +3867,7 @@
       <c r="F56" s="95"/>
       <c r="G56" s="46"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="22">
         <v>13</v>
       </c>
@@ -3892,7 +3884,7 @@
       <c r="F57" s="95"/>
       <c r="G57" s="46"/>
     </row>
-    <row r="58" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="22">
         <v>13</v>
       </c>
@@ -3911,7 +3903,7 @@
       </c>
       <c r="G58" s="46"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="22">
         <v>13</v>
       </c>
@@ -3928,7 +3920,7 @@
       <c r="F59" s="46"/>
       <c r="G59" s="46"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="11">
         <v>14</v>
       </c>
@@ -3945,7 +3937,7 @@
       <c r="F60" s="46"/>
       <c r="G60" s="46"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="11">
         <v>14</v>
       </c>
@@ -3962,7 +3954,7 @@
       <c r="F61" s="46"/>
       <c r="G61" s="46"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="11">
         <v>15</v>
       </c>
@@ -3981,7 +3973,7 @@
       <c r="F62" s="47"/>
       <c r="G62" s="47"/>
     </row>
-    <row r="63" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11">
         <v>15</v>
       </c>
@@ -4004,7 +3996,7 @@
       <c r="J63" s="8"/>
       <c r="K63" s="17"/>
     </row>
-    <row r="64" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="11">
         <v>15</v>
       </c>
@@ -4024,7 +4016,7 @@
       <c r="J64" s="17"/>
       <c r="K64" s="17"/>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" s="11">
         <v>15</v>
       </c>
@@ -4044,7 +4036,7 @@
       <c r="I65" s="17"/>
       <c r="J65" s="17"/>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" s="11">
         <v>17</v>
       </c>
@@ -4061,7 +4053,7 @@
       <c r="F66" s="46"/>
       <c r="G66" s="46"/>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" s="11">
         <v>17</v>
       </c>
@@ -4078,7 +4070,7 @@
       <c r="F67" s="46"/>
       <c r="G67" s="46"/>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" s="11">
         <v>17</v>
       </c>
@@ -4095,7 +4087,7 @@
       <c r="F68" s="46"/>
       <c r="G68" s="46"/>
     </row>
-    <row r="69" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="11">
         <v>18</v>
       </c>
@@ -4124,7 +4116,7 @@
       <c r="U69" s="7"/>
       <c r="V69" s="7"/>
     </row>
-    <row r="70" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11"/>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
@@ -4145,7 +4137,7 @@
       <c r="U70" s="7"/>
       <c r="V70" s="7"/>
     </row>
-    <row r="71" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="11"/>
       <c r="E71" s="45"/>
       <c r="F71" s="45"/>
@@ -4163,7 +4155,7 @@
       <c r="U71" s="7"/>
       <c r="V71" s="7"/>
     </row>
-    <row r="72" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="11"/>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
@@ -4184,7 +4176,7 @@
       <c r="U72" s="7"/>
       <c r="V72" s="7"/>
     </row>
-    <row r="73" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="11"/>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
@@ -4205,7 +4197,7 @@
       <c r="U73" s="7"/>
       <c r="V73" s="7"/>
     </row>
-    <row r="74" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="11"/>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
@@ -4226,7 +4218,7 @@
       <c r="U74" s="7"/>
       <c r="V74" s="7"/>
     </row>
-    <row r="75" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11"/>
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
@@ -4247,7 +4239,7 @@
       <c r="U75" s="7"/>
       <c r="V75" s="7"/>
     </row>
-    <row r="76" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="11"/>
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
@@ -4268,7 +4260,7 @@
       <c r="U76" s="7"/>
       <c r="V76" s="7"/>
     </row>
-    <row r="77" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11"/>
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
@@ -4289,7 +4281,7 @@
       <c r="U77" s="7"/>
       <c r="V77" s="7"/>
     </row>
-    <row r="78" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="11"/>
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
@@ -4310,7 +4302,7 @@
       <c r="U78" s="7"/>
       <c r="V78" s="7"/>
     </row>
-    <row r="79" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="11"/>
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
@@ -4331,7 +4323,7 @@
       <c r="U79" s="7"/>
       <c r="V79" s="7"/>
     </row>
-    <row r="80" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="11"/>
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
@@ -4354,7 +4346,7 @@
       <c r="U80" s="7"/>
       <c r="V80" s="7"/>
     </row>
-    <row r="81" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11"/>
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
@@ -4375,7 +4367,7 @@
       <c r="U81" s="7"/>
       <c r="V81" s="7"/>
     </row>
-    <row r="82" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="11"/>
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
@@ -4398,7 +4390,7 @@
       <c r="U82" s="7"/>
       <c r="V82" s="7"/>
     </row>
-    <row r="83" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
@@ -4421,7 +4413,7 @@
       <c r="U83" s="7"/>
       <c r="V83" s="7"/>
     </row>
-    <row r="84" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="11"/>
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
@@ -4444,7 +4436,7 @@
       <c r="U84" s="7"/>
       <c r="V84" s="7"/>
     </row>
-    <row r="85" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11"/>
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
@@ -4467,7 +4459,7 @@
       <c r="U85" s="7"/>
       <c r="V85" s="7"/>
     </row>
-    <row r="86" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="11"/>
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
@@ -4490,7 +4482,7 @@
       <c r="U86" s="7"/>
       <c r="V86" s="7"/>
     </row>
-    <row r="87" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11"/>
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
@@ -4513,7 +4505,7 @@
       <c r="U87" s="7"/>
       <c r="V87" s="7"/>
     </row>
-    <row r="88" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="11"/>
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
@@ -4536,7 +4528,7 @@
       <c r="U88" s="7"/>
       <c r="V88" s="7"/>
     </row>
-    <row r="89" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11"/>
       <c r="B89" s="12"/>
       <c r="C89" s="12"/>
@@ -4559,7 +4551,7 @@
       <c r="U89" s="7"/>
       <c r="V89" s="7"/>
     </row>
-    <row r="90" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="11"/>
       <c r="B90" s="12"/>
       <c r="C90" s="12"/>
@@ -4580,13 +4572,13 @@
       <c r="U90" s="7"/>
       <c r="V90" s="7"/>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A91" s="11"/>
       <c r="B91" s="12"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A92" s="24"/>
       <c r="B92" s="25"/>
     </row>

</xml_diff>

<commit_message>
rebuild with simple calendar
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0C80E5-32E2-4A85-AADB-E2B82FD78E2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5680EE25-00A1-437C-8739-0A1252679F45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="8" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="328">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1350,9 +1350,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>PR</t>
-  </si>
-  <si>
     <t>hw08_bivariate_inference</t>
   </si>
   <si>
@@ -1428,9 +1425,6 @@
     <t>Simple Linear Regression</t>
   </si>
   <si>
-    <t>Timed Quiz</t>
-  </si>
-  <si>
     <t>BBL Quiz</t>
   </si>
   <si>
@@ -1476,16 +1470,7 @@
     <t>hw</t>
   </si>
   <si>
-    <t>14 (38 min)</t>
-  </si>
-  <si>
-    <t>14 (20 min)</t>
-  </si>
-  <si>
     <t>Logistic Regression</t>
-  </si>
-  <si>
-    <t>14 (43 min)</t>
   </si>
   <si>
     <t>Confounding and Multiple Regression</t>
@@ -1499,6 +1484,39 @@
 Logistic regression
 Interaction terms
 Categorical terms</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>Peer Review</t>
+  </si>
+  <si>
+    <t>Poster prep Stage II</t>
+  </si>
+  <si>
+    <t>Poster prep Stage III</t>
+  </si>
+  <si>
+    <t>Poster prep Stage I</t>
+  </si>
+  <si>
+    <t>T-test</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>8.3</t>
   </si>
 </sst>
 </file>
@@ -1938,7 +1956,7 @@
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2162,6 +2180,24 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="5" xfId="82" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2890,7 +2926,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="62" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="62" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="59">
         <v>11</v>
       </c>
@@ -2915,7 +2951,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="62" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="62" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="59">
         <v>12</v>
       </c>
@@ -2949,7 +2985,7 @@
         <v>42108</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>185</v>
@@ -3274,22 +3310,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DC1812-FD5C-4C2B-9AB5-275F99A8591F}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="92"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" style="92" customWidth="1"/>
-    <col min="4" max="5" width="13.875" style="92" customWidth="1"/>
-    <col min="6" max="6" width="21.375" style="92" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="92" customWidth="1"/>
-    <col min="8" max="8" width="22.375" style="92" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.875" style="92" customWidth="1"/>
+    <col min="3" max="3" width="10.75" style="100" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="92" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="92" customWidth="1"/>
+    <col min="6" max="6" width="22.375" style="92" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.625" style="92" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.375" style="92" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.875" style="92" customWidth="1"/>
     <col min="10" max="10" width="28.75" style="92" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3300,26 +3337,26 @@
       <c r="B1" s="91" t="s">
         <v>247</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="99" t="s">
         <v>248</v>
       </c>
       <c r="D1" s="91" t="s">
         <v>250</v>
       </c>
       <c r="E1" s="91" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="91" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="91" t="s">
+        <v>321</v>
+      </c>
+      <c r="H1" s="91" t="s">
+        <v>298</v>
+      </c>
+      <c r="I1" s="91" t="s">
         <v>251</v>
-      </c>
-      <c r="F1" s="91" t="s">
-        <v>300</v>
-      </c>
-      <c r="G1" s="91" t="s">
-        <v>299</v>
-      </c>
-      <c r="H1" s="91" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="91" t="s">
-        <v>273</v>
       </c>
       <c r="J1" s="91" t="s">
         <v>29</v>
@@ -3335,11 +3372,11 @@
       <c r="D2" s="92" t="s">
         <v>252</v>
       </c>
-      <c r="E2" s="92" t="s">
+      <c r="F2" s="93" t="s">
+        <v>270</v>
+      </c>
+      <c r="I2" s="92" t="s">
         <v>269</v>
-      </c>
-      <c r="H2" s="93" t="s">
-        <v>270</v>
       </c>
       <c r="J2" s="93" t="s">
         <v>267</v>
@@ -3352,17 +3389,20 @@
       <c r="B3" t="s">
         <v>268</v>
       </c>
-      <c r="C3" s="92">
-        <v>2.1</v>
-      </c>
-      <c r="D3" s="92">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F3" s="92" t="s">
-        <v>306</v>
-      </c>
-      <c r="H3" s="93" t="s">
-        <v>276</v>
+      <c r="C3" s="100" t="s">
+        <v>317</v>
+      </c>
+      <c r="D3" s="103" t="s">
+        <v>319</v>
+      </c>
+      <c r="E3" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F3" s="93" t="s">
+        <v>275</v>
+      </c>
+      <c r="H3" s="92" t="s">
+        <v>304</v>
       </c>
       <c r="J3" s="93"/>
     </row>
@@ -3371,18 +3411,21 @@
         <v>1.3</v>
       </c>
       <c r="B4" t="s">
-        <v>301</v>
-      </c>
-      <c r="C4" s="95">
+        <v>299</v>
+      </c>
+      <c r="C4" s="101">
         <v>7</v>
       </c>
       <c r="D4" s="92">
         <v>1.2</v>
       </c>
-      <c r="F4" s="92" t="s">
-        <v>306</v>
-      </c>
-      <c r="H4" s="93"/>
+      <c r="E4" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F4" s="93"/>
+      <c r="H4" s="92" t="s">
+        <v>304</v>
+      </c>
       <c r="J4" s="93"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3392,18 +3435,21 @@
       <c r="B5" t="s">
         <v>271</v>
       </c>
-      <c r="C5" s="92">
-        <v>2.2000000000000002</v>
+      <c r="C5" s="100" t="s">
+        <v>317</v>
       </c>
       <c r="D5" s="92">
         <v>1.3</v>
       </c>
-      <c r="F5" s="92" t="s">
-        <v>310</v>
-      </c>
-      <c r="H5" s="93"/>
+      <c r="E5" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F5" s="93"/>
+      <c r="H5" s="92" t="s">
+        <v>308</v>
+      </c>
       <c r="J5" s="94" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3413,17 +3459,20 @@
       <c r="B6" t="s">
         <v>253</v>
       </c>
-      <c r="C6" s="92">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F6" s="92" t="s">
+      <c r="C6" s="100" t="s">
+        <v>317</v>
+      </c>
+      <c r="E6" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F6" s="93" t="s">
+        <v>276</v>
+      </c>
+      <c r="H6" s="92" t="s">
+        <v>305</v>
+      </c>
+      <c r="J6" s="92" t="s">
         <v>307</v>
-      </c>
-      <c r="H6" s="93" t="s">
-        <v>277</v>
-      </c>
-      <c r="J6" s="92" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3433,17 +3482,14 @@
       <c r="B7" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="92">
+      <c r="C7" s="100">
         <v>3</v>
       </c>
       <c r="E7" s="92" t="s">
-        <v>272</v>
-      </c>
-      <c r="G7" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H7" s="93" t="s">
-        <v>278</v>
+        <v>274</v>
+      </c>
+      <c r="F7" s="93" t="s">
+        <v>277</v>
       </c>
       <c r="I7" s="92" t="s">
         <v>272</v>
@@ -3456,18 +3502,18 @@
       <c r="B8" s="97" t="s">
         <v>256</v>
       </c>
-      <c r="C8" s="96">
+      <c r="C8" s="102">
         <v>4</v>
       </c>
       <c r="D8" s="96"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96" t="s">
-        <v>275</v>
-      </c>
-      <c r="H8" s="98"/>
-      <c r="J8" s="95" t="s">
-        <v>320</v>
+      <c r="E8" s="96" t="s">
+        <v>274</v>
+      </c>
+      <c r="F8" s="98"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="95"/>
+      <c r="J8" s="104" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3475,22 +3521,22 @@
         <v>255</v>
       </c>
       <c r="E9" s="92" t="s">
-        <v>272</v>
-      </c>
-      <c r="F9" s="92" t="s">
-        <v>308</v>
+        <v>274</v>
+      </c>
+      <c r="F9" s="93" t="s">
+        <v>266</v>
       </c>
       <c r="G9" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H9" s="93" t="s">
-        <v>266</v>
+        <v>274</v>
+      </c>
+      <c r="H9" s="92" t="s">
+        <v>306</v>
       </c>
       <c r="I9" s="92" t="s">
         <v>272</v>
       </c>
       <c r="J9" s="92" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3500,356 +3546,389 @@
       <c r="B10" t="s">
         <v>257</v>
       </c>
-      <c r="C10" s="92">
+      <c r="C10" s="100">
         <v>5</v>
       </c>
       <c r="D10" s="92">
         <v>1.4</v>
       </c>
-      <c r="G10" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H10" s="93" t="s">
-        <v>279</v>
+      <c r="E10" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F10" s="93" t="s">
+        <v>278</v>
       </c>
       <c r="I10" s="92" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="J10" s="92" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="92">
-        <v>4</v>
-      </c>
       <c r="B11" t="s">
-        <v>258</v>
-      </c>
-      <c r="C11" s="92">
-        <v>6</v>
-      </c>
-      <c r="D11" s="92" t="s">
-        <v>293</v>
-      </c>
-      <c r="F11" s="92" t="s">
-        <v>302</v>
+        <v>286</v>
+      </c>
+      <c r="F11" s="93" t="s">
+        <v>324</v>
       </c>
       <c r="G11" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H11" s="93" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="I11" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="J11" s="92" t="s">
-        <v>314</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="92">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
-      </c>
-      <c r="C12" s="92">
-        <v>7</v>
-      </c>
-      <c r="D12" s="92">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F12" s="92" t="s">
-        <v>303</v>
-      </c>
-      <c r="G12" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H12" s="93" t="s">
-        <v>281</v>
-      </c>
-      <c r="I12" s="92" t="s">
-        <v>275</v>
+        <v>258</v>
+      </c>
+      <c r="C12" s="100">
+        <v>6</v>
+      </c>
+      <c r="D12" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="E12" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F12" s="93" t="s">
+        <v>279</v>
+      </c>
+      <c r="H12" s="92" t="s">
+        <v>300</v>
       </c>
       <c r="J12" s="92" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="92">
-        <v>6.1</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>296</v>
-      </c>
-      <c r="C13" s="92">
-        <v>8</v>
-      </c>
-      <c r="D13" s="92">
-        <v>3</v>
-      </c>
-      <c r="F13" s="92" t="s">
-        <v>304</v>
-      </c>
-      <c r="H13" s="93"/>
+        <v>259</v>
+      </c>
+      <c r="C13" s="100">
+        <v>7</v>
+      </c>
+      <c r="D13" s="103" t="s">
+        <v>320</v>
+      </c>
+      <c r="E13" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F13" s="93" t="s">
+        <v>280</v>
+      </c>
+      <c r="H13" s="92" t="s">
+        <v>301</v>
+      </c>
+      <c r="J13" s="92" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="92">
-        <v>6.2</v>
-      </c>
       <c r="B14" t="s">
-        <v>294</v>
-      </c>
-      <c r="C14" s="92">
-        <v>8</v>
-      </c>
-      <c r="D14" s="92" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="F14" s="92" t="s">
-        <v>305</v>
-      </c>
-      <c r="H14" s="93"/>
+        <v>322</v>
+      </c>
+      <c r="G14" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="I14" s="92" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="92">
-        <v>7.1</v>
+        <v>6.1</v>
       </c>
       <c r="B15" t="s">
-        <v>260</v>
-      </c>
-      <c r="C15" s="92">
+        <v>295</v>
+      </c>
+      <c r="C15" s="100">
         <v>8</v>
       </c>
-      <c r="D15" s="92" t="s">
-        <v>295</v>
-      </c>
-      <c r="F15" s="92" t="s">
-        <v>313</v>
-      </c>
-      <c r="G15" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H15" s="93" t="s">
-        <v>282</v>
-      </c>
-      <c r="J15" s="92" t="s">
-        <v>314</v>
+      <c r="D15" s="92">
+        <v>3</v>
+      </c>
+      <c r="F15" s="93"/>
+      <c r="H15" s="92" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="92">
-        <v>7.2</v>
+        <v>6.2</v>
       </c>
       <c r="B16" t="s">
-        <v>290</v>
-      </c>
-      <c r="H16" s="93"/>
+        <v>293</v>
+      </c>
+      <c r="C16" s="100">
+        <v>8</v>
+      </c>
+      <c r="D16" s="92" t="s">
+        <v>296</v>
+      </c>
+      <c r="F16" s="93"/>
+      <c r="H16" s="92" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="92">
-        <v>9.1</v>
+        <v>7.1</v>
       </c>
       <c r="B17" t="s">
-        <v>261</v>
-      </c>
-      <c r="C17" s="92">
-        <v>9</v>
-      </c>
-      <c r="D17" s="92">
-        <v>6.2</v>
-      </c>
-      <c r="F17" s="92">
-        <v>6.6</v>
-      </c>
-      <c r="G17" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H17" s="93" t="s">
+        <v>260</v>
+      </c>
+      <c r="C17" s="100">
+        <v>8</v>
+      </c>
+      <c r="D17" s="92" t="s">
+        <v>294</v>
+      </c>
+      <c r="E17" s="92" t="s">
         <v>274</v>
       </c>
-      <c r="I17" s="92" t="s">
-        <v>275</v>
+      <c r="F17" s="93" t="s">
+        <v>281</v>
+      </c>
+      <c r="H17" s="92" t="s">
+        <v>311</v>
       </c>
       <c r="J17" s="92" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="92">
-        <v>9.1999999999999993</v>
+        <v>7.2</v>
       </c>
       <c r="B18" t="s">
-        <v>262</v>
-      </c>
-      <c r="C18" s="92">
-        <v>10</v>
-      </c>
-      <c r="D18" s="92">
-        <v>6.3</v>
-      </c>
-      <c r="G18" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H18" s="93"/>
+        <v>289</v>
+      </c>
+      <c r="F18" s="93"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="92">
-        <v>9.3000000000000007</v>
+        <v>9.1</v>
       </c>
       <c r="B19" t="s">
-        <v>263</v>
-      </c>
-      <c r="C19" s="92">
-        <v>11</v>
+        <v>325</v>
       </c>
       <c r="D19" s="92">
-        <v>6.4</v>
-      </c>
-      <c r="F19" s="92">
-        <v>7.1</v>
-      </c>
-      <c r="G19" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H19" s="93"/>
+        <v>6.1</v>
+      </c>
+      <c r="F19" s="93" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="92">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B20" t="s">
+        <v>261</v>
+      </c>
+      <c r="C20" s="100">
+        <v>9</v>
+      </c>
+      <c r="D20" s="92">
+        <v>6.2</v>
+      </c>
+      <c r="E20" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="H20" s="92">
+        <v>6.6</v>
+      </c>
+      <c r="J20" s="92" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="92">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="B21" t="s">
+        <v>262</v>
+      </c>
+      <c r="C21" s="100">
+        <v>10</v>
+      </c>
+      <c r="D21" s="92">
+        <v>6.3</v>
+      </c>
+      <c r="E21" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F21" s="93"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="92">
         <v>9.4</v>
       </c>
-      <c r="B20" t="s">
-        <v>298</v>
-      </c>
-      <c r="C20" s="92" t="s">
-        <v>316</v>
-      </c>
-      <c r="D20" s="92">
+      <c r="B22" t="s">
+        <v>263</v>
+      </c>
+      <c r="C22" s="100">
+        <v>11</v>
+      </c>
+      <c r="D22" s="92">
+        <v>6.4</v>
+      </c>
+      <c r="E22" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F22" s="93"/>
+      <c r="H22" s="92">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="92">
+        <v>9.5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>297</v>
+      </c>
+      <c r="C23" s="100" t="s">
+        <v>318</v>
+      </c>
+      <c r="D23" s="92">
         <v>6.5</v>
       </c>
-      <c r="F20" s="92">
+      <c r="E23" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F23" s="93"/>
+      <c r="H23" s="92">
         <v>7.3</v>
-      </c>
-      <c r="G20" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H20" s="93"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>264</v>
-      </c>
-      <c r="C21" s="92">
-        <v>12</v>
-      </c>
-      <c r="G21" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H21" s="93" t="s">
-        <v>283</v>
-      </c>
-      <c r="I21" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="J21" s="92" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>265</v>
-      </c>
-      <c r="C22" s="92">
-        <v>13</v>
-      </c>
-      <c r="H22" s="93"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>319</v>
-      </c>
-      <c r="C23" s="92" t="s">
-        <v>315</v>
-      </c>
-      <c r="G23" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H23" s="93" t="s">
-        <v>284</v>
-      </c>
-      <c r="I23" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="J23" s="92" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>317</v>
-      </c>
-      <c r="C24" s="92" t="s">
-        <v>318</v>
-      </c>
-      <c r="H24" s="93"/>
+        <v>264</v>
+      </c>
+      <c r="C24" s="100">
+        <v>12</v>
+      </c>
+      <c r="D24" s="92">
+        <v>7</v>
+      </c>
+      <c r="E24" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="F24" s="93" t="s">
+        <v>282</v>
+      </c>
+      <c r="J24" s="92" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>292</v>
-      </c>
-      <c r="E25" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H25" s="93"/>
+        <v>285</v>
+      </c>
+      <c r="F25" s="92" t="s">
+        <v>323</v>
+      </c>
+      <c r="G25" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="I25" s="92" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>265</v>
+      </c>
+      <c r="C26" s="100">
+        <v>13</v>
+      </c>
+      <c r="D26" s="92">
+        <v>8</v>
+      </c>
+      <c r="F26" s="93"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>287</v>
+        <v>314</v>
+      </c>
+      <c r="C27" s="100" t="s">
+        <v>318</v>
+      </c>
+      <c r="D27" s="92">
+        <v>8.1</v>
       </c>
       <c r="E27" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="H27" s="93"/>
-      <c r="I27" s="92" t="s">
-        <v>275</v>
+        <v>274</v>
+      </c>
+      <c r="F27" s="93" t="s">
+        <v>283</v>
+      </c>
+      <c r="J27" s="92" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>285</v>
-      </c>
-      <c r="E28" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="I28" s="92" t="s">
-        <v>275</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="C28" s="100" t="s">
+        <v>318</v>
+      </c>
+      <c r="D28" s="103" t="s">
+        <v>326</v>
+      </c>
+      <c r="F28" s="93"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>286</v>
-      </c>
-      <c r="E29" s="92" t="s">
-        <v>275</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="D29" s="103" t="s">
+        <v>327</v>
+      </c>
+      <c r="F29" s="93"/>
       <c r="I29" s="92" t="s">
-        <v>275</v>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="92">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>287</v>
+      </c>
+      <c r="C30" s="100">
+        <v>15</v>
+      </c>
+      <c r="G30" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="I30" s="92" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="92">
+        <v>16</v>
+      </c>
       <c r="B31" t="s">
         <v>288</v>
       </c>
-      <c r="C31" s="92">
-        <v>15</v>
-      </c>
-      <c r="E31" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="I31" s="92" t="s">
-        <v>275</v>
+      <c r="G31" s="92" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3857,15 +3936,7 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="92">
-        <v>16</v>
-      </c>
-      <c r="B36" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -3877,7 +3948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
@@ -4060,7 +4131,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="62" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="62" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="59">
         <v>5</v>
       </c>
@@ -4126,7 +4197,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="62" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="62" customFormat="1" ht="270" x14ac:dyDescent="0.25">
       <c r="A8" s="59">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
start to add links to quiz
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH315/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D23677-DF47-42D9-AC01-040168F2C1A6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E1B07F-B68D-0641-B9CC-BFBACFA2BAF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topic_overview" sheetId="9" r:id="rId1"/>
@@ -21,17 +21,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">points!$A$1:$D$89</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -41,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="389">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1275,13 +1269,7 @@
     <t>Topic</t>
   </si>
   <si>
-    <t>PDS Video</t>
-  </si>
-  <si>
     <t>Overview</t>
-  </si>
-  <si>
-    <t>Course Packet</t>
   </si>
   <si>
     <t>Other Notes</t>
@@ -1694,6 +1682,20 @@
   </si>
   <si>
     <t>foundations worksheet</t>
+  </si>
+  <si>
+    <t>PDS
+Video</t>
+  </si>
+  <si>
+    <t>Course
+Packet</t>
+  </si>
+  <si>
+    <t>Quiz Link</t>
+  </si>
+  <si>
+    <t>Working with R Studio IDE</t>
   </si>
 </sst>
 </file>
@@ -2147,7 +2149,7 @@
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2394,9 +2396,6 @@
     <xf numFmtId="0" fontId="30" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="5" xfId="82" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2405,6 +2404,12 @@
     </xf>
     <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="5" xfId="82" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="82" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2827,31 +2832,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9" style="92"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.75" style="107" customWidth="1"/>
-    <col min="5" max="5" width="13.875" style="92" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="106" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="92" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="92" customWidth="1"/>
-    <col min="7" max="7" width="22.375" style="92" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.625" style="92" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.375" style="92" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.375" style="92" customWidth="1"/>
-    <col min="11" max="11" width="31.625" style="92" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.875" style="92" customWidth="1"/>
-    <col min="13" max="13" width="28.75" style="92" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="92" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="92" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="92" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="21.33203125" style="92" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" style="92" customWidth="1"/>
+    <col min="13" max="13" width="31.6640625" style="92" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" style="92" customWidth="1"/>
+    <col min="15" max="15" width="28.6640625" style="92" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="92" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="92" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="97" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B1" s="91" t="s">
         <v>23</v>
@@ -2859,11 +2865,11 @@
       <c r="C1" s="91" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="106" t="s">
-        <v>248</v>
-      </c>
-      <c r="E1" s="91" t="s">
-        <v>250</v>
+      <c r="D1" s="109" t="s">
+        <v>385</v>
+      </c>
+      <c r="E1" s="110" t="s">
+        <v>386</v>
       </c>
       <c r="F1" s="91" t="s">
         <v>198</v>
@@ -2872,869 +2878,924 @@
         <v>7</v>
       </c>
       <c r="H1" s="91" t="s">
-        <v>306</v>
-      </c>
-      <c r="I1" s="97" t="s">
-        <v>289</v>
+        <v>304</v>
+      </c>
+      <c r="I1" s="91" t="s">
+        <v>326</v>
       </c>
       <c r="J1" s="97" t="s">
-        <v>328</v>
+        <v>387</v>
       </c>
       <c r="K1" s="97" t="s">
-        <v>313</v>
+        <v>287</v>
       </c>
       <c r="L1" s="97" t="s">
-        <v>251</v>
+        <v>326</v>
       </c>
       <c r="M1" s="97" t="s">
+        <v>311</v>
+      </c>
+      <c r="N1" s="97" t="s">
+        <v>249</v>
+      </c>
+      <c r="O1" s="97" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="98">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D2" s="107" t="s">
-        <v>353</v>
+        <v>248</v>
+      </c>
+      <c r="D2" s="106" t="s">
+        <v>351</v>
       </c>
       <c r="E2" s="92" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G2" s="92" t="s">
-        <v>269</v>
-      </c>
-      <c r="I2" s="98"/>
+        <v>267</v>
+      </c>
+      <c r="I2" s="92" t="s">
+        <v>388</v>
+      </c>
       <c r="J2" s="98"/>
       <c r="K2" s="98"/>
-      <c r="L2" s="98" t="s">
-        <v>268</v>
-      </c>
-      <c r="M2" s="100" t="s">
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2" s="100" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="98">
         <v>1.2</v>
       </c>
       <c r="C3" t="s">
-        <v>267</v>
-      </c>
-      <c r="D3" s="107" t="s">
-        <v>354</v>
+        <v>265</v>
+      </c>
+      <c r="D3" s="106" t="s">
+        <v>352</v>
       </c>
       <c r="E3" s="96" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F3" s="92" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G3" s="92" t="s">
-        <v>274</v>
-      </c>
-      <c r="I3" s="98" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
       <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
+      <c r="K3" s="98" t="s">
+        <v>291</v>
+      </c>
       <c r="L3" s="98"/>
-      <c r="M3" s="100"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="100"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="98">
         <v>1.3</v>
       </c>
       <c r="C4" t="s">
-        <v>290</v>
-      </c>
-      <c r="D4" s="108"/>
+        <v>288</v>
+      </c>
+      <c r="D4" s="107"/>
       <c r="E4" s="92">
         <v>1.2</v>
       </c>
       <c r="F4" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I4" s="98" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
+      <c r="K4" s="98" t="s">
+        <v>291</v>
+      </c>
       <c r="L4" s="98"/>
-      <c r="M4" s="100"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="100"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="98">
         <v>1.4</v>
       </c>
       <c r="C5" t="s">
-        <v>270</v>
-      </c>
-      <c r="D5" s="107" t="s">
-        <v>377</v>
+        <v>268</v>
+      </c>
+      <c r="D5" s="106" t="s">
+        <v>375</v>
       </c>
       <c r="E5" s="92">
         <v>1.3</v>
       </c>
       <c r="F5" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98" t="s">
-        <v>297</v>
-      </c>
-      <c r="K5" s="98" t="s">
-        <v>315</v>
-      </c>
-      <c r="L5" s="98"/>
-      <c r="M5" s="101" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="I5" s="92" t="s">
+        <v>295</v>
+      </c>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98" t="s">
+        <v>295</v>
+      </c>
+      <c r="M5" s="98" t="s">
+        <v>313</v>
+      </c>
+      <c r="N5" s="98"/>
+      <c r="O5" s="101" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="98">
         <v>2.1</v>
       </c>
       <c r="B6" s="92" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C6" t="s">
-        <v>253</v>
-      </c>
-      <c r="D6" s="107" t="s">
-        <v>378</v>
+        <v>251</v>
+      </c>
+      <c r="D6" s="106" t="s">
+        <v>376</v>
       </c>
       <c r="F6" s="92" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="92" t="s">
         <v>273</v>
       </c>
-      <c r="G6" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98" t="s">
+      <c r="I6" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98" t="s">
+        <v>292</v>
+      </c>
+      <c r="M6" s="98" t="s">
+        <v>312</v>
+      </c>
+      <c r="N6" s="98"/>
+      <c r="O6" s="98" t="s">
         <v>294</v>
       </c>
-      <c r="K6" s="98" t="s">
-        <v>314</v>
-      </c>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="98">
         <v>2.2000000000000002</v>
       </c>
       <c r="C7" t="s">
-        <v>254</v>
-      </c>
-      <c r="D7" s="107" t="s">
-        <v>355</v>
+        <v>252</v>
+      </c>
+      <c r="D7" s="106" t="s">
+        <v>353</v>
       </c>
       <c r="F7" s="92" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G7" s="92" t="s">
-        <v>382</v>
-      </c>
-      <c r="I7" s="98"/>
+        <v>380</v>
+      </c>
       <c r="J7" s="98"/>
-      <c r="K7" s="98" t="s">
-        <v>316</v>
-      </c>
-      <c r="L7" s="98" t="s">
-        <v>271</v>
-      </c>
-      <c r="M7" s="98"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98" t="s">
+        <v>314</v>
+      </c>
+      <c r="N7" s="98" t="s">
+        <v>269</v>
+      </c>
+      <c r="O7" s="98"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="99">
         <v>3.1</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C8" s="95" t="s">
-        <v>256</v>
-      </c>
-      <c r="D8" s="109" t="s">
-        <v>356</v>
+        <v>254</v>
+      </c>
+      <c r="D8" s="108" t="s">
+        <v>354</v>
       </c>
       <c r="E8" s="94"/>
       <c r="F8" s="94" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G8" s="94"/>
-      <c r="I8" s="99"/>
       <c r="J8" s="99"/>
-      <c r="K8" s="98" t="s">
-        <v>317</v>
-      </c>
-      <c r="L8" s="102"/>
-      <c r="M8" s="103" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="98" t="s">
+        <v>315</v>
+      </c>
+      <c r="N8" s="102"/>
+      <c r="O8" s="103" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="98">
         <v>3.2</v>
       </c>
       <c r="C9" t="s">
-        <v>257</v>
-      </c>
-      <c r="D9" s="107" t="s">
-        <v>357</v>
+        <v>255</v>
+      </c>
+      <c r="D9" s="106" t="s">
+        <v>355</v>
       </c>
       <c r="E9" s="92">
         <v>1.4</v>
       </c>
       <c r="F9" s="92" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G9" s="92" t="s">
-        <v>276</v>
-      </c>
-      <c r="I9" s="98"/>
+        <v>274</v>
+      </c>
       <c r="J9" s="98"/>
-      <c r="K9" s="98" t="s">
-        <v>318</v>
-      </c>
-      <c r="L9" s="98" t="s">
-        <v>273</v>
-      </c>
+      <c r="K9" s="98"/>
+      <c r="L9" s="98"/>
       <c r="M9" s="98" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+      <c r="N9" s="98" t="s">
+        <v>271</v>
+      </c>
+      <c r="O9" s="98" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="98">
         <v>4</v>
       </c>
       <c r="B10" s="92" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C10" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="107" t="s">
-        <v>358</v>
+        <v>256</v>
+      </c>
+      <c r="D10" s="106" t="s">
+        <v>356</v>
       </c>
       <c r="E10" s="92" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F10" s="92" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G10" s="92" t="s">
-        <v>277</v>
-      </c>
-      <c r="I10" s="98" t="s">
-        <v>291</v>
-      </c>
-      <c r="J10" s="98" t="s">
-        <v>329</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="I10" s="92" t="s">
+        <v>327</v>
+      </c>
+      <c r="J10" s="98"/>
       <c r="K10" s="98" t="s">
-        <v>322</v>
-      </c>
-      <c r="L10" s="98"/>
+        <v>289</v>
+      </c>
+      <c r="L10" s="98" t="s">
+        <v>327</v>
+      </c>
       <c r="M10" s="98" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="N10" s="98"/>
+      <c r="O10" s="98" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="98">
         <v>5</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C11" t="s">
-        <v>259</v>
-      </c>
-      <c r="D11" s="107" t="s">
-        <v>359</v>
+        <v>257</v>
+      </c>
+      <c r="D11" s="106" t="s">
+        <v>357</v>
       </c>
       <c r="E11" s="96" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F11" s="92" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G11" s="92" t="s">
-        <v>278</v>
-      </c>
-      <c r="I11" s="98"/>
+        <v>276</v>
+      </c>
       <c r="J11" s="98"/>
       <c r="K11" s="98"/>
       <c r="L11" s="98"/>
       <c r="M11" s="98"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="98"/>
+      <c r="O11" s="98"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="98">
         <v>6</v>
       </c>
       <c r="B12" s="92" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F12" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="H12" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I12" s="99"/>
-      <c r="J12" s="98" t="s">
-        <v>295</v>
-      </c>
-      <c r="K12" s="98" t="s">
-        <v>321</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="I12" s="92" t="s">
+        <v>293</v>
+      </c>
+      <c r="J12" s="99"/>
+      <c r="K12" s="99"/>
       <c r="L12" s="98" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="M12" s="98" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+      <c r="N12" s="98" t="s">
+        <v>269</v>
+      </c>
+      <c r="O12" s="98" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="98">
         <v>6.1</v>
       </c>
       <c r="C13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E13" s="96"/>
       <c r="G13" s="92" t="s">
-        <v>384</v>
-      </c>
-      <c r="I13" s="98"/>
+        <v>382</v>
+      </c>
+      <c r="H13" s="92" t="s">
+        <v>271</v>
+      </c>
       <c r="J13" s="98"/>
       <c r="K13" s="98"/>
       <c r="L13" s="98"/>
       <c r="M13" s="98"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="98"/>
+      <c r="O13" s="98"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="98">
         <v>6.2</v>
       </c>
       <c r="C14" t="s">
-        <v>334</v>
-      </c>
-      <c r="D14" s="107" t="s">
-        <v>360</v>
+        <v>332</v>
+      </c>
+      <c r="D14" s="106" t="s">
+        <v>358</v>
       </c>
       <c r="E14" s="92">
         <v>3</v>
       </c>
       <c r="F14" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I14" s="104" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="J14" s="104"/>
-      <c r="K14" s="98"/>
-      <c r="L14" s="98"/>
+      <c r="K14" s="104" t="s">
+        <v>290</v>
+      </c>
+      <c r="L14" s="104"/>
       <c r="M14" s="98"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="98"/>
+      <c r="O14" s="98"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="98">
         <v>7.1</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C15" t="s">
-        <v>336</v>
-      </c>
-      <c r="D15" s="107" t="s">
-        <v>371</v>
+        <v>334</v>
+      </c>
+      <c r="D15" s="106" t="s">
+        <v>369</v>
       </c>
       <c r="E15" s="92" t="s">
-        <v>335</v>
-      </c>
-      <c r="I15" s="98" t="s">
         <v>333</v>
       </c>
       <c r="J15" s="98"/>
-      <c r="K15" s="98"/>
+      <c r="K15" s="98" t="s">
+        <v>331</v>
+      </c>
       <c r="L15" s="98"/>
       <c r="M15" s="98"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="98"/>
+      <c r="O15" s="98"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="98">
         <v>7.2</v>
       </c>
       <c r="C16" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E16" s="92">
         <v>4.5</v>
       </c>
-      <c r="I16" s="98">
+      <c r="J16" s="98"/>
+      <c r="K16" s="98">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J16" s="98"/>
-      <c r="K16" s="98"/>
       <c r="L16" s="98"/>
       <c r="M16" s="98"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="98"/>
+      <c r="O16" s="98"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="98">
         <v>7.3</v>
       </c>
       <c r="C17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G17" s="92" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H17" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I17" s="98"/>
+        <v>271</v>
+      </c>
       <c r="J17" s="98"/>
       <c r="K17" s="98"/>
-      <c r="L17" s="98" t="s">
-        <v>273</v>
-      </c>
+      <c r="L17" s="98"/>
       <c r="M17" s="98"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="98" t="s">
+        <v>271</v>
+      </c>
+      <c r="O17" s="98"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="98">
         <v>8</v>
       </c>
       <c r="B18" s="92" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G18" s="92" t="s">
-        <v>380</v>
-      </c>
-      <c r="I18" s="98"/>
+        <v>378</v>
+      </c>
       <c r="J18" s="98"/>
       <c r="K18" s="98"/>
       <c r="L18" s="98"/>
       <c r="M18" s="98"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="98"/>
+      <c r="O18" s="98"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="98">
         <v>9.1</v>
       </c>
       <c r="B19" s="92" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C19" t="s">
-        <v>260</v>
-      </c>
-      <c r="D19" s="107" t="s">
-        <v>372</v>
+        <v>258</v>
+      </c>
+      <c r="D19" s="106" t="s">
+        <v>370</v>
       </c>
       <c r="E19" s="92" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F19" s="92" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G19" s="92" t="s">
-        <v>386</v>
-      </c>
-      <c r="I19" s="105" t="s">
-        <v>330</v>
+        <v>384</v>
       </c>
       <c r="J19" s="105"/>
-      <c r="K19" s="98" t="s">
-        <v>323</v>
-      </c>
-      <c r="L19" s="98"/>
+      <c r="K19" s="105" t="s">
+        <v>328</v>
+      </c>
+      <c r="L19" s="105"/>
       <c r="M19" s="98" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="N19" s="98"/>
+      <c r="O19" s="98" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="98">
         <v>9.1999999999999993</v>
       </c>
       <c r="C20" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E20" s="92">
         <v>6.1</v>
       </c>
       <c r="G20" s="92" t="s">
-        <v>272</v>
-      </c>
-      <c r="I20" s="98"/>
+        <v>270</v>
+      </c>
       <c r="J20" s="98"/>
       <c r="K20" s="98"/>
       <c r="L20" s="98"/>
       <c r="M20" s="98"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="98"/>
+      <c r="O20" s="98"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="98">
         <v>10.1</v>
       </c>
       <c r="B21" s="92" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C21" t="s">
-        <v>261</v>
-      </c>
-      <c r="D21" s="107" t="s">
-        <v>361</v>
+        <v>259</v>
+      </c>
+      <c r="D21" s="106" t="s">
+        <v>359</v>
       </c>
       <c r="E21" s="92">
         <v>6.2</v>
       </c>
       <c r="F21" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I21" s="98">
+        <v>271</v>
+      </c>
+      <c r="J21" s="98"/>
+      <c r="K21" s="98">
         <v>6.6</v>
-      </c>
-      <c r="J21" s="98"/>
-      <c r="K21" s="98" t="s">
-        <v>319</v>
       </c>
       <c r="L21" s="98"/>
       <c r="M21" s="98" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+      <c r="N21" s="98"/>
+      <c r="O21" s="98" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="98">
         <v>10.199999999999999</v>
       </c>
       <c r="C22" t="s">
-        <v>262</v>
-      </c>
-      <c r="D22" s="107" t="s">
-        <v>362</v>
+        <v>260</v>
+      </c>
+      <c r="D22" s="106" t="s">
+        <v>360</v>
       </c>
       <c r="E22" s="92">
         <v>6.3</v>
       </c>
       <c r="F22" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I22" s="98"/>
+        <v>271</v>
+      </c>
       <c r="J22" s="98"/>
-      <c r="K22" s="98" t="s">
-        <v>325</v>
-      </c>
+      <c r="K22" s="98"/>
       <c r="L22" s="98"/>
-      <c r="M22" s="98"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="98" t="s">
+        <v>323</v>
+      </c>
+      <c r="N22" s="98"/>
+      <c r="O22" s="98"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="98">
         <v>11</v>
       </c>
       <c r="B23" s="92" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C23" t="s">
-        <v>263</v>
-      </c>
-      <c r="D23" s="107" t="s">
-        <v>363</v>
+        <v>261</v>
+      </c>
+      <c r="D23" s="106" t="s">
+        <v>361</v>
       </c>
       <c r="E23" s="92">
         <v>6.4</v>
       </c>
       <c r="F23" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I23" s="98">
+        <v>271</v>
+      </c>
+      <c r="J23" s="98"/>
+      <c r="K23" s="98">
         <v>7.1</v>
       </c>
-      <c r="J23" s="98"/>
-      <c r="K23" s="98" t="s">
-        <v>320</v>
-      </c>
       <c r="L23" s="98"/>
-      <c r="M23" s="98"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="98" t="s">
+        <v>318</v>
+      </c>
+      <c r="N23" s="98"/>
+      <c r="O23" s="98"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="98">
         <v>11.1</v>
       </c>
       <c r="C24" t="s">
-        <v>337</v>
-      </c>
-      <c r="D24" s="107" t="s">
-        <v>368</v>
+        <v>335</v>
+      </c>
+      <c r="D24" s="106" t="s">
+        <v>366</v>
       </c>
       <c r="E24" s="92">
         <v>6.5</v>
       </c>
       <c r="F24" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I24" s="98">
+        <v>271</v>
+      </c>
+      <c r="J24" s="98"/>
+      <c r="K24" s="98">
         <v>7.3</v>
       </c>
-      <c r="J24" s="98"/>
-      <c r="K24" s="98" t="s">
-        <v>324</v>
-      </c>
       <c r="L24" s="98"/>
-      <c r="M24" s="98"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="98" t="s">
+        <v>322</v>
+      </c>
+      <c r="N24" s="98"/>
+      <c r="O24" s="98"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="98">
         <v>11.2</v>
       </c>
       <c r="C25" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G25" s="92" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H25" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I25" s="98"/>
+        <v>271</v>
+      </c>
       <c r="J25" s="98"/>
       <c r="K25" s="98"/>
-      <c r="L25" s="98" t="s">
-        <v>273</v>
-      </c>
+      <c r="L25" s="98"/>
       <c r="M25" s="98"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="98" t="s">
+        <v>271</v>
+      </c>
+      <c r="O25" s="98"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="98">
         <v>12</v>
       </c>
       <c r="B26" s="92" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C26" t="s">
-        <v>264</v>
-      </c>
-      <c r="D26" s="107" t="s">
-        <v>364</v>
+        <v>262</v>
+      </c>
+      <c r="D26" s="106" t="s">
+        <v>362</v>
       </c>
       <c r="E26" s="92">
         <v>7</v>
       </c>
       <c r="F26" s="92" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G26" s="92" t="s">
-        <v>279</v>
-      </c>
-      <c r="I26" s="98"/>
+        <v>277</v>
+      </c>
       <c r="J26" s="98"/>
-      <c r="K26" s="98" t="s">
-        <v>326</v>
-      </c>
+      <c r="K26" s="98"/>
       <c r="L26" s="98"/>
       <c r="M26" s="98" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="N26" s="98"/>
+      <c r="O26" s="98" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="98">
         <v>12.2</v>
       </c>
       <c r="C27" t="s">
-        <v>265</v>
-      </c>
-      <c r="D27" s="107" t="s">
-        <v>366</v>
-      </c>
-      <c r="I27" s="98"/>
+        <v>263</v>
+      </c>
+      <c r="D27" s="106" t="s">
+        <v>364</v>
+      </c>
       <c r="J27" s="98"/>
       <c r="K27" s="98"/>
       <c r="L27" s="98"/>
       <c r="M27" s="98"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="98"/>
+      <c r="O27" s="98"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="98">
         <v>12.3</v>
       </c>
       <c r="C28" t="s">
-        <v>374</v>
-      </c>
-      <c r="D28" s="107" t="s">
-        <v>365</v>
+        <v>372</v>
+      </c>
+      <c r="D28" s="106" t="s">
+        <v>363</v>
       </c>
       <c r="E28" s="96" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F28" s="92" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G28" s="92" t="s">
-        <v>280</v>
-      </c>
-      <c r="I28" s="98"/>
+        <v>278</v>
+      </c>
       <c r="J28" s="98"/>
-      <c r="K28" s="98" t="s">
-        <v>327</v>
-      </c>
+      <c r="K28" s="98"/>
       <c r="L28" s="98"/>
       <c r="M28" s="98" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+      <c r="N28" s="98"/>
+      <c r="O28" s="98" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="98">
         <v>12.4</v>
       </c>
       <c r="C29" t="s">
-        <v>373</v>
-      </c>
-      <c r="D29" s="107" t="s">
-        <v>376</v>
+        <v>371</v>
+      </c>
+      <c r="D29" s="106" t="s">
+        <v>374</v>
       </c>
       <c r="E29" s="96" t="s">
-        <v>369</v>
-      </c>
-      <c r="I29" s="98"/>
+        <v>367</v>
+      </c>
       <c r="J29" s="98"/>
       <c r="K29" s="98"/>
       <c r="L29" s="98"/>
       <c r="M29" s="98"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="98"/>
+      <c r="O29" s="98"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="98">
         <v>13</v>
       </c>
       <c r="B30" s="92" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C30" t="s">
-        <v>301</v>
-      </c>
-      <c r="D30" s="107" t="s">
-        <v>379</v>
+        <v>299</v>
+      </c>
+      <c r="D30" s="106" t="s">
+        <v>377</v>
       </c>
       <c r="E30" s="96" t="s">
-        <v>370</v>
-      </c>
-      <c r="I30" s="98"/>
+        <v>368</v>
+      </c>
       <c r="J30" s="98"/>
       <c r="K30" s="98"/>
       <c r="L30" s="98"/>
       <c r="M30" s="98"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="98"/>
+      <c r="O30" s="98"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="98">
         <v>14.1</v>
       </c>
       <c r="B31" s="92" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C31" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G31" s="92" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H31" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I31" s="98"/>
+        <v>271</v>
+      </c>
       <c r="J31" s="98"/>
       <c r="K31" s="98"/>
-      <c r="L31" s="98" t="s">
-        <v>273</v>
-      </c>
+      <c r="L31" s="98"/>
       <c r="M31" s="98"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="98" t="s">
+        <v>271</v>
+      </c>
+      <c r="O31" s="98"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="98">
         <v>14.2</v>
       </c>
       <c r="C32" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E32" s="96">
         <v>8.4</v>
       </c>
       <c r="G32" s="93"/>
-      <c r="I32" s="98"/>
       <c r="J32" s="98"/>
       <c r="K32" s="98"/>
-      <c r="L32" s="98" t="s">
-        <v>273</v>
-      </c>
+      <c r="L32" s="98"/>
       <c r="M32" s="98"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="98" t="s">
+        <v>271</v>
+      </c>
+      <c r="O32" s="98"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="98">
         <v>15</v>
       </c>
       <c r="B33" s="92" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C33" t="s">
-        <v>284</v>
-      </c>
-      <c r="D33" s="107" t="s">
-        <v>367</v>
+        <v>282</v>
+      </c>
+      <c r="D33" s="106" t="s">
+        <v>365</v>
       </c>
       <c r="H33" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I33" s="98"/>
+        <v>271</v>
+      </c>
       <c r="J33" s="98"/>
       <c r="K33" s="98"/>
-      <c r="L33" s="98" t="s">
-        <v>273</v>
-      </c>
+      <c r="L33" s="98"/>
       <c r="M33" s="98"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="98" t="s">
+        <v>271</v>
+      </c>
+      <c r="O33" s="98"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="98">
         <v>16</v>
       </c>
       <c r="B34" s="92" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C34" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H34" s="92" t="s">
-        <v>273</v>
-      </c>
-      <c r="I34" s="98"/>
+        <v>271</v>
+      </c>
       <c r="J34" s="98"/>
       <c r="K34" s="98"/>
       <c r="L34" s="98"/>
       <c r="M34" s="98"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="98"/>
+      <c r="O34" s="98"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="98">
         <v>16.100000000000001</v>
       </c>
       <c r="C35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G35" s="92" t="s">
-        <v>381</v>
-      </c>
-      <c r="I35" s="98"/>
+        <v>379</v>
+      </c>
       <c r="J35" s="98"/>
       <c r="K35" s="98"/>
       <c r="L35" s="98"/>
       <c r="M35" s="98"/>
+      <c r="N35" s="98"/>
+      <c r="O35" s="98"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M41">
+  <sortState ref="A2:O41">
     <sortCondition ref="A2:A41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3751,20 +3812,20 @@
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="36" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="36" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="36" customWidth="1"/>
-    <col min="3" max="3" width="33.625" style="36" customWidth="1"/>
-    <col min="4" max="4" width="36.125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="47.625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="45.875" style="37" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" style="37" customWidth="1"/>
     <col min="7" max="7" width="61" style="37" customWidth="1"/>
     <col min="8" max="8" width="46.5" style="37" customWidth="1"/>
-    <col min="9" max="16384" width="14.875" style="36"/>
+    <col min="9" max="16384" width="14.83203125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
@@ -3790,7 +3851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="62" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="62" customFormat="1" ht="272" x14ac:dyDescent="0.2">
       <c r="A2" s="59">
         <v>1</v>
       </c>
@@ -3816,7 +3877,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="62" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="62" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A3" s="59">
         <v>2</v>
       </c>
@@ -3843,7 +3904,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="62" customFormat="1" ht="285" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="62" customFormat="1" ht="304" x14ac:dyDescent="0.2">
       <c r="A4" s="59">
         <v>3</v>
       </c>
@@ -3870,7 +3931,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="62" customFormat="1" ht="360" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="62" customFormat="1" ht="365" x14ac:dyDescent="0.2">
       <c r="A5" s="59">
         <v>4</v>
       </c>
@@ -3897,7 +3958,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="62" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="62" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="59">
         <v>5</v>
       </c>
@@ -3924,7 +3985,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="62" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="62" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="59">
         <v>6</v>
       </c>
@@ -3951,7 +4012,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="62" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="62" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="A8" s="59">
         <v>7</v>
       </c>
@@ -3978,7 +4039,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="62" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="59">
         <v>8</v>
       </c>
@@ -3995,7 +4056,7 @@
       <c r="G9" s="89"/>
       <c r="H9" s="90"/>
     </row>
-    <row r="10" spans="1:8" s="62" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="62" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A10" s="59">
         <v>9</v>
       </c>
@@ -4022,7 +4083,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="62" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="62" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="59">
         <v>10</v>
       </c>
@@ -4049,7 +4110,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="62" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="62" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A12" s="59">
         <v>11</v>
       </c>
@@ -4074,7 +4135,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="62" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="62" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A13" s="59">
         <v>12</v>
       </c>
@@ -4101,14 +4162,14 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="62" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="62" customFormat="1" ht="192" x14ac:dyDescent="0.2">
       <c r="A14" s="59"/>
       <c r="B14" s="60">
         <f t="shared" si="0"/>
         <v>42108</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>185</v>
@@ -4124,7 +4185,7 @@
       </c>
       <c r="H14" s="64"/>
     </row>
-    <row r="15" spans="1:8" s="62" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="62" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="59">
         <v>13</v>
       </c>
@@ -4151,7 +4212,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="62" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="62" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -4176,7 +4237,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -4188,7 +4249,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="62" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="62" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="59" t="s">
         <v>0</v>
       </c>
@@ -4207,217 +4268,217 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D19" s="65"/>
       <c r="E19" s="65"/>
       <c r="F19" s="65"/>
       <c r="G19" s="65"/>
       <c r="H19" s="65"/>
     </row>
-    <row r="20" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D20" s="65"/>
       <c r="E20" s="65"/>
       <c r="F20" s="65"/>
       <c r="G20" s="65"/>
       <c r="H20" s="65"/>
     </row>
-    <row r="21" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D21" s="65"/>
       <c r="E21" s="65"/>
       <c r="F21" s="65"/>
       <c r="G21" s="65"/>
       <c r="H21" s="65"/>
     </row>
-    <row r="22" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D22" s="65"/>
       <c r="E22" s="65"/>
       <c r="F22" s="65"/>
       <c r="G22" s="65"/>
       <c r="H22" s="65"/>
     </row>
-    <row r="23" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D23" s="65"/>
       <c r="E23" s="65"/>
       <c r="F23" s="65"/>
       <c r="G23" s="65"/>
       <c r="H23" s="65"/>
     </row>
-    <row r="24" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D24" s="65"/>
       <c r="E24" s="65"/>
       <c r="F24" s="65"/>
       <c r="G24" s="65"/>
       <c r="H24" s="65"/>
     </row>
-    <row r="25" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D25" s="65"/>
       <c r="E25" s="65"/>
       <c r="F25" s="65"/>
       <c r="G25" s="65"/>
       <c r="H25" s="65"/>
     </row>
-    <row r="26" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D26" s="65"/>
       <c r="E26" s="65"/>
       <c r="F26" s="65"/>
       <c r="G26" s="65"/>
       <c r="H26" s="65"/>
     </row>
-    <row r="27" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D27" s="65"/>
       <c r="E27" s="65"/>
       <c r="F27" s="65"/>
       <c r="G27" s="65"/>
       <c r="H27" s="65"/>
     </row>
-    <row r="28" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D28" s="65"/>
       <c r="E28" s="65"/>
       <c r="F28" s="65"/>
       <c r="G28" s="65"/>
       <c r="H28" s="65"/>
     </row>
-    <row r="29" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D29" s="65"/>
       <c r="E29" s="65"/>
       <c r="F29" s="65"/>
       <c r="G29" s="65"/>
       <c r="H29" s="65"/>
     </row>
-    <row r="30" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D30" s="65"/>
       <c r="E30" s="65"/>
       <c r="F30" s="65"/>
       <c r="G30" s="65"/>
       <c r="H30" s="65"/>
     </row>
-    <row r="31" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D31" s="65"/>
       <c r="E31" s="65"/>
       <c r="F31" s="65"/>
       <c r="G31" s="65"/>
       <c r="H31" s="65"/>
     </row>
-    <row r="32" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D32" s="65"/>
       <c r="E32" s="65"/>
       <c r="F32" s="65"/>
       <c r="G32" s="65"/>
       <c r="H32" s="65"/>
     </row>
-    <row r="33" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D33" s="65"/>
       <c r="E33" s="65"/>
       <c r="F33" s="65"/>
       <c r="G33" s="65"/>
       <c r="H33" s="65"/>
     </row>
-    <row r="34" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D34" s="65"/>
       <c r="E34" s="65"/>
       <c r="F34" s="65"/>
       <c r="G34" s="65"/>
       <c r="H34" s="65"/>
     </row>
-    <row r="35" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D35" s="65"/>
       <c r="E35" s="65"/>
       <c r="F35" s="65"/>
       <c r="G35" s="65"/>
       <c r="H35" s="65"/>
     </row>
-    <row r="36" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D36" s="65"/>
       <c r="E36" s="65"/>
       <c r="F36" s="65"/>
       <c r="G36" s="65"/>
       <c r="H36" s="65"/>
     </row>
-    <row r="37" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D37" s="65"/>
       <c r="E37" s="65"/>
       <c r="F37" s="65"/>
       <c r="G37" s="65"/>
       <c r="H37" s="65"/>
     </row>
-    <row r="38" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D38" s="65"/>
       <c r="E38" s="65"/>
       <c r="F38" s="65"/>
       <c r="G38" s="65"/>
       <c r="H38" s="65"/>
     </row>
-    <row r="39" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D39" s="65"/>
       <c r="E39" s="65"/>
       <c r="F39" s="65"/>
       <c r="G39" s="65"/>
       <c r="H39" s="65"/>
     </row>
-    <row r="40" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D40" s="65"/>
       <c r="E40" s="65"/>
       <c r="F40" s="65"/>
       <c r="G40" s="65"/>
       <c r="H40" s="65"/>
     </row>
-    <row r="41" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D41" s="65"/>
       <c r="E41" s="65"/>
       <c r="F41" s="65"/>
       <c r="G41" s="65"/>
       <c r="H41" s="65"/>
     </row>
-    <row r="42" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D42" s="65"/>
       <c r="E42" s="65"/>
       <c r="F42" s="65"/>
       <c r="G42" s="65"/>
       <c r="H42" s="65"/>
     </row>
-    <row r="43" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D43" s="65"/>
       <c r="E43" s="65"/>
       <c r="F43" s="65"/>
       <c r="G43" s="65"/>
       <c r="H43" s="65"/>
     </row>
-    <row r="44" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D44" s="65"/>
       <c r="E44" s="65"/>
       <c r="F44" s="65"/>
       <c r="G44" s="65"/>
       <c r="H44" s="65"/>
     </row>
-    <row r="45" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D45" s="65"/>
       <c r="E45" s="65"/>
       <c r="F45" s="65"/>
       <c r="G45" s="65"/>
       <c r="H45" s="65"/>
     </row>
-    <row r="46" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D46" s="65"/>
       <c r="E46" s="65"/>
       <c r="F46" s="65"/>
       <c r="G46" s="65"/>
       <c r="H46" s="65"/>
     </row>
-    <row r="47" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D47" s="65"/>
       <c r="E47" s="65"/>
       <c r="F47" s="65"/>
       <c r="G47" s="65"/>
       <c r="H47" s="65"/>
     </row>
-    <row r="48" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D48" s="65"/>
       <c r="E48" s="65"/>
       <c r="F48" s="65"/>
       <c r="G48" s="65"/>
       <c r="H48" s="65"/>
     </row>
-    <row r="49" spans="3:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C49" s="36"/>
       <c r="D49" s="37"/>
       <c r="E49" s="37"/>
@@ -4440,21 +4501,21 @@
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="36" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="36" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="36" customWidth="1"/>
-    <col min="3" max="3" width="33.625" style="36" customWidth="1"/>
-    <col min="4" max="4" width="27.375" style="37" customWidth="1"/>
-    <col min="5" max="5" width="47.625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="45.875" style="37" customWidth="1"/>
-    <col min="7" max="7" width="30.125" style="37" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="37" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" style="37" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" style="37" customWidth="1"/>
     <col min="8" max="9" width="38" style="37" customWidth="1"/>
     <col min="10" max="10" width="46.5" style="37" customWidth="1"/>
-    <col min="11" max="16384" width="14.875" style="36"/>
+    <col min="11" max="16384" width="14.83203125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
@@ -4486,7 +4547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="62" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="62" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A2" s="59">
         <v>1</v>
       </c>
@@ -4519,7 +4580,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" s="62" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="62" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A3" s="59">
         <v>2</v>
       </c>
@@ -4552,7 +4613,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="62" customFormat="1" ht="240" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="62" customFormat="1" ht="256" x14ac:dyDescent="0.2">
       <c r="A4" s="59">
         <v>3</v>
       </c>
@@ -4585,7 +4646,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="62" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="62" customFormat="1" ht="320" x14ac:dyDescent="0.2">
       <c r="A5" s="59">
         <v>4</v>
       </c>
@@ -4618,7 +4679,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="62" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="62" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="59">
         <v>5</v>
       </c>
@@ -4651,7 +4712,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="62" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="62" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A7" s="59">
         <v>6</v>
       </c>
@@ -4684,7 +4745,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="62" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="62" customFormat="1" ht="272" x14ac:dyDescent="0.2">
       <c r="A8" s="59">
         <v>7</v>
       </c>
@@ -4717,7 +4778,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="62" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="62" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="A9" s="59">
         <v>8</v>
       </c>
@@ -4746,7 +4807,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="62" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="62" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="A10" s="59">
         <v>9</v>
       </c>
@@ -4779,7 +4840,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="62" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="62" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A11" s="59">
         <v>10</v>
       </c>
@@ -4812,7 +4873,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="62" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="62" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="A12" s="59">
         <v>11</v>
       </c>
@@ -4843,7 +4904,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="62" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="59">
         <v>12</v>
       </c>
@@ -4864,7 +4925,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="64"/>
     </row>
-    <row r="14" spans="1:11" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="62" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="59"/>
       <c r="B14" s="60">
         <f t="shared" si="0"/>
@@ -4881,7 +4942,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="63"/>
     </row>
-    <row r="15" spans="1:11" s="62" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="62" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="A15" s="59">
         <v>13</v>
       </c>
@@ -4912,7 +4973,7 @@
       </c>
       <c r="J15" s="64"/>
     </row>
-    <row r="16" spans="1:11" s="62" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="62" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -4945,7 +5006,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="62" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="62" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -4972,7 +5033,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="62" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="62" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="59" t="s">
         <v>0</v>
       </c>
@@ -4993,7 +5054,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D19" s="65"/>
       <c r="E19" s="65"/>
       <c r="F19" s="65"/>
@@ -5002,7 +5063,7 @@
       <c r="I19" s="65"/>
       <c r="J19" s="65"/>
     </row>
-    <row r="20" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D20" s="65"/>
       <c r="E20" s="65"/>
       <c r="F20" s="65"/>
@@ -5011,7 +5072,7 @@
       <c r="I20" s="65"/>
       <c r="J20" s="65"/>
     </row>
-    <row r="21" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D21" s="65"/>
       <c r="E21" s="65"/>
       <c r="F21" s="65"/>
@@ -5020,7 +5081,7 @@
       <c r="I21" s="65"/>
       <c r="J21" s="65"/>
     </row>
-    <row r="22" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D22" s="65"/>
       <c r="E22" s="65"/>
       <c r="F22" s="65"/>
@@ -5029,7 +5090,7 @@
       <c r="I22" s="65"/>
       <c r="J22" s="65"/>
     </row>
-    <row r="23" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D23" s="65"/>
       <c r="E23" s="65"/>
       <c r="F23" s="65"/>
@@ -5038,7 +5099,7 @@
       <c r="I23" s="65"/>
       <c r="J23" s="65"/>
     </row>
-    <row r="24" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D24" s="65"/>
       <c r="E24" s="65"/>
       <c r="F24" s="65"/>
@@ -5047,7 +5108,7 @@
       <c r="I24" s="65"/>
       <c r="J24" s="65"/>
     </row>
-    <row r="25" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D25" s="65"/>
       <c r="E25" s="65"/>
       <c r="F25" s="65"/>
@@ -5056,7 +5117,7 @@
       <c r="I25" s="65"/>
       <c r="J25" s="65"/>
     </row>
-    <row r="26" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D26" s="65"/>
       <c r="E26" s="65"/>
       <c r="F26" s="65"/>
@@ -5065,7 +5126,7 @@
       <c r="I26" s="65"/>
       <c r="J26" s="65"/>
     </row>
-    <row r="27" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D27" s="65"/>
       <c r="E27" s="65"/>
       <c r="F27" s="65"/>
@@ -5074,7 +5135,7 @@
       <c r="I27" s="65"/>
       <c r="J27" s="65"/>
     </row>
-    <row r="28" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D28" s="65"/>
       <c r="E28" s="65"/>
       <c r="F28" s="65"/>
@@ -5083,7 +5144,7 @@
       <c r="I28" s="65"/>
       <c r="J28" s="65"/>
     </row>
-    <row r="29" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D29" s="65"/>
       <c r="E29" s="65"/>
       <c r="F29" s="65"/>
@@ -5092,7 +5153,7 @@
       <c r="I29" s="65"/>
       <c r="J29" s="65"/>
     </row>
-    <row r="30" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D30" s="65"/>
       <c r="E30" s="65"/>
       <c r="F30" s="65"/>
@@ -5101,7 +5162,7 @@
       <c r="I30" s="65"/>
       <c r="J30" s="65"/>
     </row>
-    <row r="31" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D31" s="65"/>
       <c r="E31" s="65"/>
       <c r="F31" s="65"/>
@@ -5110,7 +5171,7 @@
       <c r="I31" s="65"/>
       <c r="J31" s="65"/>
     </row>
-    <row r="32" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D32" s="65"/>
       <c r="E32" s="65"/>
       <c r="F32" s="65"/>
@@ -5119,7 +5180,7 @@
       <c r="I32" s="65"/>
       <c r="J32" s="65"/>
     </row>
-    <row r="33" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D33" s="65"/>
       <c r="E33" s="65"/>
       <c r="F33" s="65"/>
@@ -5128,7 +5189,7 @@
       <c r="I33" s="65"/>
       <c r="J33" s="65"/>
     </row>
-    <row r="34" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D34" s="65"/>
       <c r="E34" s="65"/>
       <c r="F34" s="65"/>
@@ -5137,7 +5198,7 @@
       <c r="I34" s="65"/>
       <c r="J34" s="65"/>
     </row>
-    <row r="35" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D35" s="65"/>
       <c r="E35" s="65"/>
       <c r="F35" s="65"/>
@@ -5146,7 +5207,7 @@
       <c r="I35" s="65"/>
       <c r="J35" s="65"/>
     </row>
-    <row r="36" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D36" s="65"/>
       <c r="E36" s="65"/>
       <c r="F36" s="65"/>
@@ -5155,7 +5216,7 @@
       <c r="I36" s="65"/>
       <c r="J36" s="65"/>
     </row>
-    <row r="37" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D37" s="65"/>
       <c r="E37" s="65"/>
       <c r="F37" s="65"/>
@@ -5164,7 +5225,7 @@
       <c r="I37" s="65"/>
       <c r="J37" s="65"/>
     </row>
-    <row r="38" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D38" s="65"/>
       <c r="E38" s="65"/>
       <c r="F38" s="65"/>
@@ -5173,7 +5234,7 @@
       <c r="I38" s="65"/>
       <c r="J38" s="65"/>
     </row>
-    <row r="39" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D39" s="65"/>
       <c r="E39" s="65"/>
       <c r="F39" s="65"/>
@@ -5182,7 +5243,7 @@
       <c r="I39" s="65"/>
       <c r="J39" s="65"/>
     </row>
-    <row r="40" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D40" s="65"/>
       <c r="E40" s="65"/>
       <c r="F40" s="65"/>
@@ -5191,7 +5252,7 @@
       <c r="I40" s="65"/>
       <c r="J40" s="65"/>
     </row>
-    <row r="41" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D41" s="65"/>
       <c r="E41" s="65"/>
       <c r="F41" s="65"/>
@@ -5200,7 +5261,7 @@
       <c r="I41" s="65"/>
       <c r="J41" s="65"/>
     </row>
-    <row r="42" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D42" s="65"/>
       <c r="E42" s="65"/>
       <c r="F42" s="65"/>
@@ -5209,7 +5270,7 @@
       <c r="I42" s="65"/>
       <c r="J42" s="65"/>
     </row>
-    <row r="43" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D43" s="65"/>
       <c r="E43" s="65"/>
       <c r="F43" s="65"/>
@@ -5218,7 +5279,7 @@
       <c r="I43" s="65"/>
       <c r="J43" s="65"/>
     </row>
-    <row r="44" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D44" s="65"/>
       <c r="E44" s="65"/>
       <c r="F44" s="65"/>
@@ -5227,7 +5288,7 @@
       <c r="I44" s="65"/>
       <c r="J44" s="65"/>
     </row>
-    <row r="45" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D45" s="65"/>
       <c r="E45" s="65"/>
       <c r="F45" s="65"/>
@@ -5236,7 +5297,7 @@
       <c r="I45" s="65"/>
       <c r="J45" s="65"/>
     </row>
-    <row r="46" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D46" s="65"/>
       <c r="E46" s="65"/>
       <c r="F46" s="65"/>
@@ -5245,7 +5306,7 @@
       <c r="I46" s="65"/>
       <c r="J46" s="65"/>
     </row>
-    <row r="47" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D47" s="65"/>
       <c r="E47" s="65"/>
       <c r="F47" s="65"/>
@@ -5254,7 +5315,7 @@
       <c r="I47" s="65"/>
       <c r="J47" s="65"/>
     </row>
-    <row r="48" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D48" s="65"/>
       <c r="E48" s="65"/>
       <c r="F48" s="65"/>
@@ -5263,7 +5324,7 @@
       <c r="I48" s="65"/>
       <c r="J48" s="65"/>
     </row>
-    <row r="49" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D49" s="65"/>
       <c r="E49" s="65"/>
       <c r="F49" s="65"/>
@@ -5286,25 +5347,25 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="15"/>
-    <col min="2" max="2" width="40.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="15"/>
+    <col min="2" max="2" width="40.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="17"/>
+    <col min="4" max="4" width="7.6640625" style="17"/>
     <col min="5" max="5" width="10.5" style="39" customWidth="1"/>
-    <col min="6" max="6" width="7.625" style="39" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="39" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="5" customWidth="1"/>
     <col min="8" max="8" width="10" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.625" style="6"/>
-    <col min="10" max="10" width="4.625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="10.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="7.625" style="5"/>
+    <col min="9" max="9" width="7.6640625" style="6"/>
+    <col min="10" max="10" width="4.6640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="7.6640625" style="5"/>
     <col min="15" max="15" width="11.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="7.625" style="5"/>
+    <col min="16" max="16384" width="7.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -5370,7 +5431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <v>1.3</v>
       </c>
@@ -5433,7 +5494,7 @@
         <v>3.0837004405286344E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <v>1.4</v>
       </c>
@@ -5496,7 +5557,7 @@
         <v>0.21806167400881057</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>1.5</v>
       </c>
@@ -5559,7 +5620,7 @@
         <v>4.405286343612335E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>1.6</v>
       </c>
@@ -5607,7 +5668,7 @@
         <v>6.8281938325991193E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="75"/>
@@ -5662,7 +5723,7 @@
         <v>2.2026431718061675E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>2.2000000000000002</v>
       </c>
@@ -5725,7 +5786,7 @@
         <v>0.38546255506607929</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>2.2999999999999998</v>
       </c>
@@ -5784,7 +5845,7 @@
         <v>0.23127753303964757</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>2.4</v>
       </c>
@@ -5818,7 +5879,7 @@
       </c>
       <c r="Y9" s="15"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>2.5</v>
       </c>
@@ -5835,7 +5896,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>2.6</v>
       </c>
@@ -5850,7 +5911,7 @@
       </c>
       <c r="F11" s="44"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>3.1</v>
       </c>
@@ -5865,7 +5926,7 @@
       </c>
       <c r="F12" s="50"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>3.2</v>
       </c>
@@ -5880,7 +5941,7 @@
       </c>
       <c r="F13" s="50"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>3.3</v>
       </c>
@@ -5896,7 +5957,7 @@
       <c r="E14" s="40"/>
       <c r="F14" s="50"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>3.4</v>
       </c>
@@ -5913,7 +5974,7 @@
       <c r="G15" s="44"/>
       <c r="H15" s="44"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>3.5</v>
       </c>
@@ -5930,7 +5991,7 @@
       <c r="G16" s="44"/>
       <c r="H16" s="44"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>3.6</v>
       </c>
@@ -5948,7 +6009,7 @@
       <c r="G17" s="44"/>
       <c r="H17" s="44"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>4.0999999999999996</v>
       </c>
@@ -5966,7 +6027,7 @@
       <c r="G18" s="44"/>
       <c r="H18" s="44"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>4.2</v>
       </c>
@@ -5984,7 +6045,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>4.3</v>
       </c>
@@ -6002,7 +6063,7 @@
       <c r="G20" s="44"/>
       <c r="H20" s="44"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>4.4000000000000004</v>
       </c>
@@ -6018,7 +6079,7 @@
       <c r="E21" s="40"/>
       <c r="F21" s="68"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>4.5</v>
       </c>
@@ -6034,7 +6095,7 @@
       <c r="E22" s="40"/>
       <c r="F22" s="68"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>5.0999999999999996</v>
       </c>
@@ -6050,7 +6111,7 @@
       <c r="E23" s="40"/>
       <c r="F23" s="70"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>5.2</v>
       </c>
@@ -6066,7 +6127,7 @@
       <c r="E24" s="40"/>
       <c r="F24" s="69"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>5.3</v>
       </c>
@@ -6082,7 +6143,7 @@
       <c r="E25" s="40"/>
       <c r="F25" s="70"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>5.4</v>
       </c>
@@ -6098,7 +6159,7 @@
       <c r="E26" s="40"/>
       <c r="F26" s="69"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>6</v>
       </c>
@@ -6114,7 +6175,7 @@
       <c r="E27" s="40"/>
       <c r="F27" s="40"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
         <v>6</v>
       </c>
@@ -6128,7 +6189,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>6</v>
       </c>
@@ -6142,7 +6203,7 @@
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
         <v>6</v>
       </c>
@@ -6156,7 +6217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>6</v>
       </c>
@@ -6172,7 +6233,7 @@
       <c r="E31" s="40"/>
       <c r="F31" s="40"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
         <v>6</v>
       </c>
@@ -6188,7 +6249,7 @@
       <c r="E32" s="40"/>
       <c r="F32" s="40"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>7</v>
       </c>
@@ -6202,7 +6263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>7</v>
       </c>
@@ -6216,7 +6277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>7</v>
       </c>
@@ -6230,7 +6291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
         <v>7</v>
       </c>
@@ -6242,7 +6303,7 @@
       </c>
       <c r="D36" s="11"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>7</v>
       </c>
@@ -6256,7 +6317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
         <v>7</v>
       </c>
@@ -6270,7 +6331,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
         <v>7</v>
       </c>
@@ -6284,7 +6345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
         <v>8</v>
       </c>
@@ -6300,7 +6361,7 @@
       <c r="E40" s="40"/>
       <c r="F40" s="40"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>9</v>
       </c>
@@ -6316,7 +6377,7 @@
       <c r="E41" s="41"/>
       <c r="F41" s="40"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="9">
         <v>9</v>
       </c>
@@ -6332,7 +6393,7 @@
       <c r="E42" s="41"/>
       <c r="F42" s="40"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
         <v>9</v>
       </c>
@@ -6348,7 +6409,7 @@
       <c r="E43" s="41"/>
       <c r="F43" s="40"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
         <v>9</v>
       </c>
@@ -6364,7 +6425,7 @@
       <c r="E44" s="41"/>
       <c r="F44" s="40"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="9">
         <v>10</v>
       </c>
@@ -6380,7 +6441,7 @@
       <c r="E45" s="41"/>
       <c r="F45" s="40"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="9">
         <v>10</v>
       </c>
@@ -6396,7 +6457,7 @@
       <c r="E46" s="41"/>
       <c r="F46" s="40"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
         <v>10</v>
       </c>
@@ -6412,7 +6473,7 @@
       <c r="E47" s="41"/>
       <c r="F47" s="40"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <v>11</v>
       </c>
@@ -6428,7 +6489,7 @@
       <c r="E48" s="41"/>
       <c r="F48" s="40"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <v>11</v>
       </c>
@@ -6444,7 +6505,7 @@
       <c r="E49" s="41"/>
       <c r="F49" s="40"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
         <v>11</v>
       </c>
@@ -6460,7 +6521,7 @@
       <c r="E50" s="41"/>
       <c r="F50" s="40"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="9">
         <v>11</v>
       </c>
@@ -6476,7 +6537,7 @@
       <c r="E51" s="41"/>
       <c r="F51" s="40"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="9">
         <v>11</v>
       </c>
@@ -6492,7 +6553,7 @@
       <c r="E52" s="41"/>
       <c r="F52" s="40"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="9">
         <v>12</v>
       </c>
@@ -6508,7 +6569,7 @@
       <c r="E53" s="41"/>
       <c r="F53" s="40"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="9">
         <v>12</v>
       </c>
@@ -6524,7 +6585,7 @@
       <c r="E54" s="41"/>
       <c r="F54" s="40"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="20">
         <v>12</v>
       </c>
@@ -6540,7 +6601,7 @@
       <c r="E55" s="41"/>
       <c r="F55" s="40"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="20">
         <v>13</v>
       </c>
@@ -6556,7 +6617,7 @@
       <c r="E56" s="41"/>
       <c r="F56" s="40"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="20">
         <v>13</v>
       </c>
@@ -6572,7 +6633,7 @@
       <c r="E57" s="41"/>
       <c r="F57" s="40"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="20">
         <v>13</v>
       </c>
@@ -6588,7 +6649,7 @@
       <c r="E58" s="41"/>
       <c r="F58" s="40"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <v>14</v>
       </c>
@@ -6604,7 +6665,7 @@
       <c r="E59" s="41"/>
       <c r="F59" s="40"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="9">
         <v>14</v>
       </c>
@@ -6620,7 +6681,7 @@
       <c r="E60" s="41"/>
       <c r="F60" s="40"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
         <v>15</v>
       </c>
@@ -6636,7 +6697,7 @@
       <c r="E61" s="41"/>
       <c r="F61" s="41"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="9">
         <v>15</v>
       </c>
@@ -6652,7 +6713,7 @@
       <c r="E62" s="41"/>
       <c r="F62" s="41"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="9">
         <v>15</v>
       </c>
@@ -6666,7 +6727,7 @@
       <c r="E63" s="41"/>
       <c r="F63" s="40"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="9">
         <v>15</v>
       </c>
@@ -6682,7 +6743,7 @@
       <c r="E64" s="41"/>
       <c r="F64" s="40"/>
     </row>
-    <row r="65" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9">
         <v>17</v>
       </c>
@@ -6702,7 +6763,7 @@
       <c r="I65" s="6"/>
       <c r="J65" s="15"/>
     </row>
-    <row r="66" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="9">
         <v>17</v>
       </c>
@@ -6721,7 +6782,7 @@
       <c r="I66" s="15"/>
       <c r="J66" s="15"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="9">
         <v>17</v>
       </c>
@@ -6740,7 +6801,7 @@
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="9">
         <v>18</v>
       </c>
@@ -6755,7 +6816,7 @@
       </c>
       <c r="E68" s="42"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="9">
         <v>18</v>
       </c>
@@ -6769,7 +6830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="9">
         <v>18</v>
       </c>
@@ -6783,7 +6844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="9"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
@@ -6803,7 +6864,7 @@
       <c r="T71" s="5"/>
       <c r="U71" s="5"/>
     </row>
-    <row r="72" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="9"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
@@ -6823,7 +6884,7 @@
       <c r="T72" s="5"/>
       <c r="U72" s="5"/>
     </row>
-    <row r="73" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
@@ -6843,7 +6904,7 @@
       <c r="T73" s="5"/>
       <c r="U73" s="5"/>
     </row>
-    <row r="74" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="9"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
@@ -6863,7 +6924,7 @@
       <c r="T74" s="5"/>
       <c r="U74" s="5"/>
     </row>
-    <row r="75" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="9"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
@@ -6883,7 +6944,7 @@
       <c r="T75" s="5"/>
       <c r="U75" s="5"/>
     </row>
-    <row r="76" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="9"/>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
@@ -6903,7 +6964,7 @@
       <c r="T76" s="5"/>
       <c r="U76" s="5"/>
     </row>
-    <row r="77" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="9"/>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -6923,7 +6984,7 @@
       <c r="T77" s="5"/>
       <c r="U77" s="5"/>
     </row>
-    <row r="78" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="9"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
@@ -6943,7 +7004,7 @@
       <c r="T78" s="5"/>
       <c r="U78" s="5"/>
     </row>
-    <row r="79" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="9"/>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
@@ -6963,7 +7024,7 @@
       <c r="T79" s="5"/>
       <c r="U79" s="5"/>
     </row>
-    <row r="80" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="9"/>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
@@ -6983,7 +7044,7 @@
       <c r="T80" s="5"/>
       <c r="U80" s="5"/>
     </row>
-    <row r="81" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="9"/>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
@@ -7005,7 +7066,7 @@
       <c r="T81" s="5"/>
       <c r="U81" s="5"/>
     </row>
-    <row r="82" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
@@ -7025,7 +7086,7 @@
       <c r="T82" s="5"/>
       <c r="U82" s="5"/>
     </row>
-    <row r="83" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="9"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
@@ -7047,7 +7108,7 @@
       <c r="T83" s="5"/>
       <c r="U83" s="5"/>
     </row>
-    <row r="84" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="9"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
@@ -7069,7 +7130,7 @@
       <c r="T84" s="5"/>
       <c r="U84" s="5"/>
     </row>
-    <row r="85" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
@@ -7091,7 +7152,7 @@
       <c r="T85" s="5"/>
       <c r="U85" s="5"/>
     </row>
-    <row r="86" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="9"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -7113,7 +7174,7 @@
       <c r="T86" s="5"/>
       <c r="U86" s="5"/>
     </row>
-    <row r="87" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="9"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
@@ -7135,7 +7196,7 @@
       <c r="T87" s="5"/>
       <c r="U87" s="5"/>
     </row>
-    <row r="88" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="9"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
@@ -7157,7 +7218,7 @@
       <c r="T88" s="5"/>
       <c r="U88" s="5"/>
     </row>
-    <row r="89" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="9"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
@@ -7179,7 +7240,7 @@
       <c r="T89" s="5"/>
       <c r="U89" s="5"/>
     </row>
-    <row r="90" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="22"/>
       <c r="B90" s="23"/>
       <c r="C90" s="16"/>
@@ -7201,7 +7262,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="5"/>
     </row>
-    <row r="91" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="15"/>
       <c r="B91" s="16"/>
       <c r="C91" s="16"/>
@@ -7222,7 +7283,7 @@
       <c r="U91" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D94">
+  <sortState ref="A2:D94">
     <sortCondition ref="A2:A94"/>
   </sortState>
   <conditionalFormatting sqref="M2:M8">

</xml_diff>

<commit_message>
add link to welcome video
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27FBFA2-B31B-434A-A2B4-5D44E2CF1088}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31005" yWindow="1035" windowWidth="22785" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31005" yWindow="1035" windowWidth="22785" windowHeight="14265" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="topic_overview" sheetId="9" r:id="rId1"/>
@@ -21,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">points!$A$1:$D$93</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="408">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1757,17 +1756,27 @@
   <si>
     <t>[hw04_data_management](hw/hw04_data_management.html)</t>
   </si>
+  <si>
+    <t>Makeup quiz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2125,118 +2134,118 @@
   </borders>
   <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="77" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="77" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="77" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="78" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="78" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="80"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="80" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="81" applyFont="1" applyAlignment="1">
@@ -2248,27 +2257,27 @@
     <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="81" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="16" fillId="5" borderId="4" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="17" fillId="5" borderId="4" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="6" borderId="4" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2277,108 +2286,108 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="4" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="4" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="77" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="77" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="80" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="80" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="82" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2387,50 +2396,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="5" xfId="82" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="5" xfId="82" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="5" xfId="82" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="5" xfId="82" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="82" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="82" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="5" xfId="82" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="5" xfId="82" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2439,45 +2448,47 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="83">
     <cellStyle name="20% - Accent6" xfId="79" builtinId="50"/>
@@ -2558,10 +2569,10 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Percent 3" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Normal 3" xfId="80"/>
+    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Percent 3" xfId="81"/>
     <cellStyle name="Total" xfId="78" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2898,10 +2909,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -3712,7 +3723,7 @@
       <c r="K36" s="76"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K36">
+  <sortState ref="A2:K36">
     <sortCondition ref="A2:A36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3721,7 +3732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -4410,7 +4421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -5257,11 +5268,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z94"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5375,12 +5386,12 @@
         <v>161</v>
       </c>
       <c r="I2" s="6">
-        <f>SUMIF($C$2:$C$85,H2,$D$2:$D$85)</f>
-        <v>75</v>
+        <f t="shared" ref="I2:I7" si="0">SUMIF($C$2:$C$85,H2,$D$2:$D$85)</f>
+        <v>57</v>
       </c>
       <c r="J2" s="12">
-        <f>I2/$I$8</f>
-        <v>0.16853932584269662</v>
+        <f t="shared" ref="J2:J7" si="1">I2/$I$8</f>
+        <v>0.13348946135831383</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>44</v>
@@ -5443,12 +5454,12 @@
         <v>24</v>
       </c>
       <c r="I3" s="6">
-        <f>SUMIF($C$2:$C$85,H3,$D$2:$D$85)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="J3" s="12">
-        <f>I3/$I$8</f>
-        <v>0.15730337078651685</v>
+        <f t="shared" si="1"/>
+        <v>0.16393442622950818</v>
       </c>
       <c r="L3" s="16" t="s">
         <v>8</v>
@@ -5511,12 +5522,12 @@
         <v>25</v>
       </c>
       <c r="I4" s="6">
-        <f>SUMIF($C$2:$C$85,H4,$D$2:$D$85)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="J4" s="12">
-        <f>I4/$I$8</f>
-        <v>6.741573033707865E-2</v>
+        <f t="shared" si="1"/>
+        <v>7.0257611241217793E-2</v>
       </c>
       <c r="L4" s="16" t="s">
         <v>25</v>
@@ -5577,12 +5588,12 @@
         <v>13</v>
       </c>
       <c r="I5" s="6">
-        <f>SUMIF($C$2:$C$85,H5,$D$2:$D$85)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="J5" s="12">
-        <f>I5/$I$8</f>
-        <v>8.98876404494382E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.3676814988290405E-2</v>
       </c>
       <c r="L5" s="16"/>
       <c r="M5" s="6"/>
@@ -5623,8 +5634,8 @@
       <c r="B6" s="90" t="s">
         <v>365</v>
       </c>
-      <c r="C6" s="92" t="s">
-        <v>161</v>
+      <c r="C6" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D6" s="11">
         <v>1</v>
@@ -5634,12 +5645,12 @@
         <v>14</v>
       </c>
       <c r="I6" s="6">
-        <f>SUMIF($C$2:$C$85,H6,$D$2:$D$85)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J6" s="12">
-        <f>I6/$I$8</f>
-        <v>0.2247191011235955</v>
+        <f t="shared" si="1"/>
+        <v>0.23419203747072601</v>
       </c>
       <c r="L6" s="16" t="s">
         <v>13</v>
@@ -5700,12 +5711,12 @@
         <v>15</v>
       </c>
       <c r="I7" s="6">
-        <f>SUMIF($C$2:$C$85,H7,$D$2:$D$85)</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="J7" s="12">
-        <f>I7/$I$8</f>
-        <v>0.29213483146067415</v>
+        <f t="shared" si="1"/>
+        <v>0.3044496487119438</v>
       </c>
       <c r="L7" s="16" t="s">
         <v>14</v>
@@ -5770,7 +5781,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="4">
         <f>SUM(I2:I7)</f>
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="L8" s="16" t="s">
         <v>15</v>
@@ -5844,8 +5855,8 @@
       <c r="B10" s="90" t="s">
         <v>401</v>
       </c>
-      <c r="C10" s="66" t="s">
-        <v>161</v>
+      <c r="C10" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
@@ -5938,8 +5949,8 @@
       <c r="B15" s="90" t="s">
         <v>364</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>161</v>
+      <c r="C15" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D15" s="11">
         <v>1</v>
@@ -5974,8 +5985,8 @@
       <c r="B17" s="90" t="s">
         <v>366</v>
       </c>
-      <c r="C17" s="41" t="s">
-        <v>161</v>
+      <c r="C17" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D17" s="11">
         <v>1</v>
@@ -6054,8 +6065,8 @@
       <c r="B21" s="90" t="s">
         <v>367</v>
       </c>
-      <c r="C21" s="41" t="s">
-        <v>161</v>
+      <c r="C21" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D21" s="11">
         <v>1</v>
@@ -6088,8 +6099,8 @@
       <c r="B23" s="90" t="s">
         <v>368</v>
       </c>
-      <c r="C23" s="41" t="s">
-        <v>161</v>
+      <c r="C23" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D23" s="11">
         <v>1</v>
@@ -6172,8 +6183,8 @@
       <c r="B27" s="90" t="s">
         <v>369</v>
       </c>
-      <c r="C27" s="41" t="s">
-        <v>161</v>
+      <c r="C27" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D27" s="11">
         <v>1</v>
@@ -6254,8 +6265,8 @@
       <c r="B31" s="90" t="s">
         <v>370</v>
       </c>
-      <c r="C31" s="41" t="s">
-        <v>161</v>
+      <c r="C31" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D31" s="11">
         <v>1</v>
@@ -6288,8 +6299,8 @@
       <c r="B33" s="91" t="s">
         <v>371</v>
       </c>
-      <c r="C33" s="97" t="s">
-        <v>161</v>
+      <c r="C33" s="116" t="s">
+        <v>407</v>
       </c>
       <c r="D33" s="18">
         <v>1</v>
@@ -6321,8 +6332,8 @@
       <c r="B35" s="90" t="s">
         <v>373</v>
       </c>
-      <c r="C35" s="41" t="s">
-        <v>161</v>
+      <c r="C35" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D35" s="11">
         <v>1</v>
@@ -6448,8 +6459,8 @@
       <c r="B42" s="90" t="s">
         <v>375</v>
       </c>
-      <c r="C42" s="41" t="s">
-        <v>161</v>
+      <c r="C42" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D42" s="11">
         <v>1</v>
@@ -6476,8 +6487,8 @@
       <c r="B44" s="90" t="s">
         <v>376</v>
       </c>
-      <c r="C44" s="41" t="s">
-        <v>161</v>
+      <c r="C44" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D44" s="11">
         <v>1</v>
@@ -6524,8 +6535,8 @@
       <c r="B47" s="90" t="s">
         <v>382</v>
       </c>
-      <c r="C47" s="41" t="s">
-        <v>161</v>
+      <c r="C47" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D47" s="11">
         <v>1</v>
@@ -6554,8 +6565,8 @@
       <c r="B49" s="91" t="s">
         <v>384</v>
       </c>
-      <c r="C49" s="97" t="s">
-        <v>161</v>
+      <c r="C49" s="116" t="s">
+        <v>407</v>
       </c>
       <c r="D49" s="18">
         <v>1</v>
@@ -6584,8 +6595,8 @@
       <c r="B51" s="90" t="s">
         <v>386</v>
       </c>
-      <c r="C51" s="41" t="s">
-        <v>161</v>
+      <c r="C51" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D51" s="11">
         <v>1</v>
@@ -6633,8 +6644,8 @@
       <c r="B54" s="90" t="s">
         <v>391</v>
       </c>
-      <c r="C54" s="41" t="s">
-        <v>161</v>
+      <c r="C54" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D54" s="11">
         <v>1</v>
@@ -6665,8 +6676,8 @@
       <c r="B56" s="90" t="s">
         <v>393</v>
       </c>
-      <c r="C56" s="41" t="s">
-        <v>161</v>
+      <c r="C56" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D56" s="11">
         <v>1</v>
@@ -6748,8 +6759,8 @@
       <c r="B61" s="90" t="s">
         <v>395</v>
       </c>
-      <c r="C61" s="41" t="s">
-        <v>161</v>
+      <c r="C61" s="115" t="s">
+        <v>407</v>
       </c>
       <c r="D61" s="11">
         <v>1</v>
@@ -7341,7 +7352,7 @@
       <c r="B94" s="20"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D108">
+  <sortState ref="A2:D108">
     <sortCondition ref="A2:A108"/>
   </sortState>
   <conditionalFormatting sqref="N2:N8">

</xml_diff>

<commit_message>
rebuild schedule to simplify dates
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19072C12-AB44-4424-A9A2-CFC036251C33}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7857D8F-E6D8-4D10-BAB9-694A3E580DBC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31350" yWindow="1380" windowWidth="22785" windowHeight="14265" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="1230" windowWidth="22785" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topic_overview" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="397">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1152,9 +1152,6 @@
     <t>Topic</t>
   </si>
   <si>
-    <t>Overview</t>
-  </si>
-  <si>
     <t>Intro</t>
   </si>
   <si>
@@ -1197,28 +1194,7 @@
     <t>Causation</t>
   </si>
   <si>
-    <t>Pop vs Sample</t>
-  </si>
-  <si>
-    <t>Data structure &amp; types</t>
-  </si>
-  <si>
-    <t>hw08_bivariate_inference</t>
-  </si>
-  <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>hw05_univ_graphing</t>
-  </si>
-  <si>
-    <t>hw06_biv_graphing</t>
-  </si>
-  <si>
-    <t>hw09_moderation</t>
-  </si>
-  <si>
-    <t>hw10_regression</t>
   </si>
   <si>
     <t>Midterm</t>
@@ -1468,13 +1444,7 @@
     <t>3/14 (02) &amp;  3/15 (01)</t>
   </si>
   <si>
-    <t>5/13 (02) &amp; 5/14 (01)</t>
-  </si>
-  <si>
     <t xml:space="preserve">6 (2/24) </t>
-  </si>
-  <si>
-    <t>foundations worksheet</t>
   </si>
   <si>
     <t>PDS
@@ -1485,30 +1455,6 @@
 Packet</t>
   </si>
   <si>
-    <t>Working with R Studio IDE</t>
-  </si>
-  <si>
-    <t>[hw01_orientation](hw/hw01_orientation.html)</t>
-  </si>
-  <si>
-    <t>Data Camp</t>
-  </si>
-  <si>
-    <t>hw07_proposal*</t>
-  </si>
-  <si>
-    <t>Poster prep Stage II*</t>
-  </si>
-  <si>
-    <t>Poster prep Stage I*</t>
-  </si>
-  <si>
-    <t>Poster prep Stage III*</t>
-  </si>
-  <si>
-    <t>Powerpoint Poster*</t>
-  </si>
-  <si>
     <t>Research Proposal</t>
   </si>
   <si>
@@ -1527,78 +1473,15 @@
     <t>Poster Presentation</t>
   </si>
   <si>
-    <t>Due</t>
-  </si>
-  <si>
-    <t>with midterm</t>
-  </si>
-  <si>
-    <t>1/27</t>
-  </si>
-  <si>
-    <t>2/2</t>
-  </si>
-  <si>
-    <t>2/9</t>
-  </si>
-  <si>
-    <t>2/16</t>
-  </si>
-  <si>
-    <t>2/23</t>
-  </si>
-  <si>
-    <t>3/5</t>
-  </si>
-  <si>
-    <t>3/12</t>
-  </si>
-  <si>
-    <t>4/13</t>
-  </si>
-  <si>
-    <t>4/20</t>
-  </si>
-  <si>
-    <t>4/27</t>
-  </si>
-  <si>
-    <t>4/30</t>
-  </si>
-  <si>
-    <t>4/16</t>
-  </si>
-  <si>
-    <t>5/9</t>
-  </si>
-  <si>
-    <t>Take home final exam</t>
-  </si>
-  <si>
-    <t>5/15</t>
-  </si>
-  <si>
     <t>Data Camp: Intro to R</t>
   </si>
   <si>
-    <t>Intro to Basics</t>
-  </si>
-  <si>
-    <t>Intro to R</t>
-  </si>
-  <si>
     <t>PDS Course Pre-Survey</t>
   </si>
   <si>
-    <t>[MWF](https://goo.gl/forms/ZW4DwyStgjfpzSGh2) [TR](https://goo.gl/forms/AdgB28e0Gjo4tSZg1)</t>
-  </si>
-  <si>
     <t>hw01: Orientation</t>
   </si>
   <si>
-    <t>Intro to Data</t>
-  </si>
-  <si>
     <t>Data Camp: Intro to ggplot</t>
   </si>
   <si>
@@ -1725,9 +1608,6 @@
     <t>grp quiz: logistic regression</t>
   </si>
   <si>
-    <t>Introduction (to ggplot)</t>
-  </si>
-  <si>
     <t>due</t>
   </si>
   <si>
@@ -1749,19 +1629,104 @@
     <t>Data Camp: Working with R Studio IDE</t>
   </si>
   <si>
-    <t>[hw03_lit_review](hw/hw03_lit_review.html)</t>
-  </si>
-  <si>
-    <t>[hw04_data_management](hw/hw04_data_management.html)</t>
-  </si>
-  <si>
     <t>Makeup quiz</t>
   </si>
   <si>
-    <t>[hw02_codebook*](hw/hw02_persaonl_codebook.html)</t>
-  </si>
-  <si>
     <t>PR HW02</t>
+  </si>
+  <si>
+    <t>[hw01_orientation](hw/hw01_orientation.html) (Due 1/27)</t>
+  </si>
+  <si>
+    <t>[hw03_lit_review](hw/hw03_lit_review.html) (Due 2/9)</t>
+  </si>
+  <si>
+    <t>[hw04_data_management](hw/hw04_data_management.html) (Due 2/9)</t>
+  </si>
+  <si>
+    <t>hw05_univ_graphing (Due 2/16)</t>
+  </si>
+  <si>
+    <t>hw06_biv_graphing (Due 2/23)</t>
+  </si>
+  <si>
+    <t>foundations worksheet (Due with midterm)</t>
+  </si>
+  <si>
+    <t>hw08_bivariate_inference (Due 4/13)</t>
+  </si>
+  <si>
+    <t>hw09_moderation (Due 4/20)</t>
+  </si>
+  <si>
+    <t>hw10_regression (Due 4/27)</t>
+  </si>
+  <si>
+    <t>5/13 (02) &amp; 5/14 (01) (tentative)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take home final exam (Due 5/15-tentative) </t>
+  </si>
+  <si>
+    <t>[MWF](https://goo.gl/forms/ZW4DwyStgjfpzSGh2) (Due 1/24) 
+[TR](https://goo.gl/forms/AdgB28e0Gjo4tSZg1)  (Due 1/23)</t>
+  </si>
+  <si>
+    <t>Poster prep Stage I* (Draft Due 3/12, PR 3/14, Final 3/16)</t>
+  </si>
+  <si>
+    <t>Working in R Studio</t>
+  </si>
+  <si>
+    <t>Data Camp: Orientation to R Studio (Due 1/26)</t>
+  </si>
+  <si>
+    <t>Intro to the R language</t>
+  </si>
+  <si>
+    <t>Data Camp: Intro to Basics (Due 2/2)</t>
+  </si>
+  <si>
+    <t>Using R for Data Analysis</t>
+  </si>
+  <si>
+    <t>Data Camp: Intro to R (Due 2/2)</t>
+  </si>
+  <si>
+    <t>Graphing with ggplot</t>
+  </si>
+  <si>
+    <t>Data Camp: Introduction to ggplot (Due 2/16)</t>
+  </si>
+  <si>
+    <t>Data Camp: Intro to Data (Due 2/23)</t>
+  </si>
+  <si>
+    <t>Practice managing data in R</t>
+  </si>
+  <si>
+    <t>[hw02_codebook*](hw/hw02_persaonl_codebook.html) (Due 2/2, PR 2/4)</t>
+  </si>
+  <si>
+    <t>hw07_proposal* (Draft Due 3/5, PR 3/7, Final 3/9)</t>
+  </si>
+  <si>
+    <t>Poster prep Stage II* (Draft Due 4/16, PR 4/18, Final 4/20)</t>
+  </si>
+  <si>
+    <t>Poster prep Stage III* (Draft Due 4/30, PR 5/2, Final 5/4)</t>
+  </si>
+  <si>
+    <t>Powerpoint Poster* (Draft Due 5/9, PR 5/11, Final 5/13)</t>
+  </si>
+  <si>
+    <t>Overview of the class, metacognition topics, how to improve your learning</t>
+  </si>
+  <si>
+    <t>Data architecture &amp; types</t>
+  </si>
+  <si>
+    <t>Populations vs Samples, bias, representation</t>
   </si>
 </sst>
 </file>
@@ -2449,15 +2414,6 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="5" xfId="82" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2500,6 +2456,9 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="82" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="83">
     <cellStyle name="20% - Accent6" xfId="79" builtinId="50"/>
@@ -2921,10 +2880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2934,16 +2893,14 @@
     <col min="4" max="4" width="10.625" style="79" customWidth="1"/>
     <col min="5" max="5" width="13.875" style="69" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="70" customWidth="1"/>
-    <col min="7" max="7" width="22.375" style="70" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.25" style="69" customWidth="1"/>
-    <col min="9" max="9" width="18.25" style="87" customWidth="1"/>
-    <col min="10" max="10" width="22" style="69" customWidth="1"/>
-    <col min="11" max="11" width="31.625" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.25" style="115" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" style="69" customWidth="1"/>
+    <col min="9" max="9" width="31.625" style="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="69" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="69" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="74" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B1" s="68" t="s">
         <v>22</v>
@@ -2952,790 +2909,773 @@
         <v>206</v>
       </c>
       <c r="D1" s="82" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E1" s="83" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="F1" s="84" t="s">
         <v>161</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="83" t="s">
-        <v>318</v>
-      </c>
-      <c r="I1" s="86" t="s">
-        <v>330</v>
-      </c>
-      <c r="J1" s="74" t="s">
-        <v>234</v>
-      </c>
-      <c r="K1" s="74" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H1" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="I1" s="74" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="75">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="69" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D2" s="79" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="69" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="79" t="s">
-        <v>283</v>
-      </c>
-      <c r="E2" s="69" t="s">
-        <v>208</v>
-      </c>
-      <c r="G2" s="70" t="s">
-        <v>317</v>
-      </c>
-      <c r="H2" s="69" t="s">
-        <v>316</v>
-      </c>
-      <c r="I2" s="88" t="s">
-        <v>332</v>
-      </c>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G2" s="115" t="s">
+        <v>366</v>
+      </c>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="75">
         <v>1.2</v>
       </c>
       <c r="C3" t="s">
-        <v>222</v>
+        <v>396</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E3" s="73" t="s">
-        <v>241</v>
-      </c>
-      <c r="J3" s="75" t="s">
-        <v>238</v>
-      </c>
-      <c r="K3" s="75"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="H3" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="I3" s="75"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="75">
         <v>1.3</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D4" s="80"/>
       <c r="E4" s="69">
         <v>1.2</v>
       </c>
-      <c r="J4" s="75" t="s">
+      <c r="H4" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="I4" s="75"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="75"/>
+      <c r="C5" t="s">
+        <v>379</v>
+      </c>
+      <c r="G5" s="115" t="s">
+        <v>380</v>
+      </c>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="75">
+        <v>1.4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6" s="79" t="s">
+        <v>299</v>
+      </c>
+      <c r="E6" s="69">
+        <v>1.3</v>
+      </c>
+      <c r="F6" s="70" t="s">
+        <v>377</v>
+      </c>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="75"/>
+      <c r="C7" t="s">
+        <v>381</v>
+      </c>
+      <c r="G7" s="115" t="s">
+        <v>382</v>
+      </c>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="75">
+        <v>2.1</v>
+      </c>
+      <c r="B8" s="69" t="s">
+        <v>263</v>
+      </c>
+      <c r="C8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" s="79" t="s">
+        <v>300</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="G8" s="115" t="s">
+        <v>389</v>
+      </c>
+      <c r="H8" s="75"/>
+      <c r="I8" s="75" t="s">
         <v>238</v>
       </c>
-      <c r="K4" s="75"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="75">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="75"/>
+      <c r="C9" t="s">
+        <v>383</v>
+      </c>
+      <c r="G9" s="115" t="s">
+        <v>384</v>
+      </c>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="75">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="79" t="s">
+        <v>277</v>
+      </c>
+      <c r="F10" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="G10" s="115" t="s">
+        <v>367</v>
+      </c>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="76">
+        <v>3.1</v>
+      </c>
+      <c r="B11" s="71" t="s">
+        <v>264</v>
+      </c>
+      <c r="C11" s="72" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" s="81" t="s">
+        <v>278</v>
+      </c>
+      <c r="E11" s="71"/>
+      <c r="F11" s="85" t="s">
+        <v>221</v>
+      </c>
+      <c r="G11" s="116"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="75">
+        <v>3.2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" s="79" t="s">
+        <v>279</v>
+      </c>
+      <c r="E12" s="69">
         <v>1.4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F12" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="G12" s="115" t="s">
+        <v>368</v>
+      </c>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="75">
+        <v>4</v>
+      </c>
+      <c r="B13" s="69" t="s">
+        <v>265</v>
+      </c>
+      <c r="C13" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" s="79" t="s">
+        <v>280</v>
+      </c>
+      <c r="E13" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="F13" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="G13" s="115" t="s">
+        <v>369</v>
+      </c>
+      <c r="H13" s="75" t="s">
+        <v>228</v>
+      </c>
+      <c r="I13" s="75" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="75"/>
+      <c r="C14" t="s">
+        <v>385</v>
+      </c>
+      <c r="G14" s="115" t="s">
+        <v>386</v>
+      </c>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="75">
+        <v>5</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>266</v>
+      </c>
+      <c r="C15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D15" s="79" t="s">
+        <v>281</v>
+      </c>
+      <c r="E15" s="73" t="s">
+        <v>234</v>
+      </c>
+      <c r="F15" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="G15" s="115" t="s">
+        <v>370</v>
+      </c>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="75"/>
+      <c r="C16" t="s">
+        <v>388</v>
+      </c>
+      <c r="E16" s="73"/>
+      <c r="G16" s="115" t="s">
+        <v>387</v>
+      </c>
+      <c r="H16" s="75"/>
+      <c r="I16" s="75"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="75">
+        <v>6</v>
+      </c>
+      <c r="B17" s="69" t="s">
+        <v>303</v>
+      </c>
+      <c r="C17" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H17" s="76"/>
+      <c r="I17" s="75" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="75">
+        <v>6.1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>306</v>
+      </c>
+      <c r="E18" s="73"/>
+      <c r="G18" s="115" t="s">
+        <v>390</v>
+      </c>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="75">
+        <v>6.2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>256</v>
+      </c>
+      <c r="D19" s="79" t="s">
+        <v>282</v>
+      </c>
+      <c r="E19" s="69">
+        <v>3</v>
+      </c>
+      <c r="F19" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H19" s="77" t="s">
+        <v>229</v>
+      </c>
+      <c r="I19" s="75"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="75">
+        <v>7.1</v>
+      </c>
+      <c r="B20" s="69" t="s">
+        <v>268</v>
+      </c>
+      <c r="C20" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="79" t="s">
+        <v>293</v>
+      </c>
+      <c r="E20" s="69" t="s">
+        <v>257</v>
+      </c>
+      <c r="H20" s="75" t="s">
+        <v>255</v>
+      </c>
+      <c r="I20" s="75"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="75">
+        <v>7.2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>307</v>
+      </c>
+      <c r="G21" s="115" t="s">
+        <v>378</v>
+      </c>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="75">
+        <v>7.3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22" s="69">
+        <v>4.5</v>
+      </c>
+      <c r="G22" s="115" t="s">
+        <v>371</v>
+      </c>
+      <c r="H22" s="75">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I22" s="75"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="75">
+        <v>8</v>
+      </c>
+      <c r="B23" s="69" t="s">
+        <v>269</v>
+      </c>
+      <c r="C23" t="s">
+        <v>222</v>
+      </c>
+      <c r="G23" s="115" t="s">
+        <v>302</v>
+      </c>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="75">
+        <v>9.1</v>
+      </c>
+      <c r="B24" s="69" t="s">
+        <v>270</v>
+      </c>
+      <c r="C24" t="s">
+        <v>215</v>
+      </c>
+      <c r="D24" s="79" t="s">
+        <v>294</v>
+      </c>
+      <c r="E24" s="69" t="s">
+        <v>254</v>
+      </c>
+      <c r="F24" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H24" s="78" t="s">
+        <v>252</v>
+      </c>
+      <c r="I24" s="75" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="75">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C25" t="s">
+        <v>235</v>
+      </c>
+      <c r="E25" s="69">
+        <v>6.1</v>
+      </c>
+      <c r="G25" s="115" t="s">
+        <v>372</v>
+      </c>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="75">
+        <v>10.1</v>
+      </c>
+      <c r="B26" s="69" t="s">
+        <v>267</v>
+      </c>
+      <c r="C26" t="s">
+        <v>216</v>
+      </c>
+      <c r="D26" s="79" t="s">
+        <v>283</v>
+      </c>
+      <c r="E26" s="69">
+        <v>6.2</v>
+      </c>
+      <c r="F26" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H26" s="75">
+        <v>6.6</v>
+      </c>
+      <c r="I26" s="75" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="75">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D27" s="79" t="s">
+        <v>284</v>
+      </c>
+      <c r="E27" s="69">
+        <v>6.3</v>
+      </c>
+      <c r="F27" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="75">
+        <v>11</v>
+      </c>
+      <c r="B28" s="69" t="s">
+        <v>271</v>
+      </c>
+      <c r="C28" t="s">
+        <v>218</v>
+      </c>
+      <c r="D28" s="79" t="s">
+        <v>285</v>
+      </c>
+      <c r="E28" s="69">
+        <v>6.4</v>
+      </c>
+      <c r="F28" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H28" s="75">
+        <v>7.1</v>
+      </c>
+      <c r="I28" s="75" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="75">
+        <v>11.1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>259</v>
+      </c>
+      <c r="D29" s="79" t="s">
+        <v>290</v>
+      </c>
+      <c r="E29" s="69">
+        <v>6.5</v>
+      </c>
+      <c r="F29" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H29" s="75">
+        <v>7.3</v>
+      </c>
+      <c r="I29" s="75" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="75">
+        <v>11.2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>308</v>
+      </c>
+      <c r="G30" s="115" t="s">
+        <v>391</v>
+      </c>
+      <c r="H30" s="75"/>
+      <c r="I30" s="75"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="75">
+        <v>12</v>
+      </c>
+      <c r="B31" s="69" t="s">
+        <v>272</v>
+      </c>
+      <c r="C31" t="s">
+        <v>219</v>
+      </c>
+      <c r="D31" s="79" t="s">
+        <v>286</v>
+      </c>
+      <c r="E31" s="69">
+        <v>7</v>
+      </c>
+      <c r="F31" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="G31" s="115" t="s">
+        <v>373</v>
+      </c>
+      <c r="H31" s="75"/>
+      <c r="I31" s="75" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="75">
+        <v>12.2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>220</v>
+      </c>
+      <c r="D32" s="79" t="s">
+        <v>288</v>
+      </c>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="75">
+        <v>12.3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>296</v>
+      </c>
+      <c r="D33" s="79" t="s">
+        <v>287</v>
+      </c>
+      <c r="E33" s="73" t="s">
+        <v>297</v>
+      </c>
+      <c r="F33" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="G33" s="115" t="s">
+        <v>374</v>
+      </c>
+      <c r="H33" s="75"/>
+      <c r="I33" s="75" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="75">
+        <v>12.4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>295</v>
+      </c>
+      <c r="D34" s="79" t="s">
+        <v>298</v>
+      </c>
+      <c r="E34" s="73" t="s">
+        <v>291</v>
+      </c>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="75">
+        <v>13</v>
+      </c>
+      <c r="B35" s="69" t="s">
+        <v>273</v>
+      </c>
+      <c r="C35" t="s">
+        <v>231</v>
+      </c>
+      <c r="D35" s="79" t="s">
+        <v>301</v>
+      </c>
+      <c r="E35" s="73" t="s">
+        <v>292</v>
+      </c>
+      <c r="F35" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H35" s="75"/>
+      <c r="I35" s="75"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="75">
+        <v>14.1</v>
+      </c>
+      <c r="B36" s="69" t="s">
+        <v>274</v>
+      </c>
+      <c r="C36" t="s">
+        <v>309</v>
+      </c>
+      <c r="G36" s="115" t="s">
+        <v>392</v>
+      </c>
+      <c r="H36" s="75"/>
+      <c r="I36" s="75"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="75">
+        <v>14.2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>350</v>
+      </c>
+      <c r="E37" s="69">
+        <v>8.4</v>
+      </c>
+      <c r="F37" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="75">
+        <v>14.3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>224</v>
+      </c>
+      <c r="E38" s="73">
+        <v>8.4</v>
+      </c>
+      <c r="H38" s="75"/>
+      <c r="I38" s="75"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="75">
+        <v>15</v>
+      </c>
+      <c r="B39" s="69" t="s">
+        <v>260</v>
+      </c>
+      <c r="C39" t="s">
+        <v>310</v>
+      </c>
+      <c r="D39" s="79" t="s">
+        <v>289</v>
+      </c>
+      <c r="G39" s="115" t="s">
+        <v>393</v>
+      </c>
+      <c r="H39" s="75"/>
+      <c r="I39" s="75"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="75">
+        <v>16</v>
+      </c>
+      <c r="B40" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="C40" t="s">
+        <v>311</v>
+      </c>
+      <c r="G40" s="115" t="s">
+        <v>375</v>
+      </c>
+      <c r="H40" s="75"/>
+      <c r="I40" s="75"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="75">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C41" t="s">
         <v>223</v>
       </c>
-      <c r="D5" s="79" t="s">
-        <v>307</v>
-      </c>
-      <c r="E5" s="69">
-        <v>1.3</v>
-      </c>
-      <c r="F5" s="70" t="s">
-        <v>351</v>
-      </c>
-      <c r="H5" s="69" t="s">
-        <v>348</v>
-      </c>
-      <c r="I5" s="88" t="s">
-        <v>333</v>
-      </c>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="75">
-        <v>2.1</v>
-      </c>
-      <c r="B6" s="69" t="s">
-        <v>271</v>
-      </c>
-      <c r="C6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D6" s="79" t="s">
-        <v>308</v>
-      </c>
-      <c r="F6" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="G6" s="70" t="s">
-        <v>407</v>
-      </c>
-      <c r="H6" s="69" t="s">
-        <v>349</v>
-      </c>
-      <c r="I6" s="88" t="s">
-        <v>333</v>
-      </c>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="75">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C7" t="s">
-        <v>210</v>
-      </c>
-      <c r="D7" s="79" t="s">
-        <v>285</v>
-      </c>
-      <c r="F7" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="G7" s="70" t="s">
-        <v>404</v>
-      </c>
-      <c r="I7" s="88" t="s">
-        <v>334</v>
-      </c>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="76">
-        <v>3.1</v>
-      </c>
-      <c r="B8" s="71" t="s">
-        <v>272</v>
-      </c>
-      <c r="C8" s="72" t="s">
-        <v>212</v>
-      </c>
-      <c r="D8" s="81" t="s">
-        <v>286</v>
-      </c>
-      <c r="E8" s="71"/>
-      <c r="F8" s="85" t="s">
-        <v>225</v>
-      </c>
-      <c r="G8" s="85"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="75" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="75">
-        <v>3.2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>213</v>
-      </c>
-      <c r="D9" s="79" t="s">
-        <v>287</v>
-      </c>
-      <c r="E9" s="69">
-        <v>1.4</v>
-      </c>
-      <c r="F9" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="G9" s="70" t="s">
-        <v>405</v>
-      </c>
-      <c r="I9" s="88" t="s">
-        <v>334</v>
-      </c>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="75">
-        <v>4</v>
-      </c>
-      <c r="B10" s="69" t="s">
-        <v>273</v>
-      </c>
-      <c r="C10" t="s">
-        <v>214</v>
-      </c>
-      <c r="D10" s="79" t="s">
-        <v>288</v>
-      </c>
-      <c r="E10" s="69" t="s">
-        <v>233</v>
-      </c>
-      <c r="F10" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="G10" s="70" t="s">
-        <v>226</v>
-      </c>
-      <c r="H10" s="69" t="s">
-        <v>396</v>
-      </c>
-      <c r="I10" s="88" t="s">
-        <v>335</v>
-      </c>
-      <c r="J10" s="75" t="s">
-        <v>236</v>
-      </c>
-      <c r="K10" s="75" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="75">
-        <v>5</v>
-      </c>
-      <c r="B11" s="69" t="s">
-        <v>274</v>
-      </c>
-      <c r="C11" t="s">
-        <v>215</v>
-      </c>
-      <c r="D11" s="79" t="s">
-        <v>289</v>
-      </c>
-      <c r="E11" s="73" t="s">
-        <v>242</v>
-      </c>
-      <c r="F11" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="G11" s="70" t="s">
-        <v>227</v>
-      </c>
-      <c r="H11" s="69" t="s">
-        <v>353</v>
-      </c>
-      <c r="I11" s="88" t="s">
-        <v>336</v>
-      </c>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="75">
-        <v>6</v>
-      </c>
-      <c r="B12" s="69" t="s">
-        <v>312</v>
-      </c>
-      <c r="C12" t="s">
-        <v>211</v>
-      </c>
-      <c r="F12" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="J12" s="76"/>
-      <c r="K12" s="75" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="75">
-        <v>6.1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>324</v>
-      </c>
-      <c r="E13" s="73"/>
-      <c r="G13" s="70" t="s">
-        <v>319</v>
-      </c>
-      <c r="I13" s="88" t="s">
-        <v>337</v>
-      </c>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="75">
-        <v>6.2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>264</v>
-      </c>
-      <c r="D14" s="79" t="s">
-        <v>290</v>
-      </c>
-      <c r="E14" s="69">
-        <v>3</v>
-      </c>
-      <c r="F14" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="J14" s="77" t="s">
-        <v>237</v>
-      </c>
-      <c r="K14" s="75"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="75">
-        <v>7.1</v>
-      </c>
-      <c r="B15" s="69" t="s">
-        <v>276</v>
-      </c>
-      <c r="C15" t="s">
-        <v>266</v>
-      </c>
-      <c r="D15" s="79" t="s">
-        <v>301</v>
-      </c>
-      <c r="E15" s="69" t="s">
-        <v>265</v>
-      </c>
-      <c r="J15" s="75" t="s">
-        <v>263</v>
-      </c>
-      <c r="K15" s="75"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="75">
-        <v>7.2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>325</v>
-      </c>
-      <c r="G16" s="70" t="s">
-        <v>321</v>
-      </c>
-      <c r="I16" s="88" t="s">
-        <v>338</v>
-      </c>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="75">
-        <v>7.3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>261</v>
-      </c>
-      <c r="E17" s="69">
-        <v>4.5</v>
-      </c>
-      <c r="G17" s="70" t="s">
-        <v>313</v>
-      </c>
-      <c r="I17" s="88" t="s">
-        <v>331</v>
-      </c>
-      <c r="J17" s="75">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K17" s="75"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="75">
-        <v>8</v>
-      </c>
-      <c r="B18" s="69" t="s">
-        <v>277</v>
-      </c>
-      <c r="C18" t="s">
-        <v>230</v>
-      </c>
-      <c r="G18" s="70" t="s">
-        <v>310</v>
-      </c>
-      <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="75">
-        <v>9.1</v>
-      </c>
-      <c r="B19" s="69" t="s">
-        <v>278</v>
-      </c>
-      <c r="C19" t="s">
-        <v>216</v>
-      </c>
-      <c r="D19" s="79" t="s">
-        <v>302</v>
-      </c>
-      <c r="E19" s="69" t="s">
-        <v>262</v>
-      </c>
-      <c r="F19" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="J19" s="78" t="s">
-        <v>260</v>
-      </c>
-      <c r="K19" s="75" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="75">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="C20" t="s">
-        <v>243</v>
-      </c>
-      <c r="E20" s="69">
-        <v>6.1</v>
-      </c>
-      <c r="G20" s="70" t="s">
-        <v>224</v>
-      </c>
-      <c r="I20" s="88" t="s">
-        <v>339</v>
-      </c>
-      <c r="J20" s="75"/>
-      <c r="K20" s="75"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="75">
-        <v>10.1</v>
-      </c>
-      <c r="B21" s="69" t="s">
-        <v>275</v>
-      </c>
-      <c r="C21" t="s">
-        <v>217</v>
-      </c>
-      <c r="D21" s="79" t="s">
-        <v>291</v>
-      </c>
-      <c r="E21" s="69">
-        <v>6.2</v>
-      </c>
-      <c r="F21" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="J21" s="75">
-        <v>6.6</v>
-      </c>
-      <c r="K21" s="75" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="75">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="C22" t="s">
-        <v>218</v>
-      </c>
-      <c r="D22" s="79" t="s">
-        <v>292</v>
-      </c>
-      <c r="E22" s="69">
-        <v>6.3</v>
-      </c>
-      <c r="F22" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="75">
-        <v>11</v>
-      </c>
-      <c r="B23" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="C23" t="s">
-        <v>219</v>
-      </c>
-      <c r="D23" s="79" t="s">
-        <v>293</v>
-      </c>
-      <c r="E23" s="69">
-        <v>6.4</v>
-      </c>
-      <c r="F23" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="J23" s="75">
-        <v>7.1</v>
-      </c>
-      <c r="K23" s="75" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="75">
-        <v>11.1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>267</v>
-      </c>
-      <c r="D24" s="79" t="s">
-        <v>298</v>
-      </c>
-      <c r="E24" s="69">
-        <v>6.5</v>
-      </c>
-      <c r="F24" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="J24" s="75">
-        <v>7.3</v>
-      </c>
-      <c r="K24" s="75" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="75">
-        <v>11.2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>326</v>
-      </c>
-      <c r="G25" s="70" t="s">
-        <v>320</v>
-      </c>
-      <c r="I25" s="88" t="s">
-        <v>343</v>
-      </c>
-      <c r="J25" s="75"/>
-      <c r="K25" s="75"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="75">
-        <v>12</v>
-      </c>
-      <c r="B26" s="69" t="s">
-        <v>280</v>
-      </c>
-      <c r="C26" t="s">
-        <v>220</v>
-      </c>
-      <c r="D26" s="79" t="s">
-        <v>294</v>
-      </c>
-      <c r="E26" s="69">
-        <v>7</v>
-      </c>
-      <c r="F26" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="G26" s="70" t="s">
-        <v>228</v>
-      </c>
-      <c r="I26" s="88" t="s">
-        <v>340</v>
-      </c>
-      <c r="J26" s="75"/>
-      <c r="K26" s="75" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="75">
-        <v>12.2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>221</v>
-      </c>
-      <c r="D27" s="79" t="s">
-        <v>296</v>
-      </c>
-      <c r="J27" s="75"/>
-      <c r="K27" s="75"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="75">
-        <v>12.3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>304</v>
-      </c>
-      <c r="D28" s="79" t="s">
-        <v>295</v>
-      </c>
-      <c r="E28" s="73" t="s">
-        <v>305</v>
-      </c>
-      <c r="F28" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="G28" s="70" t="s">
-        <v>229</v>
-      </c>
-      <c r="I28" s="88" t="s">
-        <v>341</v>
-      </c>
-      <c r="J28" s="75"/>
-      <c r="K28" s="75" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="75">
-        <v>12.4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>303</v>
-      </c>
-      <c r="D29" s="79" t="s">
-        <v>306</v>
-      </c>
-      <c r="E29" s="73" t="s">
-        <v>299</v>
-      </c>
-      <c r="J29" s="75"/>
-      <c r="K29" s="75"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="75">
-        <v>13</v>
-      </c>
-      <c r="B30" s="69" t="s">
-        <v>281</v>
-      </c>
-      <c r="C30" t="s">
-        <v>239</v>
-      </c>
-      <c r="D30" s="79" t="s">
-        <v>309</v>
-      </c>
-      <c r="E30" s="73" t="s">
-        <v>300</v>
-      </c>
-      <c r="F30" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="J30" s="75"/>
-      <c r="K30" s="75"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="75">
-        <v>14.1</v>
-      </c>
-      <c r="B31" s="69" t="s">
-        <v>282</v>
-      </c>
-      <c r="C31" t="s">
-        <v>327</v>
-      </c>
-      <c r="G31" s="70" t="s">
-        <v>322</v>
-      </c>
-      <c r="I31" s="88" t="s">
-        <v>342</v>
-      </c>
-      <c r="J31" s="75"/>
-      <c r="K31" s="75"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="75">
-        <v>14.2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>389</v>
-      </c>
-      <c r="E32" s="69">
-        <v>8.4</v>
-      </c>
-      <c r="F32" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="I32" s="88"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="75"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="75">
-        <v>14.3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>232</v>
-      </c>
-      <c r="E33" s="73">
-        <v>8.4</v>
-      </c>
-      <c r="J33" s="75"/>
-      <c r="K33" s="75"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="75">
-        <v>15</v>
-      </c>
-      <c r="B34" s="69" t="s">
-        <v>268</v>
-      </c>
-      <c r="C34" t="s">
-        <v>328</v>
-      </c>
-      <c r="D34" s="79" t="s">
-        <v>297</v>
-      </c>
-      <c r="G34" s="70" t="s">
-        <v>323</v>
-      </c>
-      <c r="I34" s="88" t="s">
-        <v>344</v>
-      </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="75"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="75">
-        <v>16</v>
-      </c>
-      <c r="B35" s="69" t="s">
-        <v>269</v>
-      </c>
-      <c r="C35" t="s">
-        <v>329</v>
-      </c>
-      <c r="G35" s="70" t="s">
-        <v>311</v>
-      </c>
-      <c r="J35" s="75"/>
-      <c r="K35" s="75"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="75">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="C36" t="s">
-        <v>231</v>
-      </c>
-      <c r="G36" s="70" t="s">
-        <v>345</v>
-      </c>
-      <c r="I36" s="88" t="s">
-        <v>346</v>
-      </c>
-      <c r="J36" s="75"/>
-      <c r="K36" s="75"/>
+      <c r="G41" s="115" t="s">
+        <v>376</v>
+      </c>
+      <c r="H41" s="75"/>
+      <c r="I41" s="75"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K36">
-    <sortCondition ref="A2:A36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I41">
+    <sortCondition ref="A2:A41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4108,7 +4048,7 @@
         <v>42108</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>149</v>
@@ -5282,7 +5222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -5319,13 +5259,13 @@
         <v>10</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>397</v>
+        <v>357</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>399</v>
+        <v>359</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>9</v>
@@ -5387,21 +5327,21 @@
       <c r="D2" s="11">
         <v>3</v>
       </c>
-      <c r="F2" s="108" t="s">
-        <v>225</v>
-      </c>
-      <c r="G2" s="108" t="s">
-        <v>225</v>
+      <c r="F2" s="105" t="s">
+        <v>221</v>
+      </c>
+      <c r="G2" s="105" t="s">
+        <v>221</v>
       </c>
       <c r="H2" s="56" t="s">
         <v>161</v>
       </c>
       <c r="I2" s="6">
-        <f>SUMIF($C$2:$C$86,H2,$D$2:$D$86)</f>
+        <f t="shared" ref="I2:I7" si="0">SUMIF($C$2:$C$86,H2,$D$2:$D$86)</f>
         <v>57</v>
       </c>
       <c r="J2" s="12">
-        <f t="shared" ref="J2:J7" si="0">I2/$I$8</f>
+        <f t="shared" ref="J2:J7" si="1">I2/$I$8</f>
         <v>0.13194444444444445</v>
       </c>
       <c r="L2" s="5" t="s">
@@ -5446,8 +5386,8 @@
       <c r="A3" s="9">
         <v>1.2</v>
       </c>
-      <c r="B3" s="89" t="s">
-        <v>350</v>
+      <c r="B3" s="86" t="s">
+        <v>313</v>
       </c>
       <c r="C3" s="62" t="s">
         <v>25</v>
@@ -5458,18 +5398,18 @@
       <c r="E3" s="35">
         <v>42029</v>
       </c>
-      <c r="F3" s="108" t="s">
-        <v>225</v>
-      </c>
-      <c r="H3" s="101" t="s">
+      <c r="F3" s="105" t="s">
+        <v>221</v>
+      </c>
+      <c r="H3" s="98" t="s">
         <v>24</v>
       </c>
       <c r="I3" s="6">
-        <f>SUMIF($C$2:$C$86,H3,$D$2:$D$86)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="J3" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16203703703703703</v>
       </c>
       <c r="L3" s="16" t="s">
@@ -5526,18 +5466,18 @@
       <c r="E4" s="35">
         <v>42029</v>
       </c>
-      <c r="F4" s="108" t="s">
-        <v>225</v>
+      <c r="F4" s="105" t="s">
+        <v>221</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>25</v>
       </c>
       <c r="I4" s="6">
-        <f>SUMIF($C$2:$C$86,H4,$D$2:$D$86)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="J4" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.9444444444444448E-2</v>
       </c>
       <c r="L4" s="16" t="s">
@@ -5582,8 +5522,8 @@
       <c r="A5" s="9">
         <v>1.4</v>
       </c>
-      <c r="B5" s="89" t="s">
-        <v>356</v>
+      <c r="B5" s="86" t="s">
+        <v>317</v>
       </c>
       <c r="C5" s="65" t="s">
         <v>161</v>
@@ -5592,18 +5532,18 @@
         <v>2.5</v>
       </c>
       <c r="F5" s="39"/>
-      <c r="G5" s="108" t="s">
-        <v>225</v>
+      <c r="G5" s="105" t="s">
+        <v>221</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="6">
-        <f>SUMIF($C$2:$C$86,H5,$D$2:$D$86)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="J5" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.10416666666666667</v>
       </c>
       <c r="L5" s="16"/>
@@ -5642,11 +5582,11 @@
       <c r="A6" s="9">
         <v>1.5</v>
       </c>
-      <c r="B6" s="89" t="s">
-        <v>365</v>
-      </c>
-      <c r="C6" s="114" t="s">
-        <v>406</v>
+      <c r="B6" s="86" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D6" s="11">
         <v>1</v>
@@ -5656,11 +5596,11 @@
         <v>14</v>
       </c>
       <c r="I6" s="6">
-        <f>SUMIF($C$2:$C$86,H6,$D$2:$D$86)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J6" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23148148148148148</v>
       </c>
       <c r="L6" s="16" t="s">
@@ -5705,10 +5645,10 @@
       <c r="A7" s="9">
         <v>1.6</v>
       </c>
-      <c r="B7" s="89" t="s">
-        <v>403</v>
-      </c>
-      <c r="C7" s="91" t="s">
+      <c r="B7" s="86" t="s">
+        <v>363</v>
+      </c>
+      <c r="C7" s="88" t="s">
         <v>161</v>
       </c>
       <c r="D7" s="11">
@@ -5722,11 +5662,11 @@
         <v>15</v>
       </c>
       <c r="I7" s="6">
-        <f>SUMIF($C$2:$C$86,H7,$D$2:$D$86)</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="J7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.30092592592592593</v>
       </c>
       <c r="L7" s="16" t="s">
@@ -5771,10 +5711,10 @@
       <c r="A8" s="17">
         <v>1.7</v>
       </c>
-      <c r="B8" s="90" t="s">
-        <v>352</v>
-      </c>
-      <c r="C8" s="100" t="s">
+      <c r="B8" s="87" t="s">
+        <v>314</v>
+      </c>
+      <c r="C8" s="97" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="18">
@@ -5783,11 +5723,11 @@
       <c r="E8" s="35">
         <v>42030</v>
       </c>
-      <c r="F8" s="108" t="s">
-        <v>225</v>
-      </c>
-      <c r="G8" s="108" t="s">
-        <v>225</v>
+      <c r="F8" s="105" t="s">
+        <v>221</v>
+      </c>
+      <c r="G8" s="105" t="s">
+        <v>221</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="4">
@@ -5832,8 +5772,8 @@
       <c r="A9" s="9">
         <v>2.1</v>
       </c>
-      <c r="B9" s="89" t="s">
-        <v>400</v>
+      <c r="B9" s="86" t="s">
+        <v>360</v>
       </c>
       <c r="C9" s="65" t="s">
         <v>161</v>
@@ -5863,11 +5803,11 @@
       <c r="A10" s="9">
         <v>2.1</v>
       </c>
-      <c r="B10" s="89" t="s">
-        <v>401</v>
-      </c>
-      <c r="C10" s="114" t="s">
-        <v>406</v>
+      <c r="B10" s="86" t="s">
+        <v>361</v>
+      </c>
+      <c r="C10" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
@@ -5878,10 +5818,10 @@
       <c r="A11" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="91" t="s">
+      <c r="C11" s="88" t="s">
         <v>161</v>
       </c>
       <c r="D11" s="11">
@@ -5890,18 +5830,18 @@
       <c r="E11" s="35">
         <v>42036</v>
       </c>
-      <c r="F11" s="108" t="s">
-        <v>225</v>
+      <c r="F11" s="105" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B12" s="89" t="s">
-        <v>347</v>
-      </c>
-      <c r="C12" s="91" t="s">
+      <c r="B12" s="86" t="s">
+        <v>312</v>
+      </c>
+      <c r="C12" s="88" t="s">
         <v>161</v>
       </c>
       <c r="D12" s="11">
@@ -5910,18 +5850,18 @@
       <c r="E12" s="35">
         <v>42036</v>
       </c>
-      <c r="F12" s="108" t="s">
-        <v>225</v>
+      <c r="F12" s="105" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>2.5</v>
       </c>
-      <c r="B13" s="89" t="s">
+      <c r="B13" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="91" t="s">
+      <c r="C13" s="88" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="11">
@@ -5930,18 +5870,18 @@
       <c r="E13" s="35">
         <v>42036</v>
       </c>
-      <c r="F13" s="108" t="s">
-        <v>225</v>
+      <c r="F13" s="105" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>2.6</v>
       </c>
-      <c r="B14" s="116" t="s">
-        <v>408</v>
-      </c>
-      <c r="C14" s="107" t="s">
+      <c r="B14" s="113" t="s">
+        <v>365</v>
+      </c>
+      <c r="C14" s="104" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="18">
@@ -5950,7 +5890,7 @@
       <c r="E14" s="35">
         <v>42038</v>
       </c>
-      <c r="F14" s="108"/>
+      <c r="F14" s="105"/>
       <c r="H14" s="40"/>
       <c r="I14" s="40"/>
     </row>
@@ -5958,8 +5898,8 @@
       <c r="A15" s="9">
         <v>3.1</v>
       </c>
-      <c r="B15" s="89" t="s">
-        <v>357</v>
+      <c r="B15" s="86" t="s">
+        <v>318</v>
       </c>
       <c r="C15" s="41" t="s">
         <v>161</v>
@@ -5975,11 +5915,11 @@
       <c r="A16" s="9">
         <v>3.2</v>
       </c>
-      <c r="B16" s="89" t="s">
+      <c r="B16" s="86" t="s">
+        <v>325</v>
+      </c>
+      <c r="C16" s="111" t="s">
         <v>364</v>
-      </c>
-      <c r="C16" s="114" t="s">
-        <v>406</v>
       </c>
       <c r="D16" s="11">
         <v>1</v>
@@ -5992,8 +5932,8 @@
       <c r="A17" s="9">
         <v>3.3</v>
       </c>
-      <c r="B17" s="89" t="s">
-        <v>358</v>
+      <c r="B17" s="86" t="s">
+        <v>319</v>
       </c>
       <c r="C17" s="41" t="s">
         <v>161</v>
@@ -6011,11 +5951,11 @@
       <c r="A18" s="9">
         <v>3.4</v>
       </c>
-      <c r="B18" s="89" t="s">
-        <v>366</v>
-      </c>
-      <c r="C18" s="114" t="s">
-        <v>406</v>
+      <c r="B18" s="86" t="s">
+        <v>327</v>
+      </c>
+      <c r="C18" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D18" s="11">
         <v>1</v>
@@ -6028,10 +5968,10 @@
       <c r="A19" s="9">
         <v>3.5</v>
       </c>
-      <c r="B19" s="89" t="s">
-        <v>402</v>
-      </c>
-      <c r="C19" s="113" t="s">
+      <c r="B19" s="86" t="s">
+        <v>362</v>
+      </c>
+      <c r="C19" s="110" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="11">
@@ -6040,8 +5980,8 @@
       <c r="E19" s="35">
         <v>42043</v>
       </c>
-      <c r="F19" s="109" t="s">
-        <v>225</v>
+      <c r="F19" s="106" t="s">
+        <v>221</v>
       </c>
       <c r="H19" s="40"/>
       <c r="I19" s="40"/>
@@ -6050,10 +5990,10 @@
       <c r="A20" s="17">
         <v>3.6</v>
       </c>
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="112" t="s">
+      <c r="C20" s="109" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="18">
@@ -6062,8 +6002,8 @@
       <c r="E20" s="35">
         <v>42043</v>
       </c>
-      <c r="F20" s="109" t="s">
-        <v>225</v>
+      <c r="F20" s="106" t="s">
+        <v>221</v>
       </c>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>
@@ -6072,8 +6012,8 @@
       <c r="A21" s="9">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B21" s="89" t="s">
-        <v>359</v>
+      <c r="B21" s="86" t="s">
+        <v>320</v>
       </c>
       <c r="C21" s="41" t="s">
         <v>161</v>
@@ -6091,11 +6031,11 @@
       <c r="A22" s="9">
         <v>4.2</v>
       </c>
-      <c r="B22" s="89" t="s">
-        <v>367</v>
-      </c>
-      <c r="C22" s="114" t="s">
-        <v>406</v>
+      <c r="B22" s="86" t="s">
+        <v>328</v>
+      </c>
+      <c r="C22" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D22" s="11">
         <v>1</v>
@@ -6108,8 +6048,8 @@
       <c r="A23" s="9">
         <v>4.3</v>
       </c>
-      <c r="B23" s="89" t="s">
-        <v>360</v>
+      <c r="B23" s="86" t="s">
+        <v>321</v>
       </c>
       <c r="C23" s="41" t="s">
         <v>161</v>
@@ -6125,11 +6065,11 @@
       <c r="A24" s="9">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B24" s="89" t="s">
-        <v>368</v>
-      </c>
-      <c r="C24" s="114" t="s">
-        <v>406</v>
+      <c r="B24" s="86" t="s">
+        <v>329</v>
+      </c>
+      <c r="C24" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D24" s="11">
         <v>1</v>
@@ -6156,8 +6096,8 @@
       <c r="E25" s="36">
         <v>42050</v>
       </c>
-      <c r="F25" s="109" t="s">
-        <v>225</v>
+      <c r="F25" s="106" t="s">
+        <v>221</v>
       </c>
       <c r="G25" s="36"/>
       <c r="H25" s="40"/>
@@ -6167,10 +6107,10 @@
       <c r="A26" s="17">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B26" s="90" t="s">
-        <v>354</v>
-      </c>
-      <c r="C26" s="96" t="s">
+      <c r="B26" s="87" t="s">
+        <v>315</v>
+      </c>
+      <c r="C26" s="93" t="s">
         <v>161</v>
       </c>
       <c r="D26" s="18">
@@ -6179,8 +6119,8 @@
       <c r="E26" s="36">
         <v>42050</v>
       </c>
-      <c r="F26" s="109" t="s">
-        <v>225</v>
+      <c r="F26" s="106" t="s">
+        <v>221</v>
       </c>
       <c r="G26" s="36"/>
       <c r="H26" s="40"/>
@@ -6190,8 +6130,8 @@
       <c r="A27" s="9">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B27" s="89" t="s">
-        <v>361</v>
+      <c r="B27" s="86" t="s">
+        <v>322</v>
       </c>
       <c r="C27" s="41" t="s">
         <v>161</v>
@@ -6209,11 +6149,11 @@
       <c r="A28" s="9">
         <v>5.2</v>
       </c>
-      <c r="B28" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="C28" s="114" t="s">
-        <v>406</v>
+      <c r="B28" s="86" t="s">
+        <v>330</v>
+      </c>
+      <c r="C28" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D28" s="11">
         <v>1</v>
@@ -6240,8 +6180,8 @@
       <c r="E29" s="36">
         <v>42057</v>
       </c>
-      <c r="F29" s="109" t="s">
-        <v>225</v>
+      <c r="F29" s="106" t="s">
+        <v>221</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="40"/>
@@ -6251,10 +6191,10 @@
       <c r="A30" s="17">
         <v>5.4</v>
       </c>
-      <c r="B30" s="99" t="s">
+      <c r="B30" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="96" t="s">
+      <c r="C30" s="93" t="s">
         <v>161</v>
       </c>
       <c r="D30" s="18">
@@ -6263,8 +6203,8 @@
       <c r="E30" s="36">
         <v>42057</v>
       </c>
-      <c r="F30" s="109" t="s">
-        <v>225</v>
+      <c r="F30" s="106" t="s">
+        <v>221</v>
       </c>
       <c r="G30" s="36"/>
       <c r="H30" s="40"/>
@@ -6274,8 +6214,8 @@
       <c r="A31" s="9">
         <v>6.1</v>
       </c>
-      <c r="B31" s="89" t="s">
-        <v>362</v>
+      <c r="B31" s="86" t="s">
+        <v>323</v>
       </c>
       <c r="C31" s="41" t="s">
         <v>161</v>
@@ -6291,11 +6231,11 @@
       <c r="A32" s="9">
         <v>6.2</v>
       </c>
-      <c r="B32" s="89" t="s">
-        <v>370</v>
-      </c>
-      <c r="C32" s="114" t="s">
-        <v>406</v>
+      <c r="B32" s="86" t="s">
+        <v>331</v>
+      </c>
+      <c r="C32" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D32" s="11">
         <v>1</v>
@@ -6308,8 +6248,8 @@
       <c r="A33" s="9">
         <v>6.3</v>
       </c>
-      <c r="B33" s="89" t="s">
-        <v>363</v>
+      <c r="B33" s="86" t="s">
+        <v>324</v>
       </c>
       <c r="C33" s="41" t="s">
         <v>161</v>
@@ -6325,11 +6265,11 @@
       <c r="A34" s="17">
         <v>6.4</v>
       </c>
-      <c r="B34" s="90" t="s">
-        <v>371</v>
-      </c>
-      <c r="C34" s="115" t="s">
-        <v>406</v>
+      <c r="B34" s="87" t="s">
+        <v>332</v>
+      </c>
+      <c r="C34" s="112" t="s">
+        <v>364</v>
       </c>
       <c r="D34" s="18">
         <v>1</v>
@@ -6342,8 +6282,8 @@
       <c r="A35" s="9">
         <v>7.1</v>
       </c>
-      <c r="B35" s="89" t="s">
-        <v>372</v>
+      <c r="B35" s="86" t="s">
+        <v>333</v>
       </c>
       <c r="C35" s="41" t="s">
         <v>161</v>
@@ -6358,11 +6298,11 @@
       <c r="A36" s="9">
         <v>7.2</v>
       </c>
-      <c r="B36" s="89" t="s">
-        <v>373</v>
-      </c>
-      <c r="C36" s="114" t="s">
-        <v>406</v>
+      <c r="B36" s="86" t="s">
+        <v>334</v>
+      </c>
+      <c r="C36" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D36" s="11">
         <v>1</v>
@@ -6373,10 +6313,10 @@
       <c r="A37" s="17">
         <v>7.4</v>
       </c>
-      <c r="B37" s="90" t="s">
-        <v>355</v>
-      </c>
-      <c r="C37" s="102" t="s">
+      <c r="B37" s="87" t="s">
+        <v>316</v>
+      </c>
+      <c r="C37" s="99" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="18">
@@ -6385,8 +6325,8 @@
       <c r="E37" s="35">
         <v>42071</v>
       </c>
-      <c r="F37" s="109" t="s">
-        <v>225</v>
+      <c r="F37" s="106" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -6403,27 +6343,27 @@
         <v>10</v>
       </c>
       <c r="E38" s="36"/>
-      <c r="F38" s="109" t="s">
-        <v>225</v>
+      <c r="F38" s="106" t="s">
+        <v>221</v>
       </c>
       <c r="G38" s="36"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="110">
+      <c r="A39" s="107">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="98" t="s">
+      <c r="C39" s="95" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="11">
         <v>50</v>
       </c>
       <c r="E39" s="36"/>
-      <c r="F39" s="108" t="s">
-        <v>225</v>
+      <c r="F39" s="105" t="s">
+        <v>221</v>
       </c>
       <c r="G39" s="36"/>
     </row>
@@ -6443,18 +6383,18 @@
       <c r="E40" s="35">
         <v>42076</v>
       </c>
-      <c r="F40" s="108" t="s">
-        <v>225</v>
+      <c r="F40" s="105" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17">
         <v>8.4</v>
       </c>
-      <c r="B41" s="99" t="s">
+      <c r="B41" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="102" t="s">
+      <c r="C41" s="99" t="s">
         <v>15</v>
       </c>
       <c r="D41" s="18">
@@ -6463,16 +6403,16 @@
       <c r="E41" s="35">
         <v>42078</v>
       </c>
-      <c r="F41" s="108" t="s">
-        <v>225</v>
+      <c r="F41" s="105" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>9.1</v>
       </c>
-      <c r="B42" s="89" t="s">
-        <v>374</v>
+      <c r="B42" s="86" t="s">
+        <v>335</v>
       </c>
       <c r="C42" s="41" t="s">
         <v>161</v>
@@ -6485,11 +6425,11 @@
       <c r="A43" s="9">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B43" s="89" t="s">
-        <v>375</v>
-      </c>
-      <c r="C43" s="114" t="s">
-        <v>406</v>
+      <c r="B43" s="86" t="s">
+        <v>336</v>
+      </c>
+      <c r="C43" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D43" s="11">
         <v>1</v>
@@ -6499,8 +6439,8 @@
       <c r="A44" s="9">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B44" s="89" t="s">
-        <v>377</v>
+      <c r="B44" s="86" t="s">
+        <v>338</v>
       </c>
       <c r="C44" s="41" t="s">
         <v>161</v>
@@ -6513,11 +6453,11 @@
       <c r="A45" s="9">
         <v>9.4</v>
       </c>
-      <c r="B45" s="89" t="s">
-        <v>376</v>
-      </c>
-      <c r="C45" s="114" t="s">
-        <v>406</v>
+      <c r="B45" s="86" t="s">
+        <v>337</v>
+      </c>
+      <c r="C45" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D45" s="11">
         <v>1</v>
@@ -6528,10 +6468,10 @@
       <c r="A46" s="17">
         <v>9.5</v>
       </c>
-      <c r="B46" s="90" t="s">
-        <v>380</v>
-      </c>
-      <c r="C46" s="103" t="s">
+      <c r="B46" s="87" t="s">
+        <v>341</v>
+      </c>
+      <c r="C46" s="100" t="s">
         <v>25</v>
       </c>
       <c r="D46" s="18">
@@ -6546,8 +6486,8 @@
       <c r="A47" s="9">
         <v>10.1</v>
       </c>
-      <c r="B47" s="89" t="s">
-        <v>381</v>
+      <c r="B47" s="86" t="s">
+        <v>342</v>
       </c>
       <c r="C47" s="41" t="s">
         <v>161</v>
@@ -6561,11 +6501,11 @@
       <c r="A48" s="9">
         <v>10.199999999999999</v>
       </c>
-      <c r="B48" s="89" t="s">
-        <v>382</v>
-      </c>
-      <c r="C48" s="114" t="s">
-        <v>406</v>
+      <c r="B48" s="86" t="s">
+        <v>343</v>
+      </c>
+      <c r="C48" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D48" s="11">
         <v>1</v>
@@ -6576,8 +6516,8 @@
       <c r="A49" s="9">
         <v>10.3</v>
       </c>
-      <c r="B49" s="89" t="s">
-        <v>383</v>
+      <c r="B49" s="86" t="s">
+        <v>344</v>
       </c>
       <c r="C49" s="41" t="s">
         <v>161</v>
@@ -6591,11 +6531,11 @@
       <c r="A50" s="17">
         <v>10.4</v>
       </c>
-      <c r="B50" s="90" t="s">
-        <v>384</v>
-      </c>
-      <c r="C50" s="115" t="s">
-        <v>406</v>
+      <c r="B50" s="87" t="s">
+        <v>345</v>
+      </c>
+      <c r="C50" s="112" t="s">
+        <v>364</v>
       </c>
       <c r="D50" s="18">
         <v>1</v>
@@ -6606,8 +6546,8 @@
       <c r="A51" s="9">
         <v>11.1</v>
       </c>
-      <c r="B51" s="89" t="s">
-        <v>385</v>
+      <c r="B51" s="86" t="s">
+        <v>346</v>
       </c>
       <c r="C51" s="41" t="s">
         <v>161</v>
@@ -6621,11 +6561,11 @@
       <c r="A52" s="9">
         <v>11.2</v>
       </c>
-      <c r="B52" s="89" t="s">
-        <v>386</v>
-      </c>
-      <c r="C52" s="114" t="s">
-        <v>406</v>
+      <c r="B52" s="86" t="s">
+        <v>347</v>
+      </c>
+      <c r="C52" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D52" s="11">
         <v>1</v>
@@ -6638,10 +6578,10 @@
       <c r="A53" s="17">
         <v>11.3</v>
       </c>
-      <c r="B53" s="90" t="s">
-        <v>378</v>
-      </c>
-      <c r="C53" s="95" t="s">
+      <c r="B53" s="87" t="s">
+        <v>339</v>
+      </c>
+      <c r="C53" s="92" t="s">
         <v>24</v>
       </c>
       <c r="D53" s="18">
@@ -6655,8 +6595,8 @@
       <c r="A54" s="9">
         <v>12.1</v>
       </c>
-      <c r="B54" s="89" t="s">
-        <v>390</v>
+      <c r="B54" s="86" t="s">
+        <v>351</v>
       </c>
       <c r="C54" s="41" t="s">
         <v>161</v>
@@ -6670,11 +6610,11 @@
       <c r="A55" s="9">
         <v>12.2</v>
       </c>
-      <c r="B55" s="89" t="s">
-        <v>391</v>
-      </c>
-      <c r="C55" s="114" t="s">
-        <v>406</v>
+      <c r="B55" s="86" t="s">
+        <v>352</v>
+      </c>
+      <c r="C55" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D55" s="11">
         <v>1</v>
@@ -6687,8 +6627,8 @@
       <c r="A56" s="9">
         <v>12.3</v>
       </c>
-      <c r="B56" s="89" t="s">
-        <v>392</v>
+      <c r="B56" s="86" t="s">
+        <v>353</v>
       </c>
       <c r="C56" s="41" t="s">
         <v>161</v>
@@ -6702,11 +6642,11 @@
       <c r="A57" s="9">
         <v>12.4</v>
       </c>
-      <c r="B57" s="89" t="s">
-        <v>393</v>
-      </c>
-      <c r="C57" s="114" t="s">
-        <v>406</v>
+      <c r="B57" s="86" t="s">
+        <v>354</v>
+      </c>
+      <c r="C57" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D57" s="11">
         <v>1</v>
@@ -6736,8 +6676,8 @@
       <c r="A59" s="9">
         <v>12.6</v>
       </c>
-      <c r="B59" s="89" t="s">
-        <v>387</v>
+      <c r="B59" s="86" t="s">
+        <v>348</v>
       </c>
       <c r="C59" s="28" t="s">
         <v>24</v>
@@ -6753,10 +6693,10 @@
       <c r="A60" s="17">
         <v>12.7</v>
       </c>
-      <c r="B60" s="99" t="s">
+      <c r="B60" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C60" s="102" t="s">
+      <c r="C60" s="99" t="s">
         <v>15</v>
       </c>
       <c r="D60" s="18">
@@ -6770,8 +6710,8 @@
       <c r="A61" s="9">
         <v>13.1</v>
       </c>
-      <c r="B61" s="89" t="s">
-        <v>394</v>
+      <c r="B61" s="86" t="s">
+        <v>355</v>
       </c>
       <c r="C61" s="41" t="s">
         <v>161</v>
@@ -6785,11 +6725,11 @@
       <c r="A62" s="9">
         <v>13.2</v>
       </c>
-      <c r="B62" s="89" t="s">
-        <v>395</v>
-      </c>
-      <c r="C62" s="114" t="s">
-        <v>406</v>
+      <c r="B62" s="86" t="s">
+        <v>356</v>
+      </c>
+      <c r="C62" s="111" t="s">
+        <v>364</v>
       </c>
       <c r="D62" s="11">
         <v>1</v>
@@ -6802,10 +6742,10 @@
       <c r="A63" s="17">
         <v>13.5</v>
       </c>
-      <c r="B63" s="90" t="s">
-        <v>388</v>
-      </c>
-      <c r="C63" s="95" t="s">
+      <c r="B63" s="87" t="s">
+        <v>349</v>
+      </c>
+      <c r="C63" s="92" t="s">
         <v>24</v>
       </c>
       <c r="D63" s="18">
@@ -6833,13 +6773,13 @@
       <c r="G64" s="37"/>
     </row>
     <row r="65" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="104">
+      <c r="A65" s="101">
         <v>14.2</v>
       </c>
-      <c r="B65" s="105" t="s">
+      <c r="B65" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="C65" s="102" t="s">
+      <c r="C65" s="99" t="s">
         <v>15</v>
       </c>
       <c r="D65" s="18">
@@ -6887,10 +6827,10 @@
       <c r="A68" s="17">
         <v>15.2</v>
       </c>
-      <c r="B68" s="105" t="s">
+      <c r="B68" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="C68" s="106" t="s">
+      <c r="C68" s="103" t="s">
         <v>15</v>
       </c>
       <c r="D68" s="18">
@@ -6941,7 +6881,7 @@
       <c r="B71" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C71" s="98" t="s">
+      <c r="C71" s="95" t="s">
         <v>14</v>
       </c>
       <c r="D71" s="11">
@@ -6972,8 +6912,8 @@
       <c r="A73" s="9">
         <v>16</v>
       </c>
-      <c r="B73" s="89" t="s">
-        <v>379</v>
+      <c r="B73" s="86" t="s">
+        <v>340</v>
       </c>
       <c r="C73" s="63" t="s">
         <v>25</v>
@@ -6992,10 +6932,10 @@
       <c r="A74" s="17">
         <v>16</v>
       </c>
-      <c r="B74" s="99" t="s">
+      <c r="B74" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C74" s="107" t="s">
+      <c r="C74" s="104" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="18">
@@ -7021,9 +6961,9 @@
       <c r="D75" s="11">
         <v>20</v>
       </c>
-      <c r="E75" s="111"/>
-      <c r="F75" s="109" t="s">
-        <v>225</v>
+      <c r="E75" s="108"/>
+      <c r="F75" s="106" t="s">
+        <v>221</v>
       </c>
       <c r="G75" s="37"/>
     </row>
@@ -7031,13 +6971,13 @@
       <c r="A76" s="9">
         <v>17</v>
       </c>
-      <c r="B76" s="93" t="s">
+      <c r="B76" s="90" t="s">
         <v>162</v>
       </c>
       <c r="C76" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D76" s="94">
+      <c r="D76" s="91">
         <v>5</v>
       </c>
       <c r="E76" s="37"/>

</xml_diff>

<commit_message>
add lit review quiz
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43034633-E533-4227-ABDA-FB7B66B29AFA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CD7462-4FCA-4715-BED7-A80D35292613}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="2340" windowWidth="22785" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topic_overview" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="403">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1743,6 +1743,10 @@
   </si>
   <si>
     <t>Data architecture and codebooks</t>
+  </si>
+  <si>
+    <t>[MWF](https://goo.gl/forms/dR2PqvSZRqRk3SB32) (Due 2/1) 
+[TR](https://goo.gl/forms/vR1hVhjph6m06bJZ2)  (Due 1/31)</t>
   </si>
 </sst>
 </file>
@@ -2935,7 +2939,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3124,7 +3128,7 @@
         <v>276</v>
       </c>
       <c r="F10" s="70" t="s">
-        <v>220</v>
+        <v>402</v>
       </c>
       <c r="G10" s="115" t="s">
         <v>363</v>

</xml_diff>

<commit_message>
add dm prep questions
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF1A443-1614-4E32-92F8-DE23185E0B56}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC0AC9B-BC82-4F8B-83D6-1FAEDBA5D3F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31260" yWindow="225" windowWidth="22785" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2955" yWindow="1425" windowWidth="22785" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topic_overview" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="406">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1755,6 +1755,9 @@
   <si>
     <t>[MWF](https://goo.gl/forms/NRn0XMQraDHww2c62) (Due 2/5) 
 [TR](https://goo.gl/forms/PpRhgP6Ol7R1v3Kb2)  (Due 2/6)</t>
+  </si>
+  <si>
+    <t>Data management preparation questions (in class worksheet [[PDF]](lecture/lec03_dm_prep_questions.pdf)[[HTML]](lecture/lec03_dm_prep_questions.html))</t>
   </si>
 </sst>
 </file>
@@ -2890,7 +2893,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3106,7 +3109,9 @@
       <c r="F11" s="56" t="s">
         <v>403</v>
       </c>
-      <c r="G11" s="58"/>
+      <c r="G11" s="58" t="s">
+        <v>405</v>
+      </c>
       <c r="H11" s="62"/>
       <c r="I11" s="61" t="s">
         <v>240</v>
@@ -4513,7 +4518,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
note about video links
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC0AC9B-BC82-4F8B-83D6-1FAEDBA5D3F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="1425" windowWidth="22785" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2955" yWindow="1425" windowWidth="22785" windowHeight="14265" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="topic_overview" sheetId="9" r:id="rId1"/>
@@ -21,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">points!$A$1:$D$97</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1632,9 +1631,6 @@
     <t>[hw04_data_management](hw/hw04_data_management.html) (Due 2/9)</t>
   </si>
   <si>
-    <t>hw05_univ_graphing (Due 2/16)</t>
-  </si>
-  <si>
     <t>hw06_biv_graphing (Due 2/23)</t>
   </si>
   <si>
@@ -1672,22 +1668,13 @@
     <t>Intro to the R language</t>
   </si>
   <si>
-    <t>Data Camp: Intro to Basics (Due 2/2)</t>
-  </si>
-  <si>
     <t>Using R for Data Analysis</t>
   </si>
   <si>
-    <t>Data Camp: Intro to R (Due 2/2)</t>
-  </si>
-  <si>
     <t>Graphing with ggplot</t>
   </si>
   <si>
     <t>Data Camp: Introduction to ggplot (Due 2/16)</t>
-  </si>
-  <si>
-    <t>Data Camp: Intro to Data (Due 2/23)</t>
   </si>
   <si>
     <t>Practice managing data in R</t>
@@ -1757,13 +1744,25 @@
 [TR](https://goo.gl/forms/PpRhgP6Ol7R1v3Kb2)  (Due 2/6)</t>
   </si>
   <si>
-    <t>Data management preparation questions (in class worksheet [[PDF]](lecture/lec03_dm_prep_questions.pdf)[[HTML]](lecture/lec03_dm_prep_questions.html))</t>
+    <t>Data management preparation questions (not turned in [[PDF]](lecture/lec03_dm_prep_questions.pdf)[[HTML]](lecture/lec03_dm_prep_questions.html))</t>
+  </si>
+  <si>
+    <t>Data Camp: Intro to Basics (BBL Quiz Due 2/2)</t>
+  </si>
+  <si>
+    <t>Data Camp: Intro to R (BBL Quiz Due 2/2)</t>
+  </si>
+  <si>
+    <t>hw05_univ_graphing (BBL Quiz Due 2/16)</t>
+  </si>
+  <si>
+    <t>Data Camp: Intro to Data (BBL Quiz Due 2/23)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
@@ -2549,10 +2548,10 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Percent 3" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Normal 3" xfId="80"/>
+    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Percent 3" xfId="81"/>
     <cellStyle name="Total" xfId="78" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2889,11 +2888,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2945,7 +2944,7 @@
         <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D2" s="64" t="s">
         <v>274</v>
@@ -2964,7 +2963,7 @@
         <v>1.2</v>
       </c>
       <c r="C3" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D3" s="64" t="s">
         <v>275</v>
@@ -2996,10 +2995,10 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="61"/>
       <c r="C5" t="s">
+        <v>374</v>
+      </c>
+      <c r="G5" t="s">
         <v>375</v>
-      </c>
-      <c r="G5" t="s">
-        <v>376</v>
       </c>
       <c r="H5" s="61"/>
       <c r="I5" s="61"/>
@@ -3009,7 +3008,7 @@
         <v>1.4</v>
       </c>
       <c r="C6" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D6" s="64" t="s">
         <v>298</v>
@@ -3018,7 +3017,7 @@
         <v>1.3</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H6" s="61"/>
       <c r="I6" s="61" t="s">
@@ -3028,10 +3027,10 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="61"/>
       <c r="C7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G7" t="s">
-        <v>378</v>
+        <v>402</v>
       </c>
       <c r="H7" s="61"/>
       <c r="I7" s="61"/>
@@ -3044,16 +3043,16 @@
         <v>262</v>
       </c>
       <c r="C8" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D8" s="64" t="s">
         <v>299</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="G8" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="H8" s="61"/>
       <c r="I8" s="61" t="s">
@@ -3063,10 +3062,10 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="61"/>
       <c r="C9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G9" t="s">
-        <v>380</v>
+        <v>403</v>
       </c>
       <c r="H9" s="61"/>
       <c r="I9" s="61"/>
@@ -3082,7 +3081,7 @@
         <v>276</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="G10" t="s">
         <v>363</v>
@@ -3107,10 +3106,10 @@
       </c>
       <c r="E11" s="57"/>
       <c r="F11" s="56" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="G11" s="58" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="H11" s="62"/>
       <c r="I11" s="61" t="s">
@@ -3131,7 +3130,7 @@
         <v>1.4</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="G12" t="s">
         <v>364</v>
@@ -3161,7 +3160,7 @@
         <v>220</v>
       </c>
       <c r="G13" t="s">
-        <v>365</v>
+        <v>404</v>
       </c>
       <c r="H13" s="61" t="s">
         <v>227</v>
@@ -3173,10 +3172,10 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="61"/>
       <c r="C14" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G14" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H14" s="61"/>
       <c r="I14" s="61"/>
@@ -3201,7 +3200,7 @@
         <v>220</v>
       </c>
       <c r="G15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H15" s="61"/>
       <c r="I15" s="61"/>
@@ -3209,11 +3208,11 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="61"/>
       <c r="C16" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E16" s="59"/>
       <c r="G16" t="s">
-        <v>383</v>
+        <v>405</v>
       </c>
       <c r="H16" s="61"/>
       <c r="I16" s="61"/>
@@ -3245,7 +3244,7 @@
       </c>
       <c r="E18" s="59"/>
       <c r="G18" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="H18" s="61"/>
       <c r="I18" s="61"/>
@@ -3300,7 +3299,7 @@
         <v>306</v>
       </c>
       <c r="G21" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H21" s="61"/>
       <c r="I21" s="61"/>
@@ -3316,7 +3315,7 @@
         <v>4.5</v>
       </c>
       <c r="G22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H22" s="61">
         <v>4.4000000000000004</v>
@@ -3376,7 +3375,7 @@
         <v>6.1</v>
       </c>
       <c r="G25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H25" s="61"/>
       <c r="I25" s="61"/>
@@ -3485,7 +3484,7 @@
         <v>307</v>
       </c>
       <c r="G30" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="H30" s="61"/>
       <c r="I30" s="61"/>
@@ -3510,7 +3509,7 @@
         <v>220</v>
       </c>
       <c r="G31" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H31" s="61"/>
       <c r="I31" s="61" t="s">
@@ -3547,7 +3546,7 @@
         <v>220</v>
       </c>
       <c r="G33" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H33" s="61"/>
       <c r="I33" s="61" t="s">
@@ -3603,7 +3602,7 @@
         <v>308</v>
       </c>
       <c r="G36" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="H36" s="61"/>
       <c r="I36" s="61"/>
@@ -3651,7 +3650,7 @@
         <v>288</v>
       </c>
       <c r="G39" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H39" s="61"/>
       <c r="I39" s="61"/>
@@ -3667,7 +3666,7 @@
         <v>310</v>
       </c>
       <c r="G40" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H40" s="61"/>
       <c r="I40" s="61"/>
@@ -3680,13 +3679,13 @@
         <v>222</v>
       </c>
       <c r="G41" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H41" s="61"/>
       <c r="I41" s="61"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I41">
+  <sortState ref="A2:I41">
     <sortCondition ref="A2:A41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3695,7 +3694,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -3849,7 +3848,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>5</v>
       </c>
@@ -3903,7 +3902,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>7</v>
       </c>
@@ -4171,7 +4170,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -4739,7 +4738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z91"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -5043,7 +5042,7 @@
         <v>1.4</v>
       </c>
       <c r="B5" s="92" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C5" s="51" t="s">
         <v>161</v>
@@ -5102,10 +5101,10 @@
         <v>1.5</v>
       </c>
       <c r="B6" s="92" t="s">
+        <v>391</v>
+      </c>
+      <c r="C6" s="88" t="s">
         <v>395</v>
-      </c>
-      <c r="C6" s="88" t="s">
-        <v>399</v>
       </c>
       <c r="D6" s="97">
         <v>1</v>
@@ -5291,7 +5290,7 @@
         <v>2.1</v>
       </c>
       <c r="B9" s="92" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C9" s="51" t="s">
         <v>161</v>
@@ -5322,10 +5321,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" s="92" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C10" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D10" s="97">
         <v>1</v>
@@ -5356,7 +5355,7 @@
         <v>358</v>
       </c>
       <c r="C12" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D12" s="97">
         <v>1</v>
@@ -5472,7 +5471,7 @@
         <v>323</v>
       </c>
       <c r="C18" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D18" s="97">
         <v>1</v>
@@ -5506,7 +5505,7 @@
         <v>324</v>
       </c>
       <c r="C20" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D20" s="97">
         <v>1</v>
@@ -5580,7 +5579,7 @@
         <v>325</v>
       </c>
       <c r="C24" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D24" s="97">
         <v>1</v>
@@ -5614,7 +5613,7 @@
         <v>326</v>
       </c>
       <c r="C26" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D26" s="97">
         <v>1</v>
@@ -5692,7 +5691,7 @@
         <v>327</v>
       </c>
       <c r="C30" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D30" s="97">
         <v>1</v>
@@ -5764,7 +5763,7 @@
         <v>328</v>
       </c>
       <c r="C34" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D34" s="97">
         <v>1</v>
@@ -5794,7 +5793,7 @@
         <v>329</v>
       </c>
       <c r="C36" s="89" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D36" s="98">
         <v>1</v>
@@ -5823,7 +5822,7 @@
         <v>331</v>
       </c>
       <c r="C38" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D38" s="97">
         <v>1</v>
@@ -5846,7 +5845,7 @@
         <v>42067</v>
       </c>
       <c r="F39" s="95" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5854,7 +5853,7 @@
         <v>7.4</v>
       </c>
       <c r="B40" s="96" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C40" s="83" t="s">
         <v>13</v>
@@ -5960,7 +5959,7 @@
         <v>333</v>
       </c>
       <c r="C46" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D46" s="97">
         <v>1</v>
@@ -5988,7 +5987,7 @@
         <v>334</v>
       </c>
       <c r="C48" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D48" s="97">
         <v>1</v>
@@ -6033,7 +6032,7 @@
         <v>340</v>
       </c>
       <c r="C51" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D51" s="97">
         <v>1</v>
@@ -6061,7 +6060,7 @@
         <v>342</v>
       </c>
       <c r="C53" s="89" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D53" s="98">
         <v>1</v>
@@ -6089,7 +6088,7 @@
         <v>344</v>
       </c>
       <c r="C55" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D55" s="97">
         <v>1</v>
@@ -6131,7 +6130,7 @@
         <v>349</v>
       </c>
       <c r="C58" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D58" s="97">
         <v>1</v>
@@ -6159,7 +6158,7 @@
         <v>351</v>
       </c>
       <c r="C60" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D60" s="97">
         <v>1</v>
@@ -6229,7 +6228,7 @@
         <v>353</v>
       </c>
       <c r="C65" s="88" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D65" s="97">
         <v>1</v>
@@ -6746,7 +6745,7 @@
       <c r="V91" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D112">
+  <sortState ref="A2:D112">
     <sortCondition ref="A2:A112"/>
   </sortState>
   <conditionalFormatting sqref="N2:N8">

</xml_diff>

<commit_message>
add link to prob quiz
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1785,8 +1785,8 @@
     <t>[Poster prep Stage I](project.html)* (Draft Due 3/12, PR 3/14, Final 3/16)</t>
   </si>
   <si>
-    <t>[MWF]() (Due 2/26) 
-[TR]()  (Due 2/27)</t>
+    <t>[MWF](https://goo.gl/forms/rkvMKfdvnvyEmsiI2) (Due 2/26) 
+[TR](https://goo.gl/forms/bmy0TdVHTNM9M3IC3)  (Due 2/27)</t>
   </si>
 </sst>
 </file>
@@ -2931,7 +2931,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3305,7 +3305,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="61">
         <v>6.2</v>
       </c>
@@ -3318,7 +3318,7 @@
       <c r="E19" s="55">
         <v>3</v>
       </c>
-      <c r="F19" s="101" t="s">
+      <c r="F19" s="56" t="s">
         <v>413</v>
       </c>
       <c r="H19" s="61" t="s">

</xml_diff>

<commit_message>
add quiz links to schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH315/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B584D59C-03D5-4B48-BBC3-5FCF5C6E4CEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30645" yWindow="525" windowWidth="22785" windowHeight="14265" tabRatio="500"/>
+    <workbookView xWindow="2820" yWindow="520" windowWidth="22780" windowHeight="14260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topic_overview" sheetId="9" r:id="rId1"/>
@@ -20,17 +21,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">points!$A$1:$D$97</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1442,15 +1437,6 @@
     <t>Research Proposal</t>
   </si>
   <si>
-    <t>Setting up the story: Stage I</t>
-  </si>
-  <si>
-    <t>EDA: Stage II</t>
-  </si>
-  <si>
-    <t>Inferential Analysis: Stage III</t>
-  </si>
-  <si>
     <t>Poster Draft</t>
   </si>
   <si>
@@ -1774,10 +1760,6 @@
     <t>[Notes](lecture/lec02_writing_empirical_research.html)</t>
   </si>
   <si>
-    <t>[MWF]() (Due 3/2) 
-[TR]()  (Due 3/2)</t>
-  </si>
-  <si>
     <t xml:space="preserve">[hw07 research proposal](hw/hw07_research_proposal.html)* (Draft Due 3/5, PR 3/7, Final 3/9)
 </t>
   </si>
@@ -1787,12 +1769,25 @@
   <si>
     <t>[MWF](https://goo.gl/forms/rkvMKfdvnvyEmsiI2) (Due 2/26) 
 [TR](https://goo.gl/forms/bmy0TdVHTNM9M3IC3)  (Due 2/27)</t>
+  </si>
+  <si>
+    <t>Multivariable Analysis: Stage III</t>
+  </si>
+  <si>
+    <t>Bivariate analysis: Stage II</t>
+  </si>
+  <si>
+    <t>[MWF](https://goo.gl/forms/Opaan0cjxISk3rh73) (Due 3/2) 
+[TR](https://goo.gl/forms/Qhj0nd4WrgaPYJkU2)  (Due 3/2)</t>
+  </si>
+  <si>
+    <t>Setting up the story: Stage 1a, Exploratory Data Analysis: Stage 1b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
@@ -2587,10 +2582,10 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Normal 3" xfId="80"/>
-    <cellStyle name="Percent 2" xfId="52"/>
-    <cellStyle name="Percent 3" xfId="81"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Percent 3" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
     <cellStyle name="Total" xfId="78" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2927,26 +2922,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9" style="55"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.625" style="64" customWidth="1"/>
-    <col min="5" max="5" width="13.875" style="55" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="64" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="55" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="56" customWidth="1"/>
-    <col min="7" max="7" width="64.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="55" customWidth="1"/>
-    <col min="9" max="9" width="31.625" style="55" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" style="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="55" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="55" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>231</v>
       </c>
@@ -2975,7 +2970,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="61">
         <v>1.1000000000000001</v>
       </c>
@@ -2983,7 +2978,7 @@
         <v>257</v>
       </c>
       <c r="C2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D2" s="64" t="s">
         <v>270</v>
@@ -2992,17 +2987,17 @@
         <v>207</v>
       </c>
       <c r="G2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="H2" s="61"/>
       <c r="I2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="61">
         <v>1.2</v>
       </c>
       <c r="C3" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D3" s="64" t="s">
         <v>271</v>
@@ -3015,7 +3010,7 @@
       </c>
       <c r="I3" s="61"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="61">
         <v>1.3</v>
       </c>
@@ -3031,25 +3026,25 @@
       </c>
       <c r="I4" s="61"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="61">
         <v>1.4</v>
       </c>
       <c r="C5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G5" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="H5" s="61"/>
       <c r="I5" s="61"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="61">
         <v>1.5</v>
       </c>
       <c r="C6" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D6" s="64" t="s">
         <v>294</v>
@@ -3058,27 +3053,27 @@
         <v>1.3</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="H6" s="61"/>
       <c r="I6" s="61" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="61">
         <v>1.6</v>
       </c>
       <c r="C7" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G7" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H7" s="61"/>
       <c r="I7" s="61"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="61">
         <v>2.1</v>
       </c>
@@ -3086,36 +3081,36 @@
         <v>258</v>
       </c>
       <c r="C8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D8" s="64" t="s">
         <v>295</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="H8" s="61"/>
       <c r="I8" s="61" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="61">
         <v>2.2000000000000002</v>
       </c>
       <c r="C9" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G9" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H9" s="61"/>
       <c r="I9" s="61"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="61">
         <v>2.2999999999999998</v>
       </c>
@@ -3126,17 +3121,17 @@
         <v>272</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G10" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="H10" s="61"/>
       <c r="I10" s="61" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="62">
         <v>3.1</v>
       </c>
@@ -3151,17 +3146,17 @@
       </c>
       <c r="E11" s="57"/>
       <c r="F11" s="56" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G11" s="58" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="H11" s="62"/>
       <c r="I11" s="61" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="61">
         <v>3.2</v>
       </c>
@@ -3175,17 +3170,17 @@
         <v>1.4</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G12" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="H12" s="61"/>
       <c r="I12" s="61" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="61">
         <v>4.0999999999999996</v>
       </c>
@@ -3193,7 +3188,7 @@
         <v>260</v>
       </c>
       <c r="C13" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D13" s="64" t="s">
         <v>275</v>
@@ -3202,50 +3197,50 @@
         <v>2.1</v>
       </c>
       <c r="G13" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H13" s="61" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I13" s="61" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="61">
         <v>4.2</v>
       </c>
       <c r="C14" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D14" s="64" t="s">
         <v>275</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F14" s="56" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="H14" s="61"/>
       <c r="I14" s="61"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="61">
         <v>4.3</v>
       </c>
       <c r="C15" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G15" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="H15" s="99" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I15" s="61"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="61">
         <v>5.0999999999999996</v>
       </c>
@@ -3253,7 +3248,7 @@
         <v>261</v>
       </c>
       <c r="C16" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D16" s="64" t="s">
         <v>276</v>
@@ -3262,29 +3257,29 @@
         <v>229</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G16" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H16" s="61"/>
       <c r="I16" s="61"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="61">
         <v>5.2</v>
       </c>
       <c r="C17" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E17" s="59"/>
       <c r="G17" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H17" s="61"/>
       <c r="I17" s="61"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="61">
         <v>6.1</v>
       </c>
@@ -3295,17 +3290,17 @@
         <v>209</v>
       </c>
       <c r="D18" s="64" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="H18" s="62"/>
       <c r="I18" s="61" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="61">
         <v>6.2</v>
       </c>
@@ -3319,14 +3314,14 @@
         <v>3</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="H19" s="61" t="s">
         <v>224</v>
       </c>
       <c r="I19" s="61"/>
     </row>
-    <row r="20" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="61">
         <v>6.3</v>
       </c>
@@ -3334,30 +3329,30 @@
         <v>301</v>
       </c>
       <c r="E20" s="59"/>
-      <c r="F20" s="101" t="s">
-        <v>410</v>
+      <c r="F20" s="56" t="s">
+        <v>412</v>
       </c>
       <c r="G20" s="100" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="H20" s="61"/>
       <c r="I20" s="61"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="61">
         <v>6.4</v>
       </c>
       <c r="C21" t="s">
-        <v>302</v>
+        <v>413</v>
       </c>
       <c r="F21" s="101"/>
       <c r="G21" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="H21" s="61"/>
       <c r="I21" s="61"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="61">
         <v>7.1</v>
       </c>
@@ -3378,7 +3373,7 @@
       </c>
       <c r="I22" s="61"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="61">
         <v>7.2</v>
       </c>
@@ -3392,14 +3387,14 @@
         <v>218</v>
       </c>
       <c r="G23" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H23" s="61">
         <v>4.4000000000000004</v>
       </c>
       <c r="I23" s="61"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="61">
         <v>8.1</v>
       </c>
@@ -3415,7 +3410,7 @@
       <c r="H24" s="61"/>
       <c r="I24" s="61"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="61">
         <v>9.1</v>
       </c>
@@ -3441,7 +3436,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="61">
         <v>9.1999999999999993</v>
       </c>
@@ -3452,12 +3447,12 @@
         <v>6.1</v>
       </c>
       <c r="G26" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="H26" s="61"/>
       <c r="I26" s="61"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="61">
         <v>10.1</v>
       </c>
@@ -3483,7 +3478,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="61">
         <v>10.199999999999999</v>
       </c>
@@ -3504,7 +3499,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="61">
         <v>11</v>
       </c>
@@ -3530,7 +3525,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="61">
         <v>11.1</v>
       </c>
@@ -3553,20 +3548,20 @@
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="61">
         <v>11.2</v>
       </c>
       <c r="C31" t="s">
-        <v>303</v>
+        <v>411</v>
       </c>
       <c r="G31" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="H31" s="61"/>
       <c r="I31" s="61"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="61">
         <v>12</v>
       </c>
@@ -3586,14 +3581,14 @@
         <v>218</v>
       </c>
       <c r="G32" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="H32" s="61"/>
       <c r="I32" s="61" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="61">
         <v>12.2</v>
       </c>
@@ -3606,7 +3601,7 @@
       <c r="H33" s="61"/>
       <c r="I33" s="61"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="61">
         <v>12.3</v>
       </c>
@@ -3623,14 +3618,14 @@
         <v>218</v>
       </c>
       <c r="G34" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="H34" s="61"/>
       <c r="I34" s="61" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="61">
         <v>12.4</v>
       </c>
@@ -3646,7 +3641,7 @@
       <c r="H35" s="61"/>
       <c r="I35" s="61"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="61">
         <v>13</v>
       </c>
@@ -3668,7 +3663,7 @@
       <c r="H36" s="61"/>
       <c r="I36" s="61"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="61">
         <v>14.1</v>
       </c>
@@ -3676,20 +3671,20 @@
         <v>269</v>
       </c>
       <c r="C37" t="s">
-        <v>304</v>
+        <v>410</v>
       </c>
       <c r="G37" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="H37" s="61"/>
       <c r="I37" s="61"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="61">
         <v>14.2</v>
       </c>
       <c r="C38" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E38" s="55">
         <v>8.4</v>
@@ -3700,7 +3695,7 @@
       <c r="H38" s="61"/>
       <c r="I38" s="61"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="61">
         <v>14.3</v>
       </c>
@@ -3713,7 +3708,7 @@
       <c r="H39" s="61"/>
       <c r="I39" s="61"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="61">
         <v>15</v>
       </c>
@@ -3721,18 +3716,18 @@
         <v>255</v>
       </c>
       <c r="C40" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D40" s="64" t="s">
         <v>284</v>
       </c>
       <c r="G40" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="H40" s="61"/>
       <c r="I40" s="61"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="61">
         <v>16</v>
       </c>
@@ -3740,15 +3735,15 @@
         <v>256</v>
       </c>
       <c r="C41" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G41" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="H41" s="61"/>
       <c r="I41" s="61"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="61">
         <v>16.100000000000001</v>
       </c>
@@ -3756,7 +3751,7 @@
         <v>220</v>
       </c>
       <c r="G42" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="H42" s="61"/>
       <c r="I42" s="61"/>
@@ -3771,7 +3766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -3779,20 +3774,20 @@
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="25" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="25" customWidth="1"/>
-    <col min="3" max="3" width="33.625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="36.125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="47.625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="45.875" style="26" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" style="26" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" style="26" customWidth="1"/>
     <col min="7" max="7" width="61" style="26" customWidth="1"/>
     <col min="8" max="8" width="46.5" style="26" customWidth="1"/>
-    <col min="9" max="16384" width="14.875" style="25"/>
+    <col min="9" max="16384" width="14.83203125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -3818,7 +3813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -3844,7 +3839,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A3" s="38">
         <v>2</v>
       </c>
@@ -3871,7 +3866,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="304" x14ac:dyDescent="0.2">
       <c r="A4" s="38">
         <v>3</v>
       </c>
@@ -3898,7 +3893,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="360" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="365" x14ac:dyDescent="0.2">
       <c r="A5" s="38">
         <v>4</v>
       </c>
@@ -3925,7 +3920,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="38">
         <v>5</v>
       </c>
@@ -3952,7 +3947,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
         <v>6</v>
       </c>
@@ -3979,7 +3974,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A8" s="38">
         <v>7</v>
       </c>
@@ -4006,7 +4001,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="38">
         <v>8</v>
       </c>
@@ -4023,7 +4018,7 @@
       <c r="G9" s="52"/>
       <c r="H9" s="53"/>
     </row>
-    <row r="10" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A10" s="38">
         <v>9</v>
       </c>
@@ -4050,7 +4045,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="38">
         <v>10</v>
       </c>
@@ -4077,7 +4072,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A12" s="38">
         <v>11</v>
       </c>
@@ -4102,7 +4097,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A13" s="38">
         <v>12</v>
       </c>
@@ -4129,7 +4124,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A14" s="38"/>
       <c r="B14" s="39">
         <f t="shared" si="0"/>
@@ -4152,7 +4147,7 @@
       </c>
       <c r="H14" s="42"/>
     </row>
-    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="38">
         <v>13</v>
       </c>
@@ -4179,7 +4174,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="38">
         <v>14</v>
       </c>
@@ -4204,7 +4199,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="38">
         <v>15</v>
       </c>
@@ -4221,7 +4216,7 @@
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
         <v>0</v>
       </c>
@@ -4247,7 +4242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -4255,21 +4250,21 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="25" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="25" customWidth="1"/>
-    <col min="3" max="3" width="33.625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="27.375" style="26" customWidth="1"/>
-    <col min="5" max="5" width="47.625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="45.875" style="26" customWidth="1"/>
-    <col min="7" max="7" width="30.125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" style="26" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" style="26" customWidth="1"/>
     <col min="8" max="9" width="38" style="26" customWidth="1"/>
     <col min="10" max="10" width="46.5" style="26" customWidth="1"/>
-    <col min="11" max="16384" width="14.875" style="25"/>
+    <col min="11" max="16384" width="14.83203125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -4301,7 +4296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -4334,7 +4329,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="240" x14ac:dyDescent="0.2">
       <c r="A3" s="38">
         <v>2</v>
       </c>
@@ -4367,7 +4362,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="256" x14ac:dyDescent="0.2">
       <c r="A4" s="38">
         <v>3</v>
       </c>
@@ -4400,7 +4395,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="300" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="320" x14ac:dyDescent="0.2">
       <c r="A5" s="38">
         <v>4</v>
       </c>
@@ -4433,7 +4428,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="38">
         <v>5</v>
       </c>
@@ -4466,7 +4461,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="160" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
         <v>6</v>
       </c>
@@ -4499,7 +4494,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="270" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A8" s="38">
         <v>7</v>
       </c>
@@ -4532,7 +4527,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="208" x14ac:dyDescent="0.2">
       <c r="A9" s="38">
         <v>8</v>
       </c>
@@ -4561,7 +4556,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A10" s="38">
         <v>9</v>
       </c>
@@ -4594,7 +4589,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="160" x14ac:dyDescent="0.2">
       <c r="A11" s="38">
         <v>10</v>
       </c>
@@ -4627,7 +4622,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A12" s="38">
         <v>11</v>
       </c>
@@ -4658,7 +4653,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="38">
         <v>12</v>
       </c>
@@ -4679,7 +4674,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="42"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="38"/>
       <c r="B14" s="39">
         <f t="shared" si="0"/>
@@ -4696,7 +4691,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="41"/>
     </row>
-    <row r="15" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="128" x14ac:dyDescent="0.2">
       <c r="A15" s="38">
         <v>13</v>
       </c>
@@ -4727,7 +4722,7 @@
       </c>
       <c r="J15" s="42"/>
     </row>
-    <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="38">
         <v>14</v>
       </c>
@@ -4760,7 +4755,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="38">
         <v>15</v>
       </c>
@@ -4787,7 +4782,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
         <v>0</v>
       </c>
@@ -4815,33 +4810,33 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z91"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="5"/>
-    <col min="2" max="2" width="40.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="5"/>
+    <col min="2" max="2" width="40.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="8"/>
+    <col min="4" max="4" width="7.6640625" style="8"/>
     <col min="5" max="5" width="10.5" style="27" customWidth="1"/>
-    <col min="6" max="6" width="7.625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="27" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="27" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="4" customWidth="1"/>
     <col min="9" max="9" width="10" style="5" customWidth="1"/>
-    <col min="10" max="10" width="7.625" style="5"/>
-    <col min="11" max="11" width="4.625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="10.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="7.625" style="4"/>
+    <col min="10" max="10" width="7.6640625" style="5"/>
+    <col min="11" max="11" width="4.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="7.6640625" style="4"/>
     <col min="16" max="16" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="7.625" style="4"/>
+    <col min="17" max="16384" width="7.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -4855,13 +4850,13 @@
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>9</v>
@@ -4910,7 +4905,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -4978,12 +4973,12 @@
         <v>3.0837004405286344E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1.2</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>25</v>
@@ -5046,7 +5041,7 @@
         <v>0.21806167400881057</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1.3</v>
       </c>
@@ -5114,12 +5109,12 @@
         <v>4.405286343612335E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>1.4</v>
       </c>
       <c r="B5" s="92" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C5" s="51" t="s">
         <v>161</v>
@@ -5173,15 +5168,15 @@
         <v>6.8281938325991193E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>1.5</v>
       </c>
       <c r="B6" s="92" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C6" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D6" s="97">
         <v>1</v>
@@ -5236,12 +5231,12 @@
         <v>2.2026431718061675E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>1.6</v>
       </c>
       <c r="B7" s="70" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C7" s="72" t="s">
         <v>161</v>
@@ -5302,12 +5297,12 @@
         <v>0.38546255506607929</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>1.7</v>
       </c>
       <c r="B8" s="71" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C8" s="80" t="s">
         <v>24</v>
@@ -5362,12 +5357,12 @@
         <v>0.23127753303964757</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>2.1</v>
       </c>
       <c r="B9" s="92" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C9" s="51" t="s">
         <v>161</v>
@@ -5393,15 +5388,15 @@
       </c>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" s="92" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C10" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D10" s="97">
         <v>1</v>
@@ -5409,12 +5404,12 @@
       <c r="F10" s="84"/>
       <c r="G10" s="84"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>2.2999999999999998</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C11" s="51" t="s">
         <v>161</v>
@@ -5424,22 +5419,22 @@
       </c>
       <c r="F11" s="29"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>2.4</v>
       </c>
       <c r="B12" s="70" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C12" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D12" s="97">
         <v>1</v>
       </c>
       <c r="F12" s="29"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>2.5</v>
       </c>
@@ -5459,12 +5454,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>2.6</v>
       </c>
       <c r="B14" s="70" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C14" s="72" t="s">
         <v>161</v>
@@ -5481,7 +5476,7 @@
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>2.7</v>
       </c>
@@ -5503,12 +5498,12 @@
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>2.8</v>
       </c>
       <c r="B16" s="90" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C16" s="83" t="s">
         <v>13</v>
@@ -5523,12 +5518,12 @@
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>3.1</v>
       </c>
       <c r="B17" s="70" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>161</v>
@@ -5540,15 +5535,15 @@
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>3.2</v>
       </c>
       <c r="B18" s="70" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C18" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D18" s="97">
         <v>1</v>
@@ -5557,12 +5552,12 @@
       <c r="H18" s="29"/>
       <c r="I18" s="29"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>3.3</v>
       </c>
       <c r="B19" s="70" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>161</v>
@@ -5574,15 +5569,15 @@
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>3.4</v>
       </c>
       <c r="B20" s="70" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C20" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D20" s="97">
         <v>1</v>
@@ -5591,12 +5586,12 @@
       <c r="H20" s="29"/>
       <c r="I20" s="29"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>3.5</v>
       </c>
       <c r="B21" s="70" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C21" s="87" t="s">
         <v>15</v>
@@ -5613,7 +5608,7 @@
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>3.6</v>
       </c>
@@ -5633,12 +5628,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>4.0999999999999996</v>
       </c>
       <c r="B23" s="70" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>161</v>
@@ -5648,15 +5643,15 @@
       </c>
       <c r="F23" s="44"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>4.2</v>
       </c>
       <c r="B24" s="70" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C24" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D24" s="97">
         <v>1</v>
@@ -5665,12 +5660,12 @@
       <c r="H24" s="29"/>
       <c r="I24" s="29"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>4.3</v>
       </c>
       <c r="B25" s="70" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>161</v>
@@ -5682,15 +5677,15 @@
       <c r="H25" s="29"/>
       <c r="I25" s="29"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="B26" s="70" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C26" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D26" s="97">
         <v>1</v>
@@ -5699,7 +5694,7 @@
       <c r="H26" s="29"/>
       <c r="I26" s="29"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>4.5</v>
       </c>
@@ -5721,12 +5716,12 @@
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>4.5999999999999996</v>
       </c>
       <c r="B28" s="71" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C28" s="76" t="s">
         <v>161</v>
@@ -5743,12 +5738,12 @@
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>5.0999999999999996</v>
       </c>
       <c r="B29" s="70" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C29" s="30" t="s">
         <v>161</v>
@@ -5760,15 +5755,15 @@
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>5.2</v>
       </c>
       <c r="B30" s="70" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C30" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D30" s="97">
         <v>1</v>
@@ -5777,7 +5772,7 @@
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>5.3</v>
       </c>
@@ -5797,7 +5792,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>5.4</v>
       </c>
@@ -5817,12 +5812,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>6.1</v>
       </c>
       <c r="B33" s="70" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C33" s="30" t="s">
         <v>161</v>
@@ -5832,27 +5827,27 @@
       </c>
       <c r="F33" s="45"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>6.2</v>
       </c>
       <c r="B34" s="70" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C34" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D34" s="97">
         <v>1</v>
       </c>
       <c r="F34" s="45"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>6.3</v>
       </c>
       <c r="B35" s="70" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>161</v>
@@ -5862,27 +5857,27 @@
       </c>
       <c r="F35" s="45"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>6.4</v>
       </c>
       <c r="B36" s="71" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C36" s="89" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D36" s="98">
         <v>1</v>
       </c>
       <c r="F36" s="45"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>7.1</v>
       </c>
       <c r="B37" s="70" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C37" s="30" t="s">
         <v>161</v>
@@ -5891,26 +5886,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>7.2</v>
       </c>
       <c r="B38" s="70" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C38" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D38" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>7.3</v>
       </c>
       <c r="B39" s="93" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C39" s="94" t="s">
         <v>15</v>
@@ -5922,15 +5917,15 @@
         <v>42067</v>
       </c>
       <c r="F39" s="95" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>7.4</v>
       </c>
       <c r="B40" s="96" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C40" s="83" t="s">
         <v>13</v>
@@ -5940,7 +5935,7 @@
       </c>
       <c r="F40" s="84"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>8.1</v>
       </c>
@@ -5957,7 +5952,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="85">
         <v>8.1999999999999993</v>
       </c>
@@ -5974,7 +5969,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>8.3000000000000007</v>
       </c>
@@ -5994,7 +5989,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>8.4</v>
       </c>
@@ -6014,12 +6009,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>9.1</v>
       </c>
       <c r="B45" s="70" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C45" s="30" t="s">
         <v>161</v>
@@ -6028,26 +6023,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>9.1999999999999993</v>
       </c>
       <c r="B46" s="70" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C46" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D46" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>9.3000000000000007</v>
       </c>
       <c r="B47" s="70" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C47" s="30" t="s">
         <v>161</v>
@@ -6056,26 +6051,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>9.4</v>
       </c>
       <c r="B48" s="70" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C48" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D48" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>9.5</v>
       </c>
       <c r="B49" s="71" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C49" s="82" t="s">
         <v>25</v>
@@ -6087,12 +6082,12 @@
         <v>42092</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>10.1</v>
       </c>
       <c r="B50" s="70" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C50" s="30" t="s">
         <v>161</v>
@@ -6101,26 +6096,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>10.199999999999999</v>
       </c>
       <c r="B51" s="70" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C51" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D51" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>10.3</v>
       </c>
       <c r="B52" s="70" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C52" s="30" t="s">
         <v>161</v>
@@ -6129,26 +6124,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
         <v>10.4</v>
       </c>
       <c r="B53" s="71" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C53" s="89" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D53" s="98">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>11.1</v>
       </c>
       <c r="B54" s="70" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C54" s="30" t="s">
         <v>161</v>
@@ -6157,26 +6152,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <v>11.2</v>
       </c>
       <c r="B55" s="70" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C55" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D55" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>11.3</v>
       </c>
       <c r="B56" s="71" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C56" s="75" t="s">
         <v>24</v>
@@ -6185,12 +6180,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
         <v>12.1</v>
       </c>
       <c r="B57" s="70" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C57" s="30" t="s">
         <v>161</v>
@@ -6199,26 +6194,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
         <v>12.2</v>
       </c>
       <c r="B58" s="70" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C58" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D58" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
         <v>12.3</v>
       </c>
       <c r="B59" s="70" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C59" s="30" t="s">
         <v>161</v>
@@ -6227,21 +6222,21 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>12.4</v>
       </c>
       <c r="B60" s="70" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C60" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D60" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <v>12.5</v>
       </c>
@@ -6255,12 +6250,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>12.6</v>
       </c>
       <c r="B62" s="70" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C62" s="21" t="s">
         <v>24</v>
@@ -6269,7 +6264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
         <v>12.7</v>
       </c>
@@ -6283,12 +6278,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <v>13.1</v>
       </c>
       <c r="B64" s="70" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C64" s="30" t="s">
         <v>161</v>
@@ -6297,26 +6292,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>13.2</v>
       </c>
       <c r="B65" s="70" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C65" s="88" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D65" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
         <v>13.5</v>
       </c>
       <c r="B66" s="71" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C66" s="75" t="s">
         <v>24</v>
@@ -6325,7 +6320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" s="5">
         <v>14.1</v>
       </c>
@@ -6339,7 +6334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
         <v>14.2</v>
       </c>
@@ -6353,7 +6348,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>15</v>
       </c>
@@ -6367,7 +6362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
         <v>15.1</v>
       </c>
@@ -6381,7 +6376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12">
         <v>15.2</v>
       </c>
@@ -6395,7 +6390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
         <v>16</v>
       </c>
@@ -6409,7 +6404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
         <v>16</v>
       </c>
@@ -6423,7 +6418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
         <v>16</v>
       </c>
@@ -6437,7 +6432,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" s="5">
         <v>16</v>
       </c>
@@ -6451,12 +6446,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
         <v>16</v>
       </c>
       <c r="B76" s="70" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C76" s="49" t="s">
         <v>25</v>
@@ -6465,7 +6460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:22" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
         <v>16</v>
       </c>
@@ -6494,7 +6489,7 @@
       <c r="U77" s="4"/>
       <c r="V77" s="4"/>
     </row>
-    <row r="78" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="5">
         <v>17</v>
       </c>
@@ -6525,7 +6520,7 @@
       <c r="U78" s="4"/>
       <c r="V78" s="4"/>
     </row>
-    <row r="79" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5">
         <v>17</v>
       </c>
@@ -6554,7 +6549,7 @@
       <c r="U79" s="4"/>
       <c r="V79" s="4"/>
     </row>
-    <row r="80" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
         <v>17</v>
       </c>
@@ -6585,7 +6580,7 @@
       <c r="U80" s="4"/>
       <c r="V80" s="4"/>
     </row>
-    <row r="81" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="8"/>
@@ -6605,7 +6600,7 @@
       <c r="U81" s="4"/>
       <c r="V81" s="4"/>
     </row>
-    <row r="82" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="8"/>
@@ -6627,7 +6622,7 @@
       <c r="U82" s="4"/>
       <c r="V82" s="4"/>
     </row>
-    <row r="83" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="8"/>
@@ -6649,7 +6644,7 @@
       <c r="U83" s="4"/>
       <c r="V83" s="4"/>
     </row>
-    <row r="84" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="8"/>
@@ -6671,7 +6666,7 @@
       <c r="U84" s="4"/>
       <c r="V84" s="4"/>
     </row>
-    <row r="85" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="8"/>
@@ -6693,7 +6688,7 @@
       <c r="U85" s="4"/>
       <c r="V85" s="4"/>
     </row>
-    <row r="86" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="8"/>
@@ -6715,7 +6710,7 @@
       <c r="U86" s="4"/>
       <c r="V86" s="4"/>
     </row>
-    <row r="87" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="8"/>
@@ -6737,7 +6732,7 @@
       <c r="U87" s="4"/>
       <c r="V87" s="4"/>
     </row>
-    <row r="88" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="8"/>
@@ -6759,7 +6754,7 @@
       <c r="U88" s="4"/>
       <c r="V88" s="4"/>
     </row>
-    <row r="89" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="8"/>
@@ -6781,7 +6776,7 @@
       <c r="U89" s="4"/>
       <c r="V89" s="4"/>
     </row>
-    <row r="90" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="8"/>
@@ -6801,7 +6796,7 @@
       <c r="U90" s="4"/>
       <c r="V90" s="4"/>
     </row>
-    <row r="91" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="8"/>

</xml_diff>

<commit_message>
ad wk 7 and worksheets
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH315/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B584D59C-03D5-4B48-BBC3-5FCF5C6E4CEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A92571-887D-4D98-9EB0-EEAACF799C76}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="520" windowWidth="22780" windowHeight="14260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topic_overview" sheetId="9" r:id="rId1"/>
@@ -21,11 +21,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">points!$A$1:$D$97</definedName>
   </definedNames>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="416">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1420,9 +1426,6 @@
     <t>[14 (42 min)](https://passiondrivenstatistics.com/2016/10/06/r-chapter-17/)</t>
   </si>
   <si>
-    <t>3/14 (02) &amp;  3/15 (01)</t>
-  </si>
-  <si>
     <t xml:space="preserve">6 (2/24) </t>
   </si>
   <si>
@@ -1605,9 +1608,6 @@
     <t>[hw04_data_management](hw/hw04_data_management.html) (Due 2/9)</t>
   </si>
   <si>
-    <t>foundations worksheet (Due with midterm)</t>
-  </si>
-  <si>
     <t>hw08_bivariate_inference (Due 4/13)</t>
   </si>
   <si>
@@ -1781,7 +1781,19 @@
 [TR](https://goo.gl/forms/Qhj0nd4WrgaPYJkU2)  (Due 3/2)</t>
   </si>
   <si>
-    <t>Setting up the story: Stage 1a, Exploratory Data Analysis: Stage 1b</t>
+    <t xml:space="preserve">3/14 (02) &amp;  3/15 (01)  [Sample exam](reading/sample_exam_1.pdf) available. </t>
+  </si>
+  <si>
+    <t>[foundations worksheet](hw/foundations_worksheet.docx) (Due with midterm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worksheets on identifying [parameters vs statistics](hw/Parameters_v_Statistics.docx) and the [CLT](hw/Discovering_the_CLT.docx). </t>
+  </si>
+  <si>
+    <t>Poster Prep Stage I: Setting up the story &amp; exploratory data analysis</t>
+  </si>
+  <si>
+    <t>Foundations for Inference</t>
   </si>
 </sst>
 </file>
@@ -2923,25 +2935,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" style="55"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="64" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="55" customWidth="1"/>
+    <col min="4" max="4" width="10.625" style="64" customWidth="1"/>
+    <col min="5" max="5" width="13.875" style="55" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="56" customWidth="1"/>
-    <col min="7" max="7" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="55" customWidth="1"/>
-    <col min="9" max="9" width="31.6640625" style="55" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.625" style="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="55" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="55" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="60" t="s">
         <v>231</v>
       </c>
@@ -2952,10 +2964,10 @@
         <v>206</v>
       </c>
       <c r="D1" s="67" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1" s="68" t="s">
         <v>299</v>
-      </c>
-      <c r="E1" s="68" t="s">
-        <v>300</v>
       </c>
       <c r="F1" s="69" t="s">
         <v>161</v>
@@ -2970,7 +2982,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="61">
         <v>1.1000000000000001</v>
       </c>
@@ -2978,7 +2990,7 @@
         <v>257</v>
       </c>
       <c r="C2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D2" s="64" t="s">
         <v>270</v>
@@ -2987,17 +2999,17 @@
         <v>207</v>
       </c>
       <c r="G2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H2" s="61"/>
       <c r="I2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="61">
         <v>1.2</v>
       </c>
       <c r="C3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D3" s="64" t="s">
         <v>271</v>
@@ -3010,7 +3022,7 @@
       </c>
       <c r="I3" s="61"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="61">
         <v>1.3</v>
       </c>
@@ -3026,25 +3038,25 @@
       </c>
       <c r="I4" s="61"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="61">
         <v>1.4</v>
       </c>
       <c r="C5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H5" s="61"/>
       <c r="I5" s="61"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="61">
         <v>1.5</v>
       </c>
       <c r="C6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D6" s="64" t="s">
         <v>294</v>
@@ -3053,27 +3065,27 @@
         <v>1.3</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H6" s="61"/>
       <c r="I6" s="61" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="61">
         <v>1.6</v>
       </c>
       <c r="C7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H7" s="61"/>
       <c r="I7" s="61"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="61">
         <v>2.1</v>
       </c>
@@ -3081,36 +3093,36 @@
         <v>258</v>
       </c>
       <c r="C8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D8" s="64" t="s">
         <v>295</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H8" s="61"/>
       <c r="I8" s="61" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="61">
         <v>2.2000000000000002</v>
       </c>
       <c r="C9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G9" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H9" s="61"/>
       <c r="I9" s="61"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="61">
         <v>2.2999999999999998</v>
       </c>
@@ -3121,17 +3133,17 @@
         <v>272</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H10" s="61"/>
       <c r="I10" s="61" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="62">
         <v>3.1</v>
       </c>
@@ -3146,17 +3158,17 @@
       </c>
       <c r="E11" s="57"/>
       <c r="F11" s="56" t="s">
+        <v>386</v>
+      </c>
+      <c r="G11" s="58" t="s">
         <v>388</v>
-      </c>
-      <c r="G11" s="58" t="s">
-        <v>390</v>
       </c>
       <c r="H11" s="62"/>
       <c r="I11" s="61" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="61">
         <v>3.2</v>
       </c>
@@ -3170,17 +3182,17 @@
         <v>1.4</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H12" s="61"/>
       <c r="I12" s="61" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="61">
         <v>4.0999999999999996</v>
       </c>
@@ -3188,7 +3200,7 @@
         <v>260</v>
       </c>
       <c r="C13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D13" s="64" t="s">
         <v>275</v>
@@ -3197,50 +3209,50 @@
         <v>2.1</v>
       </c>
       <c r="G13" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H13" s="61" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I13" s="61" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="61">
         <v>4.2</v>
       </c>
       <c r="C14" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D14" s="64" t="s">
         <v>275</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F14" s="56" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H14" s="61"/>
       <c r="I14" s="61"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="61">
         <v>4.3</v>
       </c>
       <c r="C15" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G15" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H15" s="99" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I15" s="61"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="61">
         <v>5.0999999999999996</v>
       </c>
@@ -3248,7 +3260,7 @@
         <v>261</v>
       </c>
       <c r="C16" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D16" s="64" t="s">
         <v>276</v>
@@ -3257,50 +3269,50 @@
         <v>229</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G16" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H16" s="61"/>
       <c r="I16" s="61"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="61">
         <v>5.2</v>
       </c>
       <c r="C17" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E17" s="59"/>
       <c r="G17" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H17" s="61"/>
       <c r="I17" s="61"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="61">
         <v>6.1</v>
       </c>
       <c r="B18" s="55" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C18" t="s">
         <v>209</v>
       </c>
       <c r="D18" s="64" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H18" s="62"/>
       <c r="I18" s="61" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="61">
         <v>6.2</v>
       </c>
@@ -3314,45 +3326,45 @@
         <v>3</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H19" s="61" t="s">
         <v>224</v>
       </c>
       <c r="I19" s="61"/>
     </row>
-    <row r="20" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="61">
         <v>6.3</v>
       </c>
       <c r="C20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E20" s="59"/>
       <c r="F20" s="56" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G20" s="100" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H20" s="61"/>
       <c r="I20" s="61"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="61">
         <v>6.4</v>
       </c>
       <c r="C21" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F21" s="101"/>
       <c r="G21" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H21" s="61"/>
       <c r="I21" s="61"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="61">
         <v>7.1</v>
       </c>
@@ -3368,12 +3380,15 @@
       <c r="E22" s="55" t="s">
         <v>252</v>
       </c>
+      <c r="G22" t="s">
+        <v>413</v>
+      </c>
       <c r="H22" s="61" t="s">
         <v>250</v>
       </c>
       <c r="I22" s="61"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="61">
         <v>7.2</v>
       </c>
@@ -3386,15 +3401,12 @@
       <c r="F23" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="G23" t="s">
-        <v>358</v>
-      </c>
       <c r="H23" s="61">
         <v>4.4000000000000004</v>
       </c>
       <c r="I23" s="61"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="61">
         <v>8.1</v>
       </c>
@@ -3402,363 +3414,376 @@
         <v>264</v>
       </c>
       <c r="C24" t="s">
-        <v>219</v>
+        <v>415</v>
       </c>
       <c r="G24" t="s">
-        <v>297</v>
+        <v>412</v>
       </c>
       <c r="H24" s="61"/>
       <c r="I24" s="61"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="61">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C25" t="s">
+        <v>219</v>
+      </c>
+      <c r="G25" t="s">
+        <v>411</v>
+      </c>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="61">
         <v>9.1</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B26" s="55" t="s">
         <v>265</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>212</v>
       </c>
-      <c r="D25" s="64" t="s">
+      <c r="D26" s="64" t="s">
         <v>289</v>
       </c>
-      <c r="E25" s="55" t="s">
+      <c r="E26" s="55" t="s">
         <v>249</v>
       </c>
-      <c r="F25" s="56" t="s">
+      <c r="F26" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="H25" s="63" t="s">
+      <c r="H26" s="63" t="s">
         <v>247</v>
       </c>
-      <c r="I25" s="61" t="s">
+      <c r="I26" s="61" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="61">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="61">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>230</v>
       </c>
-      <c r="E26" s="55">
+      <c r="E27" s="55">
         <v>6.1</v>
       </c>
-      <c r="G26" t="s">
-        <v>359</v>
-      </c>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="61">
+      <c r="G27" t="s">
+        <v>357</v>
+      </c>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="61">
         <v>10.1</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B28" s="55" t="s">
         <v>262</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>213</v>
       </c>
-      <c r="D27" s="64" t="s">
+      <c r="D28" s="64" t="s">
         <v>278</v>
       </c>
-      <c r="E27" s="55">
+      <c r="E28" s="55">
         <v>6.2</v>
-      </c>
-      <c r="F27" s="56" t="s">
-        <v>218</v>
-      </c>
-      <c r="H27" s="61">
-        <v>6.6</v>
-      </c>
-      <c r="I27" s="61" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="61">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="C28" t="s">
-        <v>214</v>
-      </c>
-      <c r="D28" s="64" t="s">
-        <v>279</v>
-      </c>
-      <c r="E28" s="55">
-        <v>6.3</v>
       </c>
       <c r="F28" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="H28" s="61"/>
+      <c r="H28" s="61">
+        <v>6.6</v>
+      </c>
       <c r="I28" s="61" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="61">
-        <v>11</v>
-      </c>
-      <c r="B29" s="55" t="s">
-        <v>266</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D29" s="64" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E29" s="55">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="F29" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="H29" s="61">
-        <v>7.1</v>
-      </c>
+      <c r="H29" s="61"/>
       <c r="I29" s="61" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="61">
-        <v>11.1</v>
+        <v>11</v>
+      </c>
+      <c r="B30" s="55" t="s">
+        <v>266</v>
       </c>
       <c r="C30" t="s">
-        <v>254</v>
+        <v>215</v>
       </c>
       <c r="D30" s="64" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E30" s="55">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="F30" s="56" t="s">
         <v>218</v>
       </c>
       <c r="H30" s="61">
+        <v>7.1</v>
+      </c>
+      <c r="I30" s="61" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="61">
+        <v>11.1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>254</v>
+      </c>
+      <c r="D31" s="64" t="s">
+        <v>285</v>
+      </c>
+      <c r="E31" s="55">
+        <v>6.5</v>
+      </c>
+      <c r="F31" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="H31" s="61">
         <v>7.3</v>
       </c>
-      <c r="I30" s="61" t="s">
+      <c r="I31" s="61" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="61">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="61">
         <v>11.2</v>
       </c>
-      <c r="C31" t="s">
-        <v>411</v>
-      </c>
-      <c r="G31" t="s">
-        <v>371</v>
-      </c>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="61">
+      <c r="C32" t="s">
+        <v>409</v>
+      </c>
+      <c r="G32" t="s">
+        <v>369</v>
+      </c>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="61">
         <v>12</v>
       </c>
-      <c r="B32" s="55" t="s">
+      <c r="B33" s="55" t="s">
         <v>267</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>216</v>
       </c>
-      <c r="D32" s="64" t="s">
+      <c r="D33" s="64" t="s">
         <v>281</v>
       </c>
-      <c r="E32" s="55">
+      <c r="E33" s="55">
         <v>7</v>
       </c>
-      <c r="F32" s="56" t="s">
+      <c r="F33" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="G32" t="s">
-        <v>360</v>
-      </c>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61" t="s">
+      <c r="G33" t="s">
+        <v>358</v>
+      </c>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="61">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="61">
         <v>12.2</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>217</v>
       </c>
-      <c r="D33" s="64" t="s">
+      <c r="D34" s="64" t="s">
         <v>283</v>
       </c>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="61">
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="61">
         <v>12.3</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>291</v>
       </c>
-      <c r="D34" s="64" t="s">
+      <c r="D35" s="64" t="s">
         <v>282</v>
       </c>
-      <c r="E34" s="59" t="s">
+      <c r="E35" s="59" t="s">
         <v>292</v>
       </c>
-      <c r="F34" s="56" t="s">
+      <c r="F35" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="G34" t="s">
-        <v>361</v>
-      </c>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61" t="s">
+      <c r="G35" t="s">
+        <v>359</v>
+      </c>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="61">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="61">
         <v>12.4</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>290</v>
       </c>
-      <c r="D35" s="64" t="s">
+      <c r="D36" s="64" t="s">
         <v>293</v>
       </c>
-      <c r="E35" s="59" t="s">
+      <c r="E36" s="59" t="s">
         <v>286</v>
-      </c>
-      <c r="H35" s="61"/>
-      <c r="I35" s="61"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="61">
-        <v>13</v>
-      </c>
-      <c r="B36" s="55" t="s">
-        <v>268</v>
-      </c>
-      <c r="C36" t="s">
-        <v>226</v>
-      </c>
-      <c r="D36" s="64" t="s">
-        <v>296</v>
-      </c>
-      <c r="E36" s="59" t="s">
-        <v>287</v>
-      </c>
-      <c r="F36" s="56" t="s">
-        <v>218</v>
       </c>
       <c r="H36" s="61"/>
       <c r="I36" s="61"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="61">
-        <v>14.1</v>
+        <v>13</v>
       </c>
       <c r="B37" s="55" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C37" t="s">
-        <v>410</v>
-      </c>
-      <c r="G37" t="s">
-        <v>372</v>
+        <v>226</v>
+      </c>
+      <c r="D37" s="64" t="s">
+        <v>296</v>
+      </c>
+      <c r="E37" s="59" t="s">
+        <v>287</v>
+      </c>
+      <c r="F37" s="56" t="s">
+        <v>218</v>
       </c>
       <c r="H37" s="61"/>
       <c r="I37" s="61"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="61">
-        <v>14.2</v>
+        <v>14.1</v>
+      </c>
+      <c r="B38" s="55" t="s">
+        <v>269</v>
       </c>
       <c r="C38" t="s">
-        <v>340</v>
-      </c>
-      <c r="E38" s="55">
-        <v>8.4</v>
-      </c>
-      <c r="F38" s="56" t="s">
-        <v>218</v>
+        <v>408</v>
+      </c>
+      <c r="G38" t="s">
+        <v>370</v>
       </c>
       <c r="H38" s="61"/>
       <c r="I38" s="61"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="61">
-        <v>14.3</v>
+        <v>14.2</v>
       </c>
       <c r="C39" t="s">
-        <v>221</v>
-      </c>
-      <c r="E39" s="59">
+        <v>339</v>
+      </c>
+      <c r="E39" s="55">
         <v>8.4</v>
+      </c>
+      <c r="F39" s="56" t="s">
+        <v>218</v>
       </c>
       <c r="H39" s="61"/>
       <c r="I39" s="61"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="61">
-        <v>15</v>
-      </c>
-      <c r="B40" s="55" t="s">
-        <v>255</v>
+        <v>14.3</v>
       </c>
       <c r="C40" t="s">
-        <v>302</v>
-      </c>
-      <c r="D40" s="64" t="s">
-        <v>284</v>
-      </c>
-      <c r="G40" t="s">
-        <v>373</v>
+        <v>221</v>
+      </c>
+      <c r="E40" s="59">
+        <v>8.4</v>
       </c>
       <c r="H40" s="61"/>
       <c r="I40" s="61"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="61">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41" s="55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C41" t="s">
-        <v>303</v>
+        <v>301</v>
+      </c>
+      <c r="D41" s="64" t="s">
+        <v>284</v>
       </c>
       <c r="G41" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="H41" s="61"/>
       <c r="I41" s="61"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="61">
-        <v>16.100000000000001</v>
+        <v>16</v>
+      </c>
+      <c r="B42" s="55" t="s">
+        <v>256</v>
       </c>
       <c r="C42" t="s">
-        <v>220</v>
+        <v>302</v>
       </c>
       <c r="G42" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="H42" s="61"/>
       <c r="I42" s="61"/>
     </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="61">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C43" t="s">
+        <v>220</v>
+      </c>
+      <c r="G43" t="s">
+        <v>361</v>
+      </c>
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:I42">
-    <sortCondition ref="A2:A42"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I43">
+    <sortCondition ref="A2:A43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3774,20 +3799,20 @@
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="25" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="25" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="45.83203125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="33.625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="36.125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="47.625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="45.875" style="26" customWidth="1"/>
     <col min="7" max="7" width="61" style="26" customWidth="1"/>
     <col min="8" max="8" width="46.5" style="26" customWidth="1"/>
-    <col min="9" max="16384" width="14.83203125" style="25"/>
+    <col min="9" max="16384" width="14.875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -3813,7 +3838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -3839,7 +3864,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
         <v>2</v>
       </c>
@@ -3866,7 +3891,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
         <v>3</v>
       </c>
@@ -3893,7 +3918,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="365" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="360" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
         <v>4</v>
       </c>
@@ -3920,7 +3945,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>5</v>
       </c>
@@ -3947,7 +3972,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <v>6</v>
       </c>
@@ -3974,7 +3999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>7</v>
       </c>
@@ -4001,7 +4026,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>8</v>
       </c>
@@ -4018,7 +4043,7 @@
       <c r="G9" s="52"/>
       <c r="H9" s="53"/>
     </row>
-    <row r="10" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
         <v>9</v>
       </c>
@@ -4045,7 +4070,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>10</v>
       </c>
@@ -4072,7 +4097,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>11</v>
       </c>
@@ -4097,7 +4122,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
         <v>12</v>
       </c>
@@ -4124,7 +4149,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="39">
         <f t="shared" si="0"/>
@@ -4147,7 +4172,7 @@
       </c>
       <c r="H14" s="42"/>
     </row>
-    <row r="15" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>13</v>
       </c>
@@ -4174,7 +4199,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
         <v>14</v>
       </c>
@@ -4199,7 +4224,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
         <v>15</v>
       </c>
@@ -4216,7 +4241,7 @@
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>0</v>
       </c>
@@ -4250,21 +4275,21 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="25" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="25" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="45.83203125" style="26" customWidth="1"/>
-    <col min="7" max="7" width="30.1640625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="33.625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="27.375" style="26" customWidth="1"/>
+    <col min="5" max="5" width="47.625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="45.875" style="26" customWidth="1"/>
+    <col min="7" max="7" width="30.125" style="26" customWidth="1"/>
     <col min="8" max="9" width="38" style="26" customWidth="1"/>
     <col min="10" max="10" width="46.5" style="26" customWidth="1"/>
-    <col min="11" max="16384" width="14.83203125" style="25"/>
+    <col min="11" max="16384" width="14.875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -4296,7 +4321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -4329,7 +4354,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="240" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
         <v>2</v>
       </c>
@@ -4362,7 +4387,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="256" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
         <v>3</v>
       </c>
@@ -4395,7 +4420,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="320" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="300" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
         <v>4</v>
       </c>
@@ -4428,7 +4453,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="160" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>5</v>
       </c>
@@ -4461,7 +4486,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="160" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <v>6</v>
       </c>
@@ -4494,7 +4519,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="272" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="270" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>7</v>
       </c>
@@ -4527,7 +4552,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="208" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>8</v>
       </c>
@@ -4556,7 +4581,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="176" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
         <v>9</v>
       </c>
@@ -4589,7 +4614,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="160" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>10</v>
       </c>
@@ -4622,7 +4647,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="176" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>11</v>
       </c>
@@ -4653,7 +4678,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
         <v>12</v>
       </c>
@@ -4674,7 +4699,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="42"/>
     </row>
-    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="39">
         <f t="shared" si="0"/>
@@ -4691,7 +4716,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="41"/>
     </row>
-    <row r="15" spans="1:11" ht="128" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>13</v>
       </c>
@@ -4722,7 +4747,7 @@
       </c>
       <c r="J15" s="42"/>
     </row>
-    <row r="16" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
         <v>14</v>
       </c>
@@ -4755,7 +4780,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
         <v>15</v>
       </c>
@@ -4782,7 +4807,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>0</v>
       </c>
@@ -4817,26 +4842,26 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="5"/>
-    <col min="2" max="2" width="40.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="5"/>
+    <col min="2" max="2" width="40.625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="8"/>
+    <col min="4" max="4" width="7.625" style="8"/>
     <col min="5" max="5" width="10.5" style="27" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="7.625" style="27" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="27" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="4" customWidth="1"/>
     <col min="9" max="9" width="10" style="5" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" style="5"/>
-    <col min="11" max="11" width="4.6640625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="7.6640625" style="4"/>
+    <col min="10" max="10" width="7.625" style="5"/>
+    <col min="11" max="11" width="4.625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="10.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="7.625" style="4"/>
     <col min="16" max="16" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="7.6640625" style="4"/>
+    <col min="17" max="16384" width="7.625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -4850,13 +4875,13 @@
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>349</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>9</v>
@@ -4905,7 +4930,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -4973,12 +4998,12 @@
         <v>3.0837004405286344E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1.2</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>25</v>
@@ -5041,7 +5066,7 @@
         <v>0.21806167400881057</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1.3</v>
       </c>
@@ -5109,12 +5134,12 @@
         <v>4.405286343612335E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1.4</v>
       </c>
       <c r="B5" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C5" s="51" t="s">
         <v>161</v>
@@ -5168,15 +5193,15 @@
         <v>6.8281938325991193E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1.5</v>
       </c>
       <c r="B6" s="92" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C6" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D6" s="97">
         <v>1</v>
@@ -5231,12 +5256,12 @@
         <v>2.2026431718061675E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1.6</v>
       </c>
       <c r="B7" s="70" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C7" s="72" t="s">
         <v>161</v>
@@ -5297,12 +5322,12 @@
         <v>0.38546255506607929</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>1.7</v>
       </c>
       <c r="B8" s="71" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C8" s="80" t="s">
         <v>24</v>
@@ -5357,12 +5382,12 @@
         <v>0.23127753303964757</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>2.1</v>
       </c>
       <c r="B9" s="92" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C9" s="51" t="s">
         <v>161</v>
@@ -5388,15 +5413,15 @@
       </c>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" s="92" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C10" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D10" s="97">
         <v>1</v>
@@ -5404,12 +5429,12 @@
       <c r="F10" s="84"/>
       <c r="G10" s="84"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>2.2999999999999998</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C11" s="51" t="s">
         <v>161</v>
@@ -5419,22 +5444,22 @@
       </c>
       <c r="F11" s="29"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>2.4</v>
       </c>
       <c r="B12" s="70" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C12" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D12" s="97">
         <v>1</v>
       </c>
       <c r="F12" s="29"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>2.5</v>
       </c>
@@ -5454,12 +5479,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>2.6</v>
       </c>
       <c r="B14" s="70" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C14" s="72" t="s">
         <v>161</v>
@@ -5476,7 +5501,7 @@
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>2.7</v>
       </c>
@@ -5498,12 +5523,12 @@
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
     </row>
-    <row r="16" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>2.8</v>
       </c>
       <c r="B16" s="90" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C16" s="83" t="s">
         <v>13</v>
@@ -5518,12 +5543,12 @@
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>3.1</v>
       </c>
       <c r="B17" s="70" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>161</v>
@@ -5535,15 +5560,15 @@
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>3.2</v>
       </c>
       <c r="B18" s="70" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C18" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D18" s="97">
         <v>1</v>
@@ -5552,12 +5577,12 @@
       <c r="H18" s="29"/>
       <c r="I18" s="29"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>3.3</v>
       </c>
       <c r="B19" s="70" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>161</v>
@@ -5569,15 +5594,15 @@
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>3.4</v>
       </c>
       <c r="B20" s="70" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C20" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D20" s="97">
         <v>1</v>
@@ -5586,12 +5611,12 @@
       <c r="H20" s="29"/>
       <c r="I20" s="29"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>3.5</v>
       </c>
       <c r="B21" s="70" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C21" s="87" t="s">
         <v>15</v>
@@ -5608,7 +5633,7 @@
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
     </row>
-    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>3.6</v>
       </c>
@@ -5628,12 +5653,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>4.0999999999999996</v>
       </c>
       <c r="B23" s="70" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>161</v>
@@ -5643,15 +5668,15 @@
       </c>
       <c r="F23" s="44"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>4.2</v>
       </c>
       <c r="B24" s="70" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C24" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D24" s="97">
         <v>1</v>
@@ -5660,12 +5685,12 @@
       <c r="H24" s="29"/>
       <c r="I24" s="29"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>4.3</v>
       </c>
       <c r="B25" s="70" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>161</v>
@@ -5677,15 +5702,15 @@
       <c r="H25" s="29"/>
       <c r="I25" s="29"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="B26" s="70" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C26" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D26" s="97">
         <v>1</v>
@@ -5694,7 +5719,7 @@
       <c r="H26" s="29"/>
       <c r="I26" s="29"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>4.5</v>
       </c>
@@ -5716,12 +5741,12 @@
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
     </row>
-    <row r="28" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>4.5999999999999996</v>
       </c>
       <c r="B28" s="71" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C28" s="76" t="s">
         <v>161</v>
@@ -5738,12 +5763,12 @@
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>5.0999999999999996</v>
       </c>
       <c r="B29" s="70" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C29" s="30" t="s">
         <v>161</v>
@@ -5755,15 +5780,15 @@
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>5.2</v>
       </c>
       <c r="B30" s="70" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C30" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D30" s="97">
         <v>1</v>
@@ -5772,7 +5797,7 @@
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>5.3</v>
       </c>
@@ -5792,7 +5817,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>5.4</v>
       </c>
@@ -5812,12 +5837,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>6.1</v>
       </c>
       <c r="B33" s="70" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C33" s="30" t="s">
         <v>161</v>
@@ -5827,27 +5852,27 @@
       </c>
       <c r="F33" s="45"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>6.2</v>
       </c>
       <c r="B34" s="70" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C34" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D34" s="97">
         <v>1</v>
       </c>
       <c r="F34" s="45"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>6.3</v>
       </c>
       <c r="B35" s="70" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>161</v>
@@ -5857,27 +5882,27 @@
       </c>
       <c r="F35" s="45"/>
     </row>
-    <row r="36" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>6.4</v>
       </c>
       <c r="B36" s="71" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C36" s="89" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D36" s="98">
         <v>1</v>
       </c>
       <c r="F36" s="45"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>7.1</v>
       </c>
       <c r="B37" s="70" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C37" s="30" t="s">
         <v>161</v>
@@ -5886,26 +5911,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>7.2</v>
       </c>
       <c r="B38" s="70" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C38" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D38" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>7.3</v>
       </c>
       <c r="B39" s="93" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C39" s="94" t="s">
         <v>15</v>
@@ -5917,15 +5942,15 @@
         <v>42067</v>
       </c>
       <c r="F39" s="95" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
         <v>7.4</v>
       </c>
       <c r="B40" s="96" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C40" s="83" t="s">
         <v>13</v>
@@ -5935,7 +5960,7 @@
       </c>
       <c r="F40" s="84"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>8.1</v>
       </c>
@@ -5952,7 +5977,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="85">
         <v>8.1999999999999993</v>
       </c>
@@ -5969,7 +5994,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>8.3000000000000007</v>
       </c>
@@ -5989,7 +6014,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12">
         <v>8.4</v>
       </c>
@@ -6009,12 +6034,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>9.1</v>
       </c>
       <c r="B45" s="70" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C45" s="30" t="s">
         <v>161</v>
@@ -6023,26 +6048,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>9.1999999999999993</v>
       </c>
       <c r="B46" s="70" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C46" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D46" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>9.3000000000000007</v>
       </c>
       <c r="B47" s="70" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C47" s="30" t="s">
         <v>161</v>
@@ -6051,26 +6076,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>9.4</v>
       </c>
       <c r="B48" s="70" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C48" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D48" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="12">
         <v>9.5</v>
       </c>
       <c r="B49" s="71" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C49" s="82" t="s">
         <v>25</v>
@@ -6082,12 +6107,12 @@
         <v>42092</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>10.1</v>
       </c>
       <c r="B50" s="70" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C50" s="30" t="s">
         <v>161</v>
@@ -6096,26 +6121,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>10.199999999999999</v>
       </c>
       <c r="B51" s="70" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C51" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D51" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>10.3</v>
       </c>
       <c r="B52" s="70" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C52" s="30" t="s">
         <v>161</v>
@@ -6124,26 +6149,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12">
         <v>10.4</v>
       </c>
       <c r="B53" s="71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C53" s="89" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D53" s="98">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>11.1</v>
       </c>
       <c r="B54" s="70" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C54" s="30" t="s">
         <v>161</v>
@@ -6152,26 +6177,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>11.2</v>
       </c>
       <c r="B55" s="70" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C55" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D55" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12">
         <v>11.3</v>
       </c>
       <c r="B56" s="71" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C56" s="75" t="s">
         <v>24</v>
@@ -6180,12 +6205,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>12.1</v>
       </c>
       <c r="B57" s="70" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C57" s="30" t="s">
         <v>161</v>
@@ -6194,26 +6219,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>12.2</v>
       </c>
       <c r="B58" s="70" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C58" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D58" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>12.3</v>
       </c>
       <c r="B59" s="70" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C59" s="30" t="s">
         <v>161</v>
@@ -6222,21 +6247,21 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>12.4</v>
       </c>
       <c r="B60" s="70" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C60" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D60" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>12.5</v>
       </c>
@@ -6250,12 +6275,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>12.6</v>
       </c>
       <c r="B62" s="70" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C62" s="21" t="s">
         <v>24</v>
@@ -6264,7 +6289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12">
         <v>12.7</v>
       </c>
@@ -6278,12 +6303,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>13.1</v>
       </c>
       <c r="B64" s="70" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C64" s="30" t="s">
         <v>161</v>
@@ -6292,26 +6317,26 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>13.2</v>
       </c>
       <c r="B65" s="70" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C65" s="88" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D65" s="97">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12">
         <v>13.5</v>
       </c>
       <c r="B66" s="71" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C66" s="75" t="s">
         <v>24</v>
@@ -6320,7 +6345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>14.1</v>
       </c>
@@ -6334,7 +6359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12">
         <v>14.2</v>
       </c>
@@ -6348,7 +6373,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>15</v>
       </c>
@@ -6362,7 +6387,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>15.1</v>
       </c>
@@ -6376,7 +6401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12">
         <v>15.2</v>
       </c>
@@ -6390,7 +6415,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>16</v>
       </c>
@@ -6404,7 +6429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>16</v>
       </c>
@@ -6418,7 +6443,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>16</v>
       </c>
@@ -6432,7 +6457,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>16</v>
       </c>
@@ -6446,12 +6471,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>16</v>
       </c>
       <c r="B76" s="70" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C76" s="49" t="s">
         <v>25</v>
@@ -6460,7 +6485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:22" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12">
         <v>16</v>
       </c>
@@ -6489,7 +6514,7 @@
       <c r="U77" s="4"/>
       <c r="V77" s="4"/>
     </row>
-    <row r="78" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>17</v>
       </c>
@@ -6520,7 +6545,7 @@
       <c r="U78" s="4"/>
       <c r="V78" s="4"/>
     </row>
-    <row r="79" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>17</v>
       </c>
@@ -6549,7 +6574,7 @@
       <c r="U79" s="4"/>
       <c r="V79" s="4"/>
     </row>
-    <row r="80" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>17</v>
       </c>
@@ -6580,7 +6605,7 @@
       <c r="U80" s="4"/>
       <c r="V80" s="4"/>
     </row>
-    <row r="81" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="8"/>
@@ -6600,7 +6625,7 @@
       <c r="U81" s="4"/>
       <c r="V81" s="4"/>
     </row>
-    <row r="82" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="8"/>
@@ -6622,7 +6647,7 @@
       <c r="U82" s="4"/>
       <c r="V82" s="4"/>
     </row>
-    <row r="83" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="8"/>
@@ -6644,7 +6669,7 @@
       <c r="U83" s="4"/>
       <c r="V83" s="4"/>
     </row>
-    <row r="84" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="8"/>
@@ -6666,7 +6691,7 @@
       <c r="U84" s="4"/>
       <c r="V84" s="4"/>
     </row>
-    <row r="85" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="8"/>
@@ -6688,7 +6713,7 @@
       <c r="U85" s="4"/>
       <c r="V85" s="4"/>
     </row>
-    <row r="86" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="8"/>
@@ -6710,7 +6735,7 @@
       <c r="U86" s="4"/>
       <c r="V86" s="4"/>
     </row>
-    <row r="87" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="8"/>
@@ -6732,7 +6757,7 @@
       <c r="U87" s="4"/>
       <c r="V87" s="4"/>
     </row>
-    <row r="88" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="8"/>
@@ -6754,7 +6779,7 @@
       <c r="U88" s="4"/>
       <c r="V88" s="4"/>
     </row>
-    <row r="89" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="8"/>
@@ -6776,7 +6801,7 @@
       <c r="U89" s="4"/>
       <c r="V89" s="4"/>
     </row>
-    <row r="90" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="8"/>
@@ -6796,7 +6821,7 @@
       <c r="U90" s="4"/>
       <c r="V90" s="4"/>
     </row>
-    <row r="91" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="8"/>
@@ -6817,7 +6842,7 @@
       <c r="V91" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D112">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D112">
     <sortCondition ref="A2:A112"/>
   </sortState>
   <conditionalFormatting sqref="N2:N8">

</xml_diff>

<commit_message>
add dead week info
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23728504-F921-437A-9A28-3409E3903100}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAE7ED1-A4C1-4C0C-AAD2-EBEE85B5DD37}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topic_overview" sheetId="9" r:id="rId1"/>
@@ -1807,9 +1807,6 @@
 [TR](https://forms.gle/WJxxAK8SLSZroU627) (Due 4/17)</t>
   </si>
   <si>
-    <t>5/13  4-6pm. Tehama 116. Both sections</t>
-  </si>
-  <si>
     <t>Take home final exam (Due Wed 5/15); [Metacognition Post-Survey](https://forms.gle/P8q6hbk6eJaScixF6) (Due 5/17); [Post Assessment in R](https://forms.gle/FWAZjanJ31hTrSKK8) (Due 5/17)</t>
   </si>
   <si>
@@ -1820,9 +1817,6 @@
   </si>
   <si>
     <t>[hw09_moderation](hw/hw09_moderation.html) (Due 4/20)</t>
-  </si>
-  <si>
-    <t>e-Poster* (Draft Due 5/9, PR 5/11, Final 5/13)</t>
   </si>
   <si>
     <t>[MWF](https://forms.gle/TRdc8hLWQaqietEh7) (Due 4/21) 
@@ -1836,6 +1830,12 @@
   </si>
   <si>
     <t>Comparing models</t>
+  </si>
+  <si>
+    <t>e-Poster* (Draft Due 5/8 5pm, PR 5/11, Final 5/13 2pm)  TIMES ARE FIRM</t>
+  </si>
+  <si>
+    <t>5/13  4-6pm. Tehama 116. Both sections. I'll bring snacks!</t>
   </si>
 </sst>
 </file>
@@ -2999,7 +2999,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3652,10 +3652,10 @@
         <v>11.3</v>
       </c>
       <c r="C33" t="s">
+        <v>418</v>
+      </c>
+      <c r="G33" t="s">
         <v>419</v>
-      </c>
-      <c r="G33" t="s">
-        <v>420</v>
       </c>
       <c r="H33" s="61"/>
       <c r="I33" s="61"/>
@@ -3680,7 +3680,7 @@
         <v>415</v>
       </c>
       <c r="G34" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H34" s="61"/>
       <c r="I34" s="61" t="s">
@@ -3757,7 +3757,7 @@
         <v>285</v>
       </c>
       <c r="F38" s="56" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H38" s="61"/>
       <c r="I38" s="61"/>
@@ -3767,7 +3767,7 @@
         <v>13.1</v>
       </c>
       <c r="C39" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E39" s="59">
         <v>8.4</v>
@@ -3809,7 +3809,7 @@
         <v>14.3</v>
       </c>
       <c r="C42" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E42" s="55">
         <v>8.4</v>
@@ -3825,13 +3825,13 @@
         <v>253</v>
       </c>
       <c r="C43" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D43" s="64" t="s">
         <v>282</v>
       </c>
       <c r="G43" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="H43" s="61"/>
       <c r="I43" s="61"/>
@@ -3847,7 +3847,7 @@
         <v>299</v>
       </c>
       <c r="G44" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="H44" s="61"/>
       <c r="I44" s="61"/>
@@ -3860,7 +3860,7 @@
         <v>220</v>
       </c>
       <c r="G45" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H45" s="61"/>
       <c r="I45" s="61"/>

</xml_diff>

<commit_message>
add due dates to schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18732B2-1E0B-4B5A-BA40-84BFF1862DD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F36E03-643D-41A0-A276-DDE21E9CB1C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="354">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1046,12 +1046,6 @@
     <t>Time &amp; Location TBD</t>
   </si>
   <si>
-    <t>Take home final exam (Due Wed x/xx); [Metacognition Post-Survey](https://forms.gle/P8q6hbk6eJaScixF6) (Due x/xx); [Post Assessment in R](https://forms.gle/FWAZjanJ31hTrSKK8) (Due x/xx)</t>
-  </si>
-  <si>
-    <t>Poster prep Stage III* (Draft Due x/xx, PR x/x, Final x/x)</t>
-  </si>
-  <si>
     <t>Slack reflection</t>
   </si>
   <si>
@@ -1428,153 +1422,164 @@
     <t>Working with R and R Studio</t>
   </si>
   <si>
-    <t>Quiz 2 Due 9/3) 
+    <t>[hw02_rq_formulation*](hw/hw02_rq_formulation.html) (Due 9/8, PR 9/11)</t>
+  </si>
+  <si>
+    <t>Formulating testable hypothesis</t>
+  </si>
+  <si>
+    <t>[hw03_data_management](hw/hw03_data_management.html) (Due 9/14)</t>
+  </si>
+  <si>
+    <t>Describing data using summary measures</t>
+  </si>
+  <si>
+    <t>Describing numerical variables</t>
+  </si>
+  <si>
+    <t>Describing categorical variables</t>
+  </si>
+  <si>
+    <t>Project Stage I: Setting up the story</t>
+  </si>
+  <si>
+    <t>Calculating grouped summary statistics</t>
+  </si>
+  <si>
+    <t>Project Stage II: Exploratory Data Analysis</t>
+  </si>
+  <si>
+    <t>[Evaluation Form](https://forms.gle/Vrhf9FEqwiWYPD4N9) (Due x/xx)</t>
+  </si>
+  <si>
+    <t>Point estimates and sampling distributions</t>
+  </si>
+  <si>
+    <t>Central limit theorem</t>
+  </si>
+  <si>
+    <t>Project Stage III: Bivariate Inference</t>
+  </si>
+  <si>
+    <t>Assessing model fit</t>
+  </si>
+  <si>
+    <t>Project Stage IV: Multivariable Analysis &amp; Conclusions</t>
+  </si>
+  <si>
+    <t>Develop Research Poster</t>
+  </si>
+  <si>
+    <t>Quiz 3 (Due 9/8) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>[hw02_rq_formulation*](hw/hw02_rq_formulation.html) (Due 9/8, PR 9/11)</t>
-  </si>
-  <si>
-    <t>Formulating testable hypothesis</t>
-  </si>
-  <si>
-    <t>Quiz 3 Due x/x) 
+    <t>Quiz 4 (Due 9/15) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>[hw03_data_management](hw/hw03_data_management.html) (Due 9/14)</t>
-  </si>
-  <si>
-    <t>Describing data using summary measures</t>
-  </si>
-  <si>
-    <t>Describing numerical variables</t>
-  </si>
-  <si>
-    <t>Quiz 4 Due x/x) 
+    <t>Quiz 5 (Due 9/22) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>[hw04_univ_graphing](hw/hw04_univ_graphing.html) (Due x/x)</t>
-  </si>
-  <si>
-    <t>Describing categorical variables</t>
-  </si>
-  <si>
-    <t>Project Stage I: Setting up the story</t>
-  </si>
-  <si>
-    <t>[Poster prep Stage I](project.html)* (Draft Due x/xx, PR x/xx, Final x/xx)</t>
-  </si>
-  <si>
-    <t>Quiz 5 Due x/x) 
+    <t>Quiz 6 (Due 9/29) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>[hw05_biv_graphing](hw/hw05_biv_graphing.html) (Due x/x)</t>
-  </si>
-  <si>
-    <t>Calculating grouped summary statistics</t>
-  </si>
-  <si>
-    <t>[hw06 research proposal outline](hw/hw06_research_proposal_outline.html)</t>
-  </si>
-  <si>
-    <t>Project Stage II: Exploratory Data Analysis</t>
-  </si>
-  <si>
-    <t>Poster prep Stage II* (Draft Due x/xx, PR x/xx, Final x/xx)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x/xx  [Sample exam](reading/sample_exam_1.pdf) available. </t>
-  </si>
-  <si>
-    <t>[Evaluation Form](https://forms.gle/Vrhf9FEqwiWYPD4N9) (Due x/xx)</t>
-  </si>
-  <si>
-    <t>Point estimates and sampling distributions</t>
-  </si>
-  <si>
-    <t>Quiz 7 Due x/x) 
+    <t>Quiz 2 (Due 9/3) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>Central limit theorem</t>
-  </si>
-  <si>
-    <t>Quiz 8 Due x/x) 
+    <t>[hw04_univ_graphing](hw/hw04_univ_graphing.html) (Due 9/28)</t>
+  </si>
+  <si>
+    <t>[hw05_biv_graphing](hw/hw05_biv_graphing.html) (Due 9/28)</t>
+  </si>
+  <si>
+    <t>[hw06 research proposal outline](hw/hw06_research_proposal_outline.html)(Due 10/12)</t>
+  </si>
+  <si>
+    <t>[Poster prep Stage I](project.html)* (Draft Due 9/17, PR 9/19, Final 9/21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Due 10/4)  [Sample exam](reading/sample_exam_1.pdf) available. </t>
+  </si>
+  <si>
+    <t>Poster prep Stage II* (Draft Due 10/01, PR 10/03, Final 10/05)</t>
+  </si>
+  <si>
+    <t>Quiz 7 (Due 10/06) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>[hw07_foundations](hw/hw07_foundations.html) (Due x/xx)</t>
-  </si>
-  <si>
-    <t>Quiz 9 Due x/x) 
+    <t>Quiz 8 (Due 10/13) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>[hw08_biv_inference](hw/hw08_biv_inference.html) (Due x/xx)</t>
-  </si>
-  <si>
-    <t>Quiz 10 Due x/x) 
+    <t>[hw07_foundations](hw/hw07_foundations.html) (Due 10/19)</t>
+  </si>
+  <si>
+    <t>Quiz 9 (Due 10/20) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>Quiz 11 Due x/x) 
+    <t>[hw08_biv_inference](hw/hw08_biv_inference.html) (Due 11/02)</t>
+  </si>
+  <si>
+    <t>Quiz 10 (Due 10/27) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>[hw09_moderation](hw/hw09_moderation.html) (Due x/xx)</t>
-  </si>
-  <si>
-    <t>Quiz 12 Due x/x) 
+    <t>Quiz 11 (Due 11/03) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>hw10_regression (Due x/x)</t>
-  </si>
-  <si>
-    <t>Project Stage III: Bivariate Inference</t>
-  </si>
-  <si>
-    <t>Quiz 13 Due x/x) 
+    <t>[hw09_moderation](hw/hw09_moderation.html) (Due 11/09)</t>
+  </si>
+  <si>
+    <t>Quiz 12 (Due 11/10) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>Assessing model fit</t>
-  </si>
-  <si>
-    <t>Quiz 14 Due x/x) 
+    <t>hw10_regression (Due 11/23)</t>
+  </si>
+  <si>
+    <t>Poster prep Stage III* (Draft Due 11/12, PR 11/14, Final 11/16)</t>
+  </si>
+  <si>
+    <t>Quiz 13 (Due 11/17) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>Project Stage IV: Multivariable Analysis &amp; Conclusions</t>
-  </si>
-  <si>
-    <t>Poster prep Stage IV* (Draft Due x/xx, PR x/x, Final x/x)</t>
-  </si>
-  <si>
-    <t>Develop Research Poster</t>
-  </si>
-  <si>
-    <t>Quiz 15 Due x/x) 
+    <t>Quiz 14 (Due 11/14) 
 [Sec 01]()
 [Sec 02]()</t>
   </si>
   <si>
-    <t>e-Poster* (Draft Due x/x xpm, PR x/xx, Final x/xx xpm)  TIMES ARE FIRM</t>
+    <t>Poster prep Stage IV* (Draft Due 12/03, PR 12/05, Final 12/07)</t>
+  </si>
+  <si>
+    <t>Quiz 15 (Due 12/08) 
+[Sec 01]()
+[Sec 02]()</t>
+  </si>
+  <si>
+    <t>Take home final exam (Due x/xx); [Metacognition Post-Survey](https://forms.gle/P8q6hbk6eJaScixF6) (Due 12/20); [Post Assessment in R](https://forms.gle/FWAZjanJ31hTrSKK8) (Due 12/20)</t>
+  </si>
+  <si>
+    <t>e-Poster* (Draft Due 12/xx , PR 12/xx, Final 12/xx xpm)  TIMES ARE FIRM - Dates dependent on time of common final</t>
   </si>
 </sst>
 </file>
@@ -2161,9 +2166,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2194,9 +2196,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="82" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="82" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="80" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="82"/>
@@ -2276,9 +2275,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2286,9 +2282,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2296,8 +2289,20 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2722,8 +2727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2731,14 +2736,14 @@
     <col min="1" max="2" width="8.875" style="38"/>
     <col min="3" max="3" width="0" style="38" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.375" style="46" customWidth="1"/>
+    <col min="5" max="5" width="56.375" style="45" customWidth="1"/>
     <col min="6" max="6" width="13.875" style="38" customWidth="1"/>
-    <col min="7" max="7" width="16.875" style="39" customWidth="1"/>
+    <col min="7" max="7" width="16.875" style="97" customWidth="1"/>
     <col min="8" max="8" width="79.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="38" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>166</v>
       </c>
       <c r="B1" s="37" t="s">
@@ -2750,81 +2755,81 @@
       <c r="D1" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="51" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="44">
+    <row r="2" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="43">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="38">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F2" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="97" t="s">
+        <v>306</v>
+      </c>
+      <c r="H2" s="85" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="43">
+        <v>1.2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="43">
+        <v>1.3</v>
+      </c>
+      <c r="D4" t="s">
         <v>308</v>
       </c>
-      <c r="H2" s="87" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="44">
-        <v>1.2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="44">
-        <v>1.3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>310</v>
-      </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="45" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="44">
+      <c r="A5" s="43">
         <v>1.4</v>
       </c>
       <c r="D5" t="s">
         <v>205</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="F5" s="42"/>
+      <c r="F5" s="41"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="44">
+      <c r="A6" s="43">
         <v>1.5</v>
       </c>
       <c r="D6" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="47"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="44">
+      <c r="E6" s="46"/>
+    </row>
+    <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="43">
         <v>2.1</v>
       </c>
       <c r="B7" s="38">
@@ -2833,139 +2838,139 @@
       <c r="D7" t="s">
         <v>207</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="G7" s="39" t="s">
-        <v>312</v>
+      <c r="G7" s="97" t="s">
+        <v>330</v>
+      </c>
+      <c r="H7" s="85" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="44">
+      <c r="A8" s="43">
         <v>2.2000000000000002</v>
       </c>
       <c r="D8" t="s">
         <v>208</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="H8" s="87" t="s">
-        <v>313</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="44">
+      <c r="A9" s="43">
         <v>2.2999999999999998</v>
       </c>
       <c r="D9" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="44">
+      <c r="A10" s="43">
         <v>2.4</v>
       </c>
       <c r="D10" t="s">
         <v>150</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="45" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45">
+    <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="44">
         <v>3.1</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B11" s="39">
         <v>3</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="39" t="s">
-        <v>315</v>
-      </c>
-      <c r="H11" s="87" t="s">
-        <v>316</v>
+      <c r="F11" s="39"/>
+      <c r="G11" s="97" t="s">
+        <v>326</v>
+      </c>
+      <c r="H11" s="85" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="44">
+      <c r="A12" s="43">
         <v>3.2</v>
       </c>
       <c r="D12" t="s">
         <v>153</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="H12" s="88" t="s">
+      <c r="H12" s="86" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="44">
+      <c r="A13" s="43">
         <v>3.3</v>
       </c>
       <c r="D13" t="s">
-        <v>317</v>
-      </c>
-      <c r="H13" s="88"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="44">
+        <v>313</v>
+      </c>
+      <c r="H13" s="86"/>
+    </row>
+    <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="43">
         <v>4.0999999999999996</v>
       </c>
       <c r="B14" s="38">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>318</v>
-      </c>
-      <c r="E14" s="46" t="s">
+        <v>314</v>
+      </c>
+      <c r="E14" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="G14" s="39" t="s">
-        <v>319</v>
+      <c r="G14" s="97" t="s">
+        <v>327</v>
       </c>
       <c r="H14" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="44">
+      <c r="A15" s="43">
         <v>4.2</v>
       </c>
       <c r="D15" t="s">
-        <v>321</v>
-      </c>
-      <c r="E15" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="E15" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="F15" s="42"/>
+      <c r="F15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="44">
+      <c r="A16" s="43">
         <v>4.3</v>
       </c>
-      <c r="D16" s="89" t="s">
-        <v>322</v>
-      </c>
-      <c r="E16" s="90"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="89" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="44">
+      <c r="D16" s="87" t="s">
+        <v>316</v>
+      </c>
+      <c r="E16" s="88"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="87" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="43">
         <v>5.0999999999999996</v>
       </c>
       <c r="B17" s="38">
@@ -2974,28 +2979,28 @@
       <c r="D17" t="s">
         <v>210</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="39" t="s">
-        <v>324</v>
+      <c r="F17" s="41"/>
+      <c r="G17" s="97" t="s">
+        <v>328</v>
       </c>
       <c r="H17" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
+      <c r="A18" s="43">
         <v>5.2</v>
       </c>
       <c r="D18" t="s">
-        <v>326</v>
-      </c>
-      <c r="F18" s="42"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="44">
+        <v>317</v>
+      </c>
+      <c r="F18" s="41"/>
+    </row>
+    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="43">
         <v>6.1</v>
       </c>
       <c r="B19" s="38">
@@ -3004,98 +3009,101 @@
       <c r="D19" t="s">
         <v>151</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="H19" s="54" t="s">
-        <v>327</v>
+      <c r="G19" s="97" t="s">
+        <v>329</v>
+      </c>
+      <c r="H19" s="52" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="44">
+      <c r="A20" s="43">
         <v>6.2</v>
       </c>
       <c r="D20" t="s">
         <v>168</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="45" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="44">
+      <c r="A21" s="43">
         <v>6.3</v>
       </c>
-      <c r="D21" s="93" t="s">
+      <c r="D21" s="90" t="s">
         <v>160</v>
       </c>
-      <c r="E21" s="94"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="96"/>
-      <c r="H21" s="93" t="s">
-        <v>330</v>
+      <c r="E21" s="91"/>
+      <c r="F21" s="92"/>
+      <c r="G21" s="99"/>
+      <c r="H21" s="90" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="44">
+      <c r="A22" s="43">
         <v>6.4</v>
       </c>
       <c r="D22" t="s">
         <v>213</v>
       </c>
       <c r="H22" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="44">
+      <c r="A23" s="43">
         <v>6.5</v>
       </c>
-      <c r="D23" s="89" t="s">
-        <v>328</v>
-      </c>
-      <c r="E23" s="90"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="92"/>
-      <c r="H23" s="89" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="44">
+      <c r="D23" s="87" t="s">
+        <v>318</v>
+      </c>
+      <c r="E23" s="88"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="98"/>
+      <c r="H23" s="87" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="43">
         <v>7.1</v>
       </c>
       <c r="B24" s="38">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>332</v>
-      </c>
-      <c r="E24" s="46" t="s">
+        <v>320</v>
+      </c>
+      <c r="E24" s="45" t="s">
         <v>186</v>
       </c>
-      <c r="G24" s="39" t="s">
-        <v>333</v>
+      <c r="G24" s="97" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="44">
+      <c r="A25" s="43">
         <v>7.2</v>
       </c>
       <c r="D25" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="44">
+      <c r="A26" s="43">
         <v>7.3</v>
       </c>
       <c r="D26" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="44">
+    <row r="27" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="43">
         <v>8.1</v>
       </c>
       <c r="B27" s="38">
@@ -3104,34 +3112,34 @@
       <c r="D27" t="s">
         <v>212</v>
       </c>
-      <c r="G27" s="39" t="s">
-        <v>335</v>
+      <c r="G27" s="97" t="s">
+        <v>338</v>
       </c>
       <c r="H27" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="44">
+      <c r="A28" s="43">
         <v>8.1999999999999993</v>
       </c>
       <c r="D28" t="s">
         <v>154</v>
       </c>
-      <c r="E28" s="46" t="s">
+      <c r="E28" s="45" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="44">
+      <c r="A29" s="43">
         <v>8.3000000000000007</v>
       </c>
       <c r="D29" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="44">
+    <row r="30" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="43">
         <v>9.1</v>
       </c>
       <c r="B30" s="38">
@@ -3140,40 +3148,40 @@
       <c r="D30" t="s">
         <v>155</v>
       </c>
-      <c r="E30" s="46" t="s">
+      <c r="E30" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="G30" s="39" t="s">
-        <v>337</v>
+      <c r="G30" s="97" t="s">
+        <v>340</v>
       </c>
       <c r="H30" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="44">
+      <c r="A31" s="43">
         <v>9.1999999999999993</v>
       </c>
       <c r="D31" t="s">
         <v>156</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="45" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="44">
+      <c r="A32" s="43">
         <v>9.3000000000000007</v>
       </c>
       <c r="D32" t="s">
         <v>157</v>
       </c>
-      <c r="E32" s="46" t="s">
+      <c r="E32" s="45" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="44">
+    <row r="33" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A33" s="43">
         <v>10.1</v>
       </c>
       <c r="B33" s="38">
@@ -3182,15 +3190,15 @@
       <c r="D33" t="s">
         <v>169</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="G33" s="39" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="44">
+      <c r="G33" s="97" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A34" s="43">
         <v>11.1</v>
       </c>
       <c r="B34" s="38">
@@ -3199,40 +3207,40 @@
       <c r="D34" t="s">
         <v>158</v>
       </c>
-      <c r="E34" s="46" t="s">
+      <c r="E34" s="45" t="s">
         <v>181</v>
       </c>
-      <c r="G34" s="39" t="s">
-        <v>340</v>
+      <c r="G34" s="97" t="s">
+        <v>343</v>
       </c>
       <c r="H34" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="44">
+      <c r="A35" s="43">
         <v>11.2</v>
       </c>
       <c r="D35" t="s">
         <v>159</v>
       </c>
-      <c r="E35" s="46" t="s">
+      <c r="E35" s="45" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="44">
+      <c r="A36" s="43">
         <v>11.3</v>
       </c>
       <c r="D36" t="s">
         <v>189</v>
       </c>
-      <c r="E36" s="46" t="s">
+      <c r="E36" s="45" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="44">
+    <row r="37" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A37" s="43">
         <v>12.1</v>
       </c>
       <c r="B37" s="38">
@@ -3241,33 +3249,33 @@
       <c r="D37" t="s">
         <v>188</v>
       </c>
-      <c r="E37" s="46" t="s">
+      <c r="E37" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="F37" s="42"/>
-      <c r="G37" s="39" t="s">
-        <v>342</v>
+      <c r="F37" s="41"/>
+      <c r="G37" s="97" t="s">
+        <v>345</v>
       </c>
       <c r="H37" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="44">
+      <c r="A38" s="43">
         <v>12.2</v>
       </c>
-      <c r="D38" s="89" t="s">
-        <v>344</v>
-      </c>
-      <c r="E38" s="90"/>
-      <c r="F38" s="91"/>
-      <c r="G38" s="92"/>
-      <c r="H38" s="89" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="44">
+      <c r="D38" s="87" t="s">
+        <v>322</v>
+      </c>
+      <c r="E38" s="88"/>
+      <c r="F38" s="89"/>
+      <c r="G38" s="98"/>
+      <c r="H38" s="87" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A39" s="43">
         <v>13.1</v>
       </c>
       <c r="B39" s="38">
@@ -3276,86 +3284,89 @@
       <c r="D39" t="s">
         <v>163</v>
       </c>
-      <c r="E39" s="46" t="s">
+      <c r="E39" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="F39" s="42"/>
-      <c r="G39" s="39" t="s">
-        <v>345</v>
+      <c r="F39" s="41"/>
+      <c r="G39" s="97" t="s">
+        <v>348</v>
+      </c>
+      <c r="H39" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="44">
+      <c r="A40" s="43">
         <v>13.2</v>
       </c>
       <c r="D40" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="42"/>
+      <c r="F40" s="41"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="44">
+      <c r="A41" s="43">
         <v>14</v>
       </c>
-      <c r="D41" s="97" t="s">
+      <c r="D41" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="98"/>
-      <c r="F41" s="99"/>
+      <c r="E41" s="94"/>
+      <c r="F41" s="95"/>
       <c r="G41" s="100"/>
-      <c r="H41" s="97"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="44">
+      <c r="H41" s="93"/>
+    </row>
+    <row r="42" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A42" s="43">
         <v>15.1</v>
       </c>
       <c r="B42" s="38">
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>346</v>
-      </c>
-      <c r="F42" s="42"/>
-      <c r="G42" s="39" t="s">
-        <v>347</v>
+        <v>323</v>
+      </c>
+      <c r="F42" s="41"/>
+      <c r="G42" s="97" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="44">
+      <c r="A43" s="43">
         <v>15.2</v>
       </c>
-      <c r="D43" s="89" t="s">
-        <v>348</v>
-      </c>
-      <c r="E43" s="90"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="92"/>
-      <c r="H43" s="89" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="44">
+      <c r="D43" s="87" t="s">
+        <v>324</v>
+      </c>
+      <c r="E43" s="88"/>
+      <c r="F43" s="89"/>
+      <c r="G43" s="98"/>
+      <c r="H43" s="87" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A44" s="43">
         <v>16.100000000000001</v>
       </c>
       <c r="B44" s="38">
         <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>350</v>
-      </c>
-      <c r="E44" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="E44" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="G44" s="39" t="s">
+      <c r="G44" s="97" t="s">
         <v>351</v>
       </c>
       <c r="H44" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="44">
+      <c r="A45" s="43">
         <v>17.100000000000001</v>
       </c>
       <c r="B45" s="38">
@@ -3369,14 +3380,14 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="44">
+      <c r="A46" s="43">
         <v>17.2</v>
       </c>
       <c r="D46" t="s">
         <v>161</v>
       </c>
       <c r="H46" t="s">
-        <v>217</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3435,7 +3446,7 @@
       <c r="H1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="86" t="s">
+      <c r="I1" s="84" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3450,22 +3461,22 @@
         <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3477,25 +3488,25 @@
         <v>42248</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H3" s="30" t="s">
         <v>40</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J3" s="30"/>
     </row>
@@ -3508,25 +3519,25 @@
         <v>42255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -3538,25 +3549,25 @@
         <v>42262</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3568,23 +3579,23 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3596,16 +3607,16 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>160</v>
@@ -3626,13 +3637,13 @@
         <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>61</v>
@@ -3691,7 +3702,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>10</v>
       </c>
@@ -3700,7 +3711,7 @@
         <v>42304</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>78</v>
@@ -3727,7 +3738,7 @@
         <v>42311</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>80</v>
@@ -3752,18 +3763,18 @@
         <v>42318</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>37</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3775,13 +3786,13 @@
         <v>42325</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>94</v>
@@ -3815,7 +3826,7 @@
         <v>42339</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>83</v>
@@ -3840,7 +3851,7 @@
         <v>42346</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>84</v>
@@ -4353,7 +4364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -4468,9 +4479,9 @@
       <c r="D2" s="8">
         <v>3</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="33" t="s">
         <v>104</v>
       </c>
@@ -4482,7 +4493,7 @@
         <f t="shared" ref="J2:J7" si="0">I2/$M$8</f>
         <v>0.27554535017221582</v>
       </c>
-      <c r="K2" s="56"/>
+      <c r="K2" s="54"/>
       <c r="L2" s="33" t="s">
         <v>104</v>
       </c>
@@ -4531,22 +4542,22 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="65">
+      <c r="A3" s="63">
         <v>1.2</v>
       </c>
-      <c r="B3" s="72" t="s">
-        <v>230</v>
-      </c>
-      <c r="C3" s="79" t="s">
+      <c r="B3" s="70" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="68">
+      <c r="D3" s="66">
         <v>10</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="52" t="s">
+      <c r="E3" s="53"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="50" t="s">
         <v>24</v>
       </c>
       <c r="I3" s="5">
@@ -4557,8 +4568,8 @@
         <f t="shared" si="0"/>
         <v>0.27554535017221582</v>
       </c>
-      <c r="K3" s="55"/>
-      <c r="L3" s="52" t="s">
+      <c r="K3" s="53"/>
+      <c r="L3" s="50" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="5">
@@ -4606,21 +4617,21 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="65">
+      <c r="A4" s="63">
         <v>1.2</v>
       </c>
-      <c r="B4" s="72" t="s">
-        <v>231</v>
-      </c>
-      <c r="C4" s="71" t="s">
+      <c r="B4" s="70" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="D4" s="69">
+      <c r="D4" s="67">
         <v>2</v>
       </c>
-      <c r="E4" s="55"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="56"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="4" t="s">
         <v>25</v>
       </c>
@@ -4632,7 +4643,7 @@
         <f t="shared" si="0"/>
         <v>4.5924225028702644E-2</v>
       </c>
-      <c r="K4" s="55"/>
+      <c r="K4" s="53"/>
       <c r="L4" s="4" t="s">
         <v>25</v>
       </c>
@@ -4681,21 +4692,21 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="65">
+      <c r="A5" s="63">
         <v>1.4</v>
       </c>
-      <c r="B5" s="72" t="s">
-        <v>268</v>
-      </c>
-      <c r="C5" s="73" t="s">
+      <c r="B5" s="70" t="s">
+        <v>266</v>
+      </c>
+      <c r="C5" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="68">
+      <c r="D5" s="66">
         <v>15</v>
       </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="55"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="4" t="s">
         <v>13</v>
       </c>
@@ -4707,7 +4718,7 @@
         <f t="shared" si="0"/>
         <v>9.1848450057405287E-2</v>
       </c>
-      <c r="K5" s="56"/>
+      <c r="K5" s="54"/>
       <c r="L5" s="4" t="s">
         <v>13</v>
       </c>
@@ -4749,21 +4760,21 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="65">
+      <c r="A6" s="63">
         <v>2.1</v>
       </c>
-      <c r="B6" s="72" t="s">
-        <v>232</v>
-      </c>
-      <c r="C6" s="79" t="s">
+      <c r="B6" s="70" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="68">
+      <c r="D6" s="66">
         <v>10</v>
       </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="55"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="53"/>
       <c r="H6" s="4" t="s">
         <v>14</v>
       </c>
@@ -4775,7 +4786,7 @@
         <f t="shared" si="0"/>
         <v>0.22962112514351321</v>
       </c>
-      <c r="K6" s="55"/>
+      <c r="K6" s="53"/>
       <c r="L6" s="4" t="s">
         <v>14</v>
       </c>
@@ -4824,21 +4835,21 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="65">
+      <c r="A7" s="63">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B7" s="72" t="s">
-        <v>233</v>
-      </c>
-      <c r="C7" s="71" t="s">
+      <c r="B7" s="70" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="D7" s="69">
+      <c r="D7" s="67">
         <v>2</v>
       </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="4" t="s">
         <v>15</v>
       </c>
@@ -4850,7 +4861,7 @@
         <f t="shared" si="0"/>
         <v>0.22962112514351321</v>
       </c>
-      <c r="K7" s="55"/>
+      <c r="K7" s="53"/>
       <c r="L7" s="4" t="s">
         <v>15</v>
       </c>
@@ -4899,28 +4910,28 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="65">
+      <c r="A8" s="63">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B8" s="72" t="s">
-        <v>260</v>
-      </c>
-      <c r="C8" s="75" t="s">
+      <c r="B8" s="70" t="s">
+        <v>258</v>
+      </c>
+      <c r="C8" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D8" s="74">
         <v>10</v>
       </c>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
       <c r="H8" s="4"/>
       <c r="I8" s="3">
         <f>SUM(I2:I7)</f>
         <v>500</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="56"/>
+      <c r="K8" s="54"/>
       <c r="M8" s="3">
         <f>SUM(M2:M7)</f>
         <v>435.5</v>
@@ -4960,25 +4971,25 @@
       </c>
     </row>
     <row r="9" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="65">
+      <c r="A9" s="63">
         <v>2.4</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="75" t="s">
         <v>204</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="68">
+      <c r="D9" s="66">
         <v>4</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="Q9" s="3">
@@ -4996,1329 +5007,1329 @@
       <c r="AD9" s="5"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65">
+      <c r="A10" s="63">
         <v>3.1</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="70" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="66">
+        <v>10</v>
+      </c>
+      <c r="E10" s="53"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="63">
+        <v>3.2</v>
+      </c>
+      <c r="B11" s="70" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" s="67">
+        <v>2</v>
+      </c>
+      <c r="E11" s="53"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="63">
+        <v>3.6</v>
+      </c>
+      <c r="B12" s="70" t="s">
+        <v>259</v>
+      </c>
+      <c r="C12" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="66">
+        <v>15</v>
+      </c>
+      <c r="E12" s="53"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="63">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B13" s="70" t="s">
         <v>234</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C13" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="68">
+      <c r="D13" s="66">
         <v>10</v>
       </c>
-      <c r="E10" s="55"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="65">
-        <v>3.2</v>
-      </c>
-      <c r="B11" s="72" t="s">
+      <c r="E13" s="53"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="63">
+        <v>4.2</v>
+      </c>
+      <c r="B14" s="70" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="71" t="s">
+      <c r="C14" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="D11" s="69">
+      <c r="D14" s="67">
         <v>2</v>
       </c>
-      <c r="E11" s="55"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="65">
-        <v>3.6</v>
-      </c>
-      <c r="B12" s="72" t="s">
-        <v>261</v>
-      </c>
-      <c r="C12" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="68">
-        <v>15</v>
-      </c>
-      <c r="E12" s="55"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="65">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B13" s="72" t="s">
-        <v>236</v>
-      </c>
-      <c r="C13" s="70" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" s="68">
-        <v>10</v>
-      </c>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="65">
-        <v>4.2</v>
-      </c>
-      <c r="B14" s="72" t="s">
-        <v>237</v>
-      </c>
-      <c r="C14" s="71" t="s">
-        <v>206</v>
-      </c>
-      <c r="D14" s="69">
-        <v>2</v>
-      </c>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="65">
+      <c r="A15" s="63">
         <v>4.5</v>
       </c>
-      <c r="B15" s="72" t="s">
-        <v>262</v>
-      </c>
-      <c r="C15" s="80" t="s">
+      <c r="B15" s="70" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="68">
+      <c r="D15" s="66">
         <v>15</v>
       </c>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="65">
+      <c r="A16" s="63">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B16" s="72" t="s">
-        <v>238</v>
-      </c>
-      <c r="C16" s="70" t="s">
+      <c r="B16" s="70" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="68">
+      <c r="D16" s="66">
         <v>10</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="65">
+      <c r="A17" s="63">
         <v>5.2</v>
       </c>
-      <c r="B17" s="72" t="s">
-        <v>239</v>
-      </c>
-      <c r="C17" s="71" t="s">
+      <c r="B17" s="70" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="D17" s="69">
+      <c r="D17" s="67">
         <v>2</v>
       </c>
-      <c r="E17" s="55"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="65">
+      <c r="A18" s="63">
         <v>5.3</v>
       </c>
-      <c r="B18" s="72" t="s">
-        <v>263</v>
-      </c>
-      <c r="C18" s="80" t="s">
+      <c r="B18" s="70" t="s">
+        <v>261</v>
+      </c>
+      <c r="C18" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="68">
+      <c r="D18" s="66">
         <v>15</v>
       </c>
-      <c r="E18" s="55"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="65">
+      <c r="A19" s="63">
         <v>6.1</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="68">
+      <c r="D19" s="66">
         <v>50</v>
       </c>
-      <c r="E19" s="55"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="55"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="65">
+      <c r="A20" s="63">
         <v>6.1</v>
       </c>
-      <c r="B20" s="72" t="s">
-        <v>240</v>
-      </c>
-      <c r="C20" s="79" t="s">
+      <c r="B20" s="70" t="s">
+        <v>238</v>
+      </c>
+      <c r="C20" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="68">
+      <c r="D20" s="66">
         <v>10</v>
       </c>
-      <c r="E20" s="55"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="65">
+      <c r="A21" s="63">
         <v>6.2</v>
       </c>
-      <c r="B21" s="72" t="s">
-        <v>241</v>
-      </c>
-      <c r="C21" s="71" t="s">
+      <c r="B21" s="70" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="D21" s="69">
+      <c r="D21" s="67">
         <v>2</v>
       </c>
-      <c r="E21" s="55"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="65">
+      <c r="A22" s="63">
         <v>7.1</v>
       </c>
-      <c r="B22" s="72" t="s">
-        <v>242</v>
-      </c>
-      <c r="C22" s="79" t="s">
+      <c r="B22" s="70" t="s">
+        <v>240</v>
+      </c>
+      <c r="C22" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="68">
+      <c r="D22" s="66">
         <v>10</v>
       </c>
-      <c r="E22" s="55"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="55"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="65">
+      <c r="A23" s="63">
         <v>7.2</v>
       </c>
-      <c r="B23" s="72" t="s">
-        <v>243</v>
-      </c>
-      <c r="C23" s="71" t="s">
+      <c r="B23" s="70" t="s">
+        <v>241</v>
+      </c>
+      <c r="C23" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="D23" s="69">
+      <c r="D23" s="67">
         <v>2</v>
       </c>
-      <c r="E23" s="55"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="65">
+      <c r="A24" s="63">
         <v>7.3</v>
       </c>
-      <c r="B24" s="72" t="s">
-        <v>264</v>
-      </c>
-      <c r="C24" s="82" t="s">
+      <c r="B24" s="70" t="s">
+        <v>262</v>
+      </c>
+      <c r="C24" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="68">
+      <c r="D24" s="66">
         <v>10</v>
       </c>
-      <c r="E24" s="55"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="65">
+      <c r="A25" s="63">
         <v>8.1</v>
       </c>
-      <c r="B25" s="72" t="s">
-        <v>265</v>
-      </c>
-      <c r="C25" s="83" t="s">
+      <c r="B25" s="70" t="s">
+        <v>263</v>
+      </c>
+      <c r="C25" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="68">
+      <c r="D25" s="66">
         <v>15</v>
       </c>
-      <c r="E25" s="55"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="65">
+      <c r="A26" s="63">
         <v>8.1</v>
       </c>
-      <c r="B26" s="72" t="s">
-        <v>244</v>
-      </c>
-      <c r="C26" s="79" t="s">
+      <c r="B26" s="70" t="s">
+        <v>242</v>
+      </c>
+      <c r="C26" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="68">
+      <c r="D26" s="66">
         <v>10</v>
       </c>
-      <c r="E26" s="55"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="65">
+      <c r="A27" s="63">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B27" s="72" t="s">
-        <v>245</v>
-      </c>
-      <c r="C27" s="71" t="s">
+      <c r="B27" s="70" t="s">
+        <v>243</v>
+      </c>
+      <c r="C27" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="D27" s="69">
+      <c r="D27" s="67">
         <v>2</v>
       </c>
-      <c r="E27" s="55"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="55"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="65">
+      <c r="A28" s="63">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B28" s="72" t="s">
-        <v>225</v>
-      </c>
-      <c r="C28" s="78" t="s">
+      <c r="B28" s="70" t="s">
+        <v>223</v>
+      </c>
+      <c r="C28" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="68">
+      <c r="D28" s="66">
         <v>4</v>
       </c>
-      <c r="E28" s="55"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="65">
+      <c r="A29" s="63">
         <v>8.4</v>
       </c>
-      <c r="B29" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="C29" s="67" t="s">
+      <c r="B29" s="70" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="68">
+      <c r="D29" s="66">
         <v>15</v>
       </c>
-      <c r="E29" s="55"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="65">
+      <c r="A30" s="63">
         <v>9.1</v>
       </c>
-      <c r="B30" s="72" t="s">
-        <v>246</v>
-      </c>
-      <c r="C30" s="79" t="s">
+      <c r="B30" s="70" t="s">
+        <v>244</v>
+      </c>
+      <c r="C30" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="68">
+      <c r="D30" s="66">
         <v>10</v>
       </c>
-      <c r="E30" s="55"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="65">
+      <c r="A31" s="63">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B31" s="72" t="s">
+      <c r="B31" s="70" t="s">
+        <v>245</v>
+      </c>
+      <c r="C31" s="69" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" s="67">
+        <v>2</v>
+      </c>
+      <c r="E31" s="53"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="63">
+        <v>9.5</v>
+      </c>
+      <c r="B32" s="72" t="s">
+        <v>197</v>
+      </c>
+      <c r="C32" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="66">
+        <v>5</v>
+      </c>
+      <c r="E32" s="53"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="63">
+        <v>10.1</v>
+      </c>
+      <c r="B33" s="70" t="s">
+        <v>246</v>
+      </c>
+      <c r="C33" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="66">
+        <v>10</v>
+      </c>
+      <c r="E33" s="53"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="63">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B34" s="70" t="s">
         <v>247</v>
       </c>
-      <c r="C31" s="71" t="s">
+      <c r="C34" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="D31" s="69">
+      <c r="D34" s="67">
         <v>2</v>
       </c>
-      <c r="E31" s="55"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="65">
-        <v>9.5</v>
-      </c>
-      <c r="B32" s="74" t="s">
-        <v>197</v>
-      </c>
-      <c r="C32" s="84" t="s">
+      <c r="E34" s="53"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="63">
+        <v>11.1</v>
+      </c>
+      <c r="B35" s="70" t="s">
+        <v>248</v>
+      </c>
+      <c r="C35" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" s="66">
+        <v>10</v>
+      </c>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="63">
+        <v>11.2</v>
+      </c>
+      <c r="B36" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="C36" s="69" t="s">
+        <v>206</v>
+      </c>
+      <c r="D36" s="67">
+        <v>2</v>
+      </c>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="63">
+        <v>11.3</v>
+      </c>
+      <c r="B37" s="72" t="s">
+        <v>196</v>
+      </c>
+      <c r="C37" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="66">
+        <v>15</v>
+      </c>
+      <c r="E37" s="53"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="63">
+        <v>12.1</v>
+      </c>
+      <c r="B38" s="70" t="s">
+        <v>250</v>
+      </c>
+      <c r="C38" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="66">
+        <v>10</v>
+      </c>
+      <c r="E38" s="53"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="63">
+        <v>12.2</v>
+      </c>
+      <c r="B39" s="70" t="s">
+        <v>251</v>
+      </c>
+      <c r="C39" s="69" t="s">
+        <v>206</v>
+      </c>
+      <c r="D39" s="67">
+        <v>2</v>
+      </c>
+      <c r="E39" s="53"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="63">
+        <v>12.5</v>
+      </c>
+      <c r="B40" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="C40" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="66">
+        <v>4</v>
+      </c>
+      <c r="E40" s="53"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="63">
+        <v>12.6</v>
+      </c>
+      <c r="B41" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="C41" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="66">
+        <v>15</v>
+      </c>
+      <c r="E41" s="53"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="53"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="63">
+        <v>12.7</v>
+      </c>
+      <c r="B42" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="C42" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="66">
+        <v>15</v>
+      </c>
+      <c r="E42" s="53"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="63">
+        <v>13.1</v>
+      </c>
+      <c r="B43" s="70" t="s">
+        <v>252</v>
+      </c>
+      <c r="C43" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="66">
+        <v>10</v>
+      </c>
+      <c r="E43" s="53"/>
+      <c r="F43" s="62"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="53"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="63">
+        <v>13.2</v>
+      </c>
+      <c r="B44" s="70" t="s">
+        <v>253</v>
+      </c>
+      <c r="C44" s="69" t="s">
+        <v>206</v>
+      </c>
+      <c r="D44" s="67">
+        <v>2</v>
+      </c>
+      <c r="E44" s="53"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="63">
+        <v>13.5</v>
+      </c>
+      <c r="B45" s="72" t="s">
+        <v>199</v>
+      </c>
+      <c r="C45" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="66">
+        <v>15</v>
+      </c>
+      <c r="E45" s="53"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="53"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="63">
+        <v>14.1</v>
+      </c>
+      <c r="B46" s="70" t="s">
+        <v>224</v>
+      </c>
+      <c r="C46" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="66">
+        <v>4</v>
+      </c>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
+      <c r="K46" s="53"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="63">
+        <v>14.1</v>
+      </c>
+      <c r="B47" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="C47" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="66">
+        <v>4</v>
+      </c>
+      <c r="E47" s="53"/>
+      <c r="F47" s="62"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="53"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="63">
+        <v>14.1</v>
+      </c>
+      <c r="B48" s="70" t="s">
+        <v>254</v>
+      </c>
+      <c r="C48" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="66">
+        <v>10</v>
+      </c>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="63">
+        <v>14.2</v>
+      </c>
+      <c r="B49" s="70" t="s">
+        <v>225</v>
+      </c>
+      <c r="C49" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="66">
+        <v>15</v>
+      </c>
+      <c r="E49" s="53"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="53"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="63">
+        <v>14.2</v>
+      </c>
+      <c r="B50" s="70" t="s">
+        <v>227</v>
+      </c>
+      <c r="C50" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="66">
+        <v>15</v>
+      </c>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="63">
+        <v>14.2</v>
+      </c>
+      <c r="B51" s="70" t="s">
+        <v>255</v>
+      </c>
+      <c r="C51" s="69" t="s">
+        <v>206</v>
+      </c>
+      <c r="D51" s="67">
+        <v>2</v>
+      </c>
+      <c r="E51" s="53"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="53"/>
+      <c r="J51" s="53"/>
+      <c r="K51" s="53"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="63">
+        <v>15.1</v>
+      </c>
+      <c r="B52" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="66">
+        <v>4</v>
+      </c>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="53"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="53"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="63">
+        <v>15.1</v>
+      </c>
+      <c r="B53" s="70" t="s">
+        <v>256</v>
+      </c>
+      <c r="C53" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="66">
+        <v>10</v>
+      </c>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="53"/>
+      <c r="J53" s="53"/>
+      <c r="K53" s="53"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="63">
+        <v>15.2</v>
+      </c>
+      <c r="B54" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="66">
+        <v>10</v>
+      </c>
+      <c r="E54" s="53"/>
+      <c r="F54" s="62"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="53"/>
+      <c r="K54" s="53"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="63">
+        <v>15.2</v>
+      </c>
+      <c r="B55" s="70" t="s">
+        <v>257</v>
+      </c>
+      <c r="C55" s="69" t="s">
+        <v>206</v>
+      </c>
+      <c r="D55" s="67">
+        <v>2</v>
+      </c>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="53"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="63">
+        <v>16</v>
+      </c>
+      <c r="B56" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="66">
+        <v>5</v>
+      </c>
+      <c r="E56" s="53"/>
+      <c r="F56" s="62"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="53"/>
+      <c r="K56" s="53"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="63">
+        <v>16</v>
+      </c>
+      <c r="B57" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="66">
+        <v>10</v>
+      </c>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="53"/>
+      <c r="H57" s="53"/>
+      <c r="I57" s="53"/>
+      <c r="J57" s="53"/>
+      <c r="K57" s="53"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="63">
+        <v>16</v>
+      </c>
+      <c r="B58" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="79" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="66">
+        <v>50</v>
+      </c>
+      <c r="E58" s="53"/>
+      <c r="F58" s="62"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="53"/>
+      <c r="J58" s="53"/>
+      <c r="K58" s="53"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="63">
+        <v>16</v>
+      </c>
+      <c r="B59" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="68">
-        <v>5</v>
-      </c>
-      <c r="E32" s="55"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="65">
-        <v>10.1</v>
-      </c>
-      <c r="B33" s="72" t="s">
-        <v>248</v>
-      </c>
-      <c r="C33" s="79" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="68">
+      <c r="D59" s="66">
+        <v>2</v>
+      </c>
+      <c r="E59" s="53"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="53"/>
+      <c r="H59" s="53"/>
+      <c r="I59" s="53"/>
+      <c r="J59" s="53"/>
+      <c r="K59" s="53"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="63">
+        <v>16</v>
+      </c>
+      <c r="B60" s="70" t="s">
+        <v>217</v>
+      </c>
+      <c r="C60" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="66">
+        <v>3</v>
+      </c>
+      <c r="E60" s="53"/>
+      <c r="F60" s="62"/>
+      <c r="G60" s="53"/>
+      <c r="H60" s="53"/>
+      <c r="I60" s="53"/>
+      <c r="J60" s="53"/>
+      <c r="K60" s="53"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="63">
+        <v>16</v>
+      </c>
+      <c r="B61" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="66">
+        <v>2</v>
+      </c>
+      <c r="E61" s="53"/>
+      <c r="F61" s="62"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="53"/>
+      <c r="K61" s="53"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="63">
+        <v>16</v>
+      </c>
+      <c r="B62" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" s="66">
         <v>10</v>
       </c>
-      <c r="E33" s="55"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="65">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="B34" s="72" t="s">
-        <v>249</v>
-      </c>
-      <c r="C34" s="71" t="s">
-        <v>206</v>
-      </c>
-      <c r="D34" s="69">
-        <v>2</v>
-      </c>
-      <c r="E34" s="55"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="65">
-        <v>11.1</v>
-      </c>
-      <c r="B35" s="72" t="s">
-        <v>250</v>
-      </c>
-      <c r="C35" s="79" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="68">
-        <v>10</v>
-      </c>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="55"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="65">
-        <v>11.2</v>
-      </c>
-      <c r="B36" s="72" t="s">
-        <v>251</v>
-      </c>
-      <c r="C36" s="71" t="s">
-        <v>206</v>
-      </c>
-      <c r="D36" s="69">
-        <v>2</v>
-      </c>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="65">
-        <v>11.3</v>
-      </c>
-      <c r="B37" s="74" t="s">
-        <v>196</v>
-      </c>
-      <c r="C37" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="68">
-        <v>15</v>
-      </c>
-      <c r="E37" s="55"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="55"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="65">
-        <v>12.1</v>
-      </c>
-      <c r="B38" s="72" t="s">
-        <v>252</v>
-      </c>
-      <c r="C38" s="79" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="68">
-        <v>10</v>
-      </c>
-      <c r="E38" s="55"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="65">
-        <v>12.2</v>
-      </c>
-      <c r="B39" s="72" t="s">
-        <v>253</v>
-      </c>
-      <c r="C39" s="71" t="s">
-        <v>206</v>
-      </c>
-      <c r="D39" s="69">
-        <v>2</v>
-      </c>
-      <c r="E39" s="55"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="65">
-        <v>12.5</v>
-      </c>
-      <c r="B40" s="72" t="s">
-        <v>223</v>
-      </c>
-      <c r="C40" s="78" t="s">
+      <c r="E62" s="53"/>
+      <c r="F62" s="62"/>
+      <c r="G62" s="53"/>
+      <c r="H62" s="53"/>
+      <c r="I62" s="53"/>
+      <c r="J62" s="53"/>
+      <c r="K62" s="53"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="63">
+        <v>16</v>
+      </c>
+      <c r="B63" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="68">
-        <v>4</v>
-      </c>
-      <c r="E40" s="55"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="65">
-        <v>12.6</v>
-      </c>
-      <c r="B41" s="74" t="s">
-        <v>198</v>
-      </c>
-      <c r="C41" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="68">
-        <v>15</v>
-      </c>
-      <c r="E41" s="55"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
-      <c r="K41" s="55"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="65">
-        <v>12.7</v>
-      </c>
-      <c r="B42" s="72" t="s">
-        <v>222</v>
-      </c>
-      <c r="C42" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="68">
-        <v>15</v>
-      </c>
-      <c r="E42" s="55"/>
-      <c r="F42" s="64"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
-      <c r="K42" s="55"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="65">
-        <v>13.1</v>
-      </c>
-      <c r="B43" s="72" t="s">
-        <v>254</v>
-      </c>
-      <c r="C43" s="79" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="68">
-        <v>10</v>
-      </c>
-      <c r="E43" s="55"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="65">
-        <v>13.2</v>
-      </c>
-      <c r="B44" s="72" t="s">
-        <v>255</v>
-      </c>
-      <c r="C44" s="71" t="s">
-        <v>206</v>
-      </c>
-      <c r="D44" s="69">
-        <v>2</v>
-      </c>
-      <c r="E44" s="55"/>
-      <c r="F44" s="64"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="65">
-        <v>13.5</v>
-      </c>
-      <c r="B45" s="74" t="s">
-        <v>199</v>
-      </c>
-      <c r="C45" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="68">
-        <v>15</v>
-      </c>
-      <c r="E45" s="55"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="65">
-        <v>14.1</v>
-      </c>
-      <c r="B46" s="72" t="s">
-        <v>226</v>
-      </c>
-      <c r="C46" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="68">
-        <v>4</v>
-      </c>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="65">
-        <v>14.1</v>
-      </c>
-      <c r="B47" s="72" t="s">
-        <v>228</v>
-      </c>
-      <c r="C47" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="68">
-        <v>4</v>
-      </c>
-      <c r="E47" s="55"/>
-      <c r="F47" s="64"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="55"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="55"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="65">
-        <v>14.1</v>
-      </c>
-      <c r="B48" s="72" t="s">
-        <v>256</v>
-      </c>
-      <c r="C48" s="79" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="68">
-        <v>10</v>
-      </c>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="55"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="65">
-        <v>14.2</v>
-      </c>
-      <c r="B49" s="72" t="s">
-        <v>227</v>
-      </c>
-      <c r="C49" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49" s="68">
-        <v>15</v>
-      </c>
-      <c r="E49" s="55"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="55"/>
-      <c r="K49" s="55"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="65">
-        <v>14.2</v>
-      </c>
-      <c r="B50" s="72" t="s">
-        <v>229</v>
-      </c>
-      <c r="C50" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="68">
-        <v>15</v>
-      </c>
-      <c r="E50" s="55"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="55"/>
-      <c r="H50" s="55"/>
-      <c r="I50" s="55"/>
-      <c r="J50" s="55"/>
-      <c r="K50" s="55"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="65">
-        <v>14.2</v>
-      </c>
-      <c r="B51" s="72" t="s">
-        <v>257</v>
-      </c>
-      <c r="C51" s="71" t="s">
-        <v>206</v>
-      </c>
-      <c r="D51" s="69">
-        <v>2</v>
-      </c>
-      <c r="E51" s="55"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="55"/>
-      <c r="H51" s="55"/>
-      <c r="I51" s="55"/>
-      <c r="J51" s="55"/>
-      <c r="K51" s="55"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="65">
-        <v>15.1</v>
-      </c>
-      <c r="B52" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="C52" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="68">
-        <v>4</v>
-      </c>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="55"/>
-      <c r="I52" s="55"/>
-      <c r="J52" s="55"/>
-      <c r="K52" s="55"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="65">
-        <v>15.1</v>
-      </c>
-      <c r="B53" s="72" t="s">
-        <v>258</v>
-      </c>
-      <c r="C53" s="79" t="s">
-        <v>104</v>
-      </c>
-      <c r="D53" s="68">
-        <v>10</v>
-      </c>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="55"/>
-      <c r="H53" s="55"/>
-      <c r="I53" s="55"/>
-      <c r="J53" s="55"/>
-      <c r="K53" s="55"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="65">
-        <v>15.2</v>
-      </c>
-      <c r="B54" s="66" t="s">
-        <v>28</v>
-      </c>
-      <c r="C54" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D54" s="68">
-        <v>10</v>
-      </c>
-      <c r="E54" s="55"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="55"/>
-      <c r="H54" s="55"/>
-      <c r="I54" s="55"/>
-      <c r="J54" s="55"/>
-      <c r="K54" s="55"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="65">
-        <v>15.2</v>
-      </c>
-      <c r="B55" s="72" t="s">
-        <v>259</v>
-      </c>
-      <c r="C55" s="71" t="s">
-        <v>206</v>
-      </c>
-      <c r="D55" s="69">
-        <v>2</v>
-      </c>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
-      <c r="G55" s="55"/>
-      <c r="H55" s="55"/>
-      <c r="I55" s="55"/>
-      <c r="J55" s="55"/>
-      <c r="K55" s="55"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="65">
-        <v>16</v>
-      </c>
-      <c r="B56" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="68">
-        <v>5</v>
-      </c>
-      <c r="E56" s="55"/>
-      <c r="F56" s="64"/>
-      <c r="G56" s="55"/>
-      <c r="H56" s="55"/>
-      <c r="I56" s="55"/>
-      <c r="J56" s="55"/>
-      <c r="K56" s="55"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="65">
-        <v>16</v>
-      </c>
-      <c r="B57" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="C57" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" s="68">
-        <v>10</v>
-      </c>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="55"/>
-      <c r="H57" s="55"/>
-      <c r="I57" s="55"/>
-      <c r="J57" s="55"/>
-      <c r="K57" s="55"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="65">
-        <v>16</v>
-      </c>
-      <c r="B58" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="68">
-        <v>50</v>
-      </c>
-      <c r="E58" s="55"/>
-      <c r="F58" s="64"/>
-      <c r="G58" s="55"/>
-      <c r="H58" s="55"/>
-      <c r="I58" s="55"/>
-      <c r="J58" s="55"/>
-      <c r="K58" s="55"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="65">
-        <v>16</v>
-      </c>
-      <c r="B59" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="C59" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="D59" s="68">
-        <v>2</v>
-      </c>
-      <c r="E59" s="55"/>
-      <c r="F59" s="64"/>
-      <c r="G59" s="55"/>
-      <c r="H59" s="55"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
-      <c r="K59" s="55"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="65">
-        <v>16</v>
-      </c>
-      <c r="B60" s="72" t="s">
-        <v>219</v>
-      </c>
-      <c r="C60" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60" s="68">
-        <v>3</v>
-      </c>
-      <c r="E60" s="55"/>
-      <c r="F60" s="64"/>
-      <c r="G60" s="55"/>
-      <c r="H60" s="55"/>
-      <c r="I60" s="55"/>
-      <c r="J60" s="55"/>
-      <c r="K60" s="55"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="65">
-        <v>16</v>
-      </c>
-      <c r="B61" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" s="68">
-        <v>2</v>
-      </c>
-      <c r="E61" s="55"/>
-      <c r="F61" s="64"/>
-      <c r="G61" s="55"/>
-      <c r="H61" s="55"/>
-      <c r="I61" s="55"/>
-      <c r="J61" s="55"/>
-      <c r="K61" s="55"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="65">
-        <v>16</v>
-      </c>
-      <c r="B62" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="D62" s="68">
-        <v>10</v>
-      </c>
-      <c r="E62" s="55"/>
-      <c r="F62" s="64"/>
-      <c r="G62" s="55"/>
-      <c r="H62" s="55"/>
-      <c r="I62" s="55"/>
-      <c r="J62" s="55"/>
-      <c r="K62" s="55"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="65">
-        <v>16</v>
-      </c>
-      <c r="B63" s="85" t="s">
-        <v>105</v>
-      </c>
-      <c r="C63" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="68">
+      <c r="D63" s="66">
         <v>6</v>
       </c>
-      <c r="E63" s="55"/>
-      <c r="F63" s="64"/>
-      <c r="G63" s="55"/>
-      <c r="H63" s="55"/>
-      <c r="I63" s="55"/>
-      <c r="J63" s="55"/>
-      <c r="K63" s="55"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="62"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="53"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="65"/>
-      <c r="B64" s="72"/>
-      <c r="C64" s="79"/>
-      <c r="D64" s="68"/>
-      <c r="E64" s="55"/>
-      <c r="F64" s="64"/>
-      <c r="G64" s="55"/>
-      <c r="H64" s="55"/>
-      <c r="I64" s="55"/>
-      <c r="J64" s="55"/>
-      <c r="K64" s="55"/>
+      <c r="A64" s="63"/>
+      <c r="B64" s="70"/>
+      <c r="C64" s="77"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="62"/>
+      <c r="G64" s="53"/>
+      <c r="H64" s="53"/>
+      <c r="I64" s="53"/>
+      <c r="J64" s="53"/>
+      <c r="K64" s="53"/>
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A65" s="65"/>
-      <c r="B65" s="72"/>
-      <c r="C65" s="71"/>
-      <c r="D65" s="69"/>
-      <c r="E65" s="55"/>
-      <c r="F65" s="64"/>
-      <c r="G65" s="55"/>
-      <c r="H65" s="55"/>
-      <c r="I65" s="55"/>
-      <c r="J65" s="55"/>
-      <c r="K65" s="55"/>
+      <c r="A65" s="63"/>
+      <c r="B65" s="70"/>
+      <c r="C65" s="69"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="62"/>
+      <c r="G65" s="53"/>
+      <c r="H65" s="53"/>
+      <c r="I65" s="53"/>
+      <c r="J65" s="53"/>
+      <c r="K65" s="53"/>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A66" s="65"/>
-      <c r="B66" s="72"/>
-      <c r="C66" s="79"/>
-      <c r="D66" s="68"/>
-      <c r="E66" s="55"/>
-      <c r="F66" s="64"/>
-      <c r="G66" s="55"/>
-      <c r="H66" s="55"/>
-      <c r="I66" s="55"/>
-      <c r="J66" s="55"/>
-      <c r="K66" s="55"/>
+      <c r="A66" s="63"/>
+      <c r="B66" s="70"/>
+      <c r="C66" s="77"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="53"/>
+      <c r="F66" s="62"/>
+      <c r="G66" s="53"/>
+      <c r="H66" s="53"/>
+      <c r="I66" s="53"/>
+      <c r="J66" s="53"/>
+      <c r="K66" s="53"/>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A67" s="65"/>
-      <c r="B67" s="74"/>
-      <c r="C67" s="71"/>
-      <c r="D67" s="69"/>
-      <c r="E67" s="55"/>
-      <c r="F67" s="55"/>
-      <c r="G67" s="55"/>
-      <c r="H67" s="55"/>
-      <c r="I67" s="55"/>
-      <c r="J67" s="55"/>
-      <c r="K67" s="55"/>
+      <c r="A67" s="63"/>
+      <c r="B67" s="72"/>
+      <c r="C67" s="69"/>
+      <c r="D67" s="67"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="53"/>
+      <c r="G67" s="53"/>
+      <c r="H67" s="53"/>
+      <c r="I67" s="53"/>
+      <c r="J67" s="53"/>
+      <c r="K67" s="53"/>
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A68" s="65"/>
-      <c r="B68" s="72"/>
-      <c r="C68" s="79"/>
-      <c r="D68" s="68"/>
-      <c r="E68" s="55"/>
-      <c r="F68" s="64"/>
-      <c r="G68" s="55"/>
-      <c r="H68" s="55"/>
-      <c r="I68" s="55"/>
-      <c r="J68" s="55"/>
-      <c r="K68" s="55"/>
+      <c r="A68" s="63"/>
+      <c r="B68" s="70"/>
+      <c r="C68" s="77"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="53"/>
+      <c r="F68" s="62"/>
+      <c r="G68" s="53"/>
+      <c r="H68" s="53"/>
+      <c r="I68" s="53"/>
+      <c r="J68" s="53"/>
+      <c r="K68" s="53"/>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A69" s="65"/>
-      <c r="B69" s="72"/>
-      <c r="C69" s="71"/>
-      <c r="D69" s="69"/>
-      <c r="E69" s="55"/>
-      <c r="F69" s="64"/>
-      <c r="G69" s="55"/>
-      <c r="H69" s="55"/>
-      <c r="I69" s="55"/>
-      <c r="J69" s="55"/>
-      <c r="K69" s="55"/>
+      <c r="A69" s="63"/>
+      <c r="B69" s="70"/>
+      <c r="C69" s="69"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="62"/>
+      <c r="G69" s="53"/>
+      <c r="H69" s="53"/>
+      <c r="I69" s="53"/>
+      <c r="J69" s="53"/>
+      <c r="K69" s="53"/>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A70" s="65"/>
-      <c r="B70" s="74"/>
-      <c r="C70" s="79"/>
-      <c r="D70" s="68"/>
-      <c r="E70" s="55"/>
-      <c r="F70" s="64"/>
-      <c r="G70" s="55"/>
-      <c r="H70" s="55"/>
-      <c r="I70" s="55"/>
-      <c r="J70" s="55"/>
-      <c r="K70" s="55"/>
+      <c r="A70" s="63"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="77"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="62"/>
+      <c r="G70" s="53"/>
+      <c r="H70" s="53"/>
+      <c r="I70" s="53"/>
+      <c r="J70" s="53"/>
+      <c r="K70" s="53"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A71" s="65"/>
-      <c r="B71" s="74"/>
-      <c r="C71" s="71"/>
-      <c r="D71" s="69"/>
-      <c r="E71" s="55"/>
-      <c r="F71" s="64"/>
-      <c r="G71" s="55"/>
-      <c r="H71" s="55"/>
-      <c r="I71" s="55"/>
-      <c r="J71" s="55"/>
-      <c r="K71" s="55"/>
+      <c r="A71" s="63"/>
+      <c r="B71" s="72"/>
+      <c r="C71" s="69"/>
+      <c r="D71" s="67"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="62"/>
+      <c r="G71" s="53"/>
+      <c r="H71" s="53"/>
+      <c r="I71" s="53"/>
+      <c r="J71" s="53"/>
+      <c r="K71" s="53"/>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A72" s="65"/>
-      <c r="B72" s="72"/>
-      <c r="C72" s="79"/>
-      <c r="D72" s="68"/>
-      <c r="E72" s="55"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="55"/>
-      <c r="H72" s="55"/>
-      <c r="I72" s="55"/>
-      <c r="J72" s="55"/>
-      <c r="K72" s="55"/>
+      <c r="A72" s="63"/>
+      <c r="B72" s="70"/>
+      <c r="C72" s="77"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="62"/>
+      <c r="G72" s="53"/>
+      <c r="H72" s="53"/>
+      <c r="I72" s="53"/>
+      <c r="J72" s="53"/>
+      <c r="K72" s="53"/>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A73" s="65"/>
-      <c r="B73" s="72"/>
-      <c r="C73" s="71"/>
-      <c r="D73" s="69"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="64"/>
-      <c r="G73" s="55"/>
-      <c r="H73" s="55"/>
-      <c r="I73" s="55"/>
-      <c r="J73" s="55"/>
-      <c r="K73" s="55"/>
+      <c r="A73" s="63"/>
+      <c r="B73" s="70"/>
+      <c r="C73" s="69"/>
+      <c r="D73" s="67"/>
+      <c r="E73" s="53"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="53"/>
+      <c r="H73" s="53"/>
+      <c r="I73" s="53"/>
+      <c r="J73" s="53"/>
+      <c r="K73" s="53"/>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A74" s="65"/>
-      <c r="E74" s="55"/>
-      <c r="F74" s="64"/>
-      <c r="G74" s="55"/>
-      <c r="H74" s="55"/>
-      <c r="I74" s="55"/>
-      <c r="J74" s="55"/>
-      <c r="K74" s="55"/>
+      <c r="A74" s="63"/>
+      <c r="E74" s="53"/>
+      <c r="F74" s="62"/>
+      <c r="G74" s="53"/>
+      <c r="H74" s="53"/>
+      <c r="I74" s="53"/>
+      <c r="J74" s="53"/>
+      <c r="K74" s="53"/>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E75" s="55"/>
-      <c r="F75" s="55"/>
-      <c r="G75" s="55"/>
-      <c r="H75" s="55"/>
-      <c r="I75" s="55"/>
-      <c r="J75" s="55"/>
-      <c r="K75" s="55"/>
+      <c r="E75" s="53"/>
+      <c r="F75" s="53"/>
+      <c r="G75" s="53"/>
+      <c r="H75" s="53"/>
+      <c r="I75" s="53"/>
+      <c r="J75" s="53"/>
+      <c r="K75" s="53"/>
     </row>
     <row r="76" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="8"/>
-      <c r="E76" s="56"/>
-      <c r="F76" s="56"/>
-      <c r="G76" s="55"/>
-      <c r="H76" s="55"/>
-      <c r="I76" s="55"/>
-      <c r="J76" s="55"/>
-      <c r="K76" s="55"/>
+      <c r="E76" s="54"/>
+      <c r="F76" s="54"/>
+      <c r="G76" s="53"/>
+      <c r="H76" s="53"/>
+      <c r="I76" s="53"/>
+      <c r="J76" s="53"/>
+      <c r="K76" s="53"/>
       <c r="L76" s="4"/>
       <c r="P76" s="4"/>
       <c r="Q76" s="4"/>
@@ -6336,13 +6347,13 @@
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="8"/>
-      <c r="E77" s="55"/>
-      <c r="F77" s="64"/>
-      <c r="G77" s="55"/>
-      <c r="H77" s="55"/>
-      <c r="I77" s="55"/>
-      <c r="J77" s="55"/>
-      <c r="K77" s="55"/>
+      <c r="E77" s="53"/>
+      <c r="F77" s="62"/>
+      <c r="G77" s="53"/>
+      <c r="H77" s="53"/>
+      <c r="I77" s="53"/>
+      <c r="J77" s="53"/>
+      <c r="K77" s="53"/>
       <c r="L77" s="4"/>
       <c r="P77" s="4"/>
       <c r="Q77" s="4"/>
@@ -6363,10 +6374,10 @@
       <c r="E78" s="23"/>
       <c r="F78" s="23"/>
       <c r="G78" s="23"/>
-      <c r="H78" s="55"/>
-      <c r="I78" s="55"/>
-      <c r="J78" s="55"/>
-      <c r="K78" s="55"/>
+      <c r="H78" s="53"/>
+      <c r="I78" s="53"/>
+      <c r="J78" s="53"/>
+      <c r="K78" s="53"/>
       <c r="L78" s="4"/>
       <c r="P78" s="4"/>
       <c r="Q78" s="4"/>

</xml_diff>

<commit_message>
update hw1 and rebuild
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD601362-545C-4E5C-8A1F-B256EA9420AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104370E4-4584-40F4-8E88-34179191E4A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -1238,10 +1238,6 @@
 Properly cite relevant research</t>
   </si>
   <si>
-    <t>Learn how to use R to do and turn in homework (test markdown file, hw1 template)
-Set up an organized class folder</t>
-  </si>
-  <si>
     <t>Working with Data 
 Describing data using summary statistics
 Basic data management</t>
@@ -1581,6 +1577,11 @@
 Look through the [[research data available]](https://drive.google.com/drive/u/3/folders/1jULudBjRbHdW-uLIvmMbxRBEJJkq9crY) and pick a data set that you want to work with. 
 Read: Learning - your first job
 Read: MAI and academic achievement</t>
+  </si>
+  <si>
+    <t>Learn how to use R to do and turn in homework (test markdown file, hw1 template)
+Set up an organized class folder
+Familiarize yourself with class resources on how to learn R.  (PDS Videos, Course Notes, Math 130, R-help page on clas website)</t>
   </si>
 </sst>
 </file>
@@ -2728,7 +2729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
@@ -2777,16 +2778,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F2" s="38" t="s">
         <v>149</v>
       </c>
       <c r="G2" s="97" t="s">
+        <v>318</v>
+      </c>
+      <c r="H2" s="85" t="s">
         <v>319</v>
-      </c>
-      <c r="H2" s="85" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2794,7 +2795,7 @@
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2802,7 +2803,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E4" s="45" t="s">
         <v>169</v>
@@ -2843,10 +2844,10 @@
         <v>190</v>
       </c>
       <c r="G7" s="97" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H7" s="85" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2865,7 +2866,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2895,10 +2896,10 @@
       </c>
       <c r="F11" s="39"/>
       <c r="G11" s="97" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H11" s="85" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2920,7 +2921,7 @@
         <v>3.3</v>
       </c>
       <c r="D13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H13" s="86"/>
     </row>
@@ -2932,16 +2933,16 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E14" s="45" t="s">
         <v>174</v>
       </c>
       <c r="G14" s="97" t="s">
+        <v>324</v>
+      </c>
+      <c r="H14" t="s">
         <v>325</v>
-      </c>
-      <c r="H14" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2949,7 +2950,7 @@
         <v>4.2</v>
       </c>
       <c r="D15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E15" s="45" t="s">
         <v>174</v>
@@ -2961,13 +2962,13 @@
         <v>4.3</v>
       </c>
       <c r="D16" s="87" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E16" s="88"/>
       <c r="F16" s="89"/>
       <c r="G16" s="98"/>
       <c r="H16" s="87" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2985,10 +2986,10 @@
       </c>
       <c r="F17" s="41"/>
       <c r="G17" s="97" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2996,7 +2997,7 @@
         <v>5.2</v>
       </c>
       <c r="D18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F18" s="41"/>
     </row>
@@ -3014,10 +3015,10 @@
         <v>210</v>
       </c>
       <c r="G19" s="97" t="s">
+        <v>329</v>
+      </c>
+      <c r="H19" s="52" t="s">
         <v>330</v>
-      </c>
-      <c r="H19" s="52" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3042,7 +3043,7 @@
       <c r="F21" s="92"/>
       <c r="G21" s="99"/>
       <c r="H21" s="90" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -3053,7 +3054,7 @@
         <v>212</v>
       </c>
       <c r="H22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3061,13 +3062,13 @@
         <v>6.5</v>
       </c>
       <c r="D23" s="87" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E23" s="88"/>
       <c r="F23" s="89"/>
       <c r="G23" s="98"/>
       <c r="H23" s="87" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3078,13 +3079,13 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E24" s="45" t="s">
         <v>185</v>
       </c>
       <c r="G24" s="97" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3092,7 +3093,7 @@
         <v>7.2</v>
       </c>
       <c r="D25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3114,10 +3115,10 @@
         <v>211</v>
       </c>
       <c r="G27" s="97" t="s">
+        <v>335</v>
+      </c>
+      <c r="H27" t="s">
         <v>336</v>
-      </c>
-      <c r="H27" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3153,10 +3154,10 @@
         <v>177</v>
       </c>
       <c r="G30" s="97" t="s">
+        <v>337</v>
+      </c>
+      <c r="H30" t="s">
         <v>338</v>
-      </c>
-      <c r="H30" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3195,7 +3196,7 @@
         <v>184</v>
       </c>
       <c r="G33" s="97" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -3212,10 +3213,10 @@
         <v>180</v>
       </c>
       <c r="G34" s="97" t="s">
+        <v>340</v>
+      </c>
+      <c r="H34" t="s">
         <v>341</v>
-      </c>
-      <c r="H34" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3255,10 +3256,10 @@
       </c>
       <c r="F37" s="41"/>
       <c r="G37" s="97" t="s">
+        <v>342</v>
+      </c>
+      <c r="H37" t="s">
         <v>343</v>
-      </c>
-      <c r="H37" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3266,13 +3267,13 @@
         <v>12.2</v>
       </c>
       <c r="D38" s="87" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E38" s="88"/>
       <c r="F38" s="89"/>
       <c r="G38" s="98"/>
       <c r="H38" s="87" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -3290,7 +3291,7 @@
       </c>
       <c r="F39" s="41"/>
       <c r="G39" s="97" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3307,7 +3308,7 @@
         <v>14</v>
       </c>
       <c r="D41" s="93" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E41" s="94"/>
       <c r="F41" s="95"/>
@@ -3322,11 +3323,11 @@
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F42" s="41"/>
       <c r="G42" s="97" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3334,13 +3335,13 @@
         <v>15.2</v>
       </c>
       <c r="D43" s="87" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E43" s="88"/>
       <c r="F43" s="89"/>
       <c r="G43" s="98"/>
       <c r="H43" s="87" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -3351,16 +3352,16 @@
         <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E44" s="45" t="s">
         <v>183</v>
       </c>
       <c r="G44" s="97" t="s">
+        <v>348</v>
+      </c>
+      <c r="H44" t="s">
         <v>349</v>
-      </c>
-      <c r="H44" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3382,7 +3383,7 @@
         <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3398,9 +3399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3456,19 +3457,19 @@
         <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>263</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>271</v>
+        <v>353</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>264</v>
@@ -3489,7 +3490,7 @@
         <v>270</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>21</v>
@@ -3514,19 +3515,19 @@
         <v>42255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>100</v>
@@ -3544,25 +3545,25 @@
         <v>42262</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3574,23 +3575,23 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3602,16 +3603,16 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>160</v>
@@ -3632,13 +3633,13 @@
         <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>61</v>
@@ -3758,18 +3759,18 @@
         <v>42318</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>37</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3781,13 +3782,13 @@
         <v>42325</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>94</v>
@@ -3821,7 +3822,7 @@
         <v>42339</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>83</v>
@@ -3846,7 +3847,7 @@
         <v>42346</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>84</v>
@@ -4359,7 +4360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add hw3 and quiz3
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F95E2E-F087-435D-9832-9BC585D68DFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CADD7C2-D9F5-4B47-8B5A-3969E4855FF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="283">
   <si>
     <t>Finals Week</t>
   </si>
@@ -196,10 +196,6 @@
     <t xml:space="preserve">Introduction of probability by means of exploding kittens. </t>
   </si>
   <si>
-    <t>Identify one binary and one continuous variable in your data set of interest. 
-Come prepared with summary statistics for each (n, # missing values, #yes, mean, sd)</t>
-  </si>
-  <si>
     <t>**RAT on Foundations for Inference**
 How is an interval estimate different from a point estimate? 
 How is an interval estimate created?
@@ -207,12 +203,6 @@
   </si>
   <si>
     <t>**RAT on choosing appropriate Bivariate Analysis**</t>
-  </si>
-  <si>
-    <t>Read lecture notes on writing about empirical research
-Read instructions for first poster prep assignment
-Print out and take the sample exam. 
-Watch the PDS video 10 before Friday</t>
   </si>
   <si>
     <t xml:space="preserve">Go through a full 5 step hypothesis. 
@@ -777,11 +767,6 @@
   </si>
   <si>
     <t xml:space="preserve">Assess and describe the association between a continuous variable and a categorical variable. </t>
-  </si>
-  <si>
-    <t>Watch PDS Video 6. As always, follow along on your computer for the best results. 
-Install the `ggplot2` and `dplyr` packages in R. 
-Read the instructions for the research project - Poster preparation slides</t>
   </si>
   <si>
     <t>hw05 - bivariate graphing</t>
@@ -915,11 +900,6 @@
   </si>
   <si>
     <t>[hw03_data_management](hw/hw03_data_management.html) (Due 9/14 )</t>
-  </si>
-  <si>
-    <t>Quiz 3 (Due 9/8 ) 
-[Sec 01]()
-[Sec 02]()</t>
   </si>
   <si>
     <t>Quiz 4 (Due 9/15 ) 
@@ -1092,6 +1072,28 @@
 [[Sec 01]](https://forms.gle/46GFpQNGswFxH1YZ6)
 [[Sec 02]](https://forms.gle/5VXAvu8sxw6qvG4H7)</t>
   </si>
+  <si>
+    <t>Quiz 3 (Due 9/8 ) 
+[[Sec 01]](https://forms.gle/ot6kJ2As7WHyrZd47)
+[[Sec 02]](https://forms.gle/TodvxwrZjhb2CRvC8)</t>
+  </si>
+  <si>
+    <t>Watch PDS video 7</t>
+  </si>
+  <si>
+    <t>Read instructions for first poster prep assignment
+Review and take the sample exam. 
+Watch the PDS video 8 before Friday</t>
+  </si>
+  <si>
+    <t>Read lecture notes on writing about empirical research
+Identify one binary and one continuous variable in your data set of interest. 
+Come prepared with summary statistics for each (n, # missing values, #yes, mean, sd)</t>
+  </si>
+  <si>
+    <t>Watch PDS Video 6. As always, follow along on your computer for the best results. 
+Read the instructions for the research project - Poster preparation slides</t>
+  </si>
 </sst>
 </file>
 
@@ -1100,9 +1102,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1498,111 +1507,111 @@
   </borders>
   <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="77" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="78" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="78" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="80"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="80" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="80"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="80" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="80" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="80" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="81" applyFont="1" applyAlignment="1">
@@ -1617,10 +1626,10 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="21" fillId="5" borderId="3" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="22" fillId="5" borderId="3" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="6" borderId="3" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1629,161 +1638,158 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="3" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="80" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="80" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="80" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="82" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="4" xfId="82" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="4" xfId="82" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="4" xfId="82" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="4" xfId="82" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="82" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="80" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="82"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="80" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="82"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="80" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="80" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="80" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="80" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1805,7 +1811,7 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="82" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1820,17 +1826,27 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2255,8 +2271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2266,31 +2282,31 @@
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.375" style="42" customWidth="1"/>
     <col min="6" max="6" width="13.875" style="35" customWidth="1"/>
-    <col min="7" max="7" width="16.875" style="94" customWidth="1"/>
+    <col min="7" max="7" width="16.875" style="93" customWidth="1"/>
     <col min="8" max="8" width="79.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="35" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="93" t="s">
-        <v>74</v>
+        <v>118</v>
+      </c>
+      <c r="G1" s="92" t="s">
+        <v>72</v>
       </c>
       <c r="H1" s="48" t="s">
         <v>6</v>
@@ -2304,16 +2320,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="101" t="s">
-        <v>279</v>
-      </c>
-      <c r="H2" s="82" t="s">
-        <v>240</v>
+        <v>75</v>
+      </c>
+      <c r="G2" s="100" t="s">
+        <v>275</v>
+      </c>
+      <c r="H2" s="101" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2321,7 +2337,7 @@
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2329,10 +2345,10 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2340,10 +2356,10 @@
         <v>1.4</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F5" s="38"/>
     </row>
@@ -2352,7 +2368,7 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E6" s="43"/>
     </row>
@@ -2364,16 +2380,16 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E7" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="G7" s="101" t="s">
-        <v>281</v>
-      </c>
-      <c r="H7" s="82" t="s">
-        <v>241</v>
+        <v>115</v>
+      </c>
+      <c r="G7" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="H7" s="101" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2381,10 +2397,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2392,7 +2408,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2400,13 +2416,13 @@
         <v>2.4</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A11" s="41">
         <v>3.1</v>
       </c>
@@ -2415,17 +2431,17 @@
       </c>
       <c r="C11" s="36"/>
       <c r="D11" s="37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F11" s="36"/>
-      <c r="G11" s="94" t="s">
-        <v>243</v>
-      </c>
-      <c r="H11" s="82" t="s">
-        <v>242</v>
+      <c r="G11" s="102" t="s">
+        <v>278</v>
+      </c>
+      <c r="H11" s="81" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2433,13 +2449,13 @@
         <v>3.2</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="H12" s="83" t="s">
-        <v>134</v>
+        <v>98</v>
+      </c>
+      <c r="H12" s="82" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2447,9 +2463,9 @@
         <v>3.3</v>
       </c>
       <c r="D13" t="s">
-        <v>228</v>
-      </c>
-      <c r="H13" s="83"/>
+        <v>225</v>
+      </c>
+      <c r="H13" s="82"/>
     </row>
     <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
@@ -2459,16 +2475,16 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E14" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" s="94" t="s">
-        <v>244</v>
-      </c>
-      <c r="H14" t="s">
-        <v>245</v>
+        <v>99</v>
+      </c>
+      <c r="G14" s="102" t="s">
+        <v>240</v>
+      </c>
+      <c r="H14" s="81" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2476,10 +2492,10 @@
         <v>4.2</v>
       </c>
       <c r="D15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F15" s="38"/>
     </row>
@@ -2487,14 +2503,14 @@
       <c r="A16" s="40">
         <v>4.3</v>
       </c>
-      <c r="D16" s="84" t="s">
-        <v>231</v>
-      </c>
-      <c r="E16" s="85"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="84" t="s">
-        <v>246</v>
+      <c r="D16" s="83" t="s">
+        <v>228</v>
+      </c>
+      <c r="E16" s="84"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="83" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2505,17 +2521,17 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F17" s="38"/>
-      <c r="G17" s="94" t="s">
-        <v>248</v>
-      </c>
-      <c r="H17" t="s">
-        <v>247</v>
+      <c r="G17" s="102" t="s">
+        <v>244</v>
+      </c>
+      <c r="H17" s="81" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2523,7 +2539,7 @@
         <v>5.2</v>
       </c>
       <c r="D18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F18" s="38"/>
     </row>
@@ -2535,16 +2551,16 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="G19" s="94" t="s">
-        <v>249</v>
-      </c>
-      <c r="H19" s="49" t="s">
-        <v>250</v>
+        <v>134</v>
+      </c>
+      <c r="G19" s="102" t="s">
+        <v>245</v>
+      </c>
+      <c r="H19" s="103" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2552,24 +2568,24 @@
         <v>6.2</v>
       </c>
       <c r="D20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>6.3</v>
       </c>
-      <c r="D21" s="87" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="88"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="96"/>
-      <c r="H21" s="87" t="s">
-        <v>251</v>
+      <c r="D21" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="87"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="86" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2577,24 +2593,24 @@
         <v>6.4</v>
       </c>
       <c r="D22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H22" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <v>6.5</v>
       </c>
-      <c r="D23" s="84" t="s">
-        <v>233</v>
-      </c>
-      <c r="E23" s="85"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="84" t="s">
-        <v>253</v>
+      <c r="D23" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E23" s="84"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="94"/>
+      <c r="H23" s="83" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2605,13 +2621,13 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="G24" s="94" t="s">
-        <v>254</v>
+        <v>110</v>
+      </c>
+      <c r="G24" s="102" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2619,7 +2635,7 @@
         <v>7.2</v>
       </c>
       <c r="D25" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2627,7 +2643,7 @@
         <v>7.3</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2638,13 +2654,13 @@
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>137</v>
-      </c>
-      <c r="G27" s="94" t="s">
-        <v>255</v>
-      </c>
-      <c r="H27" t="s">
-        <v>256</v>
+        <v>135</v>
+      </c>
+      <c r="G27" s="102" t="s">
+        <v>251</v>
+      </c>
+      <c r="H27" s="81" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2652,10 +2668,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2663,7 +2679,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2674,16 +2690,16 @@
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E30" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="G30" s="94" t="s">
-        <v>257</v>
-      </c>
-      <c r="H30" t="s">
-        <v>258</v>
+        <v>102</v>
+      </c>
+      <c r="G30" s="102" t="s">
+        <v>253</v>
+      </c>
+      <c r="H30" s="81" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2691,10 +2707,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2702,10 +2718,10 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -2716,13 +2732,13 @@
         <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="G33" s="94" t="s">
-        <v>259</v>
+        <v>109</v>
+      </c>
+      <c r="G33" s="102" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -2733,16 +2749,16 @@
         <v>11</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="G34" s="94" t="s">
-        <v>260</v>
-      </c>
-      <c r="H34" t="s">
-        <v>261</v>
+        <v>105</v>
+      </c>
+      <c r="G34" s="102" t="s">
+        <v>256</v>
+      </c>
+      <c r="H34" s="81" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2750,10 +2766,10 @@
         <v>11.2</v>
       </c>
       <c r="D35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2761,10 +2777,10 @@
         <v>11.3</v>
       </c>
       <c r="D36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -2775,31 +2791,31 @@
         <v>12</v>
       </c>
       <c r="D37" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="E37" s="42" t="s">
-        <v>116</v>
-      </c>
       <c r="F37" s="38"/>
-      <c r="G37" s="94" t="s">
-        <v>262</v>
-      </c>
-      <c r="H37" t="s">
-        <v>263</v>
+      <c r="G37" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="H37" s="81" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
         <v>12.2</v>
       </c>
-      <c r="D38" s="84" t="s">
-        <v>236</v>
-      </c>
-      <c r="E38" s="85"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="95"/>
-      <c r="H38" s="84" t="s">
-        <v>264</v>
+      <c r="D38" s="83" t="s">
+        <v>233</v>
+      </c>
+      <c r="E38" s="84"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="83" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -2810,14 +2826,14 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E39" s="42" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F39" s="38"/>
-      <c r="G39" s="94" t="s">
-        <v>265</v>
+      <c r="G39" s="102" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2825,7 +2841,7 @@
         <v>13.2</v>
       </c>
       <c r="D40" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F40" s="38"/>
     </row>
@@ -2833,13 +2849,13 @@
       <c r="A41" s="40">
         <v>14</v>
       </c>
-      <c r="D41" s="90" t="s">
-        <v>271</v>
-      </c>
-      <c r="E41" s="91"/>
-      <c r="F41" s="92"/>
-      <c r="G41" s="97"/>
-      <c r="H41" s="90"/>
+      <c r="D41" s="89" t="s">
+        <v>267</v>
+      </c>
+      <c r="E41" s="90"/>
+      <c r="F41" s="91"/>
+      <c r="G41" s="96"/>
+      <c r="H41" s="89"/>
     </row>
     <row r="42" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
@@ -2849,25 +2865,25 @@
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F42" s="38"/>
-      <c r="G42" s="94" t="s">
-        <v>266</v>
+      <c r="G42" s="102" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="40">
         <v>15.2</v>
       </c>
-      <c r="D43" s="84" t="s">
-        <v>238</v>
-      </c>
-      <c r="E43" s="85"/>
-      <c r="F43" s="86"/>
-      <c r="G43" s="95"/>
-      <c r="H43" s="84" t="s">
-        <v>267</v>
+      <c r="D43" s="83" t="s">
+        <v>235</v>
+      </c>
+      <c r="E43" s="84"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="94"/>
+      <c r="H43" s="83" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -2878,16 +2894,16 @@
         <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E44" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="G44" s="94" t="s">
-        <v>268</v>
+        <v>108</v>
+      </c>
+      <c r="G44" s="102" t="s">
+        <v>264</v>
       </c>
       <c r="H44" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2895,10 +2911,10 @@
         <v>17.100000000000001</v>
       </c>
       <c r="D45" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2909,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2925,9 +2941,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,7 +2951,7 @@
     <col min="1" max="1" width="8.125" style="21" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="21" customWidth="1"/>
     <col min="3" max="3" width="33.625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="27.375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="36.5" style="22" customWidth="1"/>
     <col min="5" max="5" width="88.25" style="22" customWidth="1"/>
     <col min="6" max="6" width="34.625" style="22" customWidth="1"/>
     <col min="7" max="8" width="38" style="22" customWidth="1"/>
@@ -2968,7 +2984,7 @@
       <c r="H1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="81" t="s">
+      <c r="I1" s="80" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2983,22 +2999,22 @@
         <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3010,25 +3026,25 @@
         <v>42248</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H3" s="30" t="s">
         <v>38</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J3" s="30"/>
     </row>
@@ -3041,25 +3057,25 @@
         <v>42255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -3071,25 +3087,25 @@
         <v>42262</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3101,26 +3117,28 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>279</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>6</v>
       </c>
@@ -3129,25 +3147,25 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>280</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
         <v>7</v>
       </c>
@@ -3159,19 +3177,19 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -3186,14 +3204,14 @@
         <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -3209,19 +3227,19 @@
         <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3233,22 +3251,22 @@
         <v>42304</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3260,19 +3278,19 @@
         <v>42311</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -3285,18 +3303,18 @@
         <v>42318</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3308,19 +3326,19 @@
         <v>42325</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H14" s="27"/>
     </row>
@@ -3331,7 +3349,7 @@
         <v>42332</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -3348,20 +3366,20 @@
         <v>42339</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3373,10 +3391,10 @@
         <v>42346</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -3392,7 +3410,7 @@
         <v>42353</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3411,7 +3429,7 @@
   <dimension ref="A1:AD78"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3447,10 +3465,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2" t="s">
@@ -3523,13 +3541,13 @@
       <c r="D2" s="8">
         <v>3</v>
       </c>
-      <c r="E2" s="98" t="s">
-        <v>272</v>
-      </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="E2" s="97" t="s">
+        <v>268</v>
+      </c>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I2" s="5">
         <f>SUMIF($C$2:$C$69,H2,$D$2:$D$69)-30</f>
@@ -3539,9 +3557,9 @@
         <f t="shared" ref="J2:J7" si="0">I2/$M$8</f>
         <v>0.27554535017221582</v>
       </c>
-      <c r="K2" s="51"/>
+      <c r="K2" s="50"/>
       <c r="L2" s="31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M2" s="5">
         <v>59.5</v>
@@ -3588,23 +3606,23 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="60">
+      <c r="A3" s="59">
         <v>1.2</v>
       </c>
-      <c r="B3" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="63">
+      <c r="B3" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="62">
         <v>10</v>
       </c>
-      <c r="E3" s="99" t="s">
-        <v>272</v>
-      </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="50"/>
+      <c r="E3" s="98" t="s">
+        <v>268</v>
+      </c>
+      <c r="F3" s="50"/>
+      <c r="G3" s="49"/>
       <c r="H3" s="47" t="s">
         <v>23</v>
       </c>
@@ -3616,7 +3634,7 @@
         <f t="shared" si="0"/>
         <v>0.27554535017221582</v>
       </c>
-      <c r="K3" s="50"/>
+      <c r="K3" s="49"/>
       <c r="L3" s="47" t="s">
         <v>23</v>
       </c>
@@ -3665,23 +3683,23 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="60">
+      <c r="A4" s="59">
         <v>1.2</v>
       </c>
-      <c r="B4" s="67" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" s="64">
+      <c r="B4" s="66" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="63">
         <v>2</v>
       </c>
-      <c r="E4" s="100" t="s">
-        <v>272</v>
-      </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="51"/>
+      <c r="E4" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="F4" s="51"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
@@ -3693,7 +3711,7 @@
         <f t="shared" si="0"/>
         <v>4.5924225028702644E-2</v>
       </c>
-      <c r="K4" s="50"/>
+      <c r="K4" s="49"/>
       <c r="L4" s="4" t="s">
         <v>24</v>
       </c>
@@ -3742,23 +3760,23 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="60">
+      <c r="A5" s="59">
         <v>1.4</v>
       </c>
-      <c r="B5" s="67" t="s">
-        <v>189</v>
-      </c>
-      <c r="C5" s="68" t="s">
+      <c r="B5" s="66" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="63">
+      <c r="D5" s="62">
         <v>15</v>
       </c>
-      <c r="E5" s="100" t="s">
-        <v>272</v>
-      </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="50"/>
+      <c r="E5" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="F5" s="52"/>
+      <c r="G5" s="49"/>
       <c r="H5" s="4" t="s">
         <v>12</v>
       </c>
@@ -3770,7 +3788,7 @@
         <f t="shared" si="0"/>
         <v>9.1848450057405287E-2</v>
       </c>
-      <c r="K5" s="51"/>
+      <c r="K5" s="50"/>
       <c r="L5" s="4" t="s">
         <v>12</v>
       </c>
@@ -3812,23 +3830,23 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="60">
+      <c r="A6" s="59">
         <v>2.1</v>
       </c>
-      <c r="B6" s="67" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="63">
+      <c r="B6" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="62">
         <v>10</v>
       </c>
-      <c r="E6" s="100" t="s">
-        <v>272</v>
-      </c>
-      <c r="F6" s="53"/>
-      <c r="G6" s="50"/>
+      <c r="E6" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="F6" s="52"/>
+      <c r="G6" s="49"/>
       <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
@@ -3840,7 +3858,7 @@
         <f t="shared" si="0"/>
         <v>0.22962112514351321</v>
       </c>
-      <c r="K6" s="50"/>
+      <c r="K6" s="49"/>
       <c r="L6" s="4" t="s">
         <v>13</v>
       </c>
@@ -3889,23 +3907,23 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="60">
+      <c r="A7" s="59">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B7" s="67" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="64">
+      <c r="B7" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="63">
         <v>2</v>
       </c>
-      <c r="E7" s="100" t="s">
-        <v>272</v>
-      </c>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
+      <c r="E7" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
       <c r="H7" s="4" t="s">
         <v>14</v>
       </c>
@@ -3917,7 +3935,7 @@
         <f t="shared" si="0"/>
         <v>0.22962112514351321</v>
       </c>
-      <c r="K7" s="50"/>
+      <c r="K7" s="49"/>
       <c r="L7" s="4" t="s">
         <v>14</v>
       </c>
@@ -3966,30 +3984,30 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="60">
+      <c r="A8" s="59">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B8" s="67" t="s">
-        <v>182</v>
-      </c>
-      <c r="C8" s="70" t="s">
+      <c r="B8" s="66" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="71">
+      <c r="D8" s="70">
         <v>10</v>
       </c>
-      <c r="E8" s="100" t="s">
-        <v>272</v>
-      </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
+      <c r="E8" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
       <c r="H8" s="4"/>
       <c r="I8" s="3">
         <f>SUM(I2:I7)</f>
         <v>500</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="51"/>
+      <c r="K8" s="50"/>
       <c r="M8" s="3">
         <f>SUM(M2:M7)</f>
         <v>435.5</v>
@@ -4029,25 +4047,25 @@
       </c>
     </row>
     <row r="9" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="60">
+      <c r="A9" s="59">
         <v>2.4</v>
       </c>
-      <c r="B9" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="73" t="s">
+      <c r="B9" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="63">
+      <c r="D9" s="62">
         <v>4</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="Q9" s="3">
@@ -4065,1189 +4083,1195 @@
       <c r="AD9" s="5"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60">
+      <c r="A10" s="59">
         <v>3.1</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="62">
+        <v>10</v>
+      </c>
+      <c r="E10" s="104" t="s">
+        <v>268</v>
+      </c>
+      <c r="F10" s="52"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="59">
+        <v>3.2</v>
+      </c>
+      <c r="B11" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="63">
+        <v>2</v>
+      </c>
+      <c r="E11" s="104" t="s">
+        <v>268</v>
+      </c>
+      <c r="F11" s="52"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="59">
+        <v>3.6</v>
+      </c>
+      <c r="B12" s="66" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="62">
+        <v>15</v>
+      </c>
+      <c r="E12" s="104" t="s">
+        <v>268</v>
+      </c>
+      <c r="F12" s="50"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="59">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B13" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="65" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="63">
+      <c r="C13" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="62">
         <v>10</v>
       </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="60">
-        <v>3.2</v>
-      </c>
-      <c r="B11" s="67" t="s">
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="59">
+        <v>4.2</v>
+      </c>
+      <c r="B14" s="66" t="s">
         <v>157</v>
       </c>
-      <c r="C11" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="64">
+      <c r="C14" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="63">
         <v>2</v>
       </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="60">
-        <v>3.6</v>
-      </c>
-      <c r="B12" s="67" t="s">
-        <v>183</v>
-      </c>
-      <c r="C12" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="63">
-        <v>15</v>
-      </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="60">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B13" s="67" t="s">
-        <v>158</v>
-      </c>
-      <c r="C13" s="65" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="63">
-        <v>10</v>
-      </c>
-      <c r="E13" s="50"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="60">
-        <v>4.2</v>
-      </c>
-      <c r="B14" s="67" t="s">
-        <v>159</v>
-      </c>
-      <c r="C14" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D14" s="64">
-        <v>2</v>
-      </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="60">
+      <c r="A15" s="59">
         <v>4.5</v>
       </c>
-      <c r="B15" s="67" t="s">
-        <v>184</v>
-      </c>
-      <c r="C15" s="75" t="s">
+      <c r="B15" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="63">
+      <c r="D15" s="62">
         <v>15</v>
       </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="60">
+      <c r="A16" s="59">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B16" s="67" t="s">
-        <v>160</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="63">
+      <c r="B16" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="62">
         <v>10</v>
       </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="60">
+      <c r="A17" s="59">
         <v>5.2</v>
       </c>
-      <c r="B17" s="67" t="s">
-        <v>161</v>
-      </c>
-      <c r="C17" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D17" s="64">
+      <c r="B17" s="66" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="63">
         <v>2</v>
       </c>
-      <c r="E17" s="50"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="60">
+      <c r="A18" s="59">
         <v>5.3</v>
       </c>
-      <c r="B18" s="67" t="s">
-        <v>185</v>
-      </c>
-      <c r="C18" s="75" t="s">
+      <c r="B18" s="66" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="62">
         <v>15</v>
       </c>
-      <c r="E18" s="50"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="60">
+      <c r="A19" s="59">
         <v>6.1</v>
       </c>
-      <c r="B19" s="67" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="76" t="s">
+      <c r="B19" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="63">
+      <c r="D19" s="62">
         <v>50</v>
       </c>
-      <c r="E19" s="50"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="60">
+      <c r="A20" s="59">
         <v>6.1</v>
       </c>
-      <c r="B20" s="67" t="s">
-        <v>162</v>
-      </c>
-      <c r="C20" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="63">
+      <c r="B20" s="66" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="62">
         <v>10</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="60">
+      <c r="A21" s="59">
         <v>6.2</v>
       </c>
-      <c r="B21" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="C21" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D21" s="64">
+      <c r="B21" s="66" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="63">
         <v>2</v>
       </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="60">
+      <c r="A22" s="59">
         <v>7.1</v>
       </c>
-      <c r="B22" s="67" t="s">
-        <v>164</v>
-      </c>
-      <c r="C22" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="63">
+      <c r="B22" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="62">
         <v>10</v>
       </c>
-      <c r="E22" s="50"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="50"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="60">
+      <c r="A23" s="59">
         <v>7.2</v>
       </c>
-      <c r="B23" s="67" t="s">
-        <v>165</v>
-      </c>
-      <c r="C23" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" s="64">
+      <c r="B23" s="66" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="63">
         <v>2</v>
       </c>
-      <c r="E23" s="50"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="60">
+      <c r="A24" s="59">
         <v>7.3</v>
       </c>
-      <c r="B24" s="67" t="s">
-        <v>186</v>
-      </c>
-      <c r="C24" s="77" t="s">
+      <c r="B24" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="63">
+      <c r="D24" s="62">
         <v>10</v>
       </c>
-      <c r="E24" s="50"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="50"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="60">
+      <c r="A25" s="59">
         <v>8.1</v>
       </c>
-      <c r="B25" s="67" t="s">
-        <v>187</v>
-      </c>
-      <c r="C25" s="78" t="s">
+      <c r="B25" s="66" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="63">
+      <c r="D25" s="62">
         <v>15</v>
       </c>
-      <c r="E25" s="50"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="50"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="60">
+      <c r="A26" s="59">
         <v>8.1</v>
       </c>
-      <c r="B26" s="67" t="s">
-        <v>166</v>
-      </c>
-      <c r="C26" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="63">
+      <c r="B26" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="62">
         <v>10</v>
       </c>
-      <c r="E26" s="50"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="60">
+      <c r="A27" s="59">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B27" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="C27" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D27" s="64">
+      <c r="B27" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="63">
         <v>2</v>
       </c>
-      <c r="E27" s="50"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="60">
+      <c r="A28" s="59">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B28" s="67" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" s="73" t="s">
+      <c r="B28" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="63">
+      <c r="D28" s="62">
         <v>4</v>
       </c>
-      <c r="E28" s="50"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="50"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="60">
+      <c r="A29" s="59">
         <v>8.4</v>
       </c>
-      <c r="B29" s="67" t="s">
-        <v>146</v>
-      </c>
-      <c r="C29" s="62" t="s">
+      <c r="B29" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="63">
+      <c r="D29" s="62">
         <v>15</v>
       </c>
-      <c r="E29" s="50"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="50"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="60">
+      <c r="A30" s="59">
         <v>9.1</v>
       </c>
-      <c r="B30" s="67" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="63">
+      <c r="B30" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="62">
         <v>10</v>
       </c>
-      <c r="E30" s="50"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="50"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="60">
+      <c r="A31" s="59">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="66" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="63">
+        <v>2</v>
+      </c>
+      <c r="E31" s="49"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="59">
+        <v>9.5</v>
+      </c>
+      <c r="B32" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="62">
+        <v>5</v>
+      </c>
+      <c r="E32" s="49"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="59">
+        <v>10.1</v>
+      </c>
+      <c r="B33" s="66" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="62">
+        <v>10</v>
+      </c>
+      <c r="E33" s="49"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="59">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B34" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="C31" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D31" s="64">
+      <c r="C34" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="63">
         <v>2</v>
       </c>
-      <c r="E31" s="50"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="60">
-        <v>9.5</v>
-      </c>
-      <c r="B32" s="69" t="s">
+      <c r="E34" s="49"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="59">
+        <v>11.1</v>
+      </c>
+      <c r="B35" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="62">
+        <v>10</v>
+      </c>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="59">
+        <v>11.2</v>
+      </c>
+      <c r="B36" s="66" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="63">
+        <v>2</v>
+      </c>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="59">
+        <v>11.3</v>
+      </c>
+      <c r="B37" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="62">
+        <v>15</v>
+      </c>
+      <c r="E37" s="49"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="59">
+        <v>12.1</v>
+      </c>
+      <c r="B38" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="62">
+        <v>10</v>
+      </c>
+      <c r="E38" s="49"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="59">
+        <v>12.2</v>
+      </c>
+      <c r="B39" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" s="63">
+        <v>2</v>
+      </c>
+      <c r="E39" s="49"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="59">
+        <v>12.5</v>
+      </c>
+      <c r="B40" s="66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="62">
+        <v>4</v>
+      </c>
+      <c r="E40" s="49"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="59">
+        <v>12.6</v>
+      </c>
+      <c r="B41" s="68" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="62">
+        <v>15</v>
+      </c>
+      <c r="E41" s="49"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="59">
+        <v>12.7</v>
+      </c>
+      <c r="B42" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="62">
+        <v>15</v>
+      </c>
+      <c r="E42" s="49"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="59">
+        <v>13.1</v>
+      </c>
+      <c r="B43" s="66" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="62">
+        <v>10</v>
+      </c>
+      <c r="E43" s="49"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="49"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="59">
+        <v>13.2</v>
+      </c>
+      <c r="B44" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="63">
+        <v>2</v>
+      </c>
+      <c r="E44" s="49"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="59">
+        <v>13.5</v>
+      </c>
+      <c r="B45" s="68" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="79" t="s">
+      <c r="C45" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="62">
+        <v>15</v>
+      </c>
+      <c r="E45" s="49"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="49"/>
+      <c r="K45" s="49"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="59">
+        <v>14.1</v>
+      </c>
+      <c r="B46" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="62">
+        <v>4</v>
+      </c>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="49"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="59">
+        <v>14.1</v>
+      </c>
+      <c r="B47" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="C47" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="62">
+        <v>4</v>
+      </c>
+      <c r="E47" s="49"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="49"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="59">
+        <v>14.1</v>
+      </c>
+      <c r="B48" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" s="62">
+        <v>10</v>
+      </c>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="49"/>
+      <c r="J48" s="49"/>
+      <c r="K48" s="49"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="59">
+        <v>14.2</v>
+      </c>
+      <c r="B49" s="66" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="62">
+        <v>15</v>
+      </c>
+      <c r="E49" s="49"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="49"/>
+      <c r="J49" s="49"/>
+      <c r="K49" s="49"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="59">
+        <v>14.2</v>
+      </c>
+      <c r="B50" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="62">
+        <v>15</v>
+      </c>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="59">
+        <v>14.2</v>
+      </c>
+      <c r="B51" s="66" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D51" s="63">
+        <v>2</v>
+      </c>
+      <c r="E51" s="49"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="49"/>
+      <c r="I51" s="49"/>
+      <c r="J51" s="49"/>
+      <c r="K51" s="49"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="59">
+        <v>15.1</v>
+      </c>
+      <c r="B52" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="62">
+        <v>4</v>
+      </c>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="49"/>
+      <c r="I52" s="49"/>
+      <c r="J52" s="49"/>
+      <c r="K52" s="49"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="59">
+        <v>15.1</v>
+      </c>
+      <c r="B53" s="66" t="s">
+        <v>178</v>
+      </c>
+      <c r="C53" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" s="62">
+        <v>10</v>
+      </c>
+      <c r="E53" s="49"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
+      <c r="I53" s="49"/>
+      <c r="J53" s="49"/>
+      <c r="K53" s="49"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="59">
+        <v>15.2</v>
+      </c>
+      <c r="B54" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="62">
+        <v>10</v>
+      </c>
+      <c r="E54" s="49"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="49"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="59">
+        <v>15.2</v>
+      </c>
+      <c r="B55" s="66" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" s="63">
+        <v>2</v>
+      </c>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="49"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="49"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="59">
+        <v>16</v>
+      </c>
+      <c r="B56" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="62">
+        <v>5</v>
+      </c>
+      <c r="E56" s="49"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="49"/>
+      <c r="J56" s="49"/>
+      <c r="K56" s="49"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="59">
+        <v>16</v>
+      </c>
+      <c r="B57" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="62">
+        <v>10</v>
+      </c>
+      <c r="E57" s="49"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="49"/>
+      <c r="H57" s="49"/>
+      <c r="I57" s="49"/>
+      <c r="J57" s="49"/>
+      <c r="K57" s="49"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="59">
+        <v>16</v>
+      </c>
+      <c r="B58" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="62">
+        <v>50</v>
+      </c>
+      <c r="E58" s="49"/>
+      <c r="F58" s="58"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="49"/>
+      <c r="K58" s="49"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="59">
+        <v>16</v>
+      </c>
+      <c r="B59" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="63">
-        <v>5</v>
-      </c>
-      <c r="E32" s="50"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="60">
-        <v>10.1</v>
-      </c>
-      <c r="B33" s="67" t="s">
-        <v>170</v>
-      </c>
-      <c r="C33" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="63">
+      <c r="D59" s="62">
+        <v>2</v>
+      </c>
+      <c r="E59" s="49"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="49"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="59">
+        <v>16</v>
+      </c>
+      <c r="B60" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="C60" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="62">
+        <v>3</v>
+      </c>
+      <c r="E60" s="49"/>
+      <c r="F60" s="58"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="49"/>
+      <c r="J60" s="49"/>
+      <c r="K60" s="49"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="59">
+        <v>16</v>
+      </c>
+      <c r="B61" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="62">
+        <v>2</v>
+      </c>
+      <c r="E61" s="49"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="49"/>
+      <c r="J61" s="49"/>
+      <c r="K61" s="49"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="59">
+        <v>16</v>
+      </c>
+      <c r="B62" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" s="62">
         <v>10</v>
       </c>
-      <c r="E33" s="50"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="50"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="60">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="B34" s="67" t="s">
-        <v>171</v>
-      </c>
-      <c r="C34" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D34" s="64">
-        <v>2</v>
-      </c>
-      <c r="E34" s="50"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="50"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="60">
-        <v>11.1</v>
-      </c>
-      <c r="B35" s="67" t="s">
-        <v>172</v>
-      </c>
-      <c r="C35" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="63">
-        <v>10</v>
-      </c>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="50"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="60">
-        <v>11.2</v>
-      </c>
-      <c r="B36" s="67" t="s">
-        <v>173</v>
-      </c>
-      <c r="C36" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D36" s="64">
-        <v>2</v>
-      </c>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
-      <c r="K36" s="50"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="60">
-        <v>11.3</v>
-      </c>
-      <c r="B37" s="69" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="63">
-        <v>15</v>
-      </c>
-      <c r="E37" s="50"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="60">
-        <v>12.1</v>
-      </c>
-      <c r="B38" s="67" t="s">
-        <v>174</v>
-      </c>
-      <c r="C38" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="63">
-        <v>10</v>
-      </c>
-      <c r="E38" s="50"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="50"/>
-      <c r="K38" s="50"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="60">
-        <v>12.2</v>
-      </c>
-      <c r="B39" s="67" t="s">
-        <v>175</v>
-      </c>
-      <c r="C39" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D39" s="64">
-        <v>2</v>
-      </c>
-      <c r="E39" s="50"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
-      <c r="K39" s="50"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="60">
-        <v>12.5</v>
-      </c>
-      <c r="B40" s="67" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="73" t="s">
+      <c r="E62" s="49"/>
+      <c r="F62" s="58"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="49"/>
+      <c r="J62" s="49"/>
+      <c r="K62" s="49"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="59">
+        <v>16</v>
+      </c>
+      <c r="B63" s="79" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="63">
-        <v>4</v>
-      </c>
-      <c r="E40" s="50"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="50"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="50"/>
-      <c r="K40" s="50"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="60">
-        <v>12.6</v>
-      </c>
-      <c r="B41" s="69" t="s">
-        <v>124</v>
-      </c>
-      <c r="C41" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="63">
-        <v>15</v>
-      </c>
-      <c r="E41" s="50"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="50"/>
-      <c r="K41" s="50"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="60">
-        <v>12.7</v>
-      </c>
-      <c r="B42" s="67" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="63">
-        <v>15</v>
-      </c>
-      <c r="E42" s="50"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="50"/>
-      <c r="H42" s="50"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
-      <c r="K42" s="50"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="60">
-        <v>13.1</v>
-      </c>
-      <c r="B43" s="67" t="s">
-        <v>176</v>
-      </c>
-      <c r="C43" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" s="63">
-        <v>10</v>
-      </c>
-      <c r="E43" s="50"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="50"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="60">
-        <v>13.2</v>
-      </c>
-      <c r="B44" s="67" t="s">
-        <v>177</v>
-      </c>
-      <c r="C44" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D44" s="64">
-        <v>2</v>
-      </c>
-      <c r="E44" s="50"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="50"/>
-      <c r="K44" s="50"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="60">
-        <v>13.5</v>
-      </c>
-      <c r="B45" s="69" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="63">
-        <v>15</v>
-      </c>
-      <c r="E45" s="50"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="50"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="60">
-        <v>14.1</v>
-      </c>
-      <c r="B46" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="C46" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="63">
-        <v>4</v>
-      </c>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="60">
-        <v>14.1</v>
-      </c>
-      <c r="B47" s="67" t="s">
-        <v>150</v>
-      </c>
-      <c r="C47" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47" s="63">
-        <v>4</v>
-      </c>
-      <c r="E47" s="50"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="50"/>
-      <c r="H47" s="50"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="50"/>
-      <c r="K47" s="50"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="60">
-        <v>14.1</v>
-      </c>
-      <c r="B48" s="67" t="s">
-        <v>178</v>
-      </c>
-      <c r="C48" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D48" s="63">
-        <v>10</v>
-      </c>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
-      <c r="K48" s="50"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="60">
-        <v>14.2</v>
-      </c>
-      <c r="B49" s="67" t="s">
-        <v>149</v>
-      </c>
-      <c r="C49" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="63">
-        <v>15</v>
-      </c>
-      <c r="E49" s="50"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
-      <c r="K49" s="50"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="60">
-        <v>14.2</v>
-      </c>
-      <c r="B50" s="67" t="s">
-        <v>151</v>
-      </c>
-      <c r="C50" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="63">
-        <v>15</v>
-      </c>
-      <c r="E50" s="50"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="50"/>
-      <c r="K50" s="50"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="60">
-        <v>14.2</v>
-      </c>
-      <c r="B51" s="67" t="s">
-        <v>179</v>
-      </c>
-      <c r="C51" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D51" s="64">
-        <v>2</v>
-      </c>
-      <c r="E51" s="50"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="50"/>
-      <c r="K51" s="50"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="60">
-        <v>15.1</v>
-      </c>
-      <c r="B52" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="63">
-        <v>4</v>
-      </c>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="50"/>
-      <c r="I52" s="50"/>
-      <c r="J52" s="50"/>
-      <c r="K52" s="50"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="60">
-        <v>15.1</v>
-      </c>
-      <c r="B53" s="67" t="s">
-        <v>180</v>
-      </c>
-      <c r="C53" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="D53" s="63">
-        <v>10</v>
-      </c>
-      <c r="E53" s="50"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="50"/>
-      <c r="H53" s="50"/>
-      <c r="I53" s="50"/>
-      <c r="J53" s="50"/>
-      <c r="K53" s="50"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="60">
-        <v>15.2</v>
-      </c>
-      <c r="B54" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="C54" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="63">
-        <v>10</v>
-      </c>
-      <c r="E54" s="50"/>
-      <c r="F54" s="59"/>
-      <c r="G54" s="50"/>
-      <c r="H54" s="50"/>
-      <c r="I54" s="50"/>
-      <c r="J54" s="50"/>
-      <c r="K54" s="50"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="60">
-        <v>15.2</v>
-      </c>
-      <c r="B55" s="67" t="s">
-        <v>181</v>
-      </c>
-      <c r="C55" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D55" s="64">
-        <v>2</v>
-      </c>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="50"/>
-      <c r="I55" s="50"/>
-      <c r="J55" s="50"/>
-      <c r="K55" s="50"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="60">
-        <v>16</v>
-      </c>
-      <c r="B56" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="63">
-        <v>5</v>
-      </c>
-      <c r="E56" s="50"/>
-      <c r="F56" s="59"/>
-      <c r="G56" s="50"/>
-      <c r="H56" s="50"/>
-      <c r="I56" s="50"/>
-      <c r="J56" s="50"/>
-      <c r="K56" s="50"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="60">
-        <v>16</v>
-      </c>
-      <c r="B57" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="63">
-        <v>10</v>
-      </c>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="50"/>
-      <c r="I57" s="50"/>
-      <c r="J57" s="50"/>
-      <c r="K57" s="50"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="60">
-        <v>16</v>
-      </c>
-      <c r="B58" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="76" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58" s="63">
-        <v>50</v>
-      </c>
-      <c r="E58" s="50"/>
-      <c r="F58" s="59"/>
-      <c r="G58" s="50"/>
-      <c r="H58" s="50"/>
-      <c r="I58" s="50"/>
-      <c r="J58" s="50"/>
-      <c r="K58" s="50"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="60">
-        <v>16</v>
-      </c>
-      <c r="B59" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="D59" s="63">
-        <v>2</v>
-      </c>
-      <c r="E59" s="50"/>
-      <c r="F59" s="59"/>
-      <c r="G59" s="50"/>
-      <c r="H59" s="50"/>
-      <c r="I59" s="50"/>
-      <c r="J59" s="50"/>
-      <c r="K59" s="50"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="60">
-        <v>16</v>
-      </c>
-      <c r="B60" s="67" t="s">
-        <v>141</v>
-      </c>
-      <c r="C60" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" s="63">
-        <v>3</v>
-      </c>
-      <c r="E60" s="50"/>
-      <c r="F60" s="59"/>
-      <c r="G60" s="50"/>
-      <c r="H60" s="50"/>
-      <c r="I60" s="50"/>
-      <c r="J60" s="50"/>
-      <c r="K60" s="50"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="60">
-        <v>16</v>
-      </c>
-      <c r="B61" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="C61" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="63">
-        <v>2</v>
-      </c>
-      <c r="E61" s="50"/>
-      <c r="F61" s="59"/>
-      <c r="G61" s="50"/>
-      <c r="H61" s="50"/>
-      <c r="I61" s="50"/>
-      <c r="J61" s="50"/>
-      <c r="K61" s="50"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="60">
-        <v>16</v>
-      </c>
-      <c r="B62" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="63">
-        <v>10</v>
-      </c>
-      <c r="E62" s="50"/>
-      <c r="F62" s="59"/>
-      <c r="G62" s="50"/>
-      <c r="H62" s="50"/>
-      <c r="I62" s="50"/>
-      <c r="J62" s="50"/>
-      <c r="K62" s="50"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="60">
-        <v>16</v>
-      </c>
-      <c r="B63" s="80" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" s="63">
+      <c r="D63" s="62">
         <v>6</v>
       </c>
-      <c r="E63" s="50"/>
-      <c r="F63" s="59"/>
-      <c r="G63" s="50"/>
-      <c r="H63" s="50"/>
-      <c r="I63" s="50"/>
-      <c r="J63" s="50"/>
-      <c r="K63" s="50"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="58"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
+      <c r="J63" s="49"/>
+      <c r="K63" s="49"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E64" s="50"/>
-      <c r="F64" s="50"/>
-      <c r="G64" s="50"/>
-      <c r="H64" s="50"/>
-      <c r="I64" s="50"/>
-      <c r="J64" s="50"/>
-      <c r="K64" s="50"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="49"/>
+      <c r="J64" s="49"/>
+      <c r="K64" s="49"/>
     </row>
     <row r="65" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="8"/>
-      <c r="E65" s="51"/>
-      <c r="F65" s="51"/>
-      <c r="G65" s="50"/>
-      <c r="H65" s="50"/>
-      <c r="I65" s="50"/>
-      <c r="J65" s="50"/>
-      <c r="K65" s="50"/>
+      <c r="E65" s="50"/>
+      <c r="F65" s="50"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="49"/>
+      <c r="I65" s="49"/>
+      <c r="J65" s="49"/>
+      <c r="K65" s="49"/>
       <c r="L65" s="4"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="4"/>
@@ -5265,13 +5289,13 @@
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="8"/>
-      <c r="E66" s="50"/>
-      <c r="F66" s="59"/>
-      <c r="G66" s="50"/>
-      <c r="H66" s="50"/>
-      <c r="I66" s="50"/>
-      <c r="J66" s="50"/>
-      <c r="K66" s="50"/>
+      <c r="E66" s="49"/>
+      <c r="F66" s="58"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="49"/>
+      <c r="I66" s="49"/>
+      <c r="J66" s="49"/>
+      <c r="K66" s="49"/>
       <c r="L66" s="4"/>
       <c r="P66" s="4"/>
       <c r="Q66" s="4"/>
@@ -5292,10 +5316,10 @@
       <c r="E67" s="23"/>
       <c r="F67" s="23"/>
       <c r="G67" s="23"/>
-      <c r="H67" s="50"/>
-      <c r="I67" s="50"/>
-      <c r="J67" s="50"/>
-      <c r="K67" s="50"/>
+      <c r="H67" s="49"/>
+      <c r="I67" s="49"/>
+      <c r="J67" s="49"/>
+      <c r="K67" s="49"/>
       <c r="L67" s="4"/>
       <c r="P67" s="4"/>
       <c r="Q67" s="4"/>
@@ -5593,7 +5617,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D78">
     <sortCondition ref="A2:A78"/>
   </sortState>
-  <phoneticPr fontId="34" type="noConversion"/>
+  <phoneticPr fontId="35" type="noConversion"/>
   <conditionalFormatting sqref="R2:R8">
     <cfRule type="dataBar" priority="8">
       <dataBar>

</xml_diff>

<commit_message>
add up to wk10 quiz
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DFFE33-32AB-406F-BB96-E84A93ED6EA7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E47551-EEBD-4EBC-B701-4298059F0048}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="293">
   <si>
     <t>Finals Week</t>
   </si>
@@ -160,12 +160,6 @@
     <t>Conducting Inference using R
 Bivariate inference: T-tests
 Bivariate inference: ANOVA</t>
-  </si>
-  <si>
-    <t>Learn more about your topic area by conducting a literature review. 
-What is already known, what questions have not yet been explored? 
-The idea is to find an area where you can contribute to new research. 
-You will learn how to conduct a literature review without burning yourself out or getting lost</t>
   </si>
   <si>
     <t>Bivariate inference: Chi-squared
@@ -201,11 +195,6 @@
 Conduct and interpret an ANOVA</t>
   </si>
   <si>
-    <t>Read CN 6.2 &amp; 6.3 before Monday
-Read the instructions for the Bivariate inference assignment
-Watch the PDS video on ANOVA and read CN 6.4 before Friday</t>
-  </si>
-  <si>
     <t>Conduct and interpret a chi-squared test of association
 Calculate a linear regression equation and interpret the coefficients
 Conduct and interpret a test of correlation</t>
@@ -339,12 +328,6 @@
     <t>ANOVA</t>
   </si>
   <si>
-    <t>Chi-squared</t>
-  </si>
-  <si>
-    <t>Correlation</t>
-  </si>
-  <si>
     <t>Moderation</t>
   </si>
   <si>
@@ -357,12 +340,6 @@
     <t>Explanatory vs Response</t>
   </si>
   <si>
-    <t>Logistic Regression</t>
-  </si>
-  <si>
-    <t>T-test</t>
-  </si>
-  <si>
     <t>Order</t>
   </si>
   <si>
@@ -372,9 +349,6 @@
     <t>Probability Distributions</t>
   </si>
   <si>
-    <t>Regression</t>
-  </si>
-  <si>
     <t>[1](https://www.youtube.com/watch?v=_8A0zx51BKs)</t>
   </si>
   <si>
@@ -423,28 +397,10 @@
     <t>[14 (20-37min)](https://passiondrivenstatistics.com/2016/10/06/r-chapter-17/)</t>
   </si>
   <si>
-    <t>[8 (14 min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)</t>
-  </si>
-  <si>
-    <t>[8 (16 min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)</t>
-  </si>
-  <si>
-    <t>Multiple Regression</t>
-  </si>
-  <si>
     <t>Confounding</t>
   </si>
   <si>
     <t>[14 (39min)](https://passiondrivenstatistics.com/2016/10/06/r-chapter-17/)</t>
-  </si>
-  <si>
-    <t>[2 (7 min)](https://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)</t>
-  </si>
-  <si>
-    <t>[2 (12 min)](https://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)</t>
-  </si>
-  <si>
-    <t>[14 (42 min)](https://passiondrivenstatistics.com/2016/10/06/r-chapter-17/)</t>
   </si>
   <si>
     <t>Course
@@ -488,9 +444,6 @@
   </si>
   <si>
     <t>Data architecture and codebooks</t>
-  </si>
-  <si>
-    <t>Graphing relationships</t>
   </si>
   <si>
     <t>[Notes](lecture/lec02_writing_empirical_research.html)</t>
@@ -853,47 +806,16 @@
     <t>[hw05_biv_graphing](hw/hw05_biv_graphing.html) (Due 9/28 )</t>
   </si>
   <si>
-    <t>Quiz 6 (Due 9/29 ) 
-[Sec 01]()
-[Sec 02]()</t>
-  </si>
-  <si>
     <t>[hw06 research proposal outline](hw/hw06_research_proposal_outline.html)(Due 10/12 )</t>
   </si>
   <si>
-    <t xml:space="preserve">(In class exam 10/4 )  [Sample exam](reading/sample_exam_1.pdf) available. </t>
-  </si>
-  <si>
-    <t>[Evaluation Form](https://forms.gle/Vrhf9FEqwiWYPD4N9) (Due x/xx )</t>
-  </si>
-  <si>
     <t>Poster prep Stage II* (Draft Due 10/01, PR 10/03, Final 10/05 )</t>
   </si>
   <si>
-    <t>Quiz 7 (Due 10/06 ) 
-[Sec 01]()
-[Sec 02]()</t>
-  </si>
-  <si>
-    <t>Quiz 8 (Due 10/13 ) 
-[Sec 01]()
-[Sec 02]()</t>
-  </si>
-  <si>
     <t>[hw07_foundations](hw/hw07_foundations.html) (Due 10/19 )</t>
   </si>
   <si>
-    <t>Quiz 9 (Due 10/20 ) 
-[Sec 01]()
-[Sec 02]()</t>
-  </si>
-  <si>
     <t>[hw08_biv_inference](hw/hw08_biv_inference.html) (Due 11/02 )</t>
-  </si>
-  <si>
-    <t>Quiz 10 (Due 10/27 ) 
-[Sec 01]()
-[Sec 02]()</t>
   </si>
   <si>
     <t>Quiz 11 (Due 11/03 ) 
@@ -955,41 +877,6 @@
 Download your research data and codebook into your `project/data` folder
 Start a code file called `dm.Rmd`, save into your `project/code` folder
 Watch how an expert codes: https://www.youtube.com/watch?v=go5Au01Jrvs (hint: it's not as seamless as you may think)</t>
-  </si>
-  <si>
-    <t>Learn how to use R to do and turn in homework (test markdown file, hw1 template)
-Set up an organized class folder
-Familiarize yourself with class resources on how to learn R.  (PDS Videos, textbook(s), Course Notes, Math 130, R-help page on clas website)</t>
-  </si>
-  <si>
-    <t>Watch PDS Video 2 and 3
-Optional but helpful: [Video on developing a research topic that interests you](https://media.csuchico.edu/media/Developing+a+Research+Question+that+Interests+You/0_rxvxwbas)
-Read: How to read a journal article
-Read:Conducting a literature review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Familiarize yourself with the course website organization and bookmark this site. 
-Join the Slack workspace and post an introduction
-Acquire course materials - [Open Intro textbook](https://www.openintro.org/stat/textbook.php?stat_book=os), [Course notes packet](http://www.chicopacketpro.com/item/math-course-notes-donatello)
-Install R, R Studio and associated packages using the [[Math 130 lesson notes]](https://norcalbiostat.github.io/MATH130/notes/02_setup.html) 
-If using R Studio Cloud - make an account, join our workspace (posted in Slack), click the "New Project" button and replace "Untitled Project" with your name (first and last)
-Watch PDS video 1
-Read: Learning - your first job
-Read: MAI and academic achievement
-Look through the [[research data available]](https://drive.google.com/drive/u/3/folders/1jULudBjRbHdW-uLIvmMbxRBEJJkq9crY) and pick a data set that you want to work with. 
-Identify a research area and a partner to work with. Partner (optional).
-Schedule a time outside of class to work with your analysis partner on a weekly basis. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to the instructor, class structure, materials, requirements, expectations and resources. 
-Materials Overview [document](reading/Materials overview for Math 315.pdf) and [video]()
-Blackboard usage (grading)
-Online materials (google drive, website)
-Physical materials (course notes, textbook)
-New tools (Slack, R, R Studio, R Studio cloud)
-Learning Techniques (metacognition, quizzes, error assessments, peer reviews)
-Support structures (tutoring, community coding, Slack, Peer mentors, OH, Math 130)
-</t>
   </si>
   <si>
     <t>Quiz 1 (Due 8/29 ) 
@@ -1083,10 +970,6 @@
 Define sampling distributions, and standard errors</t>
   </si>
   <si>
-    <t>Midterm
-Self and peer evaluation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Go through a full 5 step hypothesis. </t>
   </si>
   <si>
@@ -1125,6 +1008,123 @@
     <t>Quiz 5 (Due 9/22 ) 
 [[Sec 01]](https://forms.gle/Jo4gqJ4baNV2d4M68)
 [[Sec 02]](https://forms.gle/tdK2MXM8V56CC3su7)</t>
+  </si>
+  <si>
+    <t>Quiz 6 (Due 9/29 ) 
+[[Sec 01]](https://forms.gle/ZWbdQbiRxNB9USCu9)
+[[Sec 02]](https://forms.gle/AsYjcqujuDr6Ekwy6)</t>
+  </si>
+  <si>
+    <t>[Evaluation Form](https://forms.gle/5AM55AUCuFFkqHRL7) (Due 10/05 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midterm
+</t>
+  </si>
+  <si>
+    <t>Self and peer evaluation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In class exam on Friday. [Sample exam](reading/sample_exam_1.pdf) available. </t>
+  </si>
+  <si>
+    <t>Introduction to the instructor, class structure, materials, requirements, expectations and resources. 
+Blackboard usage (grading)
+Online materials (google drive, website)
+Physical materials (course notes, textbook)
+New tools (Slack, R, R Studio, R Studio cloud)
+Learning Techniques (metacognition, quizzes, error assessments, peer reviews)
+Support structures (tutoring, community coding, Slack, Peer mentors, OH, Math 130)</t>
+  </si>
+  <si>
+    <t>Watch PDS Video 2 and 3
+Look through the [research data](https://drive.google.com/drive/u/3/folders/1jULudBjRbHdW-uLIvmMbxRBEJJkq9crY) available and pick a data set that you want to work with. 
+Identify a research area and a partner to work with. Partner (optional).
+Schedule a time outside of class to work with your analysis partner on a weekly basis. 
+Optional but helpful: [Video on developing a research topic that interests you](https://media.csuchico.edu/media/Developing+a+Research+Question+that+Interests+You/0_rxvxwbas)
+Read: How to read a journal article
+Read: Conducting a literature review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn more about your topic area by conducting a literature review. 
+What is already known, what questions have not yet been explored? 
+The idea is to find an area where you can contribute to new research. </t>
+  </si>
+  <si>
+    <t>Learn how to use R to do and turn in homework (test markdown file, hw1 template)
+Set up an organized class folder
+Introduction to class resources on how to learn R.  (PDS Videos, textbook(s), Course Notes, Math 130, R-help page on class website)</t>
+  </si>
+  <si>
+    <t>Describing relationships</t>
+  </si>
+  <si>
+    <t>[14 (42min)](https://passiondrivenstatistics.com/2016/10/06/r-chapter-17/)</t>
+  </si>
+  <si>
+    <t>[8 (16min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)</t>
+  </si>
+  <si>
+    <t>[8 (14min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)</t>
+  </si>
+  <si>
+    <t>[2 (7min)](https://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)</t>
+  </si>
+  <si>
+    <t>[2 (12min)](https://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)</t>
+  </si>
+  <si>
+    <t>Familiarize yourself with the required course materials: [ROBIN PUT LINK HERE ]
+Join the Slack workspace and post an introduction
+Install R, R Studio and associated packages onto your computer using the [Math 130 lesson on installing R](https://norcalbiostat.github.io/MATH130/notes/02_setup.html) &lt;b&gt;-OR-&lt;/b&gt;
+If using R Studio Cloud - make an account, join our workspace (posted in Slack), click the "New Project" button and replace "Untitled Project" with your name (first and last)
+Watch [PDS Video 1](https://www.youtube.com/watch?v=_8A0zx51BKs)
+Read: Learning - your first job
+Read: MAI and academic achievement
+Review the [Advice from prior Math 315 students](reading/Advice%20from%20prior%20Math%20315%20students.pdf) (Long, but skim it and you'll see themes)</t>
+  </si>
+  <si>
+    <t>Read CN 6.1-6.3 before Monday
+Read the instructions for the Bivariate inference assignment
+Watch the PDS video on ANOVA and read CN 6.4 before Friday</t>
+  </si>
+  <si>
+    <t>Quiz 7 (Due 10/06 ) 
+[[Sec 01]](https://forms.gle/89RhdsVfaPutrwku5)
+[[Sec 02]](https://forms.gle/TmawJctpFrq4itmn8)</t>
+  </si>
+  <si>
+    <t>Quiz 8 (Due 10/13 ) 
+[[Sec 01]](https://forms.gle/sbEX4x39tJwJdRBh8)
+[[Sec 02]](https://forms.gle/hC7ciiAKmi614Nrw9)</t>
+  </si>
+  <si>
+    <t>T-test analysis</t>
+  </si>
+  <si>
+    <t>Chi-squared analysis</t>
+  </si>
+  <si>
+    <t>Correlation analysis</t>
+  </si>
+  <si>
+    <t>Regression analysis</t>
+  </si>
+  <si>
+    <t>Multiple Regression analysis</t>
+  </si>
+  <si>
+    <t>Logistic Regression analysis</t>
+  </si>
+  <si>
+    <t>Quiz 9 (Due 10/20 ) 
+[[Sec 01]](https://forms.gle/o8dSPooP9b2Ui1qUA)
+[[Sec 02]](https://forms.gle/vXuuJcKARFTx7W8z6)</t>
+  </si>
+  <si>
+    <t>Quiz 10 (Due 10/27 ) 
+[[Sec 01]](https://forms.gle/CPMywhKBnM8fHiD96)
+[[Sec 02]](https://forms.gle/QEUMGXgyTdoBJKnL8)</t>
   </si>
 </sst>
 </file>
@@ -1134,9 +1134,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1553,111 +1560,111 @@
   </borders>
   <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="77" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="78" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="78" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="80"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="80" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="80"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="80" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="80" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="80" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="81" applyFont="1" applyAlignment="1">
@@ -1672,10 +1679,10 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="24" fillId="5" borderId="3" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="25" fillId="5" borderId="3" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="6" borderId="3" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1684,158 +1691,158 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="3" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="80" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="80" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="80" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="4" xfId="82" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="4" xfId="82" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="4" xfId="82" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="4" xfId="82" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="80" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="82"/>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="80" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="80" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="80" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="80" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="80" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1857,7 +1864,7 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1872,13 +1879,13 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1888,23 +1895,26 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2329,8 +2339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2339,32 +2349,32 @@
     <col min="3" max="3" width="0" style="35" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.375" style="42" customWidth="1"/>
-    <col min="6" max="6" width="13.875" style="35" customWidth="1"/>
+    <col min="6" max="6" width="11.25" style="35" customWidth="1"/>
     <col min="7" max="7" width="16.875" style="93" customWidth="1"/>
     <col min="8" max="8" width="79.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="35" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="G1" s="92" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H1" s="48" t="s">
         <v>6</v>
@@ -2378,16 +2388,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G2" s="100" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="H2" s="101" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2395,7 +2405,7 @@
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2403,10 +2413,10 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2414,13 +2424,13 @@
         <v>1.4</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2428,7 +2438,7 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E6" s="43"/>
       <c r="F6" s="35">
@@ -2443,19 +2453,19 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="E7" s="42" t="s">
-        <v>111</v>
+        <v>279</v>
       </c>
       <c r="F7" s="35">
         <v>1.3</v>
       </c>
       <c r="G7" s="100" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="H7" s="101" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2463,10 +2473,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>112</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2474,7 +2484,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D9" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2482,10 +2492,10 @@
         <v>2.4</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2497,17 +2507,17 @@
       </c>
       <c r="C11" s="36"/>
       <c r="D11" s="37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F11" s="36"/>
       <c r="G11" s="104" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="H11" s="101" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2515,10 +2525,10 @@
         <v>3.2</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F12" s="35">
         <v>1.4</v>
@@ -2530,7 +2540,7 @@
         <v>3.3</v>
       </c>
       <c r="D13" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="H13" s="82"/>
     </row>
@@ -2542,19 +2552,19 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="E14" s="42" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F14" s="35">
         <v>2.1</v>
       </c>
       <c r="G14" s="104" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="H14" s="101" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2562,13 +2572,13 @@
         <v>4.2</v>
       </c>
       <c r="D15" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2576,13 +2586,13 @@
         <v>4.3</v>
       </c>
       <c r="D16" s="83" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="E16" s="84"/>
       <c r="F16" s="85"/>
       <c r="G16" s="94"/>
       <c r="H16" s="83" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2593,19 +2603,19 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>275</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="G17" s="104" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="H17" s="101" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2613,11 +2623,13 @@
         <v>5.2</v>
       </c>
       <c r="D18" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="F18" s="38"/>
-    </row>
-    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G18" s="104"/>
+      <c r="H18" s="101"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>6.1</v>
       </c>
@@ -2625,16 +2637,16 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="G19" s="102" t="s">
-        <v>231</v>
+        <v>115</v>
+      </c>
+      <c r="G19" s="104" t="s">
+        <v>266</v>
       </c>
       <c r="H19" s="108" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2642,10 +2654,10 @@
         <v>6.2</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F20" s="35">
         <v>3</v>
@@ -2656,13 +2668,13 @@
         <v>6.3</v>
       </c>
       <c r="D21" s="86" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E21" s="87"/>
       <c r="F21" s="88"/>
       <c r="G21" s="95"/>
       <c r="H21" s="86" t="s">
-        <v>233</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2670,10 +2682,10 @@
         <v>6.4</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>234</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2681,16 +2693,16 @@
         <v>6.5</v>
       </c>
       <c r="D23" s="83" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="E23" s="84"/>
       <c r="F23" s="85"/>
       <c r="G23" s="94"/>
       <c r="H23" s="83" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
         <v>7.1</v>
       </c>
@@ -2698,16 +2710,16 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>106</v>
+        <v>278</v>
       </c>
       <c r="F24" s="35">
         <v>4</v>
       </c>
-      <c r="G24" s="102" t="s">
-        <v>236</v>
+      <c r="G24" s="104" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2715,10 +2727,10 @@
         <v>7.2</v>
       </c>
       <c r="D25" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2726,13 +2738,13 @@
         <v>7.3</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F26" s="35">
         <v>4.5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>8.1</v>
       </c>
@@ -2740,16 +2752,16 @@
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="F27" s="35">
         <v>4.7</v>
       </c>
-      <c r="G27" s="102" t="s">
-        <v>237</v>
+      <c r="G27" s="104" t="s">
+        <v>284</v>
       </c>
       <c r="H27" s="81" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2757,13 +2769,13 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>107</v>
+        <v>277</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2771,13 +2783,13 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>285</v>
       </c>
       <c r="F29" s="35">
         <v>6.1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="40">
         <v>9.1</v>
       </c>
@@ -2785,19 +2797,19 @@
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E30" s="42" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F30" s="35">
         <v>6.2</v>
       </c>
-      <c r="G30" s="102" t="s">
-        <v>239</v>
-      </c>
-      <c r="H30" s="81" t="s">
-        <v>240</v>
+      <c r="G30" s="104" t="s">
+        <v>291</v>
+      </c>
+      <c r="H30" s="101" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2805,10 +2817,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>286</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F31" s="35">
         <v>6.3</v>
@@ -2819,16 +2831,16 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>287</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F32" s="35">
         <v>6.4</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
         <v>10.1</v>
       </c>
@@ -2836,16 +2848,16 @@
         <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>89</v>
+        <v>288</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F33" s="35">
         <v>6.5</v>
       </c>
-      <c r="G33" s="102" t="s">
-        <v>241</v>
+      <c r="G33" s="104" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -2856,19 +2868,19 @@
         <v>11</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F34" s="35">
         <v>7</v>
       </c>
       <c r="G34" s="102" t="s">
-        <v>242</v>
-      </c>
-      <c r="H34" s="81" t="s">
-        <v>243</v>
+        <v>221</v>
+      </c>
+      <c r="H34" s="101" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2876,10 +2888,10 @@
         <v>11.2</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F35" s="35">
         <v>8.1</v>
@@ -2890,10 +2902,10 @@
         <v>11.3</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -2904,19 +2916,19 @@
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>108</v>
+        <v>289</v>
       </c>
       <c r="E37" s="42" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="G37" s="102" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="H37" s="81" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2924,13 +2936,13 @@
         <v>12.2</v>
       </c>
       <c r="D38" s="83" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="E38" s="84"/>
       <c r="F38" s="85"/>
       <c r="G38" s="94"/>
       <c r="H38" s="83" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -2941,16 +2953,16 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>290</v>
       </c>
       <c r="E39" s="42" t="s">
-        <v>113</v>
+        <v>276</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="G39" s="102" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2958,10 +2970,10 @@
         <v>13.2</v>
       </c>
       <c r="D40" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2969,7 +2981,7 @@
         <v>14</v>
       </c>
       <c r="D41" s="89" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="E41" s="90"/>
       <c r="F41" s="91"/>
@@ -2984,13 +2996,13 @@
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="F42" s="38">
         <v>8.4</v>
       </c>
       <c r="G42" s="102" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2998,13 +3010,13 @@
         <v>15.2</v>
       </c>
       <c r="D43" s="83" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="E43" s="84"/>
       <c r="F43" s="85"/>
       <c r="G43" s="94"/>
       <c r="H43" s="83" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -3015,16 +3027,16 @@
         <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E44" s="42" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G44" s="102" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="H44" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3032,10 +3044,10 @@
         <v>17.100000000000001</v>
       </c>
       <c r="D45" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="H45" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3046,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3063,8 +3075,8 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3109,7 +3121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="270" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="106">
         <v>1</v>
       </c>
@@ -3117,28 +3129,28 @@
         <v>42241</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>259</v>
+        <v>281</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="106">
         <v>2</v>
       </c>
@@ -3147,25 +3159,25 @@
         <v>42248</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>38</v>
+        <v>273</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="J3" s="30"/>
     </row>
@@ -3178,25 +3190,25 @@
         <v>42255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -3208,25 +3220,25 @@
         <v>42262</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3238,29 +3250,29 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="A7" s="106">
         <v>6</v>
       </c>
       <c r="B7" s="29">
@@ -3268,27 +3280,29 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="I7" s="1"/>
+        <v>268</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A8" s="28">
+      <c r="A8" s="106">
         <v>7</v>
       </c>
       <c r="B8" s="29">
@@ -3299,22 +3313,22 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>282</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3329,16 +3343,16 @@
         <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>282</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="21" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3350,22 +3364,22 @@
         <v>42297</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3377,22 +3391,22 @@
         <v>42304</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3404,19 +3418,19 @@
         <v>42311</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -3429,18 +3443,18 @@
         <v>42318</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="1" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3452,19 +3466,19 @@
         <v>42325</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H14" s="27"/>
     </row>
@@ -3475,7 +3489,7 @@
         <v>42332</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -3492,20 +3506,20 @@
         <v>42339</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3517,10 +3531,10 @@
         <v>42346</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -3536,7 +3550,7 @@
         <v>42353</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3554,8 +3568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD78"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,10 +3605,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2" t="s">
@@ -3668,12 +3682,12 @@
         <v>3</v>
       </c>
       <c r="E2" s="97" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F2" s="50"/>
       <c r="G2" s="50"/>
       <c r="H2" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I2" s="5">
         <f>SUMIF($C$2:$C$69,H2,$D$2:$D$69)-30</f>
@@ -3685,7 +3699,7 @@
       </c>
       <c r="K2" s="50"/>
       <c r="L2" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M2" s="5">
         <v>59.5</v>
@@ -3736,16 +3750,16 @@
         <v>1.2</v>
       </c>
       <c r="B3" s="66" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="C3" s="73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="62">
         <v>10</v>
       </c>
       <c r="E3" s="98" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F3" s="50"/>
       <c r="G3" s="49"/>
@@ -3813,16 +3827,16 @@
         <v>1.2</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C4" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D4" s="63">
         <v>2</v>
       </c>
       <c r="E4" s="99" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="50"/>
@@ -3890,7 +3904,7 @@
         <v>1.4</v>
       </c>
       <c r="B5" s="66" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="C5" s="67" t="s">
         <v>23</v>
@@ -3899,7 +3913,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="99" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F5" s="52"/>
       <c r="G5" s="49"/>
@@ -3960,16 +3974,16 @@
         <v>2.1</v>
       </c>
       <c r="B6" s="66" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" s="62">
         <v>10</v>
       </c>
       <c r="E6" s="99" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F6" s="52"/>
       <c r="G6" s="49"/>
@@ -4037,16 +4051,16 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B7" s="66" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D7" s="63">
         <v>2</v>
       </c>
       <c r="E7" s="99" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -4114,7 +4128,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B8" s="66" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C8" s="69" t="s">
         <v>14</v>
@@ -4123,7 +4137,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="99" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
@@ -4177,7 +4191,7 @@
         <v>2.4</v>
       </c>
       <c r="B9" s="71" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C9" s="72" t="s">
         <v>12</v>
@@ -4213,16 +4227,16 @@
         <v>3.1</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="62">
         <v>10</v>
       </c>
       <c r="E10" s="103" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F10" s="52"/>
       <c r="G10" s="49"/>
@@ -4236,16 +4250,16 @@
         <v>3.2</v>
       </c>
       <c r="B11" s="66" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D11" s="63">
         <v>2</v>
       </c>
       <c r="E11" s="103" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="49"/>
@@ -4259,7 +4273,7 @@
         <v>3.6</v>
       </c>
       <c r="B12" s="66" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C12" s="74" t="s">
         <v>23</v>
@@ -4268,7 +4282,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="103" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F12" s="50"/>
       <c r="G12" s="49"/>
@@ -4282,16 +4296,16 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B13" s="66" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D13" s="62">
         <v>10</v>
       </c>
       <c r="E13" s="105" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F13" s="50"/>
       <c r="G13" s="49"/>
@@ -4305,16 +4319,16 @@
         <v>4.2</v>
       </c>
       <c r="B14" s="66" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C14" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D14" s="63">
         <v>2</v>
       </c>
       <c r="E14" s="105" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="49"/>
@@ -4330,7 +4344,7 @@
         <v>4.5</v>
       </c>
       <c r="B15" s="66" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C15" s="74" t="s">
         <v>23</v>
@@ -4339,7 +4353,7 @@
         <v>15</v>
       </c>
       <c r="E15" s="105" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F15" s="50"/>
       <c r="G15" s="49"/>
@@ -4355,16 +4369,16 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B16" s="66" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D16" s="62">
         <v>10</v>
       </c>
       <c r="E16" s="105" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F16" s="53"/>
       <c r="G16" s="49"/>
@@ -4380,16 +4394,16 @@
         <v>5.2</v>
       </c>
       <c r="B17" s="66" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D17" s="63">
         <v>2</v>
       </c>
       <c r="E17" s="105" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F17" s="53"/>
       <c r="G17" s="49"/>
@@ -4405,7 +4419,7 @@
         <v>5.3</v>
       </c>
       <c r="B18" s="66" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="C18" s="74" t="s">
         <v>23</v>
@@ -4414,7 +4428,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="105" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="F18" s="53"/>
       <c r="G18" s="49"/>
@@ -4430,7 +4444,7 @@
         <v>6.1</v>
       </c>
       <c r="B19" s="66" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C19" s="75" t="s">
         <v>13</v>
@@ -4453,15 +4467,17 @@
         <v>6.1</v>
       </c>
       <c r="B20" s="66" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C20" s="73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D20" s="62">
         <v>10</v>
       </c>
-      <c r="E20" s="49"/>
+      <c r="E20" s="109" t="s">
+        <v>233</v>
+      </c>
       <c r="F20" s="50"/>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
@@ -4476,15 +4492,17 @@
         <v>6.2</v>
       </c>
       <c r="B21" s="66" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D21" s="63">
         <v>2</v>
       </c>
-      <c r="E21" s="49"/>
+      <c r="E21" s="109" t="s">
+        <v>233</v>
+      </c>
       <c r="F21" s="50"/>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
@@ -4496,18 +4514,20 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="59">
-        <v>7.1</v>
-      </c>
-      <c r="B22" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="C22" s="73" t="s">
-        <v>68</v>
+        <v>6.3</v>
+      </c>
+      <c r="B22" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="78" t="s">
+        <v>24</v>
       </c>
       <c r="D22" s="62">
-        <v>10</v>
-      </c>
-      <c r="E22" s="49"/>
+        <v>5</v>
+      </c>
+      <c r="E22" s="109" t="s">
+        <v>233</v>
+      </c>
       <c r="F22" s="55"/>
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
@@ -4517,18 +4537,20 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="59">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="B23" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="C23" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="D23" s="63">
-        <v>2</v>
-      </c>
-      <c r="E23" s="49"/>
+        <v>143</v>
+      </c>
+      <c r="C23" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="62">
+        <v>10</v>
+      </c>
+      <c r="E23" s="109" t="s">
+        <v>233</v>
+      </c>
       <c r="F23" s="56"/>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
@@ -4538,19 +4560,19 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="59">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="B24" s="66" t="s">
-        <v>179</v>
-      </c>
-      <c r="C24" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="62">
-        <v>10</v>
-      </c>
-      <c r="E24" s="107" t="s">
-        <v>254</v>
+        <v>144</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="63">
+        <v>2</v>
+      </c>
+      <c r="E24" s="109" t="s">
+        <v>233</v>
       </c>
       <c r="F24" s="55"/>
       <c r="G24" s="49"/>
@@ -4563,18 +4585,20 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="59">
-        <v>8.1</v>
+        <v>7.3</v>
       </c>
       <c r="B25" s="66" t="s">
-        <v>180</v>
-      </c>
-      <c r="C25" s="77" t="s">
-        <v>23</v>
+        <v>165</v>
+      </c>
+      <c r="C25" s="76" t="s">
+        <v>14</v>
       </c>
       <c r="D25" s="62">
-        <v>15</v>
-      </c>
-      <c r="E25" s="49"/>
+        <v>10</v>
+      </c>
+      <c r="E25" s="107" t="s">
+        <v>233</v>
+      </c>
       <c r="F25" s="56"/>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
@@ -4589,13 +4613,13 @@
         <v>8.1</v>
       </c>
       <c r="B26" s="66" t="s">
-        <v>159</v>
-      </c>
-      <c r="C26" s="73" t="s">
-        <v>68</v>
+        <v>166</v>
+      </c>
+      <c r="C26" s="77" t="s">
+        <v>23</v>
       </c>
       <c r="D26" s="62">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E26" s="49"/>
       <c r="F26" s="50"/>
@@ -4609,18 +4633,20 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="59">
-        <v>8.1999999999999993</v>
+        <v>8.1</v>
       </c>
       <c r="B27" s="66" t="s">
-        <v>160</v>
-      </c>
-      <c r="C27" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="D27" s="63">
-        <v>2</v>
-      </c>
-      <c r="E27" s="49"/>
+        <v>145</v>
+      </c>
+      <c r="C27" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="62">
+        <v>10</v>
+      </c>
+      <c r="E27" s="109" t="s">
+        <v>233</v>
+      </c>
       <c r="F27" s="50"/>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
@@ -4632,18 +4658,20 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="59">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="B28" s="66" t="s">
-        <v>140</v>
-      </c>
-      <c r="C28" s="72" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="62">
-        <v>4</v>
-      </c>
-      <c r="E28" s="49"/>
+        <v>146</v>
+      </c>
+      <c r="C28" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="63">
+        <v>2</v>
+      </c>
+      <c r="E28" s="109" t="s">
+        <v>233</v>
+      </c>
       <c r="F28" s="55"/>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
@@ -4655,16 +4683,16 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="59">
-        <v>8.4</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="B29" s="66" t="s">
-        <v>139</v>
-      </c>
-      <c r="C29" s="61" t="s">
-        <v>14</v>
+        <v>126</v>
+      </c>
+      <c r="C29" s="72" t="s">
+        <v>12</v>
       </c>
       <c r="D29" s="62">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E29" s="49"/>
       <c r="F29" s="56"/>
@@ -4678,16 +4706,16 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="59">
-        <v>9.1</v>
+        <v>8.4</v>
       </c>
       <c r="B30" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="C30" s="73" t="s">
-        <v>68</v>
+        <v>125</v>
+      </c>
+      <c r="C30" s="61" t="s">
+        <v>14</v>
       </c>
       <c r="D30" s="62">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E30" s="49"/>
       <c r="F30" s="50"/>
@@ -4701,16 +4729,16 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="59">
-        <v>9.1999999999999993</v>
+        <v>9.1</v>
       </c>
       <c r="B31" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="C31" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="D31" s="63">
-        <v>2</v>
+        <v>147</v>
+      </c>
+      <c r="C31" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="62">
+        <v>10</v>
       </c>
       <c r="E31" s="49"/>
       <c r="F31" s="50"/>
@@ -4722,16 +4750,16 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="59">
-        <v>9.5</v>
-      </c>
-      <c r="B32" s="68" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" s="78" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="62">
-        <v>5</v>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B32" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="63">
+        <v>2</v>
       </c>
       <c r="E32" s="49"/>
       <c r="F32" s="56"/>
@@ -4746,10 +4774,10 @@
         <v>10.1</v>
       </c>
       <c r="B33" s="66" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C33" s="73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D33" s="62">
         <v>10</v>
@@ -4767,10 +4795,10 @@
         <v>10.199999999999999</v>
       </c>
       <c r="B34" s="66" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C34" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D34" s="63">
         <v>2</v>
@@ -4788,10 +4816,10 @@
         <v>11.1</v>
       </c>
       <c r="B35" s="66" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C35" s="73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D35" s="62">
         <v>10</v>
@@ -4809,10 +4837,10 @@
         <v>11.2</v>
       </c>
       <c r="B36" s="66" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C36" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D36" s="63">
         <v>2</v>
@@ -4830,7 +4858,7 @@
         <v>11.3</v>
       </c>
       <c r="B37" s="68" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C37" s="74" t="s">
         <v>23</v>
@@ -4851,10 +4879,10 @@
         <v>12.1</v>
       </c>
       <c r="B38" s="66" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C38" s="73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D38" s="62">
         <v>10</v>
@@ -4872,10 +4900,10 @@
         <v>12.2</v>
       </c>
       <c r="B39" s="66" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C39" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D39" s="63">
         <v>2</v>
@@ -4893,7 +4921,7 @@
         <v>12.5</v>
       </c>
       <c r="B40" s="66" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C40" s="72" t="s">
         <v>12</v>
@@ -4914,7 +4942,7 @@
         <v>12.6</v>
       </c>
       <c r="B41" s="68" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C41" s="74" t="s">
         <v>23</v>
@@ -4935,7 +4963,7 @@
         <v>12.7</v>
       </c>
       <c r="B42" s="66" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C42" s="61" t="s">
         <v>14</v>
@@ -4956,10 +4984,10 @@
         <v>13.1</v>
       </c>
       <c r="B43" s="66" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C43" s="73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D43" s="62">
         <v>10</v>
@@ -4977,10 +5005,10 @@
         <v>13.2</v>
       </c>
       <c r="B44" s="66" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="C44" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D44" s="63">
         <v>2</v>
@@ -4998,7 +5026,7 @@
         <v>13.5</v>
       </c>
       <c r="B45" s="68" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C45" s="74" t="s">
         <v>23</v>
@@ -5019,7 +5047,7 @@
         <v>14.1</v>
       </c>
       <c r="B46" s="66" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="C46" s="72" t="s">
         <v>12</v>
@@ -5040,7 +5068,7 @@
         <v>14.1</v>
       </c>
       <c r="B47" s="66" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C47" s="72" t="s">
         <v>12</v>
@@ -5061,10 +5089,10 @@
         <v>14.1</v>
       </c>
       <c r="B48" s="66" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C48" s="73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D48" s="62">
         <v>10</v>
@@ -5082,7 +5110,7 @@
         <v>14.2</v>
       </c>
       <c r="B49" s="66" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C49" s="61" t="s">
         <v>14</v>
@@ -5103,7 +5131,7 @@
         <v>14.2</v>
       </c>
       <c r="B50" s="66" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C50" s="61" t="s">
         <v>14</v>
@@ -5124,10 +5152,10 @@
         <v>14.2</v>
       </c>
       <c r="B51" s="66" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C51" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D51" s="63">
         <v>2</v>
@@ -5166,10 +5194,10 @@
         <v>15.1</v>
       </c>
       <c r="B53" s="66" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C53" s="73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D53" s="62">
         <v>10</v>
@@ -5208,10 +5236,10 @@
         <v>15.2</v>
       </c>
       <c r="B55" s="66" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C55" s="65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D55" s="63">
         <v>2</v>
@@ -5313,7 +5341,7 @@
         <v>16</v>
       </c>
       <c r="B60" s="66" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C60" s="72" t="s">
         <v>12</v>
@@ -5376,7 +5404,7 @@
         <v>16</v>
       </c>
       <c r="B63" s="79" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C63" s="72" t="s">
         <v>12</v>
@@ -5754,10 +5782,10 @@
       <c r="Z78" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D78">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E78">
     <sortCondition ref="A2:A78"/>
   </sortState>
-  <phoneticPr fontId="37" type="noConversion"/>
+  <phoneticPr fontId="38" type="noConversion"/>
   <conditionalFormatting sqref="R2:R8">
     <cfRule type="dataBar" priority="8">
       <dataBar>

</xml_diff>

<commit_message>
add all the thigns
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B6E2F6-5423-4CE2-AA6C-EEA63FF9FB0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDF07B5-C6E3-4ADB-B47B-72DCCB3AEE9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="1095" windowWidth="24000" windowHeight="12915" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="297">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1001,27 +1001,130 @@
 The idea is to find an area where you can contribute to new research. </t>
   </si>
   <si>
-    <t>Learn how to use R to do and turn in homework (test markdown file, hw1 template)
+    <t>Describing relationships</t>
+  </si>
+  <si>
+    <t>[14 (42min)](https://passiondrivenstatistics.com/2016/10/06/r-chapter-17/)</t>
+  </si>
+  <si>
+    <t>[8 (16min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)</t>
+  </si>
+  <si>
+    <t>[8 (14min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)</t>
+  </si>
+  <si>
+    <t>[2 (7min)](https://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)</t>
+  </si>
+  <si>
+    <t>[2 (12min)](https://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)</t>
+  </si>
+  <si>
+    <t>Read CN 6.1-6.3 before Monday
+Read the instructions for the Bivariate inference assignment
+Watch the PDS video on ANOVA and read CN 6.4 before Friday</t>
+  </si>
+  <si>
+    <t>T-test analysis</t>
+  </si>
+  <si>
+    <t>Chi-squared analysis</t>
+  </si>
+  <si>
+    <t>Correlation analysis</t>
+  </si>
+  <si>
+    <t>Regression analysis</t>
+  </si>
+  <si>
+    <t>Multiple Regression analysis</t>
+  </si>
+  <si>
+    <t>Logistic Regression analysis</t>
+  </si>
+  <si>
+    <t>Quiz 10 (Due 10/27 ) 
+[[Sec 01]](https://forms.gle/CPMywhKBnM8fHiD96)
+[[Sec 02]](https://forms.gle/QEUMGXgyTdoBJKnL8)</t>
+  </si>
+  <si>
+    <t>Study design</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>Quiz 13 (Due 11/17 ) 
+[[Sec 01]](https://forms.gle/TZSWziSqpk4yFBTb6)
+[[Sec 02]](https://forms.gle/1LoH1WdvKvSToz8L7)</t>
+  </si>
+  <si>
+    <t>Quiz 11 (Due 11/03 ) 
+[[Sec 01]](https://forms.gle/ENYkP4FwqcvwqmfKA)
+[[Sec 02]](https://forms.gle/QqR4g8WjXnJSh2HX8)</t>
+  </si>
+  <si>
+    <t>Quiz 12 (Due 11/10 ) 
+[[Sec 01]](https://forms.gle/y96Ebhj982kwPHoX6)
+[[Sec 02]](https://forms.gle/dxhYEygUG7WDCYJK9)</t>
+  </si>
+  <si>
+    <t>Quiz 14 (Due 11/14 ) 
+[[Sec 01]](https://forms.gle/BSimfYAa9xuF3D9u7)
+[Sec 02]()</t>
+  </si>
+  <si>
+    <t>Quiz 01 (Due 08/29 ) 
+[[Sec01]](https://forms.gle/4CEBJqDaJ9Y23Ddm8)
+[[Sec02]](https://forms.gle/7zCnaLTe1Hrc6LwD7)</t>
+  </si>
+  <si>
+    <t>Quiz 02 (Due 09/03 ) 
+[[Sec01]](https://forms.gle/46GFpQNGswFxH1YZ6)
+[[Sec02]](https://forms.gle/5VXAvu8sxw6qvG4H7)</t>
+  </si>
+  <si>
+    <t>Quiz 03 (Due 09/08 ) 
+[[Sec 01]](https://forms.gle/ot6kJ2As7WHyrZd47)
+[[Sec 02]](https://forms.gle/TodvxwrZjhb2CRvC8)</t>
+  </si>
+  <si>
+    <t>Quiz 04 (Due 09/15 ) 
+[[Sec 01]](https://forms.gle/k5Kys9VCCec7oTw5A)
+[[Sec 02]](https://forms.gle/cZxx2dMYAejj9AHs5)</t>
+  </si>
+  <si>
+    <t>Quiz 05 (Due 09/22 ) 
+[[Sec 01]](https://forms.gle/Jo4gqJ4baNV2d4M68)
+[[Sec 02]](https://forms.gle/tdK2MXM8V56CC3su7)</t>
+  </si>
+  <si>
+    <t>Quiz 06 (Due 09/29 ) 
+[[Sec 01]](https://forms.gle/ZWbdQbiRxNB9USCu9)
+[[Sec 02]](https://forms.gle/AsYjcqujuDr6Ekwy6)</t>
+  </si>
+  <si>
+    <t>Quiz 07 (Due 10/06 ) 
+[[Sec 01]](https://forms.gle/89RhdsVfaPutrwku5)
+[[Sec 02]](https://forms.gle/TmawJctpFrq4itmn8)</t>
+  </si>
+  <si>
+    <t>Quiz 09 (Due 10/20 ) 
+[[Sec 01]](https://forms.gle/o8dSPooP9b2Ui1qUA)
+[[Sec 02]](https://forms.gle/vXuuJcKARFTx7W8z6)</t>
+  </si>
+  <si>
+    <t>Quiz 08 (Due 10/13 ) 
+[[Sec 01]](https://forms.gle/sbEX4x39tJwJdRBh8)
+[[Sec 02]](https://forms.gle/hC7ciiAKmi614Nrw9)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn how to use R to do and turn in homework (test markdown file, hw1 template)
 Set up an organized class folder
-Introduction to class resources on how to learn R.  (PDS Videos, textbook(s), Course Notes, Math 130, R-help page on class website)</t>
-  </si>
-  <si>
-    <t>Describing relationships</t>
-  </si>
-  <si>
-    <t>[14 (42min)](https://passiondrivenstatistics.com/2016/10/06/r-chapter-17/)</t>
-  </si>
-  <si>
-    <t>[8 (16min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)</t>
-  </si>
-  <si>
-    <t>[8 (14min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)</t>
-  </si>
-  <si>
-    <t>[2 (7min)](https://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)</t>
-  </si>
-  <si>
-    <t>[2 (12min)](https://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)</t>
+Introduction to class resources on how to learn R.  (PDS Videos, textbook(s), Course Notes, Math 130, R-help page on class website)
+321 Binder exercise - Learning how to Learn. </t>
   </si>
   <si>
     <t>Familiarize yourself with the required course materials: [ROBIN PUT LINK HERE ]
@@ -1029,108 +1132,13 @@
 Install R, R Studio and associated packages onto your computer using the [Math 130 lesson on installing R](https://norcalbiostat.github.io/MATH130/notes/02_setup.html) &lt;b&gt;-OR-&lt;/b&gt;
 If using R Studio Cloud - make an account, join our workspace (posted in Slack), click the "New Project" button and replace "Untitled Project" with your name (first and last)
 Watch [PDS Video 1](https://www.youtube.com/watch?v=_8A0zx51BKs)
+Prepare your Learning Journal (before Wed)
 Read: Learning - your first job
 Read: MAI and academic achievement
 Review the [Advice from prior Math 315 students](reading/Advice%20from%20prior%20Math%20315%20students.pdf) (Long, but skim it and you'll see themes)</t>
   </si>
   <si>
-    <t>Read CN 6.1-6.3 before Monday
-Read the instructions for the Bivariate inference assignment
-Watch the PDS video on ANOVA and read CN 6.4 before Friday</t>
-  </si>
-  <si>
-    <t>T-test analysis</t>
-  </si>
-  <si>
-    <t>Chi-squared analysis</t>
-  </si>
-  <si>
-    <t>Correlation analysis</t>
-  </si>
-  <si>
-    <t>Regression analysis</t>
-  </si>
-  <si>
-    <t>Multiple Regression analysis</t>
-  </si>
-  <si>
-    <t>Logistic Regression analysis</t>
-  </si>
-  <si>
-    <t>Quiz 10 (Due 10/27 ) 
-[[Sec 01]](https://forms.gle/CPMywhKBnM8fHiD96)
-[[Sec 02]](https://forms.gle/QEUMGXgyTdoBJKnL8)</t>
-  </si>
-  <si>
-    <t>Study design</t>
-  </si>
-  <si>
-    <t>8.1</t>
-  </si>
-  <si>
-    <t>Quiz 13 (Due 11/17 ) 
-[[Sec 01]](https://forms.gle/TZSWziSqpk4yFBTb6)
-[[Sec 02]](https://forms.gle/1LoH1WdvKvSToz8L7)</t>
-  </si>
-  <si>
-    <t>Quiz 11 (Due 11/03 ) 
-[[Sec 01]](https://forms.gle/ENYkP4FwqcvwqmfKA)
-[[Sec 02]](https://forms.gle/QqR4g8WjXnJSh2HX8)</t>
-  </si>
-  <si>
-    <t>Quiz 12 (Due 11/10 ) 
-[[Sec 01]](https://forms.gle/y96Ebhj982kwPHoX6)
-[[Sec 02]](https://forms.gle/dxhYEygUG7WDCYJK9)</t>
-  </si>
-  <si>
-    <t>Quiz 14 (Due 11/14 ) 
-[[Sec 01]](https://forms.gle/BSimfYAa9xuF3D9u7)
-[Sec 02]()</t>
-  </si>
-  <si>
-    <t>Quiz 01 (Due 08/29 ) 
-[[Sec01]](https://forms.gle/4CEBJqDaJ9Y23Ddm8)
-[[Sec02]](https://forms.gle/7zCnaLTe1Hrc6LwD7)</t>
-  </si>
-  <si>
-    <t>Quiz 02 (Due 09/03 ) 
-[[Sec01]](https://forms.gle/46GFpQNGswFxH1YZ6)
-[[Sec02]](https://forms.gle/5VXAvu8sxw6qvG4H7)</t>
-  </si>
-  <si>
-    <t>Quiz 03 (Due 09/08 ) 
-[[Sec 01]](https://forms.gle/ot6kJ2As7WHyrZd47)
-[[Sec 02]](https://forms.gle/TodvxwrZjhb2CRvC8)</t>
-  </si>
-  <si>
-    <t>Quiz 04 (Due 09/15 ) 
-[[Sec 01]](https://forms.gle/k5Kys9VCCec7oTw5A)
-[[Sec 02]](https://forms.gle/cZxx2dMYAejj9AHs5)</t>
-  </si>
-  <si>
-    <t>Quiz 05 (Due 09/22 ) 
-[[Sec 01]](https://forms.gle/Jo4gqJ4baNV2d4M68)
-[[Sec 02]](https://forms.gle/tdK2MXM8V56CC3su7)</t>
-  </si>
-  <si>
-    <t>Quiz 06 (Due 09/29 ) 
-[[Sec 01]](https://forms.gle/ZWbdQbiRxNB9USCu9)
-[[Sec 02]](https://forms.gle/AsYjcqujuDr6Ekwy6)</t>
-  </si>
-  <si>
-    <t>Quiz 07 (Due 10/06 ) 
-[[Sec 01]](https://forms.gle/89RhdsVfaPutrwku5)
-[[Sec 02]](https://forms.gle/TmawJctpFrq4itmn8)</t>
-  </si>
-  <si>
-    <t>Quiz 09 (Due 10/20 ) 
-[[Sec 01]](https://forms.gle/o8dSPooP9b2Ui1qUA)
-[[Sec 02]](https://forms.gle/vXuuJcKARFTx7W8z6)</t>
-  </si>
-  <si>
-    <t>Quiz 08 (Due 10/13 ) 
-[[Sec 01]](https://forms.gle/sbEX4x39tJwJdRBh8)
-[[Sec 02]](https://forms.gle/hC7ciiAKmi614Nrw9)</t>
+    <t>Thinking about learning</t>
   </si>
 </sst>
 </file>
@@ -1724,12 +1732,12 @@
     <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1739,7 +1747,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="80" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="80" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="80" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1781,12 +1789,12 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="80" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="80" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82"/>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1795,22 +1803,19 @@
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="80" applyBorder="1" applyAlignment="1">
@@ -1825,23 +1830,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1870,54 +1875,57 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2340,10 +2348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2353,7 +2361,7 @@
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.375" style="42" customWidth="1"/>
     <col min="6" max="6" width="11.25" style="35" customWidth="1"/>
-    <col min="7" max="7" width="16.875" style="95" customWidth="1"/>
+    <col min="7" max="7" width="16.875" style="94" customWidth="1"/>
     <col min="8" max="8" width="79.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2376,7 +2384,7 @@
       <c r="F1" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="104" t="s">
+      <c r="G1" s="103" t="s">
         <v>66</v>
       </c>
       <c r="H1" s="48" t="s">
@@ -2396,10 +2404,10 @@
       <c r="F2" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="95" t="s">
-        <v>286</v>
-      </c>
-      <c r="H2" s="96" t="s">
+      <c r="G2" s="94" t="s">
+        <v>284</v>
+      </c>
+      <c r="H2" s="95" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2416,10 +2424,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>83</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2427,13 +2432,10 @@
         <v>1.4</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>196</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>252</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2441,647 +2443,661 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="35">
-        <v>1.2</v>
+        <v>111</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
-        <v>2.1</v>
-      </c>
-      <c r="B7" s="35">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>269</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E7" s="43"/>
       <c r="F7" s="35">
-        <v>1.3</v>
-      </c>
-      <c r="G7" s="95" t="s">
-        <v>287</v>
-      </c>
-      <c r="H7" s="96" t="s">
-        <v>212</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
+      </c>
+      <c r="B8" s="35">
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>270</v>
+        <v>268</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1.3</v>
+      </c>
+      <c r="G8" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="H8" s="95" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D9" t="s">
-        <v>198</v>
+        <v>114</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
         <v>2.4</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E11" s="42" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="41">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="41">
         <v>3.1</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B12" s="36">
         <v>3</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37" t="s">
+      <c r="C12" s="36"/>
+      <c r="D12" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="E12" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="98" t="s">
-        <v>288</v>
-      </c>
-      <c r="H11" s="96" t="s">
+      <c r="F12" s="36"/>
+      <c r="G12" s="97" t="s">
+        <v>286</v>
+      </c>
+      <c r="H12" s="95" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="40">
-        <v>3.2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" s="35">
-        <v>1.4</v>
-      </c>
-      <c r="H12" s="82"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D13" t="s">
-        <v>199</v>
-      </c>
-      <c r="H13" s="82"/>
+        <v>73</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="35">
+        <v>1.4</v>
+      </c>
+      <c r="H13" s="81"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B14" s="35">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="D14" t="s">
-        <v>200</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="35">
-        <v>2.1</v>
-      </c>
-      <c r="G14" s="98" t="s">
-        <v>289</v>
-      </c>
-      <c r="H14" s="96" t="s">
-        <v>214</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="H14" s="81"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B15" s="35">
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="38" t="s">
-        <v>253</v>
+      <c r="F15" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="G15" s="97" t="s">
+        <v>287</v>
+      </c>
+      <c r="H15" s="95" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
-        <v>4.3</v>
-      </c>
-      <c r="D16" s="83" t="s">
-        <v>202</v>
-      </c>
-      <c r="E16" s="84"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="83" t="s">
-        <v>215</v>
+        <v>4.2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>201</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B17" s="35">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>265</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>255</v>
-      </c>
-      <c r="G17" s="98" t="s">
-        <v>290</v>
-      </c>
-      <c r="H17" s="96" t="s">
-        <v>216</v>
+        <v>4.3</v>
+      </c>
+      <c r="D17" s="82" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="83"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="82" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
-        <v>5.2</v>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B18" s="35">
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>203</v>
-      </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="96"/>
+        <v>264</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="G18" s="97" t="s">
+        <v>288</v>
+      </c>
+      <c r="H18" s="95" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
-        <v>6.1</v>
-      </c>
-      <c r="B19" s="35">
-        <v>6</v>
+        <v>5.2</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="G19" s="98" t="s">
-        <v>291</v>
-      </c>
-      <c r="H19" s="102" t="s">
-        <v>217</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="95"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
-        <v>6.2</v>
+        <v>6.1</v>
+      </c>
+      <c r="B20" s="35">
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="35">
-        <v>3</v>
+        <v>115</v>
+      </c>
+      <c r="G20" s="97" t="s">
+        <v>289</v>
+      </c>
+      <c r="H20" s="101" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
-        <v>6.3</v>
-      </c>
-      <c r="D21" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="87"/>
-      <c r="F21" s="88"/>
-      <c r="G21" s="106"/>
-      <c r="H21" s="86" t="s">
-        <v>260</v>
+        <v>6.2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="35">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
-        <v>6.4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>117</v>
-      </c>
-      <c r="H22" t="s">
-        <v>257</v>
+        <v>6.3</v>
+      </c>
+      <c r="D22" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="86"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="85" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
-        <v>6.5</v>
-      </c>
-      <c r="D23" s="83" t="s">
-        <v>204</v>
-      </c>
-      <c r="E23" s="84"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="83" t="s">
-        <v>218</v>
+        <v>6.4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
-        <v>7.1</v>
-      </c>
-      <c r="B24" s="35">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>205</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>268</v>
-      </c>
-      <c r="F24" s="35">
-        <v>4</v>
-      </c>
-      <c r="G24" s="98" t="s">
-        <v>292</v>
+        <v>6.5</v>
+      </c>
+      <c r="D24" s="82" t="s">
+        <v>204</v>
+      </c>
+      <c r="E24" s="83"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="82" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="40">
-        <v>7.2</v>
+        <v>7.1</v>
+      </c>
+      <c r="B25" s="35">
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>206</v>
-      </c>
-      <c r="F25" s="38" t="s">
-        <v>254</v>
+        <v>205</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>267</v>
+      </c>
+      <c r="F25" s="35">
+        <v>4</v>
+      </c>
+      <c r="G25" s="97" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="35">
-        <v>4.5</v>
+        <v>206</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
-        <v>8.1</v>
-      </c>
-      <c r="B27" s="35">
-        <v>8</v>
+        <v>7.3</v>
       </c>
       <c r="D27" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F27" s="35">
-        <v>4.7</v>
-      </c>
-      <c r="G27" s="98" t="s">
-        <v>294</v>
-      </c>
-      <c r="H27" s="81" t="s">
-        <v>219</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
-        <v>8.1999999999999993</v>
+        <v>8.1</v>
+      </c>
+      <c r="B28" s="35">
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="F28" s="35" t="s">
-        <v>235</v>
+        <v>116</v>
+      </c>
+      <c r="F28" s="35">
+        <v>4.7</v>
+      </c>
+      <c r="G28" s="97" t="s">
+        <v>292</v>
+      </c>
+      <c r="H28" s="80" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D29" t="s">
-        <v>273</v>
-      </c>
-      <c r="F29" s="35">
-        <v>6.1</v>
+        <v>74</v>
+      </c>
+      <c r="E29" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="40">
-        <v>9.1</v>
-      </c>
-      <c r="B30" s="35">
-        <v>9</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="42" t="s">
-        <v>91</v>
+        <v>271</v>
       </c>
       <c r="F30" s="35">
-        <v>6.2</v>
-      </c>
-      <c r="G30" s="98" t="s">
-        <v>293</v>
-      </c>
-      <c r="H30" s="96" t="s">
-        <v>220</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
-        <v>9.1999999999999993</v>
+        <v>9.1</v>
+      </c>
+      <c r="B31" s="35">
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>274</v>
+        <v>75</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F31" s="35">
-        <v>6.3</v>
+        <v>6.2</v>
+      </c>
+      <c r="G31" s="97" t="s">
+        <v>291</v>
+      </c>
+      <c r="H31" s="95" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="40">
-        <v>9.3000000000000007</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D32" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F32" s="35">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
-        <v>10.1</v>
-      </c>
-      <c r="B33" s="35">
-        <v>10</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D33" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F33" s="35">
-        <v>6.5</v>
-      </c>
-      <c r="G33" s="98" t="s">
-        <v>279</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
-        <v>11.1</v>
+        <v>10.1</v>
       </c>
       <c r="B34" s="35">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>274</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F34" s="35">
-        <v>7</v>
-      </c>
-      <c r="G34" s="98" t="s">
-        <v>283</v>
-      </c>
-      <c r="H34" s="96" t="s">
-        <v>221</v>
+        <v>6.5</v>
+      </c>
+      <c r="G34" s="97" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
-        <v>11.2</v>
+        <v>11.1</v>
+      </c>
+      <c r="B35" s="35">
+        <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="F35" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35" s="35">
+        <v>7</v>
+      </c>
+      <c r="G35" s="97" t="s">
         <v>281</v>
+      </c>
+      <c r="H35" s="95" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="40">
-        <v>11.3</v>
+        <v>11.2</v>
       </c>
       <c r="D36" t="s">
-        <v>280</v>
+        <v>77</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>96</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>256</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
-        <v>12.1</v>
-      </c>
-      <c r="B37" s="35">
-        <v>12</v>
+        <v>11.3</v>
       </c>
       <c r="D37" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" s="42" t="s">
-        <v>95</v>
+        <v>278</v>
       </c>
       <c r="F37" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="G37" s="98" t="s">
-        <v>284</v>
-      </c>
-      <c r="H37" s="81" t="s">
-        <v>222</v>
-      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
-        <v>12.2</v>
+        <v>12.1</v>
+      </c>
+      <c r="B38" s="35">
+        <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>277</v>
+        <v>99</v>
       </c>
       <c r="E38" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="F38" s="38"/>
+        <v>95</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="G38" s="97" t="s">
+        <v>282</v>
+      </c>
+      <c r="H38" s="80" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
-        <v>12.4</v>
-      </c>
-      <c r="D39" s="83" t="s">
-        <v>207</v>
-      </c>
-      <c r="E39" s="84"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="105"/>
-      <c r="H39" s="83" t="s">
-        <v>223</v>
-      </c>
+        <v>12.2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>275</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="F39" s="38"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="40">
-        <v>13.1</v>
-      </c>
-      <c r="B40" s="35">
-        <v>13</v>
-      </c>
-      <c r="D40" t="s">
-        <v>278</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>266</v>
-      </c>
-      <c r="F40" s="38" t="s">
-        <v>237</v>
-      </c>
-      <c r="G40" s="98" t="s">
-        <v>282</v>
+        <v>12.4</v>
+      </c>
+      <c r="D40" s="82" t="s">
+        <v>207</v>
+      </c>
+      <c r="E40" s="83"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="104"/>
+      <c r="H40" s="82" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="40">
-        <v>13.2</v>
+        <v>13.1</v>
+      </c>
+      <c r="B41" s="35">
+        <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>107</v>
+        <v>276</v>
+      </c>
+      <c r="E41" s="42" t="s">
+        <v>265</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>236</v>
+        <v>237</v>
+      </c>
+      <c r="G41" s="97" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
-        <v>14</v>
-      </c>
-      <c r="D42" s="89" t="s">
-        <v>228</v>
-      </c>
-      <c r="E42" s="90"/>
-      <c r="F42" s="91"/>
-      <c r="G42" s="107"/>
-      <c r="H42" s="89"/>
+        <v>13.2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>107</v>
+      </c>
+      <c r="F42" s="38" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="40">
-        <v>15.1</v>
-      </c>
-      <c r="B43" s="35">
         <v>14</v>
       </c>
-      <c r="D43" t="s">
-        <v>208</v>
-      </c>
-      <c r="F43" s="38">
-        <v>8.4</v>
-      </c>
-      <c r="G43" s="108" t="s">
-        <v>285</v>
-      </c>
+      <c r="D43" s="88" t="s">
+        <v>228</v>
+      </c>
+      <c r="E43" s="89"/>
+      <c r="F43" s="90"/>
+      <c r="G43" s="106"/>
+      <c r="H43" s="88"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
-        <v>15.2</v>
-      </c>
-      <c r="D44" s="83" t="s">
-        <v>209</v>
-      </c>
-      <c r="E44" s="84"/>
-      <c r="F44" s="85"/>
-      <c r="G44" s="105"/>
-      <c r="H44" s="83" t="s">
-        <v>224</v>
+        <v>15.1</v>
+      </c>
+      <c r="B44" s="35">
+        <v>14</v>
+      </c>
+      <c r="D44" t="s">
+        <v>208</v>
+      </c>
+      <c r="F44" s="38">
+        <v>8.4</v>
+      </c>
+      <c r="G44" s="107" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="B45" s="35">
-        <v>15</v>
-      </c>
-      <c r="D45" t="s">
-        <v>210</v>
-      </c>
-      <c r="E45" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="G45" s="108" t="s">
-        <v>225</v>
-      </c>
-      <c r="H45" t="s">
-        <v>226</v>
+        <v>15.2</v>
+      </c>
+      <c r="D45" s="82" t="s">
+        <v>209</v>
+      </c>
+      <c r="E45" s="83"/>
+      <c r="F45" s="84"/>
+      <c r="G45" s="104"/>
+      <c r="H45" s="82" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
-        <v>17.100000000000001</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="B46" s="35">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>210</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" s="107" t="s">
+        <v>225</v>
       </c>
       <c r="H46" t="s">
-        <v>119</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="B47" s="35">
+        <v>16</v>
+      </c>
+      <c r="D47" t="s">
+        <v>102</v>
+      </c>
+      <c r="H47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="40">
         <v>17.2</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>15</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H48" t="s">
         <v>227</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H47">
-    <sortCondition ref="A2:A47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H48">
+    <sortCondition ref="A2:A48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3093,8 +3109,8 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3135,12 +3151,12 @@
       <c r="H1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="80" t="s">
+      <c r="I1" s="79" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A2" s="100">
+      <c r="A2" s="99">
         <v>1</v>
       </c>
       <c r="B2" s="29">
@@ -3153,13 +3169,13 @@
         <v>179</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>271</v>
+        <v>295</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>261</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>264</v>
+        <v>294</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>178</v>
@@ -3169,7 +3185,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="100">
+      <c r="A3" s="99">
         <v>2</v>
       </c>
       <c r="B3" s="29">
@@ -3200,7 +3216,7 @@
       <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" s="100">
+      <c r="A4" s="99">
         <v>3</v>
       </c>
       <c r="B4" s="29">
@@ -3230,7 +3246,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A5" s="100">
+      <c r="A5" s="99">
         <v>4</v>
       </c>
       <c r="B5" s="29">
@@ -3260,7 +3276,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="100">
+      <c r="A6" s="99">
         <v>5</v>
       </c>
       <c r="B6" s="29">
@@ -3290,7 +3306,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="100">
+      <c r="A7" s="99">
         <v>6</v>
       </c>
       <c r="B7" s="29">
@@ -3320,7 +3336,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A8" s="100">
+      <c r="A8" s="99">
         <v>7</v>
       </c>
       <c r="B8" s="29">
@@ -3364,7 +3380,7 @@
         <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -3586,8 +3602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD78"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3699,10 +3715,12 @@
       <c r="D2" s="8">
         <v>3</v>
       </c>
-      <c r="E2" s="92" t="s">
-        <v>229</v>
-      </c>
-      <c r="F2" s="50"/>
+      <c r="E2" s="91" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G2" s="50"/>
       <c r="H2" s="31" t="s">
         <v>66</v>
@@ -3764,22 +3782,24 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="59">
+      <c r="A3" s="58">
         <v>1.2</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="62">
+      <c r="D3" s="61">
         <v>10</v>
       </c>
-      <c r="E3" s="93" t="s">
-        <v>229</v>
-      </c>
-      <c r="F3" s="50"/>
+      <c r="E3" s="92" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G3" s="49"/>
       <c r="H3" s="47" t="s">
         <v>23</v>
@@ -3841,19 +3861,19 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="59">
+      <c r="A4" s="58">
         <v>1.2</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="63">
+      <c r="D4" s="62">
         <v>2</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="93" t="s">
         <v>229</v>
       </c>
       <c r="F4" s="51"/>
@@ -3918,22 +3938,24 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="59">
+      <c r="A5" s="58">
         <v>1.4</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="65" t="s">
         <v>168</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="62">
+      <c r="D5" s="61">
         <v>15</v>
       </c>
-      <c r="E5" s="94" t="s">
-        <v>229</v>
-      </c>
-      <c r="F5" s="52"/>
+      <c r="E5" s="93" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" s="108" t="s">
+        <v>293</v>
+      </c>
       <c r="G5" s="49"/>
       <c r="H5" s="4" t="s">
         <v>12</v>
@@ -3988,22 +4010,24 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="59">
+      <c r="A6" s="58">
         <v>2.1</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="61">
         <v>10</v>
       </c>
-      <c r="E6" s="94" t="s">
-        <v>229</v>
-      </c>
-      <c r="F6" s="52"/>
+      <c r="E6" s="93" t="s">
+        <v>229</v>
+      </c>
+      <c r="F6" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G6" s="49"/>
       <c r="H6" s="4" t="s">
         <v>13</v>
@@ -4065,19 +4089,19 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="59">
+      <c r="A7" s="58">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="63">
+      <c r="D7" s="62">
         <v>2</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="93" t="s">
         <v>229</v>
       </c>
       <c r="F7" s="50"/>
@@ -4142,22 +4166,24 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59">
+      <c r="A8" s="58">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="65" t="s">
         <v>161</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="70">
+      <c r="D8" s="69">
         <v>10</v>
       </c>
-      <c r="E8" s="94" t="s">
-        <v>229</v>
-      </c>
-      <c r="F8" s="50"/>
+      <c r="E8" s="93" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" s="108" t="s">
+        <v>293</v>
+      </c>
       <c r="G8" s="50"/>
       <c r="H8" s="4"/>
       <c r="I8" s="3">
@@ -4205,20 +4231,22 @@
       </c>
     </row>
     <row r="9" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="59">
+      <c r="A9" s="58">
         <v>2.4</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="61">
         <v>4</v>
       </c>
       <c r="E9" s="49"/>
-      <c r="F9" s="50"/>
+      <c r="F9" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G9" s="50"/>
       <c r="H9" s="50"/>
       <c r="I9" s="50"/>
@@ -4241,22 +4269,24 @@
       <c r="AD9" s="5"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59">
+      <c r="A10" s="58">
         <v>3.1</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="62">
+      <c r="D10" s="61">
         <v>10</v>
       </c>
-      <c r="E10" s="97" t="s">
-        <v>229</v>
-      </c>
-      <c r="F10" s="52"/>
+      <c r="E10" s="96" t="s">
+        <v>229</v>
+      </c>
+      <c r="F10" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G10" s="49"/>
       <c r="H10" s="50"/>
       <c r="I10" s="50"/>
@@ -4264,19 +4294,19 @@
       <c r="K10" s="50"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="59">
+      <c r="A11" s="58">
         <v>3.2</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="65" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="62">
         <v>2</v>
       </c>
-      <c r="E11" s="97" t="s">
+      <c r="E11" s="96" t="s">
         <v>229</v>
       </c>
       <c r="F11" s="52"/>
@@ -4287,22 +4317,24 @@
       <c r="K11" s="49"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="59">
+      <c r="A12" s="58">
         <v>3.6</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="65" t="s">
         <v>162</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="C12" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="62">
+      <c r="D12" s="61">
         <v>15</v>
       </c>
-      <c r="E12" s="97" t="s">
-        <v>229</v>
-      </c>
-      <c r="F12" s="50"/>
+      <c r="E12" s="96" t="s">
+        <v>229</v>
+      </c>
+      <c r="F12" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
       <c r="I12" s="49"/>
@@ -4310,22 +4342,24 @@
       <c r="K12" s="49"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="59">
+      <c r="A13" s="58">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="65" t="s">
         <v>137</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D13" s="61">
         <v>10</v>
       </c>
-      <c r="E13" s="99" t="s">
-        <v>229</v>
-      </c>
-      <c r="F13" s="50"/>
+      <c r="E13" s="98" t="s">
+        <v>229</v>
+      </c>
+      <c r="F13" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G13" s="49"/>
       <c r="H13" s="49"/>
       <c r="I13" s="49"/>
@@ -4333,19 +4367,19 @@
       <c r="K13" s="49"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="59">
+      <c r="A14" s="58">
         <v>4.2</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="65" t="s">
         <v>138</v>
       </c>
-      <c r="C14" s="65" t="s">
+      <c r="C14" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="63">
+      <c r="D14" s="62">
         <v>2</v>
       </c>
-      <c r="E14" s="99" t="s">
+      <c r="E14" s="98" t="s">
         <v>229</v>
       </c>
       <c r="F14" s="50"/>
@@ -4358,22 +4392,24 @@
       <c r="M14" s="24"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="59">
+      <c r="A15" s="58">
         <v>4.5</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="65" t="s">
         <v>163</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="61">
         <v>15</v>
       </c>
-      <c r="E15" s="99" t="s">
-        <v>229</v>
-      </c>
-      <c r="F15" s="50"/>
+      <c r="E15" s="98" t="s">
+        <v>229</v>
+      </c>
+      <c r="F15" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
       <c r="I15" s="49"/>
@@ -4383,22 +4419,24 @@
       <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="59">
+      <c r="A16" s="58">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="65" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="61">
         <v>10</v>
       </c>
-      <c r="E16" s="99" t="s">
-        <v>229</v>
-      </c>
-      <c r="F16" s="53"/>
+      <c r="E16" s="98" t="s">
+        <v>229</v>
+      </c>
+      <c r="F16" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
       <c r="I16" s="49"/>
@@ -4408,19 +4446,19 @@
       <c r="M16" s="24"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="59">
+      <c r="A17" s="58">
         <v>5.2</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="C17" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="63">
+      <c r="D17" s="62">
         <v>2</v>
       </c>
-      <c r="E17" s="99" t="s">
+      <c r="E17" s="98" t="s">
         <v>229</v>
       </c>
       <c r="F17" s="53"/>
@@ -4433,22 +4471,24 @@
       <c r="M17" s="24"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="59">
+      <c r="A18" s="58">
         <v>5.3</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="65" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="62">
+      <c r="D18" s="61">
         <v>15</v>
       </c>
-      <c r="E18" s="99" t="s">
-        <v>229</v>
-      </c>
-      <c r="F18" s="53"/>
+      <c r="E18" s="98" t="s">
+        <v>229</v>
+      </c>
+      <c r="F18" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
       <c r="I18" s="49"/>
@@ -4458,20 +4498,22 @@
       <c r="M18" s="24"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="59">
+      <c r="A19" s="58">
         <v>6.1</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="62">
+      <c r="D19" s="61">
         <v>50</v>
       </c>
       <c r="E19" s="49"/>
-      <c r="F19" s="54"/>
+      <c r="F19" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G19" s="49"/>
       <c r="H19" s="49"/>
       <c r="I19" s="49"/>
@@ -4481,22 +4523,24 @@
       <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="59">
+      <c r="A20" s="58">
         <v>6.1</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="61">
         <v>10</v>
       </c>
-      <c r="E20" s="103" t="s">
-        <v>229</v>
-      </c>
-      <c r="F20" s="50"/>
+      <c r="E20" s="102" t="s">
+        <v>229</v>
+      </c>
+      <c r="F20" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
@@ -4506,19 +4550,19 @@
       <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="59">
+      <c r="A21" s="58">
         <v>6.2</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="C21" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="63">
+      <c r="D21" s="62">
         <v>2</v>
       </c>
-      <c r="E21" s="103" t="s">
+      <c r="E21" s="102" t="s">
         <v>229</v>
       </c>
       <c r="F21" s="50"/>
@@ -4531,22 +4575,24 @@
       <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="59">
+      <c r="A22" s="58">
         <v>6.3</v>
       </c>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="78" t="s">
+      <c r="C22" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="62">
+      <c r="D22" s="61">
         <v>5</v>
       </c>
-      <c r="E22" s="103" t="s">
-        <v>229</v>
-      </c>
-      <c r="F22" s="55"/>
+      <c r="E22" s="102" t="s">
+        <v>229</v>
+      </c>
+      <c r="F22" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
@@ -4554,22 +4600,24 @@
       <c r="K22" s="49"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="59">
+      <c r="A23" s="58">
         <v>7.1</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="65" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="62">
+      <c r="D23" s="61">
         <v>10</v>
       </c>
-      <c r="E23" s="103" t="s">
-        <v>229</v>
-      </c>
-      <c r="F23" s="56"/>
+      <c r="E23" s="102" t="s">
+        <v>229</v>
+      </c>
+      <c r="F23" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
       <c r="I23" s="49"/>
@@ -4577,22 +4625,22 @@
       <c r="K23" s="49"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="59">
+      <c r="A24" s="58">
         <v>7.2</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="65" t="s">
         <v>144</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D24" s="63">
+      <c r="D24" s="62">
         <v>2</v>
       </c>
-      <c r="E24" s="103" t="s">
-        <v>229</v>
-      </c>
-      <c r="F24" s="55"/>
+      <c r="E24" s="102" t="s">
+        <v>229</v>
+      </c>
+      <c r="F24" s="54"/>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
       <c r="I24" s="49"/>
@@ -4602,22 +4650,24 @@
       <c r="M24" s="24"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="59">
+      <c r="A25" s="58">
         <v>7.3</v>
       </c>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="65" t="s">
         <v>165</v>
       </c>
-      <c r="C25" s="76" t="s">
+      <c r="C25" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="62">
+      <c r="D25" s="61">
         <v>10</v>
       </c>
-      <c r="E25" s="101" t="s">
-        <v>229</v>
-      </c>
-      <c r="F25" s="56"/>
+      <c r="E25" s="100" t="s">
+        <v>229</v>
+      </c>
+      <c r="F25" s="108" t="s">
+        <v>293</v>
+      </c>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
       <c r="I25" s="49"/>
@@ -4627,20 +4677,22 @@
       <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="59">
+      <c r="A26" s="58">
         <v>8.1</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="C26" s="77" t="s">
+      <c r="C26" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="61">
         <v>15</v>
       </c>
       <c r="E26" s="49"/>
-      <c r="F26" s="50"/>
+      <c r="F26" s="108" t="s">
+        <v>293</v>
+      </c>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
       <c r="I26" s="49"/>
@@ -4650,22 +4702,24 @@
       <c r="M26" s="24"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="59">
+      <c r="A27" s="58">
         <v>8.1</v>
       </c>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="65" t="s">
         <v>145</v>
       </c>
-      <c r="C27" s="73" t="s">
+      <c r="C27" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="61">
         <v>10</v>
       </c>
-      <c r="E27" s="103" t="s">
-        <v>229</v>
-      </c>
-      <c r="F27" s="50"/>
+      <c r="E27" s="102" t="s">
+        <v>229</v>
+      </c>
+      <c r="F27" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
@@ -4675,22 +4729,22 @@
       <c r="M27" s="24"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="59">
+      <c r="A28" s="58">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B28" s="66" t="s">
+      <c r="B28" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="65" t="s">
+      <c r="C28" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="63">
+      <c r="D28" s="62">
         <v>2</v>
       </c>
-      <c r="E28" s="103" t="s">
-        <v>229</v>
-      </c>
-      <c r="F28" s="55"/>
+      <c r="E28" s="102" t="s">
+        <v>229</v>
+      </c>
+      <c r="F28" s="54"/>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
       <c r="I28" s="49"/>
@@ -4700,20 +4754,22 @@
       <c r="M28" s="24"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="59">
+      <c r="A29" s="58">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="72" t="s">
+      <c r="C29" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="61">
         <v>4</v>
       </c>
       <c r="E29" s="49"/>
-      <c r="F29" s="56"/>
+      <c r="F29" s="108" t="s">
+        <v>293</v>
+      </c>
       <c r="G29" s="49"/>
       <c r="H29" s="49"/>
       <c r="I29" s="49"/>
@@ -4723,20 +4779,22 @@
       <c r="M29" s="24"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="59">
+      <c r="A30" s="58">
         <v>8.4</v>
       </c>
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="61" t="s">
+      <c r="C30" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="62">
+      <c r="D30" s="61">
         <v>15</v>
       </c>
       <c r="E30" s="49"/>
-      <c r="F30" s="50"/>
+      <c r="F30" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
       <c r="I30" s="49"/>
@@ -4746,20 +4804,24 @@
       <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="59">
+      <c r="A31" s="58">
         <v>9.1</v>
       </c>
-      <c r="B31" s="66" t="s">
+      <c r="B31" s="65" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="73" t="s">
+      <c r="C31" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="62">
+      <c r="D31" s="61">
         <v>10</v>
       </c>
-      <c r="E31" s="49"/>
-      <c r="F31" s="50"/>
+      <c r="E31" s="108" t="s">
+        <v>229</v>
+      </c>
+      <c r="F31" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
       <c r="I31" s="49"/>
@@ -4767,20 +4829,20 @@
       <c r="K31" s="49"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="59">
+      <c r="A32" s="58">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B32" s="66" t="s">
+      <c r="B32" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="C32" s="65" t="s">
+      <c r="C32" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="63">
+      <c r="D32" s="62">
         <v>2</v>
       </c>
       <c r="E32" s="49"/>
-      <c r="F32" s="56"/>
+      <c r="F32" s="55"/>
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
       <c r="I32" s="49"/>
@@ -4788,20 +4850,24 @@
       <c r="K32" s="49"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="59">
+      <c r="A33" s="58">
         <v>10.1</v>
       </c>
-      <c r="B33" s="66" t="s">
+      <c r="B33" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="C33" s="73" t="s">
+      <c r="C33" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="62">
+      <c r="D33" s="61">
         <v>10</v>
       </c>
-      <c r="E33" s="49"/>
-      <c r="F33" s="56"/>
+      <c r="E33" s="108" t="s">
+        <v>229</v>
+      </c>
+      <c r="F33" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
       <c r="I33" s="49"/>
@@ -4809,20 +4875,20 @@
       <c r="K33" s="49"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="59">
+      <c r="A34" s="58">
         <v>10.199999999999999</v>
       </c>
-      <c r="B34" s="66" t="s">
+      <c r="B34" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="65" t="s">
+      <c r="C34" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D34" s="63">
+      <c r="D34" s="62">
         <v>2</v>
       </c>
       <c r="E34" s="49"/>
-      <c r="F34" s="56"/>
+      <c r="F34" s="55"/>
       <c r="G34" s="49"/>
       <c r="H34" s="49"/>
       <c r="I34" s="49"/>
@@ -4830,20 +4896,24 @@
       <c r="K34" s="49"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="59">
+      <c r="A35" s="58">
         <v>11.1</v>
       </c>
-      <c r="B35" s="66" t="s">
+      <c r="B35" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="C35" s="73" t="s">
+      <c r="C35" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="62">
+      <c r="D35" s="61">
         <v>10</v>
       </c>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
+      <c r="E35" s="108" t="s">
+        <v>229</v>
+      </c>
+      <c r="F35" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G35" s="49"/>
       <c r="H35" s="49"/>
       <c r="I35" s="49"/>
@@ -4851,16 +4921,16 @@
       <c r="K35" s="49"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="59">
+      <c r="A36" s="58">
         <v>11.2</v>
       </c>
-      <c r="B36" s="66" t="s">
+      <c r="B36" s="65" t="s">
         <v>152</v>
       </c>
-      <c r="C36" s="65" t="s">
+      <c r="C36" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="63">
+      <c r="D36" s="62">
         <v>2</v>
       </c>
       <c r="E36" s="49"/>
@@ -4872,20 +4942,22 @@
       <c r="K36" s="49"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="59">
+      <c r="A37" s="58">
         <v>11.3</v>
       </c>
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="74" t="s">
+      <c r="C37" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="62">
+      <c r="D37" s="61">
         <v>15</v>
       </c>
       <c r="E37" s="49"/>
-      <c r="F37" s="57"/>
+      <c r="F37" s="56" t="s">
+        <v>229</v>
+      </c>
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
       <c r="I37" s="49"/>
@@ -4893,20 +4965,24 @@
       <c r="K37" s="49"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="59">
+      <c r="A38" s="58">
         <v>12.1</v>
       </c>
-      <c r="B38" s="66" t="s">
+      <c r="B38" s="65" t="s">
         <v>153</v>
       </c>
-      <c r="C38" s="73" t="s">
+      <c r="C38" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="62">
+      <c r="D38" s="61">
         <v>10</v>
       </c>
-      <c r="E38" s="49"/>
-      <c r="F38" s="50"/>
+      <c r="E38" s="108" t="s">
+        <v>229</v>
+      </c>
+      <c r="F38" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
       <c r="I38" s="49"/>
@@ -4914,16 +4990,16 @@
       <c r="K38" s="49"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="59">
+      <c r="A39" s="58">
         <v>12.2</v>
       </c>
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="65" t="s">
         <v>154</v>
       </c>
-      <c r="C39" s="65" t="s">
+      <c r="C39" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="63">
+      <c r="D39" s="62">
         <v>2</v>
       </c>
       <c r="E39" s="49"/>
@@ -4935,20 +5011,22 @@
       <c r="K39" s="49"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="59">
+      <c r="A40" s="58">
         <v>12.5</v>
       </c>
-      <c r="B40" s="66" t="s">
+      <c r="B40" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="72" t="s">
+      <c r="C40" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="62">
+      <c r="D40" s="61">
         <v>4</v>
       </c>
       <c r="E40" s="49"/>
-      <c r="F40" s="50"/>
+      <c r="F40" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G40" s="49"/>
       <c r="H40" s="49"/>
       <c r="I40" s="49"/>
@@ -4956,20 +5034,22 @@
       <c r="K40" s="49"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="59">
+      <c r="A41" s="58">
         <v>12.6</v>
       </c>
-      <c r="B41" s="68" t="s">
+      <c r="B41" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="74" t="s">
+      <c r="C41" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="62">
+      <c r="D41" s="61">
         <v>15</v>
       </c>
       <c r="E41" s="49"/>
-      <c r="F41" s="50"/>
+      <c r="F41" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G41" s="49"/>
       <c r="H41" s="49"/>
       <c r="I41" s="49"/>
@@ -4977,20 +5057,22 @@
       <c r="K41" s="49"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="59">
+      <c r="A42" s="58">
         <v>12.7</v>
       </c>
-      <c r="B42" s="66" t="s">
+      <c r="B42" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="C42" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="62">
+      <c r="D42" s="61">
         <v>15</v>
       </c>
       <c r="E42" s="49"/>
-      <c r="F42" s="58"/>
+      <c r="F42" s="108" t="s">
+        <v>293</v>
+      </c>
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
       <c r="I42" s="49"/>
@@ -4998,20 +5080,22 @@
       <c r="K42" s="49"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="59">
+      <c r="A43" s="58">
         <v>13.1</v>
       </c>
-      <c r="B43" s="66" t="s">
+      <c r="B43" s="65" t="s">
         <v>155</v>
       </c>
-      <c r="C43" s="73" t="s">
+      <c r="C43" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="62">
+      <c r="D43" s="61">
         <v>10</v>
       </c>
       <c r="E43" s="49"/>
-      <c r="F43" s="58"/>
+      <c r="F43" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G43" s="49"/>
       <c r="H43" s="49"/>
       <c r="I43" s="49"/>
@@ -5019,20 +5103,20 @@
       <c r="K43" s="49"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="59">
+      <c r="A44" s="58">
         <v>13.2</v>
       </c>
-      <c r="B44" s="66" t="s">
+      <c r="B44" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="C44" s="65" t="s">
+      <c r="C44" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="63">
+      <c r="D44" s="62">
         <v>2</v>
       </c>
       <c r="E44" s="49"/>
-      <c r="F44" s="58"/>
+      <c r="F44" s="57"/>
       <c r="G44" s="49"/>
       <c r="H44" s="49"/>
       <c r="I44" s="49"/>
@@ -5040,20 +5124,22 @@
       <c r="K44" s="49"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="59">
+      <c r="A45" s="58">
         <v>13.5</v>
       </c>
-      <c r="B45" s="68" t="s">
+      <c r="B45" s="67" t="s">
         <v>106</v>
       </c>
-      <c r="C45" s="74" t="s">
+      <c r="C45" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="62">
+      <c r="D45" s="61">
         <v>15</v>
       </c>
       <c r="E45" s="49"/>
-      <c r="F45" s="58"/>
+      <c r="F45" s="108" t="s">
+        <v>293</v>
+      </c>
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
       <c r="I45" s="49"/>
@@ -5061,20 +5147,22 @@
       <c r="K45" s="49"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="59">
+      <c r="A46" s="58">
         <v>14.1</v>
       </c>
-      <c r="B46" s="66" t="s">
+      <c r="B46" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="C46" s="72" t="s">
+      <c r="C46" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D46" s="62">
+      <c r="D46" s="61">
         <v>4</v>
       </c>
       <c r="E46" s="49"/>
-      <c r="F46" s="49"/>
+      <c r="F46" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G46" s="49"/>
       <c r="H46" s="49"/>
       <c r="I46" s="49"/>
@@ -5082,20 +5170,22 @@
       <c r="K46" s="49"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="59">
+      <c r="A47" s="58">
         <v>14.1</v>
       </c>
-      <c r="B47" s="66" t="s">
+      <c r="B47" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="C47" s="72" t="s">
+      <c r="C47" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="62">
+      <c r="D47" s="61">
         <v>4</v>
       </c>
       <c r="E47" s="49"/>
-      <c r="F47" s="58"/>
+      <c r="F47" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G47" s="49"/>
       <c r="H47" s="49"/>
       <c r="I47" s="49"/>
@@ -5103,20 +5193,22 @@
       <c r="K47" s="49"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="59">
+      <c r="A48" s="58">
         <v>14.1</v>
       </c>
-      <c r="B48" s="66" t="s">
+      <c r="B48" s="65" t="s">
         <v>157</v>
       </c>
-      <c r="C48" s="73" t="s">
+      <c r="C48" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D48" s="62">
+      <c r="D48" s="61">
         <v>10</v>
       </c>
       <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
+      <c r="F48" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
       <c r="I48" s="49"/>
@@ -5124,20 +5216,22 @@
       <c r="K48" s="49"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="59">
+      <c r="A49" s="58">
         <v>14.2</v>
       </c>
-      <c r="B49" s="66" t="s">
+      <c r="B49" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="C49" s="61" t="s">
+      <c r="C49" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="62">
+      <c r="D49" s="61">
         <v>15</v>
       </c>
       <c r="E49" s="49"/>
-      <c r="F49" s="58"/>
+      <c r="F49" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G49" s="49"/>
       <c r="H49" s="49"/>
       <c r="I49" s="49"/>
@@ -5145,20 +5239,22 @@
       <c r="K49" s="49"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="59">
+      <c r="A50" s="58">
         <v>14.2</v>
       </c>
-      <c r="B50" s="66" t="s">
+      <c r="B50" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="61" t="s">
+      <c r="C50" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="D50" s="62">
+      <c r="D50" s="61">
         <v>15</v>
       </c>
       <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
+      <c r="F50" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G50" s="49"/>
       <c r="H50" s="49"/>
       <c r="I50" s="49"/>
@@ -5166,20 +5262,20 @@
       <c r="K50" s="49"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="59">
+      <c r="A51" s="58">
         <v>14.2</v>
       </c>
-      <c r="B51" s="66" t="s">
+      <c r="B51" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="C51" s="65" t="s">
+      <c r="C51" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D51" s="63">
+      <c r="D51" s="62">
         <v>2</v>
       </c>
       <c r="E51" s="49"/>
-      <c r="F51" s="58"/>
+      <c r="F51" s="57"/>
       <c r="G51" s="49"/>
       <c r="H51" s="49"/>
       <c r="I51" s="49"/>
@@ -5187,20 +5283,22 @@
       <c r="K51" s="49"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="59">
+      <c r="A52" s="58">
         <v>15.1</v>
       </c>
-      <c r="B52" s="60" t="s">
+      <c r="B52" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="72" t="s">
+      <c r="C52" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D52" s="62">
+      <c r="D52" s="61">
         <v>4</v>
       </c>
       <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
+      <c r="F52" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G52" s="49"/>
       <c r="H52" s="49"/>
       <c r="I52" s="49"/>
@@ -5208,20 +5306,22 @@
       <c r="K52" s="49"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="59">
+      <c r="A53" s="58">
         <v>15.1</v>
       </c>
-      <c r="B53" s="66" t="s">
+      <c r="B53" s="65" t="s">
         <v>159</v>
       </c>
-      <c r="C53" s="73" t="s">
+      <c r="C53" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D53" s="62">
+      <c r="D53" s="61">
         <v>10</v>
       </c>
       <c r="E53" s="49"/>
-      <c r="F53" s="49"/>
+      <c r="F53" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G53" s="49"/>
       <c r="H53" s="49"/>
       <c r="I53" s="49"/>
@@ -5229,20 +5329,22 @@
       <c r="K53" s="49"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="59">
+      <c r="A54" s="58">
         <v>15.2</v>
       </c>
-      <c r="B54" s="60" t="s">
+      <c r="B54" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C54" s="61" t="s">
+      <c r="C54" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="62">
+      <c r="D54" s="61">
         <v>10</v>
       </c>
       <c r="E54" s="49"/>
-      <c r="F54" s="58"/>
+      <c r="F54" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G54" s="49"/>
       <c r="H54" s="49"/>
       <c r="I54" s="49"/>
@@ -5250,16 +5352,16 @@
       <c r="K54" s="49"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="59">
+      <c r="A55" s="58">
         <v>15.2</v>
       </c>
-      <c r="B55" s="66" t="s">
+      <c r="B55" s="65" t="s">
         <v>160</v>
       </c>
-      <c r="C55" s="65" t="s">
+      <c r="C55" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D55" s="63">
+      <c r="D55" s="62">
         <v>2</v>
       </c>
       <c r="E55" s="49"/>
@@ -5271,20 +5373,22 @@
       <c r="K55" s="49"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="59">
+      <c r="A56" s="58">
         <v>16</v>
       </c>
-      <c r="B56" s="60" t="s">
+      <c r="B56" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C56" s="72" t="s">
+      <c r="C56" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D56" s="62">
+      <c r="D56" s="61">
         <v>5</v>
       </c>
       <c r="E56" s="49"/>
-      <c r="F56" s="58"/>
+      <c r="F56" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G56" s="49"/>
       <c r="H56" s="49"/>
       <c r="I56" s="49"/>
@@ -5292,20 +5396,22 @@
       <c r="K56" s="49"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="59">
+      <c r="A57" s="58">
         <v>16</v>
       </c>
-      <c r="B57" s="60" t="s">
+      <c r="B57" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="61" t="s">
+      <c r="C57" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="62">
+      <c r="D57" s="61">
         <v>10</v>
       </c>
       <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
+      <c r="F57" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G57" s="49"/>
       <c r="H57" s="49"/>
       <c r="I57" s="49"/>
@@ -5313,20 +5419,22 @@
       <c r="K57" s="49"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="59">
+      <c r="A58" s="58">
         <v>16</v>
       </c>
-      <c r="B58" s="60" t="s">
+      <c r="B58" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="75" t="s">
+      <c r="C58" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D58" s="62">
+      <c r="D58" s="61">
         <v>50</v>
       </c>
       <c r="E58" s="49"/>
-      <c r="F58" s="58"/>
+      <c r="F58" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G58" s="49"/>
       <c r="H58" s="49"/>
       <c r="I58" s="49"/>
@@ -5334,20 +5442,22 @@
       <c r="K58" s="49"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="59">
+      <c r="A59" s="58">
         <v>16</v>
       </c>
-      <c r="B59" s="60" t="s">
+      <c r="B59" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="78" t="s">
+      <c r="C59" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="D59" s="62">
+      <c r="D59" s="61">
         <v>2</v>
       </c>
       <c r="E59" s="49"/>
-      <c r="F59" s="58"/>
+      <c r="F59" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G59" s="49"/>
       <c r="H59" s="49"/>
       <c r="I59" s="49"/>
@@ -5355,20 +5465,22 @@
       <c r="K59" s="49"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="59">
+      <c r="A60" s="58">
         <v>16</v>
       </c>
-      <c r="B60" s="66" t="s">
+      <c r="B60" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="C60" s="72" t="s">
+      <c r="C60" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D60" s="62">
+      <c r="D60" s="61">
         <v>3</v>
       </c>
       <c r="E60" s="49"/>
-      <c r="F60" s="58"/>
+      <c r="F60" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G60" s="49"/>
       <c r="H60" s="49"/>
       <c r="I60" s="49"/>
@@ -5376,20 +5488,22 @@
       <c r="K60" s="49"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="59">
+      <c r="A61" s="58">
         <v>16</v>
       </c>
-      <c r="B61" s="60" t="s">
+      <c r="B61" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="C61" s="72" t="s">
+      <c r="C61" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D61" s="62">
+      <c r="D61" s="61">
         <v>2</v>
       </c>
       <c r="E61" s="49"/>
-      <c r="F61" s="58"/>
+      <c r="F61" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
       <c r="I61" s="49"/>
@@ -5397,20 +5511,22 @@
       <c r="K61" s="49"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="59">
+      <c r="A62" s="58">
         <v>16</v>
       </c>
-      <c r="B62" s="60" t="s">
+      <c r="B62" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="78" t="s">
+      <c r="C62" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="D62" s="62">
+      <c r="D62" s="61">
         <v>10</v>
       </c>
       <c r="E62" s="49"/>
-      <c r="F62" s="58"/>
+      <c r="F62" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
       <c r="I62" s="49"/>
@@ -5418,20 +5534,22 @@
       <c r="K62" s="49"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="59">
+      <c r="A63" s="58">
         <v>16</v>
       </c>
-      <c r="B63" s="79" t="s">
+      <c r="B63" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="72" t="s">
+      <c r="C63" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D63" s="62">
+      <c r="D63" s="61">
         <v>6</v>
       </c>
       <c r="E63" s="49"/>
-      <c r="F63" s="58"/>
+      <c r="F63" s="108" t="s">
+        <v>229</v>
+      </c>
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
       <c r="I63" s="49"/>
@@ -5476,7 +5594,7 @@
       <c r="C66" s="4"/>
       <c r="D66" s="8"/>
       <c r="E66" s="49"/>
-      <c r="F66" s="58"/>
+      <c r="F66" s="57"/>
       <c r="G66" s="49"/>
       <c r="H66" s="49"/>
       <c r="I66" s="49"/>

</xml_diff>

<commit_message>
add links to schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDF07B5-C6E3-4ADB-B47B-72DCCB3AEE9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A93A464-4604-4808-B428-3E34249AB76E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -1127,18 +1127,18 @@
 321 Binder exercise - Learning how to Learn. </t>
   </si>
   <si>
-    <t>Familiarize yourself with the required course materials: [ROBIN PUT LINK HERE ]
+    <t>Thinking about learning</t>
+  </si>
+  <si>
+    <t>Familiarize yourself with the required [course materials](reading/Materials%20overview.pdf)
 Join the Slack workspace and post an introduction
 Install R, R Studio and associated packages onto your computer using the [Math 130 lesson on installing R](https://norcalbiostat.github.io/MATH130/notes/02_setup.html) &lt;b&gt;-OR-&lt;/b&gt;
 If using R Studio Cloud - make an account, join our workspace (posted in Slack), click the "New Project" button and replace "Untitled Project" with your name (first and last)
-Watch [PDS Video 1](https://www.youtube.com/watch?v=_8A0zx51BKs)
-Prepare your Learning Journal (before Wed)
-Read: Learning - your first job
-Read: MAI and academic achievement
+Watch PDS Video 1 (link on [notes page](https://norcalbiostat.github.io/MATH315/notes.html))
+Prepare your Learning Journal before wed (See [HW01](hw/hw01_introduction.html))
+Read: Learning - your first job (all reading links are on materials page)
+Read: [MAI and academic achievement](reading/MAI%20and%20academic%20achievement%20in%20college%20students%20(Young,%20Fry,%202008).pdf
 Review the [Advice from prior Math 315 students](reading/Advice%20from%20prior%20Math%20315%20students.pdf) (Long, but skim it and you'll see themes)</t>
-  </si>
-  <si>
-    <t>Thinking about learning</t>
   </si>
 </sst>
 </file>
@@ -2350,7 +2350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2424,7 +2424,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3108,9 +3108,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3155,7 +3155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A2" s="99">
         <v>1</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>179</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>261</v>

</xml_diff>

<commit_message>
fix typo and work on bridge
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20346"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A93A464-4604-4808-B428-3E34249AB76E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FDB00A-26E5-4AF8-9088-ADC0F67662F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -26,14 +26,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -42,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="299">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1121,13 +1113,13 @@
     <t>-</t>
   </si>
   <si>
+    <t>Thinking about learning</t>
+  </si>
+  <si>
     <t xml:space="preserve">Learn how to use R to do and turn in homework (test markdown file, hw1 template)
 Set up an organized class folder
 Introduction to class resources on how to learn R.  (PDS Videos, textbook(s), Course Notes, Math 130, R-help page on class website)
-321 Binder exercise - Learning how to Learn. </t>
-  </si>
-  <si>
-    <t>Thinking about learning</t>
+321 Bridge exercise - Learning how to Learn. </t>
   </si>
   <si>
     <t>Familiarize yourself with the required [course materials](reading/Materials%20overview.pdf)
@@ -1137,8 +1129,14 @@
 Watch PDS Video 1 (link on [notes page](https://norcalbiostat.github.io/MATH315/notes.html))
 Prepare your Learning Journal before wed (See [HW01](hw/hw01_introduction.html))
 Read: Learning - your first job (all reading links are on materials page)
-Read: [MAI and academic achievement](reading/MAI%20and%20academic%20achievement%20in%20college%20students%20(Young,%20Fry,%202008).pdf
+Read: [MAI and academic achievement](reading/MAI%20and%20academic%20achievement%20in%20college%20students%20(Young,%20Fry,%202008).pdf)
 Review the [Advice from prior Math 315 students](reading/Advice%20from%20prior%20Math%20315%20students.pdf) (Long, but skim it and you'll see themes)</t>
+  </si>
+  <si>
+    <t>321 Bridge</t>
+  </si>
+  <si>
+    <t>Reproducible Research</t>
   </si>
 </sst>
 </file>
@@ -1657,7 +1655,7 @@
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1926,6 +1924,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2350,8 +2351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2424,7 +2425,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3096,7 +3097,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H48">
+  <sortState ref="A2:H48">
     <sortCondition ref="A2:A48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3108,9 +3109,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3122,7 +3123,7 @@
     <col min="5" max="5" width="88.25" style="22" customWidth="1"/>
     <col min="6" max="6" width="34.625" style="22" customWidth="1"/>
     <col min="7" max="8" width="38" style="22" customWidth="1"/>
-    <col min="9" max="9" width="39.125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="25.375" style="21" customWidth="1"/>
     <col min="10" max="16384" width="14.875" style="21"/>
   </cols>
   <sheetData>
@@ -3154,6 +3155,9 @@
       <c r="I1" s="79" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="109" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A2" s="99">
@@ -3175,13 +3179,16 @@
         <v>261</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>178</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>167</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -5918,7 +5925,7 @@
       <c r="Z78" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E78">
+  <sortState ref="A2:E78">
     <sortCondition ref="A2:A78"/>
   </sortState>
   <phoneticPr fontId="38" type="noConversion"/>

</xml_diff>

<commit_message>
add lily and fix quiz 3 schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20346"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FDB00A-26E5-4AF8-9088-ADC0F67662F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CB1383-BC85-46EF-BBA7-A27A8748CA21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30465" yWindow="1230" windowWidth="21090" windowHeight="13665" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -26,6 +26,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -822,11 +830,6 @@
     <t>Poster prep Stage IV* (Draft Due 12/03, PR 12/05, Final 12/07 )</t>
   </si>
   <si>
-    <t>Quiz 15 (Due 12/08 ) 
-[Sec 01]()
-[Sec 02]()</t>
-  </si>
-  <si>
     <t xml:space="preserve">e-Poster*  (Draft Due 12/xx , PR 12/xx, Final 12/xx xpm ) TIMES ARE FIRM - Dates dependent on time of common final </t>
   </si>
   <si>
@@ -1034,80 +1037,15 @@
     <t>Logistic Regression analysis</t>
   </si>
   <si>
-    <t>Quiz 10 (Due 10/27 ) 
-[[Sec 01]](https://forms.gle/CPMywhKBnM8fHiD96)
-[[Sec 02]](https://forms.gle/QEUMGXgyTdoBJKnL8)</t>
-  </si>
-  <si>
     <t>Study design</t>
   </si>
   <si>
     <t>8.1</t>
-  </si>
-  <si>
-    <t>Quiz 13 (Due 11/17 ) 
-[[Sec 01]](https://forms.gle/TZSWziSqpk4yFBTb6)
-[[Sec 02]](https://forms.gle/1LoH1WdvKvSToz8L7)</t>
-  </si>
-  <si>
-    <t>Quiz 11 (Due 11/03 ) 
-[[Sec 01]](https://forms.gle/ENYkP4FwqcvwqmfKA)
-[[Sec 02]](https://forms.gle/QqR4g8WjXnJSh2HX8)</t>
-  </si>
-  <si>
-    <t>Quiz 12 (Due 11/10 ) 
-[[Sec 01]](https://forms.gle/y96Ebhj982kwPHoX6)
-[[Sec 02]](https://forms.gle/dxhYEygUG7WDCYJK9)</t>
-  </si>
-  <si>
-    <t>Quiz 14 (Due 11/14 ) 
-[[Sec 01]](https://forms.gle/BSimfYAa9xuF3D9u7)
-[Sec 02]()</t>
   </si>
   <si>
     <t>Quiz 01 (Due 08/29 ) 
 [[Sec01]](https://forms.gle/4CEBJqDaJ9Y23Ddm8)
 [[Sec02]](https://forms.gle/7zCnaLTe1Hrc6LwD7)</t>
-  </si>
-  <si>
-    <t>Quiz 02 (Due 09/03 ) 
-[[Sec01]](https://forms.gle/46GFpQNGswFxH1YZ6)
-[[Sec02]](https://forms.gle/5VXAvu8sxw6qvG4H7)</t>
-  </si>
-  <si>
-    <t>Quiz 03 (Due 09/08 ) 
-[[Sec 01]](https://forms.gle/ot6kJ2As7WHyrZd47)
-[[Sec 02]](https://forms.gle/TodvxwrZjhb2CRvC8)</t>
-  </si>
-  <si>
-    <t>Quiz 04 (Due 09/15 ) 
-[[Sec 01]](https://forms.gle/k5Kys9VCCec7oTw5A)
-[[Sec 02]](https://forms.gle/cZxx2dMYAejj9AHs5)</t>
-  </si>
-  <si>
-    <t>Quiz 05 (Due 09/22 ) 
-[[Sec 01]](https://forms.gle/Jo4gqJ4baNV2d4M68)
-[[Sec 02]](https://forms.gle/tdK2MXM8V56CC3su7)</t>
-  </si>
-  <si>
-    <t>Quiz 06 (Due 09/29 ) 
-[[Sec 01]](https://forms.gle/ZWbdQbiRxNB9USCu9)
-[[Sec 02]](https://forms.gle/AsYjcqujuDr6Ekwy6)</t>
-  </si>
-  <si>
-    <t>Quiz 07 (Due 10/06 ) 
-[[Sec 01]](https://forms.gle/89RhdsVfaPutrwku5)
-[[Sec 02]](https://forms.gle/TmawJctpFrq4itmn8)</t>
-  </si>
-  <si>
-    <t>Quiz 09 (Due 10/20 ) 
-[[Sec 01]](https://forms.gle/o8dSPooP9b2Ui1qUA)
-[[Sec 02]](https://forms.gle/vXuuJcKARFTx7W8z6)</t>
-  </si>
-  <si>
-    <t>Quiz 08 (Due 10/13 ) 
-[[Sec 01]](https://forms.gle/sbEX4x39tJwJdRBh8)
-[[Sec 02]](https://forms.gle/hC7ciiAKmi614Nrw9)</t>
   </si>
   <si>
     <t>-</t>
@@ -1137,6 +1075,77 @@
   </si>
   <si>
     <t>Reproducible Research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz 02 (Due 09/03 ) 
+[[10am]](https://forms.gle/TcWHzcfEn4ych7TJA)
+[[12pm]](https://forms.gle/JmzgBUXc4KYE34Y36)
+</t>
+  </si>
+  <si>
+    <t>Quiz 10 (Due 10/27 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 09 (Due 10/20 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 08 (Due 10/13 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 11 (Due 11/03 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 13 (Due 11/17 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 14 (Due 11/14 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 15 (Due 12/08 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 12 (Due 11/10 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 07 (Due 10/06 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 06 (Due 09/29 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 05 (Due 09/22 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 04 (Due 09/15 ) 
+[[10am]]()
+[[12pm]]()</t>
+  </si>
+  <si>
+    <t>Quiz 03 (Due 09/08 ) 
+[[10am]](https://forms.gle/W1GyjHgcGDrAN6GK8)
+[[12pm]](https://forms.gle/yYRae4eWMBvCwSbu6)</t>
   </si>
 </sst>
 </file>
@@ -1655,7 +1664,7 @@
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1919,14 +1928,20 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2351,8 +2366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2362,7 +2377,7 @@
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.375" style="42" customWidth="1"/>
     <col min="6" max="6" width="11.25" style="35" customWidth="1"/>
-    <col min="7" max="7" width="16.875" style="94" customWidth="1"/>
+    <col min="7" max="7" width="60.75" style="94" customWidth="1"/>
     <col min="8" max="8" width="79.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2380,7 +2395,7 @@
         <v>68</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>101</v>
@@ -2406,7 +2421,7 @@
         <v>69</v>
       </c>
       <c r="G2" s="94" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="H2" s="95" t="s">
         <v>211</v>
@@ -2425,7 +2440,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2450,7 +2465,7 @@
         <v>84</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2465,7 +2480,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
         <v>2.1</v>
       </c>
@@ -2476,12 +2491,12 @@
         <v>113</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F8" s="35">
         <v>1.3</v>
       </c>
-      <c r="G8" s="94" t="s">
+      <c r="G8" s="109" t="s">
         <v>285</v>
       </c>
       <c r="H8" s="95" t="s">
@@ -2496,7 +2511,7 @@
         <v>114</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2518,7 +2533,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>3.1</v>
       </c>
@@ -2533,8 +2548,8 @@
         <v>86</v>
       </c>
       <c r="F12" s="36"/>
-      <c r="G12" s="97" t="s">
-        <v>286</v>
+      <c r="G12" s="110" t="s">
+        <v>298</v>
       </c>
       <c r="H12" s="95" t="s">
         <v>213</v>
@@ -2564,7 +2579,7 @@
       </c>
       <c r="H14" s="81"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>4.0999999999999996</v>
       </c>
@@ -2580,8 +2595,8 @@
       <c r="F15" s="35">
         <v>2.1</v>
       </c>
-      <c r="G15" s="97" t="s">
-        <v>287</v>
+      <c r="G15" s="110" t="s">
+        <v>297</v>
       </c>
       <c r="H15" s="95" t="s">
         <v>214</v>
@@ -2598,7 +2613,7 @@
         <v>88</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2615,7 +2630,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>5.0999999999999996</v>
       </c>
@@ -2623,16 +2638,16 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>89</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>255</v>
-      </c>
-      <c r="G18" s="97" t="s">
-        <v>288</v>
+        <v>254</v>
+      </c>
+      <c r="G18" s="110" t="s">
+        <v>296</v>
       </c>
       <c r="H18" s="95" t="s">
         <v>216</v>
@@ -2649,7 +2664,7 @@
       <c r="G19" s="97"/>
       <c r="H19" s="95"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>6.1</v>
       </c>
@@ -2662,8 +2677,8 @@
       <c r="E20" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="G20" s="97" t="s">
-        <v>289</v>
+      <c r="G20" s="110" t="s">
+        <v>295</v>
       </c>
       <c r="H20" s="101" t="s">
         <v>217</v>
@@ -2694,7 +2709,7 @@
       <c r="F22" s="87"/>
       <c r="G22" s="105"/>
       <c r="H22" s="85" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2705,7 +2720,7 @@
         <v>117</v>
       </c>
       <c r="H23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2722,7 +2737,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="40">
         <v>7.1</v>
       </c>
@@ -2733,13 +2748,13 @@
         <v>205</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F25" s="35">
         <v>4</v>
       </c>
-      <c r="G25" s="97" t="s">
-        <v>290</v>
+      <c r="G25" s="110" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2750,7 +2765,7 @@
         <v>206</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2764,7 +2779,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
         <v>8.1</v>
       </c>
@@ -2777,8 +2792,8 @@
       <c r="F28" s="35">
         <v>4.7</v>
       </c>
-      <c r="G28" s="97" t="s">
-        <v>292</v>
+      <c r="G28" s="110" t="s">
+        <v>288</v>
       </c>
       <c r="H28" s="80" t="s">
         <v>219</v>
@@ -2792,10 +2807,10 @@
         <v>74</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2803,13 +2818,13 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F30" s="35">
         <v>6.1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
         <v>9.1</v>
       </c>
@@ -2825,8 +2840,8 @@
       <c r="F31" s="35">
         <v>6.2</v>
       </c>
-      <c r="G31" s="97" t="s">
-        <v>291</v>
+      <c r="G31" s="110" t="s">
+        <v>287</v>
       </c>
       <c r="H31" s="95" t="s">
         <v>220</v>
@@ -2837,7 +2852,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E32" s="42" t="s">
         <v>92</v>
@@ -2851,7 +2866,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E33" s="42" t="s">
         <v>93</v>
@@ -2860,7 +2875,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>10.1</v>
       </c>
@@ -2868,7 +2883,7 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E34" s="42" t="s">
         <v>98</v>
@@ -2876,11 +2891,11 @@
       <c r="F34" s="35">
         <v>6.5</v>
       </c>
-      <c r="G34" s="97" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G34" s="110" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>11.1</v>
       </c>
@@ -2896,8 +2911,8 @@
       <c r="F35" s="35">
         <v>7</v>
       </c>
-      <c r="G35" s="97" t="s">
-        <v>281</v>
+      <c r="G35" s="110" t="s">
+        <v>289</v>
       </c>
       <c r="H35" s="95" t="s">
         <v>221</v>
@@ -2914,7 +2929,7 @@
         <v>96</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2922,13 +2937,13 @@
         <v>11.3</v>
       </c>
       <c r="D37" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
         <v>12.1</v>
       </c>
@@ -2942,10 +2957,10 @@
         <v>95</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>256</v>
-      </c>
-      <c r="G38" s="97" t="s">
-        <v>282</v>
+        <v>255</v>
+      </c>
+      <c r="G38" s="110" t="s">
+        <v>293</v>
       </c>
       <c r="H38" s="80" t="s">
         <v>222</v>
@@ -2956,7 +2971,7 @@
         <v>12.2</v>
       </c>
       <c r="D39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E39" s="42" t="s">
         <v>100</v>
@@ -2977,7 +2992,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A41" s="40">
         <v>13.1</v>
       </c>
@@ -2985,16 +3000,16 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E41" s="42" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>237</v>
-      </c>
-      <c r="G41" s="97" t="s">
-        <v>280</v>
+        <v>236</v>
+      </c>
+      <c r="G41" s="110" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3005,7 +3020,7 @@
         <v>107</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3013,14 +3028,14 @@
         <v>14</v>
       </c>
       <c r="D43" s="88" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E43" s="89"/>
       <c r="F43" s="90"/>
       <c r="G43" s="106"/>
       <c r="H43" s="88"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
         <v>15.1</v>
       </c>
@@ -3033,8 +3048,8 @@
       <c r="F44" s="38">
         <v>8.4</v>
       </c>
-      <c r="G44" s="107" t="s">
-        <v>283</v>
+      <c r="G44" s="111" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3051,7 +3066,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
         <v>16.100000000000001</v>
       </c>
@@ -3064,11 +3079,11 @@
       <c r="E46" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="G46" s="107" t="s">
+      <c r="G46" s="111" t="s">
+        <v>292</v>
+      </c>
+      <c r="H46" t="s">
         <v>225</v>
-      </c>
-      <c r="H46" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3093,11 +3108,11 @@
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H48">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H48">
     <sortCondition ref="A2:A48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3155,8 +3170,8 @@
       <c r="I1" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="109" t="s">
-        <v>297</v>
+      <c r="J1" s="108" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -3173,13 +3188,13 @@
         <v>179</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>178</v>
@@ -3188,7 +3203,7 @@
         <v>167</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3206,7 +3221,7 @@
         <v>173</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
@@ -3215,7 +3230,7 @@
         <v>172</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>171</v>
@@ -3237,7 +3252,7 @@
         <v>177</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>186</v>
@@ -3246,7 +3261,7 @@
         <v>180</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>169</v>
@@ -3267,7 +3282,7 @@
         <v>176</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>185</v>
@@ -3291,22 +3306,22 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>183</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>184</v>
@@ -3321,28 +3336,28 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>244</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="99">
         <v>7</v>
       </c>
@@ -3354,22 +3369,22 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3387,13 +3402,13 @@
         <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3723,10 +3738,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>229</v>
-      </c>
-      <c r="F2" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F2" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G2" s="50"/>
       <c r="H2" s="31" t="s">
@@ -3802,10 +3817,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="92" t="s">
-        <v>229</v>
-      </c>
-      <c r="F3" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F3" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G3" s="49"/>
       <c r="H3" s="47" t="s">
@@ -3881,7 +3896,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="93" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="50"/>
@@ -3958,10 +3973,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="93" t="s">
-        <v>229</v>
-      </c>
-      <c r="F5" s="108" t="s">
-        <v>293</v>
+        <v>228</v>
+      </c>
+      <c r="F5" s="107" t="s">
+        <v>279</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="4" t="s">
@@ -4030,10 +4045,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="93" t="s">
-        <v>229</v>
-      </c>
-      <c r="F6" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F6" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="4" t="s">
@@ -4109,7 +4124,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="93" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -4186,10 +4201,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="93" t="s">
-        <v>229</v>
-      </c>
-      <c r="F8" s="108" t="s">
-        <v>293</v>
+        <v>228</v>
+      </c>
+      <c r="F8" s="107" t="s">
+        <v>279</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="4"/>
@@ -4251,8 +4266,8 @@
         <v>4</v>
       </c>
       <c r="E9" s="49"/>
-      <c r="F9" s="108" t="s">
-        <v>229</v>
+      <c r="F9" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G9" s="50"/>
       <c r="H9" s="50"/>
@@ -4289,10 +4304,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="96" t="s">
-        <v>229</v>
-      </c>
-      <c r="F10" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F10" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="50"/>
@@ -4314,7 +4329,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="49"/>
@@ -4337,10 +4352,10 @@
         <v>15</v>
       </c>
       <c r="E12" s="96" t="s">
-        <v>229</v>
-      </c>
-      <c r="F12" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F12" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
@@ -4362,10 +4377,10 @@
         <v>10</v>
       </c>
       <c r="E13" s="98" t="s">
-        <v>229</v>
-      </c>
-      <c r="F13" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F13" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G13" s="49"/>
       <c r="H13" s="49"/>
@@ -4387,7 +4402,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="98" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="49"/>
@@ -4412,10 +4427,10 @@
         <v>15</v>
       </c>
       <c r="E15" s="98" t="s">
-        <v>229</v>
-      </c>
-      <c r="F15" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F15" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
@@ -4439,10 +4454,10 @@
         <v>10</v>
       </c>
       <c r="E16" s="98" t="s">
-        <v>229</v>
-      </c>
-      <c r="F16" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F16" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
@@ -4466,7 +4481,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="98" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F17" s="53"/>
       <c r="G17" s="49"/>
@@ -4491,10 +4506,10 @@
         <v>15</v>
       </c>
       <c r="E18" s="98" t="s">
-        <v>229</v>
-      </c>
-      <c r="F18" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F18" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
@@ -4518,8 +4533,8 @@
         <v>50</v>
       </c>
       <c r="E19" s="49"/>
-      <c r="F19" s="108" t="s">
-        <v>229</v>
+      <c r="F19" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G19" s="49"/>
       <c r="H19" s="49"/>
@@ -4543,10 +4558,10 @@
         <v>10</v>
       </c>
       <c r="E20" s="102" t="s">
-        <v>229</v>
-      </c>
-      <c r="F20" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F20" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
@@ -4570,7 +4585,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="102" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="49"/>
@@ -4595,10 +4610,10 @@
         <v>5</v>
       </c>
       <c r="E22" s="102" t="s">
-        <v>229</v>
-      </c>
-      <c r="F22" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F22" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
@@ -4620,10 +4635,10 @@
         <v>10</v>
       </c>
       <c r="E23" s="102" t="s">
-        <v>229</v>
-      </c>
-      <c r="F23" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F23" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
@@ -4645,7 +4660,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="102" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F24" s="54"/>
       <c r="G24" s="49"/>
@@ -4670,10 +4685,10 @@
         <v>10</v>
       </c>
       <c r="E25" s="100" t="s">
-        <v>229</v>
-      </c>
-      <c r="F25" s="108" t="s">
-        <v>293</v>
+        <v>228</v>
+      </c>
+      <c r="F25" s="107" t="s">
+        <v>279</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
@@ -4697,8 +4712,8 @@
         <v>15</v>
       </c>
       <c r="E26" s="49"/>
-      <c r="F26" s="108" t="s">
-        <v>293</v>
+      <c r="F26" s="107" t="s">
+        <v>279</v>
       </c>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
@@ -4722,10 +4737,10 @@
         <v>10</v>
       </c>
       <c r="E27" s="102" t="s">
-        <v>229</v>
-      </c>
-      <c r="F27" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="F27" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
@@ -4749,7 +4764,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="102" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F28" s="54"/>
       <c r="G28" s="49"/>
@@ -4774,8 +4789,8 @@
         <v>4</v>
       </c>
       <c r="E29" s="49"/>
-      <c r="F29" s="108" t="s">
-        <v>293</v>
+      <c r="F29" s="107" t="s">
+        <v>279</v>
       </c>
       <c r="G29" s="49"/>
       <c r="H29" s="49"/>
@@ -4799,8 +4814,8 @@
         <v>15</v>
       </c>
       <c r="E30" s="49"/>
-      <c r="F30" s="108" t="s">
-        <v>229</v>
+      <c r="F30" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
@@ -4823,11 +4838,11 @@
       <c r="D31" s="61">
         <v>10</v>
       </c>
-      <c r="E31" s="108" t="s">
-        <v>229</v>
-      </c>
-      <c r="F31" s="108" t="s">
-        <v>229</v>
+      <c r="E31" s="107" t="s">
+        <v>228</v>
+      </c>
+      <c r="F31" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
@@ -4869,11 +4884,11 @@
       <c r="D33" s="61">
         <v>10</v>
       </c>
-      <c r="E33" s="108" t="s">
-        <v>229</v>
-      </c>
-      <c r="F33" s="108" t="s">
-        <v>229</v>
+      <c r="E33" s="107" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
@@ -4915,11 +4930,11 @@
       <c r="D35" s="61">
         <v>10</v>
       </c>
-      <c r="E35" s="108" t="s">
-        <v>229</v>
-      </c>
-      <c r="F35" s="108" t="s">
-        <v>229</v>
+      <c r="E35" s="107" t="s">
+        <v>228</v>
+      </c>
+      <c r="F35" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G35" s="49"/>
       <c r="H35" s="49"/>
@@ -4963,7 +4978,7 @@
       </c>
       <c r="E37" s="49"/>
       <c r="F37" s="56" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
@@ -4984,11 +4999,11 @@
       <c r="D38" s="61">
         <v>10</v>
       </c>
-      <c r="E38" s="108" t="s">
-        <v>229</v>
-      </c>
-      <c r="F38" s="108" t="s">
-        <v>229</v>
+      <c r="E38" s="107" t="s">
+        <v>228</v>
+      </c>
+      <c r="F38" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
@@ -5031,8 +5046,8 @@
         <v>4</v>
       </c>
       <c r="E40" s="49"/>
-      <c r="F40" s="108" t="s">
-        <v>229</v>
+      <c r="F40" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G40" s="49"/>
       <c r="H40" s="49"/>
@@ -5054,8 +5069,8 @@
         <v>15</v>
       </c>
       <c r="E41" s="49"/>
-      <c r="F41" s="108" t="s">
-        <v>229</v>
+      <c r="F41" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G41" s="49"/>
       <c r="H41" s="49"/>
@@ -5077,8 +5092,8 @@
         <v>15</v>
       </c>
       <c r="E42" s="49"/>
-      <c r="F42" s="108" t="s">
-        <v>293</v>
+      <c r="F42" s="107" t="s">
+        <v>279</v>
       </c>
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
@@ -5100,8 +5115,8 @@
         <v>10</v>
       </c>
       <c r="E43" s="49"/>
-      <c r="F43" s="108" t="s">
-        <v>229</v>
+      <c r="F43" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G43" s="49"/>
       <c r="H43" s="49"/>
@@ -5144,8 +5159,8 @@
         <v>15</v>
       </c>
       <c r="E45" s="49"/>
-      <c r="F45" s="108" t="s">
-        <v>293</v>
+      <c r="F45" s="107" t="s">
+        <v>279</v>
       </c>
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
@@ -5167,8 +5182,8 @@
         <v>4</v>
       </c>
       <c r="E46" s="49"/>
-      <c r="F46" s="108" t="s">
-        <v>229</v>
+      <c r="F46" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G46" s="49"/>
       <c r="H46" s="49"/>
@@ -5190,8 +5205,8 @@
         <v>4</v>
       </c>
       <c r="E47" s="49"/>
-      <c r="F47" s="108" t="s">
-        <v>229</v>
+      <c r="F47" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G47" s="49"/>
       <c r="H47" s="49"/>
@@ -5213,8 +5228,8 @@
         <v>10</v>
       </c>
       <c r="E48" s="49"/>
-      <c r="F48" s="108" t="s">
-        <v>229</v>
+      <c r="F48" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
@@ -5236,8 +5251,8 @@
         <v>15</v>
       </c>
       <c r="E49" s="49"/>
-      <c r="F49" s="108" t="s">
-        <v>229</v>
+      <c r="F49" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G49" s="49"/>
       <c r="H49" s="49"/>
@@ -5259,8 +5274,8 @@
         <v>15</v>
       </c>
       <c r="E50" s="49"/>
-      <c r="F50" s="108" t="s">
-        <v>229</v>
+      <c r="F50" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G50" s="49"/>
       <c r="H50" s="49"/>
@@ -5303,8 +5318,8 @@
         <v>4</v>
       </c>
       <c r="E52" s="49"/>
-      <c r="F52" s="108" t="s">
-        <v>229</v>
+      <c r="F52" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G52" s="49"/>
       <c r="H52" s="49"/>
@@ -5326,8 +5341,8 @@
         <v>10</v>
       </c>
       <c r="E53" s="49"/>
-      <c r="F53" s="108" t="s">
-        <v>229</v>
+      <c r="F53" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G53" s="49"/>
       <c r="H53" s="49"/>
@@ -5349,8 +5364,8 @@
         <v>10</v>
       </c>
       <c r="E54" s="49"/>
-      <c r="F54" s="108" t="s">
-        <v>229</v>
+      <c r="F54" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G54" s="49"/>
       <c r="H54" s="49"/>
@@ -5393,8 +5408,8 @@
         <v>5</v>
       </c>
       <c r="E56" s="49"/>
-      <c r="F56" s="108" t="s">
-        <v>229</v>
+      <c r="F56" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G56" s="49"/>
       <c r="H56" s="49"/>
@@ -5416,8 +5431,8 @@
         <v>10</v>
       </c>
       <c r="E57" s="49"/>
-      <c r="F57" s="108" t="s">
-        <v>229</v>
+      <c r="F57" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G57" s="49"/>
       <c r="H57" s="49"/>
@@ -5439,8 +5454,8 @@
         <v>50</v>
       </c>
       <c r="E58" s="49"/>
-      <c r="F58" s="108" t="s">
-        <v>229</v>
+      <c r="F58" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G58" s="49"/>
       <c r="H58" s="49"/>
@@ -5462,8 +5477,8 @@
         <v>2</v>
       </c>
       <c r="E59" s="49"/>
-      <c r="F59" s="108" t="s">
-        <v>229</v>
+      <c r="F59" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G59" s="49"/>
       <c r="H59" s="49"/>
@@ -5485,8 +5500,8 @@
         <v>3</v>
       </c>
       <c r="E60" s="49"/>
-      <c r="F60" s="108" t="s">
-        <v>229</v>
+      <c r="F60" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G60" s="49"/>
       <c r="H60" s="49"/>
@@ -5508,8 +5523,8 @@
         <v>2</v>
       </c>
       <c r="E61" s="49"/>
-      <c r="F61" s="108" t="s">
-        <v>229</v>
+      <c r="F61" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
@@ -5531,8 +5546,8 @@
         <v>10</v>
       </c>
       <c r="E62" s="49"/>
-      <c r="F62" s="108" t="s">
-        <v>229</v>
+      <c r="F62" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
@@ -5554,8 +5569,8 @@
         <v>6</v>
       </c>
       <c r="E63" s="49"/>
-      <c r="F63" s="108" t="s">
-        <v>229</v>
+      <c r="F63" s="107" t="s">
+        <v>228</v>
       </c>
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
@@ -5925,7 +5940,7 @@
       <c r="Z78" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:E78">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E78">
     <sortCondition ref="A2:A78"/>
   </sortState>
   <phoneticPr fontId="38" type="noConversion"/>

</xml_diff>

<commit_message>
update schedule pts page
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CB1383-BC85-46EF-BBA7-A27A8748CA21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AA19E6-CB02-4F51-85AB-E83B9634975E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30465" yWindow="1230" windowWidth="21090" windowHeight="13665" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="570" windowWidth="24165" windowHeight="14295" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -2366,7 +2366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -3357,7 +3357,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="99">
         <v>7</v>
       </c>
@@ -3624,8 +3624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD78"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K67" sqref="K67:K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4340,7 +4340,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="58">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="B12" s="65" t="s">
         <v>162</v>
@@ -4415,22 +4415,20 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="58">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>163</v>
-      </c>
-      <c r="C15" s="73" t="s">
-        <v>23</v>
+        <v>126</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D15" s="61">
-        <v>15</v>
-      </c>
-      <c r="E15" s="98" t="s">
-        <v>228</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E15" s="49"/>
       <c r="F15" s="107" t="s">
-        <v>228</v>
+        <v>279</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
@@ -4442,20 +4440,18 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="58">
-        <v>5.0999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="63" t="s">
-        <v>66</v>
+        <v>125</v>
+      </c>
+      <c r="C16" s="60" t="s">
+        <v>14</v>
       </c>
       <c r="D16" s="61">
-        <v>10</v>
-      </c>
-      <c r="E16" s="98" t="s">
-        <v>228</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E16" s="49"/>
       <c r="F16" s="107" t="s">
         <v>228</v>
       </c>
@@ -4469,21 +4465,23 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="58">
-        <v>5.2</v>
+        <v>4.5</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="62">
-        <v>2</v>
+        <v>163</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="61">
+        <v>15</v>
       </c>
       <c r="E17" s="98" t="s">
         <v>228</v>
       </c>
-      <c r="F17" s="53"/>
+      <c r="F17" s="107" t="s">
+        <v>228</v>
+      </c>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
@@ -4494,16 +4492,16 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="58">
-        <v>5.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" s="73" t="s">
-        <v>23</v>
+        <v>139</v>
+      </c>
+      <c r="C18" s="63" t="s">
+        <v>66</v>
       </c>
       <c r="D18" s="61">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E18" s="98" t="s">
         <v>228</v>
@@ -4521,21 +4519,21 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="58">
-        <v>6.1</v>
+        <v>5.2</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="61">
-        <v>50</v>
-      </c>
-      <c r="E19" s="49"/>
-      <c r="F19" s="107" t="s">
-        <v>228</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="C19" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="62">
+        <v>2</v>
+      </c>
+      <c r="E19" s="98" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" s="53"/>
       <c r="G19" s="49"/>
       <c r="H19" s="49"/>
       <c r="I19" s="49"/>
@@ -4546,18 +4544,18 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="58">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="72" t="s">
-        <v>66</v>
+        <v>164</v>
+      </c>
+      <c r="C20" s="73" t="s">
+        <v>23</v>
       </c>
       <c r="D20" s="61">
-        <v>10</v>
-      </c>
-      <c r="E20" s="102" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="98" t="s">
         <v>228</v>
       </c>
       <c r="F20" s="107" t="s">
@@ -4573,21 +4571,23 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="58">
-        <v>6.2</v>
+        <v>6.1</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>142</v>
-      </c>
-      <c r="C21" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="62">
-        <v>2</v>
+        <v>141</v>
+      </c>
+      <c r="C21" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="61">
+        <v>10</v>
       </c>
       <c r="E21" s="102" t="s">
         <v>228</v>
       </c>
-      <c r="F21" s="50"/>
+      <c r="F21" s="107" t="s">
+        <v>228</v>
+      </c>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
       <c r="I21" s="49"/>
@@ -4598,23 +4598,21 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="58">
-        <v>6.3</v>
-      </c>
-      <c r="B22" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="61">
-        <v>5</v>
+        <v>6.2</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="62">
+        <v>2</v>
       </c>
       <c r="E22" s="102" t="s">
         <v>228</v>
       </c>
-      <c r="F22" s="107" t="s">
-        <v>228</v>
-      </c>
+      <c r="F22" s="50"/>
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
@@ -4623,20 +4621,18 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="58">
-        <v>7.1</v>
+        <v>6.3</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>143</v>
-      </c>
-      <c r="C23" s="72" t="s">
-        <v>66</v>
+        <v>124</v>
+      </c>
+      <c r="C23" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D23" s="61">
-        <v>10</v>
-      </c>
-      <c r="E23" s="102" t="s">
-        <v>228</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E23" s="49"/>
       <c r="F23" s="107" t="s">
         <v>228</v>
       </c>
@@ -4648,21 +4644,21 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="58">
-        <v>7.2</v>
+        <v>6.4</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>144</v>
-      </c>
-      <c r="C24" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="62">
-        <v>2</v>
-      </c>
-      <c r="E24" s="102" t="s">
-        <v>228</v>
-      </c>
-      <c r="F24" s="54"/>
+        <v>123</v>
+      </c>
+      <c r="C24" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="61">
+        <v>15</v>
+      </c>
+      <c r="E24" s="49"/>
+      <c r="F24" s="107" t="s">
+        <v>279</v>
+      </c>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
       <c r="I24" s="49"/>
@@ -4673,22 +4669,20 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="58">
-        <v>7.3</v>
+        <v>6.5</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>165</v>
-      </c>
-      <c r="C25" s="75" t="s">
-        <v>14</v>
+        <v>78</v>
+      </c>
+      <c r="C25" s="74" t="s">
+        <v>13</v>
       </c>
       <c r="D25" s="61">
-        <v>10</v>
-      </c>
-      <c r="E25" s="100" t="s">
-        <v>228</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E25" s="49"/>
       <c r="F25" s="107" t="s">
-        <v>279</v>
+        <v>228</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
@@ -4700,20 +4694,22 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="58">
-        <v>8.1</v>
-      </c>
-      <c r="B26" s="65" t="s">
-        <v>166</v>
-      </c>
-      <c r="C26" s="76" t="s">
-        <v>23</v>
+        <v>6.6</v>
+      </c>
+      <c r="B26" s="67" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="77" t="s">
+        <v>24</v>
       </c>
       <c r="D26" s="61">
-        <v>15</v>
-      </c>
-      <c r="E26" s="49"/>
+        <v>5</v>
+      </c>
+      <c r="E26" s="102" t="s">
+        <v>228</v>
+      </c>
       <c r="F26" s="107" t="s">
-        <v>279</v>
+        <v>228</v>
       </c>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
@@ -4725,10 +4721,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="58">
-        <v>8.1</v>
+        <v>7.1</v>
       </c>
       <c r="B27" s="65" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C27" s="72" t="s">
         <v>66</v>
@@ -4752,10 +4748,10 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="58">
-        <v>8.1999999999999993</v>
+        <v>7.2</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C28" s="64" t="s">
         <v>112</v>
@@ -4777,18 +4773,20 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="58">
-        <v>8.3000000000000007</v>
+        <v>7.3</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>126</v>
-      </c>
-      <c r="C29" s="71" t="s">
-        <v>12</v>
+        <v>165</v>
+      </c>
+      <c r="C29" s="75" t="s">
+        <v>14</v>
       </c>
       <c r="D29" s="61">
-        <v>4</v>
-      </c>
-      <c r="E29" s="49"/>
+        <v>10</v>
+      </c>
+      <c r="E29" s="100" t="s">
+        <v>228</v>
+      </c>
       <c r="F29" s="107" t="s">
         <v>279</v>
       </c>
@@ -4802,18 +4800,20 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="58">
-        <v>8.4</v>
+        <v>8.1</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="C30" s="60" t="s">
-        <v>14</v>
+        <v>145</v>
+      </c>
+      <c r="C30" s="72" t="s">
+        <v>66</v>
       </c>
       <c r="D30" s="61">
-        <v>15</v>
-      </c>
-      <c r="E30" s="49"/>
+        <v>10</v>
+      </c>
+      <c r="E30" s="102" t="s">
+        <v>228</v>
+      </c>
       <c r="F30" s="107" t="s">
         <v>228</v>
       </c>
@@ -4827,23 +4827,21 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="58">
-        <v>9.1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>147</v>
-      </c>
-      <c r="C31" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="61">
-        <v>10</v>
-      </c>
-      <c r="E31" s="107" t="s">
-        <v>228</v>
-      </c>
-      <c r="F31" s="107" t="s">
-        <v>228</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="C31" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="62">
+        <v>2</v>
+      </c>
+      <c r="E31" s="102" t="s">
+        <v>228</v>
+      </c>
+      <c r="F31" s="54"/>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
       <c r="I31" s="49"/>
@@ -4852,19 +4850,21 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="58">
-        <v>9.1999999999999993</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D32" s="62">
-        <v>2</v>
+        <v>166</v>
+      </c>
+      <c r="C32" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="61">
+        <v>15</v>
       </c>
       <c r="E32" s="49"/>
-      <c r="F32" s="55"/>
+      <c r="F32" s="107" t="s">
+        <v>279</v>
+      </c>
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
       <c r="I32" s="49"/>
@@ -4873,10 +4873,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="58">
-        <v>10.1</v>
+        <v>9.1</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C33" s="72" t="s">
         <v>66</v>
@@ -4898,10 +4898,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="58">
-        <v>10.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C34" s="64" t="s">
         <v>112</v>
@@ -4919,10 +4919,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="58">
-        <v>11.1</v>
+        <v>10.1</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C35" s="72" t="s">
         <v>66</v>
@@ -4944,10 +4944,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="58">
-        <v>11.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C36" s="64" t="s">
         <v>112</v>
@@ -4956,7 +4956,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
+      <c r="F36" s="55"/>
       <c r="G36" s="49"/>
       <c r="H36" s="49"/>
       <c r="I36" s="49"/>
@@ -4965,7 +4965,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="58">
-        <v>11.3</v>
+        <v>10.3</v>
       </c>
       <c r="B37" s="67" t="s">
         <v>103</v>
@@ -4988,10 +4988,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="58">
-        <v>12.1</v>
+        <v>11.1</v>
       </c>
       <c r="B38" s="65" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C38" s="72" t="s">
         <v>66</v>
@@ -5013,10 +5013,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="58">
-        <v>12.2</v>
+        <v>11.2</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C39" s="64" t="s">
         <v>112</v>
@@ -5025,7 +5025,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="49"/>
-      <c r="F39" s="50"/>
+      <c r="F39" s="49"/>
       <c r="G39" s="49"/>
       <c r="H39" s="49"/>
       <c r="I39" s="49"/>
@@ -5034,16 +5034,16 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="58">
-        <v>12.5</v>
-      </c>
-      <c r="B40" s="65" t="s">
-        <v>124</v>
-      </c>
-      <c r="C40" s="71" t="s">
-        <v>12</v>
+        <v>11.3</v>
+      </c>
+      <c r="B40" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="73" t="s">
+        <v>23</v>
       </c>
       <c r="D40" s="61">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E40" s="49"/>
       <c r="F40" s="107" t="s">
@@ -5057,18 +5057,20 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="58">
-        <v>12.6</v>
-      </c>
-      <c r="B41" s="67" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="73" t="s">
-        <v>23</v>
+        <v>12.1</v>
+      </c>
+      <c r="B41" s="65" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="72" t="s">
+        <v>66</v>
       </c>
       <c r="D41" s="61">
-        <v>15</v>
-      </c>
-      <c r="E41" s="49"/>
+        <v>10</v>
+      </c>
+      <c r="E41" s="107" t="s">
+        <v>228</v>
+      </c>
       <c r="F41" s="107" t="s">
         <v>228</v>
       </c>
@@ -5080,21 +5082,19 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="58">
-        <v>12.7</v>
+        <v>12.2</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>123</v>
-      </c>
-      <c r="C42" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="61">
-        <v>15</v>
+        <v>154</v>
+      </c>
+      <c r="C42" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="62">
+        <v>2</v>
       </c>
       <c r="E42" s="49"/>
-      <c r="F42" s="107" t="s">
-        <v>279</v>
-      </c>
+      <c r="F42" s="50"/>
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
       <c r="I42" s="49"/>
@@ -5103,16 +5103,16 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="58">
-        <v>13.1</v>
+        <v>12.2</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="C43" s="72" t="s">
-        <v>66</v>
+        <v>127</v>
+      </c>
+      <c r="C43" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D43" s="61">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E43" s="49"/>
       <c r="F43" s="107" t="s">
@@ -5126,19 +5126,21 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="58">
-        <v>13.2</v>
+        <v>12.3</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>156</v>
-      </c>
-      <c r="C44" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D44" s="62">
-        <v>2</v>
+        <v>128</v>
+      </c>
+      <c r="C44" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="61">
+        <v>15</v>
       </c>
       <c r="E44" s="49"/>
-      <c r="F44" s="57"/>
+      <c r="F44" s="107" t="s">
+        <v>228</v>
+      </c>
       <c r="G44" s="49"/>
       <c r="H44" s="49"/>
       <c r="I44" s="49"/>
@@ -5147,20 +5149,20 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="58">
-        <v>13.5</v>
-      </c>
-      <c r="B45" s="67" t="s">
-        <v>106</v>
-      </c>
-      <c r="C45" s="73" t="s">
-        <v>23</v>
+        <v>13.1</v>
+      </c>
+      <c r="B45" s="65" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" s="72" t="s">
+        <v>66</v>
       </c>
       <c r="D45" s="61">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E45" s="49"/>
       <c r="F45" s="107" t="s">
-        <v>279</v>
+        <v>228</v>
       </c>
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
@@ -5170,21 +5172,19 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="58">
-        <v>14.1</v>
+        <v>13.2</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="61">
-        <v>4</v>
+        <v>156</v>
+      </c>
+      <c r="C46" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" s="62">
+        <v>2</v>
       </c>
       <c r="E46" s="49"/>
-      <c r="F46" s="107" t="s">
-        <v>228</v>
-      </c>
+      <c r="F46" s="57"/>
       <c r="G46" s="49"/>
       <c r="H46" s="49"/>
       <c r="I46" s="49"/>
@@ -5193,20 +5193,20 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="58">
-        <v>14.1</v>
-      </c>
-      <c r="B47" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="C47" s="71" t="s">
-        <v>12</v>
+        <v>13.3</v>
+      </c>
+      <c r="B47" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="73" t="s">
+        <v>23</v>
       </c>
       <c r="D47" s="61">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E47" s="49"/>
       <c r="F47" s="107" t="s">
-        <v>228</v>
+        <v>279</v>
       </c>
       <c r="G47" s="49"/>
       <c r="H47" s="49"/>
@@ -5242,18 +5242,16 @@
         <v>14.2</v>
       </c>
       <c r="B49" s="65" t="s">
-        <v>128</v>
-      </c>
-      <c r="C49" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="61">
-        <v>15</v>
+        <v>158</v>
+      </c>
+      <c r="C49" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="62">
+        <v>2</v>
       </c>
       <c r="E49" s="49"/>
-      <c r="F49" s="107" t="s">
-        <v>228</v>
-      </c>
+      <c r="F49" s="57"/>
       <c r="G49" s="49"/>
       <c r="H49" s="49"/>
       <c r="I49" s="49"/>
@@ -5262,16 +5260,16 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="58">
-        <v>14.2</v>
+        <v>14.3</v>
       </c>
       <c r="B50" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="C50" s="60" t="s">
-        <v>14</v>
+        <v>129</v>
+      </c>
+      <c r="C50" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D50" s="61">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E50" s="49"/>
       <c r="F50" s="107" t="s">
@@ -5285,19 +5283,21 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="58">
-        <v>14.2</v>
+        <v>14.4</v>
       </c>
       <c r="B51" s="65" t="s">
-        <v>158</v>
-      </c>
-      <c r="C51" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D51" s="62">
-        <v>2</v>
+        <v>130</v>
+      </c>
+      <c r="C51" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="61">
+        <v>15</v>
       </c>
       <c r="E51" s="49"/>
-      <c r="F51" s="57"/>
+      <c r="F51" s="107" t="s">
+        <v>228</v>
+      </c>
       <c r="G51" s="49"/>
       <c r="H51" s="49"/>
       <c r="I51" s="49"/>
@@ -5308,14 +5308,14 @@
       <c r="A52" s="58">
         <v>15.1</v>
       </c>
-      <c r="B52" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="71" t="s">
-        <v>12</v>
+      <c r="B52" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" s="72" t="s">
+        <v>66</v>
       </c>
       <c r="D52" s="61">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E52" s="49"/>
       <c r="F52" s="107" t="s">
@@ -5329,21 +5329,19 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="58">
-        <v>15.1</v>
+        <v>15.2</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>159</v>
-      </c>
-      <c r="C53" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="D53" s="61">
-        <v>10</v>
+        <v>160</v>
+      </c>
+      <c r="C53" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" s="62">
+        <v>2</v>
       </c>
       <c r="E53" s="49"/>
-      <c r="F53" s="107" t="s">
-        <v>228</v>
-      </c>
+      <c r="F53" s="49"/>
       <c r="G53" s="49"/>
       <c r="H53" s="49"/>
       <c r="I53" s="49"/>
@@ -5352,16 +5350,16 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="58">
-        <v>15.2</v>
+        <v>15.3</v>
       </c>
       <c r="B54" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="C54" s="60" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="C54" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D54" s="61">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E54" s="49"/>
       <c r="F54" s="107" t="s">
@@ -5375,19 +5373,21 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="58">
-        <v>15.2</v>
-      </c>
-      <c r="B55" s="65" t="s">
-        <v>160</v>
-      </c>
-      <c r="C55" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D55" s="62">
-        <v>2</v>
+        <v>15.4</v>
+      </c>
+      <c r="B55" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="61">
+        <v>10</v>
       </c>
       <c r="E55" s="49"/>
-      <c r="F55" s="49"/>
+      <c r="F55" s="107" t="s">
+        <v>228</v>
+      </c>
       <c r="G55" s="49"/>
       <c r="H55" s="49"/>
       <c r="I55" s="49"/>
@@ -5940,8 +5940,8 @@
       <c r="Z78" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E78">
-    <sortCondition ref="A2:A78"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F83">
+    <sortCondition ref="A2:A83"/>
   </sortState>
   <phoneticPr fontId="38" type="noConversion"/>
   <conditionalFormatting sqref="R2:R8">

</xml_diff>

<commit_message>
add wk04 and fix date typo on schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B7092C-1F11-4AC4-BE25-442EEC83A52A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC628B07-B0F9-47CF-B6E7-DA61F06F8EC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30375" yWindow="450" windowWidth="24165" windowHeight="14295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28815" yWindow="90" windowWidth="24165" windowHeight="14295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -797,9 +797,6 @@
     <t>[hw03_data_management](hw/hw03_data_management.html) (Due 9/14 )</t>
   </si>
   <si>
-    <t>[hw04_univ_graphing](hw/hw04_univ_graphing.html) (Due 9/28 )</t>
-  </si>
-  <si>
     <t>[Poster prep Stage I](project.html)* (Draft Due 9/17, PR 9/19, Final 9/21 )</t>
   </si>
   <si>
@@ -1146,6 +1143,9 @@
     <t>Quiz 04 (Due 09/15 ) 
 [[10am]](https://forms.gle/nmKqV5W4WCXMyPhg8)
 [[12pm]](https://forms.gle/achD9kHHbAMWezMu6)</t>
+  </si>
+  <si>
+    <t>[hw04_univ_graphing](hw/hw04_univ_graphing.html) (Due 9/21 )</t>
   </si>
 </sst>
 </file>
@@ -2366,8 +2366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2395,7 +2395,7 @@
         <v>68</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>101</v>
@@ -2421,7 +2421,7 @@
         <v>69</v>
       </c>
       <c r="G2" s="94" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H2" s="95" t="s">
         <v>211</v>
@@ -2440,7 +2440,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2465,7 +2465,7 @@
         <v>84</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2491,13 +2491,13 @@
         <v>113</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F8" s="35">
         <v>1.3</v>
       </c>
       <c r="G8" s="109" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H8" s="95" t="s">
         <v>212</v>
@@ -2511,7 +2511,7 @@
         <v>114</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="110" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H12" s="95" t="s">
         <v>213</v>
@@ -2596,10 +2596,10 @@
         <v>2.1</v>
       </c>
       <c r="G15" s="110" t="s">
+        <v>297</v>
+      </c>
+      <c r="H15" s="95" t="s">
         <v>298</v>
-      </c>
-      <c r="H15" s="95" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2613,7 +2613,7 @@
         <v>88</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2627,7 +2627,7 @@
       <c r="F17" s="84"/>
       <c r="G17" s="104"/>
       <c r="H17" s="82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2638,19 +2638,19 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>89</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G18" s="110" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H18" s="95" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2678,10 +2678,10 @@
         <v>115</v>
       </c>
       <c r="G20" s="110" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H20" s="101" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2709,7 +2709,7 @@
       <c r="F22" s="87"/>
       <c r="G22" s="105"/>
       <c r="H22" s="85" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2720,7 +2720,7 @@
         <v>117</v>
       </c>
       <c r="H23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2734,7 +2734,7 @@
       <c r="F24" s="84"/>
       <c r="G24" s="104"/>
       <c r="H24" s="82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2748,13 +2748,13 @@
         <v>205</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F25" s="35">
         <v>4</v>
       </c>
       <c r="G25" s="110" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2765,7 +2765,7 @@
         <v>206</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2793,10 +2793,10 @@
         <v>4.7</v>
       </c>
       <c r="G28" s="110" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H28" s="80" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2807,10 +2807,10 @@
         <v>74</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2818,7 +2818,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F30" s="35">
         <v>6.1</v>
@@ -2841,10 +2841,10 @@
         <v>6.2</v>
       </c>
       <c r="G31" s="110" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H31" s="95" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2852,7 +2852,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E32" s="42" t="s">
         <v>92</v>
@@ -2866,7 +2866,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E33" s="42" t="s">
         <v>93</v>
@@ -2883,7 +2883,7 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E34" s="42" t="s">
         <v>98</v>
@@ -2892,7 +2892,7 @@
         <v>6.5</v>
       </c>
       <c r="G34" s="110" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2912,10 +2912,10 @@
         <v>7</v>
       </c>
       <c r="G35" s="110" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H35" s="95" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2929,7 +2929,7 @@
         <v>96</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2937,10 +2937,10 @@
         <v>11.3</v>
       </c>
       <c r="D37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2957,13 +2957,13 @@
         <v>95</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G38" s="110" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H38" s="80" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2971,7 +2971,7 @@
         <v>12.2</v>
       </c>
       <c r="D39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E39" s="42" t="s">
         <v>100</v>
@@ -2989,7 +2989,7 @@
       <c r="F40" s="84"/>
       <c r="G40" s="104"/>
       <c r="H40" s="82" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3000,16 +3000,16 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E41" s="42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G41" s="110" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3020,7 +3020,7 @@
         <v>107</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3028,7 +3028,7 @@
         <v>14</v>
       </c>
       <c r="D43" s="88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E43" s="89"/>
       <c r="F43" s="90"/>
@@ -3049,7 +3049,7 @@
         <v>8.4</v>
       </c>
       <c r="G44" s="111" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3063,7 +3063,7 @@
       <c r="F45" s="84"/>
       <c r="G45" s="104"/>
       <c r="H45" s="82" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3080,10 +3080,10 @@
         <v>97</v>
       </c>
       <c r="G46" s="111" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3171,7 +3171,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="108" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -3188,13 +3188,13 @@
         <v>179</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>178</v>
@@ -3203,7 +3203,7 @@
         <v>167</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3221,7 +3221,7 @@
         <v>173</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
@@ -3230,7 +3230,7 @@
         <v>172</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>171</v>
@@ -3252,7 +3252,7 @@
         <v>177</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>186</v>
@@ -3261,7 +3261,7 @@
         <v>180</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>169</v>
@@ -3282,7 +3282,7 @@
         <v>176</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>185</v>
@@ -3306,22 +3306,22 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>183</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>184</v>
@@ -3336,28 +3336,28 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="99">
         <v>7</v>
       </c>
@@ -3369,22 +3369,22 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3402,13 +3402,13 @@
         <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3738,10 +3738,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F2" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G2" s="50"/>
       <c r="H2" s="31" t="s">
@@ -3817,10 +3817,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="92" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F3" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G3" s="49"/>
       <c r="H3" s="47" t="s">
@@ -3896,7 +3896,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="50"/>
@@ -3973,10 +3973,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F5" s="107" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="4" t="s">
@@ -4045,10 +4045,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F6" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="4" t="s">
@@ -4124,7 +4124,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -4201,10 +4201,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F8" s="107" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="4"/>
@@ -4267,7 +4267,7 @@
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G9" s="50"/>
       <c r="H9" s="50"/>
@@ -4304,10 +4304,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="96" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F10" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="50"/>
@@ -4329,7 +4329,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="96" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="49"/>
@@ -4352,10 +4352,10 @@
         <v>15</v>
       </c>
       <c r="E12" s="96" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F12" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
@@ -4377,10 +4377,10 @@
         <v>10</v>
       </c>
       <c r="E13" s="98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F13" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G13" s="49"/>
       <c r="H13" s="49"/>
@@ -4402,7 +4402,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="49"/>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="E15" s="49"/>
       <c r="F15" s="107" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
@@ -4453,7 +4453,7 @@
       </c>
       <c r="E16" s="49"/>
       <c r="F16" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
@@ -4477,10 +4477,10 @@
         <v>15</v>
       </c>
       <c r="E17" s="98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F17" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
@@ -4504,10 +4504,10 @@
         <v>10</v>
       </c>
       <c r="E18" s="98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F18" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
@@ -4531,7 +4531,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F19" s="53"/>
       <c r="G19" s="49"/>
@@ -4556,10 +4556,10 @@
         <v>15</v>
       </c>
       <c r="E20" s="98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F20" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
@@ -4583,10 +4583,10 @@
         <v>10</v>
       </c>
       <c r="E21" s="102" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F21" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
@@ -4610,7 +4610,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="102" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F22" s="50"/>
       <c r="G22" s="49"/>
@@ -4634,7 +4634,7 @@
       </c>
       <c r="E23" s="49"/>
       <c r="F23" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="E24" s="49"/>
       <c r="F24" s="107" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
@@ -4682,7 +4682,7 @@
       </c>
       <c r="E25" s="49"/>
       <c r="F25" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
@@ -4706,10 +4706,10 @@
         <v>5</v>
       </c>
       <c r="E26" s="102" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F26" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
@@ -4733,10 +4733,10 @@
         <v>10</v>
       </c>
       <c r="E27" s="102" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F27" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
@@ -4760,7 +4760,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="102" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F28" s="54"/>
       <c r="G28" s="49"/>
@@ -4785,10 +4785,10 @@
         <v>10</v>
       </c>
       <c r="E29" s="100" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F29" s="107" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G29" s="49"/>
       <c r="H29" s="49"/>
@@ -4812,10 +4812,10 @@
         <v>10</v>
       </c>
       <c r="E30" s="102" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F30" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
@@ -4839,7 +4839,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="102" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F31" s="54"/>
       <c r="G31" s="49"/>
@@ -4863,7 +4863,7 @@
       </c>
       <c r="E32" s="49"/>
       <c r="F32" s="107" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
@@ -4885,10 +4885,10 @@
         <v>10</v>
       </c>
       <c r="E33" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F33" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
@@ -4931,10 +4931,10 @@
         <v>10</v>
       </c>
       <c r="E35" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F35" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G35" s="49"/>
       <c r="H35" s="49"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="E37" s="49"/>
       <c r="F37" s="56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
@@ -5000,10 +5000,10 @@
         <v>10</v>
       </c>
       <c r="E38" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F38" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="E40" s="49"/>
       <c r="F40" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G40" s="49"/>
       <c r="H40" s="49"/>
@@ -5069,10 +5069,10 @@
         <v>10</v>
       </c>
       <c r="E41" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F41" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G41" s="49"/>
       <c r="H41" s="49"/>
@@ -5116,7 +5116,7 @@
       </c>
       <c r="E43" s="49"/>
       <c r="F43" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G43" s="49"/>
       <c r="H43" s="49"/>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="E44" s="49"/>
       <c r="F44" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G44" s="49"/>
       <c r="H44" s="49"/>
@@ -5162,7 +5162,7 @@
       </c>
       <c r="E45" s="49"/>
       <c r="F45" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="E47" s="49"/>
       <c r="F47" s="107" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G47" s="49"/>
       <c r="H47" s="49"/>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="E48" s="49"/>
       <c r="F48" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
@@ -5273,7 +5273,7 @@
       </c>
       <c r="E50" s="49"/>
       <c r="F50" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G50" s="49"/>
       <c r="H50" s="49"/>
@@ -5296,7 +5296,7 @@
       </c>
       <c r="E51" s="49"/>
       <c r="F51" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G51" s="49"/>
       <c r="H51" s="49"/>
@@ -5319,7 +5319,7 @@
       </c>
       <c r="E52" s="49"/>
       <c r="F52" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G52" s="49"/>
       <c r="H52" s="49"/>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="E54" s="49"/>
       <c r="F54" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G54" s="49"/>
       <c r="H54" s="49"/>
@@ -5386,7 +5386,7 @@
       </c>
       <c r="E55" s="49"/>
       <c r="F55" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G55" s="49"/>
       <c r="H55" s="49"/>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="E56" s="49"/>
       <c r="F56" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G56" s="49"/>
       <c r="H56" s="49"/>
@@ -5432,7 +5432,7 @@
       </c>
       <c r="E57" s="49"/>
       <c r="F57" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G57" s="49"/>
       <c r="H57" s="49"/>
@@ -5455,7 +5455,7 @@
       </c>
       <c r="E58" s="49"/>
       <c r="F58" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G58" s="49"/>
       <c r="H58" s="49"/>
@@ -5478,7 +5478,7 @@
       </c>
       <c r="E59" s="49"/>
       <c r="F59" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G59" s="49"/>
       <c r="H59" s="49"/>
@@ -5501,7 +5501,7 @@
       </c>
       <c r="E60" s="49"/>
       <c r="F60" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G60" s="49"/>
       <c r="H60" s="49"/>
@@ -5524,7 +5524,7 @@
       </c>
       <c r="E61" s="49"/>
       <c r="F61" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="E62" s="49"/>
       <c r="F62" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
@@ -5570,7 +5570,7 @@
       </c>
       <c r="E63" s="49"/>
       <c r="F63" s="107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>

</xml_diff>

<commit_message>
fix quiz 5 links
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137FA092-B19F-4A4C-958C-2787CE07D9B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACADF2A2-1A6B-4490-8098-B6BDEABC3D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="points" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">points!$A$1:$J$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">points!$A$1:$J$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="301">
   <si>
     <t>Finals Week</t>
   </si>
@@ -902,11 +902,6 @@
   <si>
     <t>Analyzing relationships
 Grouped summary statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROBIN OUT OF TOWN
-Discuss how to quantify and describe associations between two quantitative variables
-Explore the [Datasaurus dozen](https://itsalocke.com/datasaurus/) - or, why you should always plot your data. </t>
   </si>
   <si>
     <t>Start the foundations assignment
@@ -1113,11 +1108,6 @@
 [[12pm]]()</t>
   </si>
   <si>
-    <t>Quiz 05 (Due 09/22 ) 
-[[10am]]()
-[[12pm]]()</t>
-  </si>
-  <si>
     <t>Quiz 03 (Due 09/08 ) 
 [[10am]](https://forms.gle/W1GyjHgcGDrAN6GK8)
 [[12pm]](https://forms.gle/yYRae4eWMBvCwSbu6)</t>
@@ -1157,6 +1147,14 @@
     <t xml:space="preserve">Robin is out of town (Class NOT cancelled)
 Discuss how to quantify and describe associations between two quantitative variables
 Explore the [Datasaurus dozen](https://itsalocke.com/datasaurus/) - or, why you should always plot your data. </t>
+  </si>
+  <si>
+    <t>Learning journal check</t>
+  </si>
+  <si>
+    <t>Quiz 05 (Due 09/22 ) 
+[[10am]](https://forms.gle/tMCUh9cYcCtd4AuT9)
+[[12pm]](https://forms.gle/pa77KXTKYGb86s718)</t>
   </si>
 </sst>
 </file>
@@ -1166,9 +1164,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1598,111 +1603,111 @@
   </borders>
   <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="77" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="78" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="78" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="80"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="80" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="80"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="80" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" xfId="80" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="80" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="80" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="81" applyFont="1" applyAlignment="1">
@@ -1717,10 +1722,10 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="25" fillId="5" borderId="3" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="26" fillId="5" borderId="3" xfId="79" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="6" borderId="3" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1729,96 +1734,99 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="3" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="3" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="81" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="80" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="80" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="82" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="4" xfId="82" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="4" xfId="82" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="4" xfId="82" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="4" xfId="82" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="82" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="80" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="80" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="82"/>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1833,51 +1841,48 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="80" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="80" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="80" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="80" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="80" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" xfId="80" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1899,56 +1904,56 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="82" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="82" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1960,9 +1965,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="83">
     <cellStyle name="20% - Accent6" xfId="79" builtinId="50"/>
@@ -2386,8 +2392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2441,7 +2447,7 @@
         <v>69</v>
       </c>
       <c r="G2" s="94" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H2" s="95" t="s">
         <v>211</v>
@@ -2460,7 +2466,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2485,7 +2491,7 @@
         <v>84</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2511,13 +2517,13 @@
         <v>113</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F8" s="35">
         <v>1.3</v>
       </c>
       <c r="G8" s="109" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H8" s="95" t="s">
         <v>212</v>
@@ -2531,7 +2537,7 @@
         <v>114</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2569,7 +2575,7 @@
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="110" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H12" s="95" t="s">
         <v>213</v>
@@ -2616,10 +2622,10 @@
         <v>2.1</v>
       </c>
       <c r="G15" s="110" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H15" s="95" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2633,7 +2639,7 @@
         <v>88</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2658,16 +2664,16 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>89</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G18" s="110" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="H18" s="95" t="s">
         <v>215</v>
@@ -2698,7 +2704,7 @@
         <v>115</v>
       </c>
       <c r="G20" s="110" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H20" s="101" t="s">
         <v>216</v>
@@ -2729,7 +2735,7 @@
       <c r="F22" s="87"/>
       <c r="G22" s="105"/>
       <c r="H22" s="85" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2740,7 +2746,7 @@
         <v>117</v>
       </c>
       <c r="H23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2768,13 +2774,13 @@
         <v>205</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F25" s="35">
         <v>4</v>
       </c>
       <c r="G25" s="110" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2785,7 +2791,7 @@
         <v>206</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2813,7 +2819,7 @@
         <v>4.7</v>
       </c>
       <c r="G28" s="110" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H28" s="80" t="s">
         <v>218</v>
@@ -2827,7 +2833,7 @@
         <v>74</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F29" s="35" t="s">
         <v>231</v>
@@ -2838,7 +2844,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F30" s="35">
         <v>6.1</v>
@@ -2861,7 +2867,7 @@
         <v>6.2</v>
       </c>
       <c r="G31" s="110" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H31" s="95" t="s">
         <v>219</v>
@@ -2872,7 +2878,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E32" s="42" t="s">
         <v>92</v>
@@ -2886,7 +2892,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E33" s="42" t="s">
         <v>93</v>
@@ -2903,7 +2909,7 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E34" s="42" t="s">
         <v>98</v>
@@ -2912,7 +2918,7 @@
         <v>6.5</v>
       </c>
       <c r="G34" s="110" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2932,7 +2938,7 @@
         <v>7</v>
       </c>
       <c r="G35" s="110" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H35" s="95" t="s">
         <v>220</v>
@@ -2949,7 +2955,7 @@
         <v>96</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2957,10 +2963,10 @@
         <v>11.3</v>
       </c>
       <c r="D37" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2977,10 +2983,10 @@
         <v>95</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G38" s="110" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H38" s="80" t="s">
         <v>221</v>
@@ -2991,7 +2997,7 @@
         <v>12.2</v>
       </c>
       <c r="D39" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E39" s="42" t="s">
         <v>100</v>
@@ -3020,16 +3026,16 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E41" s="42" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F41" s="38" t="s">
         <v>233</v>
       </c>
       <c r="G41" s="110" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3069,7 +3075,7 @@
         <v>8.4</v>
       </c>
       <c r="G44" s="111" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3100,7 +3106,7 @@
         <v>97</v>
       </c>
       <c r="G46" s="111" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H46" t="s">
         <v>224</v>
@@ -3144,7 +3150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
@@ -3191,7 +3197,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="108" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -3208,13 +3214,13 @@
         <v>179</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>178</v>
@@ -3223,7 +3229,7 @@
         <v>167</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3241,7 +3247,7 @@
         <v>173</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
@@ -3250,7 +3256,7 @@
         <v>172</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>171</v>
@@ -3272,7 +3278,7 @@
         <v>177</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>186</v>
@@ -3281,7 +3287,7 @@
         <v>180</v>
       </c>
       <c r="H4" s="112" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>169</v>
@@ -3341,7 +3347,7 @@
         <v>183</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>184</v>
@@ -3365,16 +3371,16 @@
         <v>240</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -3395,16 +3401,16 @@
         <v>229</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>234</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -3422,15 +3428,15 @@
         <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3644,10 +3650,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AD78"/>
+  <dimension ref="A1:AD80"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K67" sqref="K67:K68"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3770,12 +3776,12 @@
         <v>66</v>
       </c>
       <c r="I2" s="5">
-        <f>SUMIF($C$2:$C$69,H2,$D$2:$D$69)-30</f>
-        <v>120</v>
+        <f>SUMIF($C$2:$C$71,H2,$D$2:$D$71)-30</f>
+        <v>110</v>
       </c>
       <c r="J2" s="9">
         <f t="shared" ref="J2:J7" si="0">I2/$M$8</f>
-        <v>0.27554535017221582</v>
+        <v>0.2525832376578645</v>
       </c>
       <c r="K2" s="50"/>
       <c r="L2" s="31" t="s">
@@ -3835,9 +3841,7 @@
       <c r="C3" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="61">
-        <v>10</v>
-      </c>
+      <c r="D3" s="61"/>
       <c r="E3" s="92" t="s">
         <v>227</v>
       </c>
@@ -3849,7 +3853,7 @@
         <v>23</v>
       </c>
       <c r="I3" s="5">
-        <f>SUMIF($C$2:$C$69,H3,$D$2:$D$69)</f>
+        <f>SUMIF($C$2:$C$71,H3,$D$2:$D$71)</f>
         <v>120</v>
       </c>
       <c r="J3" s="9">
@@ -3926,7 +3930,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="5">
-        <f>SUMIF($C$2:$C$69,H4,$D$2:$D$69)</f>
+        <f>SUMIF($C$2:$C$71,H4,$D$2:$D$71)</f>
         <v>20</v>
       </c>
       <c r="J4" s="9">
@@ -3998,19 +4002,19 @@
         <v>227</v>
       </c>
       <c r="F5" s="107" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="5">
-        <f>SUMIF($C$2:$C$69,H5,$D$2:$D$69)</f>
-        <v>40</v>
+        <f>SUMIF($C$2:$C$71,H5,$D$2:$D$71)</f>
+        <v>50</v>
       </c>
       <c r="J5" s="9">
         <f t="shared" si="0"/>
-        <v>9.1848450057405287E-2</v>
+        <v>0.11481056257175661</v>
       </c>
       <c r="K5" s="50"/>
       <c r="L5" s="4" t="s">
@@ -4077,7 +4081,7 @@
         <v>13</v>
       </c>
       <c r="I6" s="5">
-        <f>SUMIF($C$2:$C$69,H6,$D$2:$D$69)</f>
+        <f>SUMIF($C$2:$C$71,H6,$D$2:$D$71)</f>
         <v>100</v>
       </c>
       <c r="J6" s="9">
@@ -4154,7 +4158,7 @@
         <v>14</v>
       </c>
       <c r="I7" s="5">
-        <f>SUMIF($C$2:$C$69,H7,$D$2:$D$69)</f>
+        <f>SUMIF($C$2:$C$71,H7,$D$2:$D$71)</f>
         <v>100</v>
       </c>
       <c r="J7" s="9">
@@ -4226,7 +4230,7 @@
         <v>227</v>
       </c>
       <c r="F8" s="107" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="4"/>
@@ -4450,7 +4454,7 @@
       </c>
       <c r="E15" s="49"/>
       <c r="F15" s="107" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
@@ -4679,7 +4683,7 @@
       </c>
       <c r="E24" s="49"/>
       <c r="F24" s="107" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
@@ -4743,23 +4747,19 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="58">
-        <v>7.1</v>
-      </c>
-      <c r="B27" s="65" t="s">
-        <v>143</v>
-      </c>
-      <c r="C27" s="72" t="s">
-        <v>66</v>
+        <v>6.7</v>
+      </c>
+      <c r="B27" s="113" t="s">
+        <v>299</v>
+      </c>
+      <c r="C27" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D27" s="61">
-        <v>10</v>
-      </c>
-      <c r="E27" s="102" t="s">
-        <v>227</v>
-      </c>
-      <c r="F27" s="107" t="s">
-        <v>227</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E27" s="102"/>
+      <c r="F27" s="107"/>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
@@ -4770,21 +4770,23 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="58">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>144</v>
-      </c>
-      <c r="C28" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" s="62">
-        <v>2</v>
+        <v>143</v>
+      </c>
+      <c r="C28" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="61">
+        <v>10</v>
       </c>
       <c r="E28" s="102" t="s">
         <v>227</v>
       </c>
-      <c r="F28" s="54"/>
+      <c r="F28" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
       <c r="I28" s="49"/>
@@ -4795,23 +4797,21 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="58">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>165</v>
-      </c>
-      <c r="C29" s="75" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="61">
-        <v>10</v>
-      </c>
-      <c r="E29" s="100" t="s">
-        <v>227</v>
-      </c>
-      <c r="F29" s="107" t="s">
-        <v>275</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C29" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="62">
+        <v>2</v>
+      </c>
+      <c r="E29" s="102" t="s">
+        <v>227</v>
+      </c>
+      <c r="F29" s="54"/>
       <c r="G29" s="49"/>
       <c r="H29" s="49"/>
       <c r="I29" s="49"/>
@@ -4822,22 +4822,22 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="58">
-        <v>8.1</v>
+        <v>7.3</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>145</v>
-      </c>
-      <c r="C30" s="72" t="s">
-        <v>66</v>
+        <v>165</v>
+      </c>
+      <c r="C30" s="75" t="s">
+        <v>14</v>
       </c>
       <c r="D30" s="61">
         <v>10</v>
       </c>
-      <c r="E30" s="102" t="s">
+      <c r="E30" s="100" t="s">
         <v>227</v>
       </c>
       <c r="F30" s="107" t="s">
-        <v>227</v>
+        <v>274</v>
       </c>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
@@ -4849,44 +4849,48 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="58">
-        <v>8.1999999999999993</v>
+        <v>8.1</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>146</v>
-      </c>
-      <c r="C31" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" s="62">
-        <v>2</v>
+        <v>145</v>
+      </c>
+      <c r="C31" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="61">
+        <v>10</v>
       </c>
       <c r="E31" s="102" t="s">
         <v>227</v>
       </c>
-      <c r="F31" s="54"/>
+      <c r="F31" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
       <c r="I31" s="49"/>
       <c r="J31" s="49"/>
       <c r="K31" s="49"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="58">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>166</v>
-      </c>
-      <c r="C32" s="76" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="61">
-        <v>15</v>
-      </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="107" t="s">
-        <v>275</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="C32" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="62">
+        <v>2</v>
+      </c>
+      <c r="E32" s="102" t="s">
+        <v>227</v>
+      </c>
+      <c r="F32" s="54"/>
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
       <c r="I32" s="49"/>
@@ -4895,22 +4899,20 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="58">
-        <v>9.1</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>147</v>
-      </c>
-      <c r="C33" s="72" t="s">
-        <v>66</v>
+        <v>166</v>
+      </c>
+      <c r="C33" s="76" t="s">
+        <v>23</v>
       </c>
       <c r="D33" s="61">
-        <v>10</v>
-      </c>
-      <c r="E33" s="107" t="s">
-        <v>227</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E33" s="49"/>
       <c r="F33" s="107" t="s">
-        <v>227</v>
+        <v>274</v>
       </c>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
@@ -4920,19 +4922,23 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="58">
-        <v>9.1999999999999993</v>
+        <v>9.1</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="C34" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="62">
-        <v>2</v>
-      </c>
-      <c r="E34" s="49"/>
-      <c r="F34" s="55"/>
+        <v>147</v>
+      </c>
+      <c r="C34" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="61">
+        <v>10</v>
+      </c>
+      <c r="E34" s="107" t="s">
+        <v>227</v>
+      </c>
+      <c r="F34" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G34" s="49"/>
       <c r="H34" s="49"/>
       <c r="I34" s="49"/>
@@ -4941,23 +4947,19 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="58">
-        <v>10.1</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" s="61">
-        <v>10</v>
-      </c>
-      <c r="E35" s="107" t="s">
-        <v>227</v>
-      </c>
-      <c r="F35" s="107" t="s">
-        <v>227</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="C35" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="62">
+        <v>2</v>
+      </c>
+      <c r="E35" s="49"/>
+      <c r="F35" s="55"/>
       <c r="G35" s="49"/>
       <c r="H35" s="49"/>
       <c r="I35" s="49"/>
@@ -4966,19 +4968,23 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="58">
-        <v>10.199999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D36" s="62">
-        <v>2</v>
-      </c>
-      <c r="E36" s="49"/>
-      <c r="F36" s="55"/>
+        <v>149</v>
+      </c>
+      <c r="C36" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="61">
+        <v>10</v>
+      </c>
+      <c r="E36" s="107" t="s">
+        <v>227</v>
+      </c>
+      <c r="F36" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G36" s="49"/>
       <c r="H36" s="49"/>
       <c r="I36" s="49"/>
@@ -4987,21 +4993,19 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="58">
-        <v>10.3</v>
-      </c>
-      <c r="B37" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="C37" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="61">
-        <v>15</v>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B37" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="62">
+        <v>2</v>
       </c>
       <c r="E37" s="49"/>
-      <c r="F37" s="56" t="s">
-        <v>227</v>
-      </c>
+      <c r="F37" s="55"/>
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
       <c r="I37" s="49"/>
@@ -5010,21 +5014,19 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="58">
-        <v>11.1</v>
-      </c>
-      <c r="B38" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="C38" s="72" t="s">
-        <v>66</v>
+        <v>10.3</v>
+      </c>
+      <c r="B38" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="73" t="s">
+        <v>23</v>
       </c>
       <c r="D38" s="61">
-        <v>10</v>
-      </c>
-      <c r="E38" s="107" t="s">
-        <v>227</v>
-      </c>
-      <c r="F38" s="107" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="49"/>
+      <c r="F38" s="56" t="s">
         <v>227</v>
       </c>
       <c r="G38" s="49"/>
@@ -5035,19 +5037,23 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="58">
-        <v>11.2</v>
+        <v>11.1</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" s="62">
-        <v>2</v>
-      </c>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
+        <v>151</v>
+      </c>
+      <c r="C39" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="61">
+        <v>10</v>
+      </c>
+      <c r="E39" s="107" t="s">
+        <v>227</v>
+      </c>
+      <c r="F39" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G39" s="49"/>
       <c r="H39" s="49"/>
       <c r="I39" s="49"/>
@@ -5056,21 +5062,19 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="58">
-        <v>11.3</v>
-      </c>
-      <c r="B40" s="67" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="61">
-        <v>15</v>
+        <v>11.2</v>
+      </c>
+      <c r="B40" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="62">
+        <v>2</v>
       </c>
       <c r="E40" s="49"/>
-      <c r="F40" s="107" t="s">
-        <v>227</v>
-      </c>
+      <c r="F40" s="49"/>
       <c r="G40" s="49"/>
       <c r="H40" s="49"/>
       <c r="I40" s="49"/>
@@ -5079,20 +5083,18 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="58">
-        <v>12.1</v>
-      </c>
-      <c r="B41" s="65" t="s">
-        <v>153</v>
-      </c>
-      <c r="C41" s="72" t="s">
-        <v>66</v>
+        <v>11.3</v>
+      </c>
+      <c r="B41" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="73" t="s">
+        <v>23</v>
       </c>
       <c r="D41" s="61">
-        <v>10</v>
-      </c>
-      <c r="E41" s="107" t="s">
-        <v>227</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E41" s="49"/>
       <c r="F41" s="107" t="s">
         <v>227</v>
       </c>
@@ -5104,19 +5106,23 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="58">
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>154</v>
-      </c>
-      <c r="C42" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" s="62">
-        <v>2</v>
-      </c>
-      <c r="E42" s="49"/>
-      <c r="F42" s="50"/>
+        <v>153</v>
+      </c>
+      <c r="C42" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="61">
+        <v>10</v>
+      </c>
+      <c r="E42" s="107" t="s">
+        <v>227</v>
+      </c>
+      <c r="F42" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
       <c r="I42" s="49"/>
@@ -5128,18 +5134,16 @@
         <v>12.2</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="C43" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D43" s="61">
-        <v>4</v>
+        <v>154</v>
+      </c>
+      <c r="C43" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="62">
+        <v>2</v>
       </c>
       <c r="E43" s="49"/>
-      <c r="F43" s="107" t="s">
-        <v>227</v>
-      </c>
+      <c r="F43" s="50"/>
       <c r="G43" s="49"/>
       <c r="H43" s="49"/>
       <c r="I43" s="49"/>
@@ -5148,16 +5152,16 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="58">
-        <v>12.3</v>
+        <v>12.2</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>128</v>
-      </c>
-      <c r="C44" s="60" t="s">
-        <v>14</v>
+        <v>127</v>
+      </c>
+      <c r="C44" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D44" s="61">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E44" s="49"/>
       <c r="F44" s="107" t="s">
@@ -5171,16 +5175,16 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="58">
-        <v>13.1</v>
+        <v>12.3</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="C45" s="72" t="s">
-        <v>66</v>
+        <v>128</v>
+      </c>
+      <c r="C45" s="60" t="s">
+        <v>14</v>
       </c>
       <c r="D45" s="61">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E45" s="49"/>
       <c r="F45" s="107" t="s">
@@ -5194,19 +5198,21 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="58">
-        <v>13.2</v>
+        <v>13.1</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>156</v>
-      </c>
-      <c r="C46" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D46" s="62">
-        <v>2</v>
+        <v>155</v>
+      </c>
+      <c r="C46" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="61">
+        <v>10</v>
       </c>
       <c r="E46" s="49"/>
-      <c r="F46" s="57"/>
+      <c r="F46" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G46" s="49"/>
       <c r="H46" s="49"/>
       <c r="I46" s="49"/>
@@ -5215,21 +5221,19 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="58">
-        <v>13.3</v>
-      </c>
-      <c r="B47" s="67" t="s">
-        <v>106</v>
-      </c>
-      <c r="C47" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="61">
-        <v>15</v>
+        <v>13.2</v>
+      </c>
+      <c r="B47" s="65" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="62">
+        <v>2</v>
       </c>
       <c r="E47" s="49"/>
-      <c r="F47" s="107" t="s">
-        <v>275</v>
-      </c>
+      <c r="F47" s="57"/>
       <c r="G47" s="49"/>
       <c r="H47" s="49"/>
       <c r="I47" s="49"/>
@@ -5238,20 +5242,20 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="58">
-        <v>14.1</v>
-      </c>
-      <c r="B48" s="65" t="s">
-        <v>157</v>
-      </c>
-      <c r="C48" s="72" t="s">
-        <v>66</v>
+        <v>13.3</v>
+      </c>
+      <c r="B48" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="73" t="s">
+        <v>23</v>
       </c>
       <c r="D48" s="61">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E48" s="49"/>
       <c r="F48" s="107" t="s">
-        <v>227</v>
+        <v>274</v>
       </c>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
@@ -5259,62 +5263,62 @@
       <c r="J48" s="49"/>
       <c r="K48" s="49"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="58">
-        <v>14.2</v>
+        <v>14.1</v>
       </c>
       <c r="B49" s="65" t="s">
-        <v>158</v>
-      </c>
-      <c r="C49" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="62">
-        <v>2</v>
+        <v>157</v>
+      </c>
+      <c r="C49" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" s="61">
+        <v>10</v>
       </c>
       <c r="E49" s="49"/>
-      <c r="F49" s="57"/>
+      <c r="F49" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G49" s="49"/>
       <c r="H49" s="49"/>
       <c r="I49" s="49"/>
       <c r="J49" s="49"/>
       <c r="K49" s="49"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="58">
-        <v>14.3</v>
+        <v>14.2</v>
       </c>
       <c r="B50" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="C50" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" s="61">
-        <v>4</v>
+        <v>158</v>
+      </c>
+      <c r="C50" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" s="62">
+        <v>2</v>
       </c>
       <c r="E50" s="49"/>
-      <c r="F50" s="107" t="s">
-        <v>227</v>
-      </c>
+      <c r="F50" s="57"/>
       <c r="G50" s="49"/>
       <c r="H50" s="49"/>
       <c r="I50" s="49"/>
       <c r="J50" s="49"/>
       <c r="K50" s="49"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="58">
-        <v>14.4</v>
+        <v>14.3</v>
       </c>
       <c r="B51" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="C51" s="60" t="s">
-        <v>14</v>
+        <v>129</v>
+      </c>
+      <c r="C51" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D51" s="61">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E51" s="49"/>
       <c r="F51" s="107" t="s">
@@ -5326,18 +5330,18 @@
       <c r="J51" s="49"/>
       <c r="K51" s="49"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="58">
-        <v>15.1</v>
+        <v>14.4</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>159</v>
-      </c>
-      <c r="C52" s="72" t="s">
-        <v>66</v>
+        <v>130</v>
+      </c>
+      <c r="C52" s="60" t="s">
+        <v>14</v>
       </c>
       <c r="D52" s="61">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E52" s="49"/>
       <c r="F52" s="107" t="s">
@@ -5349,62 +5353,62 @@
       <c r="J52" s="49"/>
       <c r="K52" s="49"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="58">
-        <v>15.2</v>
+        <v>15.1</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>160</v>
-      </c>
-      <c r="C53" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="62">
-        <v>2</v>
+        <v>159</v>
+      </c>
+      <c r="C53" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="61">
+        <v>10</v>
       </c>
       <c r="E53" s="49"/>
-      <c r="F53" s="49"/>
+      <c r="F53" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G53" s="49"/>
       <c r="H53" s="49"/>
       <c r="I53" s="49"/>
       <c r="J53" s="49"/>
       <c r="K53" s="49"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="58">
-        <v>15.3</v>
-      </c>
-      <c r="B54" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="C54" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" s="61">
-        <v>4</v>
+        <v>15.2</v>
+      </c>
+      <c r="B54" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="62">
+        <v>2</v>
       </c>
       <c r="E54" s="49"/>
-      <c r="F54" s="107" t="s">
-        <v>227</v>
-      </c>
+      <c r="F54" s="49"/>
       <c r="G54" s="49"/>
       <c r="H54" s="49"/>
       <c r="I54" s="49"/>
       <c r="J54" s="49"/>
       <c r="K54" s="49"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="58">
-        <v>15.4</v>
+        <v>15.3</v>
       </c>
       <c r="B55" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="C55" s="60" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="C55" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D55" s="61">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E55" s="49"/>
       <c r="F55" s="107" t="s">
@@ -5416,18 +5420,18 @@
       <c r="J55" s="49"/>
       <c r="K55" s="49"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="58">
-        <v>16</v>
+        <v>15.4</v>
       </c>
       <c r="B56" s="59" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="71" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="C56" s="60" t="s">
+        <v>14</v>
       </c>
       <c r="D56" s="61">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E56" s="49"/>
       <c r="F56" s="107" t="s">
@@ -5439,41 +5443,41 @@
       <c r="J56" s="49"/>
       <c r="K56" s="49"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="58">
-        <v>16</v>
-      </c>
-      <c r="B57" s="59" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57" s="60" t="s">
-        <v>14</v>
+        <v>15.5</v>
+      </c>
+      <c r="B57" s="113" t="s">
+        <v>299</v>
+      </c>
+      <c r="C57" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D57" s="61">
-        <v>10</v>
-      </c>
-      <c r="E57" s="49"/>
-      <c r="F57" s="107" t="s">
-        <v>227</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E57" s="102"/>
+      <c r="F57" s="107"/>
       <c r="G57" s="49"/>
       <c r="H57" s="49"/>
       <c r="I57" s="49"/>
       <c r="J57" s="49"/>
       <c r="K57" s="49"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" s="24"/>
+      <c r="M57" s="24"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="58">
         <v>16</v>
       </c>
       <c r="B58" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="74" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="C58" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D58" s="61">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E58" s="49"/>
       <c r="F58" s="107" t="s">
@@ -5485,18 +5489,18 @@
       <c r="J58" s="49"/>
       <c r="K58" s="49"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="58">
         <v>16</v>
       </c>
       <c r="B59" s="59" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="77" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="C59" s="60" t="s">
+        <v>14</v>
       </c>
       <c r="D59" s="61">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E59" s="49"/>
       <c r="F59" s="107" t="s">
@@ -5508,18 +5512,18 @@
       <c r="J59" s="49"/>
       <c r="K59" s="49"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="58">
         <v>16</v>
       </c>
-      <c r="B60" s="65" t="s">
-        <v>120</v>
-      </c>
-      <c r="C60" s="71" t="s">
-        <v>12</v>
+      <c r="B60" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="74" t="s">
+        <v>13</v>
       </c>
       <c r="D60" s="61">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E60" s="49"/>
       <c r="F60" s="107" t="s">
@@ -5531,15 +5535,15 @@
       <c r="J60" s="49"/>
       <c r="K60" s="49"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="58">
         <v>16</v>
       </c>
       <c r="B61" s="59" t="s">
-        <v>33</v>
-      </c>
-      <c r="C61" s="71" t="s">
-        <v>12</v>
+        <v>32</v>
+      </c>
+      <c r="C61" s="77" t="s">
+        <v>24</v>
       </c>
       <c r="D61" s="61">
         <v>2</v>
@@ -5554,18 +5558,18 @@
       <c r="J61" s="49"/>
       <c r="K61" s="49"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="58">
         <v>16</v>
       </c>
-      <c r="B62" s="59" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="77" t="s">
-        <v>24</v>
+      <c r="B62" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="71" t="s">
+        <v>12</v>
       </c>
       <c r="D62" s="61">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E62" s="49"/>
       <c r="F62" s="107" t="s">
@@ -5577,18 +5581,18 @@
       <c r="J62" s="49"/>
       <c r="K62" s="49"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="58">
         <v>16</v>
       </c>
-      <c r="B63" s="78" t="s">
-        <v>67</v>
+      <c r="B63" s="59" t="s">
+        <v>33</v>
       </c>
       <c r="C63" s="71" t="s">
         <v>12</v>
       </c>
       <c r="D63" s="61">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E63" s="49"/>
       <c r="F63" s="107" t="s">
@@ -5600,70 +5604,68 @@
       <c r="J63" s="49"/>
       <c r="K63" s="49"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="58">
+        <v>16</v>
+      </c>
+      <c r="B64" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="D64" s="61">
+        <v>10</v>
+      </c>
       <c r="E64" s="49"/>
-      <c r="F64" s="49"/>
+      <c r="F64" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G64" s="49"/>
       <c r="H64" s="49"/>
       <c r="I64" s="49"/>
       <c r="J64" s="49"/>
       <c r="K64" s="49"/>
     </row>
-    <row r="65" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="50"/>
-      <c r="F65" s="50"/>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A65" s="58">
+        <v>16</v>
+      </c>
+      <c r="B65" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="61">
+        <v>6</v>
+      </c>
+      <c r="E65" s="49"/>
+      <c r="F65" s="107" t="s">
+        <v>227</v>
+      </c>
       <c r="G65" s="49"/>
       <c r="H65" s="49"/>
       <c r="I65" s="49"/>
       <c r="J65" s="49"/>
       <c r="K65" s="49"/>
-      <c r="L65" s="4"/>
-      <c r="P65" s="4"/>
-      <c r="Q65" s="4"/>
-      <c r="R65" s="4"/>
-      <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
-      <c r="U65" s="4"/>
-      <c r="V65" s="4"/>
-      <c r="W65" s="4"/>
-      <c r="X65" s="4"/>
-      <c r="Y65" s="4"/>
-      <c r="Z65" s="4"/>
-    </row>
-    <row r="66" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="8"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E66" s="49"/>
-      <c r="F66" s="57"/>
+      <c r="F66" s="49"/>
       <c r="G66" s="49"/>
       <c r="H66" s="49"/>
       <c r="I66" s="49"/>
       <c r="J66" s="49"/>
       <c r="K66" s="49"/>
-      <c r="L66" s="4"/>
-      <c r="P66" s="4"/>
-      <c r="Q66" s="4"/>
-      <c r="R66" s="4"/>
-      <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
-      <c r="U66" s="4"/>
-      <c r="V66" s="4"/>
-      <c r="W66" s="4"/>
-      <c r="X66" s="4"/>
-      <c r="Y66" s="4"/>
-      <c r="Z66" s="4"/>
-    </row>
-    <row r="67" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="8"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="49"/>
       <c r="H67" s="49"/>
       <c r="I67" s="49"/>
       <c r="J67" s="49"/>
@@ -5681,17 +5683,17 @@
       <c r="Y67" s="4"/>
       <c r="Z67" s="4"/>
     </row>
-    <row r="68" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="8"/>
-      <c r="E68" s="23"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="23"/>
-      <c r="H68" s="23"/>
-      <c r="I68" s="23"/>
-      <c r="J68" s="23"/>
-      <c r="K68" s="23"/>
+      <c r="E68" s="49"/>
+      <c r="F68" s="57"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="49"/>
+      <c r="J68" s="49"/>
+      <c r="K68" s="49"/>
       <c r="L68" s="4"/>
       <c r="P68" s="4"/>
       <c r="Q68" s="4"/>
@@ -5705,20 +5707,18 @@
       <c r="Y68" s="4"/>
       <c r="Z68" s="4"/>
     </row>
-    <row r="69" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="8"/>
       <c r="E69" s="23"/>
       <c r="F69" s="23"/>
       <c r="G69" s="23"/>
-      <c r="H69" s="23"/>
-      <c r="I69" s="23"/>
-      <c r="J69" s="23"/>
-      <c r="K69" s="23"/>
+      <c r="H69" s="49"/>
+      <c r="I69" s="49"/>
+      <c r="J69" s="49"/>
+      <c r="K69" s="49"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
-      <c r="N69" s="4"/>
       <c r="P69" s="4"/>
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
@@ -5731,7 +5731,7 @@
       <c r="Y69" s="4"/>
       <c r="Z69" s="4"/>
     </row>
-    <row r="70" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="8"/>
@@ -5743,8 +5743,6 @@
       <c r="J70" s="23"/>
       <c r="K70" s="23"/>
       <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="4"/>
       <c r="P70" s="4"/>
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
@@ -5757,7 +5755,7 @@
       <c r="Y70" s="4"/>
       <c r="Z70" s="4"/>
     </row>
-    <row r="71" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="8"/>
@@ -5783,7 +5781,7 @@
       <c r="Y71" s="4"/>
       <c r="Z71" s="4"/>
     </row>
-    <row r="72" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="8"/>
@@ -5809,7 +5807,7 @@
       <c r="Y72" s="4"/>
       <c r="Z72" s="4"/>
     </row>
-    <row r="73" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="8"/>
@@ -5835,7 +5833,7 @@
       <c r="Y73" s="4"/>
       <c r="Z73" s="4"/>
     </row>
-    <row r="74" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="8"/>
@@ -5861,7 +5859,7 @@
       <c r="Y74" s="4"/>
       <c r="Z74" s="4"/>
     </row>
-    <row r="75" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="8"/>
@@ -5887,7 +5885,7 @@
       <c r="Y75" s="4"/>
       <c r="Z75" s="4"/>
     </row>
-    <row r="76" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="8"/>
@@ -5913,7 +5911,7 @@
       <c r="Y76" s="4"/>
       <c r="Z76" s="4"/>
     </row>
-    <row r="77" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="8"/>
@@ -5925,6 +5923,8 @@
       <c r="J77" s="23"/>
       <c r="K77" s="23"/>
       <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
       <c r="P77" s="4"/>
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
@@ -5937,7 +5937,7 @@
       <c r="Y77" s="4"/>
       <c r="Z77" s="4"/>
     </row>
-    <row r="78" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="8"/>
@@ -5949,6 +5949,8 @@
       <c r="J78" s="23"/>
       <c r="K78" s="23"/>
       <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
       <c r="P78" s="4"/>
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
@@ -5961,11 +5963,59 @@
       <c r="Y78" s="4"/>
       <c r="Z78" s="4"/>
     </row>
+    <row r="79" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="23"/>
+      <c r="G79" s="23"/>
+      <c r="H79" s="23"/>
+      <c r="I79" s="23"/>
+      <c r="J79" s="23"/>
+      <c r="K79" s="23"/>
+      <c r="L79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="4"/>
+      <c r="R79" s="4"/>
+      <c r="S79" s="4"/>
+      <c r="T79" s="4"/>
+      <c r="U79" s="4"/>
+      <c r="V79" s="4"/>
+      <c r="W79" s="4"/>
+      <c r="X79" s="4"/>
+      <c r="Y79" s="4"/>
+      <c r="Z79" s="4"/>
+    </row>
+    <row r="80" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="23"/>
+      <c r="I80" s="23"/>
+      <c r="J80" s="23"/>
+      <c r="K80" s="23"/>
+      <c r="L80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
+      <c r="S80" s="4"/>
+      <c r="T80" s="4"/>
+      <c r="U80" s="4"/>
+      <c r="V80" s="4"/>
+      <c r="W80" s="4"/>
+      <c r="X80" s="4"/>
+      <c r="Y80" s="4"/>
+      <c r="Z80" s="4"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F83">
-    <sortCondition ref="A2:A83"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F85">
+    <sortCondition ref="A2:A85"/>
   </sortState>
-  <phoneticPr fontId="38" type="noConversion"/>
+  <phoneticPr fontId="39" type="noConversion"/>
   <conditionalFormatting sqref="R2:R8">
     <cfRule type="dataBar" priority="8">
       <dataBar>

</xml_diff>

<commit_message>
add final schedule to calendar
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH315/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACADF2A2-1A6B-4490-8098-B6BDEABC3D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5DA8F9-AAA2-9746-A56F-5FF23E56CB09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -20,19 +20,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">points!$A$1:$J$65</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -458,9 +450,6 @@
     <t>wknum</t>
   </si>
   <si>
-    <t>Time &amp; Location TBD</t>
-  </si>
-  <si>
     <t>Slack reflection</t>
   </si>
   <si>
@@ -1103,11 +1092,6 @@
 [[12pm]]()</t>
   </si>
   <si>
-    <t>Quiz 06 (Due 09/29 ) 
-[[10am]]()
-[[12pm]]()</t>
-  </si>
-  <si>
     <t>Quiz 03 (Due 09/08 ) 
 [[10am]](https://forms.gle/W1GyjHgcGDrAN6GK8)
 [[12pm]](https://forms.gle/yYRae4eWMBvCwSbu6)</t>
@@ -1155,6 +1139,14 @@
     <t>Quiz 05 (Due 09/22 ) 
 [[10am]](https://forms.gle/tMCUh9cYcCtd4AuT9)
 [[12pm]](https://forms.gle/pa77KXTKYGb86s718)</t>
+  </si>
+  <si>
+    <t>Monday 4-6pm ARTS 112</t>
+  </si>
+  <si>
+    <t>Quiz 06 (Due 09/29 ) 
+[[10am]](https://forms.gle/9Vxb5HyC6dzPLyh96)
+[[12pm]](https://forms.gle/uEeNikFti8BJx4MJ7)</t>
   </si>
 </sst>
 </file>
@@ -2392,22 +2384,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="D12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.875" style="35"/>
+    <col min="1" max="2" width="8.83203125" style="35"/>
     <col min="3" max="3" width="0" style="35" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.375" style="42" customWidth="1"/>
-    <col min="6" max="6" width="11.25" style="35" customWidth="1"/>
-    <col min="7" max="7" width="60.75" style="94" customWidth="1"/>
-    <col min="8" max="8" width="79.75" customWidth="1"/>
+    <col min="5" max="5" width="56.33203125" style="42" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="60.6640625" style="94" customWidth="1"/>
+    <col min="8" max="8" width="79.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="35" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="35" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>80</v>
       </c>
@@ -2421,7 +2413,7 @@
         <v>68</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>101</v>
@@ -2433,7 +2425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="40">
         <v>1.1000000000000001</v>
       </c>
@@ -2441,46 +2433,46 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>69</v>
       </c>
       <c r="G2" s="94" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H2" s="95" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="40">
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="40">
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
         <v>1.4</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E5" s="42" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="40">
         <v>1.5</v>
       </c>
@@ -2491,10 +2483,10 @@
         <v>84</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="40">
         <v>1.6</v>
       </c>
@@ -2506,7 +2498,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="40">
         <v>2.1</v>
       </c>
@@ -2517,19 +2509,19 @@
         <v>113</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F8" s="35">
         <v>1.3</v>
       </c>
       <c r="G8" s="109" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H8" s="95" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="40">
         <v>2.2000000000000002</v>
       </c>
@@ -2537,18 +2529,18 @@
         <v>114</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="40">
         <v>2.2999999999999998</v>
       </c>
       <c r="D10" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="40">
         <v>2.4</v>
       </c>
@@ -2559,7 +2551,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="41">
         <v>3.1</v>
       </c>
@@ -2575,13 +2567,13 @@
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="110" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H12" s="95" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40">
         <v>3.2</v>
       </c>
@@ -2596,16 +2588,16 @@
       </c>
       <c r="H13" s="81"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="40">
         <v>3.3</v>
       </c>
       <c r="D14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H14" s="81"/>
     </row>
-    <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="40">
         <v>4.0999999999999996</v>
       </c>
@@ -2613,7 +2605,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>88</v>
@@ -2622,41 +2614,41 @@
         <v>2.1</v>
       </c>
       <c r="G15" s="110" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H15" s="95" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="40">
         <v>4.2</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>88</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="40">
         <v>4.3</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E17" s="83"/>
       <c r="F17" s="84"/>
       <c r="G17" s="104"/>
       <c r="H17" s="82" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="40">
         <v>5.0999999999999996</v>
       </c>
@@ -2664,33 +2656,33 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>89</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G18" s="110" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H18" s="95" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="40">
         <v>5.2</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19" s="38"/>
       <c r="G19" s="97"/>
       <c r="H19" s="95"/>
     </row>
-    <row r="20" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="40">
         <v>6.1</v>
       </c>
@@ -2704,13 +2696,13 @@
         <v>115</v>
       </c>
       <c r="G20" s="110" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="H20" s="101" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="40">
         <v>6.2</v>
       </c>
@@ -2724,7 +2716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="40">
         <v>6.3</v>
       </c>
@@ -2735,10 +2727,10 @@
       <c r="F22" s="87"/>
       <c r="G22" s="105"/>
       <c r="H22" s="85" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="40">
         <v>6.4</v>
       </c>
@@ -2746,24 +2738,24 @@
         <v>117</v>
       </c>
       <c r="H23" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="40">
         <v>6.5</v>
       </c>
       <c r="D24" s="82" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E24" s="83"/>
       <c r="F24" s="84"/>
       <c r="G24" s="104"/>
       <c r="H24" s="82" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="40">
         <v>7.1</v>
       </c>
@@ -2771,30 +2763,30 @@
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F25" s="35">
         <v>4</v>
       </c>
       <c r="G25" s="110" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="40">
         <v>7.2</v>
       </c>
       <c r="D26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="40">
         <v>7.3</v>
       </c>
@@ -2805,7 +2797,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="40">
         <v>8.1</v>
       </c>
@@ -2819,13 +2811,13 @@
         <v>4.7</v>
       </c>
       <c r="G28" s="110" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H28" s="80" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="40">
         <v>8.1999999999999993</v>
       </c>
@@ -2833,24 +2825,24 @@
         <v>74</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="40">
         <v>8.3000000000000007</v>
       </c>
       <c r="D30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F30" s="35">
         <v>6.1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="40">
         <v>9.1</v>
       </c>
@@ -2867,18 +2859,18 @@
         <v>6.2</v>
       </c>
       <c r="G31" s="110" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H31" s="95" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="40">
         <v>9.1999999999999993</v>
       </c>
       <c r="D32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E32" s="42" t="s">
         <v>92</v>
@@ -2887,12 +2879,12 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="40">
         <v>9.3000000000000007</v>
       </c>
       <c r="D33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E33" s="42" t="s">
         <v>93</v>
@@ -2901,7 +2893,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="40">
         <v>10.1</v>
       </c>
@@ -2909,7 +2901,7 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E34" s="42" t="s">
         <v>98</v>
@@ -2918,10 +2910,10 @@
         <v>6.5</v>
       </c>
       <c r="G34" s="110" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="40">
         <v>11.1</v>
       </c>
@@ -2938,13 +2930,13 @@
         <v>7</v>
       </c>
       <c r="G35" s="110" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H35" s="95" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="40">
         <v>11.2</v>
       </c>
@@ -2955,21 +2947,21 @@
         <v>96</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="40">
         <v>11.3</v>
       </c>
       <c r="D37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="40">
         <v>12.1</v>
       </c>
@@ -2983,42 +2975,42 @@
         <v>95</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G38" s="110" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H38" s="80" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="40">
         <v>12.2</v>
       </c>
       <c r="D39" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E39" s="42" t="s">
         <v>100</v>
       </c>
       <c r="F39" s="38"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="40">
         <v>12.4</v>
       </c>
       <c r="D40" s="82" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E40" s="83"/>
       <c r="F40" s="84"/>
       <c r="G40" s="104"/>
       <c r="H40" s="82" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="40">
         <v>13.1</v>
       </c>
@@ -3026,19 +3018,19 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E41" s="42" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G41" s="110" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="40">
         <v>13.2</v>
       </c>
@@ -3046,22 +3038,22 @@
         <v>107</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="40">
         <v>14</v>
       </c>
       <c r="D43" s="88" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E43" s="89"/>
       <c r="F43" s="90"/>
       <c r="G43" s="106"/>
       <c r="H43" s="88"/>
     </row>
-    <row r="44" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="40">
         <v>15.1</v>
       </c>
@@ -3069,30 +3061,30 @@
         <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F44" s="38">
         <v>8.4</v>
       </c>
       <c r="G44" s="111" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="40">
         <v>15.2</v>
       </c>
       <c r="D45" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E45" s="83"/>
       <c r="F45" s="84"/>
       <c r="G45" s="104"/>
       <c r="H45" s="82" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="40">
         <v>16.100000000000001</v>
       </c>
@@ -3100,19 +3092,19 @@
         <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E46" s="42" t="s">
         <v>97</v>
       </c>
       <c r="G46" s="111" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H46" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="40">
         <v>17.100000000000001</v>
       </c>
@@ -3123,10 +3115,10 @@
         <v>102</v>
       </c>
       <c r="H47" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="40">
         <v>17.2</v>
       </c>
@@ -3134,11 +3126,11 @@
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H48">
+  <sortState ref="A2:H48">
     <sortCondition ref="A2:A48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3155,20 +3147,20 @@
       <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="21" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="21" customWidth="1"/>
-    <col min="3" max="3" width="33.625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" style="21" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="22" customWidth="1"/>
-    <col min="5" max="5" width="88.25" style="22" customWidth="1"/>
-    <col min="6" max="6" width="34.625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="88.1640625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" style="22" customWidth="1"/>
     <col min="7" max="8" width="38" style="22" customWidth="1"/>
-    <col min="9" max="9" width="25.375" style="21" customWidth="1"/>
-    <col min="10" max="16384" width="14.875" style="21"/>
+    <col min="9" max="9" width="25.33203125" style="21" customWidth="1"/>
+    <col min="10" max="16384" width="14.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
@@ -3197,10 +3189,10 @@
         <v>7</v>
       </c>
       <c r="J1" s="108" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="240" x14ac:dyDescent="0.2">
       <c r="A2" s="99">
         <v>1</v>
       </c>
@@ -3211,28 +3203,28 @@
         <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="99">
         <v>2</v>
       </c>
@@ -3241,29 +3233,29 @@
         <v>42248</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A4" s="99">
         <v>3</v>
       </c>
@@ -3272,28 +3264,28 @@
         <v>42255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H4" s="112" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="160" x14ac:dyDescent="0.2">
       <c r="A5" s="99">
         <v>4</v>
       </c>
@@ -3302,28 +3294,28 @@
         <v>42262</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" s="99">
         <v>5</v>
       </c>
@@ -3332,28 +3324,28 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>236</v>
-      </c>
       <c r="G6" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="I6" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="99">
         <v>6</v>
       </c>
@@ -3362,28 +3354,28 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A8" s="99">
         <v>7</v>
       </c>
@@ -3395,25 +3387,25 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" ht="224" x14ac:dyDescent="0.2">
       <c r="A9" s="28">
         <v>8</v>
       </c>
@@ -3428,18 +3420,18 @@
         <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="21" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="28">
         <v>9</v>
       </c>
@@ -3466,7 +3458,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="28">
         <v>10</v>
       </c>
@@ -3475,7 +3467,7 @@
         <v>42304</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>52</v>
@@ -3493,7 +3485,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="28">
         <v>11</v>
       </c>
@@ -3502,7 +3494,7 @@
         <v>42311</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>54</v>
@@ -3518,7 +3510,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="28">
         <v>12</v>
       </c>
@@ -3527,21 +3519,21 @@
         <v>42318</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A14" s="28">
         <v>13</v>
       </c>
@@ -3550,13 +3542,13 @@
         <v>42325</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>61</v>
@@ -3566,7 +3558,7 @@
       </c>
       <c r="H14" s="27"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="28"/>
       <c r="B15" s="29">
         <f t="shared" si="0"/>
@@ -3581,7 +3573,7 @@
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
     </row>
-    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="28">
         <v>14</v>
       </c>
@@ -3590,7 +3582,7 @@
         <v>42339</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>57</v>
@@ -3606,7 +3598,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="28">
         <v>15</v>
       </c>
@@ -3615,7 +3607,7 @@
         <v>42346</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>58</v>
@@ -3625,7 +3617,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
         <v>0</v>
       </c>
@@ -3656,26 +3648,26 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="5"/>
-    <col min="2" max="2" width="35.75" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="5"/>
+    <col min="2" max="2" width="35.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="8"/>
+    <col min="4" max="4" width="7.6640625" style="8"/>
     <col min="5" max="5" width="10.5" style="23" customWidth="1"/>
-    <col min="6" max="6" width="7.625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="23" customWidth="1"/>
     <col min="7" max="11" width="10.5" style="23" customWidth="1"/>
     <col min="12" max="12" width="13.5" style="4" customWidth="1"/>
     <col min="13" max="13" width="10" style="5" customWidth="1"/>
-    <col min="14" max="14" width="7.625" style="5"/>
-    <col min="15" max="15" width="4.625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="10.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="7.625" style="4"/>
+    <col min="14" max="14" width="7.6640625" style="5"/>
+    <col min="15" max="15" width="4.6640625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="7.6640625" style="4"/>
     <col min="20" max="20" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="7.625" style="4"/>
+    <col min="21" max="16384" width="7.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -3752,7 +3744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -3766,10 +3758,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F2" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G2" s="50"/>
       <c r="H2" s="31" t="s">
@@ -3831,22 +3823,22 @@
         <v>3.0837004405286344E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="58">
         <v>1.2</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" s="72" t="s">
         <v>66</v>
       </c>
       <c r="D3" s="61"/>
       <c r="E3" s="92" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F3" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G3" s="49"/>
       <c r="H3" s="47" t="s">
@@ -3908,12 +3900,12 @@
         <v>0.21806167400881057</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="58">
         <v>1.2</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C4" s="64" t="s">
         <v>112</v>
@@ -3922,7 +3914,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="93" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="50"/>
@@ -3985,12 +3977,12 @@
         <v>4.405286343612335E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="58">
         <v>1.4</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" s="66" t="s">
         <v>23</v>
@@ -3999,10 +3991,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="93" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F5" s="107" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="4" t="s">
@@ -4057,12 +4049,12 @@
         <v>6.8281938325991193E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="58">
         <v>2.1</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" s="72" t="s">
         <v>66</v>
@@ -4071,10 +4063,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="93" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F6" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="4" t="s">
@@ -4136,12 +4128,12 @@
         <v>2.2026431718061675E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="58">
         <v>2.2000000000000002</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="64" t="s">
         <v>112</v>
@@ -4150,7 +4142,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="93" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -4213,12 +4205,12 @@
         <v>0.38546255506607929</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="58">
         <v>2.2999999999999998</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="68" t="s">
         <v>14</v>
@@ -4227,10 +4219,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="93" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F8" s="107" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="4"/>
@@ -4278,7 +4270,7 @@
         <v>0.23127753303964757</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="58">
         <v>2.4</v>
       </c>
@@ -4293,7 +4285,7 @@
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G9" s="50"/>
       <c r="H9" s="50"/>
@@ -4316,12 +4308,12 @@
       </c>
       <c r="AD9" s="5"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="58">
         <v>3.1</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C10" s="63" t="s">
         <v>66</v>
@@ -4330,10 +4322,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="96" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F10" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="50"/>
@@ -4341,12 +4333,12 @@
       <c r="J10" s="50"/>
       <c r="K10" s="50"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="58">
         <v>3.2</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C11" s="64" t="s">
         <v>112</v>
@@ -4355,7 +4347,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="96" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="49"/>
@@ -4364,12 +4356,12 @@
       <c r="J11" s="49"/>
       <c r="K11" s="49"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="58">
         <v>3.3</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C12" s="73" t="s">
         <v>23</v>
@@ -4378,10 +4370,10 @@
         <v>15</v>
       </c>
       <c r="E12" s="96" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F12" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
@@ -4389,12 +4381,12 @@
       <c r="J12" s="49"/>
       <c r="K12" s="49"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="58">
         <v>4.0999999999999996</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" s="63" t="s">
         <v>66</v>
@@ -4403,10 +4395,10 @@
         <v>10</v>
       </c>
       <c r="E13" s="98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F13" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G13" s="49"/>
       <c r="H13" s="49"/>
@@ -4414,12 +4406,12 @@
       <c r="J13" s="49"/>
       <c r="K13" s="49"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="58">
         <v>4.2</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" s="64" t="s">
         <v>112</v>
@@ -4428,7 +4420,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="49"/>
@@ -4439,12 +4431,12 @@
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="58">
         <v>4.3</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C15" s="71" t="s">
         <v>12</v>
@@ -4454,7 +4446,7 @@
       </c>
       <c r="E15" s="49"/>
       <c r="F15" s="107" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
@@ -4464,12 +4456,12 @@
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="58">
         <v>4.4000000000000004</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" s="60" t="s">
         <v>14</v>
@@ -4479,7 +4471,7 @@
       </c>
       <c r="E16" s="49"/>
       <c r="F16" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
@@ -4489,12 +4481,12 @@
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="58">
         <v>4.5</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" s="73" t="s">
         <v>23</v>
@@ -4503,10 +4495,10 @@
         <v>15</v>
       </c>
       <c r="E17" s="98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F17" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
@@ -4516,12 +4508,12 @@
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="58">
         <v>5.0999999999999996</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C18" s="63" t="s">
         <v>66</v>
@@ -4530,10 +4522,10 @@
         <v>10</v>
       </c>
       <c r="E18" s="98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F18" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
@@ -4543,12 +4535,12 @@
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="58">
         <v>5.2</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="64" t="s">
         <v>112</v>
@@ -4557,7 +4549,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F19" s="53"/>
       <c r="G19" s="49"/>
@@ -4568,12 +4560,12 @@
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="58">
         <v>5.3</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C20" s="73" t="s">
         <v>23</v>
@@ -4582,10 +4574,10 @@
         <v>15</v>
       </c>
       <c r="E20" s="98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F20" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
@@ -4595,12 +4587,12 @@
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="58">
         <v>6.1</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C21" s="72" t="s">
         <v>66</v>
@@ -4609,10 +4601,10 @@
         <v>10</v>
       </c>
       <c r="E21" s="102" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F21" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
@@ -4622,12 +4614,12 @@
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="58">
         <v>6.2</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C22" s="64" t="s">
         <v>112</v>
@@ -4636,7 +4628,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="102" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F22" s="50"/>
       <c r="G22" s="49"/>
@@ -4645,12 +4637,12 @@
       <c r="J22" s="49"/>
       <c r="K22" s="49"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="58">
         <v>6.3</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C23" s="71" t="s">
         <v>12</v>
@@ -4660,7 +4652,7 @@
       </c>
       <c r="E23" s="49"/>
       <c r="F23" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
@@ -4668,12 +4660,12 @@
       <c r="J23" s="49"/>
       <c r="K23" s="49"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="58">
         <v>6.4</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C24" s="60" t="s">
         <v>14</v>
@@ -4683,7 +4675,7 @@
       </c>
       <c r="E24" s="49"/>
       <c r="F24" s="107" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
@@ -4693,7 +4685,7 @@
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="58">
         <v>6.5</v>
       </c>
@@ -4708,7 +4700,7 @@
       </c>
       <c r="E25" s="49"/>
       <c r="F25" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
@@ -4718,7 +4710,7 @@
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="58">
         <v>6.6</v>
       </c>
@@ -4732,10 +4724,10 @@
         <v>5</v>
       </c>
       <c r="E26" s="102" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F26" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
@@ -4745,12 +4737,12 @@
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="58">
         <v>6.7</v>
       </c>
       <c r="B27" s="113" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C27" s="71" t="s">
         <v>12</v>
@@ -4768,12 +4760,12 @@
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="58">
         <v>7.1</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C28" s="72" t="s">
         <v>66</v>
@@ -4782,10 +4774,10 @@
         <v>10</v>
       </c>
       <c r="E28" s="102" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F28" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
@@ -4795,12 +4787,12 @@
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="58">
         <v>7.2</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C29" s="64" t="s">
         <v>112</v>
@@ -4809,7 +4801,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="102" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F29" s="54"/>
       <c r="G29" s="49"/>
@@ -4820,12 +4812,12 @@
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="58">
         <v>7.3</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C30" s="75" t="s">
         <v>14</v>
@@ -4834,10 +4826,10 @@
         <v>10</v>
       </c>
       <c r="E30" s="100" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F30" s="107" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
@@ -4847,12 +4839,12 @@
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="58">
         <v>8.1</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C31" s="72" t="s">
         <v>66</v>
@@ -4861,10 +4853,10 @@
         <v>10</v>
       </c>
       <c r="E31" s="102" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F31" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
@@ -4874,12 +4866,12 @@
       <c r="L31" s="24"/>
       <c r="M31" s="24"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="58">
         <v>8.1999999999999993</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C32" s="64" t="s">
         <v>112</v>
@@ -4888,7 +4880,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="102" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F32" s="54"/>
       <c r="G32" s="49"/>
@@ -4897,12 +4889,12 @@
       <c r="J32" s="49"/>
       <c r="K32" s="49"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="58">
         <v>8.3000000000000007</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C33" s="76" t="s">
         <v>23</v>
@@ -4912,7 +4904,7 @@
       </c>
       <c r="E33" s="49"/>
       <c r="F33" s="107" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
@@ -4920,12 +4912,12 @@
       <c r="J33" s="49"/>
       <c r="K33" s="49"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="58">
         <v>9.1</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C34" s="72" t="s">
         <v>66</v>
@@ -4934,10 +4926,10 @@
         <v>10</v>
       </c>
       <c r="E34" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F34" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G34" s="49"/>
       <c r="H34" s="49"/>
@@ -4945,12 +4937,12 @@
       <c r="J34" s="49"/>
       <c r="K34" s="49"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="58">
         <v>9.1999999999999993</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35" s="64" t="s">
         <v>112</v>
@@ -4966,12 +4958,12 @@
       <c r="J35" s="49"/>
       <c r="K35" s="49"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="58">
         <v>10.1</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C36" s="72" t="s">
         <v>66</v>
@@ -4980,10 +4972,10 @@
         <v>10</v>
       </c>
       <c r="E36" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F36" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G36" s="49"/>
       <c r="H36" s="49"/>
@@ -4991,12 +4983,12 @@
       <c r="J36" s="49"/>
       <c r="K36" s="49"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="58">
         <v>10.199999999999999</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C37" s="64" t="s">
         <v>112</v>
@@ -5012,7 +5004,7 @@
       <c r="J37" s="49"/>
       <c r="K37" s="49"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="58">
         <v>10.3</v>
       </c>
@@ -5027,7 +5019,7 @@
       </c>
       <c r="E38" s="49"/>
       <c r="F38" s="56" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
@@ -5035,12 +5027,12 @@
       <c r="J38" s="49"/>
       <c r="K38" s="49"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="58">
         <v>11.1</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C39" s="72" t="s">
         <v>66</v>
@@ -5049,10 +5041,10 @@
         <v>10</v>
       </c>
       <c r="E39" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F39" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G39" s="49"/>
       <c r="H39" s="49"/>
@@ -5060,12 +5052,12 @@
       <c r="J39" s="49"/>
       <c r="K39" s="49"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="58">
         <v>11.2</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C40" s="64" t="s">
         <v>112</v>
@@ -5081,7 +5073,7 @@
       <c r="J40" s="49"/>
       <c r="K40" s="49"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="58">
         <v>11.3</v>
       </c>
@@ -5096,7 +5088,7 @@
       </c>
       <c r="E41" s="49"/>
       <c r="F41" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G41" s="49"/>
       <c r="H41" s="49"/>
@@ -5104,12 +5096,12 @@
       <c r="J41" s="49"/>
       <c r="K41" s="49"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="58">
         <v>12.1</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C42" s="72" t="s">
         <v>66</v>
@@ -5118,10 +5110,10 @@
         <v>10</v>
       </c>
       <c r="E42" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F42" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
@@ -5129,12 +5121,12 @@
       <c r="J42" s="49"/>
       <c r="K42" s="49"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="58">
         <v>12.2</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C43" s="64" t="s">
         <v>112</v>
@@ -5150,12 +5142,12 @@
       <c r="J43" s="49"/>
       <c r="K43" s="49"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="58">
         <v>12.2</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C44" s="71" t="s">
         <v>12</v>
@@ -5165,7 +5157,7 @@
       </c>
       <c r="E44" s="49"/>
       <c r="F44" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G44" s="49"/>
       <c r="H44" s="49"/>
@@ -5173,12 +5165,12 @@
       <c r="J44" s="49"/>
       <c r="K44" s="49"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="58">
         <v>12.3</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C45" s="60" t="s">
         <v>14</v>
@@ -5188,7 +5180,7 @@
       </c>
       <c r="E45" s="49"/>
       <c r="F45" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
@@ -5196,12 +5188,12 @@
       <c r="J45" s="49"/>
       <c r="K45" s="49"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="58">
         <v>13.1</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C46" s="72" t="s">
         <v>66</v>
@@ -5211,7 +5203,7 @@
       </c>
       <c r="E46" s="49"/>
       <c r="F46" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G46" s="49"/>
       <c r="H46" s="49"/>
@@ -5219,12 +5211,12 @@
       <c r="J46" s="49"/>
       <c r="K46" s="49"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="58">
         <v>13.2</v>
       </c>
       <c r="B47" s="65" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C47" s="64" t="s">
         <v>112</v>
@@ -5240,7 +5232,7 @@
       <c r="J47" s="49"/>
       <c r="K47" s="49"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="58">
         <v>13.3</v>
       </c>
@@ -5255,7 +5247,7 @@
       </c>
       <c r="E48" s="49"/>
       <c r="F48" s="107" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
@@ -5263,12 +5255,12 @@
       <c r="J48" s="49"/>
       <c r="K48" s="49"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="58">
         <v>14.1</v>
       </c>
       <c r="B49" s="65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C49" s="72" t="s">
         <v>66</v>
@@ -5278,7 +5270,7 @@
       </c>
       <c r="E49" s="49"/>
       <c r="F49" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G49" s="49"/>
       <c r="H49" s="49"/>
@@ -5286,12 +5278,12 @@
       <c r="J49" s="49"/>
       <c r="K49" s="49"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="58">
         <v>14.2</v>
       </c>
       <c r="B50" s="65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C50" s="64" t="s">
         <v>112</v>
@@ -5307,12 +5299,12 @@
       <c r="J50" s="49"/>
       <c r="K50" s="49"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="58">
         <v>14.3</v>
       </c>
       <c r="B51" s="65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C51" s="71" t="s">
         <v>12</v>
@@ -5322,7 +5314,7 @@
       </c>
       <c r="E51" s="49"/>
       <c r="F51" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G51" s="49"/>
       <c r="H51" s="49"/>
@@ -5330,12 +5322,12 @@
       <c r="J51" s="49"/>
       <c r="K51" s="49"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="58">
         <v>14.4</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C52" s="60" t="s">
         <v>14</v>
@@ -5345,7 +5337,7 @@
       </c>
       <c r="E52" s="49"/>
       <c r="F52" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G52" s="49"/>
       <c r="H52" s="49"/>
@@ -5353,12 +5345,12 @@
       <c r="J52" s="49"/>
       <c r="K52" s="49"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="58">
         <v>15.1</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C53" s="72" t="s">
         <v>66</v>
@@ -5368,7 +5360,7 @@
       </c>
       <c r="E53" s="49"/>
       <c r="F53" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G53" s="49"/>
       <c r="H53" s="49"/>
@@ -5376,12 +5368,12 @@
       <c r="J53" s="49"/>
       <c r="K53" s="49"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="58">
         <v>15.2</v>
       </c>
       <c r="B54" s="65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C54" s="64" t="s">
         <v>112</v>
@@ -5397,7 +5389,7 @@
       <c r="J54" s="49"/>
       <c r="K54" s="49"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="58">
         <v>15.3</v>
       </c>
@@ -5412,7 +5404,7 @@
       </c>
       <c r="E55" s="49"/>
       <c r="F55" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G55" s="49"/>
       <c r="H55" s="49"/>
@@ -5420,7 +5412,7 @@
       <c r="J55" s="49"/>
       <c r="K55" s="49"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="58">
         <v>15.4</v>
       </c>
@@ -5435,7 +5427,7 @@
       </c>
       <c r="E56" s="49"/>
       <c r="F56" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G56" s="49"/>
       <c r="H56" s="49"/>
@@ -5443,12 +5435,12 @@
       <c r="J56" s="49"/>
       <c r="K56" s="49"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="58">
         <v>15.5</v>
       </c>
       <c r="B57" s="113" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C57" s="71" t="s">
         <v>12</v>
@@ -5466,7 +5458,7 @@
       <c r="L57" s="24"/>
       <c r="M57" s="24"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="58">
         <v>16</v>
       </c>
@@ -5481,7 +5473,7 @@
       </c>
       <c r="E58" s="49"/>
       <c r="F58" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G58" s="49"/>
       <c r="H58" s="49"/>
@@ -5489,7 +5481,7 @@
       <c r="J58" s="49"/>
       <c r="K58" s="49"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="58">
         <v>16</v>
       </c>
@@ -5504,7 +5496,7 @@
       </c>
       <c r="E59" s="49"/>
       <c r="F59" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G59" s="49"/>
       <c r="H59" s="49"/>
@@ -5512,7 +5504,7 @@
       <c r="J59" s="49"/>
       <c r="K59" s="49"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="58">
         <v>16</v>
       </c>
@@ -5527,7 +5519,7 @@
       </c>
       <c r="E60" s="49"/>
       <c r="F60" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G60" s="49"/>
       <c r="H60" s="49"/>
@@ -5535,7 +5527,7 @@
       <c r="J60" s="49"/>
       <c r="K60" s="49"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="58">
         <v>16</v>
       </c>
@@ -5550,7 +5542,7 @@
       </c>
       <c r="E61" s="49"/>
       <c r="F61" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
@@ -5558,12 +5550,12 @@
       <c r="J61" s="49"/>
       <c r="K61" s="49"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="58">
         <v>16</v>
       </c>
       <c r="B62" s="65" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C62" s="71" t="s">
         <v>12</v>
@@ -5573,7 +5565,7 @@
       </c>
       <c r="E62" s="49"/>
       <c r="F62" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
@@ -5581,7 +5573,7 @@
       <c r="J62" s="49"/>
       <c r="K62" s="49"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="58">
         <v>16</v>
       </c>
@@ -5596,7 +5588,7 @@
       </c>
       <c r="E63" s="49"/>
       <c r="F63" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
@@ -5604,7 +5596,7 @@
       <c r="J63" s="49"/>
       <c r="K63" s="49"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="58">
         <v>16</v>
       </c>
@@ -5619,7 +5611,7 @@
       </c>
       <c r="E64" s="49"/>
       <c r="F64" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G64" s="49"/>
       <c r="H64" s="49"/>
@@ -5627,7 +5619,7 @@
       <c r="J64" s="49"/>
       <c r="K64" s="49"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="58">
         <v>16</v>
       </c>
@@ -5642,7 +5634,7 @@
       </c>
       <c r="E65" s="49"/>
       <c r="F65" s="107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G65" s="49"/>
       <c r="H65" s="49"/>
@@ -5650,7 +5642,7 @@
       <c r="J65" s="49"/>
       <c r="K65" s="49"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="E66" s="49"/>
       <c r="F66" s="49"/>
       <c r="G66" s="49"/>
@@ -5659,7 +5651,7 @@
       <c r="J66" s="49"/>
       <c r="K66" s="49"/>
     </row>
-    <row r="67" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="8"/>
@@ -5683,7 +5675,7 @@
       <c r="Y67" s="4"/>
       <c r="Z67" s="4"/>
     </row>
-    <row r="68" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="8"/>
@@ -5707,7 +5699,7 @@
       <c r="Y68" s="4"/>
       <c r="Z68" s="4"/>
     </row>
-    <row r="69" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="8"/>
@@ -5731,7 +5723,7 @@
       <c r="Y69" s="4"/>
       <c r="Z69" s="4"/>
     </row>
-    <row r="70" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="8"/>
@@ -5755,7 +5747,7 @@
       <c r="Y70" s="4"/>
       <c r="Z70" s="4"/>
     </row>
-    <row r="71" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="8"/>
@@ -5781,7 +5773,7 @@
       <c r="Y71" s="4"/>
       <c r="Z71" s="4"/>
     </row>
-    <row r="72" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="8"/>
@@ -5807,7 +5799,7 @@
       <c r="Y72" s="4"/>
       <c r="Z72" s="4"/>
     </row>
-    <row r="73" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="8"/>
@@ -5833,7 +5825,7 @@
       <c r="Y73" s="4"/>
       <c r="Z73" s="4"/>
     </row>
-    <row r="74" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="8"/>
@@ -5859,7 +5851,7 @@
       <c r="Y74" s="4"/>
       <c r="Z74" s="4"/>
     </row>
-    <row r="75" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="8"/>
@@ -5885,7 +5877,7 @@
       <c r="Y75" s="4"/>
       <c r="Z75" s="4"/>
     </row>
-    <row r="76" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="8"/>
@@ -5911,7 +5903,7 @@
       <c r="Y76" s="4"/>
       <c r="Z76" s="4"/>
     </row>
-    <row r="77" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="8"/>
@@ -5937,7 +5929,7 @@
       <c r="Y77" s="4"/>
       <c r="Z77" s="4"/>
     </row>
-    <row r="78" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="8"/>
@@ -5963,7 +5955,7 @@
       <c r="Y78" s="4"/>
       <c r="Z78" s="4"/>
     </row>
-    <row r="79" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="8"/>
@@ -5987,7 +5979,7 @@
       <c r="Y79" s="4"/>
       <c r="Z79" s="4"/>
     </row>
-    <row r="80" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="8"/>
@@ -6012,7 +6004,7 @@
       <c r="Z80" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F85">
+  <sortState ref="A2:F85">
     <sortCondition ref="A2:A85"/>
   </sortState>
   <phoneticPr fontId="39" type="noConversion"/>

</xml_diff>

<commit_message>
start new CLT activity
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH315/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5DA8F9-AAA2-9746-A56F-5FF23E56CB09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81103DC6-A0FA-8A4F-8013-3D6B8E390617}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="307">
   <si>
     <t>Finals Week</t>
   </si>
@@ -142,21 +142,6 @@
   </si>
   <si>
     <t>Veterans Day -  Campus closed</t>
-  </si>
-  <si>
-    <t>Foundations for Inference
-Confidence Intervals
-Hypothesis Testing</t>
-  </si>
-  <si>
-    <t>Conducting Inference using R
-Bivariate inference: T-tests
-Bivariate inference: ANOVA</t>
-  </si>
-  <si>
-    <t>Bivariate inference: Chi-squared
-Bivariate Inference - Correlation
-Bivariate Inference - Linear Regression</t>
   </si>
   <si>
     <t>Introduction to the class, logistics
@@ -173,9 +158,6 @@
 Calculate appropriate grouped summary statistics
 Describe the relationship between two variables in plain English
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction of probability by means of exploding kittens. </t>
   </si>
   <si>
     <t>Explain the difference between practical and statistical significance
@@ -192,12 +174,6 @@
 Conduct and interpret a test of correlation</t>
   </si>
   <si>
-    <t xml:space="preserve">Watch the assigned PDS Videos on correlation and tests for equal proportions
-Complete the T-Test and ANOVA questions in the Homework
-Review the AS Notebook on Simple Linear Regression
-</t>
-  </si>
-  <si>
     <t>How to use the chi-squared distribution to test if the proportion of an event is equally likely across multiple groups</t>
   </si>
   <si>
@@ -458,11 +434,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Open work day - Finish Bivariate inference
-Moderation
-</t>
-  </si>
-  <si>
     <t>Poster Prep II: EDA</t>
   </si>
   <si>
@@ -759,12 +730,6 @@
     <t>Project Stage II: Exploratory Data Analysis</t>
   </si>
   <si>
-    <t>Point estimates and sampling distributions</t>
-  </si>
-  <si>
-    <t>Central limit theorem</t>
-  </si>
-  <si>
     <t>Project Stage III: Bivariate Inference</t>
   </si>
   <si>
@@ -792,9 +757,6 @@
     <t>[hw05_biv_graphing](hw/hw05_biv_graphing.html) (Due 9/28 )</t>
   </si>
   <si>
-    <t>[hw06 research proposal outline](hw/hw06_research_proposal_outline.html)(Due 10/12 )</t>
-  </si>
-  <si>
     <t>Poster prep Stage II* (Draft Due 10/01, PR 10/03, Final 10/05 )</t>
   </si>
   <si>
@@ -829,11 +791,6 @@
   </si>
   <si>
     <t>PDS Chapter</t>
-  </si>
-  <si>
-    <t>Read lecture notes on writing about empirical research
-Identify one binary and one continuous variable in your data set of interest. 
-Come prepared with summary statistics for each (n, # missing values, #yes, mean, sd)</t>
   </si>
   <si>
     <t>Watch PDS Video 6. As always, follow along on your computer for the best results. 
@@ -878,49 +835,20 @@
 Calculate a simple probability of an event. </t>
   </si>
   <si>
-    <t>Writing about research
-Midterm
-Probability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read instructions for first poster prep assignment
-Watch the PDS video 8
-Review and take the sample exam. 
-</t>
-  </si>
-  <si>
     <t>Analyzing relationships
 Grouped summary statistics</t>
   </si>
   <si>
-    <t>Start the foundations assignment
-Introduce point estimates such as the sample mean and proportion as estimates of a population
-Visualize through simulation what happens to these point estimates as sample sizes get large
-Define sampling distributions, and standard errors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go through a full 5 step hypothesis. </t>
-  </si>
-  <si>
     <t>hw06- research proposal outline</t>
   </si>
   <si>
     <t>hw07 - foundations for inference</t>
   </si>
   <si>
-    <t>Week 6 group quiz
-How is writing about empirical research different than other types of writing like essays?  
-Midterm review
-Poster prep stage II</t>
-  </si>
-  <si>
     <t>1.1</t>
   </si>
   <si>
     <t>2.2</t>
-  </si>
-  <si>
-    <t>4.4</t>
   </si>
   <si>
     <t>2.3</t>
@@ -934,9 +862,6 @@
   <si>
     <t xml:space="preserve">Midterm
 </t>
-  </si>
-  <si>
-    <t>Self and peer evaluation</t>
   </si>
   <si>
     <t xml:space="preserve">In class exam on Friday. [Sample exam](reading/sample_exam_1.pdf) available. </t>
@@ -1038,9 +963,6 @@
     <t>321 Bridge</t>
   </si>
   <si>
-    <t>Reproducible Research</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quiz 02 (Due 09/03 ) 
 [[10am]](https://forms.gle/TcWHzcfEn4ych7TJA)
 [[12pm]](https://forms.gle/JmzgBUXc4KYE34Y36)
@@ -1117,17 +1039,6 @@
 </t>
   </si>
   <si>
-    <t>Watch how an expert codes: https://www.youtube.com/watch?v=go5Au01Jrvs (hint: it's not as seamless as you may think)
-Read CN 6.1-6.3 before Monday
-Read the instructions for the Bivariate inference assignment
-Watch the PDS video on ANOVA and read CN 6.4 before Friday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watching an expert walk through an analysis. [[Video]](https://www.youtube.com/watch?v=go5Au01Jrvs)
-This is the guy that _created_  ggplot, dplyr and many other transformative packages for R
-Things to note is that he makes mistakes (quite a few). He shrugs it off, fixes it and continues. His coding is like a stream of consciousness narrative. This helps you (and he) understand not just what he's doing, but why he's doing it. He takes notes on what he's doing, this is super important! </t>
-  </si>
-  <si>
     <t xml:space="preserve">Robin is out of town (Class NOT cancelled)
 Discuss how to quantify and describe associations between two quantitative variables
 Explore the [Datasaurus dozen](https://itsalocke.com/datasaurus/) - or, why you should always plot your data. </t>
@@ -1147,6 +1058,126 @@
     <t>Quiz 06 (Due 09/29 ) 
 [[10am]](https://forms.gle/9Vxb5HyC6dzPLyh96)
 [[12pm]](https://forms.gle/uEeNikFti8BJx4MJ7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How is statistics done in your field? </t>
+  </si>
+  <si>
+    <t>hw 08- bivariate inference</t>
+  </si>
+  <si>
+    <t>Week 6 group quiz
+How is writing about empirical research different than other types of writing like essays?  
+321-Bridge. Now what do you think about how Statistics is used in your discipline? 
+Poster prep stage II</t>
+  </si>
+  <si>
+    <t>3.1-3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read lecture notes on writing about empirical research
+Read the poster prep stage II instructions. Choose the plots that you want to showcase. 
+Review and take the sample exam. 
+Watch the PDS video 8 (up to about 10 minutes)
+Read the course packet up through Section 3.2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start the foundations assignment
+Watching an expert walk through an analysis. [[Video]](https://www.youtube.com/watch?v=go5Au01Jrvs)
+This is the guy that _created_  ggplot, dplyr and many other transformative packages for R
+Things to note is that he makes mistakes (quite a few). He shrugs it off, fixes it and continues. His coding is like a stream of consciousness narrative. This helps you (and he) understand not just what he's doing, but why he's doing it. He takes notes on what he's doing, this is super important! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify one binary and one continuous variable in your data set of interest. 
+Come prepared with summary statistics for each (n, # missing values, #yes, mean, sd)
+Watch how an expert codes: https://www.youtube.com/watch?v=go5Au01Jrvs (hint: it's not as seamless as you may think)
+Read CN 6.1-6.3 before Monday
+</t>
+  </si>
+  <si>
+    <t>Watch the assigned PDS Videos on correlation and tests for equal proportions
+Complete the T-Test and ANOVA questions in the Homework
+Review the AS Notebook on Simple Linear Regression
+Read the instructions for the Bivariate inference assignment
+Watch the PDS video on ANOVA and read CN 6.4 before Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Normal and T Distributions. </t>
+  </si>
+  <si>
+    <t>3.3-3.4</t>
+  </si>
+  <si>
+    <t>Writing about research
+Midterm
+Probability Distributions</t>
+  </si>
+  <si>
+    <t>Self and peer evaluation
+Poster prep stage II
+Record die roll data into Google spreadsheet</t>
+  </si>
+  <si>
+    <t>Discovering the CLT Worksheet (Handout) (Due 10/12 )</t>
+  </si>
+  <si>
+    <t>[hw06 research proposal outline](hw/hw06_research_proposal_outline.html) (Due 10/12 )</t>
+  </si>
+  <si>
+    <t>Populations vs Samples</t>
+  </si>
+  <si>
+    <t>Sampling distributions and the CLT</t>
+  </si>
+  <si>
+    <t>4-4,2</t>
+  </si>
+  <si>
+    <t>4.3-4.4</t>
+  </si>
+  <si>
+    <t>Normal and T distributions
+Sampling distributions
+Central Limit Theorem
+Interval estimates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foundations for Inference
+Hypothesis Testing
+Bivariate inference: T-tests
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bivariate inference: ANOVA
+Bivariate inference: Chi-squared
+Bivariate Inference - Correlation
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bivariate Inference - Linear Regression
+Moderation
+</t>
+  </si>
+  <si>
+    <t>Record in-class die rolls in [[this google spreadsheet]]() Be sure to find your section and group! (Due Tue )</t>
+  </si>
+  <si>
+    <t>Introduction of probability by means of exploding kittens. 
+Simulating distributions of random variables (In class activity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure your die rolling data is recorded in Google drive. (Tue)
+Watch video, fill out course packet 3.4-3.5 (Mon).
+Read course packet 4.1-4.4 (Wed)
+Watch video, fill out course packet sections 4.5-4.6 (Friday)
+</t>
+  </si>
+  <si>
+    <t>The "All" vs the "Small": Samples and populations. 
+Sampling distributions - revisiting our die rolling. 
+Discovering the Central Limit Theorem (Start of Foundations Homework)
+Calculating probabilities of an average</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="40">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1442,7 +1473,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1542,6 +1573,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,7 +1715,7 @@
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1961,6 +1998,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="80" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="83">
     <cellStyle name="20% - Accent6" xfId="79" builtinId="50"/>
@@ -2382,50 +2431,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="8.83203125" style="35"/>
     <col min="3" max="3" width="0" style="35" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.33203125" style="42" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" style="35" customWidth="1"/>
-    <col min="7" max="7" width="60.6640625" style="94" customWidth="1"/>
+    <col min="7" max="7" width="18" style="94" customWidth="1"/>
     <col min="8" max="8" width="79.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="35" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="35" customFormat="1" ht="33" thickBot="1">
       <c r="A1" s="39" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G1" s="103" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H1" s="48" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="40">
         <v>1.1000000000000001</v>
       </c>
@@ -2433,72 +2482,72 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G2" s="94" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="H2" s="95" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="40">
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="40">
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="40">
         <v>1.4</v>
       </c>
       <c r="D5" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="40">
         <v>1.5</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="40">
         <v>1.6</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E7" s="43"/>
       <c r="F7" s="35">
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="68">
       <c r="A8" s="40">
         <v>2.1</v>
       </c>
@@ -2506,52 +2555,52 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="F8" s="35">
         <v>1.3</v>
       </c>
       <c r="G8" s="109" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="H8" s="95" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="40">
         <v>2.2000000000000002</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="40">
         <v>2.2999999999999998</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="40">
         <v>2.4</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="51">
       <c r="A12" s="41">
         <v>3.1</v>
       </c>
@@ -2560,44 +2609,44 @@
       </c>
       <c r="C12" s="36"/>
       <c r="D12" s="37" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="110" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="H12" s="95" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="40">
         <v>3.2</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F13" s="35">
         <v>1.4</v>
       </c>
       <c r="H13" s="81"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="40">
         <v>3.3</v>
       </c>
       <c r="D14" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H14" s="81"/>
     </row>
-    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="51">
       <c r="A15" s="40">
         <v>4.0999999999999996</v>
       </c>
@@ -2605,50 +2654,50 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F15" s="35">
         <v>2.1</v>
       </c>
       <c r="G15" s="110" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="H15" s="95" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="40">
         <v>4.2</v>
       </c>
       <c r="D16" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E16" s="42" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="40">
         <v>4.3</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E17" s="83"/>
       <c r="F17" s="84"/>
       <c r="G17" s="104"/>
       <c r="H17" s="82" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="24" customHeight="1">
       <c r="A18" s="40">
         <v>5.0999999999999996</v>
       </c>
@@ -2656,33 +2705,33 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="G18" s="110" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="H18" s="95" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="40">
         <v>5.2</v>
       </c>
       <c r="D19" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F19" s="38"/>
       <c r="G19" s="97"/>
       <c r="H19" s="95"/>
     </row>
-    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="26" customHeight="1">
       <c r="A20" s="40">
         <v>6.1</v>
       </c>
@@ -2690,448 +2739,466 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G20" s="110" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="H20" s="101" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="40">
         <v>6.2</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="F21" s="35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="H21" s="85" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="40">
         <v>6.3</v>
       </c>
       <c r="D22" s="85" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E22" s="86"/>
       <c r="F22" s="87"/>
       <c r="G22" s="105"/>
       <c r="H22" s="85" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="40">
         <v>6.4</v>
       </c>
       <c r="D23" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H23" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="40">
         <v>6.5</v>
       </c>
       <c r="D24" s="82" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E24" s="83"/>
       <c r="F24" s="84"/>
       <c r="G24" s="104"/>
       <c r="H24" s="82" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="68">
       <c r="A25" s="40">
         <v>7.1</v>
       </c>
       <c r="B25" s="35">
         <v>7</v>
       </c>
-      <c r="D25" t="s">
-        <v>204</v>
+      <c r="D25" s="115" t="s">
+        <v>289</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>261</v>
-      </c>
-      <c r="F25" s="35">
-        <v>4</v>
-      </c>
-      <c r="G25" s="110" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="G25" s="116" t="s">
+        <v>270</v>
+      </c>
+      <c r="H25" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17">
       <c r="A26" s="40">
         <v>7.2</v>
       </c>
-      <c r="D26" t="s">
-        <v>205</v>
-      </c>
-      <c r="F26" s="38" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D26" s="115" t="s">
+        <v>295</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="G26" s="110"/>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="40">
         <v>7.3</v>
       </c>
-      <c r="D27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="35">
+      <c r="D27" s="80" t="s">
+        <v>296</v>
+      </c>
+      <c r="F27" s="38" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="40">
+        <v>7.4</v>
+      </c>
+      <c r="D28" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="35">
         <v>4.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="40">
+    <row r="29" spans="1:8" ht="51">
+      <c r="A29" s="40">
         <v>8.1</v>
       </c>
-      <c r="B28" s="35">
+      <c r="B29" s="35">
         <v>8</v>
       </c>
-      <c r="D28" t="s">
-        <v>116</v>
-      </c>
-      <c r="F28" s="35">
+      <c r="D29" s="80" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" s="35">
         <v>4.7</v>
       </c>
-      <c r="G28" s="110" t="s">
-        <v>282</v>
-      </c>
-      <c r="H28" s="80" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="40">
+      <c r="G29" s="116" t="s">
+        <v>264</v>
+      </c>
+      <c r="H29" s="85" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="40">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D29" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" s="42" t="s">
-        <v>260</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="40">
+      <c r="D30" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>243</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="40">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D30" t="s">
-        <v>264</v>
-      </c>
-      <c r="F30" s="35">
+      <c r="D31" t="s">
+        <v>247</v>
+      </c>
+      <c r="F31" s="35">
         <v>6.1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A31" s="40">
+    <row r="32" spans="1:8" ht="51">
+      <c r="A32" s="40">
         <v>9.1</v>
       </c>
-      <c r="B31" s="35">
+      <c r="B32" s="35">
         <v>9</v>
       </c>
-      <c r="D31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" s="42" t="s">
+      <c r="D32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="35">
+        <v>6.2</v>
+      </c>
+      <c r="G32" s="110" t="s">
+        <v>263</v>
+      </c>
+      <c r="H32" s="95" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="40">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D33" t="s">
+        <v>248</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="35">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="40">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D34" t="s">
+        <v>249</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F34" s="35">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="51">
+      <c r="A35" s="40">
+        <v>10.1</v>
+      </c>
+      <c r="B35" s="35">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>250</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35" s="35">
+        <v>6.5</v>
+      </c>
+      <c r="G35" s="110" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="51">
+      <c r="A36" s="40">
+        <v>11.1</v>
+      </c>
+      <c r="B36" s="35">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="35">
+        <v>7</v>
+      </c>
+      <c r="G36" s="110" t="s">
+        <v>265</v>
+      </c>
+      <c r="H36" s="95" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="40">
+        <v>11.2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="F31" s="35">
-        <v>6.2</v>
-      </c>
-      <c r="G31" s="110" t="s">
-        <v>281</v>
-      </c>
-      <c r="H31" s="95" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="40">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="D32" t="s">
-        <v>265</v>
-      </c>
-      <c r="E32" s="42" t="s">
+      <c r="F37" s="38" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="40">
+        <v>11.3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>253</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="51">
+      <c r="A39" s="40">
+        <v>12.1</v>
+      </c>
+      <c r="B39" s="35">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>94</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="F39" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="G39" s="110" t="s">
+        <v>269</v>
+      </c>
+      <c r="H39" s="80" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="40">
+        <v>12.2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>251</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="38"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="40">
+        <v>12.4</v>
+      </c>
+      <c r="D41" s="82" t="s">
+        <v>198</v>
+      </c>
+      <c r="E41" s="83"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="104"/>
+      <c r="H41" s="82" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="51">
+      <c r="A42" s="40">
+        <v>13.1</v>
+      </c>
+      <c r="B42" s="35">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s">
+        <v>252</v>
+      </c>
+      <c r="E42" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="F42" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="G42" s="110" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="40">
+        <v>13.2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" s="38" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="40">
+        <v>14</v>
+      </c>
+      <c r="D44" s="88" t="s">
+        <v>216</v>
+      </c>
+      <c r="E44" s="89"/>
+      <c r="F44" s="90"/>
+      <c r="G44" s="106"/>
+      <c r="H44" s="88"/>
+    </row>
+    <row r="45" spans="1:8" ht="51">
+      <c r="A45" s="40">
+        <v>15.1</v>
+      </c>
+      <c r="B45" s="35">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
+        <v>199</v>
+      </c>
+      <c r="F45" s="38">
+        <v>8.4</v>
+      </c>
+      <c r="G45" s="111" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="40">
+        <v>15.2</v>
+      </c>
+      <c r="D46" s="82" t="s">
+        <v>200</v>
+      </c>
+      <c r="E46" s="83"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="104"/>
+      <c r="H46" s="82" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="51">
+      <c r="A47" s="40">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="B47" s="35">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>201</v>
+      </c>
+      <c r="E47" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="35">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="40">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="D33" t="s">
-        <v>266</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="F33" s="35">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A34" s="40">
-        <v>10.1</v>
-      </c>
-      <c r="B34" s="35">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>267</v>
-      </c>
-      <c r="E34" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F34" s="35">
-        <v>6.5</v>
-      </c>
-      <c r="G34" s="110" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A35" s="40">
-        <v>11.1</v>
-      </c>
-      <c r="B35" s="35">
-        <v>11</v>
-      </c>
-      <c r="D35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E35" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" s="35">
-        <v>7</v>
-      </c>
-      <c r="G35" s="110" t="s">
-        <v>283</v>
-      </c>
-      <c r="H35" s="95" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="40">
-        <v>11.2</v>
-      </c>
-      <c r="D36" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="F36" s="38" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="40">
-        <v>11.3</v>
-      </c>
-      <c r="D37" t="s">
-        <v>270</v>
-      </c>
-      <c r="F37" s="38" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A38" s="40">
-        <v>12.1</v>
-      </c>
-      <c r="B38" s="35">
-        <v>12</v>
-      </c>
-      <c r="D38" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="F38" s="38" t="s">
-        <v>250</v>
-      </c>
-      <c r="G38" s="110" t="s">
-        <v>287</v>
-      </c>
-      <c r="H38" s="80" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="40">
-        <v>12.2</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="G47" s="111" t="s">
         <v>268</v>
       </c>
-      <c r="E39" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="F39" s="38"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="40">
-        <v>12.4</v>
-      </c>
-      <c r="D40" s="82" t="s">
-        <v>206</v>
-      </c>
-      <c r="E40" s="83"/>
-      <c r="F40" s="84"/>
-      <c r="G40" s="104"/>
-      <c r="H40" s="82" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A41" s="40">
-        <v>13.1</v>
-      </c>
-      <c r="B41" s="35">
-        <v>13</v>
-      </c>
-      <c r="D41" t="s">
-        <v>269</v>
-      </c>
-      <c r="E41" s="42" t="s">
-        <v>259</v>
-      </c>
-      <c r="F41" s="38" t="s">
-        <v>232</v>
-      </c>
-      <c r="G41" s="110" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="40">
-        <v>13.2</v>
-      </c>
-      <c r="D42" t="s">
-        <v>107</v>
-      </c>
-      <c r="F42" s="38" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="40">
-        <v>14</v>
-      </c>
-      <c r="D43" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E43" s="89"/>
-      <c r="F43" s="90"/>
-      <c r="G43" s="106"/>
-      <c r="H43" s="88"/>
-    </row>
-    <row r="44" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A44" s="40">
-        <v>15.1</v>
-      </c>
-      <c r="B44" s="35">
-        <v>14</v>
-      </c>
-      <c r="D44" t="s">
-        <v>207</v>
-      </c>
-      <c r="F44" s="38">
-        <v>8.4</v>
-      </c>
-      <c r="G44" s="111" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="40">
-        <v>15.2</v>
-      </c>
-      <c r="D45" s="82" t="s">
-        <v>208</v>
-      </c>
-      <c r="E45" s="83"/>
-      <c r="F45" s="84"/>
-      <c r="G45" s="104"/>
-      <c r="H45" s="82" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="40">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="B46" s="35">
+      <c r="H47" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="40">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="B48" s="35">
+        <v>16</v>
+      </c>
+      <c r="D48" t="s">
+        <v>97</v>
+      </c>
+      <c r="H48" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="40">
+        <v>17.2</v>
+      </c>
+      <c r="D49" t="s">
         <v>15</v>
       </c>
-      <c r="D46" t="s">
-        <v>209</v>
-      </c>
-      <c r="E46" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="G46" s="111" t="s">
-        <v>286</v>
-      </c>
-      <c r="H46" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="40">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="B47" s="35">
-        <v>16</v>
-      </c>
-      <c r="D47" t="s">
-        <v>102</v>
-      </c>
-      <c r="H47" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="40">
-        <v>17.2</v>
-      </c>
-      <c r="D48" t="s">
-        <v>15</v>
-      </c>
-      <c r="H48" t="s">
-        <v>224</v>
+      <c r="H49" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H48">
-    <sortCondition ref="A2:A48"/>
+  <sortState ref="A2:H49">
+    <sortCondition ref="A2:A49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3142,12 +3209,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.1640625" style="21" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="21" customWidth="1"/>
@@ -3160,7 +3227,7 @@
     <col min="10" max="16384" width="14.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
@@ -3189,10 +3256,10 @@
         <v>7</v>
       </c>
       <c r="J1" s="108" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="240" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="240">
       <c r="A2" s="99">
         <v>1</v>
       </c>
@@ -3200,31 +3267,31 @@
         <v>42241</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="144">
       <c r="A3" s="99">
         <v>2</v>
       </c>
@@ -3233,29 +3300,29 @@
         <v>42248</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="1:10" ht="192" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="192">
       <c r="A4" s="99">
         <v>3</v>
       </c>
@@ -3264,28 +3331,28 @@
         <v>42255</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="H4" s="112" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="160" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="160">
       <c r="A5" s="99">
         <v>4</v>
       </c>
@@ -3294,28 +3361,28 @@
         <v>42262</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" ht="128">
       <c r="A6" s="99">
         <v>5</v>
       </c>
@@ -3324,28 +3391,28 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="112">
       <c r="A7" s="99">
         <v>6</v>
       </c>
@@ -3354,28 +3421,29 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>238</v>
+        <v>291</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>239</v>
+        <v>285</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>245</v>
+        <v>283</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>252</v>
+        <v>304</v>
+      </c>
+      <c r="H7" s="117" t="s">
+        <v>236</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="176" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+      <c r="J7" s="114"/>
+    </row>
+    <row r="8" spans="1:10" ht="176">
       <c r="A8" s="99">
         <v>7</v>
       </c>
@@ -3384,28 +3452,26 @@
         <v>42283</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>299</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>241</v>
+        <v>306</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>242</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="224" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="256">
       <c r="A9" s="28">
         <v>8</v>
       </c>
@@ -3414,24 +3480,24 @@
         <v>42290</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>300</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="80">
       <c r="A10" s="28">
         <v>9</v>
       </c>
@@ -3440,25 +3506,28 @@
         <v>42297</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>301</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>288</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="112">
       <c r="A11" s="28">
         <v>10</v>
       </c>
@@ -3467,25 +3536,25 @@
         <v>42304</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>121</v>
+        <v>302</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="96">
       <c r="A12" s="28">
         <v>11</v>
       </c>
@@ -3494,23 +3563,23 @@
         <v>42311</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="64">
       <c r="A13" s="28">
         <v>12</v>
       </c>
@@ -3519,21 +3588,21 @@
         <v>42318</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="128">
       <c r="A14" s="28">
         <v>13</v>
       </c>
@@ -3542,30 +3611,30 @@
         <v>42325</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H14" s="27"/>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="16">
       <c r="A15" s="28"/>
       <c r="B15" s="29">
         <f t="shared" si="0"/>
         <v>42332</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -3573,7 +3642,7 @@
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
     </row>
-    <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="80">
       <c r="A16" s="28">
         <v>14</v>
       </c>
@@ -3582,23 +3651,23 @@
         <v>42339</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="32">
       <c r="A17" s="28">
         <v>15</v>
       </c>
@@ -3607,17 +3676,17 @@
         <v>42346</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="32">
       <c r="A18" s="28" t="s">
         <v>0</v>
       </c>
@@ -3626,7 +3695,7 @@
         <v>42353</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3644,11 +3713,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD80"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.6640625" style="5"/>
     <col min="2" max="2" width="35.6640625" style="4" customWidth="1"/>
@@ -3667,7 +3736,7 @@
     <col min="21" max="16384" width="7.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="18" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -3681,10 +3750,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2" t="s">
@@ -3744,7 +3813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" ht="17" thickTop="1">
       <c r="A2" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -3758,14 +3827,14 @@
         <v>3</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F2" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G2" s="50"/>
       <c r="H2" s="31" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I2" s="5">
         <f>SUMIF($C$2:$C$71,H2,$D$2:$D$71)-30</f>
@@ -3777,7 +3846,7 @@
       </c>
       <c r="K2" s="50"/>
       <c r="L2" s="31" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M2" s="5">
         <v>59.5</v>
@@ -3823,22 +3892,22 @@
         <v>3.0837004405286344E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="16">
       <c r="A3" s="58">
         <v>1.2</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D3" s="61"/>
       <c r="E3" s="92" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F3" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G3" s="49"/>
       <c r="H3" s="47" t="s">
@@ -3900,21 +3969,21 @@
         <v>0.21806167400881057</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" ht="16">
       <c r="A4" s="58">
         <v>1.2</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C4" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D4" s="62">
         <v>2</v>
       </c>
       <c r="E4" s="93" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="50"/>
@@ -3977,12 +4046,12 @@
         <v>4.405286343612335E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="16">
       <c r="A5" s="58">
         <v>1.4</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C5" s="66" t="s">
         <v>23</v>
@@ -3991,10 +4060,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="93" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F5" s="107" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="4" t="s">
@@ -4049,24 +4118,24 @@
         <v>6.8281938325991193E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="16">
       <c r="A6" s="58">
         <v>2.1</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D6" s="61">
         <v>10</v>
       </c>
       <c r="E6" s="93" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F6" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="4" t="s">
@@ -4128,21 +4197,21 @@
         <v>2.2026431718061675E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="16">
       <c r="A7" s="58">
         <v>2.2000000000000002</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D7" s="62">
         <v>2</v>
       </c>
       <c r="E7" s="93" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -4205,12 +4274,12 @@
         <v>0.38546255506607929</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="17" thickBot="1">
       <c r="A8" s="58">
         <v>2.2999999999999998</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C8" s="68" t="s">
         <v>14</v>
@@ -4219,10 +4288,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="93" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F8" s="107" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="4"/>
@@ -4270,12 +4339,12 @@
         <v>0.23127753303964757</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="58">
         <v>2.4</v>
       </c>
       <c r="B9" s="70" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C9" s="71" t="s">
         <v>12</v>
@@ -4285,7 +4354,7 @@
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G9" s="50"/>
       <c r="H9" s="50"/>
@@ -4308,24 +4377,24 @@
       </c>
       <c r="AD9" s="5"/>
     </row>
-    <row r="10" spans="1:30" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" ht="16" thickTop="1">
       <c r="A10" s="58">
         <v>3.1</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D10" s="61">
         <v>10</v>
       </c>
       <c r="E10" s="96" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F10" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="50"/>
@@ -4333,21 +4402,21 @@
       <c r="J10" s="50"/>
       <c r="K10" s="50"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30">
       <c r="A11" s="58">
         <v>3.2</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D11" s="62">
         <v>2</v>
       </c>
       <c r="E11" s="96" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="49"/>
@@ -4356,12 +4425,12 @@
       <c r="J11" s="49"/>
       <c r="K11" s="49"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30">
       <c r="A12" s="58">
         <v>3.3</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C12" s="73" t="s">
         <v>23</v>
@@ -4370,10 +4439,10 @@
         <v>15</v>
       </c>
       <c r="E12" s="96" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F12" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
@@ -4381,24 +4450,24 @@
       <c r="J12" s="49"/>
       <c r="K12" s="49"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30">
       <c r="A13" s="58">
         <v>4.0999999999999996</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D13" s="61">
         <v>10</v>
       </c>
       <c r="E13" s="98" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F13" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G13" s="49"/>
       <c r="H13" s="49"/>
@@ -4406,21 +4475,21 @@
       <c r="J13" s="49"/>
       <c r="K13" s="49"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30">
       <c r="A14" s="58">
         <v>4.2</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D14" s="62">
         <v>2</v>
       </c>
       <c r="E14" s="98" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="49"/>
@@ -4431,12 +4500,12 @@
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30">
       <c r="A15" s="58">
         <v>4.3</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C15" s="71" t="s">
         <v>12</v>
@@ -4446,7 +4515,7 @@
       </c>
       <c r="E15" s="49"/>
       <c r="F15" s="107" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
@@ -4456,12 +4525,12 @@
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30">
       <c r="A16" s="58">
         <v>4.4000000000000004</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C16" s="60" t="s">
         <v>14</v>
@@ -4471,7 +4540,7 @@
       </c>
       <c r="E16" s="49"/>
       <c r="F16" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
@@ -4481,12 +4550,12 @@
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" s="58">
         <v>4.5</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C17" s="73" t="s">
         <v>23</v>
@@ -4495,10 +4564,10 @@
         <v>15</v>
       </c>
       <c r="E17" s="98" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F17" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
@@ -4508,24 +4577,24 @@
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" s="58">
         <v>5.0999999999999996</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D18" s="61">
         <v>10</v>
       </c>
       <c r="E18" s="98" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F18" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
@@ -4535,21 +4604,21 @@
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" s="58">
         <v>5.2</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D19" s="62">
         <v>2</v>
       </c>
       <c r="E19" s="98" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F19" s="53"/>
       <c r="G19" s="49"/>
@@ -4560,12 +4629,12 @@
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" s="58">
         <v>5.3</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C20" s="73" t="s">
         <v>23</v>
@@ -4574,10 +4643,10 @@
         <v>15</v>
       </c>
       <c r="E20" s="98" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F20" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
@@ -4587,24 +4656,24 @@
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" s="58">
         <v>6.1</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D21" s="61">
         <v>10</v>
       </c>
       <c r="E21" s="102" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F21" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
@@ -4614,21 +4683,21 @@
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" s="58">
         <v>6.2</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C22" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D22" s="62">
         <v>2</v>
       </c>
       <c r="E22" s="102" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F22" s="50"/>
       <c r="G22" s="49"/>
@@ -4637,12 +4706,12 @@
       <c r="J22" s="49"/>
       <c r="K22" s="49"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" s="58">
         <v>6.3</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C23" s="71" t="s">
         <v>12</v>
@@ -4652,7 +4721,7 @@
       </c>
       <c r="E23" s="49"/>
       <c r="F23" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
@@ -4660,12 +4729,12 @@
       <c r="J23" s="49"/>
       <c r="K23" s="49"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" s="58">
         <v>6.4</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C24" s="60" t="s">
         <v>14</v>
@@ -4675,7 +4744,7 @@
       </c>
       <c r="E24" s="49"/>
       <c r="F24" s="107" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
@@ -4685,12 +4754,12 @@
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" s="58">
         <v>6.5</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C25" s="74" t="s">
         <v>13</v>
@@ -4700,7 +4769,7 @@
       </c>
       <c r="E25" s="49"/>
       <c r="F25" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
@@ -4710,12 +4779,12 @@
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" s="58">
         <v>6.6</v>
       </c>
       <c r="B26" s="67" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C26" s="77" t="s">
         <v>24</v>
@@ -4724,10 +4793,10 @@
         <v>5</v>
       </c>
       <c r="E26" s="102" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F26" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
@@ -4737,12 +4806,12 @@
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" s="58">
         <v>6.7</v>
       </c>
       <c r="B27" s="113" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="C27" s="71" t="s">
         <v>12</v>
@@ -4760,24 +4829,24 @@
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" s="58">
         <v>7.1</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C28" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D28" s="61">
         <v>10</v>
       </c>
       <c r="E28" s="102" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F28" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
@@ -4787,21 +4856,21 @@
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="A29" s="58">
         <v>7.2</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C29" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D29" s="62">
         <v>2</v>
       </c>
       <c r="E29" s="102" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F29" s="54"/>
       <c r="G29" s="49"/>
@@ -4812,12 +4881,12 @@
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" s="58">
         <v>7.3</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C30" s="75" t="s">
         <v>14</v>
@@ -4826,10 +4895,10 @@
         <v>10</v>
       </c>
       <c r="E30" s="100" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F30" s="107" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
@@ -4839,24 +4908,24 @@
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="58">
         <v>8.1</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C31" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D31" s="61">
         <v>10</v>
       </c>
       <c r="E31" s="102" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F31" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
@@ -4866,21 +4935,21 @@
       <c r="L31" s="24"/>
       <c r="M31" s="24"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="58">
         <v>8.1999999999999993</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C32" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D32" s="62">
         <v>2</v>
       </c>
       <c r="E32" s="102" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F32" s="54"/>
       <c r="G32" s="49"/>
@@ -4889,12 +4958,12 @@
       <c r="J32" s="49"/>
       <c r="K32" s="49"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" s="58">
         <v>8.3000000000000007</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C33" s="76" t="s">
         <v>23</v>
@@ -4904,7 +4973,7 @@
       </c>
       <c r="E33" s="49"/>
       <c r="F33" s="107" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
@@ -4912,24 +4981,24 @@
       <c r="J33" s="49"/>
       <c r="K33" s="49"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" s="58">
         <v>9.1</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C34" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D34" s="61">
         <v>10</v>
       </c>
       <c r="E34" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F34" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G34" s="49"/>
       <c r="H34" s="49"/>
@@ -4937,15 +5006,15 @@
       <c r="J34" s="49"/>
       <c r="K34" s="49"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" s="58">
         <v>9.1999999999999993</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C35" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D35" s="62">
         <v>2</v>
@@ -4958,24 +5027,24 @@
       <c r="J35" s="49"/>
       <c r="K35" s="49"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" s="58">
         <v>10.1</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C36" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D36" s="61">
         <v>10</v>
       </c>
       <c r="E36" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F36" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G36" s="49"/>
       <c r="H36" s="49"/>
@@ -4983,15 +5052,15 @@
       <c r="J36" s="49"/>
       <c r="K36" s="49"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" s="58">
         <v>10.199999999999999</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C37" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D37" s="62">
         <v>2</v>
@@ -5004,12 +5073,12 @@
       <c r="J37" s="49"/>
       <c r="K37" s="49"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38" s="58">
         <v>10.3</v>
       </c>
       <c r="B38" s="67" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C38" s="73" t="s">
         <v>23</v>
@@ -5019,7 +5088,7 @@
       </c>
       <c r="E38" s="49"/>
       <c r="F38" s="56" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
@@ -5027,24 +5096,24 @@
       <c r="J38" s="49"/>
       <c r="K38" s="49"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39" s="58">
         <v>11.1</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C39" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D39" s="61">
         <v>10</v>
       </c>
       <c r="E39" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F39" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G39" s="49"/>
       <c r="H39" s="49"/>
@@ -5052,15 +5121,15 @@
       <c r="J39" s="49"/>
       <c r="K39" s="49"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" s="58">
         <v>11.2</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C40" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D40" s="62">
         <v>2</v>
@@ -5073,12 +5142,12 @@
       <c r="J40" s="49"/>
       <c r="K40" s="49"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41" s="58">
         <v>11.3</v>
       </c>
       <c r="B41" s="67" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C41" s="73" t="s">
         <v>23</v>
@@ -5088,7 +5157,7 @@
       </c>
       <c r="E41" s="49"/>
       <c r="F41" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G41" s="49"/>
       <c r="H41" s="49"/>
@@ -5096,24 +5165,24 @@
       <c r="J41" s="49"/>
       <c r="K41" s="49"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" s="58">
         <v>12.1</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C42" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D42" s="61">
         <v>10</v>
       </c>
       <c r="E42" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F42" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
@@ -5121,15 +5190,15 @@
       <c r="J42" s="49"/>
       <c r="K42" s="49"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" s="58">
         <v>12.2</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C43" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D43" s="62">
         <v>2</v>
@@ -5142,12 +5211,12 @@
       <c r="J43" s="49"/>
       <c r="K43" s="49"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44" s="58">
         <v>12.2</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C44" s="71" t="s">
         <v>12</v>
@@ -5157,7 +5226,7 @@
       </c>
       <c r="E44" s="49"/>
       <c r="F44" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G44" s="49"/>
       <c r="H44" s="49"/>
@@ -5165,12 +5234,12 @@
       <c r="J44" s="49"/>
       <c r="K44" s="49"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" s="58">
         <v>12.3</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C45" s="60" t="s">
         <v>14</v>
@@ -5180,7 +5249,7 @@
       </c>
       <c r="E45" s="49"/>
       <c r="F45" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
@@ -5188,22 +5257,22 @@
       <c r="J45" s="49"/>
       <c r="K45" s="49"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" s="58">
         <v>13.1</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C46" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D46" s="61">
         <v>10</v>
       </c>
       <c r="E46" s="49"/>
       <c r="F46" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G46" s="49"/>
       <c r="H46" s="49"/>
@@ -5211,15 +5280,15 @@
       <c r="J46" s="49"/>
       <c r="K46" s="49"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="A47" s="58">
         <v>13.2</v>
       </c>
       <c r="B47" s="65" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C47" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D47" s="62">
         <v>2</v>
@@ -5232,12 +5301,12 @@
       <c r="J47" s="49"/>
       <c r="K47" s="49"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="A48" s="58">
         <v>13.3</v>
       </c>
       <c r="B48" s="67" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C48" s="73" t="s">
         <v>23</v>
@@ -5247,7 +5316,7 @@
       </c>
       <c r="E48" s="49"/>
       <c r="F48" s="107" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
@@ -5255,22 +5324,22 @@
       <c r="J48" s="49"/>
       <c r="K48" s="49"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13">
       <c r="A49" s="58">
         <v>14.1</v>
       </c>
       <c r="B49" s="65" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C49" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D49" s="61">
         <v>10</v>
       </c>
       <c r="E49" s="49"/>
       <c r="F49" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G49" s="49"/>
       <c r="H49" s="49"/>
@@ -5278,15 +5347,15 @@
       <c r="J49" s="49"/>
       <c r="K49" s="49"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13">
       <c r="A50" s="58">
         <v>14.2</v>
       </c>
       <c r="B50" s="65" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C50" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D50" s="62">
         <v>2</v>
@@ -5299,12 +5368,12 @@
       <c r="J50" s="49"/>
       <c r="K50" s="49"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13">
       <c r="A51" s="58">
         <v>14.3</v>
       </c>
       <c r="B51" s="65" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C51" s="71" t="s">
         <v>12</v>
@@ -5314,7 +5383,7 @@
       </c>
       <c r="E51" s="49"/>
       <c r="F51" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G51" s="49"/>
       <c r="H51" s="49"/>
@@ -5322,12 +5391,12 @@
       <c r="J51" s="49"/>
       <c r="K51" s="49"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13">
       <c r="A52" s="58">
         <v>14.4</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C52" s="60" t="s">
         <v>14</v>
@@ -5337,7 +5406,7 @@
       </c>
       <c r="E52" s="49"/>
       <c r="F52" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G52" s="49"/>
       <c r="H52" s="49"/>
@@ -5345,22 +5414,22 @@
       <c r="J52" s="49"/>
       <c r="K52" s="49"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13">
       <c r="A53" s="58">
         <v>15.1</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C53" s="72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D53" s="61">
         <v>10</v>
       </c>
       <c r="E53" s="49"/>
       <c r="F53" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G53" s="49"/>
       <c r="H53" s="49"/>
@@ -5368,15 +5437,15 @@
       <c r="J53" s="49"/>
       <c r="K53" s="49"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13">
       <c r="A54" s="58">
         <v>15.2</v>
       </c>
       <c r="B54" s="65" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C54" s="64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D54" s="62">
         <v>2</v>
@@ -5389,7 +5458,7 @@
       <c r="J54" s="49"/>
       <c r="K54" s="49"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13">
       <c r="A55" s="58">
         <v>15.3</v>
       </c>
@@ -5404,7 +5473,7 @@
       </c>
       <c r="E55" s="49"/>
       <c r="F55" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G55" s="49"/>
       <c r="H55" s="49"/>
@@ -5412,7 +5481,7 @@
       <c r="J55" s="49"/>
       <c r="K55" s="49"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13">
       <c r="A56" s="58">
         <v>15.4</v>
       </c>
@@ -5427,7 +5496,7 @@
       </c>
       <c r="E56" s="49"/>
       <c r="F56" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G56" s="49"/>
       <c r="H56" s="49"/>
@@ -5435,12 +5504,12 @@
       <c r="J56" s="49"/>
       <c r="K56" s="49"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13">
       <c r="A57" s="58">
         <v>15.5</v>
       </c>
       <c r="B57" s="113" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="C57" s="71" t="s">
         <v>12</v>
@@ -5458,7 +5527,7 @@
       <c r="L57" s="24"/>
       <c r="M57" s="24"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13">
       <c r="A58" s="58">
         <v>16</v>
       </c>
@@ -5473,7 +5542,7 @@
       </c>
       <c r="E58" s="49"/>
       <c r="F58" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G58" s="49"/>
       <c r="H58" s="49"/>
@@ -5481,7 +5550,7 @@
       <c r="J58" s="49"/>
       <c r="K58" s="49"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13">
       <c r="A59" s="58">
         <v>16</v>
       </c>
@@ -5496,7 +5565,7 @@
       </c>
       <c r="E59" s="49"/>
       <c r="F59" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G59" s="49"/>
       <c r="H59" s="49"/>
@@ -5504,7 +5573,7 @@
       <c r="J59" s="49"/>
       <c r="K59" s="49"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13">
       <c r="A60" s="58">
         <v>16</v>
       </c>
@@ -5519,7 +5588,7 @@
       </c>
       <c r="E60" s="49"/>
       <c r="F60" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G60" s="49"/>
       <c r="H60" s="49"/>
@@ -5527,7 +5596,7 @@
       <c r="J60" s="49"/>
       <c r="K60" s="49"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13">
       <c r="A61" s="58">
         <v>16</v>
       </c>
@@ -5542,7 +5611,7 @@
       </c>
       <c r="E61" s="49"/>
       <c r="F61" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
@@ -5550,12 +5619,12 @@
       <c r="J61" s="49"/>
       <c r="K61" s="49"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13">
       <c r="A62" s="58">
         <v>16</v>
       </c>
       <c r="B62" s="65" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C62" s="71" t="s">
         <v>12</v>
@@ -5565,7 +5634,7 @@
       </c>
       <c r="E62" s="49"/>
       <c r="F62" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
@@ -5573,7 +5642,7 @@
       <c r="J62" s="49"/>
       <c r="K62" s="49"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13">
       <c r="A63" s="58">
         <v>16</v>
       </c>
@@ -5588,7 +5657,7 @@
       </c>
       <c r="E63" s="49"/>
       <c r="F63" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
@@ -5596,7 +5665,7 @@
       <c r="J63" s="49"/>
       <c r="K63" s="49"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13">
       <c r="A64" s="58">
         <v>16</v>
       </c>
@@ -5611,7 +5680,7 @@
       </c>
       <c r="E64" s="49"/>
       <c r="F64" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G64" s="49"/>
       <c r="H64" s="49"/>
@@ -5619,12 +5688,12 @@
       <c r="J64" s="49"/>
       <c r="K64" s="49"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26">
       <c r="A65" s="58">
         <v>16</v>
       </c>
       <c r="B65" s="78" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C65" s="71" t="s">
         <v>12</v>
@@ -5634,7 +5703,7 @@
       </c>
       <c r="E65" s="49"/>
       <c r="F65" s="107" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G65" s="49"/>
       <c r="H65" s="49"/>
@@ -5642,7 +5711,7 @@
       <c r="J65" s="49"/>
       <c r="K65" s="49"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26">
       <c r="E66" s="49"/>
       <c r="F66" s="49"/>
       <c r="G66" s="49"/>
@@ -5651,7 +5720,7 @@
       <c r="J66" s="49"/>
       <c r="K66" s="49"/>
     </row>
-    <row r="67" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" s="5" customFormat="1">
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="8"/>
@@ -5675,7 +5744,7 @@
       <c r="Y67" s="4"/>
       <c r="Z67" s="4"/>
     </row>
-    <row r="68" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" s="5" customFormat="1">
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="8"/>
@@ -5699,7 +5768,7 @@
       <c r="Y68" s="4"/>
       <c r="Z68" s="4"/>
     </row>
-    <row r="69" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" s="5" customFormat="1">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="8"/>
@@ -5723,7 +5792,7 @@
       <c r="Y69" s="4"/>
       <c r="Z69" s="4"/>
     </row>
-    <row r="70" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" s="5" customFormat="1">
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="8"/>
@@ -5747,7 +5816,7 @@
       <c r="Y70" s="4"/>
       <c r="Z70" s="4"/>
     </row>
-    <row r="71" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" s="5" customFormat="1">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="8"/>
@@ -5773,7 +5842,7 @@
       <c r="Y71" s="4"/>
       <c r="Z71" s="4"/>
     </row>
-    <row r="72" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" s="5" customFormat="1">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="8"/>
@@ -5799,7 +5868,7 @@
       <c r="Y72" s="4"/>
       <c r="Z72" s="4"/>
     </row>
-    <row r="73" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" s="5" customFormat="1">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="8"/>
@@ -5825,7 +5894,7 @@
       <c r="Y73" s="4"/>
       <c r="Z73" s="4"/>
     </row>
-    <row r="74" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" s="5" customFormat="1">
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="8"/>
@@ -5851,7 +5920,7 @@
       <c r="Y74" s="4"/>
       <c r="Z74" s="4"/>
     </row>
-    <row r="75" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" s="5" customFormat="1">
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="8"/>
@@ -5877,7 +5946,7 @@
       <c r="Y75" s="4"/>
       <c r="Z75" s="4"/>
     </row>
-    <row r="76" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" s="5" customFormat="1">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="8"/>
@@ -5903,7 +5972,7 @@
       <c r="Y76" s="4"/>
       <c r="Z76" s="4"/>
     </row>
-    <row r="77" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" s="5" customFormat="1">
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="8"/>
@@ -5929,7 +5998,7 @@
       <c r="Y77" s="4"/>
       <c r="Z77" s="4"/>
     </row>
-    <row r="78" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" s="5" customFormat="1">
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="8"/>
@@ -5955,7 +6024,7 @@
       <c r="Y78" s="4"/>
       <c r="Z78" s="4"/>
     </row>
-    <row r="79" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26" s="5" customFormat="1">
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="8"/>
@@ -5979,7 +6048,7 @@
       <c r="Y79" s="4"/>
       <c r="Z79" s="4"/>
     </row>
-    <row r="80" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" s="5" customFormat="1">
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="8"/>

</xml_diff>

<commit_message>
update schedule and add wk6 index
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH315/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81103DC6-A0FA-8A4F-8013-3D6B8E390617}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC8A7EA-1B76-40D1-A5CD-20F62CD0F89A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -20,11 +20,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">points!$A$1:$J$65</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -34,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="305">
   <si>
     <t>Finals Week</t>
   </si>
@@ -560,9 +568,6 @@
     <t>hw05 Bivariate graphing</t>
   </si>
   <si>
-    <t>hw 06 research proposal outline</t>
-  </si>
-  <si>
     <t>hw 07 Foundations for inference</t>
   </si>
   <si>
@@ -829,17 +834,8 @@
 Conduct a full 5 step hypothesis test</t>
   </si>
   <si>
-    <t xml:space="preserve">Describe how empirical research is different than other types of writing
-Identify the typical five sections of a research proposal
-Explain the basic concepts of probability
-Calculate a simple probability of an event. </t>
-  </si>
-  <si>
     <t>Analyzing relationships
 Grouped summary statistics</t>
-  </si>
-  <si>
-    <t>hw06- research proposal outline</t>
   </si>
   <si>
     <t>hw07 - foundations for inference</t>
@@ -1055,27 +1051,112 @@
     <t>Monday 4-6pm ARTS 112</t>
   </si>
   <si>
-    <t>Quiz 06 (Due 09/29 ) 
-[[10am]](https://forms.gle/9Vxb5HyC6dzPLyh96)
-[[12pm]](https://forms.gle/uEeNikFti8BJx4MJ7)</t>
-  </si>
-  <si>
     <t xml:space="preserve">How is statistics done in your field? </t>
   </si>
   <si>
     <t>hw 08- bivariate inference</t>
   </si>
   <si>
-    <t>Week 6 group quiz
-How is writing about empirical research different than other types of writing like essays?  
-321-Bridge. Now what do you think about how Statistics is used in your discipline? 
-Poster prep stage II</t>
-  </si>
-  <si>
     <t>3.1-3.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Read lecture notes on writing about empirical research
+    <t xml:space="preserve">Start the foundations assignment
+Watching an expert walk through an analysis. [[Video]](https://www.youtube.com/watch?v=go5Au01Jrvs)
+This is the guy that _created_  ggplot, dplyr and many other transformative packages for R
+Things to note is that he makes mistakes (quite a few). He shrugs it off, fixes it and continues. His coding is like a stream of consciousness narrative. This helps you (and he) understand not just what he's doing, but why he's doing it. He takes notes on what he's doing, this is super important! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify one binary and one continuous variable in your data set of interest. 
+Come prepared with summary statistics for each (n, # missing values, #yes, mean, sd)
+Watch how an expert codes: https://www.youtube.com/watch?v=go5Au01Jrvs (hint: it's not as seamless as you may think)
+Read CN 6.1-6.3 before Monday
+</t>
+  </si>
+  <si>
+    <t>Watch the assigned PDS Videos on correlation and tests for equal proportions
+Complete the T-Test and ANOVA questions in the Homework
+Review the AS Notebook on Simple Linear Regression
+Read the instructions for the Bivariate inference assignment
+Watch the PDS video on ANOVA and read CN 6.4 before Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Normal and T Distributions. </t>
+  </si>
+  <si>
+    <t>3.3-3.4</t>
+  </si>
+  <si>
+    <t>Self and peer evaluation
+Poster prep stage II
+Record die roll data into Google spreadsheet</t>
+  </si>
+  <si>
+    <t>Populations vs Samples</t>
+  </si>
+  <si>
+    <t>Sampling distributions and the CLT</t>
+  </si>
+  <si>
+    <t>4-4,2</t>
+  </si>
+  <si>
+    <t>4.3-4.4</t>
+  </si>
+  <si>
+    <t>Normal and T distributions
+Sampling distributions
+Central Limit Theorem
+Interval estimates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foundations for Inference
+Hypothesis Testing
+Bivariate inference: T-tests
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bivariate inference: ANOVA
+Bivariate inference: Chi-squared
+Bivariate Inference - Correlation
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bivariate Inference - Linear Regression
+Moderation
+</t>
+  </si>
+  <si>
+    <t>Record in-class die rolls in [[this google spreadsheet]]() Be sure to find your section and group! (Due Tue )</t>
+  </si>
+  <si>
+    <t>Introduction of probability by means of exploding kittens. 
+Simulating distributions of random variables (In class activity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure your die rolling data is recorded in Google drive. (Tue)
+Watch video, fill out course packet 3.4-3.5 (Mon).
+Read course packet 4.1-4.4 (Wed)
+Watch video, fill out course packet sections 4.5-4.6 (Friday)
+</t>
+  </si>
+  <si>
+    <t>The "All" vs the "Small": Samples and populations. 
+Sampling distributions - revisiting our die rolling. 
+Discovering the Central Limit Theorem (Start of Foundations Homework)
+Calculating probabilities of an average</t>
+  </si>
+  <si>
+    <t>Bridging your learning
+Catching up
+Midterm
+Probability Distributions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the basic concepts of probability
+Calculate a simple probability of an event. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 Read the poster prep stage II instructions. Choose the plots that you want to showcase. 
 Review and take the sample exam. 
 Watch the PDS video 8 (up to about 10 minutes)
@@ -1083,101 +1164,21 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Start the foundations assignment
-Watching an expert walk through an analysis. [[Video]](https://www.youtube.com/watch?v=go5Au01Jrvs)
-This is the guy that _created_  ggplot, dplyr and many other transformative packages for R
-Things to note is that he makes mistakes (quite a few). He shrugs it off, fixes it and continues. His coding is like a stream of consciousness narrative. This helps you (and he) understand not just what he's doing, but why he's doing it. He takes notes on what he's doing, this is super important! </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identify one binary and one continuous variable in your data set of interest. 
-Come prepared with summary statistics for each (n, # missing values, #yes, mean, sd)
-Watch how an expert codes: https://www.youtube.com/watch?v=go5Au01Jrvs (hint: it's not as seamless as you may think)
-Read CN 6.1-6.3 before Monday
-</t>
-  </si>
-  <si>
-    <t>Watch the assigned PDS Videos on correlation and tests for equal proportions
-Complete the T-Test and ANOVA questions in the Homework
-Review the AS Notebook on Simple Linear Regression
-Read the instructions for the Bivariate inference assignment
-Watch the PDS video on ANOVA and read CN 6.4 before Friday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Normal and T Distributions. </t>
-  </si>
-  <si>
-    <t>3.3-3.4</t>
-  </si>
-  <si>
-    <t>Writing about research
-Midterm
-Probability Distributions</t>
-  </si>
-  <si>
-    <t>Self and peer evaluation
-Poster prep stage II
-Record die roll data into Google spreadsheet</t>
-  </si>
-  <si>
-    <t>Discovering the CLT Worksheet (Handout) (Due 10/12 )</t>
-  </si>
-  <si>
-    <t>[hw06 research proposal outline](hw/hw06_research_proposal_outline.html) (Due 10/12 )</t>
-  </si>
-  <si>
-    <t>Populations vs Samples</t>
-  </si>
-  <si>
-    <t>Sampling distributions and the CLT</t>
-  </si>
-  <si>
-    <t>4-4,2</t>
-  </si>
-  <si>
-    <t>4.3-4.4</t>
-  </si>
-  <si>
-    <t>Normal and T distributions
-Sampling distributions
-Central Limit Theorem
-Interval estimates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foundations for Inference
-Hypothesis Testing
-Bivariate inference: T-tests
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bivariate inference: ANOVA
-Bivariate inference: Chi-squared
-Bivariate Inference - Correlation
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bivariate Inference - Linear Regression
-Moderation
-</t>
-  </si>
-  <si>
-    <t>Record in-class die rolls in [[this google spreadsheet]]() Be sure to find your section and group! (Due Tue )</t>
-  </si>
-  <si>
-    <t>Introduction of probability by means of exploding kittens. 
-Simulating distributions of random variables (In class activity)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make sure your die rolling data is recorded in Google drive. (Tue)
-Watch video, fill out course packet 3.4-3.5 (Mon).
-Read course packet 4.1-4.4 (Wed)
-Watch video, fill out course packet sections 4.5-4.6 (Friday)
-</t>
-  </si>
-  <si>
-    <t>The "All" vs the "Small": Samples and populations. 
-Sampling distributions - revisiting our die rolling. 
-Discovering the Central Limit Theorem (Start of Foundations Homework)
-Calculating probabilities of an average</t>
+    <t>Week 6 group quiz
+How is writing about empirical research different than other types of writing like essays?  
+Creating learning bridges Now what do you think about how Statistics is used in your discipline? 
+Poster prep stage II</t>
+  </si>
+  <si>
+    <t>Bridging your learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show me your learning journal some time this week. </t>
+  </si>
+  <si>
+    <t>Quiz 06 (Due 09/30 ) 
+[[10am]](https://forms.gle/9Vxb5HyC6dzPLyh96)
+[[12pm]](https://forms.gle/uEeNikFti8BJx4MJ7)</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1188,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2431,24 +2432,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="35"/>
+    <col min="1" max="2" width="8.875" style="35"/>
     <col min="3" max="3" width="0" style="35" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.33203125" style="42" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="56.375" style="42" customWidth="1"/>
+    <col min="6" max="6" width="11.125" style="35" customWidth="1"/>
     <col min="7" max="7" width="18" style="94" customWidth="1"/>
-    <col min="8" max="8" width="79.6640625" customWidth="1"/>
+    <col min="8" max="8" width="79.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="35" customFormat="1" ht="33" thickBot="1">
+    <row r="1" spans="1:8" s="35" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>75</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>63</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>96</v>
@@ -2474,7 +2475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="40">
         <v>1.1000000000000001</v>
       </c>
@@ -2482,46 +2483,46 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>64</v>
       </c>
       <c r="G2" s="94" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H2" s="95" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="40">
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="40">
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="40">
         <v>1.4</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E5" s="42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
         <v>1.5</v>
       </c>
@@ -2532,10 +2533,10 @@
         <v>79</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
         <v>1.6</v>
       </c>
@@ -2547,7 +2548,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="68">
+    <row r="8" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
         <v>2.1</v>
       </c>
@@ -2558,19 +2559,19 @@
         <v>108</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F8" s="35">
         <v>1.3</v>
       </c>
       <c r="G8" s="109" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H8" s="95" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
         <v>2.2000000000000002</v>
       </c>
@@ -2578,18 +2579,18 @@
         <v>109</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
         <v>2.2999999999999998</v>
       </c>
       <c r="D10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>2.4</v>
       </c>
@@ -2600,7 +2601,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="51">
+    <row r="12" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>3.1</v>
       </c>
@@ -2616,13 +2617,13 @@
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="110" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H12" s="95" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>3.2</v>
       </c>
@@ -2637,16 +2638,16 @@
       </c>
       <c r="H13" s="81"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>3.3</v>
       </c>
       <c r="D14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H14" s="81"/>
     </row>
-    <row r="15" spans="1:8" ht="51">
+    <row r="15" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>4.0999999999999996</v>
       </c>
@@ -2654,7 +2655,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>83</v>
@@ -2663,41 +2664,41 @@
         <v>2.1</v>
       </c>
       <c r="G15" s="110" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="H15" s="95" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>4.2</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>83</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <v>4.3</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" s="83"/>
       <c r="F17" s="84"/>
       <c r="G17" s="104"/>
       <c r="H17" s="82" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="24" customHeight="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>5.0999999999999996</v>
       </c>
@@ -2705,33 +2706,33 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>84</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G18" s="110" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H18" s="95" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>5.2</v>
       </c>
       <c r="D19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F19" s="38"/>
       <c r="G19" s="97"/>
       <c r="H19" s="95"/>
     </row>
-    <row r="20" spans="1:8" ht="26" customHeight="1">
+    <row r="20" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>6.1</v>
       </c>
@@ -2745,13 +2746,11 @@
         <v>110</v>
       </c>
       <c r="G20" s="110" t="s">
-        <v>280</v>
-      </c>
-      <c r="H20" s="101" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>304</v>
+      </c>
+      <c r="H20" s="101"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>6.2</v>
       </c>
@@ -2762,443 +2761,451 @@
         <v>85</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="H21" s="85" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <v>6.3</v>
       </c>
-      <c r="D22" s="85" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="86"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="85" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="D22" t="s">
+        <v>302</v>
+      </c>
+      <c r="H22" s="95" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <v>6.4</v>
       </c>
-      <c r="D23" t="s">
-        <v>112</v>
-      </c>
-      <c r="H23" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="D23" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="86"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="85" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
         <v>6.5</v>
       </c>
-      <c r="D24" s="82" t="s">
+      <c r="D24" t="s">
+        <v>112</v>
+      </c>
+      <c r="H24" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="40">
+        <v>6.6</v>
+      </c>
+      <c r="D25" s="82" t="s">
+        <v>196</v>
+      </c>
+      <c r="E25" s="83"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="104"/>
+      <c r="H25" s="82" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="40">
+        <v>7.1</v>
+      </c>
+      <c r="B26" s="35">
+        <v>7</v>
+      </c>
+      <c r="D26" s="115" t="s">
+        <v>283</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>241</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="G26" s="116" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="40">
+        <v>7.2</v>
+      </c>
+      <c r="D27" s="115" t="s">
+        <v>286</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="G27" s="110"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="40">
+        <v>7.3</v>
+      </c>
+      <c r="D28" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="F28" s="38" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="40">
+        <v>7.4</v>
+      </c>
+      <c r="D29" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="35">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="40">
+        <v>8.1</v>
+      </c>
+      <c r="B30" s="35">
+        <v>8</v>
+      </c>
+      <c r="D30" s="80" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="35">
+        <v>4.7</v>
+      </c>
+      <c r="G30" s="116" t="s">
+        <v>261</v>
+      </c>
+      <c r="H30" s="85" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="40">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D31" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="40">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D32" t="s">
+        <v>244</v>
+      </c>
+      <c r="F32" s="35">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="40">
+        <v>9.1</v>
+      </c>
+      <c r="B33" s="35">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="35">
+        <v>6.2</v>
+      </c>
+      <c r="G33" s="110" t="s">
+        <v>260</v>
+      </c>
+      <c r="H33" s="95" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="40">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D34" t="s">
+        <v>245</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="35">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="40">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D35" t="s">
+        <v>246</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="35">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="40">
+        <v>10.1</v>
+      </c>
+      <c r="B36" s="35">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>247</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="35">
+        <v>6.5</v>
+      </c>
+      <c r="G36" s="110" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="40">
+        <v>11.1</v>
+      </c>
+      <c r="B37" s="35">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="35">
+        <v>7</v>
+      </c>
+      <c r="G37" s="110" t="s">
+        <v>262</v>
+      </c>
+      <c r="H37" s="95" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="40">
+        <v>11.2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="40">
+        <v>11.3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>250</v>
+      </c>
+      <c r="F39" s="38" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="40">
+        <v>12.1</v>
+      </c>
+      <c r="B40" s="35">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="G40" s="110" t="s">
+        <v>266</v>
+      </c>
+      <c r="H40" s="80" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="40">
+        <v>12.2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>248</v>
+      </c>
+      <c r="E41" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" s="38"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="40">
+        <v>12.4</v>
+      </c>
+      <c r="D42" s="82" t="s">
         <v>197</v>
       </c>
-      <c r="E24" s="83"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="82" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="68">
-      <c r="A25" s="40">
-        <v>7.1</v>
-      </c>
-      <c r="B25" s="35">
-        <v>7</v>
-      </c>
-      <c r="D25" s="115" t="s">
-        <v>289</v>
-      </c>
-      <c r="E25" s="42" t="s">
-        <v>244</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>290</v>
-      </c>
-      <c r="G25" s="116" t="s">
-        <v>270</v>
-      </c>
-      <c r="H25" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="17">
-      <c r="A26" s="40">
-        <v>7.2</v>
-      </c>
-      <c r="D26" s="115" t="s">
-        <v>295</v>
-      </c>
-      <c r="F26" s="35" t="s">
-        <v>297</v>
-      </c>
-      <c r="G26" s="110"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="40">
-        <v>7.3</v>
-      </c>
-      <c r="D27" s="80" t="s">
-        <v>296</v>
-      </c>
-      <c r="F27" s="38" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="40">
-        <v>7.4</v>
-      </c>
-      <c r="D28" s="80" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="35">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="51">
-      <c r="A29" s="40">
-        <v>8.1</v>
-      </c>
-      <c r="B29" s="35">
-        <v>8</v>
-      </c>
-      <c r="D29" s="80" t="s">
-        <v>111</v>
-      </c>
-      <c r="F29" s="35">
-        <v>4.7</v>
-      </c>
-      <c r="G29" s="116" t="s">
-        <v>264</v>
-      </c>
-      <c r="H29" s="85" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="40">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="D30" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="42" t="s">
-        <v>243</v>
-      </c>
-      <c r="F30" s="35" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="40">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D31" t="s">
-        <v>247</v>
-      </c>
-      <c r="F31" s="35">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="51">
-      <c r="A32" s="40">
-        <v>9.1</v>
-      </c>
-      <c r="B32" s="35">
-        <v>9</v>
-      </c>
-      <c r="D32" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" s="35">
-        <v>6.2</v>
-      </c>
-      <c r="G32" s="110" t="s">
-        <v>263</v>
-      </c>
-      <c r="H32" s="95" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="40">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="D33" t="s">
-        <v>248</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F33" s="35">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="40">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="E42" s="83"/>
+      <c r="F42" s="84"/>
+      <c r="G42" s="104"/>
+      <c r="H42" s="82" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="40">
+        <v>13.1</v>
+      </c>
+      <c r="B43" s="35">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
         <v>249</v>
       </c>
-      <c r="E34" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="F34" s="35">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="51">
-      <c r="A35" s="40">
-        <v>10.1</v>
-      </c>
-      <c r="B35" s="35">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>250</v>
-      </c>
-      <c r="E35" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35" s="35">
-        <v>6.5</v>
-      </c>
-      <c r="G35" s="110" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="51">
-      <c r="A36" s="40">
-        <v>11.1</v>
-      </c>
-      <c r="B36" s="35">
-        <v>11</v>
-      </c>
-      <c r="D36" t="s">
-        <v>71</v>
-      </c>
-      <c r="E36" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="F36" s="35">
-        <v>7</v>
-      </c>
-      <c r="G36" s="110" t="s">
-        <v>265</v>
-      </c>
-      <c r="H36" s="95" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="40">
-        <v>11.2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="F37" s="38" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="40">
-        <v>11.3</v>
-      </c>
-      <c r="D38" t="s">
-        <v>253</v>
-      </c>
-      <c r="F38" s="38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="51">
-      <c r="A39" s="40">
-        <v>12.1</v>
-      </c>
-      <c r="B39" s="35">
-        <v>12</v>
-      </c>
-      <c r="D39" t="s">
-        <v>94</v>
-      </c>
-      <c r="E39" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="F39" s="38" t="s">
-        <v>234</v>
-      </c>
-      <c r="G39" s="110" t="s">
-        <v>269</v>
-      </c>
-      <c r="H39" s="80" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="40">
-        <v>12.2</v>
-      </c>
-      <c r="D40" t="s">
-        <v>251</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="F40" s="38"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="40">
-        <v>12.4</v>
-      </c>
-      <c r="D41" s="82" t="s">
-        <v>198</v>
-      </c>
-      <c r="E41" s="83"/>
-      <c r="F41" s="84"/>
-      <c r="G41" s="104"/>
-      <c r="H41" s="82" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="51">
-      <c r="A42" s="40">
-        <v>13.1</v>
-      </c>
-      <c r="B42" s="35">
-        <v>13</v>
-      </c>
-      <c r="D42" t="s">
-        <v>252</v>
-      </c>
-      <c r="E42" s="42" t="s">
-        <v>242</v>
-      </c>
-      <c r="F42" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="G42" s="110" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="40">
-        <v>13.2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>102</v>
+      <c r="E43" s="42" t="s">
+        <v>239</v>
       </c>
       <c r="F43" s="38" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="G43" s="110" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
+        <v>13.2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F44" s="38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="40">
         <v>14</v>
       </c>
-      <c r="D44" s="88" t="s">
-        <v>216</v>
-      </c>
-      <c r="E44" s="89"/>
-      <c r="F44" s="90"/>
-      <c r="G44" s="106"/>
-      <c r="H44" s="88"/>
-    </row>
-    <row r="45" spans="1:8" ht="51">
-      <c r="A45" s="40">
+      <c r="D45" s="88" t="s">
+        <v>215</v>
+      </c>
+      <c r="E45" s="89"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="106"/>
+      <c r="H45" s="88"/>
+    </row>
+    <row r="46" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="40">
         <v>15.1</v>
       </c>
-      <c r="B45" s="35">
+      <c r="B46" s="35">
         <v>14</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
+        <v>198</v>
+      </c>
+      <c r="F46" s="38">
+        <v>8.4</v>
+      </c>
+      <c r="G46" s="111" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="40">
+        <v>15.2</v>
+      </c>
+      <c r="D47" s="82" t="s">
         <v>199</v>
       </c>
-      <c r="F45" s="38">
-        <v>8.4</v>
-      </c>
-      <c r="G45" s="111" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="40">
-        <v>15.2</v>
-      </c>
-      <c r="D46" s="82" t="s">
+      <c r="E47" s="83"/>
+      <c r="F47" s="84"/>
+      <c r="G47" s="104"/>
+      <c r="H47" s="82" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="40">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="B48" s="35">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
         <v>200</v>
       </c>
-      <c r="E46" s="83"/>
-      <c r="F46" s="84"/>
-      <c r="G46" s="104"/>
-      <c r="H46" s="82" t="s">
+      <c r="E48" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="111" t="s">
+        <v>265</v>
+      </c>
+      <c r="H48" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="51">
-      <c r="A47" s="40">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="B47" s="35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="40">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="B49" s="35">
+        <v>16</v>
+      </c>
+      <c r="D49" t="s">
+        <v>97</v>
+      </c>
+      <c r="H49" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="40">
+        <v>17.2</v>
+      </c>
+      <c r="D50" t="s">
         <v>15</v>
       </c>
-      <c r="D47" t="s">
-        <v>201</v>
-      </c>
-      <c r="E47" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="G47" s="111" t="s">
-        <v>268</v>
-      </c>
-      <c r="H47" t="s">
+      <c r="H50" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="40">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="B48" s="35">
-        <v>16</v>
-      </c>
-      <c r="D48" t="s">
-        <v>97</v>
-      </c>
-      <c r="H48" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="40">
-        <v>17.2</v>
-      </c>
-      <c r="D49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H49" t="s">
-        <v>215</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:H49">
-    <sortCondition ref="A2:A49"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H50">
+    <sortCondition ref="A2:A50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3209,25 +3216,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="21" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="21" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="33.625" style="21" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="22" customWidth="1"/>
-    <col min="5" max="5" width="88.1640625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="88.125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="34.625" style="22" customWidth="1"/>
     <col min="7" max="8" width="38" style="22" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" style="21" customWidth="1"/>
-    <col min="10" max="16384" width="14.83203125" style="21"/>
+    <col min="9" max="9" width="25.375" style="21" customWidth="1"/>
+    <col min="10" max="16384" width="14.875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
@@ -3256,10 +3263,10 @@
         <v>7</v>
       </c>
       <c r="J1" s="108" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="240">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A2" s="99">
         <v>1</v>
       </c>
@@ -3270,28 +3277,28 @@
         <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="144">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="99">
         <v>2</v>
       </c>
@@ -3300,29 +3307,29 @@
         <v>42248</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="1:10" ht="192">
+    <row r="4" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="99">
         <v>3</v>
       </c>
@@ -3331,28 +3338,28 @@
         <v>42255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H4" s="112" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="160">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="99">
         <v>4</v>
       </c>
@@ -3361,28 +3368,28 @@
         <v>42262</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="128">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="99">
         <v>5</v>
       </c>
@@ -3391,28 +3398,28 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="G6" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="I6" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="112">
+    </row>
+    <row r="7" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="99">
         <v>6</v>
       </c>
@@ -3421,29 +3428,29 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>227</v>
+        <v>299</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H7" s="117" t="s">
+        <v>233</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="H7" s="117" t="s">
-        <v>236</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>292</v>
-      </c>
       <c r="J7" s="114"/>
     </row>
-    <row r="8" spans="1:10" ht="176">
+    <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="99">
         <v>7</v>
       </c>
@@ -3452,26 +3459,24 @@
         <v>42283</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="256">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>8</v>
       </c>
@@ -3480,24 +3485,24 @@
         <v>42290</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="21" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="80">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="28">
         <v>9</v>
       </c>
@@ -3506,13 +3511,13 @@
         <v>42297</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>41</v>
@@ -3524,10 +3529,10 @@
         <v>43</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="112">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>10</v>
       </c>
@@ -3536,7 +3541,7 @@
         <v>42304</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>47</v>
@@ -3554,7 +3559,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="96">
+    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>11</v>
       </c>
@@ -3579,7 +3584,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="64">
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>12</v>
       </c>
@@ -3588,21 +3593,21 @@
         <v>42318</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="128">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="28">
         <v>13</v>
       </c>
@@ -3611,13 +3616,13 @@
         <v>42325</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>56</v>
@@ -3627,7 +3632,7 @@
       </c>
       <c r="H14" s="27"/>
     </row>
-    <row r="15" spans="1:10" ht="16">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="29">
         <f t="shared" si="0"/>
@@ -3642,7 +3647,7 @@
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
     </row>
-    <row r="16" spans="1:10" ht="80">
+    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="28">
         <v>14</v>
       </c>
@@ -3651,7 +3656,7 @@
         <v>42339</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>52</v>
@@ -3667,7 +3672,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="32">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
         <v>15</v>
       </c>
@@ -3676,7 +3681,7 @@
         <v>42346</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>53</v>
@@ -3686,7 +3691,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="32">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>0</v>
       </c>
@@ -3714,29 +3719,29 @@
   <dimension ref="A1:AD80"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="5"/>
-    <col min="2" max="2" width="35.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="5"/>
+    <col min="2" max="2" width="35.625" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="8"/>
+    <col min="4" max="4" width="7.625" style="8"/>
     <col min="5" max="5" width="10.5" style="23" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="7.625" style="23" customWidth="1"/>
     <col min="7" max="11" width="10.5" style="23" customWidth="1"/>
     <col min="12" max="12" width="13.5" style="4" customWidth="1"/>
     <col min="13" max="13" width="10" style="5" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" style="5"/>
-    <col min="15" max="15" width="4.6640625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="7.6640625" style="4"/>
+    <col min="14" max="14" width="7.625" style="5"/>
+    <col min="15" max="15" width="4.625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="10.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="7.625" style="4"/>
     <col min="20" max="20" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="7.6640625" style="4"/>
+    <col min="21" max="16384" width="7.625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18" thickBot="1">
+    <row r="1" spans="1:30" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -3813,7 +3818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="17" thickTop="1">
+    <row r="2" spans="1:30" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -3827,10 +3832,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F2" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G2" s="50"/>
       <c r="H2" s="31" t="s">
@@ -3892,7 +3897,7 @@
         <v>3.0837004405286344E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="16">
+    <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="58">
         <v>1.2</v>
       </c>
@@ -3904,10 +3909,10 @@
       </c>
       <c r="D3" s="61"/>
       <c r="E3" s="92" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F3" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G3" s="49"/>
       <c r="H3" s="47" t="s">
@@ -3969,7 +3974,7 @@
         <v>0.21806167400881057</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="16">
+    <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="58">
         <v>1.2</v>
       </c>
@@ -3983,7 +3988,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="50"/>
@@ -4046,12 +4051,12 @@
         <v>4.405286343612335E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="16">
+    <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="58">
         <v>1.4</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="66" t="s">
         <v>23</v>
@@ -4060,10 +4065,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F5" s="107" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="4" t="s">
@@ -4118,7 +4123,7 @@
         <v>6.8281938325991193E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="16">
+    <row r="6" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="58">
         <v>2.1</v>
       </c>
@@ -4132,10 +4137,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F6" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="4" t="s">
@@ -4197,7 +4202,7 @@
         <v>2.2026431718061675E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="16">
+    <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="58">
         <v>2.2000000000000002</v>
       </c>
@@ -4211,7 +4216,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -4220,11 +4225,11 @@
       </c>
       <c r="I7" s="5">
         <f>SUMIF($C$2:$C$71,H7,$D$2:$D$71)</f>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J7" s="9">
         <f t="shared" si="0"/>
-        <v>0.22962112514351321</v>
+        <v>0.20665901262916189</v>
       </c>
       <c r="K7" s="49"/>
       <c r="L7" s="4" t="s">
@@ -4274,7 +4279,7 @@
         <v>0.38546255506607929</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="17" thickBot="1">
+    <row r="8" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="58">
         <v>2.2999999999999998</v>
       </c>
@@ -4288,16 +4293,16 @@
         <v>10</v>
       </c>
       <c r="E8" s="93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F8" s="107" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="4"/>
       <c r="I8" s="3">
         <f>SUM(I2:I7)</f>
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="50"/>
@@ -4339,7 +4344,7 @@
         <v>0.23127753303964757</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="17" thickTop="1" thickBot="1">
+    <row r="9" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="58">
         <v>2.4</v>
       </c>
@@ -4354,7 +4359,7 @@
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G9" s="50"/>
       <c r="H9" s="50"/>
@@ -4377,7 +4382,7 @@
       </c>
       <c r="AD9" s="5"/>
     </row>
-    <row r="10" spans="1:30" ht="16" thickTop="1">
+    <row r="10" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="58">
         <v>3.1</v>
       </c>
@@ -4391,10 +4396,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="96" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F10" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="50"/>
@@ -4402,7 +4407,7 @@
       <c r="J10" s="50"/>
       <c r="K10" s="50"/>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="58">
         <v>3.2</v>
       </c>
@@ -4416,7 +4421,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="96" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="49"/>
@@ -4425,7 +4430,7 @@
       <c r="J11" s="49"/>
       <c r="K11" s="49"/>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="58">
         <v>3.3</v>
       </c>
@@ -4439,10 +4444,10 @@
         <v>15</v>
       </c>
       <c r="E12" s="96" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F12" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
@@ -4450,7 +4455,7 @@
       <c r="J12" s="49"/>
       <c r="K12" s="49"/>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="58">
         <v>4.0999999999999996</v>
       </c>
@@ -4464,10 +4469,10 @@
         <v>10</v>
       </c>
       <c r="E13" s="98" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F13" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G13" s="49"/>
       <c r="H13" s="49"/>
@@ -4475,7 +4480,7 @@
       <c r="J13" s="49"/>
       <c r="K13" s="49"/>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="58">
         <v>4.2</v>
       </c>
@@ -4489,7 +4494,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="98" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="49"/>
@@ -4500,7 +4505,7 @@
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="58">
         <v>4.3</v>
       </c>
@@ -4515,7 +4520,7 @@
       </c>
       <c r="E15" s="49"/>
       <c r="F15" s="107" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
@@ -4525,7 +4530,7 @@
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="58">
         <v>4.4000000000000004</v>
       </c>
@@ -4540,7 +4545,7 @@
       </c>
       <c r="E16" s="49"/>
       <c r="F16" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
@@ -4550,7 +4555,7 @@
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="58">
         <v>4.5</v>
       </c>
@@ -4564,10 +4569,10 @@
         <v>15</v>
       </c>
       <c r="E17" s="98" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F17" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
@@ -4577,7 +4582,7 @@
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="58">
         <v>5.0999999999999996</v>
       </c>
@@ -4591,10 +4596,10 @@
         <v>10</v>
       </c>
       <c r="E18" s="98" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F18" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
@@ -4604,7 +4609,7 @@
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="58">
         <v>5.2</v>
       </c>
@@ -4618,7 +4623,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="98" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F19" s="53"/>
       <c r="G19" s="49"/>
@@ -4629,7 +4634,7 @@
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="58">
         <v>5.3</v>
       </c>
@@ -4643,10 +4648,10 @@
         <v>15</v>
       </c>
       <c r="E20" s="98" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F20" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
@@ -4656,7 +4661,7 @@
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="58">
         <v>6.1</v>
       </c>
@@ -4670,10 +4675,10 @@
         <v>10</v>
       </c>
       <c r="E21" s="102" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F21" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
@@ -4683,7 +4688,7 @@
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="58">
         <v>6.2</v>
       </c>
@@ -4697,7 +4702,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="102" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F22" s="50"/>
       <c r="G22" s="49"/>
@@ -4706,7 +4711,7 @@
       <c r="J22" s="49"/>
       <c r="K22" s="49"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="58">
         <v>6.3</v>
       </c>
@@ -4721,7 +4726,7 @@
       </c>
       <c r="E23" s="49"/>
       <c r="F23" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
@@ -4729,7 +4734,7 @@
       <c r="J23" s="49"/>
       <c r="K23" s="49"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="58">
         <v>6.4</v>
       </c>
@@ -4744,7 +4749,7 @@
       </c>
       <c r="E24" s="49"/>
       <c r="F24" s="107" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
@@ -4754,7 +4759,7 @@
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="58">
         <v>6.5</v>
       </c>
@@ -4769,7 +4774,7 @@
       </c>
       <c r="E25" s="49"/>
       <c r="F25" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
@@ -4779,7 +4784,7 @@
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="58">
         <v>6.6</v>
       </c>
@@ -4793,10 +4798,10 @@
         <v>5</v>
       </c>
       <c r="E26" s="102" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F26" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
@@ -4806,12 +4811,12 @@
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="58">
         <v>6.7</v>
       </c>
       <c r="B27" s="113" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C27" s="71" t="s">
         <v>12</v>
@@ -4829,7 +4834,7 @@
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="58">
         <v>7.1</v>
       </c>
@@ -4843,10 +4848,10 @@
         <v>10</v>
       </c>
       <c r="E28" s="102" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F28" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
@@ -4856,7 +4861,7 @@
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="58">
         <v>7.2</v>
       </c>
@@ -4870,7 +4875,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="102" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F29" s="54"/>
       <c r="G29" s="49"/>
@@ -4881,25 +4886,13 @@
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
     </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="58">
-        <v>7.3</v>
-      </c>
-      <c r="B30" s="65" t="s">
-        <v>158</v>
-      </c>
-      <c r="C30" s="75" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="61">
-        <v>10</v>
-      </c>
-      <c r="E30" s="100" t="s">
-        <v>217</v>
-      </c>
-      <c r="F30" s="107" t="s">
-        <v>256</v>
-      </c>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="58"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="100"/>
+      <c r="F30" s="107"/>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
       <c r="I30" s="49"/>
@@ -4908,7 +4901,7 @@
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="58">
         <v>8.1</v>
       </c>
@@ -4922,10 +4915,10 @@
         <v>10</v>
       </c>
       <c r="E31" s="102" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F31" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
@@ -4935,7 +4928,7 @@
       <c r="L31" s="24"/>
       <c r="M31" s="24"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="58">
         <v>8.1999999999999993</v>
       </c>
@@ -4949,7 +4942,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="102" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F32" s="54"/>
       <c r="G32" s="49"/>
@@ -4958,12 +4951,12 @@
       <c r="J32" s="49"/>
       <c r="K32" s="49"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="58">
         <v>8.3000000000000007</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C33" s="76" t="s">
         <v>23</v>
@@ -4973,7 +4966,7 @@
       </c>
       <c r="E33" s="49"/>
       <c r="F33" s="107" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
@@ -4981,7 +4974,7 @@
       <c r="J33" s="49"/>
       <c r="K33" s="49"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="58">
         <v>9.1</v>
       </c>
@@ -4995,10 +4988,10 @@
         <v>10</v>
       </c>
       <c r="E34" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F34" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G34" s="49"/>
       <c r="H34" s="49"/>
@@ -5006,7 +4999,7 @@
       <c r="J34" s="49"/>
       <c r="K34" s="49"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="58">
         <v>9.1999999999999993</v>
       </c>
@@ -5027,7 +5020,7 @@
       <c r="J35" s="49"/>
       <c r="K35" s="49"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="58">
         <v>10.1</v>
       </c>
@@ -5041,10 +5034,10 @@
         <v>10</v>
       </c>
       <c r="E36" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F36" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G36" s="49"/>
       <c r="H36" s="49"/>
@@ -5052,7 +5045,7 @@
       <c r="J36" s="49"/>
       <c r="K36" s="49"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="58">
         <v>10.199999999999999</v>
       </c>
@@ -5073,7 +5066,7 @@
       <c r="J37" s="49"/>
       <c r="K37" s="49"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="58">
         <v>10.3</v>
       </c>
@@ -5088,7 +5081,7 @@
       </c>
       <c r="E38" s="49"/>
       <c r="F38" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
@@ -5096,7 +5089,7 @@
       <c r="J38" s="49"/>
       <c r="K38" s="49"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="58">
         <v>11.1</v>
       </c>
@@ -5110,10 +5103,10 @@
         <v>10</v>
       </c>
       <c r="E39" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F39" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G39" s="49"/>
       <c r="H39" s="49"/>
@@ -5121,7 +5114,7 @@
       <c r="J39" s="49"/>
       <c r="K39" s="49"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="58">
         <v>11.2</v>
       </c>
@@ -5142,7 +5135,7 @@
       <c r="J40" s="49"/>
       <c r="K40" s="49"/>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="58">
         <v>11.3</v>
       </c>
@@ -5157,7 +5150,7 @@
       </c>
       <c r="E41" s="49"/>
       <c r="F41" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G41" s="49"/>
       <c r="H41" s="49"/>
@@ -5165,7 +5158,7 @@
       <c r="J41" s="49"/>
       <c r="K41" s="49"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="58">
         <v>12.1</v>
       </c>
@@ -5179,10 +5172,10 @@
         <v>10</v>
       </c>
       <c r="E42" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F42" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
@@ -5190,7 +5183,7 @@
       <c r="J42" s="49"/>
       <c r="K42" s="49"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="58">
         <v>12.2</v>
       </c>
@@ -5211,7 +5204,7 @@
       <c r="J43" s="49"/>
       <c r="K43" s="49"/>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="58">
         <v>12.2</v>
       </c>
@@ -5226,7 +5219,7 @@
       </c>
       <c r="E44" s="49"/>
       <c r="F44" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G44" s="49"/>
       <c r="H44" s="49"/>
@@ -5234,7 +5227,7 @@
       <c r="J44" s="49"/>
       <c r="K44" s="49"/>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="58">
         <v>12.3</v>
       </c>
@@ -5249,7 +5242,7 @@
       </c>
       <c r="E45" s="49"/>
       <c r="F45" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
@@ -5257,7 +5250,7 @@
       <c r="J45" s="49"/>
       <c r="K45" s="49"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="58">
         <v>13.1</v>
       </c>
@@ -5272,7 +5265,7 @@
       </c>
       <c r="E46" s="49"/>
       <c r="F46" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G46" s="49"/>
       <c r="H46" s="49"/>
@@ -5280,7 +5273,7 @@
       <c r="J46" s="49"/>
       <c r="K46" s="49"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="58">
         <v>13.2</v>
       </c>
@@ -5301,7 +5294,7 @@
       <c r="J47" s="49"/>
       <c r="K47" s="49"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="58">
         <v>13.3</v>
       </c>
@@ -5316,7 +5309,7 @@
       </c>
       <c r="E48" s="49"/>
       <c r="F48" s="107" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
@@ -5324,7 +5317,7 @@
       <c r="J48" s="49"/>
       <c r="K48" s="49"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="58">
         <v>14.1</v>
       </c>
@@ -5339,7 +5332,7 @@
       </c>
       <c r="E49" s="49"/>
       <c r="F49" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G49" s="49"/>
       <c r="H49" s="49"/>
@@ -5347,7 +5340,7 @@
       <c r="J49" s="49"/>
       <c r="K49" s="49"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="58">
         <v>14.2</v>
       </c>
@@ -5368,7 +5361,7 @@
       <c r="J50" s="49"/>
       <c r="K50" s="49"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="58">
         <v>14.3</v>
       </c>
@@ -5383,7 +5376,7 @@
       </c>
       <c r="E51" s="49"/>
       <c r="F51" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G51" s="49"/>
       <c r="H51" s="49"/>
@@ -5391,7 +5384,7 @@
       <c r="J51" s="49"/>
       <c r="K51" s="49"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="58">
         <v>14.4</v>
       </c>
@@ -5406,7 +5399,7 @@
       </c>
       <c r="E52" s="49"/>
       <c r="F52" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G52" s="49"/>
       <c r="H52" s="49"/>
@@ -5414,7 +5407,7 @@
       <c r="J52" s="49"/>
       <c r="K52" s="49"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="58">
         <v>15.1</v>
       </c>
@@ -5429,7 +5422,7 @@
       </c>
       <c r="E53" s="49"/>
       <c r="F53" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G53" s="49"/>
       <c r="H53" s="49"/>
@@ -5437,7 +5430,7 @@
       <c r="J53" s="49"/>
       <c r="K53" s="49"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="58">
         <v>15.2</v>
       </c>
@@ -5458,7 +5451,7 @@
       <c r="J54" s="49"/>
       <c r="K54" s="49"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="58">
         <v>15.3</v>
       </c>
@@ -5473,7 +5466,7 @@
       </c>
       <c r="E55" s="49"/>
       <c r="F55" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G55" s="49"/>
       <c r="H55" s="49"/>
@@ -5481,7 +5474,7 @@
       <c r="J55" s="49"/>
       <c r="K55" s="49"/>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="58">
         <v>15.4</v>
       </c>
@@ -5496,7 +5489,7 @@
       </c>
       <c r="E56" s="49"/>
       <c r="F56" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G56" s="49"/>
       <c r="H56" s="49"/>
@@ -5504,12 +5497,12 @@
       <c r="J56" s="49"/>
       <c r="K56" s="49"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="58">
         <v>15.5</v>
       </c>
       <c r="B57" s="113" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C57" s="71" t="s">
         <v>12</v>
@@ -5527,7 +5520,7 @@
       <c r="L57" s="24"/>
       <c r="M57" s="24"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="58">
         <v>16</v>
       </c>
@@ -5542,7 +5535,7 @@
       </c>
       <c r="E58" s="49"/>
       <c r="F58" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G58" s="49"/>
       <c r="H58" s="49"/>
@@ -5550,7 +5543,7 @@
       <c r="J58" s="49"/>
       <c r="K58" s="49"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="58">
         <v>16</v>
       </c>
@@ -5565,7 +5558,7 @@
       </c>
       <c r="E59" s="49"/>
       <c r="F59" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G59" s="49"/>
       <c r="H59" s="49"/>
@@ -5573,7 +5566,7 @@
       <c r="J59" s="49"/>
       <c r="K59" s="49"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="58">
         <v>16</v>
       </c>
@@ -5588,7 +5581,7 @@
       </c>
       <c r="E60" s="49"/>
       <c r="F60" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G60" s="49"/>
       <c r="H60" s="49"/>
@@ -5596,7 +5589,7 @@
       <c r="J60" s="49"/>
       <c r="K60" s="49"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="58">
         <v>16</v>
       </c>
@@ -5611,7 +5604,7 @@
       </c>
       <c r="E61" s="49"/>
       <c r="F61" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
@@ -5619,7 +5612,7 @@
       <c r="J61" s="49"/>
       <c r="K61" s="49"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="58">
         <v>16</v>
       </c>
@@ -5634,7 +5627,7 @@
       </c>
       <c r="E62" s="49"/>
       <c r="F62" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
@@ -5642,7 +5635,7 @@
       <c r="J62" s="49"/>
       <c r="K62" s="49"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="58">
         <v>16</v>
       </c>
@@ -5657,7 +5650,7 @@
       </c>
       <c r="E63" s="49"/>
       <c r="F63" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
@@ -5665,7 +5658,7 @@
       <c r="J63" s="49"/>
       <c r="K63" s="49"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="58">
         <v>16</v>
       </c>
@@ -5680,7 +5673,7 @@
       </c>
       <c r="E64" s="49"/>
       <c r="F64" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G64" s="49"/>
       <c r="H64" s="49"/>
@@ -5688,7 +5681,7 @@
       <c r="J64" s="49"/>
       <c r="K64" s="49"/>
     </row>
-    <row r="65" spans="1:26">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="58">
         <v>16</v>
       </c>
@@ -5703,7 +5696,7 @@
       </c>
       <c r="E65" s="49"/>
       <c r="F65" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G65" s="49"/>
       <c r="H65" s="49"/>
@@ -5711,7 +5704,7 @@
       <c r="J65" s="49"/>
       <c r="K65" s="49"/>
     </row>
-    <row r="66" spans="1:26">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E66" s="49"/>
       <c r="F66" s="49"/>
       <c r="G66" s="49"/>
@@ -5720,7 +5713,7 @@
       <c r="J66" s="49"/>
       <c r="K66" s="49"/>
     </row>
-    <row r="67" spans="1:26" s="5" customFormat="1">
+    <row r="67" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="8"/>
@@ -5744,7 +5737,7 @@
       <c r="Y67" s="4"/>
       <c r="Z67" s="4"/>
     </row>
-    <row r="68" spans="1:26" s="5" customFormat="1">
+    <row r="68" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="8"/>
@@ -5768,7 +5761,7 @@
       <c r="Y68" s="4"/>
       <c r="Z68" s="4"/>
     </row>
-    <row r="69" spans="1:26" s="5" customFormat="1">
+    <row r="69" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="8"/>
@@ -5792,7 +5785,7 @@
       <c r="Y69" s="4"/>
       <c r="Z69" s="4"/>
     </row>
-    <row r="70" spans="1:26" s="5" customFormat="1">
+    <row r="70" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="8"/>
@@ -5816,7 +5809,7 @@
       <c r="Y70" s="4"/>
       <c r="Z70" s="4"/>
     </row>
-    <row r="71" spans="1:26" s="5" customFormat="1">
+    <row r="71" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="8"/>
@@ -5842,7 +5835,7 @@
       <c r="Y71" s="4"/>
       <c r="Z71" s="4"/>
     </row>
-    <row r="72" spans="1:26" s="5" customFormat="1">
+    <row r="72" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="8"/>
@@ -5868,7 +5861,7 @@
       <c r="Y72" s="4"/>
       <c r="Z72" s="4"/>
     </row>
-    <row r="73" spans="1:26" s="5" customFormat="1">
+    <row r="73" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="8"/>
@@ -5894,7 +5887,7 @@
       <c r="Y73" s="4"/>
       <c r="Z73" s="4"/>
     </row>
-    <row r="74" spans="1:26" s="5" customFormat="1">
+    <row r="74" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="8"/>
@@ -5920,7 +5913,7 @@
       <c r="Y74" s="4"/>
       <c r="Z74" s="4"/>
     </row>
-    <row r="75" spans="1:26" s="5" customFormat="1">
+    <row r="75" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="8"/>
@@ -5946,7 +5939,7 @@
       <c r="Y75" s="4"/>
       <c r="Z75" s="4"/>
     </row>
-    <row r="76" spans="1:26" s="5" customFormat="1">
+    <row r="76" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="8"/>
@@ -5972,7 +5965,7 @@
       <c r="Y76" s="4"/>
       <c r="Z76" s="4"/>
     </row>
-    <row r="77" spans="1:26" s="5" customFormat="1">
+    <row r="77" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="8"/>
@@ -5998,7 +5991,7 @@
       <c r="Y77" s="4"/>
       <c r="Z77" s="4"/>
     </row>
-    <row r="78" spans="1:26" s="5" customFormat="1">
+    <row r="78" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="8"/>
@@ -6024,7 +6017,7 @@
       <c r="Y78" s="4"/>
       <c r="Z78" s="4"/>
     </row>
-    <row r="79" spans="1:26" s="5" customFormat="1">
+    <row r="79" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="8"/>
@@ -6048,7 +6041,7 @@
       <c r="Y79" s="4"/>
       <c r="Z79" s="4"/>
     </row>
-    <row r="80" spans="1:26" s="5" customFormat="1">
+    <row r="80" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="8"/>
@@ -6073,7 +6066,7 @@
       <c r="Z80" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F85">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F85">
     <sortCondition ref="A2:A85"/>
   </sortState>
   <phoneticPr fontId="39" type="noConversion"/>

</xml_diff>

<commit_message>
fix week 7 schedule detail
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC8A7EA-1B76-40D1-A5CD-20F62CD0F89A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5144493B-1C01-4156-A696-112E3A72E356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29160" yWindow="435" windowWidth="27870" windowHeight="14595" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="305">
   <si>
     <t>Finals Week</t>
   </si>
@@ -854,13 +854,6 @@
   </si>
   <si>
     <t>[Evaluation Form](https://forms.gle/5AM55AUCuFFkqHRL7) (Due 10/05 )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Midterm
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In class exam on Friday. [Sample exam](reading/sample_exam_1.pdf) available. </t>
   </si>
   <si>
     <t>Introduction to the instructor, class structure, materials, requirements, expectations and resources. 
@@ -1126,13 +1119,6 @@
 </t>
   </si>
   <si>
-    <t>Record in-class die rolls in [[this google spreadsheet]]() Be sure to find your section and group! (Due Tue )</t>
-  </si>
-  <si>
-    <t>Introduction of probability by means of exploding kittens. 
-Simulating distributions of random variables (In class activity)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Make sure your die rolling data is recorded in Google drive. (Tue)
 Watch video, fill out course packet 3.4-3.5 (Mon).
 Read course packet 4.1-4.4 (Wed)
@@ -1156,29 +1142,42 @@
 Calculate a simple probability of an event. </t>
   </si>
   <si>
-    <t xml:space="preserve">
-Read the poster prep stage II instructions. Choose the plots that you want to showcase. 
-Review and take the sample exam. 
-Watch the PDS video 8 (up to about 10 minutes)
-Read the course packet up through Section 3.2
-</t>
-  </si>
-  <si>
-    <t>Week 6 group quiz
-How is writing about empirical research different than other types of writing like essays?  
-Creating learning bridges Now what do you think about how Statistics is used in your discipline? 
-Poster prep stage II</t>
-  </si>
-  <si>
     <t>Bridging your learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show me your learning journal some time this week. </t>
   </si>
   <si>
     <t>Quiz 06 (Due 09/30 ) 
 [[10am]](https://forms.gle/9Vxb5HyC6dzPLyh96)
 [[12pm]](https://forms.gle/uEeNikFti8BJx4MJ7)</t>
+  </si>
+  <si>
+    <t>Week 6 group quiz
+Introduction of probability by means of exploding kittens. 
+Simulating distributions of random variables (In class activity)</t>
+  </si>
+  <si>
+    <t>Tue 8-9pm [[Zoom review session]](https://csuchico.zoom.us/j/5808362949)</t>
+  </si>
+  <si>
+    <t>Read the poster prep stage II instructions. Choose the plots that you want to showcase. (Draft due Tue)
+Review and take the sample exam. 
+Have questions ready for the midterm review session (Tue at 8-9pm) [[Zoom link]](https://csuchico.zoom.us/j/5808362949). You will need a headset or earbuds. The session will be recorded and all info will be posted in the &lt;span style="color:blue"&gt;#midterm-review&lt;/span&gt; Slack channel 
+Watch the PDS video 8 (up to about 10 minutes)
+Read the course packet up through Section 3.2</t>
+  </si>
+  <si>
+    <t>Record in-class die rolls in [[this google spreadsheet]]() Be sure to find your section and group! (Due Fri )</t>
+  </si>
+  <si>
+    <t>Learning journal checkin (Due before Fri)</t>
+  </si>
+  <si>
+    <t>In class exam on Friday. [Sample exam](reading/sample_exam_1.pdf) available.  
+Review session will be recorded and posted in  &lt;span style="color:blue"&gt;#midterm-review&lt;/span&gt;  Slack channel.</t>
+  </si>
+  <si>
+    <t>Learning journal work: Creating learning bridges. Reflect and update on your prior bridge entry. 
+Poster prep stage II - Describing relationships
+Catching up!</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1715,7 @@
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2010,6 +2009,9 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2434,8 +2436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2489,7 +2491,7 @@
         <v>64</v>
       </c>
       <c r="G2" s="94" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H2" s="95" t="s">
         <v>201</v>
@@ -2508,7 +2510,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2559,13 +2561,13 @@
         <v>108</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F8" s="35">
         <v>1.3</v>
       </c>
       <c r="G8" s="109" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H8" s="95" t="s">
         <v>202</v>
@@ -2579,7 +2581,7 @@
         <v>109</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2617,7 +2619,7 @@
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="110" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H12" s="95" t="s">
         <v>203</v>
@@ -2664,10 +2666,10 @@
         <v>2.1</v>
       </c>
       <c r="G15" s="110" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H15" s="95" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2706,7 +2708,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>84</v>
@@ -2715,7 +2717,7 @@
         <v>230</v>
       </c>
       <c r="G18" s="110" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H18" s="95" t="s">
         <v>205</v>
@@ -2746,7 +2748,7 @@
         <v>110</v>
       </c>
       <c r="G20" s="110" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="H20" s="101"/>
     </row>
@@ -2761,10 +2763,10 @@
         <v>85</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H21" s="85" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2772,13 +2774,13 @@
         <v>6.3</v>
       </c>
       <c r="D22" t="s">
+        <v>296</v>
+      </c>
+      <c r="H22" s="95" t="s">
         <v>302</v>
       </c>
-      <c r="H22" s="95" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <v>6.4</v>
       </c>
@@ -2787,9 +2789,11 @@
       </c>
       <c r="E23" s="86"/>
       <c r="F23" s="87"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="85" t="s">
-        <v>234</v>
+      <c r="G23" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="H23" s="118" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2825,16 +2829,16 @@
         <v>7</v>
       </c>
       <c r="D26" s="115" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G26" s="116" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2842,10 +2846,10 @@
         <v>7.2</v>
       </c>
       <c r="D27" s="115" t="s">
+        <v>284</v>
+      </c>
+      <c r="F27" s="35" t="s">
         <v>286</v>
-      </c>
-      <c r="F27" s="35" t="s">
-        <v>288</v>
       </c>
       <c r="G27" s="110"/>
     </row>
@@ -2854,10 +2858,10 @@
         <v>7.3</v>
       </c>
       <c r="D28" s="80" t="s">
+        <v>285</v>
+      </c>
+      <c r="F28" s="38" t="s">
         <v>287</v>
-      </c>
-      <c r="F28" s="38" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2885,7 +2889,7 @@
         <v>4.7</v>
       </c>
       <c r="G30" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H30" s="85" t="s">
         <v>207</v>
@@ -2899,7 +2903,7 @@
         <v>69</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F31" s="35" t="s">
         <v>219</v>
@@ -2910,7 +2914,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F32" s="35">
         <v>6.1</v>
@@ -2933,7 +2937,7 @@
         <v>6.2</v>
       </c>
       <c r="G33" s="110" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H33" s="95" t="s">
         <v>208</v>
@@ -2944,7 +2948,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D34" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E34" s="42" t="s">
         <v>87</v>
@@ -2958,7 +2962,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D35" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>88</v>
@@ -2975,7 +2979,7 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E36" s="42" t="s">
         <v>93</v>
@@ -2984,7 +2988,7 @@
         <v>6.5</v>
       </c>
       <c r="G36" s="110" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3004,7 +3008,7 @@
         <v>7</v>
       </c>
       <c r="G37" s="110" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H37" s="95" t="s">
         <v>209</v>
@@ -3021,7 +3025,7 @@
         <v>91</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3029,7 +3033,7 @@
         <v>11.3</v>
       </c>
       <c r="D39" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F39" s="38" t="s">
         <v>231</v>
@@ -3052,7 +3056,7 @@
         <v>231</v>
       </c>
       <c r="G40" s="110" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H40" s="80" t="s">
         <v>210</v>
@@ -3063,7 +3067,7 @@
         <v>12.2</v>
       </c>
       <c r="D41" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E41" s="42" t="s">
         <v>95</v>
@@ -3092,16 +3096,16 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E43" s="42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F43" s="38" t="s">
         <v>221</v>
       </c>
       <c r="G43" s="110" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3141,7 +3145,7 @@
         <v>8.4</v>
       </c>
       <c r="G46" s="111" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3172,7 +3176,7 @@
         <v>92</v>
       </c>
       <c r="G48" s="111" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H48" t="s">
         <v>213</v>
@@ -3189,7 +3193,7 @@
         <v>97</v>
       </c>
       <c r="H49" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3216,9 +3220,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,7 +3267,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="108" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -3280,13 +3284,13 @@
         <v>171</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>170</v>
@@ -3295,7 +3299,7 @@
         <v>159</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3313,7 +3317,7 @@
         <v>165</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
@@ -3322,7 +3326,7 @@
         <v>164</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>163</v>
@@ -3344,7 +3348,7 @@
         <v>169</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>178</v>
@@ -3353,7 +3357,7 @@
         <v>172</v>
       </c>
       <c r="H4" s="112" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>161</v>
@@ -3413,13 +3417,13 @@
         <v>175</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="99">
         <v>6</v>
       </c>
@@ -3428,25 +3432,25 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>300</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="H7" s="117" t="s">
-        <v>233</v>
+        <v>73</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J7" s="114"/>
     </row>
@@ -3459,16 +3463,16 @@
         <v>42283</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>222</v>
@@ -3485,16 +3489,16 @@
         <v>42290</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -3511,13 +3515,13 @@
         <v>42297</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>41</v>
@@ -3529,7 +3533,7 @@
         <v>43</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3541,7 +3545,7 @@
         <v>42304</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>47</v>
@@ -4068,7 +4072,7 @@
         <v>216</v>
       </c>
       <c r="F5" s="107" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="4" t="s">
@@ -4296,7 +4300,7 @@
         <v>216</v>
       </c>
       <c r="F8" s="107" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="4"/>
@@ -4520,7 +4524,7 @@
       </c>
       <c r="E15" s="49"/>
       <c r="F15" s="107" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
@@ -4749,7 +4753,7 @@
       </c>
       <c r="E24" s="49"/>
       <c r="F24" s="107" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
@@ -4816,7 +4820,7 @@
         <v>6.7</v>
       </c>
       <c r="B27" s="113" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C27" s="71" t="s">
         <v>12</v>
@@ -4966,7 +4970,7 @@
       </c>
       <c r="E33" s="49"/>
       <c r="F33" s="107" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
@@ -5309,7 +5313,7 @@
       </c>
       <c r="E48" s="49"/>
       <c r="F48" s="107" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
@@ -5502,7 +5506,7 @@
         <v>15.5</v>
       </c>
       <c r="B57" s="113" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C57" s="71" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
fix wk 7 mats
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20346"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5144493B-1C01-4156-A696-112E3A72E356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5BD66C-8130-48B5-B360-2C429FF8D18A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29160" yWindow="435" windowWidth="27870" windowHeight="14595" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29160" yWindow="435" windowWidth="27870" windowHeight="14595" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -26,14 +26,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -42,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="304">
   <si>
     <t>Finals Week</t>
   </si>
@@ -166,15 +158,6 @@
 Calculate appropriate grouped summary statistics
 Describe the relationship between two variables in plain English
 </t>
-  </si>
-  <si>
-    <t>Explain the difference between practical and statistical significance
-Distinguish between a Type I and Type II error
-Explain the concept of p-hacking
-Conduct a hypothesis test in R
-Identify an appropriate analysis depending on the data types in question
-Conduct and interpret a two-sample T-test
-Conduct and interpret an ANOVA</t>
   </si>
   <si>
     <t>Conduct and interpret a chi-squared test of association
@@ -425,9 +408,6 @@
     <t>[Notes](lecture/lec02_writing_empirical_research.html)</t>
   </si>
   <si>
-    <t>Foundations for Inference</t>
-  </si>
-  <si>
     <t>Self and Peer Evaluation</t>
   </si>
   <si>
@@ -765,9 +745,6 @@
     <t>Poster prep Stage II* (Draft Due 10/01, PR 10/03, Final 10/05 )</t>
   </si>
   <si>
-    <t>[hw07_foundations](hw/hw07_foundations.html) (Due 10/19 )</t>
-  </si>
-  <si>
     <t>[hw08_biv_inference](hw/hw08_biv_inference.html) (Due 11/02 )</t>
   </si>
   <si>
@@ -802,18 +779,10 @@
 Read the instructions for the research project - Poster preparation slides</t>
   </si>
   <si>
-    <t>4, 5</t>
-  </si>
-  <si>
     <t>8.4.3</t>
   </si>
   <si>
     <t>8.3</t>
-  </si>
-  <si>
-    <t>How is an interval estimate different from a point estimate? 
-How is an interval estimate created?
-Define the margin of error</t>
   </si>
   <si>
     <t>Watch PDS video 7
@@ -825,20 +794,8 @@
 Contingency tables - not nearly as simple as you think they  are. </t>
   </si>
   <si>
-    <t>Calculate a point estimate on a data set
-Describe the behavior of a point estimate as sample size increases
-Construct and interpret a confidence interval
-Calculate and explain the Margin of Error
-Calculate and explain what the standard error of the mean is, and explain how it is different from a standard deviation
-Explain what can make the width of a confidence interval larger or smaller
-Conduct a full 5 step hypothesis test</t>
-  </si>
-  <si>
     <t>Analyzing relationships
 Grouped summary statistics</t>
-  </si>
-  <si>
-    <t>hw07 - foundations for inference</t>
   </si>
   <si>
     <t>1.1</t>
@@ -888,16 +845,10 @@
     <t>[8 (16min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)</t>
   </si>
   <si>
-    <t>[8 (14min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)</t>
-  </si>
-  <si>
     <t>[2 (7min)](https://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)</t>
   </si>
   <si>
     <t>[2 (12min)](https://passiondrivenstatistics.com/2015/06/02/chapter-2-draft-version/)</t>
-  </si>
-  <si>
-    <t>T-test analysis</t>
   </si>
   <si>
     <t>Chi-squared analysis</t>
@@ -998,11 +949,6 @@
 [[12pm]]()</t>
   </si>
   <si>
-    <t>Quiz 07 (Due 10/06 ) 
-[[10am]]()
-[[12pm]]()</t>
-  </si>
-  <si>
     <t>Quiz 03 (Due 09/08 ) 
 [[10am]](https://forms.gle/W1GyjHgcGDrAN6GK8)
 [[12pm]](https://forms.gle/yYRae4eWMBvCwSbu6)</t>
@@ -1053,19 +999,6 @@
     <t>3.1-3.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Start the foundations assignment
-Watching an expert walk through an analysis. [[Video]](https://www.youtube.com/watch?v=go5Au01Jrvs)
-This is the guy that _created_  ggplot, dplyr and many other transformative packages for R
-Things to note is that he makes mistakes (quite a few). He shrugs it off, fixes it and continues. His coding is like a stream of consciousness narrative. This helps you (and he) understand not just what he's doing, but why he's doing it. He takes notes on what he's doing, this is super important! </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identify one binary and one continuous variable in your data set of interest. 
-Come prepared with summary statistics for each (n, # missing values, #yes, mean, sd)
-Watch how an expert codes: https://www.youtube.com/watch?v=go5Au01Jrvs (hint: it's not as seamless as you may think)
-Read CN 6.1-6.3 before Monday
-</t>
-  </si>
-  <si>
     <t>Watch the assigned PDS Videos on correlation and tests for equal proportions
 Complete the T-Test and ANOVA questions in the Homework
 Review the AS Notebook on Simple Linear Regression
@@ -1079,35 +1012,6 @@
     <t>3.3-3.4</t>
   </si>
   <si>
-    <t>Self and peer evaluation
-Poster prep stage II
-Record die roll data into Google spreadsheet</t>
-  </si>
-  <si>
-    <t>Populations vs Samples</t>
-  </si>
-  <si>
-    <t>Sampling distributions and the CLT</t>
-  </si>
-  <si>
-    <t>4-4,2</t>
-  </si>
-  <si>
-    <t>4.3-4.4</t>
-  </si>
-  <si>
-    <t>Normal and T distributions
-Sampling distributions
-Central Limit Theorem
-Interval estimates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foundations for Inference
-Hypothesis Testing
-Bivariate inference: T-tests
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bivariate inference: ANOVA
 Bivariate inference: Chi-squared
 Bivariate Inference - Correlation
@@ -1119,29 +1023,12 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Make sure your die rolling data is recorded in Google drive. (Tue)
-Watch video, fill out course packet 3.4-3.5 (Mon).
-Read course packet 4.1-4.4 (Wed)
-Watch video, fill out course packet sections 4.5-4.6 (Friday)
-</t>
-  </si>
-  <si>
-    <t>The "All" vs the "Small": Samples and populations. 
-Sampling distributions - revisiting our die rolling. 
-Discovering the Central Limit Theorem (Start of Foundations Homework)
-Calculating probabilities of an average</t>
-  </si>
-  <si>
     <t>Bridging your learning
 Catching up
 Midterm
 Probability Distributions</t>
   </si>
   <si>
-    <t xml:space="preserve">Explain the basic concepts of probability
-Calculate a simple probability of an event. </t>
-  </si>
-  <si>
     <t>Bridging your learning</t>
   </si>
   <si>
@@ -1150,34 +1037,133 @@
 [[12pm]](https://forms.gle/uEeNikFti8BJx4MJ7)</t>
   </si>
   <si>
-    <t>Week 6 group quiz
+    <t>Tue 8-9pm [[Zoom review session]](https://csuchico.zoom.us/j/5808362949)</t>
+  </si>
+  <si>
+    <t>Learning journal checkin (Due before Fri)</t>
+  </si>
+  <si>
+    <t>In class exam on Friday. [Sample exam](reading/sample_exam_1.pdf) available.  
+Review session will be recorded and posted in  &lt;span style="color:blue"&gt;#midterm-review&lt;/span&gt;  Slack channel.</t>
+  </si>
+  <si>
+    <t>Learning journal work: Creating learning bridges. Reflect and update on your prior bridge entry. 
+Poster prep stage II - Describing relationships
+Catching up!</t>
+  </si>
+  <si>
+    <t>Self and peer evaluation
+Poster prep stage II</t>
+  </si>
+  <si>
+    <t>Calculate a simple probability of an event. 
+Describe a probability distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 6 group quiz
 Introduction of probability by means of exploding kittens. 
-Simulating distributions of random variables (In class activity)</t>
-  </si>
-  <si>
-    <t>Tue 8-9pm [[Zoom review session]](https://csuchico.zoom.us/j/5808362949)</t>
+Discuss probability distributions (CP 3.1, 3.2)
+</t>
   </si>
   <si>
     <t>Read the poster prep stage II instructions. Choose the plots that you want to showcase. (Draft due Tue)
 Review and take the sample exam. 
 Have questions ready for the midterm review session (Tue at 8-9pm) [[Zoom link]](https://csuchico.zoom.us/j/5808362949). You will need a headset or earbuds. The session will be recorded and all info will be posted in the &lt;span style="color:blue"&gt;#midterm-review&lt;/span&gt; Slack channel 
 Watch the PDS video 8 (up to about 10 minutes)
-Read the course packet up through Section 3.2</t>
-  </si>
-  <si>
-    <t>Record in-class die rolls in [[this google spreadsheet]]() Be sure to find your section and group! (Due Fri )</t>
-  </si>
-  <si>
-    <t>Learning journal checkin (Due before Fri)</t>
-  </si>
-  <si>
-    <t>In class exam on Friday. [Sample exam](reading/sample_exam_1.pdf) available.  
-Review session will be recorded and posted in  &lt;span style="color:blue"&gt;#midterm-review&lt;/span&gt;  Slack channel.</t>
-  </si>
-  <si>
-    <t>Learning journal work: Creating learning bridges. Reflect and update on your prior bridge entry. 
-Poster prep stage II - Describing relationships
-Catching up!</t>
+Read the course packet Section 3.1-3.2</t>
+  </si>
+  <si>
+    <t>Sampling distributions
+Normal and T distributions
+Central Limit Theorem
+Interval estimates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point estimates as a "best guess"
+Simulating distributions of random variables [[In class activity]](hw/activity_samp_dist.html)
+</t>
+  </si>
+  <si>
+    <t>Calculate a point estimate on a data set
+Describe the behavior of a point estimate as sample size increases
+Construct and interpret a confidence interval
+Calculate and explain the Margin of Error
+Calculate and explain what the standard error of the mean is, and explain how it is different from a standard deviation
+Explain what can make the width of a confidence interval larger or smaller</t>
+  </si>
+  <si>
+    <t>Explain the difference between practical and statistical significance
+Distinguish between a Type I and Type II error
+Explain the concept of p-hacking
+Conduct a hypothesis test in R
+Identify an appropriate analysis depending on the data types in question
+Conduct and interpret a two-sample T-test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch Dr.D's video, fill out course packet 3.3-3.5 (Mon).
+Watch video, fill out course packet sections 4.5-4.6 (Wed)
+Identify one binary and one continuous variable in your data set of interest. (Fri)
+Be ready and able to calculate summary statistics for each (n, # missing values, #yes, mean, sd)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interval estimation - in class activity
+</t>
+  </si>
+  <si>
+    <t>Discovering the Central Limit Theorem
+Calculating probabilities of an average
+How is an interval estimate different from a point estimate? 
+How is an interval estimate created?</t>
+  </si>
+  <si>
+    <t>hw07 - foundations for inference
+Interval estimation - in class activity</t>
+  </si>
+  <si>
+    <t>[hw07_foundations](hw/hw07_foundations.html) (Due 10/12 ) AND 
+Interval estimation worksheet (Due 10/14 )</t>
+  </si>
+  <si>
+    <t>Sampling Distributions</t>
+  </si>
+  <si>
+    <t>Central Limit Theorem</t>
+  </si>
+  <si>
+    <t>[[Example analysis]](https://www.youtube.com/watch?v=go5Au01Jrvs)</t>
+  </si>
+  <si>
+    <t>Univariate analysis in R</t>
+  </si>
+  <si>
+    <t>Two-sample T-test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypothesis Testing Framework
+Univariate Inference
+Bivariate inference: T-tests
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch an expert walk through an analysis. [[Video]](https://www.youtube.com/watch?v=go5Au01Jrvs). This is the guy that _created_  ggplot, dplyr and many other transformative packages for R. Things to note is that he makes mistakes (quite a few). He shrugs it off, fixes it and continues. His coding is like a stream of consciousness narrative. This helps you (and he) understand not just what he's doing, but why he's doing it. He takes notes on what he's doing, this is super important! 
+Read CN 4.7 before Monday
+</t>
+  </si>
+  <si>
+    <t>Quiz 07 (Due 10/09 ) 
+[[10am]](https://forms.gle/np9DS7iABYFmYju27)
+[[12pm]](https://forms.gle/qm33T7qHW6cUnwTk7)</t>
+  </si>
+  <si>
+    <t>[8 (14min)](https://passiondrivenstatistics.com/2015/07/15/chapter-10/)
+Dr. Ds video [[TBD]]()</t>
+  </si>
+  <si>
+    <t>4.5-4.6</t>
+  </si>
+  <si>
+    <t>4.1-4.3</t>
   </si>
 </sst>
 </file>
@@ -1715,7 +1701,7 @@
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1919,13 +1905,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1973,9 +1952,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2001,17 +1977,23 @@
     <xf numFmtId="0" fontId="32" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2436,8 +2418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2447,31 +2429,31 @@
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.375" style="42" customWidth="1"/>
     <col min="6" max="6" width="11.125" style="35" customWidth="1"/>
-    <col min="7" max="7" width="18" style="94" customWidth="1"/>
+    <col min="7" max="7" width="18" style="91" customWidth="1"/>
     <col min="8" max="8" width="79.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="35" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="103" t="s">
-        <v>61</v>
+        <v>95</v>
+      </c>
+      <c r="G1" s="100" t="s">
+        <v>60</v>
       </c>
       <c r="H1" s="48" t="s">
         <v>6</v>
@@ -2485,16 +2467,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" s="94" t="s">
-        <v>250</v>
-      </c>
-      <c r="H2" s="95" t="s">
-        <v>201</v>
+        <v>63</v>
+      </c>
+      <c r="G2" s="91" t="s">
+        <v>241</v>
+      </c>
+      <c r="H2" s="92" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2502,7 +2484,7 @@
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2510,7 +2492,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2518,10 +2500,10 @@
         <v>1.4</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2529,13 +2511,13 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2543,7 +2525,7 @@
         <v>1.6</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="43"/>
       <c r="F7" s="35">
@@ -2558,19 +2540,19 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F8" s="35">
         <v>1.3</v>
       </c>
-      <c r="G8" s="109" t="s">
-        <v>256</v>
-      </c>
-      <c r="H8" s="95" t="s">
-        <v>202</v>
+      <c r="G8" s="105" t="s">
+        <v>247</v>
+      </c>
+      <c r="H8" s="92" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2578,10 +2560,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2589,7 +2571,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2597,10 +2579,10 @@
         <v>2.4</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
@@ -2612,17 +2594,17 @@
       </c>
       <c r="C12" s="36"/>
       <c r="D12" s="37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F12" s="36"/>
-      <c r="G12" s="110" t="s">
-        <v>266</v>
-      </c>
-      <c r="H12" s="95" t="s">
-        <v>203</v>
+      <c r="G12" s="106" t="s">
+        <v>256</v>
+      </c>
+      <c r="H12" s="92" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2630,10 +2612,10 @@
         <v>3.2</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F13" s="35">
         <v>1.4</v>
@@ -2645,7 +2627,7 @@
         <v>3.3</v>
       </c>
       <c r="D14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H14" s="81"/>
     </row>
@@ -2657,19 +2639,19 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" s="35">
         <v>2.1</v>
       </c>
-      <c r="G15" s="110" t="s">
-        <v>267</v>
-      </c>
-      <c r="H15" s="95" t="s">
-        <v>268</v>
+      <c r="G15" s="106" t="s">
+        <v>257</v>
+      </c>
+      <c r="H15" s="92" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2677,13 +2659,13 @@
         <v>4.2</v>
       </c>
       <c r="D16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E16" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2691,13 +2673,13 @@
         <v>4.3</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E17" s="83"/>
       <c r="F17" s="84"/>
-      <c r="G17" s="104"/>
+      <c r="G17" s="101"/>
       <c r="H17" s="82" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -2708,19 +2690,19 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="G18" s="110" t="s">
-        <v>273</v>
-      </c>
-      <c r="H18" s="95" t="s">
-        <v>205</v>
+        <v>223</v>
+      </c>
+      <c r="G18" s="106" t="s">
+        <v>263</v>
+      </c>
+      <c r="H18" s="92" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2728,11 +2710,11 @@
         <v>5.2</v>
       </c>
       <c r="D19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F19" s="38"/>
-      <c r="G19" s="97"/>
-      <c r="H19" s="95"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="92"/>
     </row>
     <row r="20" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
@@ -2742,58 +2724,56 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="G20" s="110" t="s">
-        <v>297</v>
-      </c>
-      <c r="H20" s="101"/>
+        <v>109</v>
+      </c>
+      <c r="G20" s="106" t="s">
+        <v>275</v>
+      </c>
+      <c r="H20" s="98"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>6.2</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>277</v>
-      </c>
-      <c r="H21" s="85" t="s">
-        <v>301</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="H21" s="98"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <v>6.3</v>
       </c>
       <c r="D22" t="s">
-        <v>296</v>
-      </c>
-      <c r="H22" s="95" t="s">
-        <v>302</v>
+        <v>274</v>
+      </c>
+      <c r="H22" s="92" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <v>6.4</v>
       </c>
-      <c r="D23" s="85" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="86"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="105" t="s">
-        <v>299</v>
-      </c>
-      <c r="H23" s="118" t="s">
-        <v>303</v>
+      <c r="D23" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="115"/>
+      <c r="F23" s="116"/>
+      <c r="G23" s="94" t="s">
+        <v>276</v>
+      </c>
+      <c r="H23" s="98" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2801,10 +2781,10 @@
         <v>6.5</v>
       </c>
       <c r="D24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H24" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2812,67 +2792,70 @@
         <v>6.6</v>
       </c>
       <c r="D25" s="82" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E25" s="83"/>
       <c r="F25" s="84"/>
-      <c r="G25" s="104"/>
+      <c r="G25" s="101"/>
       <c r="H25" s="82" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>7.1</v>
       </c>
       <c r="B26" s="35">
         <v>7</v>
       </c>
-      <c r="D26" s="115" t="s">
-        <v>281</v>
-      </c>
-      <c r="E26" s="42" t="s">
-        <v>239</v>
+      <c r="D26" s="98" t="s">
+        <v>269</v>
+      </c>
+      <c r="E26" s="113" t="s">
+        <v>301</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>282</v>
-      </c>
-      <c r="G26" s="116" t="s">
-        <v>265</v>
+        <v>270</v>
+      </c>
+      <c r="G26" s="106" t="s">
+        <v>300</v>
+      </c>
+      <c r="H26" s="98" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>7.2</v>
       </c>
-      <c r="D27" s="115" t="s">
-        <v>284</v>
+      <c r="D27" s="98" t="s">
+        <v>293</v>
       </c>
       <c r="F27" s="35" t="s">
-        <v>286</v>
-      </c>
-      <c r="G27" s="110"/>
+        <v>303</v>
+      </c>
+      <c r="G27" s="106"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
         <v>7.3</v>
       </c>
-      <c r="D28" s="80" t="s">
-        <v>285</v>
-      </c>
-      <c r="F28" s="38" t="s">
-        <v>287</v>
+      <c r="D28" s="92" t="s">
+        <v>294</v>
+      </c>
+      <c r="F28" s="38">
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
         <v>7.4</v>
       </c>
-      <c r="D29" s="80" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="35">
-        <v>4.5</v>
+      <c r="D29" s="92" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2882,31 +2865,31 @@
       <c r="B30" s="35">
         <v>8</v>
       </c>
-      <c r="D30" s="80" t="s">
-        <v>111</v>
+      <c r="D30" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>231</v>
       </c>
       <c r="F30" s="35">
         <v>4.7</v>
       </c>
-      <c r="G30" s="116" t="s">
-        <v>259</v>
-      </c>
-      <c r="H30" s="85" t="s">
-        <v>207</v>
+      <c r="G30" s="111" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D31" s="80" t="s">
-        <v>69</v>
+      <c r="D31" s="92" t="s">
+        <v>296</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>238</v>
-      </c>
-      <c r="F31" s="35" t="s">
-        <v>219</v>
+        <v>295</v>
+      </c>
+      <c r="F31" s="35">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2914,7 +2897,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D32" t="s">
-        <v>242</v>
+        <v>297</v>
       </c>
       <c r="F32" s="35">
         <v>6.1</v>
@@ -2928,19 +2911,19 @@
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F33" s="35">
         <v>6.2</v>
       </c>
-      <c r="G33" s="110" t="s">
-        <v>258</v>
-      </c>
-      <c r="H33" s="95" t="s">
-        <v>208</v>
+      <c r="G33" s="106" t="s">
+        <v>249</v>
+      </c>
+      <c r="H33" s="92" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2948,10 +2931,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D34" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F34" s="35">
         <v>6.3</v>
@@ -2962,10 +2945,10 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D35" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F35" s="35">
         <v>6.4</v>
@@ -2979,16 +2962,16 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F36" s="35">
         <v>6.5</v>
       </c>
-      <c r="G36" s="110" t="s">
-        <v>257</v>
+      <c r="G36" s="106" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2999,19 +2982,19 @@
         <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E37" s="42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F37" s="35">
         <v>7</v>
       </c>
-      <c r="G37" s="110" t="s">
-        <v>260</v>
-      </c>
-      <c r="H37" s="95" t="s">
-        <v>209</v>
+      <c r="G37" s="106" t="s">
+        <v>251</v>
+      </c>
+      <c r="H37" s="92" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3019,13 +3002,13 @@
         <v>11.2</v>
       </c>
       <c r="D38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E38" s="42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3033,10 +3016,10 @@
         <v>11.3</v>
       </c>
       <c r="D39" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3047,19 +3030,19 @@
         <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E40" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>231</v>
-      </c>
-      <c r="G40" s="110" t="s">
-        <v>264</v>
+        <v>224</v>
+      </c>
+      <c r="G40" s="106" t="s">
+        <v>255</v>
       </c>
       <c r="H40" s="80" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3067,10 +3050,10 @@
         <v>12.2</v>
       </c>
       <c r="D41" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="E41" s="42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F41" s="38"/>
     </row>
@@ -3079,13 +3062,13 @@
         <v>12.4</v>
       </c>
       <c r="D42" s="82" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E42" s="83"/>
       <c r="F42" s="84"/>
-      <c r="G42" s="104"/>
+      <c r="G42" s="101"/>
       <c r="H42" s="82" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3096,16 +3079,16 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="E43" s="42" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F43" s="38" t="s">
-        <v>221</v>
-      </c>
-      <c r="G43" s="110" t="s">
-        <v>261</v>
+        <v>217</v>
+      </c>
+      <c r="G43" s="106" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3113,23 +3096,23 @@
         <v>13.2</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F44" s="38" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
         <v>14</v>
       </c>
-      <c r="D45" s="88" t="s">
-        <v>215</v>
-      </c>
-      <c r="E45" s="89"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="106"/>
-      <c r="H45" s="88"/>
+      <c r="D45" s="85" t="s">
+        <v>212</v>
+      </c>
+      <c r="E45" s="86"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="102"/>
+      <c r="H45" s="85"/>
     </row>
     <row r="46" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
@@ -3139,13 +3122,13 @@
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F46" s="38">
         <v>8.4</v>
       </c>
-      <c r="G46" s="111" t="s">
-        <v>262</v>
+      <c r="G46" s="107" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3153,13 +3136,13 @@
         <v>15.2</v>
       </c>
       <c r="D47" s="82" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E47" s="83"/>
       <c r="F47" s="84"/>
-      <c r="G47" s="104"/>
+      <c r="G47" s="101"/>
       <c r="H47" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3170,16 +3153,16 @@
         <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E48" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="G48" s="111" t="s">
-        <v>263</v>
+        <v>91</v>
+      </c>
+      <c r="G48" s="107" t="s">
+        <v>254</v>
       </c>
       <c r="H48" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3190,10 +3173,10 @@
         <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H49" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3204,11 +3187,11 @@
         <v>15</v>
       </c>
       <c r="H50" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H50">
+  <sortState ref="A2:H50">
     <sortCondition ref="A2:A50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3220,9 +3203,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3266,12 +3249,12 @@
       <c r="I1" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="108" t="s">
-        <v>255</v>
+      <c r="J1" s="104" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
-      <c r="A2" s="99">
+      <c r="A2" s="96">
         <v>1</v>
       </c>
       <c r="B2" s="29">
@@ -3281,29 +3264,29 @@
         <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="99">
+      <c r="A3" s="96">
         <v>2</v>
       </c>
       <c r="B3" s="29">
@@ -3311,30 +3294,30 @@
         <v>42248</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" s="99">
+      <c r="A4" s="96">
         <v>3</v>
       </c>
       <c r="B4" s="29">
@@ -3342,29 +3325,29 @@
         <v>42255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="H4" s="112" t="s">
-        <v>269</v>
+        <v>170</v>
+      </c>
+      <c r="H4" s="108" t="s">
+        <v>259</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A5" s="99">
+      <c r="A5" s="96">
         <v>4</v>
       </c>
       <c r="B5" s="29">
@@ -3372,29 +3355,29 @@
         <v>42262</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="99">
+      <c r="A6" s="96">
         <v>5</v>
       </c>
       <c r="B6" s="29">
@@ -3402,29 +3385,29 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="99">
+      <c r="A7" s="96">
         <v>6</v>
       </c>
       <c r="B7" s="29">
@@ -3432,30 +3415,30 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="H7" s="117" t="s">
-        <v>73</v>
+        <v>282</v>
+      </c>
+      <c r="H7" s="112" t="s">
+        <v>72</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="J7" s="114"/>
-    </row>
-    <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A8" s="99">
+        <v>280</v>
+      </c>
+      <c r="J7" s="110"/>
+    </row>
+    <row r="8" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A8" s="96">
         <v>7</v>
       </c>
       <c r="B8" s="29">
@@ -3463,25 +3446,29 @@
         <v>42283</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>292</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="240" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+        <v>290</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="114">
         <v>8</v>
       </c>
       <c r="B9" s="29">
@@ -3489,25 +3476,20 @@
         <v>42290</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>287</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>278</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="21" t="s">
-        <v>227</v>
-      </c>
     </row>
     <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="28">
+      <c r="A10" s="114">
         <v>9</v>
       </c>
       <c r="B10" s="29">
@@ -3515,29 +3497,29 @@
         <v>42297</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="I10" s="21" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
+      <c r="A11" s="114">
         <v>10</v>
       </c>
       <c r="B11" s="29">
@@ -3545,26 +3527,26 @@
         <v>42304</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="28">
+      <c r="A12" s="114">
         <v>11</v>
       </c>
       <c r="B12" s="29">
@@ -3572,24 +3554,24 @@
         <v>42311</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+      <c r="A13" s="114">
         <v>12</v>
       </c>
       <c r="B13" s="29">
@@ -3597,22 +3579,22 @@
         <v>42318</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A14" s="28">
+      <c r="A14" s="114">
         <v>13</v>
       </c>
       <c r="B14" s="29">
@@ -3620,30 +3602,30 @@
         <v>42325</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="F14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="27" t="s">
-        <v>57</v>
-      </c>
       <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="114"/>
       <c r="B15" s="29">
         <f t="shared" si="0"/>
         <v>42332</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -3652,7 +3634,7 @@
       <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="28">
+      <c r="A16" s="114">
         <v>14</v>
       </c>
       <c r="B16" s="29">
@@ -3660,24 +3642,24 @@
         <v>42339</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="114">
         <v>15</v>
       </c>
       <c r="B17" s="29">
@@ -3685,10 +3667,10 @@
         <v>42346</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -3704,7 +3686,7 @@
         <v>42353</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3722,8 +3704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD80"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3759,10 +3741,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2" t="s">
@@ -3835,15 +3817,15 @@
       <c r="D2" s="8">
         <v>3</v>
       </c>
-      <c r="E2" s="91" t="s">
-        <v>216</v>
-      </c>
-      <c r="F2" s="107" t="s">
-        <v>216</v>
+      <c r="E2" s="88" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G2" s="50"/>
       <c r="H2" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I2" s="5">
         <f>SUMIF($C$2:$C$71,H2,$D$2:$D$71)-30</f>
@@ -3855,7 +3837,7 @@
       </c>
       <c r="K2" s="50"/>
       <c r="L2" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M2" s="5">
         <v>59.5</v>
@@ -3906,17 +3888,17 @@
         <v>1.2</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="61"/>
-      <c r="E3" s="92" t="s">
-        <v>216</v>
-      </c>
-      <c r="F3" s="107" t="s">
-        <v>216</v>
+      <c r="E3" s="89" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G3" s="49"/>
       <c r="H3" s="47" t="s">
@@ -3983,16 +3965,16 @@
         <v>1.2</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C4" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" s="62">
         <v>2</v>
       </c>
-      <c r="E4" s="93" t="s">
-        <v>216</v>
+      <c r="E4" s="90" t="s">
+        <v>213</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="50"/>
@@ -4060,7 +4042,7 @@
         <v>1.4</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C5" s="66" t="s">
         <v>23</v>
@@ -4068,11 +4050,11 @@
       <c r="D5" s="61">
         <v>15</v>
       </c>
-      <c r="E5" s="93" t="s">
-        <v>216</v>
-      </c>
-      <c r="F5" s="107" t="s">
-        <v>251</v>
+      <c r="E5" s="90" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="103" t="s">
+        <v>242</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="4" t="s">
@@ -4132,19 +4114,19 @@
         <v>2.1</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="61">
         <v>10</v>
       </c>
-      <c r="E6" s="93" t="s">
-        <v>216</v>
-      </c>
-      <c r="F6" s="107" t="s">
-        <v>216</v>
+      <c r="E6" s="90" t="s">
+        <v>213</v>
+      </c>
+      <c r="F6" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="4" t="s">
@@ -4211,16 +4193,16 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="62">
         <v>2</v>
       </c>
-      <c r="E7" s="93" t="s">
-        <v>216</v>
+      <c r="E7" s="90" t="s">
+        <v>213</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -4288,7 +4270,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C8" s="68" t="s">
         <v>14</v>
@@ -4296,11 +4278,11 @@
       <c r="D8" s="69">
         <v>10</v>
       </c>
-      <c r="E8" s="93" t="s">
-        <v>216</v>
-      </c>
-      <c r="F8" s="107" t="s">
-        <v>251</v>
+      <c r="E8" s="90" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="103" t="s">
+        <v>242</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="4"/>
@@ -4353,7 +4335,7 @@
         <v>2.4</v>
       </c>
       <c r="B9" s="70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="71" t="s">
         <v>12</v>
@@ -4362,8 +4344,8 @@
         <v>4</v>
       </c>
       <c r="E9" s="49"/>
-      <c r="F9" s="107" t="s">
-        <v>216</v>
+      <c r="F9" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G9" s="50"/>
       <c r="H9" s="50"/>
@@ -4391,19 +4373,19 @@
         <v>3.1</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="61">
         <v>10</v>
       </c>
-      <c r="E10" s="96" t="s">
-        <v>216</v>
-      </c>
-      <c r="F10" s="107" t="s">
-        <v>216</v>
+      <c r="E10" s="93" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="50"/>
@@ -4416,16 +4398,16 @@
         <v>3.2</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="62">
         <v>2</v>
       </c>
-      <c r="E11" s="96" t="s">
-        <v>216</v>
+      <c r="E11" s="93" t="s">
+        <v>213</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="49"/>
@@ -4439,7 +4421,7 @@
         <v>3.3</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C12" s="73" t="s">
         <v>23</v>
@@ -4447,11 +4429,11 @@
       <c r="D12" s="61">
         <v>15</v>
       </c>
-      <c r="E12" s="96" t="s">
-        <v>216</v>
-      </c>
-      <c r="F12" s="107" t="s">
-        <v>216</v>
+      <c r="E12" s="93" t="s">
+        <v>213</v>
+      </c>
+      <c r="F12" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
@@ -4464,19 +4446,19 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="61">
         <v>10</v>
       </c>
-      <c r="E13" s="98" t="s">
-        <v>216</v>
-      </c>
-      <c r="F13" s="107" t="s">
-        <v>216</v>
+      <c r="E13" s="95" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G13" s="49"/>
       <c r="H13" s="49"/>
@@ -4489,16 +4471,16 @@
         <v>4.2</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D14" s="62">
         <v>2</v>
       </c>
-      <c r="E14" s="98" t="s">
-        <v>216</v>
+      <c r="E14" s="95" t="s">
+        <v>213</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="49"/>
@@ -4514,7 +4496,7 @@
         <v>4.3</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C15" s="71" t="s">
         <v>12</v>
@@ -4523,8 +4505,8 @@
         <v>4</v>
       </c>
       <c r="E15" s="49"/>
-      <c r="F15" s="107" t="s">
-        <v>251</v>
+      <c r="F15" s="103" t="s">
+        <v>242</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
@@ -4539,7 +4521,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C16" s="60" t="s">
         <v>14</v>
@@ -4548,8 +4530,8 @@
         <v>15</v>
       </c>
       <c r="E16" s="49"/>
-      <c r="F16" s="107" t="s">
-        <v>216</v>
+      <c r="F16" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
@@ -4564,7 +4546,7 @@
         <v>4.5</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C17" s="73" t="s">
         <v>23</v>
@@ -4572,11 +4554,11 @@
       <c r="D17" s="61">
         <v>15</v>
       </c>
-      <c r="E17" s="98" t="s">
-        <v>216</v>
-      </c>
-      <c r="F17" s="107" t="s">
-        <v>216</v>
+      <c r="E17" s="95" t="s">
+        <v>213</v>
+      </c>
+      <c r="F17" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
@@ -4591,19 +4573,19 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="61">
         <v>10</v>
       </c>
-      <c r="E18" s="98" t="s">
-        <v>216</v>
-      </c>
-      <c r="F18" s="107" t="s">
-        <v>216</v>
+      <c r="E18" s="95" t="s">
+        <v>213</v>
+      </c>
+      <c r="F18" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
@@ -4618,16 +4600,16 @@
         <v>5.2</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" s="62">
         <v>2</v>
       </c>
-      <c r="E19" s="98" t="s">
-        <v>216</v>
+      <c r="E19" s="95" t="s">
+        <v>213</v>
       </c>
       <c r="F19" s="53"/>
       <c r="G19" s="49"/>
@@ -4643,7 +4625,7 @@
         <v>5.3</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C20" s="73" t="s">
         <v>23</v>
@@ -4651,11 +4633,11 @@
       <c r="D20" s="61">
         <v>15</v>
       </c>
-      <c r="E20" s="98" t="s">
-        <v>216</v>
-      </c>
-      <c r="F20" s="107" t="s">
-        <v>216</v>
+      <c r="E20" s="95" t="s">
+        <v>213</v>
+      </c>
+      <c r="F20" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
@@ -4670,19 +4652,19 @@
         <v>6.1</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="61">
         <v>10</v>
       </c>
-      <c r="E21" s="102" t="s">
-        <v>216</v>
-      </c>
-      <c r="F21" s="107" t="s">
-        <v>216</v>
+      <c r="E21" s="99" t="s">
+        <v>213</v>
+      </c>
+      <c r="F21" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
@@ -4697,16 +4679,16 @@
         <v>6.2</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" s="62">
         <v>2</v>
       </c>
-      <c r="E22" s="102" t="s">
-        <v>216</v>
+      <c r="E22" s="99" t="s">
+        <v>213</v>
       </c>
       <c r="F22" s="50"/>
       <c r="G22" s="49"/>
@@ -4720,7 +4702,7 @@
         <v>6.3</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C23" s="71" t="s">
         <v>12</v>
@@ -4729,8 +4711,8 @@
         <v>4</v>
       </c>
       <c r="E23" s="49"/>
-      <c r="F23" s="107" t="s">
-        <v>216</v>
+      <c r="F23" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
@@ -4743,7 +4725,7 @@
         <v>6.4</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C24" s="60" t="s">
         <v>14</v>
@@ -4752,8 +4734,8 @@
         <v>15</v>
       </c>
       <c r="E24" s="49"/>
-      <c r="F24" s="107" t="s">
-        <v>251</v>
+      <c r="F24" s="103" t="s">
+        <v>242</v>
       </c>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
@@ -4768,7 +4750,7 @@
         <v>6.5</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="74" t="s">
         <v>13</v>
@@ -4777,8 +4759,8 @@
         <v>50</v>
       </c>
       <c r="E25" s="49"/>
-      <c r="F25" s="107" t="s">
-        <v>216</v>
+      <c r="F25" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
@@ -4793,7 +4775,7 @@
         <v>6.6</v>
       </c>
       <c r="B26" s="67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="77" t="s">
         <v>24</v>
@@ -4801,11 +4783,11 @@
       <c r="D26" s="61">
         <v>5</v>
       </c>
-      <c r="E26" s="102" t="s">
-        <v>216</v>
-      </c>
-      <c r="F26" s="107" t="s">
-        <v>216</v>
+      <c r="E26" s="99" t="s">
+        <v>213</v>
+      </c>
+      <c r="F26" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
@@ -4819,8 +4801,8 @@
       <c r="A27" s="58">
         <v>6.7</v>
       </c>
-      <c r="B27" s="113" t="s">
-        <v>272</v>
+      <c r="B27" s="109" t="s">
+        <v>262</v>
       </c>
       <c r="C27" s="71" t="s">
         <v>12</v>
@@ -4828,8 +4810,8 @@
       <c r="D27" s="61">
         <v>5</v>
       </c>
-      <c r="E27" s="102"/>
-      <c r="F27" s="107"/>
+      <c r="E27" s="99"/>
+      <c r="F27" s="103"/>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
@@ -4843,19 +4825,19 @@
         <v>7.1</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C28" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="61">
         <v>10</v>
       </c>
-      <c r="E28" s="102" t="s">
-        <v>216</v>
-      </c>
-      <c r="F28" s="107" t="s">
-        <v>216</v>
+      <c r="E28" s="99" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
@@ -4870,16 +4852,16 @@
         <v>7.2</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C29" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D29" s="62">
         <v>2</v>
       </c>
-      <c r="E29" s="102" t="s">
-        <v>216</v>
+      <c r="E29" s="99" t="s">
+        <v>213</v>
       </c>
       <c r="F29" s="54"/>
       <c r="G29" s="49"/>
@@ -4895,8 +4877,8 @@
       <c r="B30" s="65"/>
       <c r="C30" s="75"/>
       <c r="D30" s="61"/>
-      <c r="E30" s="100"/>
-      <c r="F30" s="107"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="103"/>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
       <c r="I30" s="49"/>
@@ -4910,19 +4892,19 @@
         <v>8.1</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C31" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" s="61">
         <v>10</v>
       </c>
-      <c r="E31" s="102" t="s">
-        <v>216</v>
-      </c>
-      <c r="F31" s="107" t="s">
-        <v>216</v>
+      <c r="E31" s="99" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
@@ -4937,16 +4919,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C32" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D32" s="62">
         <v>2</v>
       </c>
-      <c r="E32" s="102" t="s">
-        <v>216</v>
+      <c r="E32" s="99" t="s">
+        <v>213</v>
       </c>
       <c r="F32" s="54"/>
       <c r="G32" s="49"/>
@@ -4960,7 +4942,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C33" s="76" t="s">
         <v>23</v>
@@ -4969,8 +4951,8 @@
         <v>15</v>
       </c>
       <c r="E33" s="49"/>
-      <c r="F33" s="107" t="s">
-        <v>251</v>
+      <c r="F33" s="103" t="s">
+        <v>242</v>
       </c>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
@@ -4983,19 +4965,19 @@
         <v>9.1</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C34" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="61">
         <v>10</v>
       </c>
-      <c r="E34" s="107" t="s">
-        <v>216</v>
-      </c>
-      <c r="F34" s="107" t="s">
-        <v>216</v>
+      <c r="E34" s="103" t="s">
+        <v>213</v>
+      </c>
+      <c r="F34" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G34" s="49"/>
       <c r="H34" s="49"/>
@@ -5008,10 +4990,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C35" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D35" s="62">
         <v>2</v>
@@ -5029,19 +5011,19 @@
         <v>10.1</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C36" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36" s="61">
         <v>10</v>
       </c>
-      <c r="E36" s="107" t="s">
-        <v>216</v>
-      </c>
-      <c r="F36" s="107" t="s">
-        <v>216</v>
+      <c r="E36" s="103" t="s">
+        <v>213</v>
+      </c>
+      <c r="F36" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G36" s="49"/>
       <c r="H36" s="49"/>
@@ -5054,10 +5036,10 @@
         <v>10.199999999999999</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C37" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D37" s="62">
         <v>2</v>
@@ -5075,7 +5057,7 @@
         <v>10.3</v>
       </c>
       <c r="B38" s="67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C38" s="73" t="s">
         <v>23</v>
@@ -5085,7 +5067,7 @@
       </c>
       <c r="E38" s="49"/>
       <c r="F38" s="56" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
@@ -5098,19 +5080,19 @@
         <v>11.1</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C39" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" s="61">
         <v>10</v>
       </c>
-      <c r="E39" s="107" t="s">
-        <v>216</v>
-      </c>
-      <c r="F39" s="107" t="s">
-        <v>216</v>
+      <c r="E39" s="103" t="s">
+        <v>213</v>
+      </c>
+      <c r="F39" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G39" s="49"/>
       <c r="H39" s="49"/>
@@ -5123,10 +5105,10 @@
         <v>11.2</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C40" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D40" s="62">
         <v>2</v>
@@ -5144,7 +5126,7 @@
         <v>11.3</v>
       </c>
       <c r="B41" s="67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C41" s="73" t="s">
         <v>23</v>
@@ -5153,8 +5135,8 @@
         <v>15</v>
       </c>
       <c r="E41" s="49"/>
-      <c r="F41" s="107" t="s">
-        <v>216</v>
+      <c r="F41" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G41" s="49"/>
       <c r="H41" s="49"/>
@@ -5167,19 +5149,19 @@
         <v>12.1</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C42" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" s="61">
         <v>10</v>
       </c>
-      <c r="E42" s="107" t="s">
-        <v>216</v>
-      </c>
-      <c r="F42" s="107" t="s">
-        <v>216</v>
+      <c r="E42" s="103" t="s">
+        <v>213</v>
+      </c>
+      <c r="F42" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
@@ -5192,10 +5174,10 @@
         <v>12.2</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C43" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D43" s="62">
         <v>2</v>
@@ -5213,7 +5195,7 @@
         <v>12.2</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C44" s="71" t="s">
         <v>12</v>
@@ -5222,8 +5204,8 @@
         <v>4</v>
       </c>
       <c r="E44" s="49"/>
-      <c r="F44" s="107" t="s">
-        <v>216</v>
+      <c r="F44" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G44" s="49"/>
       <c r="H44" s="49"/>
@@ -5236,7 +5218,7 @@
         <v>12.3</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C45" s="60" t="s">
         <v>14</v>
@@ -5245,8 +5227,8 @@
         <v>15</v>
       </c>
       <c r="E45" s="49"/>
-      <c r="F45" s="107" t="s">
-        <v>216</v>
+      <c r="F45" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
@@ -5259,17 +5241,17 @@
         <v>13.1</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C46" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D46" s="61">
         <v>10</v>
       </c>
       <c r="E46" s="49"/>
-      <c r="F46" s="107" t="s">
-        <v>216</v>
+      <c r="F46" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G46" s="49"/>
       <c r="H46" s="49"/>
@@ -5282,10 +5264,10 @@
         <v>13.2</v>
       </c>
       <c r="B47" s="65" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C47" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D47" s="62">
         <v>2</v>
@@ -5303,7 +5285,7 @@
         <v>13.3</v>
       </c>
       <c r="B48" s="67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C48" s="73" t="s">
         <v>23</v>
@@ -5312,8 +5294,8 @@
         <v>15</v>
       </c>
       <c r="E48" s="49"/>
-      <c r="F48" s="107" t="s">
-        <v>251</v>
+      <c r="F48" s="103" t="s">
+        <v>242</v>
       </c>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
@@ -5326,17 +5308,17 @@
         <v>14.1</v>
       </c>
       <c r="B49" s="65" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C49" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" s="61">
         <v>10</v>
       </c>
       <c r="E49" s="49"/>
-      <c r="F49" s="107" t="s">
-        <v>216</v>
+      <c r="F49" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G49" s="49"/>
       <c r="H49" s="49"/>
@@ -5349,10 +5331,10 @@
         <v>14.2</v>
       </c>
       <c r="B50" s="65" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C50" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D50" s="62">
         <v>2</v>
@@ -5370,7 +5352,7 @@
         <v>14.3</v>
       </c>
       <c r="B51" s="65" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C51" s="71" t="s">
         <v>12</v>
@@ -5379,8 +5361,8 @@
         <v>4</v>
       </c>
       <c r="E51" s="49"/>
-      <c r="F51" s="107" t="s">
-        <v>216</v>
+      <c r="F51" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G51" s="49"/>
       <c r="H51" s="49"/>
@@ -5393,7 +5375,7 @@
         <v>14.4</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C52" s="60" t="s">
         <v>14</v>
@@ -5402,8 +5384,8 @@
         <v>15</v>
       </c>
       <c r="E52" s="49"/>
-      <c r="F52" s="107" t="s">
-        <v>216</v>
+      <c r="F52" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G52" s="49"/>
       <c r="H52" s="49"/>
@@ -5416,17 +5398,17 @@
         <v>15.1</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C53" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D53" s="61">
         <v>10</v>
       </c>
       <c r="E53" s="49"/>
-      <c r="F53" s="107" t="s">
-        <v>216</v>
+      <c r="F53" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G53" s="49"/>
       <c r="H53" s="49"/>
@@ -5439,10 +5421,10 @@
         <v>15.2</v>
       </c>
       <c r="B54" s="65" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C54" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D54" s="62">
         <v>2</v>
@@ -5469,8 +5451,8 @@
         <v>4</v>
       </c>
       <c r="E55" s="49"/>
-      <c r="F55" s="107" t="s">
-        <v>216</v>
+      <c r="F55" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G55" s="49"/>
       <c r="H55" s="49"/>
@@ -5492,8 +5474,8 @@
         <v>10</v>
       </c>
       <c r="E56" s="49"/>
-      <c r="F56" s="107" t="s">
-        <v>216</v>
+      <c r="F56" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G56" s="49"/>
       <c r="H56" s="49"/>
@@ -5505,8 +5487,8 @@
       <c r="A57" s="58">
         <v>15.5</v>
       </c>
-      <c r="B57" s="113" t="s">
-        <v>272</v>
+      <c r="B57" s="109" t="s">
+        <v>262</v>
       </c>
       <c r="C57" s="71" t="s">
         <v>12</v>
@@ -5514,8 +5496,8 @@
       <c r="D57" s="61">
         <v>5</v>
       </c>
-      <c r="E57" s="102"/>
-      <c r="F57" s="107"/>
+      <c r="E57" s="99"/>
+      <c r="F57" s="103"/>
       <c r="G57" s="49"/>
       <c r="H57" s="49"/>
       <c r="I57" s="49"/>
@@ -5538,8 +5520,8 @@
         <v>5</v>
       </c>
       <c r="E58" s="49"/>
-      <c r="F58" s="107" t="s">
-        <v>216</v>
+      <c r="F58" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G58" s="49"/>
       <c r="H58" s="49"/>
@@ -5561,8 +5543,8 @@
         <v>10</v>
       </c>
       <c r="E59" s="49"/>
-      <c r="F59" s="107" t="s">
-        <v>216</v>
+      <c r="F59" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G59" s="49"/>
       <c r="H59" s="49"/>
@@ -5584,8 +5566,8 @@
         <v>50</v>
       </c>
       <c r="E60" s="49"/>
-      <c r="F60" s="107" t="s">
-        <v>216</v>
+      <c r="F60" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G60" s="49"/>
       <c r="H60" s="49"/>
@@ -5607,8 +5589,8 @@
         <v>2</v>
       </c>
       <c r="E61" s="49"/>
-      <c r="F61" s="107" t="s">
-        <v>216</v>
+      <c r="F61" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
@@ -5621,7 +5603,7 @@
         <v>16</v>
       </c>
       <c r="B62" s="65" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C62" s="71" t="s">
         <v>12</v>
@@ -5630,8 +5612,8 @@
         <v>3</v>
       </c>
       <c r="E62" s="49"/>
-      <c r="F62" s="107" t="s">
-        <v>216</v>
+      <c r="F62" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
@@ -5653,8 +5635,8 @@
         <v>2</v>
       </c>
       <c r="E63" s="49"/>
-      <c r="F63" s="107" t="s">
-        <v>216</v>
+      <c r="F63" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
@@ -5676,8 +5658,8 @@
         <v>10</v>
       </c>
       <c r="E64" s="49"/>
-      <c r="F64" s="107" t="s">
-        <v>216</v>
+      <c r="F64" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G64" s="49"/>
       <c r="H64" s="49"/>
@@ -5690,7 +5672,7 @@
         <v>16</v>
       </c>
       <c r="B65" s="78" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C65" s="71" t="s">
         <v>12</v>
@@ -5699,8 +5681,8 @@
         <v>6</v>
       </c>
       <c r="E65" s="49"/>
-      <c r="F65" s="107" t="s">
-        <v>216</v>
+      <c r="F65" s="103" t="s">
+        <v>213</v>
       </c>
       <c r="G65" s="49"/>
       <c r="H65" s="49"/>
@@ -6070,7 +6052,7 @@
       <c r="Z80" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F85">
+  <sortState ref="A2:F85">
     <sortCondition ref="A2:A85"/>
   </sortState>
   <phoneticPr fontId="39" type="noConversion"/>

</xml_diff>

<commit_message>
add rest of wk9 quizzes
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCC40D2-03D7-437E-B7A9-B45A48D30420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C0C02E-07BC-435D-B11E-C9FD9139B013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29280" yWindow="1155" windowWidth="24765" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -1146,16 +1146,6 @@
 Example of a single sample hypothesis test</t>
   </si>
   <si>
-    <t>Quiz 09b (Due 10/22 ) 
-[[10am]]()
-[[12pm]]()</t>
-  </si>
-  <si>
-    <t>Quiz 09c (Due 10/24 ) 
-[[10am]]()
-[[12pm]]()</t>
-  </si>
-  <si>
     <t>Quiz 09a (Due 10/20 ) 
 [[10am]](https://forms.gle/mt1XCqcvL7Sp4VdH8)
 [[12pm]](https://forms.gle/KH7REGGTG5GEk34m6)</t>
@@ -1163,6 +1153,16 @@
   <si>
     <t>Develop Research Poster
 Second chance exam</t>
+  </si>
+  <si>
+    <t>Quiz 09b (Due 10/22 ) 
+[[10am]](https://forms.gle/PuXQrQqmyNUBx5NK7)
+[[12pm]](https://forms.gle/qVsdx2wfDiHFLNpx9)</t>
+  </si>
+  <si>
+    <t>Quiz 09c (Due 10/24 ) 
+[[10am]](https://forms.gle/YdFuFcoYeWHdMtwo8)
+[[12pm]](https://forms.gle/fWKTwy8uXamWVS5FA)</t>
   </si>
 </sst>
 </file>
@@ -2411,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="B33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2916,11 +2916,11 @@
         <v>6.2</v>
       </c>
       <c r="G33" s="105" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H33" s="91"/>
     </row>
-    <row r="34" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A34" s="39">
         <v>9.1999999999999993</v>
       </c>
@@ -2933,11 +2933,11 @@
       <c r="F34" s="34">
         <v>6.3</v>
       </c>
-      <c r="G34" s="106" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="G34" s="105" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A35" s="39">
         <v>9.3000000000000007</v>
       </c>
@@ -2950,8 +2950,8 @@
       <c r="F35" s="34">
         <v>6.4</v>
       </c>
-      <c r="G35" s="106" t="s">
-        <v>304</v>
+      <c r="G35" s="105" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3153,7 +3153,7 @@
         <v>15</v>
       </c>
       <c r="D48" s="116" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E48" s="41" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
add 2wks of quizzes and hw
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C0C02E-07BC-435D-B11E-C9FD9139B013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C116B9DD-45C2-4E31-A43F-FF2B077E9287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29280" yWindow="1155" windowWidth="24765" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -676,9 +676,6 @@
     <t>[hw09_moderation](hw/hw09_moderation.html) (Due 11/09 )</t>
   </si>
   <si>
-    <t>hw10_regression (Due 11/2 3)</t>
-  </si>
-  <si>
     <t>Poster prep Stage III* (Draft Due 11/12, PR 11/14, Final 11/16 )</t>
   </si>
   <si>
@@ -831,16 +828,6 @@
 </t>
   </si>
   <si>
-    <t>Quiz 10 (Due 10/27 ) 
-[[10am]]()
-[[12pm]]()</t>
-  </si>
-  <si>
-    <t>Quiz 11 (Due 11/03 ) 
-[[10am]]()
-[[12pm]]()</t>
-  </si>
-  <si>
     <t>Quiz 13 (Due 11/17 ) 
 [[10am]]()
 [[12pm]]()</t>
@@ -852,11 +839,6 @@
   </si>
   <si>
     <t>Quiz 15 (Due 12/08 ) 
-[[10am]]()
-[[12pm]]()</t>
-  </si>
-  <si>
-    <t>Quiz 12 (Due 11/10 ) 
 [[10am]]()
 [[12pm]]()</t>
   </si>
@@ -1163,6 +1145,24 @@
     <t>Quiz 09c (Due 10/24 ) 
 [[10am]](https://forms.gle/YdFuFcoYeWHdMtwo8)
 [[12pm]](https://forms.gle/fWKTwy8uXamWVS5FA)</t>
+  </si>
+  <si>
+    <t>Quiz 10 (Due 10/27 ) 
+[[10am]](https://forms.gle/Krz3ykSGRwo83GRU6)
+[[12pm]](https://forms.gle/ohfgYKgBTC7vfCQk8)</t>
+  </si>
+  <si>
+    <t>Quiz 11 (Due 11/03 ) 
+[[10am]](https://forms.gle/iA2P2pu534FKGJwu6)
+[[12pm]](https://forms.gle/7LL6AGpAZFPrPgqWA)</t>
+  </si>
+  <si>
+    <t>Quiz 12 (Due 11/10 ) 
+[[10am]](https://forms.gle/yhtcXVUo2Wmx1RWo6)
+[[12pm]](https://forms.gle/CfriRP93zjqD9E1y9)</t>
+  </si>
+  <si>
+    <t>[hw10_regression](hw/hw10_regression.html) (Due 11/23 )</t>
   </si>
 </sst>
 </file>
@@ -1886,7 +1886,6 @@
     <xf numFmtId="0" fontId="33" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1987,6 +1986,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2411,8 +2413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="B36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2422,7 +2424,7 @@
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.375" style="41" customWidth="1"/>
     <col min="6" max="6" width="11.125" style="34" customWidth="1"/>
-    <col min="7" max="7" width="18.625" style="90" customWidth="1"/>
+    <col min="7" max="7" width="18.625" style="89" customWidth="1"/>
     <col min="8" max="8" width="79.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2440,12 +2442,12 @@
         <v>52</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="99" t="s">
+      <c r="G1" s="98" t="s">
         <v>50</v>
       </c>
       <c r="H1" s="47" t="s">
@@ -2465,10 +2467,10 @@
       <c r="F2" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="90" t="s">
-        <v>223</v>
-      </c>
-      <c r="H2" s="91" t="s">
+      <c r="G2" s="89" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" s="90" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2485,7 +2487,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2510,7 +2512,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2536,15 +2538,15 @@
         <v>97</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F8" s="34">
         <v>1.3</v>
       </c>
-      <c r="G8" s="104" t="s">
-        <v>229</v>
-      </c>
-      <c r="H8" s="91" t="s">
+      <c r="G8" s="103" t="s">
+        <v>228</v>
+      </c>
+      <c r="H8" s="90" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2556,7 +2558,7 @@
         <v>98</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2593,10 +2595,10 @@
         <v>70</v>
       </c>
       <c r="F12" s="35"/>
-      <c r="G12" s="105" t="s">
-        <v>236</v>
-      </c>
-      <c r="H12" s="91" t="s">
+      <c r="G12" s="104" t="s">
+        <v>232</v>
+      </c>
+      <c r="H12" s="90" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2613,7 +2615,7 @@
       <c r="F13" s="34">
         <v>1.4</v>
       </c>
-      <c r="H13" s="80"/>
+      <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="39">
@@ -2622,7 +2624,7 @@
       <c r="D14" t="s">
         <v>174</v>
       </c>
-      <c r="H14" s="80"/>
+      <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A15" s="39">
@@ -2640,11 +2642,11 @@
       <c r="F15" s="34">
         <v>2.1</v>
       </c>
-      <c r="G15" s="105" t="s">
-        <v>237</v>
-      </c>
-      <c r="H15" s="91" t="s">
-        <v>238</v>
+      <c r="G15" s="104" t="s">
+        <v>233</v>
+      </c>
+      <c r="H15" s="90" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2658,20 +2660,20 @@
         <v>72</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="39">
         <v>4.3</v>
       </c>
-      <c r="D17" s="81" t="s">
+      <c r="D17" s="80" t="s">
         <v>177</v>
       </c>
-      <c r="E17" s="82"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="81" t="s">
+      <c r="E17" s="81"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="99"/>
+      <c r="H17" s="80" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2683,18 +2685,18 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E18" s="41" t="s">
         <v>73</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="G18" s="105" t="s">
-        <v>243</v>
-      </c>
-      <c r="H18" s="91" t="s">
+        <v>204</v>
+      </c>
+      <c r="G18" s="104" t="s">
+        <v>239</v>
+      </c>
+      <c r="H18" s="90" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2706,8 +2708,8 @@
         <v>178</v>
       </c>
       <c r="F19" s="37"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="91"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="90"/>
     </row>
     <row r="20" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="39">
@@ -2722,10 +2724,10 @@
       <c r="E20" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="105" t="s">
-        <v>253</v>
-      </c>
-      <c r="H20" s="97"/>
+      <c r="G20" s="104" t="s">
+        <v>249</v>
+      </c>
+      <c r="H20" s="96"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="39">
@@ -2738,35 +2740,35 @@
         <v>74</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>247</v>
-      </c>
-      <c r="H21" s="97"/>
+        <v>243</v>
+      </c>
+      <c r="H21" s="96"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <v>6.3</v>
       </c>
       <c r="D22" t="s">
-        <v>252</v>
-      </c>
-      <c r="H22" s="91" t="s">
-        <v>255</v>
+        <v>248</v>
+      </c>
+      <c r="H22" s="90" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="39">
         <v>6.4</v>
       </c>
-      <c r="D23" s="91" t="s">
+      <c r="D23" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="113"/>
-      <c r="F23" s="114"/>
-      <c r="G23" s="93" t="s">
-        <v>254</v>
-      </c>
-      <c r="H23" s="97" t="s">
-        <v>256</v>
+      <c r="E23" s="112"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="92" t="s">
+        <v>250</v>
+      </c>
+      <c r="H23" s="96" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2777,20 +2779,20 @@
         <v>100</v>
       </c>
       <c r="H24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="39">
         <v>6.6</v>
       </c>
-      <c r="D25" s="81" t="s">
+      <c r="D25" s="80" t="s">
         <v>179</v>
       </c>
-      <c r="E25" s="82"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="100"/>
-      <c r="H25" s="81" t="s">
+      <c r="E25" s="81"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="99"/>
+      <c r="H25" s="80" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2801,54 +2803,54 @@
       <c r="B26" s="34">
         <v>7</v>
       </c>
-      <c r="D26" s="97" t="s">
-        <v>248</v>
-      </c>
-      <c r="E26" s="111" t="s">
-        <v>275</v>
+      <c r="D26" s="96" t="s">
+        <v>244</v>
+      </c>
+      <c r="E26" s="110" t="s">
+        <v>271</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="G26" s="105" t="s">
-        <v>276</v>
-      </c>
-      <c r="H26" s="97" t="s">
-        <v>278</v>
+        <v>245</v>
+      </c>
+      <c r="G26" s="104" t="s">
+        <v>272</v>
+      </c>
+      <c r="H26" s="96" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="39">
         <v>7.2</v>
       </c>
-      <c r="D27" s="97" t="s">
-        <v>266</v>
+      <c r="D27" s="96" t="s">
+        <v>262</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>273</v>
-      </c>
-      <c r="G27" s="105"/>
+        <v>269</v>
+      </c>
+      <c r="G27" s="104"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="39">
         <v>7.3</v>
       </c>
-      <c r="D28" s="91" t="s">
-        <v>267</v>
+      <c r="D28" s="90" t="s">
+        <v>263</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="39">
         <v>7.4</v>
       </c>
-      <c r="D29" s="91" t="s">
+      <c r="D29" s="90" t="s">
         <v>65</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
@@ -2858,31 +2860,31 @@
       <c r="B30" s="34">
         <v>8</v>
       </c>
-      <c r="D30" s="91" t="s">
+      <c r="D30" s="90" t="s">
         <v>58</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F30" s="34">
         <v>4.7</v>
       </c>
-      <c r="G30" s="105" t="s">
-        <v>277</v>
-      </c>
-      <c r="H30" s="91" t="s">
-        <v>300</v>
+      <c r="G30" s="104" t="s">
+        <v>273</v>
+      </c>
+      <c r="H30" s="90" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="39">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D31" s="91" t="s">
-        <v>269</v>
+      <c r="D31" s="90" t="s">
+        <v>265</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F31" s="34">
         <v>5</v>
@@ -2893,7 +2895,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D32" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F32" s="34">
         <v>6.1</v>
@@ -2915,17 +2917,17 @@
       <c r="F33" s="34">
         <v>6.2</v>
       </c>
-      <c r="G33" s="105" t="s">
-        <v>303</v>
-      </c>
-      <c r="H33" s="91"/>
+      <c r="G33" s="104" t="s">
+        <v>299</v>
+      </c>
+      <c r="H33" s="90"/>
     </row>
     <row r="34" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A34" s="39">
         <v>9.1999999999999993</v>
       </c>
       <c r="D34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E34" s="41" t="s">
         <v>76</v>
@@ -2933,8 +2935,8 @@
       <c r="F34" s="34">
         <v>6.3</v>
       </c>
-      <c r="G34" s="105" t="s">
-        <v>305</v>
+      <c r="G34" s="104" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="126" x14ac:dyDescent="0.25">
@@ -2942,7 +2944,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E35" s="41" t="s">
         <v>77</v>
@@ -2950,11 +2952,11 @@
       <c r="F35" s="34">
         <v>6.4</v>
       </c>
-      <c r="G35" s="105" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G35" s="104" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A36" s="39">
         <v>10.1</v>
       </c>
@@ -2962,7 +2964,7 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E36" s="41" t="s">
         <v>82</v>
@@ -2970,11 +2972,11 @@
       <c r="F36" s="34">
         <v>6.5</v>
       </c>
-      <c r="G36" s="106" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G36" s="116" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A37" s="39">
         <v>11.1</v>
       </c>
@@ -2990,10 +2992,10 @@
       <c r="F37" s="34">
         <v>7</v>
       </c>
-      <c r="G37" s="106" t="s">
-        <v>231</v>
-      </c>
-      <c r="H37" s="79" t="s">
+      <c r="G37" s="104" t="s">
+        <v>304</v>
+      </c>
+      <c r="H37" s="90" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3008,7 +3010,7 @@
         <v>80</v>
       </c>
       <c r="F38" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3016,13 +3018,13 @@
         <v>11.3</v>
       </c>
       <c r="D39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A40" s="39">
         <v>12.1</v>
       </c>
@@ -3036,13 +3038,13 @@
         <v>79</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="G40" s="106" t="s">
-        <v>235</v>
-      </c>
-      <c r="H40" s="79" t="s">
-        <v>190</v>
+        <v>205</v>
+      </c>
+      <c r="G40" s="104" t="s">
+        <v>305</v>
+      </c>
+      <c r="H40" s="90" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3050,7 +3052,7 @@
         <v>12.2</v>
       </c>
       <c r="D41" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E41" s="41" t="s">
         <v>84</v>
@@ -3061,14 +3063,14 @@
       <c r="A42" s="39">
         <v>12.4</v>
       </c>
-      <c r="D42" s="81" t="s">
+      <c r="D42" s="80" t="s">
         <v>180</v>
       </c>
-      <c r="E42" s="82"/>
-      <c r="F42" s="83"/>
-      <c r="G42" s="100"/>
-      <c r="H42" s="81" t="s">
-        <v>191</v>
+      <c r="E42" s="81"/>
+      <c r="F42" s="82"/>
+      <c r="G42" s="99"/>
+      <c r="H42" s="80" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3079,16 +3081,16 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E43" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F43" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="G43" s="106" t="s">
-        <v>232</v>
+        <v>198</v>
+      </c>
+      <c r="G43" s="105" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3099,20 +3101,20 @@
         <v>91</v>
       </c>
       <c r="F44" s="37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="39">
         <v>14</v>
       </c>
-      <c r="D45" s="84" t="s">
-        <v>194</v>
-      </c>
-      <c r="E45" s="85"/>
-      <c r="F45" s="86"/>
-      <c r="G45" s="101"/>
-      <c r="H45" s="84"/>
+      <c r="D45" s="83" t="s">
+        <v>193</v>
+      </c>
+      <c r="E45" s="84"/>
+      <c r="F45" s="85"/>
+      <c r="G45" s="100"/>
+      <c r="H45" s="83"/>
     </row>
     <row r="46" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="39">
@@ -3127,22 +3129,22 @@
       <c r="F46" s="37">
         <v>8.4</v>
       </c>
-      <c r="G46" s="106" t="s">
-        <v>233</v>
+      <c r="G46" s="105" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="39">
         <v>15.2</v>
       </c>
-      <c r="D47" s="81" t="s">
+      <c r="D47" s="80" t="s">
         <v>182</v>
       </c>
-      <c r="E47" s="82"/>
-      <c r="F47" s="83"/>
-      <c r="G47" s="100"/>
-      <c r="H47" s="81" t="s">
-        <v>192</v>
+      <c r="E47" s="81"/>
+      <c r="F47" s="82"/>
+      <c r="G47" s="99"/>
+      <c r="H47" s="80" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3152,17 +3154,17 @@
       <c r="B48" s="34">
         <v>15</v>
       </c>
-      <c r="D48" s="116" t="s">
-        <v>304</v>
+      <c r="D48" s="115" t="s">
+        <v>300</v>
       </c>
       <c r="E48" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="G48" s="106" t="s">
-        <v>234</v>
+      <c r="G48" s="105" t="s">
+        <v>231</v>
       </c>
       <c r="H48" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3176,7 +3178,7 @@
         <v>86</v>
       </c>
       <c r="H49" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3187,7 +3189,7 @@
         <v>15</v>
       </c>
       <c r="H50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3249,12 +3251,12 @@
       <c r="I1" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="103" t="s">
-        <v>228</v>
+      <c r="J1" s="102" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
-      <c r="A2" s="95">
+      <c r="A2" s="94">
         <v>1</v>
       </c>
       <c r="B2" s="28">
@@ -3267,13 +3269,13 @@
         <v>158</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>157</v>
@@ -3282,11 +3284,11 @@
         <v>146</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="95">
+      <c r="A3" s="94">
         <v>2</v>
       </c>
       <c r="B3" s="28">
@@ -3300,7 +3302,7 @@
         <v>152</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
@@ -3309,7 +3311,7 @@
         <v>151</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>150</v>
@@ -3317,7 +3319,7 @@
       <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" s="95">
+      <c r="A4" s="94">
         <v>3</v>
       </c>
       <c r="B4" s="28">
@@ -3331,7 +3333,7 @@
         <v>156</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>165</v>
@@ -3339,15 +3341,15 @@
       <c r="G4" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H4" s="107" t="s">
-        <v>239</v>
+      <c r="H4" s="106" t="s">
+        <v>235</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A5" s="95">
+      <c r="A5" s="94">
         <v>4</v>
       </c>
       <c r="B5" s="28">
@@ -3361,7 +3363,7 @@
         <v>155</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>164</v>
@@ -3377,7 +3379,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="95">
+      <c r="A6" s="94">
         <v>5</v>
       </c>
       <c r="B6" s="28">
@@ -3385,29 +3387,29 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>162</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="95">
+      <c r="A7" s="94">
         <v>6</v>
       </c>
       <c r="B7" s="28">
@@ -3415,30 +3417,30 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="H7" s="110" t="s">
+        <v>256</v>
+      </c>
+      <c r="H7" s="109" t="s">
         <v>62</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="J7" s="109"/>
+        <v>254</v>
+      </c>
+      <c r="J7" s="108"/>
     </row>
     <row r="8" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A8" s="95">
+      <c r="A8" s="94">
         <v>7</v>
       </c>
       <c r="B8" s="28">
@@ -3446,29 +3448,29 @@
         <v>42283</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>283</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A9" s="95">
+      <c r="A9" s="94">
         <v>8</v>
       </c>
       <c r="B9" s="28">
@@ -3476,26 +3478,26 @@
         <v>42290</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="95">
+      <c r="A10" s="94">
         <v>9</v>
       </c>
       <c r="B10" s="28">
@@ -3503,16 +3505,16 @@
         <v>42297</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>39</v>
@@ -3521,11 +3523,11 @@
         <v>40</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="95">
+      <c r="A11" s="94">
         <v>10</v>
       </c>
       <c r="B11" s="28">
@@ -3533,26 +3535,26 @@
         <v>42304</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="112">
+      <c r="A12" s="111">
         <v>11</v>
       </c>
       <c r="B12" s="28">
@@ -3560,7 +3562,7 @@
         <v>42311</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>43</v>
@@ -3573,11 +3575,11 @@
         <v>49</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="112">
+      <c r="A13" s="111">
         <v>12</v>
       </c>
       <c r="B13" s="28">
@@ -3585,7 +3587,7 @@
         <v>42318</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -3593,14 +3595,14 @@
         <v>35</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="112">
+      <c r="A14" s="111">
         <v>13</v>
       </c>
       <c r="B14" s="28">
@@ -3614,16 +3616,16 @@
         <v>169</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="115" t="s">
-        <v>290</v>
-      </c>
-      <c r="G14" s="115" t="s">
-        <v>296</v>
+      <c r="F14" s="114" t="s">
+        <v>286</v>
+      </c>
+      <c r="G14" s="114" t="s">
+        <v>292</v>
       </c>
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="112"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="28">
         <f t="shared" si="0"/>
         <v>42332</v>
@@ -3638,7 +3640,7 @@
       <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="112">
+      <c r="A16" s="111">
         <v>14</v>
       </c>
       <c r="B16" s="28">
@@ -3663,7 +3665,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="112">
+      <c r="A17" s="111">
         <v>15</v>
       </c>
       <c r="B17" s="28">
@@ -3678,7 +3680,7 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>49</v>
@@ -3827,11 +3829,11 @@
       <c r="D2" s="8">
         <v>3</v>
       </c>
-      <c r="E2" s="87" t="s">
-        <v>195</v>
-      </c>
-      <c r="F2" s="102" t="s">
-        <v>195</v>
+      <c r="E2" s="86" t="s">
+        <v>194</v>
+      </c>
+      <c r="F2" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G2" s="49"/>
       <c r="H2" s="30" t="s">
@@ -3904,11 +3906,11 @@
         <v>50</v>
       </c>
       <c r="D3" s="60"/>
-      <c r="E3" s="88" t="s">
-        <v>195</v>
-      </c>
-      <c r="F3" s="102" t="s">
-        <v>195</v>
+      <c r="E3" s="87" t="s">
+        <v>194</v>
+      </c>
+      <c r="F3" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G3" s="48"/>
       <c r="H3" s="46" t="s">
@@ -3983,8 +3985,8 @@
       <c r="D4" s="61">
         <v>2</v>
       </c>
-      <c r="E4" s="89" t="s">
-        <v>195</v>
+      <c r="E4" s="88" t="s">
+        <v>194</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="49"/>
@@ -4060,11 +4062,11 @@
       <c r="D5" s="60">
         <v>15</v>
       </c>
-      <c r="E5" s="89" t="s">
-        <v>195</v>
-      </c>
-      <c r="F5" s="102" t="s">
-        <v>224</v>
+      <c r="E5" s="88" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="101" t="s">
+        <v>223</v>
       </c>
       <c r="G5" s="48"/>
       <c r="H5" s="4" t="s">
@@ -4132,11 +4134,11 @@
       <c r="D6" s="60">
         <v>10</v>
       </c>
-      <c r="E6" s="89" t="s">
-        <v>195</v>
-      </c>
-      <c r="F6" s="102" t="s">
-        <v>195</v>
+      <c r="E6" s="88" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G6" s="48"/>
       <c r="H6" s="4" t="s">
@@ -4211,8 +4213,8 @@
       <c r="D7" s="61">
         <v>2</v>
       </c>
-      <c r="E7" s="89" t="s">
-        <v>195</v>
+      <c r="E7" s="88" t="s">
+        <v>194</v>
       </c>
       <c r="F7" s="49"/>
       <c r="G7" s="49"/>
@@ -4288,11 +4290,11 @@
       <c r="D8" s="68">
         <v>10</v>
       </c>
-      <c r="E8" s="89" t="s">
-        <v>195</v>
-      </c>
-      <c r="F8" s="102" t="s">
-        <v>224</v>
+      <c r="E8" s="88" t="s">
+        <v>194</v>
+      </c>
+      <c r="F8" s="101" t="s">
+        <v>223</v>
       </c>
       <c r="G8" s="49"/>
       <c r="H8" s="4"/>
@@ -4354,8 +4356,8 @@
         <v>4</v>
       </c>
       <c r="E9" s="48"/>
-      <c r="F9" s="102" t="s">
-        <v>195</v>
+      <c r="F9" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G9" s="49"/>
       <c r="H9" s="49"/>
@@ -4391,11 +4393,11 @@
       <c r="D10" s="60">
         <v>10</v>
       </c>
-      <c r="E10" s="92" t="s">
-        <v>195</v>
-      </c>
-      <c r="F10" s="102" t="s">
-        <v>195</v>
+      <c r="E10" s="91" t="s">
+        <v>194</v>
+      </c>
+      <c r="F10" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G10" s="48"/>
       <c r="H10" s="49"/>
@@ -4416,8 +4418,8 @@
       <c r="D11" s="61">
         <v>2</v>
       </c>
-      <c r="E11" s="92" t="s">
-        <v>195</v>
+      <c r="E11" s="91" t="s">
+        <v>194</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="48"/>
@@ -4439,11 +4441,11 @@
       <c r="D12" s="60">
         <v>15</v>
       </c>
-      <c r="E12" s="92" t="s">
-        <v>195</v>
-      </c>
-      <c r="F12" s="102" t="s">
-        <v>195</v>
+      <c r="E12" s="91" t="s">
+        <v>194</v>
+      </c>
+      <c r="F12" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G12" s="48"/>
       <c r="H12" s="48"/>
@@ -4464,11 +4466,11 @@
       <c r="D13" s="60">
         <v>10</v>
       </c>
-      <c r="E13" s="94" t="s">
-        <v>195</v>
-      </c>
-      <c r="F13" s="102" t="s">
-        <v>195</v>
+      <c r="E13" s="93" t="s">
+        <v>194</v>
+      </c>
+      <c r="F13" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G13" s="48"/>
       <c r="H13" s="48"/>
@@ -4489,8 +4491,8 @@
       <c r="D14" s="61">
         <v>2</v>
       </c>
-      <c r="E14" s="94" t="s">
-        <v>195</v>
+      <c r="E14" s="93" t="s">
+        <v>194</v>
       </c>
       <c r="F14" s="49"/>
       <c r="G14" s="48"/>
@@ -4515,8 +4517,8 @@
         <v>4</v>
       </c>
       <c r="E15" s="48"/>
-      <c r="F15" s="102" t="s">
-        <v>224</v>
+      <c r="F15" s="101" t="s">
+        <v>223</v>
       </c>
       <c r="G15" s="48"/>
       <c r="H15" s="48"/>
@@ -4540,8 +4542,8 @@
         <v>15</v>
       </c>
       <c r="E16" s="48"/>
-      <c r="F16" s="102" t="s">
-        <v>195</v>
+      <c r="F16" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G16" s="48"/>
       <c r="H16" s="48"/>
@@ -4564,11 +4566,11 @@
       <c r="D17" s="60">
         <v>15</v>
       </c>
-      <c r="E17" s="94" t="s">
-        <v>195</v>
-      </c>
-      <c r="F17" s="102" t="s">
-        <v>195</v>
+      <c r="E17" s="93" t="s">
+        <v>194</v>
+      </c>
+      <c r="F17" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G17" s="48"/>
       <c r="H17" s="48"/>
@@ -4591,11 +4593,11 @@
       <c r="D18" s="60">
         <v>10</v>
       </c>
-      <c r="E18" s="94" t="s">
-        <v>195</v>
-      </c>
-      <c r="F18" s="102" t="s">
-        <v>195</v>
+      <c r="E18" s="93" t="s">
+        <v>194</v>
+      </c>
+      <c r="F18" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G18" s="48"/>
       <c r="H18" s="48"/>
@@ -4618,8 +4620,8 @@
       <c r="D19" s="61">
         <v>2</v>
       </c>
-      <c r="E19" s="94" t="s">
-        <v>195</v>
+      <c r="E19" s="93" t="s">
+        <v>194</v>
       </c>
       <c r="F19" s="52"/>
       <c r="G19" s="48"/>
@@ -4643,11 +4645,11 @@
       <c r="D20" s="60">
         <v>15</v>
       </c>
-      <c r="E20" s="94" t="s">
-        <v>195</v>
-      </c>
-      <c r="F20" s="102" t="s">
-        <v>195</v>
+      <c r="E20" s="93" t="s">
+        <v>194</v>
+      </c>
+      <c r="F20" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G20" s="48"/>
       <c r="H20" s="48"/>
@@ -4670,11 +4672,11 @@
       <c r="D21" s="60">
         <v>10</v>
       </c>
-      <c r="E21" s="98" t="s">
-        <v>195</v>
-      </c>
-      <c r="F21" s="102" t="s">
-        <v>195</v>
+      <c r="E21" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="F21" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G21" s="48"/>
       <c r="H21" s="48"/>
@@ -4697,8 +4699,8 @@
       <c r="D22" s="61">
         <v>2</v>
       </c>
-      <c r="E22" s="98" t="s">
-        <v>195</v>
+      <c r="E22" s="97" t="s">
+        <v>194</v>
       </c>
       <c r="F22" s="49"/>
       <c r="G22" s="48"/>
@@ -4721,8 +4723,8 @@
         <v>4</v>
       </c>
       <c r="E23" s="48"/>
-      <c r="F23" s="102" t="s">
-        <v>195</v>
+      <c r="F23" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G23" s="48"/>
       <c r="H23" s="48"/>
@@ -4744,8 +4746,8 @@
         <v>15</v>
       </c>
       <c r="E24" s="48"/>
-      <c r="F24" s="102" t="s">
-        <v>224</v>
+      <c r="F24" s="101" t="s">
+        <v>223</v>
       </c>
       <c r="G24" s="48"/>
       <c r="H24" s="48"/>
@@ -4769,8 +4771,8 @@
         <v>50</v>
       </c>
       <c r="E25" s="48"/>
-      <c r="F25" s="102" t="s">
-        <v>195</v>
+      <c r="F25" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G25" s="48"/>
       <c r="H25" s="48"/>
@@ -4793,11 +4795,11 @@
       <c r="D26" s="60">
         <v>5</v>
       </c>
-      <c r="E26" s="98" t="s">
-        <v>195</v>
-      </c>
-      <c r="F26" s="102" t="s">
-        <v>195</v>
+      <c r="E26" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="F26" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G26" s="48"/>
       <c r="H26" s="48"/>
@@ -4811,8 +4813,8 @@
       <c r="A27" s="57">
         <v>6.7</v>
       </c>
-      <c r="B27" s="108" t="s">
-        <v>242</v>
+      <c r="B27" s="107" t="s">
+        <v>238</v>
       </c>
       <c r="C27" s="70" t="s">
         <v>12</v>
@@ -4820,8 +4822,8 @@
       <c r="D27" s="60">
         <v>5</v>
       </c>
-      <c r="E27" s="98"/>
-      <c r="F27" s="102"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="101"/>
       <c r="G27" s="48"/>
       <c r="H27" s="48"/>
       <c r="I27" s="48"/>
@@ -4843,11 +4845,11 @@
       <c r="D28" s="60">
         <v>10</v>
       </c>
-      <c r="E28" s="98" t="s">
-        <v>195</v>
-      </c>
-      <c r="F28" s="102" t="s">
-        <v>195</v>
+      <c r="E28" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="F28" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G28" s="48"/>
       <c r="H28" s="48"/>
@@ -4870,8 +4872,8 @@
       <c r="D29" s="61">
         <v>2</v>
       </c>
-      <c r="E29" s="98" t="s">
-        <v>195</v>
+      <c r="E29" s="97" t="s">
+        <v>194</v>
       </c>
       <c r="F29" s="53"/>
       <c r="G29" s="48"/>
@@ -4887,8 +4889,8 @@
       <c r="B30" s="64"/>
       <c r="C30" s="74"/>
       <c r="D30" s="60"/>
-      <c r="E30" s="96"/>
-      <c r="F30" s="102"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="101"/>
       <c r="G30" s="48"/>
       <c r="H30" s="48"/>
       <c r="I30" s="48"/>
@@ -4910,11 +4912,11 @@
       <c r="D31" s="60">
         <v>10</v>
       </c>
-      <c r="E31" s="98" t="s">
-        <v>195</v>
-      </c>
-      <c r="F31" s="102" t="s">
-        <v>195</v>
+      <c r="E31" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="F31" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G31" s="48"/>
       <c r="H31" s="48"/>
@@ -4937,8 +4939,8 @@
       <c r="D32" s="61">
         <v>2</v>
       </c>
-      <c r="E32" s="98" t="s">
-        <v>195</v>
+      <c r="E32" s="97" t="s">
+        <v>194</v>
       </c>
       <c r="F32" s="53"/>
       <c r="G32" s="48"/>
@@ -4961,8 +4963,8 @@
         <v>15</v>
       </c>
       <c r="E33" s="48"/>
-      <c r="F33" s="102" t="s">
-        <v>224</v>
+      <c r="F33" s="101" t="s">
+        <v>223</v>
       </c>
       <c r="G33" s="48"/>
       <c r="H33" s="48"/>
@@ -4983,11 +4985,11 @@
       <c r="D34" s="60">
         <v>10</v>
       </c>
-      <c r="E34" s="102" t="s">
-        <v>195</v>
-      </c>
-      <c r="F34" s="102" t="s">
-        <v>195</v>
+      <c r="E34" s="101" t="s">
+        <v>194</v>
+      </c>
+      <c r="F34" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G34" s="48"/>
       <c r="H34" s="48"/>
@@ -5029,11 +5031,11 @@
       <c r="D36" s="60">
         <v>10</v>
       </c>
-      <c r="E36" s="102" t="s">
-        <v>195</v>
-      </c>
-      <c r="F36" s="102" t="s">
-        <v>195</v>
+      <c r="E36" s="101" t="s">
+        <v>194</v>
+      </c>
+      <c r="F36" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G36" s="48"/>
       <c r="H36" s="48"/>
@@ -5077,7 +5079,7 @@
       </c>
       <c r="E38" s="48"/>
       <c r="F38" s="55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G38" s="48"/>
       <c r="H38" s="48"/>
@@ -5098,11 +5100,11 @@
       <c r="D39" s="60">
         <v>10</v>
       </c>
-      <c r="E39" s="102" t="s">
-        <v>195</v>
-      </c>
-      <c r="F39" s="102" t="s">
-        <v>195</v>
+      <c r="E39" s="101" t="s">
+        <v>194</v>
+      </c>
+      <c r="F39" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G39" s="48"/>
       <c r="H39" s="48"/>
@@ -5145,8 +5147,8 @@
         <v>15</v>
       </c>
       <c r="E41" s="48"/>
-      <c r="F41" s="102" t="s">
-        <v>195</v>
+      <c r="F41" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G41" s="48"/>
       <c r="H41" s="48"/>
@@ -5167,11 +5169,11 @@
       <c r="D42" s="60">
         <v>10</v>
       </c>
-      <c r="E42" s="102" t="s">
-        <v>195</v>
-      </c>
-      <c r="F42" s="102" t="s">
-        <v>195</v>
+      <c r="E42" s="101" t="s">
+        <v>194</v>
+      </c>
+      <c r="F42" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G42" s="48"/>
       <c r="H42" s="48"/>
@@ -5214,8 +5216,8 @@
         <v>4</v>
       </c>
       <c r="E44" s="48"/>
-      <c r="F44" s="102" t="s">
-        <v>195</v>
+      <c r="F44" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G44" s="48"/>
       <c r="H44" s="48"/>
@@ -5237,8 +5239,8 @@
         <v>15</v>
       </c>
       <c r="E45" s="48"/>
-      <c r="F45" s="102" t="s">
-        <v>195</v>
+      <c r="F45" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G45" s="48"/>
       <c r="H45" s="48"/>
@@ -5260,8 +5262,8 @@
         <v>10</v>
       </c>
       <c r="E46" s="48"/>
-      <c r="F46" s="102" t="s">
-        <v>195</v>
+      <c r="F46" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G46" s="48"/>
       <c r="H46" s="48"/>
@@ -5304,8 +5306,8 @@
         <v>15</v>
       </c>
       <c r="E48" s="48"/>
-      <c r="F48" s="102" t="s">
-        <v>224</v>
+      <c r="F48" s="101" t="s">
+        <v>223</v>
       </c>
       <c r="G48" s="48"/>
       <c r="H48" s="48"/>
@@ -5327,8 +5329,8 @@
         <v>10</v>
       </c>
       <c r="E49" s="48"/>
-      <c r="F49" s="102" t="s">
-        <v>195</v>
+      <c r="F49" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G49" s="48"/>
       <c r="H49" s="48"/>
@@ -5371,8 +5373,8 @@
         <v>4</v>
       </c>
       <c r="E51" s="48"/>
-      <c r="F51" s="102" t="s">
-        <v>195</v>
+      <c r="F51" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G51" s="48"/>
       <c r="H51" s="48"/>
@@ -5394,8 +5396,8 @@
         <v>15</v>
       </c>
       <c r="E52" s="48"/>
-      <c r="F52" s="102" t="s">
-        <v>195</v>
+      <c r="F52" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G52" s="48"/>
       <c r="H52" s="48"/>
@@ -5417,8 +5419,8 @@
         <v>10</v>
       </c>
       <c r="E53" s="48"/>
-      <c r="F53" s="102" t="s">
-        <v>195</v>
+      <c r="F53" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G53" s="48"/>
       <c r="H53" s="48"/>
@@ -5461,8 +5463,8 @@
         <v>4</v>
       </c>
       <c r="E55" s="48"/>
-      <c r="F55" s="102" t="s">
-        <v>195</v>
+      <c r="F55" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G55" s="48"/>
       <c r="H55" s="48"/>
@@ -5484,8 +5486,8 @@
         <v>10</v>
       </c>
       <c r="E56" s="48"/>
-      <c r="F56" s="102" t="s">
-        <v>195</v>
+      <c r="F56" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G56" s="48"/>
       <c r="H56" s="48"/>
@@ -5497,8 +5499,8 @@
       <c r="A57" s="57">
         <v>15.5</v>
       </c>
-      <c r="B57" s="108" t="s">
-        <v>242</v>
+      <c r="B57" s="107" t="s">
+        <v>238</v>
       </c>
       <c r="C57" s="70" t="s">
         <v>12</v>
@@ -5506,8 +5508,8 @@
       <c r="D57" s="60">
         <v>5</v>
       </c>
-      <c r="E57" s="98"/>
-      <c r="F57" s="102"/>
+      <c r="E57" s="97"/>
+      <c r="F57" s="101"/>
       <c r="G57" s="48"/>
       <c r="H57" s="48"/>
       <c r="I57" s="48"/>
@@ -5530,8 +5532,8 @@
         <v>5</v>
       </c>
       <c r="E58" s="48"/>
-      <c r="F58" s="102" t="s">
-        <v>195</v>
+      <c r="F58" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G58" s="48"/>
       <c r="H58" s="48"/>
@@ -5553,8 +5555,8 @@
         <v>10</v>
       </c>
       <c r="E59" s="48"/>
-      <c r="F59" s="102" t="s">
-        <v>195</v>
+      <c r="F59" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G59" s="48"/>
       <c r="H59" s="48"/>
@@ -5576,8 +5578,8 @@
         <v>50</v>
       </c>
       <c r="E60" s="48"/>
-      <c r="F60" s="102" t="s">
-        <v>195</v>
+      <c r="F60" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G60" s="48"/>
       <c r="H60" s="48"/>
@@ -5599,8 +5601,8 @@
         <v>2</v>
       </c>
       <c r="E61" s="48"/>
-      <c r="F61" s="102" t="s">
-        <v>195</v>
+      <c r="F61" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G61" s="48"/>
       <c r="H61" s="48"/>
@@ -5622,8 +5624,8 @@
         <v>3</v>
       </c>
       <c r="E62" s="48"/>
-      <c r="F62" s="102" t="s">
-        <v>195</v>
+      <c r="F62" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G62" s="48"/>
       <c r="H62" s="48"/>
@@ -5645,8 +5647,8 @@
         <v>2</v>
       </c>
       <c r="E63" s="48"/>
-      <c r="F63" s="102" t="s">
-        <v>195</v>
+      <c r="F63" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G63" s="48"/>
       <c r="H63" s="48"/>
@@ -5668,8 +5670,8 @@
         <v>10</v>
       </c>
       <c r="E64" s="48"/>
-      <c r="F64" s="102" t="s">
-        <v>195</v>
+      <c r="F64" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G64" s="48"/>
       <c r="H64" s="48"/>
@@ -5691,8 +5693,8 @@
         <v>6</v>
       </c>
       <c r="E65" s="48"/>
-      <c r="F65" s="102" t="s">
-        <v>195</v>
+      <c r="F65" s="101" t="s">
+        <v>194</v>
       </c>
       <c r="G65" s="48"/>
       <c r="H65" s="48"/>

</xml_diff>

<commit_message>
add final time to schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C116B9DD-45C2-4E31-A43F-FF2B077E9287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA608678-72DD-4AE9-8563-B98419F7CC55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3150" yWindow="1155" windowWidth="24765" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="308">
   <si>
     <t>Finals Week</t>
   </si>
@@ -680,9 +680,6 @@
   </si>
   <si>
     <t>Poster prep Stage IV* (Draft Due 12/03, PR 12/05, Final 12/07 )</t>
-  </si>
-  <si>
-    <t>Take home final exam (Due x/xx ); [Metacognition Post-Survey](https://forms.gle/P8q6hbk6eJaScixF6) (Due 12/20 ); [Post Assessment in R](https://forms.gle/FWAZjanJ31hTrSKK8) (Due 12/20 )</t>
   </si>
   <si>
     <t xml:space="preserve">Go relax and take a well deserved break. </t>
@@ -881,9 +878,6 @@
 [[12pm]](https://forms.gle/pa77KXTKYGb86s718)</t>
   </si>
   <si>
-    <t>Monday 4-6pm ARTS 112</t>
-  </si>
-  <si>
     <t xml:space="preserve">How is statistics done in your field? </t>
   </si>
   <si>
@@ -1037,9 +1031,6 @@
 Be ready and able to calculate summary statistics for each (n, # missing values, #yes, mean, sd)</t>
   </si>
   <si>
-    <t xml:space="preserve">e-Poster*  (Draft Due 12/11 , PR 12/13, Final 12/16 12pm ) TIMES ARE FIRM - Dates dependent on time of common final </t>
-  </si>
-  <si>
     <t>Simulating distributions of random variables [[In class activity]](hw/activity_samp_dist.html)</t>
   </si>
   <si>
@@ -1133,10 +1124,6 @@
 [[12pm]](https://forms.gle/KH7REGGTG5GEk34m6)</t>
   </si>
   <si>
-    <t>Develop Research Poster
-Second chance exam</t>
-  </si>
-  <si>
     <t>Quiz 09b (Due 10/22 ) 
 [[10am]](https://forms.gle/PuXQrQqmyNUBx5NK7)
 [[12pm]](https://forms.gle/qVsdx2wfDiHFLNpx9)</t>
@@ -1157,12 +1144,29 @@
 [[12pm]](https://forms.gle/7LL6AGpAZFPrPgqWA)</t>
   </si>
   <si>
-    <t>Quiz 12 (Due 11/10 ) 
+    <t>[hw10_regression](hw/hw10_regression.html) (Due 11/23 )</t>
+  </si>
+  <si>
+    <t>Monday 4-6pm THMA 116</t>
+  </si>
+  <si>
+    <t>Take home final exam (Due 12/18 ); [Metacognition Post-Survey](https://forms.gle/P8q6hbk6eJaScixF6) (Due 12/20 ); [Post Assessment in R](https://forms.gle/FWAZjanJ31hTrSKK8) (Due 12/20 )</t>
+  </si>
+  <si>
+    <t>Distributed on Wednesday 12/11</t>
+  </si>
+  <si>
+    <t>e-Poster*  (Draft Due 12/11 , PR 12/13, Final 12/16 12pm ) TIMES ARE FIRM
+Makeup midterm 12/13</t>
+  </si>
+  <si>
+    <t>Develop Research Poster
+Makeup midterm</t>
+  </si>
+  <si>
+    <t>Quiz 12 (Due 11/12 ) 
 [[10am]](https://forms.gle/yhtcXVUo2Wmx1RWo6)
 [[12pm]](https://forms.gle/CfriRP93zjqD9E1y9)</t>
-  </si>
-  <si>
-    <t>[hw10_regression](hw/hw10_regression.html) (Due 11/23 )</t>
   </si>
 </sst>
 </file>
@@ -1694,7 +1698,7 @@
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1950,15 +1954,6 @@
     <xf numFmtId="0" fontId="33" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1988,7 +1983,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -2413,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="D27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2442,7 +2440,7 @@
         <v>52</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>85</v>
@@ -2468,7 +2466,7 @@
         <v>53</v>
       </c>
       <c r="G2" s="89" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H2" s="90" t="s">
         <v>183</v>
@@ -2487,7 +2485,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2512,7 +2510,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2527,7 +2525,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
         <v>2.1</v>
       </c>
@@ -2538,13 +2536,13 @@
         <v>97</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F8" s="34">
         <v>1.3</v>
       </c>
-      <c r="G8" s="103" t="s">
-        <v>228</v>
+      <c r="G8" s="89" t="s">
+        <v>227</v>
       </c>
       <c r="H8" s="90" t="s">
         <v>184</v>
@@ -2558,7 +2556,7 @@
         <v>98</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2580,7 +2578,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>3.1</v>
       </c>
@@ -2595,8 +2593,8 @@
         <v>70</v>
       </c>
       <c r="F12" s="35"/>
-      <c r="G12" s="104" t="s">
-        <v>232</v>
+      <c r="G12" s="92" t="s">
+        <v>231</v>
       </c>
       <c r="H12" s="90" t="s">
         <v>185</v>
@@ -2626,7 +2624,7 @@
       </c>
       <c r="H14" s="79"/>
     </row>
-    <row r="15" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="39">
         <v>4.0999999999999996</v>
       </c>
@@ -2642,11 +2640,11 @@
       <c r="F15" s="34">
         <v>2.1</v>
       </c>
-      <c r="G15" s="104" t="s">
+      <c r="G15" s="92" t="s">
+        <v>232</v>
+      </c>
+      <c r="H15" s="90" t="s">
         <v>233</v>
-      </c>
-      <c r="H15" s="90" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2660,7 +2658,7 @@
         <v>72</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2685,16 +2683,16 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E18" s="41" t="s">
         <v>73</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="G18" s="104" t="s">
-        <v>239</v>
+        <v>203</v>
+      </c>
+      <c r="G18" s="92" t="s">
+        <v>238</v>
       </c>
       <c r="H18" s="90" t="s">
         <v>187</v>
@@ -2724,8 +2722,8 @@
       <c r="E20" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="104" t="s">
-        <v>249</v>
+      <c r="G20" s="92" t="s">
+        <v>247</v>
       </c>
       <c r="H20" s="96"/>
     </row>
@@ -2740,7 +2738,7 @@
         <v>74</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H21" s="96"/>
     </row>
@@ -2749,10 +2747,10 @@
         <v>6.3</v>
       </c>
       <c r="D22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H22" s="90" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2762,13 +2760,13 @@
       <c r="D23" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="112"/>
-      <c r="F23" s="113"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="110"/>
       <c r="G23" s="92" t="s">
+        <v>248</v>
+      </c>
+      <c r="H23" s="96" t="s">
         <v>250</v>
-      </c>
-      <c r="H23" s="96" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2779,7 +2777,7 @@
         <v>100</v>
       </c>
       <c r="H24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2796,7 +2794,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A26" s="39">
         <v>7.1</v>
       </c>
@@ -2804,19 +2802,19 @@
         <v>7</v>
       </c>
       <c r="D26" s="96" t="s">
-        <v>244</v>
-      </c>
-      <c r="E26" s="110" t="s">
-        <v>271</v>
+        <v>242</v>
+      </c>
+      <c r="E26" s="107" t="s">
+        <v>269</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="G26" s="104" t="s">
+        <v>243</v>
+      </c>
+      <c r="G26" s="92" t="s">
+        <v>270</v>
+      </c>
+      <c r="H26" s="96" t="s">
         <v>272</v>
-      </c>
-      <c r="H26" s="96" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2824,22 +2822,22 @@
         <v>7.2</v>
       </c>
       <c r="D27" s="96" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>269</v>
-      </c>
-      <c r="G27" s="104"/>
+        <v>267</v>
+      </c>
+      <c r="G27" s="92"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="39">
         <v>7.3</v>
       </c>
       <c r="D28" s="90" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2850,10 +2848,10 @@
         <v>65</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="39">
         <v>8.1</v>
       </c>
@@ -2864,16 +2862,16 @@
         <v>58</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F30" s="34">
         <v>4.7</v>
       </c>
-      <c r="G30" s="104" t="s">
-        <v>273</v>
+      <c r="G30" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="H30" s="90" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2881,10 +2879,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D31" s="90" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F31" s="34">
         <v>5</v>
@@ -2895,13 +2893,13 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D32" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F32" s="34">
         <v>6.1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="39">
         <v>9.1</v>
       </c>
@@ -2917,17 +2915,17 @@
       <c r="F33" s="34">
         <v>6.2</v>
       </c>
-      <c r="G33" s="104" t="s">
-        <v>299</v>
+      <c r="G33" s="92" t="s">
+        <v>296</v>
       </c>
       <c r="H33" s="90"/>
     </row>
-    <row r="34" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="39">
         <v>9.1999999999999993</v>
       </c>
       <c r="D34" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E34" s="41" t="s">
         <v>76</v>
@@ -2935,16 +2933,16 @@
       <c r="F34" s="34">
         <v>6.3</v>
       </c>
-      <c r="G34" s="104" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+      <c r="G34" s="92" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="39">
         <v>9.3000000000000007</v>
       </c>
       <c r="D35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E35" s="41" t="s">
         <v>77</v>
@@ -2952,11 +2950,11 @@
       <c r="F35" s="34">
         <v>6.4</v>
       </c>
-      <c r="G35" s="104" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="G35" s="92" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="39">
         <v>10.1</v>
       </c>
@@ -2964,7 +2962,7 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E36" s="41" t="s">
         <v>82</v>
@@ -2972,11 +2970,11 @@
       <c r="F36" s="34">
         <v>6.5</v>
       </c>
-      <c r="G36" s="116" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="G36" s="113" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="39">
         <v>11.1</v>
       </c>
@@ -2992,8 +2990,8 @@
       <c r="F37" s="34">
         <v>7</v>
       </c>
-      <c r="G37" s="104" t="s">
-        <v>304</v>
+      <c r="G37" s="92" t="s">
+        <v>300</v>
       </c>
       <c r="H37" s="90" t="s">
         <v>189</v>
@@ -3010,7 +3008,7 @@
         <v>80</v>
       </c>
       <c r="F38" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3018,13 +3016,13 @@
         <v>11.3</v>
       </c>
       <c r="D39" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="39">
         <v>12.1</v>
       </c>
@@ -3038,13 +3036,13 @@
         <v>79</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="G40" s="104" t="s">
-        <v>305</v>
+        <v>204</v>
+      </c>
+      <c r="G40" s="92" t="s">
+        <v>307</v>
       </c>
       <c r="H40" s="90" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3052,7 +3050,7 @@
         <v>12.2</v>
       </c>
       <c r="D41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E41" s="41" t="s">
         <v>84</v>
@@ -3073,7 +3071,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="39">
         <v>13.1</v>
       </c>
@@ -3081,16 +3079,16 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E43" s="41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F43" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="G43" s="105" t="s">
-        <v>229</v>
+        <v>197</v>
+      </c>
+      <c r="G43" s="114" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3101,7 +3099,7 @@
         <v>91</v>
       </c>
       <c r="F44" s="37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3109,14 +3107,14 @@
         <v>14</v>
       </c>
       <c r="D45" s="83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E45" s="84"/>
       <c r="F45" s="85"/>
       <c r="G45" s="100"/>
       <c r="H45" s="83"/>
     </row>
-    <row r="46" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="39">
         <v>15.1</v>
       </c>
@@ -3129,8 +3127,8 @@
       <c r="F46" s="37">
         <v>8.4</v>
       </c>
-      <c r="G46" s="105" t="s">
-        <v>230</v>
+      <c r="G46" s="114" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3147,24 +3145,24 @@
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="39">
         <v>16.100000000000001</v>
       </c>
       <c r="B48" s="34">
         <v>15</v>
       </c>
-      <c r="D48" s="115" t="s">
-        <v>300</v>
+      <c r="D48" s="112" t="s">
+        <v>306</v>
       </c>
       <c r="E48" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="G48" s="105" t="s">
-        <v>231</v>
-      </c>
-      <c r="H48" t="s">
-        <v>276</v>
+      <c r="G48" s="114" t="s">
+        <v>230</v>
+      </c>
+      <c r="H48" s="112" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3178,7 +3176,7 @@
         <v>86</v>
       </c>
       <c r="H49" t="s">
-        <v>240</v>
+        <v>302</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3188,8 +3186,11 @@
       <c r="D50" t="s">
         <v>15</v>
       </c>
+      <c r="E50" s="41" t="s">
+        <v>304</v>
+      </c>
       <c r="H50" t="s">
-        <v>192</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -3252,7 +3253,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="102" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -3269,13 +3270,13 @@
         <v>158</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>157</v>
@@ -3284,7 +3285,7 @@
         <v>146</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3302,7 +3303,7 @@
         <v>152</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>20</v>
@@ -3311,7 +3312,7 @@
         <v>151</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>150</v>
@@ -3333,7 +3334,7 @@
         <v>156</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>165</v>
@@ -3341,8 +3342,8 @@
       <c r="G4" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H4" s="106" t="s">
-        <v>235</v>
+      <c r="H4" s="103" t="s">
+        <v>234</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>148</v>
@@ -3363,7 +3364,7 @@
         <v>155</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>164</v>
@@ -3387,22 +3388,22 @@
         <v>42269</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>162</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>163</v>
@@ -3417,27 +3418,27 @@
         <v>42276</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="H7" s="109" t="s">
+        <v>254</v>
+      </c>
+      <c r="H7" s="106" t="s">
         <v>62</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="J7" s="108"/>
+        <v>252</v>
+      </c>
+      <c r="J7" s="105"/>
     </row>
     <row r="8" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="94">
@@ -3448,25 +3449,25 @@
         <v>42283</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="I8" s="29" t="s">
         <v>259</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3478,22 +3479,22 @@
         <v>42290</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3505,16 +3506,16 @@
         <v>42297</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>39</v>
@@ -3523,7 +3524,7 @@
         <v>40</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3535,26 +3536,26 @@
         <v>42304</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="111">
+      <c r="A12" s="108">
         <v>11</v>
       </c>
       <c r="B12" s="28">
@@ -3562,7 +3563,7 @@
         <v>42311</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>43</v>
@@ -3575,11 +3576,11 @@
         <v>49</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="111">
+      <c r="A13" s="108">
         <v>12</v>
       </c>
       <c r="B13" s="28">
@@ -3587,7 +3588,7 @@
         <v>42318</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -3595,14 +3596,14 @@
         <v>35</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="111">
+      <c r="A14" s="108">
         <v>13</v>
       </c>
       <c r="B14" s="28">
@@ -3616,16 +3617,16 @@
         <v>169</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="114" t="s">
-        <v>286</v>
-      </c>
-      <c r="G14" s="114" t="s">
-        <v>292</v>
+      <c r="F14" s="111" t="s">
+        <v>283</v>
+      </c>
+      <c r="G14" s="111" t="s">
+        <v>289</v>
       </c>
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="111"/>
+      <c r="A15" s="108"/>
       <c r="B15" s="28">
         <f t="shared" si="0"/>
         <v>42332</v>
@@ -3640,7 +3641,7 @@
       <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="111">
+      <c r="A16" s="108">
         <v>14</v>
       </c>
       <c r="B16" s="28">
@@ -3665,7 +3666,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="111">
+      <c r="A17" s="108">
         <v>15</v>
       </c>
       <c r="B17" s="28">
@@ -3680,7 +3681,7 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>49</v>
@@ -3830,10 +3831,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="86" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F2" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G2" s="49"/>
       <c r="H2" s="30" t="s">
@@ -3907,10 +3908,10 @@
       </c>
       <c r="D3" s="60"/>
       <c r="E3" s="87" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F3" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G3" s="48"/>
       <c r="H3" s="46" t="s">
@@ -3986,7 +3987,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="88" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="49"/>
@@ -4063,10 +4064,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="88" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F5" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G5" s="48"/>
       <c r="H5" s="4" t="s">
@@ -4135,10 +4136,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="88" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F6" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G6" s="48"/>
       <c r="H6" s="4" t="s">
@@ -4214,7 +4215,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="88" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F7" s="49"/>
       <c r="G7" s="49"/>
@@ -4291,10 +4292,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="88" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F8" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G8" s="49"/>
       <c r="H8" s="4"/>
@@ -4357,7 +4358,7 @@
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G9" s="49"/>
       <c r="H9" s="49"/>
@@ -4394,10 +4395,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="91" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F10" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G10" s="48"/>
       <c r="H10" s="49"/>
@@ -4419,7 +4420,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="91" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="48"/>
@@ -4442,10 +4443,10 @@
         <v>15</v>
       </c>
       <c r="E12" s="91" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F12" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G12" s="48"/>
       <c r="H12" s="48"/>
@@ -4467,10 +4468,10 @@
         <v>10</v>
       </c>
       <c r="E13" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F13" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G13" s="48"/>
       <c r="H13" s="48"/>
@@ -4492,7 +4493,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F14" s="49"/>
       <c r="G14" s="48"/>
@@ -4518,7 +4519,7 @@
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G15" s="48"/>
       <c r="H15" s="48"/>
@@ -4543,7 +4544,7 @@
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G16" s="48"/>
       <c r="H16" s="48"/>
@@ -4567,10 +4568,10 @@
         <v>15</v>
       </c>
       <c r="E17" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F17" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G17" s="48"/>
       <c r="H17" s="48"/>
@@ -4594,10 +4595,10 @@
         <v>10</v>
       </c>
       <c r="E18" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F18" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G18" s="48"/>
       <c r="H18" s="48"/>
@@ -4621,7 +4622,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F19" s="52"/>
       <c r="G19" s="48"/>
@@ -4646,10 +4647,10 @@
         <v>15</v>
       </c>
       <c r="E20" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F20" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G20" s="48"/>
       <c r="H20" s="48"/>
@@ -4673,10 +4674,10 @@
         <v>10</v>
       </c>
       <c r="E21" s="97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F21" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G21" s="48"/>
       <c r="H21" s="48"/>
@@ -4700,7 +4701,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F22" s="49"/>
       <c r="G22" s="48"/>
@@ -4724,7 +4725,7 @@
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G23" s="48"/>
       <c r="H23" s="48"/>
@@ -4747,7 +4748,7 @@
       </c>
       <c r="E24" s="48"/>
       <c r="F24" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G24" s="48"/>
       <c r="H24" s="48"/>
@@ -4772,7 +4773,7 @@
       </c>
       <c r="E25" s="48"/>
       <c r="F25" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G25" s="48"/>
       <c r="H25" s="48"/>
@@ -4796,10 +4797,10 @@
         <v>5</v>
       </c>
       <c r="E26" s="97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F26" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G26" s="48"/>
       <c r="H26" s="48"/>
@@ -4813,8 +4814,8 @@
       <c r="A27" s="57">
         <v>6.7</v>
       </c>
-      <c r="B27" s="107" t="s">
-        <v>238</v>
+      <c r="B27" s="104" t="s">
+        <v>237</v>
       </c>
       <c r="C27" s="70" t="s">
         <v>12</v>
@@ -4846,10 +4847,10 @@
         <v>10</v>
       </c>
       <c r="E28" s="97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F28" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G28" s="48"/>
       <c r="H28" s="48"/>
@@ -4873,7 +4874,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F29" s="53"/>
       <c r="G29" s="48"/>
@@ -4913,10 +4914,10 @@
         <v>10</v>
       </c>
       <c r="E31" s="97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F31" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G31" s="48"/>
       <c r="H31" s="48"/>
@@ -4940,7 +4941,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F32" s="53"/>
       <c r="G32" s="48"/>
@@ -4964,7 +4965,7 @@
       </c>
       <c r="E33" s="48"/>
       <c r="F33" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G33" s="48"/>
       <c r="H33" s="48"/>
@@ -4986,10 +4987,10 @@
         <v>10</v>
       </c>
       <c r="E34" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F34" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G34" s="48"/>
       <c r="H34" s="48"/>
@@ -5032,10 +5033,10 @@
         <v>10</v>
       </c>
       <c r="E36" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F36" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G36" s="48"/>
       <c r="H36" s="48"/>
@@ -5079,7 +5080,7 @@
       </c>
       <c r="E38" s="48"/>
       <c r="F38" s="55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G38" s="48"/>
       <c r="H38" s="48"/>
@@ -5101,10 +5102,10 @@
         <v>10</v>
       </c>
       <c r="E39" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F39" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G39" s="48"/>
       <c r="H39" s="48"/>
@@ -5148,7 +5149,7 @@
       </c>
       <c r="E41" s="48"/>
       <c r="F41" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G41" s="48"/>
       <c r="H41" s="48"/>
@@ -5170,10 +5171,10 @@
         <v>10</v>
       </c>
       <c r="E42" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F42" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G42" s="48"/>
       <c r="H42" s="48"/>
@@ -5217,7 +5218,7 @@
       </c>
       <c r="E44" s="48"/>
       <c r="F44" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G44" s="48"/>
       <c r="H44" s="48"/>
@@ -5240,7 +5241,7 @@
       </c>
       <c r="E45" s="48"/>
       <c r="F45" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G45" s="48"/>
       <c r="H45" s="48"/>
@@ -5263,7 +5264,7 @@
       </c>
       <c r="E46" s="48"/>
       <c r="F46" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G46" s="48"/>
       <c r="H46" s="48"/>
@@ -5307,7 +5308,7 @@
       </c>
       <c r="E48" s="48"/>
       <c r="F48" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G48" s="48"/>
       <c r="H48" s="48"/>
@@ -5330,7 +5331,7 @@
       </c>
       <c r="E49" s="48"/>
       <c r="F49" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G49" s="48"/>
       <c r="H49" s="48"/>
@@ -5374,7 +5375,7 @@
       </c>
       <c r="E51" s="48"/>
       <c r="F51" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G51" s="48"/>
       <c r="H51" s="48"/>
@@ -5397,7 +5398,7 @@
       </c>
       <c r="E52" s="48"/>
       <c r="F52" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G52" s="48"/>
       <c r="H52" s="48"/>
@@ -5420,7 +5421,7 @@
       </c>
       <c r="E53" s="48"/>
       <c r="F53" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G53" s="48"/>
       <c r="H53" s="48"/>
@@ -5464,7 +5465,7 @@
       </c>
       <c r="E55" s="48"/>
       <c r="F55" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G55" s="48"/>
       <c r="H55" s="48"/>
@@ -5487,7 +5488,7 @@
       </c>
       <c r="E56" s="48"/>
       <c r="F56" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G56" s="48"/>
       <c r="H56" s="48"/>
@@ -5499,8 +5500,8 @@
       <c r="A57" s="57">
         <v>15.5</v>
       </c>
-      <c r="B57" s="107" t="s">
-        <v>238</v>
+      <c r="B57" s="104" t="s">
+        <v>237</v>
       </c>
       <c r="C57" s="70" t="s">
         <v>12</v>
@@ -5533,7 +5534,7 @@
       </c>
       <c r="E58" s="48"/>
       <c r="F58" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G58" s="48"/>
       <c r="H58" s="48"/>
@@ -5556,7 +5557,7 @@
       </c>
       <c r="E59" s="48"/>
       <c r="F59" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G59" s="48"/>
       <c r="H59" s="48"/>
@@ -5579,7 +5580,7 @@
       </c>
       <c r="E60" s="48"/>
       <c r="F60" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G60" s="48"/>
       <c r="H60" s="48"/>
@@ -5602,7 +5603,7 @@
       </c>
       <c r="E61" s="48"/>
       <c r="F61" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G61" s="48"/>
       <c r="H61" s="48"/>
@@ -5625,7 +5626,7 @@
       </c>
       <c r="E62" s="48"/>
       <c r="F62" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G62" s="48"/>
       <c r="H62" s="48"/>
@@ -5648,7 +5649,7 @@
       </c>
       <c r="E63" s="48"/>
       <c r="F63" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G63" s="48"/>
       <c r="H63" s="48"/>
@@ -5671,7 +5672,7 @@
       </c>
       <c r="E64" s="48"/>
       <c r="F64" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G64" s="48"/>
       <c r="H64" s="48"/>
@@ -5694,7 +5695,7 @@
       </c>
       <c r="E65" s="48"/>
       <c r="F65" s="101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G65" s="48"/>
       <c r="H65" s="48"/>

</xml_diff>

<commit_message>
add hw10 adj schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20346"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA608678-72DD-4AE9-8563-B98419F7CC55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4DA171-158B-4458-8400-23C69C075F23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3150" yWindow="1155" windowWidth="24765" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,14 +26,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -676,9 +668,6 @@
     <t>[hw09_moderation](hw/hw09_moderation.html) (Due 11/09 )</t>
   </si>
   <si>
-    <t>Poster prep Stage III* (Draft Due 11/12, PR 11/14, Final 11/16 )</t>
-  </si>
-  <si>
     <t>Poster prep Stage IV* (Draft Due 12/03, PR 12/05, Final 12/07 )</t>
   </si>
   <si>
@@ -1167,6 +1156,9 @@
     <t>Quiz 12 (Due 11/12 ) 
 [[10am]](https://forms.gle/yhtcXVUo2Wmx1RWo6)
 [[12pm]](https://forms.gle/CfriRP93zjqD9E1y9)</t>
+  </si>
+  <si>
+    <t>Poster prep Stage III* (Draft Due 11/14, PR 11/16, Final 11/18 )</t>
   </si>
 </sst>
 </file>
@@ -2412,7 +2404,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2440,7 +2432,7 @@
         <v>52</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>85</v>
@@ -2466,7 +2458,7 @@
         <v>53</v>
       </c>
       <c r="G2" s="89" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H2" s="90" t="s">
         <v>183</v>
@@ -2485,7 +2477,7 @@
         <v>1.3</v>
       </c>
       <c r="D4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2510,7 +2502,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2536,13 +2528,13 @@
         <v>97</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F8" s="34">
         <v>1.3</v>
       </c>
       <c r="G8" s="89" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H8" s="90" t="s">
         <v>184</v>
@@ -2556,7 +2548,7 @@
         <v>98</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2594,7 +2586,7 @@
       </c>
       <c r="F12" s="35"/>
       <c r="G12" s="92" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H12" s="90" t="s">
         <v>185</v>
@@ -2641,10 +2633,10 @@
         <v>2.1</v>
       </c>
       <c r="G15" s="92" t="s">
+        <v>231</v>
+      </c>
+      <c r="H15" s="90" t="s">
         <v>232</v>
-      </c>
-      <c r="H15" s="90" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2658,7 +2650,7 @@
         <v>72</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2683,16 +2675,16 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E18" s="41" t="s">
         <v>73</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G18" s="92" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H18" s="90" t="s">
         <v>187</v>
@@ -2723,7 +2715,7 @@
         <v>99</v>
       </c>
       <c r="G20" s="92" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H20" s="96"/>
     </row>
@@ -2738,7 +2730,7 @@
         <v>74</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H21" s="96"/>
     </row>
@@ -2747,10 +2739,10 @@
         <v>6.3</v>
       </c>
       <c r="D22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H22" s="90" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2763,10 +2755,10 @@
       <c r="E23" s="109"/>
       <c r="F23" s="110"/>
       <c r="G23" s="92" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H23" s="96" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2777,7 +2769,7 @@
         <v>100</v>
       </c>
       <c r="H24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2802,19 +2794,19 @@
         <v>7</v>
       </c>
       <c r="D26" s="96" t="s">
+        <v>241</v>
+      </c>
+      <c r="E26" s="107" t="s">
+        <v>268</v>
+      </c>
+      <c r="F26" s="34" t="s">
         <v>242</v>
       </c>
-      <c r="E26" s="107" t="s">
+      <c r="G26" s="92" t="s">
         <v>269</v>
       </c>
-      <c r="F26" s="34" t="s">
-        <v>243</v>
-      </c>
-      <c r="G26" s="92" t="s">
-        <v>270</v>
-      </c>
       <c r="H26" s="96" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2822,10 +2814,10 @@
         <v>7.2</v>
       </c>
       <c r="D27" s="96" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G27" s="92"/>
     </row>
@@ -2834,10 +2826,10 @@
         <v>7.3</v>
       </c>
       <c r="D28" s="90" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2848,7 +2840,7 @@
         <v>65</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2862,16 +2854,16 @@
         <v>58</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F30" s="34">
         <v>4.7</v>
       </c>
       <c r="G30" s="92" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H30" s="90" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2879,10 +2871,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D31" s="90" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F31" s="34">
         <v>5</v>
@@ -2893,7 +2885,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F32" s="34">
         <v>6.1</v>
@@ -2916,7 +2908,7 @@
         <v>6.2</v>
       </c>
       <c r="G33" s="92" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H33" s="90"/>
     </row>
@@ -2925,7 +2917,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D34" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E34" s="41" t="s">
         <v>76</v>
@@ -2934,7 +2926,7 @@
         <v>6.3</v>
       </c>
       <c r="G34" s="92" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2942,7 +2934,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E35" s="41" t="s">
         <v>77</v>
@@ -2951,7 +2943,7 @@
         <v>6.4</v>
       </c>
       <c r="G35" s="92" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2962,7 +2954,7 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E36" s="41" t="s">
         <v>82</v>
@@ -2971,7 +2963,7 @@
         <v>6.5</v>
       </c>
       <c r="G36" s="113" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2991,7 +2983,7 @@
         <v>7</v>
       </c>
       <c r="G37" s="92" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H37" s="90" t="s">
         <v>189</v>
@@ -3008,7 +3000,7 @@
         <v>80</v>
       </c>
       <c r="F38" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3016,10 +3008,10 @@
         <v>11.3</v>
       </c>
       <c r="D39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3036,13 +3028,13 @@
         <v>79</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G40" s="92" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H40" s="90" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3050,7 +3042,7 @@
         <v>12.2</v>
       </c>
       <c r="D41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E41" s="41" t="s">
         <v>84</v>
@@ -3068,7 +3060,7 @@
       <c r="F42" s="82"/>
       <c r="G42" s="99"/>
       <c r="H42" s="80" t="s">
-        <v>190</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3079,16 +3071,16 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E43" s="41" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F43" s="37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G43" s="114" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3099,7 +3091,7 @@
         <v>91</v>
       </c>
       <c r="F44" s="37" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3107,7 +3099,7 @@
         <v>14</v>
       </c>
       <c r="D45" s="83" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E45" s="84"/>
       <c r="F45" s="85"/>
@@ -3128,7 +3120,7 @@
         <v>8.4</v>
       </c>
       <c r="G46" s="114" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3142,7 +3134,7 @@
       <c r="F47" s="82"/>
       <c r="G47" s="99"/>
       <c r="H47" s="80" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -3153,16 +3145,16 @@
         <v>15</v>
       </c>
       <c r